<commit_message>
new goblin skill image
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="1450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="1451">
   <si>
     <t>夜色</t>
   </si>
@@ -5333,10 +5333,15 @@
     <t>s.Atk.Source*=1.2;</t>
   </si>
   <si>
-    <t>s.Summon(2,51000019);</t>
-  </si>
-  <si>
     <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,"A","L",10,s.Position,"curseoff")) o.ClearDebuff();</t>
+  </si>
+  <si>
+    <t>s.Summon(3,51000019);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gebulin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6458,108 +6463,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="宋体"/>
@@ -6774,6 +6677,40 @@
           <color theme="4"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -7426,6 +7363,40 @@
           <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -8054,6 +8025,40 @@
           <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -8469,80 +8474,80 @@
     <tableColumn id="26" name="CheckDamage" dataDxfId="58"/>
     <tableColumn id="29" name="AfterHit" dataDxfId="57"/>
     <tableColumn id="5" name="CheckSpecial" dataDxfId="56"/>
-    <tableColumn id="9" name="SpecialCd" dataDxfId="2"/>
-    <tableColumn id="25" name="Active" dataDxfId="55"/>
-    <tableColumn id="20" name="IsRandom" dataDxfId="54"/>
-    <tableColumn id="23" name="GetDescript" dataDxfId="53"/>
-    <tableColumn id="8" name="DescriptBuffId" dataDxfId="52"/>
-    <tableColumn id="17" name="Effect" dataDxfId="51"/>
-    <tableColumn id="6" name="Cover" dataDxfId="50"/>
-    <tableColumn id="18" name="Mark" dataDxfId="49"/>
-    <tableColumn id="19" name="Icon" dataDxfId="48"/>
-    <tableColumn id="7" name="Remark" dataDxfId="47"/>
+    <tableColumn id="9" name="SpecialCd" dataDxfId="55"/>
+    <tableColumn id="25" name="Active" dataDxfId="54"/>
+    <tableColumn id="20" name="IsRandom" dataDxfId="53"/>
+    <tableColumn id="23" name="GetDescript" dataDxfId="52"/>
+    <tableColumn id="8" name="DescriptBuffId" dataDxfId="51"/>
+    <tableColumn id="17" name="Effect" dataDxfId="50"/>
+    <tableColumn id="6" name="Cover" dataDxfId="49"/>
+    <tableColumn id="18" name="Mark" dataDxfId="48"/>
+    <tableColumn id="19" name="Icon" dataDxfId="47"/>
+    <tableColumn id="7" name="Remark" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表3_2" displayName="表3_2" ref="A3:T5" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表3_2" displayName="表3_2" ref="A3:T5" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A3:T5"/>
   <sortState ref="A4:T346">
     <sortCondition ref="A3:A346"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="43"/>
-    <tableColumn id="2" name="Name" dataDxfId="42"/>
-    <tableColumn id="3" name="Type" dataDxfId="41"/>
-    <tableColumn id="24" name="OnAdd" dataDxfId="40"/>
-    <tableColumn id="4" name="OnRemove" dataDxfId="39"/>
-    <tableColumn id="27" name="CanBurst" dataDxfId="38"/>
-    <tableColumn id="22" name="CheckHit" dataDxfId="37"/>
-    <tableColumn id="26" name="CheckDamage" dataDxfId="36"/>
-    <tableColumn id="29" name="AfterHit" dataDxfId="35"/>
-    <tableColumn id="5" name="CheckSpecial" dataDxfId="34"/>
-    <tableColumn id="9" name="SpecialCd" dataDxfId="1"/>
-    <tableColumn id="25" name="Active" dataDxfId="33"/>
-    <tableColumn id="20" name="IsRandom" dataDxfId="32"/>
-    <tableColumn id="23" name="GetDescript" dataDxfId="31"/>
-    <tableColumn id="8" name="DescriptBuffId" dataDxfId="30"/>
-    <tableColumn id="17" name="Effect" dataDxfId="29"/>
-    <tableColumn id="6" name="Cover" dataDxfId="28"/>
-    <tableColumn id="18" name="Mark" dataDxfId="27"/>
-    <tableColumn id="19" name="Icon" dataDxfId="26"/>
-    <tableColumn id="7" name="Remark" dataDxfId="25"/>
+    <tableColumn id="1" name="Id" dataDxfId="42"/>
+    <tableColumn id="2" name="Name" dataDxfId="41"/>
+    <tableColumn id="3" name="Type" dataDxfId="40"/>
+    <tableColumn id="24" name="OnAdd" dataDxfId="39"/>
+    <tableColumn id="4" name="OnRemove" dataDxfId="38"/>
+    <tableColumn id="27" name="CanBurst" dataDxfId="37"/>
+    <tableColumn id="22" name="CheckHit" dataDxfId="36"/>
+    <tableColumn id="26" name="CheckDamage" dataDxfId="35"/>
+    <tableColumn id="29" name="AfterHit" dataDxfId="34"/>
+    <tableColumn id="5" name="CheckSpecial" dataDxfId="33"/>
+    <tableColumn id="9" name="SpecialCd" dataDxfId="32"/>
+    <tableColumn id="25" name="Active" dataDxfId="31"/>
+    <tableColumn id="20" name="IsRandom" dataDxfId="30"/>
+    <tableColumn id="23" name="GetDescript" dataDxfId="29"/>
+    <tableColumn id="8" name="DescriptBuffId" dataDxfId="28"/>
+    <tableColumn id="17" name="Effect" dataDxfId="27"/>
+    <tableColumn id="6" name="Cover" dataDxfId="26"/>
+    <tableColumn id="18" name="Mark" dataDxfId="25"/>
+    <tableColumn id="19" name="Icon" dataDxfId="24"/>
+    <tableColumn id="7" name="Remark" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表3_23" displayName="表3_23" ref="A3:T19" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表3_23" displayName="表3_23" ref="A3:T19" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A3:T19"/>
   <sortState ref="A4:T346">
     <sortCondition ref="A3:A346"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="21"/>
-    <tableColumn id="2" name="Name" dataDxfId="20"/>
-    <tableColumn id="3" name="Type" dataDxfId="19"/>
-    <tableColumn id="24" name="OnAdd" dataDxfId="18"/>
-    <tableColumn id="4" name="OnRemove" dataDxfId="17"/>
-    <tableColumn id="27" name="CanBurst" dataDxfId="16"/>
-    <tableColumn id="22" name="CheckHit" dataDxfId="15"/>
-    <tableColumn id="26" name="CheckDamage" dataDxfId="14"/>
-    <tableColumn id="29" name="AfterHit" dataDxfId="13"/>
-    <tableColumn id="5" name="CheckSpecial" dataDxfId="12"/>
-    <tableColumn id="9" name="SpecialCd" dataDxfId="0"/>
-    <tableColumn id="25" name="Active" dataDxfId="11"/>
-    <tableColumn id="20" name="IsRandom" dataDxfId="10"/>
-    <tableColumn id="23" name="GetDescript" dataDxfId="9"/>
-    <tableColumn id="8" name="DescriptBuffId" dataDxfId="8"/>
-    <tableColumn id="17" name="Effect" dataDxfId="7"/>
-    <tableColumn id="6" name="Cover" dataDxfId="6"/>
-    <tableColumn id="18" name="Mark" dataDxfId="5"/>
-    <tableColumn id="19" name="Icon" dataDxfId="4"/>
-    <tableColumn id="7" name="Remark" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="3" name="Type" dataDxfId="17"/>
+    <tableColumn id="24" name="OnAdd" dataDxfId="16"/>
+    <tableColumn id="4" name="OnRemove" dataDxfId="15"/>
+    <tableColumn id="27" name="CanBurst" dataDxfId="14"/>
+    <tableColumn id="22" name="CheckHit" dataDxfId="13"/>
+    <tableColumn id="26" name="CheckDamage" dataDxfId="12"/>
+    <tableColumn id="29" name="AfterHit" dataDxfId="11"/>
+    <tableColumn id="5" name="CheckSpecial" dataDxfId="10"/>
+    <tableColumn id="9" name="SpecialCd" dataDxfId="9"/>
+    <tableColumn id="25" name="Active" dataDxfId="8"/>
+    <tableColumn id="20" name="IsRandom" dataDxfId="7"/>
+    <tableColumn id="23" name="GetDescript" dataDxfId="6"/>
+    <tableColumn id="8" name="DescriptBuffId" dataDxfId="5"/>
+    <tableColumn id="17" name="Effect" dataDxfId="4"/>
+    <tableColumn id="6" name="Cover" dataDxfId="3"/>
+    <tableColumn id="18" name="Mark" dataDxfId="2"/>
+    <tableColumn id="19" name="Icon" dataDxfId="1"/>
+    <tableColumn id="7" name="Remark" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8841,7 +8846,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C283" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J285" sqref="J285"/>
+      <selection pane="bottomRight" activeCell="S286" sqref="S286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9050,7 +9055,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="48">
+    <row r="4" spans="1:20" ht="45.6">
       <c r="A4">
         <v>55000001</v>
       </c>
@@ -9096,7 +9101,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="60">
+    <row r="5" spans="1:20" ht="57">
       <c r="A5">
         <v>55000002</v>
       </c>
@@ -9140,7 +9145,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="24">
+    <row r="6" spans="1:20" ht="22.8">
       <c r="A6">
         <v>55000003</v>
       </c>
@@ -9184,7 +9189,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="48">
+    <row r="7" spans="1:20" ht="45.6">
       <c r="A7">
         <v>55000004</v>
       </c>
@@ -9230,7 +9235,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="48">
+    <row r="8" spans="1:20" ht="45.6">
       <c r="A8">
         <v>55000005</v>
       </c>
@@ -9276,7 +9281,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="48">
+    <row r="9" spans="1:20" ht="45.6">
       <c r="A9">
         <v>55000006</v>
       </c>
@@ -9322,7 +9327,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="48">
+    <row r="10" spans="1:20" ht="45.6">
       <c r="A10">
         <v>55000007</v>
       </c>
@@ -9368,7 +9373,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="48">
+    <row r="11" spans="1:20" ht="45.6">
       <c r="A11">
         <v>55000008</v>
       </c>
@@ -9414,7 +9419,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="48">
+    <row r="12" spans="1:20" ht="45.6">
       <c r="A12">
         <v>55000009</v>
       </c>
@@ -9460,7 +9465,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="48">
+    <row r="13" spans="1:20" ht="45.6">
       <c r="A13">
         <v>55000010</v>
       </c>
@@ -9506,7 +9511,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="48">
+    <row r="14" spans="1:20" ht="45.6">
       <c r="A14">
         <v>55000011</v>
       </c>
@@ -9552,7 +9557,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="48">
+    <row r="15" spans="1:20" ht="45.6">
       <c r="A15">
         <v>55000012</v>
       </c>
@@ -9598,7 +9603,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="48">
+    <row r="16" spans="1:20" ht="45.6">
       <c r="A16">
         <v>55000013</v>
       </c>
@@ -9644,7 +9649,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="48">
+    <row r="17" spans="1:20" ht="45.6">
       <c r="A17">
         <v>55000014</v>
       </c>
@@ -9690,7 +9695,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="48">
+    <row r="18" spans="1:20" ht="45.6">
       <c r="A18">
         <v>55000015</v>
       </c>
@@ -9736,7 +9741,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="48">
+    <row r="19" spans="1:20" ht="45.6">
       <c r="A19">
         <v>55000016</v>
       </c>
@@ -9782,7 +9787,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="48">
+    <row r="20" spans="1:20" ht="45.6">
       <c r="A20">
         <v>55000017</v>
       </c>
@@ -9828,7 +9833,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="48">
+    <row r="21" spans="1:20" ht="45.6">
       <c r="A21">
         <v>55000018</v>
       </c>
@@ -9874,7 +9879,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="48">
+    <row r="22" spans="1:20" ht="45.6">
       <c r="A22">
         <v>55000019</v>
       </c>
@@ -9920,7 +9925,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="48">
+    <row r="23" spans="1:20" ht="45.6">
       <c r="A23">
         <v>55000020</v>
       </c>
@@ -10008,7 +10013,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="36">
+    <row r="25" spans="1:20" ht="34.200000000000003">
       <c r="A25">
         <v>55000029</v>
       </c>
@@ -10052,7 +10057,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="48">
+    <row r="26" spans="1:20" ht="45.6">
       <c r="A26">
         <v>55000030</v>
       </c>
@@ -10098,7 +10103,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="36">
+    <row r="27" spans="1:20" ht="34.200000000000003">
       <c r="A27">
         <v>55000031</v>
       </c>
@@ -10144,7 +10149,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="36">
+    <row r="28" spans="1:20" ht="34.200000000000003">
       <c r="A28">
         <v>55000032</v>
       </c>
@@ -10234,7 +10239,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="60">
+    <row r="30" spans="1:20" ht="57">
       <c r="A30">
         <v>55000034</v>
       </c>
@@ -10278,7 +10283,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="36">
+    <row r="31" spans="1:20" ht="34.200000000000003">
       <c r="A31">
         <v>55000035</v>
       </c>
@@ -10322,7 +10327,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="48">
+    <row r="32" spans="1:20" ht="45.6">
       <c r="A32">
         <v>55000036</v>
       </c>
@@ -10368,7 +10373,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="48">
+    <row r="33" spans="1:20" ht="45.6">
       <c r="A33">
         <v>55000037</v>
       </c>
@@ -10412,7 +10417,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="48">
+    <row r="34" spans="1:20" ht="45.6">
       <c r="A34">
         <v>55000038</v>
       </c>
@@ -10456,7 +10461,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="48">
+    <row r="35" spans="1:20" ht="45.6">
       <c r="A35">
         <v>55000039</v>
       </c>
@@ -10500,7 +10505,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="48">
+    <row r="36" spans="1:20" ht="45.6">
       <c r="A36">
         <v>55000040</v>
       </c>
@@ -10544,7 +10549,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="48">
+    <row r="37" spans="1:20" ht="45.6">
       <c r="A37">
         <v>55000041</v>
       </c>
@@ -10592,7 +10597,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="48">
+    <row r="38" spans="1:20" ht="45.6">
       <c r="A38">
         <v>55000042</v>
       </c>
@@ -10638,7 +10643,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="24">
+    <row r="39" spans="1:20" ht="22.8">
       <c r="A39">
         <v>55000043</v>
       </c>
@@ -10682,7 +10687,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="36">
+    <row r="40" spans="1:20" ht="34.200000000000003">
       <c r="A40">
         <v>55000044</v>
       </c>
@@ -10726,7 +10731,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="36">
+    <row r="41" spans="1:20" ht="34.200000000000003">
       <c r="A41">
         <v>55000045</v>
       </c>
@@ -10770,7 +10775,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="48">
+    <row r="42" spans="1:20" ht="34.200000000000003">
       <c r="A42">
         <v>55000046</v>
       </c>
@@ -10814,7 +10819,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="48">
+    <row r="43" spans="1:20" ht="45.6">
       <c r="A43">
         <v>55000047</v>
       </c>
@@ -10860,7 +10865,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="36">
+    <row r="44" spans="1:20" ht="34.200000000000003">
       <c r="A44">
         <v>55000048</v>
       </c>
@@ -10906,7 +10911,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="48">
+    <row r="45" spans="1:20" ht="45.6">
       <c r="A45">
         <v>55000049</v>
       </c>
@@ -10950,7 +10955,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="48">
+    <row r="46" spans="1:20" ht="45.6">
       <c r="A46">
         <v>55000050</v>
       </c>
@@ -11040,7 +11045,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="48">
+    <row r="48" spans="1:20" ht="45.6">
       <c r="A48">
         <v>55000061</v>
       </c>
@@ -11086,7 +11091,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="36">
+    <row r="49" spans="1:20" ht="34.200000000000003">
       <c r="A49">
         <v>55000062</v>
       </c>
@@ -11130,7 +11135,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="48">
+    <row r="50" spans="1:20" ht="45.6">
       <c r="A50">
         <v>55000063</v>
       </c>
@@ -11176,7 +11181,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="84">
+    <row r="51" spans="1:20" ht="79.8">
       <c r="A51">
         <v>55000064</v>
       </c>
@@ -11224,7 +11229,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="48">
+    <row r="52" spans="1:20" ht="45.6">
       <c r="A52">
         <v>55000065</v>
       </c>
@@ -11270,7 +11275,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="48">
+    <row r="53" spans="1:20" ht="45.6">
       <c r="A53">
         <v>55000066</v>
       </c>
@@ -11316,7 +11321,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="48">
+    <row r="54" spans="1:20" ht="45.6">
       <c r="A54">
         <v>55000067</v>
       </c>
@@ -11362,7 +11367,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="48">
+    <row r="55" spans="1:20" ht="45.6">
       <c r="A55">
         <v>55000068</v>
       </c>
@@ -11408,7 +11413,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="48">
+    <row r="56" spans="1:20" ht="45.6">
       <c r="A56">
         <v>55000069</v>
       </c>
@@ -11454,7 +11459,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="48">
+    <row r="57" spans="1:20" ht="45.6">
       <c r="A57">
         <v>55000070</v>
       </c>
@@ -11500,7 +11505,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="48">
+    <row r="58" spans="1:20" ht="45.6">
       <c r="A58">
         <v>55000071</v>
       </c>
@@ -11546,7 +11551,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="48">
+    <row r="59" spans="1:20" ht="45.6">
       <c r="A59">
         <v>55000072</v>
       </c>
@@ -11592,7 +11597,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="48">
+    <row r="60" spans="1:20" ht="45.6">
       <c r="A60">
         <v>55000073</v>
       </c>
@@ -11638,7 +11643,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="24">
+    <row r="61" spans="1:20" ht="22.8">
       <c r="A61">
         <v>55000074</v>
       </c>
@@ -11682,7 +11687,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="144">
+    <row r="62" spans="1:20" ht="136.80000000000001">
       <c r="A62">
         <v>55000075</v>
       </c>
@@ -11730,7 +11735,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="36">
+    <row r="63" spans="1:20" ht="34.200000000000003">
       <c r="A63">
         <v>55000076</v>
       </c>
@@ -11774,7 +11779,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="48">
+    <row r="64" spans="1:20" ht="45.6">
       <c r="A64">
         <v>55000077</v>
       </c>
@@ -11820,7 +11825,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="24">
+    <row r="65" spans="1:20" ht="22.8">
       <c r="A65">
         <v>55000078</v>
       </c>
@@ -11864,7 +11869,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="24">
+    <row r="66" spans="1:20" ht="22.8">
       <c r="A66">
         <v>55000079</v>
       </c>
@@ -11910,7 +11915,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="24">
+    <row r="67" spans="1:20" ht="22.8">
       <c r="A67">
         <v>55000080</v>
       </c>
@@ -11956,7 +11961,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="24">
+    <row r="68" spans="1:20" ht="22.8">
       <c r="A68">
         <v>55000081</v>
       </c>
@@ -12000,7 +12005,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="36">
+    <row r="69" spans="1:20" ht="34.200000000000003">
       <c r="A69">
         <v>55000082</v>
       </c>
@@ -12046,7 +12051,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="72">
+    <row r="70" spans="1:20" ht="57">
       <c r="A70">
         <v>55000083</v>
       </c>
@@ -12094,7 +12099,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="24">
+    <row r="71" spans="1:20" ht="22.8">
       <c r="A71">
         <v>55000084</v>
       </c>
@@ -12142,7 +12147,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="48">
+    <row r="72" spans="1:20" ht="45.6">
       <c r="A72">
         <v>55000085</v>
       </c>
@@ -12188,7 +12193,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="48">
+    <row r="73" spans="1:20" ht="45.6">
       <c r="A73">
         <v>55000086</v>
       </c>
@@ -12234,7 +12239,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="36">
+    <row r="74" spans="1:20" ht="34.200000000000003">
       <c r="A74">
         <v>55000087</v>
       </c>
@@ -12278,7 +12283,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="36">
+    <row r="75" spans="1:20" ht="34.200000000000003">
       <c r="A75">
         <v>55000088</v>
       </c>
@@ -12322,7 +12327,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="24">
+    <row r="76" spans="1:20" ht="22.8">
       <c r="A76">
         <v>55000089</v>
       </c>
@@ -12366,7 +12371,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="48">
+    <row r="77" spans="1:20" ht="45.6">
       <c r="A77">
         <v>55000090</v>
       </c>
@@ -12410,7 +12415,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="24">
+    <row r="78" spans="1:20" ht="22.8">
       <c r="A78">
         <v>55000091</v>
       </c>
@@ -12454,7 +12459,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="48">
+    <row r="79" spans="1:20" ht="45.6">
       <c r="A79">
         <v>55000092</v>
       </c>
@@ -12502,7 +12507,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="36">
+    <row r="80" spans="1:20" ht="34.200000000000003">
       <c r="A80">
         <v>55000093</v>
       </c>
@@ -12546,7 +12551,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="36">
+    <row r="81" spans="1:20" ht="34.200000000000003">
       <c r="A81">
         <v>55000094</v>
       </c>
@@ -12590,7 +12595,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="36">
+    <row r="82" spans="1:20" ht="34.200000000000003">
       <c r="A82">
         <v>55000095</v>
       </c>
@@ -12634,7 +12639,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="108">
+    <row r="83" spans="1:20" ht="102.6">
       <c r="A83">
         <v>55000096</v>
       </c>
@@ -12678,7 +12683,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="60">
+    <row r="84" spans="1:20" ht="57">
       <c r="A84">
         <v>55000097</v>
       </c>
@@ -12724,7 +12729,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="108">
+    <row r="85" spans="1:20" ht="102.6">
       <c r="A85">
         <v>55000098</v>
       </c>
@@ -12775,7 +12780,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="36">
+    <row r="86" spans="1:20" ht="34.200000000000003">
       <c r="A86">
         <v>55000099</v>
       </c>
@@ -12819,7 +12824,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="36">
+    <row r="87" spans="1:20" ht="34.200000000000003">
       <c r="A87">
         <v>55000100</v>
       </c>
@@ -12867,7 +12872,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="24">
+    <row r="88" spans="1:20" ht="22.8">
       <c r="A88">
         <v>55000101</v>
       </c>
@@ -12911,7 +12916,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="24">
+    <row r="89" spans="1:20" ht="22.8">
       <c r="A89">
         <v>55000102</v>
       </c>
@@ -12997,7 +13002,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="48">
+    <row r="91" spans="1:20" ht="45.6">
       <c r="A91">
         <v>55000104</v>
       </c>
@@ -13043,7 +13048,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="108">
+    <row r="92" spans="1:20" ht="102.6">
       <c r="A92">
         <v>55000105</v>
       </c>
@@ -13094,7 +13099,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="72">
+    <row r="93" spans="1:20" ht="68.400000000000006">
       <c r="A93">
         <v>55000106</v>
       </c>
@@ -13140,7 +13145,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="48">
+    <row r="94" spans="1:20" ht="45.6">
       <c r="A94">
         <v>55000107</v>
       </c>
@@ -13186,7 +13191,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="60">
+    <row r="95" spans="1:20" ht="57">
       <c r="A95">
         <v>55000108</v>
       </c>
@@ -13232,7 +13237,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="36">
+    <row r="96" spans="1:20" ht="34.200000000000003">
       <c r="A96">
         <v>55000109</v>
       </c>
@@ -13276,7 +13281,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="36">
+    <row r="97" spans="1:20" ht="34.200000000000003">
       <c r="A97">
         <v>55000110</v>
       </c>
@@ -13320,7 +13325,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="36">
+    <row r="98" spans="1:20" ht="34.200000000000003">
       <c r="A98">
         <v>55000111</v>
       </c>
@@ -13368,7 +13373,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="24">
+    <row r="99" spans="1:20" ht="22.8">
       <c r="A99">
         <v>55000112</v>
       </c>
@@ -13414,7 +13419,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="48">
+    <row r="100" spans="1:20" ht="45.6">
       <c r="A100">
         <v>55000113</v>
       </c>
@@ -13460,7 +13465,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="36">
+    <row r="101" spans="1:20" ht="34.200000000000003">
       <c r="A101">
         <v>55000114</v>
       </c>
@@ -13504,7 +13509,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="48">
+    <row r="102" spans="1:20" ht="45.6">
       <c r="A102">
         <v>55000115</v>
       </c>
@@ -13552,7 +13557,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="24">
+    <row r="103" spans="1:20" ht="22.8">
       <c r="A103">
         <v>55000116</v>
       </c>
@@ -13596,7 +13601,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="72">
+    <row r="104" spans="1:20" ht="68.400000000000006">
       <c r="A104">
         <v>55000117</v>
       </c>
@@ -13642,7 +13647,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="48">
+    <row r="105" spans="1:20" ht="45.6">
       <c r="A105">
         <v>55000118</v>
       </c>
@@ -13688,7 +13693,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="48">
+    <row r="106" spans="1:20" ht="45.6">
       <c r="A106">
         <v>55000119</v>
       </c>
@@ -13734,7 +13739,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="36">
+    <row r="107" spans="1:20" ht="34.200000000000003">
       <c r="A107">
         <v>55000120</v>
       </c>
@@ -13778,7 +13783,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="36">
+    <row r="108" spans="1:20" ht="34.200000000000003">
       <c r="A108">
         <v>55000121</v>
       </c>
@@ -13826,7 +13831,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="48">
+    <row r="109" spans="1:20" ht="45.6">
       <c r="A109">
         <v>55000122</v>
       </c>
@@ -13872,7 +13877,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="48">
+    <row r="110" spans="1:20" ht="45.6">
       <c r="A110">
         <v>55000123</v>
       </c>
@@ -13918,7 +13923,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="48">
+    <row r="111" spans="1:20" ht="45.6">
       <c r="A111">
         <v>55000124</v>
       </c>
@@ -13964,7 +13969,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="36">
+    <row r="112" spans="1:20" ht="34.200000000000003">
       <c r="A112">
         <v>55000125</v>
       </c>
@@ -14008,7 +14013,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="60">
+    <row r="113" spans="1:20" ht="57">
       <c r="A113">
         <v>55000126</v>
       </c>
@@ -14136,7 +14141,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="24">
+    <row r="116" spans="1:20" ht="22.8">
       <c r="A116">
         <v>55000129</v>
       </c>
@@ -14180,7 +14185,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="24">
+    <row r="117" spans="1:20" ht="22.8">
       <c r="A117">
         <v>55000130</v>
       </c>
@@ -14224,7 +14229,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="36">
+    <row r="118" spans="1:20" ht="34.200000000000003">
       <c r="A118">
         <v>55000131</v>
       </c>
@@ -14268,7 +14273,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="36">
+    <row r="119" spans="1:20" ht="34.200000000000003">
       <c r="A119">
         <v>55000132</v>
       </c>
@@ -14312,7 +14317,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="144">
+    <row r="120" spans="1:20" ht="136.80000000000001">
       <c r="A120">
         <v>55000133</v>
       </c>
@@ -14356,7 +14361,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="60">
+    <row r="121" spans="1:20" ht="57">
       <c r="A121">
         <v>55000134</v>
       </c>
@@ -14402,7 +14407,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="48">
+    <row r="122" spans="1:20" ht="45.6">
       <c r="A122">
         <v>55000135</v>
       </c>
@@ -14446,7 +14451,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="36">
+    <row r="123" spans="1:20" ht="34.200000000000003">
       <c r="A123">
         <v>55000136</v>
       </c>
@@ -14490,7 +14495,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="48">
+    <row r="124" spans="1:20" ht="45.6">
       <c r="A124">
         <v>55000137</v>
       </c>
@@ -14536,7 +14541,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="36">
+    <row r="125" spans="1:20" ht="34.200000000000003">
       <c r="A125">
         <v>55000138</v>
       </c>
@@ -14580,7 +14585,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="48">
+    <row r="126" spans="1:20" ht="45.6">
       <c r="A126">
         <v>55000139</v>
       </c>
@@ -14626,7 +14631,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="60">
+    <row r="127" spans="1:20" ht="57">
       <c r="A127">
         <v>55000140</v>
       </c>
@@ -14672,7 +14677,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="48">
+    <row r="128" spans="1:20" ht="45.6">
       <c r="A128">
         <v>55000141</v>
       </c>
@@ -14718,7 +14723,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="36">
+    <row r="129" spans="1:20" ht="34.200000000000003">
       <c r="A129">
         <v>55000142</v>
       </c>
@@ -14762,7 +14767,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="24">
+    <row r="130" spans="1:20" ht="22.8">
       <c r="A130">
         <v>55000143</v>
       </c>
@@ -14811,7 +14816,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="48">
+    <row r="131" spans="1:20" ht="45.6">
       <c r="A131">
         <v>55000144</v>
       </c>
@@ -14857,7 +14862,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="36">
+    <row r="132" spans="1:20" ht="34.200000000000003">
       <c r="A132">
         <v>55000145</v>
       </c>
@@ -14901,7 +14906,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="48">
+    <row r="133" spans="1:20" ht="45.6">
       <c r="A133">
         <v>55000146</v>
       </c>
@@ -14947,7 +14952,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="36">
+    <row r="134" spans="1:20" ht="34.200000000000003">
       <c r="A134">
         <v>55000147</v>
       </c>
@@ -14991,7 +14996,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="48">
+    <row r="135" spans="1:20" ht="45.6">
       <c r="A135">
         <v>55000148</v>
       </c>
@@ -15037,7 +15042,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="36">
+    <row r="136" spans="1:20" ht="34.200000000000003">
       <c r="A136">
         <v>55000149</v>
       </c>
@@ -15081,7 +15086,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="36">
+    <row r="137" spans="1:20" ht="34.200000000000003">
       <c r="A137">
         <v>55000150</v>
       </c>
@@ -15125,7 +15130,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="36">
+    <row r="138" spans="1:20" ht="34.200000000000003">
       <c r="A138">
         <v>55000151</v>
       </c>
@@ -15171,7 +15176,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="24">
+    <row r="139" spans="1:20" ht="22.8">
       <c r="A139">
         <v>55000152</v>
       </c>
@@ -15219,7 +15224,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="48">
+    <row r="140" spans="1:20" ht="45.6">
       <c r="A140">
         <v>55000153</v>
       </c>
@@ -15265,7 +15270,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="24">
+    <row r="141" spans="1:20" ht="22.8">
       <c r="A141">
         <v>55000154</v>
       </c>
@@ -15309,7 +15314,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="24">
+    <row r="142" spans="1:20" ht="22.8">
       <c r="A142">
         <v>55000155</v>
       </c>
@@ -15353,7 +15358,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="24">
+    <row r="143" spans="1:20" ht="22.8">
       <c r="A143">
         <v>55000156</v>
       </c>
@@ -15397,7 +15402,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="36">
+    <row r="144" spans="1:20" ht="34.200000000000003">
       <c r="A144">
         <v>55000157</v>
       </c>
@@ -15441,7 +15446,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="24">
+    <row r="145" spans="1:20" ht="22.8">
       <c r="A145">
         <v>55000158</v>
       </c>
@@ -15487,7 +15492,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="48">
+    <row r="146" spans="1:20" ht="45.6">
       <c r="A146">
         <v>55000159</v>
       </c>
@@ -15533,7 +15538,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="36">
+    <row r="147" spans="1:20" ht="34.200000000000003">
       <c r="A147">
         <v>55000160</v>
       </c>
@@ -15577,7 +15582,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="60">
+    <row r="148" spans="1:20" ht="57">
       <c r="A148">
         <v>55000161</v>
       </c>
@@ -15623,7 +15628,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="48">
+    <row r="149" spans="1:20" ht="45.6">
       <c r="A149">
         <v>55000162</v>
       </c>
@@ -15669,7 +15674,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="48">
+    <row r="150" spans="1:20" ht="45.6">
       <c r="A150">
         <v>55000163</v>
       </c>
@@ -15719,7 +15724,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="48">
+    <row r="151" spans="1:20" ht="45.6">
       <c r="A151">
         <v>55000164</v>
       </c>
@@ -15763,7 +15768,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="36">
+    <row r="152" spans="1:20" ht="34.200000000000003">
       <c r="A152">
         <v>55000165</v>
       </c>
@@ -15809,7 +15814,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="48">
+    <row r="153" spans="1:20" ht="45.6">
       <c r="A153">
         <v>55000166</v>
       </c>
@@ -15853,7 +15858,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="36">
+    <row r="154" spans="1:20" ht="34.200000000000003">
       <c r="A154">
         <v>55000167</v>
       </c>
@@ -15899,7 +15904,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="84">
+    <row r="155" spans="1:20" ht="79.8">
       <c r="A155">
         <v>55000168</v>
       </c>
@@ -15946,7 +15951,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="72">
+    <row r="156" spans="1:20" ht="68.400000000000006">
       <c r="A156">
         <v>55000169</v>
       </c>
@@ -15994,7 +15999,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="48">
+    <row r="157" spans="1:20" ht="45.6">
       <c r="A157">
         <v>55000170</v>
       </c>
@@ -16082,7 +16087,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="48">
+    <row r="159" spans="1:20" ht="45.6">
       <c r="A159">
         <v>55000172</v>
       </c>
@@ -16128,7 +16133,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="48">
+    <row r="160" spans="1:20" ht="45.6">
       <c r="A160">
         <v>55000173</v>
       </c>
@@ -16174,7 +16179,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="48">
+    <row r="161" spans="1:20" ht="45.6">
       <c r="A161">
         <v>55000174</v>
       </c>
@@ -16222,7 +16227,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="48">
+    <row r="162" spans="1:20" ht="45.6">
       <c r="A162">
         <v>55000175</v>
       </c>
@@ -16268,7 +16273,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="36">
+    <row r="163" spans="1:20" ht="34.200000000000003">
       <c r="A163">
         <v>55000176</v>
       </c>
@@ -16316,7 +16321,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="24">
+    <row r="164" spans="1:20" ht="22.8">
       <c r="A164">
         <v>55000177</v>
       </c>
@@ -16362,7 +16367,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="132">
+    <row r="165" spans="1:20" ht="125.4">
       <c r="A165">
         <v>55000178</v>
       </c>
@@ -16408,7 +16413,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="108">
+    <row r="166" spans="1:20" ht="102.6">
       <c r="A166">
         <v>55000179</v>
       </c>
@@ -16454,7 +16459,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="48">
+    <row r="167" spans="1:20" ht="45.6">
       <c r="A167">
         <v>55000180</v>
       </c>
@@ -16502,7 +16507,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="36">
+    <row r="168" spans="1:20" ht="34.200000000000003">
       <c r="A168">
         <v>55000181</v>
       </c>
@@ -16546,7 +16551,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="36">
+    <row r="169" spans="1:20" ht="34.200000000000003">
       <c r="A169">
         <v>55000182</v>
       </c>
@@ -16594,7 +16599,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="108">
+    <row r="170" spans="1:20" ht="79.8">
       <c r="A170">
         <v>55000183</v>
       </c>
@@ -16638,7 +16643,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="24">
+    <row r="171" spans="1:20" ht="22.8">
       <c r="A171">
         <v>55000184</v>
       </c>
@@ -16682,7 +16687,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="36">
+    <row r="172" spans="1:20" ht="34.200000000000003">
       <c r="A172">
         <v>55000185</v>
       </c>
@@ -16726,7 +16731,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="48">
+    <row r="173" spans="1:20" ht="45.6">
       <c r="A173">
         <v>55000186</v>
       </c>
@@ -16772,7 +16777,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="60">
+    <row r="174" spans="1:20" ht="57">
       <c r="A174">
         <v>55000187</v>
       </c>
@@ -16816,7 +16821,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="24">
+    <row r="175" spans="1:20" ht="22.8">
       <c r="A175">
         <v>55000188</v>
       </c>
@@ -16860,7 +16865,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="48">
+    <row r="176" spans="1:20" ht="45.6">
       <c r="A176">
         <v>55000189</v>
       </c>
@@ -16908,7 +16913,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="48">
+    <row r="177" spans="1:20" ht="45.6">
       <c r="A177">
         <v>55000190</v>
       </c>
@@ -16954,7 +16959,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="60">
+    <row r="178" spans="1:20" ht="57">
       <c r="A178">
         <v>55000191</v>
       </c>
@@ -17002,7 +17007,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="72">
+    <row r="179" spans="1:20" ht="68.400000000000006">
       <c r="A179">
         <v>55000192</v>
       </c>
@@ -17048,7 +17053,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="36">
+    <row r="180" spans="1:20" ht="34.200000000000003">
       <c r="A180">
         <v>55000193</v>
       </c>
@@ -17094,7 +17099,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="48">
+    <row r="181" spans="1:20" ht="45.6">
       <c r="A181">
         <v>55000194</v>
       </c>
@@ -17140,7 +17145,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="72">
+    <row r="182" spans="1:20" ht="68.400000000000006">
       <c r="A182">
         <v>55000195</v>
       </c>
@@ -17184,7 +17189,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="72">
+    <row r="183" spans="1:20" ht="68.400000000000006">
       <c r="A183">
         <v>55000196</v>
       </c>
@@ -17228,7 +17233,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="36">
+    <row r="184" spans="1:20" ht="34.200000000000003">
       <c r="A184">
         <v>55000197</v>
       </c>
@@ -17272,7 +17277,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="36">
+    <row r="185" spans="1:20" ht="34.200000000000003">
       <c r="A185">
         <v>55000198</v>
       </c>
@@ -17360,7 +17365,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="48">
+    <row r="187" spans="1:20" ht="45.6">
       <c r="A187">
         <v>55000200</v>
       </c>
@@ -17404,7 +17409,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="36">
+    <row r="188" spans="1:20" ht="34.200000000000003">
       <c r="A188">
         <v>55000201</v>
       </c>
@@ -17450,7 +17455,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="48">
+    <row r="189" spans="1:20" ht="45.6">
       <c r="A189">
         <v>55000202</v>
       </c>
@@ -17496,7 +17501,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="36">
+    <row r="190" spans="1:20" ht="34.200000000000003">
       <c r="A190">
         <v>55000203</v>
       </c>
@@ -17540,7 +17545,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="48">
+    <row r="191" spans="1:20" ht="45.6">
       <c r="A191">
         <v>55000204</v>
       </c>
@@ -17586,7 +17591,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="24">
+    <row r="192" spans="1:20" ht="22.8">
       <c r="A192">
         <v>55000205</v>
       </c>
@@ -17630,7 +17635,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="132">
+    <row r="193" spans="1:20" ht="125.4">
       <c r="A193">
         <v>55000206</v>
       </c>
@@ -17676,7 +17681,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="24">
+    <row r="194" spans="1:20" ht="22.8">
       <c r="A194">
         <v>55000207</v>
       </c>
@@ -17764,7 +17769,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="48">
+    <row r="196" spans="1:20" ht="45.6">
       <c r="A196">
         <v>55000209</v>
       </c>
@@ -17810,7 +17815,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="60">
+    <row r="197" spans="1:20" ht="57">
       <c r="A197">
         <v>55000210</v>
       </c>
@@ -17858,7 +17863,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="48">
+    <row r="198" spans="1:20" ht="45.6">
       <c r="A198">
         <v>55000211</v>
       </c>
@@ -17904,7 +17909,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="24">
+    <row r="199" spans="1:20" ht="22.8">
       <c r="A199">
         <v>55000212</v>
       </c>
@@ -17950,7 +17955,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="48">
+    <row r="200" spans="1:20" ht="45.6">
       <c r="A200">
         <v>55000213</v>
       </c>
@@ -17996,7 +18001,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="36">
+    <row r="201" spans="1:20" ht="34.200000000000003">
       <c r="A201">
         <v>55000214</v>
       </c>
@@ -18040,7 +18045,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="108">
+    <row r="202" spans="1:20" ht="102.6">
       <c r="A202">
         <v>55000215</v>
       </c>
@@ -18091,7 +18096,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="48">
+    <row r="203" spans="1:20" ht="45.6">
       <c r="A203">
         <v>55000216</v>
       </c>
@@ -18137,7 +18142,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="24">
+    <row r="204" spans="1:20" ht="22.8">
       <c r="A204">
         <v>55000217</v>
       </c>
@@ -18271,7 +18276,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="48">
+    <row r="207" spans="1:20" ht="45.6">
       <c r="A207">
         <v>55000220</v>
       </c>
@@ -18317,7 +18322,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="24">
+    <row r="208" spans="1:20" ht="22.8">
       <c r="A208">
         <v>55000221</v>
       </c>
@@ -18361,7 +18366,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="48">
+    <row r="209" spans="1:20" ht="45.6">
       <c r="A209">
         <v>55000222</v>
       </c>
@@ -18407,7 +18412,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="48">
+    <row r="210" spans="1:20" ht="45.6">
       <c r="A210">
         <v>55000223</v>
       </c>
@@ -18453,7 +18458,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="48">
+    <row r="211" spans="1:20" ht="45.6">
       <c r="A211">
         <v>55000224</v>
       </c>
@@ -18499,7 +18504,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="60">
+    <row r="212" spans="1:20" ht="57">
       <c r="A212">
         <v>55000225</v>
       </c>
@@ -18545,7 +18550,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="132">
+    <row r="213" spans="1:20" ht="125.4">
       <c r="A213">
         <v>55000226</v>
       </c>
@@ -18591,7 +18596,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="36">
+    <row r="214" spans="1:20" ht="34.200000000000003">
       <c r="A214">
         <v>55000227</v>
       </c>
@@ -18637,7 +18642,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="24">
+    <row r="215" spans="1:20" ht="22.8">
       <c r="A215">
         <v>55000228</v>
       </c>
@@ -18681,7 +18686,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="36">
+    <row r="216" spans="1:20" ht="34.200000000000003">
       <c r="A216">
         <v>55000229</v>
       </c>
@@ -18727,7 +18732,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="36">
+    <row r="217" spans="1:20" ht="34.200000000000003">
       <c r="A217">
         <v>55000230</v>
       </c>
@@ -18771,7 +18776,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="24">
+    <row r="218" spans="1:20" ht="22.8">
       <c r="A218">
         <v>55000231</v>
       </c>
@@ -18815,7 +18820,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="60">
+    <row r="219" spans="1:20" ht="57">
       <c r="A219">
         <v>55000232</v>
       </c>
@@ -18859,7 +18864,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="48">
+    <row r="220" spans="1:20" ht="45.6">
       <c r="A220">
         <v>55000233</v>
       </c>
@@ -18903,7 +18908,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="48">
+    <row r="221" spans="1:20" ht="45.6">
       <c r="A221">
         <v>55000234</v>
       </c>
@@ -18949,7 +18954,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="84">
+    <row r="222" spans="1:20" ht="79.8">
       <c r="A222">
         <v>55000235</v>
       </c>
@@ -18993,7 +18998,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="36">
+    <row r="223" spans="1:20" ht="34.200000000000003">
       <c r="A223">
         <v>55000236</v>
       </c>
@@ -19079,7 +19084,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="24">
+    <row r="225" spans="1:20" ht="22.8">
       <c r="A225">
         <v>55000238</v>
       </c>
@@ -19123,7 +19128,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="36">
+    <row r="226" spans="1:20" ht="34.200000000000003">
       <c r="A226">
         <v>55000239</v>
       </c>
@@ -19167,7 +19172,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="96">
+    <row r="227" spans="1:20" ht="91.2">
       <c r="A227">
         <v>55000240</v>
       </c>
@@ -19218,7 +19223,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="24">
+    <row r="228" spans="1:20" ht="22.8">
       <c r="A228">
         <v>55000241</v>
       </c>
@@ -19265,7 +19270,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="36">
+    <row r="229" spans="1:20" ht="34.200000000000003">
       <c r="A229">
         <v>55000242</v>
       </c>
@@ -19311,7 +19316,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="36">
+    <row r="230" spans="1:20" ht="34.200000000000003">
       <c r="A230">
         <v>55000243</v>
       </c>
@@ -19355,7 +19360,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="108">
+    <row r="231" spans="1:20" ht="102.6">
       <c r="A231">
         <v>55000244</v>
       </c>
@@ -19405,7 +19410,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="36">
+    <row r="232" spans="1:20" ht="34.200000000000003">
       <c r="A232">
         <v>55000245</v>
       </c>
@@ -19449,7 +19454,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="36">
+    <row r="233" spans="1:20" ht="34.200000000000003">
       <c r="A233">
         <v>55000246</v>
       </c>
@@ -19495,7 +19500,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="72">
+    <row r="234" spans="1:20" ht="68.400000000000006">
       <c r="A234">
         <v>55000247</v>
       </c>
@@ -19541,7 +19546,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="48">
+    <row r="235" spans="1:20" ht="45.6">
       <c r="A235">
         <v>55000248</v>
       </c>
@@ -19589,7 +19594,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="36">
+    <row r="236" spans="1:20" ht="34.200000000000003">
       <c r="A236">
         <v>55000249</v>
       </c>
@@ -19635,7 +19640,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="48">
+    <row r="237" spans="1:20" ht="45.6">
       <c r="A237">
         <v>55000250</v>
       </c>
@@ -19723,7 +19728,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="24">
+    <row r="239" spans="1:20" ht="22.8">
       <c r="A239">
         <v>55000252</v>
       </c>
@@ -19769,7 +19774,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="36">
+    <row r="240" spans="1:20" ht="34.200000000000003">
       <c r="A240">
         <v>55000253</v>
       </c>
@@ -19815,7 +19820,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="36">
+    <row r="241" spans="1:20" ht="34.200000000000003">
       <c r="A241">
         <v>55000254</v>
       </c>
@@ -19945,7 +19950,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="48">
+    <row r="244" spans="1:20" ht="45.6">
       <c r="A244">
         <v>55000257</v>
       </c>
@@ -19993,7 +19998,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="36">
+    <row r="245" spans="1:20" ht="34.200000000000003">
       <c r="A245">
         <v>55000258</v>
       </c>
@@ -20037,7 +20042,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="48">
+    <row r="246" spans="1:20" ht="45.6">
       <c r="A246">
         <v>55000259</v>
       </c>
@@ -20085,7 +20090,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="96">
+    <row r="247" spans="1:20" ht="91.2">
       <c r="A247">
         <v>55000260</v>
       </c>
@@ -20131,7 +20136,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="96">
+    <row r="248" spans="1:20" ht="91.2">
       <c r="A248">
         <v>55000261</v>
       </c>
@@ -20175,7 +20180,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="36">
+    <row r="249" spans="1:20" ht="34.200000000000003">
       <c r="A249">
         <v>55000262</v>
       </c>
@@ -20219,7 +20224,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="24">
+    <row r="250" spans="1:20" ht="22.8">
       <c r="A250">
         <v>55000263</v>
       </c>
@@ -20267,7 +20272,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="48">
+    <row r="251" spans="1:20" ht="45.6">
       <c r="A251">
         <v>55000264</v>
       </c>
@@ -20313,7 +20318,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="48">
+    <row r="252" spans="1:20" ht="45.6">
       <c r="A252">
         <v>55000265</v>
       </c>
@@ -20357,7 +20362,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="48">
+    <row r="253" spans="1:20" ht="45.6">
       <c r="A253">
         <v>55000266</v>
       </c>
@@ -20401,7 +20406,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="24">
+    <row r="254" spans="1:20" ht="22.8">
       <c r="A254">
         <v>55000267</v>
       </c>
@@ -20447,7 +20452,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="24">
+    <row r="255" spans="1:20" ht="22.8">
       <c r="A255">
         <v>55000268</v>
       </c>
@@ -20491,7 +20496,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="48">
+    <row r="256" spans="1:20" ht="45.6">
       <c r="A256">
         <v>55000269</v>
       </c>
@@ -20535,7 +20540,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="48">
+    <row r="257" spans="1:20" ht="45.6">
       <c r="A257">
         <v>55000270</v>
       </c>
@@ -20581,7 +20586,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="36">
+    <row r="258" spans="1:20" ht="34.200000000000003">
       <c r="A258">
         <v>55000271</v>
       </c>
@@ -20627,7 +20632,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="36">
+    <row r="259" spans="1:20" ht="34.200000000000003">
       <c r="A259">
         <v>55000272</v>
       </c>
@@ -20671,7 +20676,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="48">
+    <row r="260" spans="1:20" ht="45.6">
       <c r="A260">
         <v>55000273</v>
       </c>
@@ -20715,7 +20720,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="96">
+    <row r="261" spans="1:20" ht="91.2">
       <c r="A261">
         <v>55000274</v>
       </c>
@@ -20759,7 +20764,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="48">
+    <row r="262" spans="1:20" ht="45.6">
       <c r="A262">
         <v>55000275</v>
       </c>
@@ -20805,7 +20810,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="48">
+    <row r="263" spans="1:20" ht="45.6">
       <c r="A263">
         <v>55000276</v>
       </c>
@@ -20851,7 +20856,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="24">
+    <row r="264" spans="1:20" ht="22.8">
       <c r="A264">
         <v>55000277</v>
       </c>
@@ -20895,7 +20900,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="24">
+    <row r="265" spans="1:20" ht="22.8">
       <c r="A265">
         <v>55000278</v>
       </c>
@@ -20939,7 +20944,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="24">
+    <row r="266" spans="1:20" ht="22.8">
       <c r="A266">
         <v>55000279</v>
       </c>
@@ -20983,7 +20988,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="48">
+    <row r="267" spans="1:20" ht="45.6">
       <c r="A267">
         <v>55000280</v>
       </c>
@@ -21027,7 +21032,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="24">
+    <row r="268" spans="1:20" ht="22.8">
       <c r="A268">
         <v>55000281</v>
       </c>
@@ -21071,7 +21076,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="180">
+    <row r="269" spans="1:20" ht="171">
       <c r="A269">
         <v>55000282</v>
       </c>
@@ -21117,7 +21122,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="48">
+    <row r="270" spans="1:20" ht="45.6">
       <c r="A270">
         <v>55000284</v>
       </c>
@@ -21165,7 +21170,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="48">
+    <row r="271" spans="1:20" ht="45.6">
       <c r="A271">
         <v>55000285</v>
       </c>
@@ -21253,7 +21258,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="36">
+    <row r="273" spans="1:20" ht="34.200000000000003">
       <c r="A273">
         <v>55000287</v>
       </c>
@@ -21299,7 +21304,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="24">
+    <row r="274" spans="1:20" ht="22.8">
       <c r="A274">
         <v>55000288</v>
       </c>
@@ -21345,7 +21350,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="144">
+    <row r="275" spans="1:20" ht="136.80000000000001">
       <c r="A275">
         <v>55000289</v>
       </c>
@@ -21389,7 +21394,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="96">
+    <row r="276" spans="1:20" ht="91.2">
       <c r="A276">
         <v>55000290</v>
       </c>
@@ -21433,7 +21438,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="84">
+    <row r="277" spans="1:20" ht="79.8">
       <c r="A277">
         <v>55000291</v>
       </c>
@@ -21477,7 +21482,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="48">
+    <row r="278" spans="1:20" ht="45.6">
       <c r="A278">
         <v>55000292</v>
       </c>
@@ -21525,7 +21530,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="60">
+    <row r="279" spans="1:20" ht="57">
       <c r="A279">
         <v>55000293</v>
       </c>
@@ -21569,7 +21574,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="108">
+    <row r="280" spans="1:20" ht="102.6">
       <c r="A280">
         <v>55000294</v>
       </c>
@@ -21662,7 +21667,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="24">
+    <row r="282" spans="1:20" ht="22.8">
       <c r="A282">
         <v>55000296</v>
       </c>
@@ -21706,7 +21711,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="120">
+    <row r="283" spans="1:20" ht="114">
       <c r="A283">
         <v>55000297</v>
       </c>
@@ -21752,7 +21757,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="108">
+    <row r="284" spans="1:20" ht="102.6">
       <c r="A284">
         <v>55000298</v>
       </c>
@@ -21798,7 +21803,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="36">
+    <row r="285" spans="1:20" ht="34.200000000000003">
       <c r="A285">
         <v>55000299</v>
       </c>
@@ -21846,7 +21851,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="24">
+    <row r="286" spans="1:20" ht="22.8">
       <c r="A286">
         <v>55000300</v>
       </c>
@@ -21863,7 +21868,7 @@
       <c r="H286" s="17"/>
       <c r="I286" s="17"/>
       <c r="J286" s="21" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="K286" s="60">
         <v>2</v>
@@ -21887,14 +21892,14 @@
       <c r="R286" s="1">
         <v>2500</v>
       </c>
-      <c r="S286" s="45" t="s">
-        <v>953</v>
+      <c r="S286" s="31" t="s">
+        <v>1450</v>
       </c>
       <c r="T286" s="53" t="s">
         <v>1429</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="108">
+    <row r="287" spans="1:20" ht="102.6">
       <c r="A287">
         <v>55000324</v>
       </c>
@@ -21945,7 +21950,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="108">
+    <row r="288" spans="1:20" ht="102.6">
       <c r="A288">
         <v>55000325</v>
       </c>
@@ -21995,7 +22000,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="96">
+    <row r="289" spans="1:20" ht="91.2">
       <c r="A289">
         <v>55000326</v>
       </c>
@@ -22045,7 +22050,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="108">
+    <row r="290" spans="1:20" ht="102.6">
       <c r="A290">
         <v>55000327</v>
       </c>
@@ -22095,7 +22100,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="108">
+    <row r="291" spans="1:20" ht="102.6">
       <c r="A291">
         <v>55000328</v>
       </c>
@@ -22146,7 +22151,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="108">
+    <row r="292" spans="1:20" ht="102.6">
       <c r="A292">
         <v>55000329</v>
       </c>
@@ -22197,7 +22202,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="108">
+    <row r="293" spans="1:20" ht="102.6">
       <c r="A293">
         <v>55000330</v>
       </c>
@@ -22248,7 +22253,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="108">
+    <row r="294" spans="1:20" ht="102.6">
       <c r="A294">
         <v>55000331</v>
       </c>
@@ -22299,7 +22304,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="96">
+    <row r="295" spans="1:20" ht="91.2">
       <c r="A295">
         <v>55000332</v>
       </c>
@@ -22343,7 +22348,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="228">
+    <row r="296" spans="1:20" ht="216.6">
       <c r="A296">
         <v>55000333</v>
       </c>
@@ -22387,7 +22392,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="108">
+    <row r="297" spans="1:20" ht="102.6">
       <c r="A297">
         <v>55000334</v>
       </c>
@@ -22438,7 +22443,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="108">
+    <row r="298" spans="1:20" ht="91.2">
       <c r="A298">
         <v>55000335</v>
       </c>
@@ -22455,7 +22460,7 @@
       <c r="H298" s="17"/>
       <c r="I298" s="17"/>
       <c r="J298" s="21" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="K298" s="60"/>
       <c r="L298" s="1" t="s">
@@ -22482,7 +22487,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="48">
+    <row r="299" spans="1:20" ht="45.6">
       <c r="A299">
         <v>55000340</v>
       </c>
@@ -22530,7 +22535,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="36">
+    <row r="300" spans="1:20" ht="34.200000000000003">
       <c r="A300">
         <v>55000341</v>
       </c>
@@ -22576,7 +22581,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="180">
+    <row r="301" spans="1:20" ht="171">
       <c r="A301">
         <v>55000342</v>
       </c>
@@ -22620,7 +22625,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="180">
+    <row r="302" spans="1:20" ht="171">
       <c r="A302">
         <v>55000343</v>
       </c>
@@ -22664,7 +22669,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="36">
+    <row r="303" spans="1:20" ht="34.200000000000003">
       <c r="A303" t="s">
         <v>1369</v>
       </c>
@@ -22932,7 +22937,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="96">
+    <row r="4" spans="1:20" ht="91.2">
       <c r="A4">
         <v>55010003</v>
       </c>
@@ -22976,7 +22981,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="96">
+    <row r="5" spans="1:20" ht="91.2">
       <c r="A5">
         <v>55010004</v>
       </c>
@@ -23244,7 +23249,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="48">
+    <row r="4" spans="1:20" ht="45.6">
       <c r="A4">
         <v>55020001</v>
       </c>
@@ -23290,7 +23295,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="48">
+    <row r="5" spans="1:20" ht="45.6">
       <c r="A5">
         <v>55020002</v>
       </c>
@@ -23336,7 +23341,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="48">
+    <row r="6" spans="1:20" ht="45.6">
       <c r="A6">
         <v>55020003</v>
       </c>
@@ -23382,7 +23387,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="48">
+    <row r="7" spans="1:20" ht="45.6">
       <c r="A7">
         <v>55020004</v>
       </c>
@@ -23428,7 +23433,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="48">
+    <row r="8" spans="1:20" ht="45.6">
       <c r="A8">
         <v>55020005</v>
       </c>
@@ -23474,7 +23479,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="48">
+    <row r="9" spans="1:20" ht="45.6">
       <c r="A9">
         <v>55020006</v>
       </c>
@@ -23520,7 +23525,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="48">
+    <row r="10" spans="1:20" ht="45.6">
       <c r="A10">
         <v>55020007</v>
       </c>
@@ -23566,7 +23571,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="48">
+    <row r="11" spans="1:20" ht="45.6">
       <c r="A11">
         <v>55020008</v>
       </c>
@@ -23612,7 +23617,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="48">
+    <row r="12" spans="1:20" ht="45.6">
       <c r="A12">
         <v>55020009</v>
       </c>
@@ -23658,7 +23663,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="48">
+    <row r="13" spans="1:20" ht="45.6">
       <c r="A13">
         <v>55020010</v>
       </c>
@@ -23704,7 +23709,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="48">
+    <row r="14" spans="1:20" ht="45.6">
       <c r="A14">
         <v>55020011</v>
       </c>
@@ -23750,7 +23755,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="48">
+    <row r="15" spans="1:20" ht="45.6">
       <c r="A15">
         <v>55020012</v>
       </c>
@@ -23796,7 +23801,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="48">
+    <row r="16" spans="1:20" ht="45.6">
       <c r="A16">
         <v>55020013</v>
       </c>
@@ -23842,7 +23847,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="48">
+    <row r="17" spans="1:20" ht="45.6">
       <c r="A17">
         <v>55020014</v>
       </c>
@@ -23888,7 +23893,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="48">
+    <row r="18" spans="1:20" ht="45.6">
       <c r="A18">
         <v>55020015</v>
       </c>
@@ -23934,7 +23939,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="48">
+    <row r="19" spans="1:20" ht="45.6">
       <c r="A19">
         <v>55020016</v>
       </c>
@@ -24609,5 +24614,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix the bug of aoe effect offset
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -8846,7 +8846,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C283" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S286" sqref="S286"/>
+      <selection pane="bottomRight" activeCell="R286" sqref="R286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -21890,7 +21890,7 @@
       </c>
       <c r="Q286" s="1"/>
       <c r="R286" s="1">
-        <v>2500</v>
+        <v>6000</v>
       </c>
       <c r="S286" s="31" t="s">
         <v>1450</v>

</xml_diff>

<commit_message>
fix the monster config error
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="1" r:id="rId1"/>
@@ -8843,30 +8843,30 @@
   <dimension ref="A1:T303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C283" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C297" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R286" sqref="R286"/>
+      <selection pane="bottomRight" activeCell="D297" sqref="D297"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" customWidth="1"/>
-    <col min="6" max="8" width="8.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.75" customWidth="1"/>
+    <col min="6" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="17.375" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" customWidth="1"/>
-    <col min="14" max="14" width="23.44140625" customWidth="1"/>
+    <col min="11" max="11" width="8.125" customWidth="1"/>
+    <col min="12" max="12" width="7.375" customWidth="1"/>
+    <col min="13" max="13" width="6.375" customWidth="1"/>
+    <col min="14" max="14" width="23.5" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="17" width="7.6640625" customWidth="1"/>
-    <col min="18" max="18" width="7.109375" customWidth="1"/>
-    <col min="21" max="21" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="7.625" customWidth="1"/>
+    <col min="18" max="18" width="7.125" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -9055,7 +9055,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="45.6">
+    <row r="4" spans="1:20" ht="36">
       <c r="A4">
         <v>55000001</v>
       </c>
@@ -9101,7 +9101,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="57">
+    <row r="5" spans="1:20" ht="48">
       <c r="A5">
         <v>55000002</v>
       </c>
@@ -9145,7 +9145,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="22.8">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>55000003</v>
       </c>
@@ -9189,7 +9189,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="45.6">
+    <row r="7" spans="1:20" ht="36">
       <c r="A7">
         <v>55000004</v>
       </c>
@@ -9235,7 +9235,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="45.6">
+    <row r="8" spans="1:20" ht="36">
       <c r="A8">
         <v>55000005</v>
       </c>
@@ -9281,7 +9281,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="45.6">
+    <row r="9" spans="1:20" ht="36">
       <c r="A9">
         <v>55000006</v>
       </c>
@@ -9327,7 +9327,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="45.6">
+    <row r="10" spans="1:20" ht="36">
       <c r="A10">
         <v>55000007</v>
       </c>
@@ -9373,7 +9373,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="45.6">
+    <row r="11" spans="1:20" ht="36">
       <c r="A11">
         <v>55000008</v>
       </c>
@@ -9419,7 +9419,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="45.6">
+    <row r="12" spans="1:20" ht="36">
       <c r="A12">
         <v>55000009</v>
       </c>
@@ -9465,7 +9465,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="45.6">
+    <row r="13" spans="1:20" ht="36">
       <c r="A13">
         <v>55000010</v>
       </c>
@@ -9511,7 +9511,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="45.6">
+    <row r="14" spans="1:20" ht="36">
       <c r="A14">
         <v>55000011</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="45.6">
+    <row r="15" spans="1:20" ht="36">
       <c r="A15">
         <v>55000012</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="45.6">
+    <row r="16" spans="1:20" ht="36">
       <c r="A16">
         <v>55000013</v>
       </c>
@@ -9649,7 +9649,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="45.6">
+    <row r="17" spans="1:20" ht="36">
       <c r="A17">
         <v>55000014</v>
       </c>
@@ -9695,7 +9695,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="45.6">
+    <row r="18" spans="1:20" ht="36">
       <c r="A18">
         <v>55000015</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="45.6">
+    <row r="19" spans="1:20" ht="36">
       <c r="A19">
         <v>55000016</v>
       </c>
@@ -9787,7 +9787,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="45.6">
+    <row r="20" spans="1:20" ht="36">
       <c r="A20">
         <v>55000017</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="45.6">
+    <row r="21" spans="1:20" ht="36">
       <c r="A21">
         <v>55000018</v>
       </c>
@@ -9879,7 +9879,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="45.6">
+    <row r="22" spans="1:20" ht="36">
       <c r="A22">
         <v>55000019</v>
       </c>
@@ -9925,7 +9925,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="45.6">
+    <row r="23" spans="1:20" ht="48">
       <c r="A23">
         <v>55000020</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="28.8">
+    <row r="24" spans="1:20" ht="27">
       <c r="A24">
         <v>55000021</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="34.200000000000003">
+    <row r="25" spans="1:20" ht="24">
       <c r="A25">
         <v>55000029</v>
       </c>
@@ -10057,7 +10057,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="45.6">
+    <row r="26" spans="1:20" ht="36">
       <c r="A26">
         <v>55000030</v>
       </c>
@@ -10103,7 +10103,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="34.200000000000003">
+    <row r="27" spans="1:20" ht="24">
       <c r="A27">
         <v>55000031</v>
       </c>
@@ -10149,7 +10149,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="34.200000000000003">
+    <row r="28" spans="1:20" ht="24">
       <c r="A28">
         <v>55000032</v>
       </c>
@@ -10239,7 +10239,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="57">
+    <row r="30" spans="1:20" ht="48">
       <c r="A30">
         <v>55000034</v>
       </c>
@@ -10283,7 +10283,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="34.200000000000003">
+    <row r="31" spans="1:20" ht="24">
       <c r="A31">
         <v>55000035</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="45.6">
+    <row r="32" spans="1:20" ht="36">
       <c r="A32">
         <v>55000036</v>
       </c>
@@ -10373,7 +10373,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="45.6">
+    <row r="33" spans="1:20" ht="48">
       <c r="A33">
         <v>55000037</v>
       </c>
@@ -10417,7 +10417,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="45.6">
+    <row r="34" spans="1:20" ht="36">
       <c r="A34">
         <v>55000038</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="45.6">
+    <row r="35" spans="1:20" ht="36">
       <c r="A35">
         <v>55000039</v>
       </c>
@@ -10505,7 +10505,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="45.6">
+    <row r="36" spans="1:20" ht="36">
       <c r="A36">
         <v>55000040</v>
       </c>
@@ -10549,7 +10549,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="45.6">
+    <row r="37" spans="1:20" ht="36">
       <c r="A37">
         <v>55000041</v>
       </c>
@@ -10597,7 +10597,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="45.6">
+    <row r="38" spans="1:20" ht="48">
       <c r="A38">
         <v>55000042</v>
       </c>
@@ -10643,7 +10643,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="22.8">
+    <row r="39" spans="1:20" ht="24">
       <c r="A39">
         <v>55000043</v>
       </c>
@@ -10687,7 +10687,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="34.200000000000003">
+    <row r="40" spans="1:20" ht="24">
       <c r="A40">
         <v>55000044</v>
       </c>
@@ -10731,7 +10731,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="34.200000000000003">
+    <row r="41" spans="1:20" ht="36">
       <c r="A41">
         <v>55000045</v>
       </c>
@@ -10775,7 +10775,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="34.200000000000003">
+    <row r="42" spans="1:20" ht="36">
       <c r="A42">
         <v>55000046</v>
       </c>
@@ -10819,7 +10819,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="45.6">
+    <row r="43" spans="1:20" ht="36">
       <c r="A43">
         <v>55000047</v>
       </c>
@@ -10865,7 +10865,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="34.200000000000003">
+    <row r="44" spans="1:20" ht="36">
       <c r="A44">
         <v>55000048</v>
       </c>
@@ -10911,7 +10911,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="45.6">
+    <row r="45" spans="1:20" ht="48">
       <c r="A45">
         <v>55000049</v>
       </c>
@@ -10955,7 +10955,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="45.6">
+    <row r="46" spans="1:20" ht="48">
       <c r="A46">
         <v>55000050</v>
       </c>
@@ -11045,7 +11045,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="45.6">
+    <row r="48" spans="1:20" ht="36">
       <c r="A48">
         <v>55000061</v>
       </c>
@@ -11091,7 +11091,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="34.200000000000003">
+    <row r="49" spans="1:20" ht="24">
       <c r="A49">
         <v>55000062</v>
       </c>
@@ -11135,7 +11135,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="45.6">
+    <row r="50" spans="1:20" ht="36">
       <c r="A50">
         <v>55000063</v>
       </c>
@@ -11181,7 +11181,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="79.8">
+    <row r="51" spans="1:20" ht="72">
       <c r="A51">
         <v>55000064</v>
       </c>
@@ -11229,7 +11229,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="45.6">
+    <row r="52" spans="1:20" ht="48">
       <c r="A52">
         <v>55000065</v>
       </c>
@@ -11275,7 +11275,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="45.6">
+    <row r="53" spans="1:20" ht="48">
       <c r="A53">
         <v>55000066</v>
       </c>
@@ -11321,7 +11321,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="45.6">
+    <row r="54" spans="1:20" ht="48">
       <c r="A54">
         <v>55000067</v>
       </c>
@@ -11367,7 +11367,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="45.6">
+    <row r="55" spans="1:20" ht="48">
       <c r="A55">
         <v>55000068</v>
       </c>
@@ -11413,7 +11413,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="45.6">
+    <row r="56" spans="1:20" ht="48">
       <c r="A56">
         <v>55000069</v>
       </c>
@@ -11459,7 +11459,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="45.6">
+    <row r="57" spans="1:20" ht="48">
       <c r="A57">
         <v>55000070</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="45.6">
+    <row r="58" spans="1:20" ht="48">
       <c r="A58">
         <v>55000071</v>
       </c>
@@ -11551,7 +11551,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="45.6">
+    <row r="59" spans="1:20" ht="48">
       <c r="A59">
         <v>55000072</v>
       </c>
@@ -11597,7 +11597,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="45.6">
+    <row r="60" spans="1:20" ht="36">
       <c r="A60">
         <v>55000073</v>
       </c>
@@ -11643,7 +11643,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="22.8">
+    <row r="61" spans="1:20" ht="24">
       <c r="A61">
         <v>55000074</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="136.80000000000001">
+    <row r="62" spans="1:20" ht="120">
       <c r="A62">
         <v>55000075</v>
       </c>
@@ -11735,7 +11735,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="34.200000000000003">
+    <row r="63" spans="1:20" ht="24">
       <c r="A63">
         <v>55000076</v>
       </c>
@@ -11779,7 +11779,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="45.6">
+    <row r="64" spans="1:20" ht="36">
       <c r="A64">
         <v>55000077</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="22.8">
+    <row r="65" spans="1:20" ht="24">
       <c r="A65">
         <v>55000078</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="22.8">
+    <row r="66" spans="1:20" ht="24">
       <c r="A66">
         <v>55000079</v>
       </c>
@@ -11915,7 +11915,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="22.8">
+    <row r="67" spans="1:20" ht="24">
       <c r="A67">
         <v>55000080</v>
       </c>
@@ -11961,7 +11961,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="22.8">
+    <row r="68" spans="1:20" ht="24">
       <c r="A68">
         <v>55000081</v>
       </c>
@@ -12005,7 +12005,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="34.200000000000003">
+    <row r="69" spans="1:20" ht="24">
       <c r="A69">
         <v>55000082</v>
       </c>
@@ -12051,7 +12051,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="57">
+    <row r="70" spans="1:20" ht="48">
       <c r="A70">
         <v>55000083</v>
       </c>
@@ -12099,7 +12099,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="22.8">
+    <row r="71" spans="1:20" ht="24">
       <c r="A71">
         <v>55000084</v>
       </c>
@@ -12147,7 +12147,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="45.6">
+    <row r="72" spans="1:20" ht="36">
       <c r="A72">
         <v>55000085</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="45.6">
+    <row r="73" spans="1:20" ht="36">
       <c r="A73">
         <v>55000086</v>
       </c>
@@ -12239,7 +12239,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="34.200000000000003">
+    <row r="74" spans="1:20" ht="24">
       <c r="A74">
         <v>55000087</v>
       </c>
@@ -12283,7 +12283,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="34.200000000000003">
+    <row r="75" spans="1:20" ht="24">
       <c r="A75">
         <v>55000088</v>
       </c>
@@ -12327,7 +12327,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="22.8">
+    <row r="76" spans="1:20" ht="24">
       <c r="A76">
         <v>55000089</v>
       </c>
@@ -12371,7 +12371,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="45.6">
+    <row r="77" spans="1:20" ht="48">
       <c r="A77">
         <v>55000090</v>
       </c>
@@ -12415,7 +12415,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="22.8">
+    <row r="78" spans="1:20" ht="24">
       <c r="A78">
         <v>55000091</v>
       </c>
@@ -12459,7 +12459,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="45.6">
+    <row r="79" spans="1:20" ht="36">
       <c r="A79">
         <v>55000092</v>
       </c>
@@ -12507,7 +12507,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="34.200000000000003">
+    <row r="80" spans="1:20" ht="24">
       <c r="A80">
         <v>55000093</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="34.200000000000003">
+    <row r="81" spans="1:20" ht="24">
       <c r="A81">
         <v>55000094</v>
       </c>
@@ -12595,7 +12595,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="34.200000000000003">
+    <row r="82" spans="1:20" ht="24">
       <c r="A82">
         <v>55000095</v>
       </c>
@@ -12639,7 +12639,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="102.6">
+    <row r="83" spans="1:20" ht="84">
       <c r="A83">
         <v>55000096</v>
       </c>
@@ -12683,7 +12683,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="57">
+    <row r="84" spans="1:20" ht="48">
       <c r="A84">
         <v>55000097</v>
       </c>
@@ -12729,7 +12729,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="102.6">
+    <row r="85" spans="1:20" ht="84">
       <c r="A85">
         <v>55000098</v>
       </c>
@@ -12780,7 +12780,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="34.200000000000003">
+    <row r="86" spans="1:20" ht="36">
       <c r="A86">
         <v>55000099</v>
       </c>
@@ -12824,7 +12824,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="34.200000000000003">
+    <row r="87" spans="1:20" ht="36">
       <c r="A87">
         <v>55000100</v>
       </c>
@@ -12872,7 +12872,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="22.8">
+    <row r="88" spans="1:20">
       <c r="A88">
         <v>55000101</v>
       </c>
@@ -12916,7 +12916,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="22.8">
+    <row r="89" spans="1:20">
       <c r="A89">
         <v>55000102</v>
       </c>
@@ -13002,7 +13002,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="45.6">
+    <row r="91" spans="1:20" ht="36">
       <c r="A91">
         <v>55000104</v>
       </c>
@@ -13048,7 +13048,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="102.6">
+    <row r="92" spans="1:20" ht="96">
       <c r="A92">
         <v>55000105</v>
       </c>
@@ -13099,7 +13099,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="68.400000000000006">
+    <row r="93" spans="1:20" ht="48">
       <c r="A93">
         <v>55000106</v>
       </c>
@@ -13145,7 +13145,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="45.6">
+    <row r="94" spans="1:20" ht="36">
       <c r="A94">
         <v>55000107</v>
       </c>
@@ -13191,7 +13191,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="57">
+    <row r="95" spans="1:20" ht="48">
       <c r="A95">
         <v>55000108</v>
       </c>
@@ -13237,7 +13237,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="34.200000000000003">
+    <row r="96" spans="1:20" ht="36">
       <c r="A96">
         <v>55000109</v>
       </c>
@@ -13281,7 +13281,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="34.200000000000003">
+    <row r="97" spans="1:20" ht="24">
       <c r="A97">
         <v>55000110</v>
       </c>
@@ -13325,7 +13325,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="34.200000000000003">
+    <row r="98" spans="1:20" ht="36">
       <c r="A98">
         <v>55000111</v>
       </c>
@@ -13373,7 +13373,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="22.8">
+    <row r="99" spans="1:20" ht="24">
       <c r="A99">
         <v>55000112</v>
       </c>
@@ -13419,7 +13419,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="45.6">
+    <row r="100" spans="1:20" ht="48">
       <c r="A100">
         <v>55000113</v>
       </c>
@@ -13465,7 +13465,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="34.200000000000003">
+    <row r="101" spans="1:20" ht="24">
       <c r="A101">
         <v>55000114</v>
       </c>
@@ -13509,7 +13509,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="45.6">
+    <row r="102" spans="1:20" ht="36">
       <c r="A102">
         <v>55000115</v>
       </c>
@@ -13557,7 +13557,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="22.8">
+    <row r="103" spans="1:20" ht="24">
       <c r="A103">
         <v>55000116</v>
       </c>
@@ -13601,7 +13601,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="68.400000000000006">
+    <row r="104" spans="1:20" ht="60">
       <c r="A104">
         <v>55000117</v>
       </c>
@@ -13647,7 +13647,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="45.6">
+    <row r="105" spans="1:20" ht="48">
       <c r="A105">
         <v>55000118</v>
       </c>
@@ -13693,7 +13693,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="45.6">
+    <row r="106" spans="1:20" ht="48">
       <c r="A106">
         <v>55000119</v>
       </c>
@@ -13739,7 +13739,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="34.200000000000003">
+    <row r="107" spans="1:20" ht="24">
       <c r="A107">
         <v>55000120</v>
       </c>
@@ -13783,7 +13783,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="34.200000000000003">
+    <row r="108" spans="1:20" ht="24">
       <c r="A108">
         <v>55000121</v>
       </c>
@@ -13831,7 +13831,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="45.6">
+    <row r="109" spans="1:20" ht="36">
       <c r="A109">
         <v>55000122</v>
       </c>
@@ -13877,7 +13877,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="45.6">
+    <row r="110" spans="1:20" ht="36">
       <c r="A110">
         <v>55000123</v>
       </c>
@@ -13923,7 +13923,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="45.6">
+    <row r="111" spans="1:20" ht="48">
       <c r="A111">
         <v>55000124</v>
       </c>
@@ -13969,7 +13969,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="34.200000000000003">
+    <row r="112" spans="1:20" ht="36">
       <c r="A112">
         <v>55000125</v>
       </c>
@@ -14013,7 +14013,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="57">
+    <row r="113" spans="1:20" ht="48">
       <c r="A113">
         <v>55000126</v>
       </c>
@@ -14141,7 +14141,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="22.8">
+    <row r="116" spans="1:20" ht="24">
       <c r="A116">
         <v>55000129</v>
       </c>
@@ -14185,7 +14185,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="22.8">
+    <row r="117" spans="1:20" ht="24">
       <c r="A117">
         <v>55000130</v>
       </c>
@@ -14229,7 +14229,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="34.200000000000003">
+    <row r="118" spans="1:20" ht="24">
       <c r="A118">
         <v>55000131</v>
       </c>
@@ -14273,7 +14273,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="34.200000000000003">
+    <row r="119" spans="1:20" ht="36">
       <c r="A119">
         <v>55000132</v>
       </c>
@@ -14317,7 +14317,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="136.80000000000001">
+    <row r="120" spans="1:20" ht="120">
       <c r="A120">
         <v>55000133</v>
       </c>
@@ -14361,7 +14361,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="57">
+    <row r="121" spans="1:20" ht="60">
       <c r="A121">
         <v>55000134</v>
       </c>
@@ -14407,7 +14407,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="45.6">
+    <row r="122" spans="1:20" ht="36">
       <c r="A122">
         <v>55000135</v>
       </c>
@@ -14451,7 +14451,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="34.200000000000003">
+    <row r="123" spans="1:20" ht="24">
       <c r="A123">
         <v>55000136</v>
       </c>
@@ -14495,7 +14495,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="45.6">
+    <row r="124" spans="1:20" ht="48">
       <c r="A124">
         <v>55000137</v>
       </c>
@@ -14541,7 +14541,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="34.200000000000003">
+    <row r="125" spans="1:20" ht="36">
       <c r="A125">
         <v>55000138</v>
       </c>
@@ -14585,7 +14585,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="45.6">
+    <row r="126" spans="1:20" ht="48">
       <c r="A126">
         <v>55000139</v>
       </c>
@@ -14631,7 +14631,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="57">
+    <row r="127" spans="1:20" ht="48">
       <c r="A127">
         <v>55000140</v>
       </c>
@@ -14677,7 +14677,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="45.6">
+    <row r="128" spans="1:20" ht="48">
       <c r="A128">
         <v>55000141</v>
       </c>
@@ -14723,7 +14723,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="34.200000000000003">
+    <row r="129" spans="1:20" ht="36">
       <c r="A129">
         <v>55000142</v>
       </c>
@@ -14767,7 +14767,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="22.8">
+    <row r="130" spans="1:20" ht="24">
       <c r="A130">
         <v>55000143</v>
       </c>
@@ -14816,7 +14816,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="45.6">
+    <row r="131" spans="1:20" ht="48">
       <c r="A131">
         <v>55000144</v>
       </c>
@@ -14862,7 +14862,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="34.200000000000003">
+    <row r="132" spans="1:20" ht="24">
       <c r="A132">
         <v>55000145</v>
       </c>
@@ -14906,7 +14906,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="45.6">
+    <row r="133" spans="1:20" ht="48">
       <c r="A133">
         <v>55000146</v>
       </c>
@@ -14952,7 +14952,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="34.200000000000003">
+    <row r="134" spans="1:20" ht="36">
       <c r="A134">
         <v>55000147</v>
       </c>
@@ -14996,7 +14996,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="45.6">
+    <row r="135" spans="1:20" ht="48">
       <c r="A135">
         <v>55000148</v>
       </c>
@@ -15042,7 +15042,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="34.200000000000003">
+    <row r="136" spans="1:20" ht="36">
       <c r="A136">
         <v>55000149</v>
       </c>
@@ -15086,7 +15086,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="34.200000000000003">
+    <row r="137" spans="1:20" ht="24">
       <c r="A137">
         <v>55000150</v>
       </c>
@@ -15130,7 +15130,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="34.200000000000003">
+    <row r="138" spans="1:20" ht="36">
       <c r="A138">
         <v>55000151</v>
       </c>
@@ -15176,7 +15176,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="22.8">
+    <row r="139" spans="1:20" ht="24">
       <c r="A139">
         <v>55000152</v>
       </c>
@@ -15224,7 +15224,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="45.6">
+    <row r="140" spans="1:20" ht="48">
       <c r="A140">
         <v>55000153</v>
       </c>
@@ -15270,7 +15270,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="22.8">
+    <row r="141" spans="1:20" ht="24">
       <c r="A141">
         <v>55000154</v>
       </c>
@@ -15314,7 +15314,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="22.8">
+    <row r="142" spans="1:20" ht="24">
       <c r="A142">
         <v>55000155</v>
       </c>
@@ -15358,7 +15358,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="22.8">
+    <row r="143" spans="1:20" ht="24">
       <c r="A143">
         <v>55000156</v>
       </c>
@@ -15402,7 +15402,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="34.200000000000003">
+    <row r="144" spans="1:20" ht="36">
       <c r="A144">
         <v>55000157</v>
       </c>
@@ -15446,7 +15446,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="22.8">
+    <row r="145" spans="1:20" ht="24">
       <c r="A145">
         <v>55000158</v>
       </c>
@@ -15492,7 +15492,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="45.6">
+    <row r="146" spans="1:20" ht="36">
       <c r="A146">
         <v>55000159</v>
       </c>
@@ -15538,7 +15538,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="34.200000000000003">
+    <row r="147" spans="1:20" ht="24">
       <c r="A147">
         <v>55000160</v>
       </c>
@@ -15582,7 +15582,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="57">
+    <row r="148" spans="1:20" ht="48">
       <c r="A148">
         <v>55000161</v>
       </c>
@@ -15628,7 +15628,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="45.6">
+    <row r="149" spans="1:20" ht="48">
       <c r="A149">
         <v>55000162</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="45.6">
+    <row r="150" spans="1:20" ht="36">
       <c r="A150">
         <v>55000163</v>
       </c>
@@ -15724,7 +15724,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="45.6">
+    <row r="151" spans="1:20" ht="36">
       <c r="A151">
         <v>55000164</v>
       </c>
@@ -15768,7 +15768,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="34.200000000000003">
+    <row r="152" spans="1:20" ht="24">
       <c r="A152">
         <v>55000165</v>
       </c>
@@ -15814,7 +15814,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="45.6">
+    <row r="153" spans="1:20" ht="48">
       <c r="A153">
         <v>55000166</v>
       </c>
@@ -15858,7 +15858,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="34.200000000000003">
+    <row r="154" spans="1:20" ht="24">
       <c r="A154">
         <v>55000167</v>
       </c>
@@ -15904,7 +15904,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="79.8">
+    <row r="155" spans="1:20" ht="72">
       <c r="A155">
         <v>55000168</v>
       </c>
@@ -15951,7 +15951,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="68.400000000000006">
+    <row r="156" spans="1:20" ht="60">
       <c r="A156">
         <v>55000169</v>
       </c>
@@ -15999,7 +15999,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="45.6">
+    <row r="157" spans="1:20" ht="48">
       <c r="A157">
         <v>55000170</v>
       </c>
@@ -16087,7 +16087,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="45.6">
+    <row r="159" spans="1:20" ht="36">
       <c r="A159">
         <v>55000172</v>
       </c>
@@ -16133,7 +16133,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="45.6">
+    <row r="160" spans="1:20" ht="36">
       <c r="A160">
         <v>55000173</v>
       </c>
@@ -16179,7 +16179,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="45.6">
+    <row r="161" spans="1:20" ht="36">
       <c r="A161">
         <v>55000174</v>
       </c>
@@ -16227,7 +16227,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="45.6">
+    <row r="162" spans="1:20" ht="36">
       <c r="A162">
         <v>55000175</v>
       </c>
@@ -16273,7 +16273,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="34.200000000000003">
+    <row r="163" spans="1:20" ht="36">
       <c r="A163">
         <v>55000176</v>
       </c>
@@ -16321,7 +16321,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="22.8">
+    <row r="164" spans="1:20" ht="24">
       <c r="A164">
         <v>55000177</v>
       </c>
@@ -16367,7 +16367,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="125.4">
+    <row r="165" spans="1:20" ht="108">
       <c r="A165">
         <v>55000178</v>
       </c>
@@ -16413,7 +16413,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="102.6">
+    <row r="166" spans="1:20" ht="96">
       <c r="A166">
         <v>55000179</v>
       </c>
@@ -16459,7 +16459,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="45.6">
+    <row r="167" spans="1:20" ht="36">
       <c r="A167">
         <v>55000180</v>
       </c>
@@ -16507,7 +16507,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="34.200000000000003">
+    <row r="168" spans="1:20" ht="24">
       <c r="A168">
         <v>55000181</v>
       </c>
@@ -16551,7 +16551,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="34.200000000000003">
+    <row r="169" spans="1:20" ht="24">
       <c r="A169">
         <v>55000182</v>
       </c>
@@ -16599,7 +16599,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="79.8">
+    <row r="170" spans="1:20" ht="84">
       <c r="A170">
         <v>55000183</v>
       </c>
@@ -16643,7 +16643,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="22.8">
+    <row r="171" spans="1:20" ht="24">
       <c r="A171">
         <v>55000184</v>
       </c>
@@ -16687,7 +16687,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="34.200000000000003">
+    <row r="172" spans="1:20" ht="36">
       <c r="A172">
         <v>55000185</v>
       </c>
@@ -16731,7 +16731,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="45.6">
+    <row r="173" spans="1:20" ht="36">
       <c r="A173">
         <v>55000186</v>
       </c>
@@ -16777,7 +16777,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="57">
+    <row r="174" spans="1:20" ht="48">
       <c r="A174">
         <v>55000187</v>
       </c>
@@ -16821,7 +16821,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="22.8">
+    <row r="175" spans="1:20" ht="24">
       <c r="A175">
         <v>55000188</v>
       </c>
@@ -16865,7 +16865,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="45.6">
+    <row r="176" spans="1:20" ht="36">
       <c r="A176">
         <v>55000189</v>
       </c>
@@ -16913,7 +16913,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="45.6">
+    <row r="177" spans="1:20" ht="36">
       <c r="A177">
         <v>55000190</v>
       </c>
@@ -16959,7 +16959,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="57">
+    <row r="178" spans="1:20" ht="48">
       <c r="A178">
         <v>55000191</v>
       </c>
@@ -17007,7 +17007,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="68.400000000000006">
+    <row r="179" spans="1:20" ht="60">
       <c r="A179">
         <v>55000192</v>
       </c>
@@ -17053,7 +17053,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="34.200000000000003">
+    <row r="180" spans="1:20" ht="24">
       <c r="A180">
         <v>55000193</v>
       </c>
@@ -17099,7 +17099,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="45.6">
+    <row r="181" spans="1:20" ht="48">
       <c r="A181">
         <v>55000194</v>
       </c>
@@ -17145,7 +17145,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="68.400000000000006">
+    <row r="182" spans="1:20" ht="60">
       <c r="A182">
         <v>55000195</v>
       </c>
@@ -17189,7 +17189,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="68.400000000000006">
+    <row r="183" spans="1:20" ht="60">
       <c r="A183">
         <v>55000196</v>
       </c>
@@ -17233,7 +17233,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="34.200000000000003">
+    <row r="184" spans="1:20" ht="24">
       <c r="A184">
         <v>55000197</v>
       </c>
@@ -17277,7 +17277,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="34.200000000000003">
+    <row r="185" spans="1:20" ht="36">
       <c r="A185">
         <v>55000198</v>
       </c>
@@ -17365,7 +17365,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="45.6">
+    <row r="187" spans="1:20" ht="48">
       <c r="A187">
         <v>55000200</v>
       </c>
@@ -17409,7 +17409,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="34.200000000000003">
+    <row r="188" spans="1:20" ht="36">
       <c r="A188">
         <v>55000201</v>
       </c>
@@ -17455,7 +17455,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="45.6">
+    <row r="189" spans="1:20" ht="48">
       <c r="A189">
         <v>55000202</v>
       </c>
@@ -17501,7 +17501,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="34.200000000000003">
+    <row r="190" spans="1:20" ht="24">
       <c r="A190">
         <v>55000203</v>
       </c>
@@ -17545,7 +17545,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="45.6">
+    <row r="191" spans="1:20" ht="48">
       <c r="A191">
         <v>55000204</v>
       </c>
@@ -17591,7 +17591,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="22.8">
+    <row r="192" spans="1:20" ht="24">
       <c r="A192">
         <v>55000205</v>
       </c>
@@ -17635,7 +17635,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="125.4">
+    <row r="193" spans="1:20" ht="96">
       <c r="A193">
         <v>55000206</v>
       </c>
@@ -17681,7 +17681,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="22.8">
+    <row r="194" spans="1:20" ht="24">
       <c r="A194">
         <v>55000207</v>
       </c>
@@ -17769,7 +17769,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="45.6">
+    <row r="196" spans="1:20" ht="48">
       <c r="A196">
         <v>55000209</v>
       </c>
@@ -17815,7 +17815,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="57">
+    <row r="197" spans="1:20" ht="48">
       <c r="A197">
         <v>55000210</v>
       </c>
@@ -17863,7 +17863,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="45.6">
+    <row r="198" spans="1:20" ht="48">
       <c r="A198">
         <v>55000211</v>
       </c>
@@ -17909,7 +17909,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="22.8">
+    <row r="199" spans="1:20" ht="24">
       <c r="A199">
         <v>55000212</v>
       </c>
@@ -17955,7 +17955,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="45.6">
+    <row r="200" spans="1:20" ht="48">
       <c r="A200">
         <v>55000213</v>
       </c>
@@ -18001,7 +18001,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="34.200000000000003">
+    <row r="201" spans="1:20" ht="24">
       <c r="A201">
         <v>55000214</v>
       </c>
@@ -18045,7 +18045,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="102.6">
+    <row r="202" spans="1:20" ht="84">
       <c r="A202">
         <v>55000215</v>
       </c>
@@ -18096,7 +18096,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="45.6">
+    <row r="203" spans="1:20" ht="36">
       <c r="A203">
         <v>55000216</v>
       </c>
@@ -18142,7 +18142,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="22.8">
+    <row r="204" spans="1:20" ht="24">
       <c r="A204">
         <v>55000217</v>
       </c>
@@ -18276,7 +18276,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="45.6">
+    <row r="207" spans="1:20" ht="36">
       <c r="A207">
         <v>55000220</v>
       </c>
@@ -18322,7 +18322,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="22.8">
+    <row r="208" spans="1:20" ht="24">
       <c r="A208">
         <v>55000221</v>
       </c>
@@ -18366,7 +18366,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="45.6">
+    <row r="209" spans="1:20" ht="36">
       <c r="A209">
         <v>55000222</v>
       </c>
@@ -18412,7 +18412,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="45.6">
+    <row r="210" spans="1:20" ht="36">
       <c r="A210">
         <v>55000223</v>
       </c>
@@ -18458,7 +18458,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="45.6">
+    <row r="211" spans="1:20" ht="36">
       <c r="A211">
         <v>55000224</v>
       </c>
@@ -18504,7 +18504,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="57">
+    <row r="212" spans="1:20" ht="48">
       <c r="A212">
         <v>55000225</v>
       </c>
@@ -18550,7 +18550,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="125.4">
+    <row r="213" spans="1:20" ht="96">
       <c r="A213">
         <v>55000226</v>
       </c>
@@ -18596,7 +18596,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="34.200000000000003">
+    <row r="214" spans="1:20" ht="24">
       <c r="A214">
         <v>55000227</v>
       </c>
@@ -18642,7 +18642,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="22.8">
+    <row r="215" spans="1:20" ht="24">
       <c r="A215">
         <v>55000228</v>
       </c>
@@ -18686,7 +18686,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="34.200000000000003">
+    <row r="216" spans="1:20" ht="24">
       <c r="A216">
         <v>55000229</v>
       </c>
@@ -18732,7 +18732,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="34.200000000000003">
+    <row r="217" spans="1:20" ht="24">
       <c r="A217">
         <v>55000230</v>
       </c>
@@ -18776,7 +18776,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="22.8">
+    <row r="218" spans="1:20" ht="24">
       <c r="A218">
         <v>55000231</v>
       </c>
@@ -18820,7 +18820,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="57">
+    <row r="219" spans="1:20" ht="48">
       <c r="A219">
         <v>55000232</v>
       </c>
@@ -18864,7 +18864,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="45.6">
+    <row r="220" spans="1:20" ht="36">
       <c r="A220">
         <v>55000233</v>
       </c>
@@ -18908,7 +18908,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="45.6">
+    <row r="221" spans="1:20" ht="36">
       <c r="A221">
         <v>55000234</v>
       </c>
@@ -18954,7 +18954,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="79.8">
+    <row r="222" spans="1:20" ht="72">
       <c r="A222">
         <v>55000235</v>
       </c>
@@ -18998,7 +18998,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="34.200000000000003">
+    <row r="223" spans="1:20" ht="24">
       <c r="A223">
         <v>55000236</v>
       </c>
@@ -19084,7 +19084,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="22.8">
+    <row r="225" spans="1:20" ht="24">
       <c r="A225">
         <v>55000238</v>
       </c>
@@ -19128,7 +19128,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="34.200000000000003">
+    <row r="226" spans="1:20" ht="24">
       <c r="A226">
         <v>55000239</v>
       </c>
@@ -19172,7 +19172,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="91.2">
+    <row r="227" spans="1:20" ht="84">
       <c r="A227">
         <v>55000240</v>
       </c>
@@ -19223,7 +19223,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="22.8">
+    <row r="228" spans="1:20" ht="24">
       <c r="A228">
         <v>55000241</v>
       </c>
@@ -19270,7 +19270,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="34.200000000000003">
+    <row r="229" spans="1:20" ht="24">
       <c r="A229">
         <v>55000242</v>
       </c>
@@ -19316,7 +19316,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="34.200000000000003">
+    <row r="230" spans="1:20" ht="36">
       <c r="A230">
         <v>55000243</v>
       </c>
@@ -19360,7 +19360,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="102.6">
+    <row r="231" spans="1:20" ht="84">
       <c r="A231">
         <v>55000244</v>
       </c>
@@ -19410,7 +19410,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="34.200000000000003">
+    <row r="232" spans="1:20" ht="24">
       <c r="A232">
         <v>55000245</v>
       </c>
@@ -19454,7 +19454,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="34.200000000000003">
+    <row r="233" spans="1:20" ht="36">
       <c r="A233">
         <v>55000246</v>
       </c>
@@ -19500,7 +19500,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="68.400000000000006">
+    <row r="234" spans="1:20" ht="48">
       <c r="A234">
         <v>55000247</v>
       </c>
@@ -19546,7 +19546,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="45.6">
+    <row r="235" spans="1:20" ht="36">
       <c r="A235">
         <v>55000248</v>
       </c>
@@ -19594,7 +19594,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="34.200000000000003">
+    <row r="236" spans="1:20" ht="24">
       <c r="A236">
         <v>55000249</v>
       </c>
@@ -19640,7 +19640,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="45.6">
+    <row r="237" spans="1:20" ht="36">
       <c r="A237">
         <v>55000250</v>
       </c>
@@ -19684,7 +19684,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="28.8">
+    <row r="238" spans="1:20" ht="27">
       <c r="A238">
         <v>55000251</v>
       </c>
@@ -19728,7 +19728,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="22.8">
+    <row r="239" spans="1:20" ht="24">
       <c r="A239">
         <v>55000252</v>
       </c>
@@ -19774,7 +19774,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="34.200000000000003">
+    <row r="240" spans="1:20" ht="36">
       <c r="A240">
         <v>55000253</v>
       </c>
@@ -19820,7 +19820,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="34.200000000000003">
+    <row r="241" spans="1:20" ht="36">
       <c r="A241">
         <v>55000254</v>
       </c>
@@ -19950,7 +19950,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="45.6">
+    <row r="244" spans="1:20" ht="36">
       <c r="A244">
         <v>55000257</v>
       </c>
@@ -19998,7 +19998,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="34.200000000000003">
+    <row r="245" spans="1:20" ht="24">
       <c r="A245">
         <v>55000258</v>
       </c>
@@ -20042,7 +20042,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="45.6">
+    <row r="246" spans="1:20" ht="36">
       <c r="A246">
         <v>55000259</v>
       </c>
@@ -20090,7 +20090,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="91.2">
+    <row r="247" spans="1:20" ht="84">
       <c r="A247">
         <v>55000260</v>
       </c>
@@ -20136,7 +20136,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="91.2">
+    <row r="248" spans="1:20" ht="84">
       <c r="A248">
         <v>55000261</v>
       </c>
@@ -20180,7 +20180,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="34.200000000000003">
+    <row r="249" spans="1:20" ht="24">
       <c r="A249">
         <v>55000262</v>
       </c>
@@ -20224,7 +20224,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="22.8">
+    <row r="250" spans="1:20" ht="24">
       <c r="A250">
         <v>55000263</v>
       </c>
@@ -20272,7 +20272,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="45.6">
+    <row r="251" spans="1:20" ht="36">
       <c r="A251">
         <v>55000264</v>
       </c>
@@ -20318,7 +20318,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="45.6">
+    <row r="252" spans="1:20" ht="36">
       <c r="A252">
         <v>55000265</v>
       </c>
@@ -20362,7 +20362,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="45.6">
+    <row r="253" spans="1:20" ht="48">
       <c r="A253">
         <v>55000266</v>
       </c>
@@ -20406,7 +20406,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="22.8">
+    <row r="254" spans="1:20" ht="24">
       <c r="A254">
         <v>55000267</v>
       </c>
@@ -20452,7 +20452,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="22.8">
+    <row r="255" spans="1:20" ht="24">
       <c r="A255">
         <v>55000268</v>
       </c>
@@ -20496,7 +20496,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="45.6">
+    <row r="256" spans="1:20" ht="48">
       <c r="A256">
         <v>55000269</v>
       </c>
@@ -20540,7 +20540,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="45.6">
+    <row r="257" spans="1:20" ht="48">
       <c r="A257">
         <v>55000270</v>
       </c>
@@ -20586,7 +20586,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="34.200000000000003">
+    <row r="258" spans="1:20" ht="36">
       <c r="A258">
         <v>55000271</v>
       </c>
@@ -20632,7 +20632,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="34.200000000000003">
+    <row r="259" spans="1:20" ht="24">
       <c r="A259">
         <v>55000272</v>
       </c>
@@ -20676,7 +20676,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="45.6">
+    <row r="260" spans="1:20" ht="36">
       <c r="A260">
         <v>55000273</v>
       </c>
@@ -20720,7 +20720,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="91.2">
+    <row r="261" spans="1:20" ht="84">
       <c r="A261">
         <v>55000274</v>
       </c>
@@ -20764,7 +20764,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="45.6">
+    <row r="262" spans="1:20" ht="36">
       <c r="A262">
         <v>55000275</v>
       </c>
@@ -20810,7 +20810,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="45.6">
+    <row r="263" spans="1:20" ht="36">
       <c r="A263">
         <v>55000276</v>
       </c>
@@ -20856,7 +20856,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="22.8">
+    <row r="264" spans="1:20">
       <c r="A264">
         <v>55000277</v>
       </c>
@@ -20900,7 +20900,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="22.8">
+    <row r="265" spans="1:20" ht="24">
       <c r="A265">
         <v>55000278</v>
       </c>
@@ -20944,7 +20944,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="22.8">
+    <row r="266" spans="1:20">
       <c r="A266">
         <v>55000279</v>
       </c>
@@ -20988,7 +20988,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="45.6">
+    <row r="267" spans="1:20" ht="36">
       <c r="A267">
         <v>55000280</v>
       </c>
@@ -21032,7 +21032,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="22.8">
+    <row r="268" spans="1:20" ht="24">
       <c r="A268">
         <v>55000281</v>
       </c>
@@ -21076,7 +21076,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="171">
+    <row r="269" spans="1:20" ht="144">
       <c r="A269">
         <v>55000282</v>
       </c>
@@ -21122,7 +21122,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="45.6">
+    <row r="270" spans="1:20" ht="36">
       <c r="A270">
         <v>55000284</v>
       </c>
@@ -21170,7 +21170,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="45.6">
+    <row r="271" spans="1:20" ht="48">
       <c r="A271">
         <v>55000285</v>
       </c>
@@ -21258,7 +21258,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="34.200000000000003">
+    <row r="273" spans="1:20" ht="36">
       <c r="A273">
         <v>55000287</v>
       </c>
@@ -21304,7 +21304,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="22.8">
+    <row r="274" spans="1:20" ht="24">
       <c r="A274">
         <v>55000288</v>
       </c>
@@ -21350,7 +21350,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="136.80000000000001">
+    <row r="275" spans="1:20" ht="120">
       <c r="A275">
         <v>55000289</v>
       </c>
@@ -21394,7 +21394,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="91.2">
+    <row r="276" spans="1:20" ht="84">
       <c r="A276">
         <v>55000290</v>
       </c>
@@ -21438,7 +21438,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="79.8">
+    <row r="277" spans="1:20" ht="60">
       <c r="A277">
         <v>55000291</v>
       </c>
@@ -21482,7 +21482,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="45.6">
+    <row r="278" spans="1:20" ht="36">
       <c r="A278">
         <v>55000292</v>
       </c>
@@ -21530,7 +21530,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="57">
+    <row r="279" spans="1:20" ht="48">
       <c r="A279">
         <v>55000293</v>
       </c>
@@ -21574,7 +21574,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="102.6">
+    <row r="280" spans="1:20" ht="84">
       <c r="A280">
         <v>55000294</v>
       </c>
@@ -21667,7 +21667,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="22.8">
+    <row r="282" spans="1:20" ht="24">
       <c r="A282">
         <v>55000296</v>
       </c>
@@ -21711,7 +21711,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="114">
+    <row r="283" spans="1:20" ht="96">
       <c r="A283">
         <v>55000297</v>
       </c>
@@ -21757,7 +21757,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="102.6">
+    <row r="284" spans="1:20" ht="84">
       <c r="A284">
         <v>55000298</v>
       </c>
@@ -21803,7 +21803,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="34.200000000000003">
+    <row r="285" spans="1:20" ht="24">
       <c r="A285">
         <v>55000299</v>
       </c>
@@ -21851,7 +21851,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="22.8">
+    <row r="286" spans="1:20" ht="24">
       <c r="A286">
         <v>55000300</v>
       </c>
@@ -21899,7 +21899,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="102.6">
+    <row r="287" spans="1:20" ht="96">
       <c r="A287">
         <v>55000324</v>
       </c>
@@ -21950,7 +21950,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="102.6">
+    <row r="288" spans="1:20" ht="84">
       <c r="A288">
         <v>55000325</v>
       </c>
@@ -22000,7 +22000,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="91.2">
+    <row r="289" spans="1:20" ht="84">
       <c r="A289">
         <v>55000326</v>
       </c>
@@ -22050,7 +22050,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="102.6">
+    <row r="290" spans="1:20" ht="96">
       <c r="A290">
         <v>55000327</v>
       </c>
@@ -22100,7 +22100,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="102.6">
+    <row r="291" spans="1:20" ht="84">
       <c r="A291">
         <v>55000328</v>
       </c>
@@ -22151,7 +22151,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="102.6">
+    <row r="292" spans="1:20" ht="84">
       <c r="A292">
         <v>55000329</v>
       </c>
@@ -22202,7 +22202,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="102.6">
+    <row r="293" spans="1:20" ht="96">
       <c r="A293">
         <v>55000330</v>
       </c>
@@ -22253,7 +22253,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="102.6">
+    <row r="294" spans="1:20" ht="84">
       <c r="A294">
         <v>55000331</v>
       </c>
@@ -22304,7 +22304,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="91.2">
+    <row r="295" spans="1:20" ht="72">
       <c r="A295">
         <v>55000332</v>
       </c>
@@ -22348,7 +22348,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="216.6">
+    <row r="296" spans="1:20" ht="180">
       <c r="A296">
         <v>55000333</v>
       </c>
@@ -22392,7 +22392,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="102.6">
+    <row r="297" spans="1:20" ht="96">
       <c r="A297">
         <v>55000334</v>
       </c>
@@ -22443,7 +22443,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="91.2">
+    <row r="298" spans="1:20" ht="84">
       <c r="A298">
         <v>55000335</v>
       </c>
@@ -22487,7 +22487,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="45.6">
+    <row r="299" spans="1:20" ht="48">
       <c r="A299">
         <v>55000340</v>
       </c>
@@ -22535,7 +22535,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="34.200000000000003">
+    <row r="300" spans="1:20" ht="24">
       <c r="A300">
         <v>55000341</v>
       </c>
@@ -22581,7 +22581,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="171">
+    <row r="301" spans="1:20" ht="144">
       <c r="A301">
         <v>55000342</v>
       </c>
@@ -22625,7 +22625,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="171">
+    <row r="302" spans="1:20" ht="144">
       <c r="A302">
         <v>55000343</v>
       </c>
@@ -22669,7 +22669,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="34.200000000000003">
+    <row r="303" spans="1:20" ht="36">
       <c r="A303" t="s">
         <v>1369</v>
       </c>
@@ -22735,20 +22735,20 @@
       <selection pane="bottomRight" activeCell="K1" sqref="K1:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" customWidth="1"/>
-    <col min="4" max="8" width="8.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" customWidth="1"/>
-    <col min="10" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" customWidth="1"/>
-    <col min="14" max="14" width="23.44140625" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="17" width="7.6640625" customWidth="1"/>
-    <col min="18" max="18" width="7.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="4" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="22.25" customWidth="1"/>
+    <col min="10" max="11" width="8.5" customWidth="1"/>
+    <col min="12" max="12" width="7.375" customWidth="1"/>
+    <col min="13" max="13" width="6.375" customWidth="1"/>
+    <col min="14" max="14" width="23.5" customWidth="1"/>
+    <col min="15" max="15" width="6.625" customWidth="1"/>
+    <col min="16" max="17" width="7.625" customWidth="1"/>
+    <col min="18" max="18" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -22937,7 +22937,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="91.2">
+    <row r="4" spans="1:20" ht="84">
       <c r="A4">
         <v>55010003</v>
       </c>
@@ -22981,7 +22981,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="91.2">
+    <row r="5" spans="1:20" ht="84">
       <c r="A5">
         <v>55010004</v>
       </c>
@@ -23047,20 +23047,20 @@
       <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.75" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" customWidth="1"/>
-    <col min="4" max="8" width="8.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" customWidth="1"/>
-    <col min="10" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" customWidth="1"/>
-    <col min="13" max="13" width="6.33203125" customWidth="1"/>
-    <col min="14" max="14" width="23.44140625" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="17" width="7.6640625" customWidth="1"/>
-    <col min="18" max="18" width="7.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="4" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="22.25" customWidth="1"/>
+    <col min="10" max="11" width="8.5" customWidth="1"/>
+    <col min="12" max="12" width="7.375" customWidth="1"/>
+    <col min="13" max="13" width="6.375" customWidth="1"/>
+    <col min="14" max="14" width="23.5" customWidth="1"/>
+    <col min="15" max="15" width="6.625" customWidth="1"/>
+    <col min="16" max="17" width="7.625" customWidth="1"/>
+    <col min="18" max="18" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -23249,7 +23249,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="45.6">
+    <row r="4" spans="1:20" ht="36">
       <c r="A4">
         <v>55020001</v>
       </c>
@@ -23295,7 +23295,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="45.6">
+    <row r="5" spans="1:20" ht="36">
       <c r="A5">
         <v>55020002</v>
       </c>
@@ -23341,7 +23341,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="45.6">
+    <row r="6" spans="1:20" ht="36">
       <c r="A6">
         <v>55020003</v>
       </c>
@@ -23387,7 +23387,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="45.6">
+    <row r="7" spans="1:20" ht="36">
       <c r="A7">
         <v>55020004</v>
       </c>
@@ -23433,7 +23433,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="45.6">
+    <row r="8" spans="1:20" ht="36">
       <c r="A8">
         <v>55020005</v>
       </c>
@@ -23479,7 +23479,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="45.6">
+    <row r="9" spans="1:20" ht="36">
       <c r="A9">
         <v>55020006</v>
       </c>
@@ -23525,7 +23525,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="45.6">
+    <row r="10" spans="1:20" ht="36">
       <c r="A10">
         <v>55020007</v>
       </c>
@@ -23571,7 +23571,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="45.6">
+    <row r="11" spans="1:20" ht="36">
       <c r="A11">
         <v>55020008</v>
       </c>
@@ -23617,7 +23617,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="45.6">
+    <row r="12" spans="1:20" ht="36">
       <c r="A12">
         <v>55020009</v>
       </c>
@@ -23663,7 +23663,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="45.6">
+    <row r="13" spans="1:20" ht="36">
       <c r="A13">
         <v>55020010</v>
       </c>
@@ -23709,7 +23709,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="45.6">
+    <row r="14" spans="1:20" ht="36">
       <c r="A14">
         <v>55020011</v>
       </c>
@@ -23755,7 +23755,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="45.6">
+    <row r="15" spans="1:20" ht="36">
       <c r="A15">
         <v>55020012</v>
       </c>
@@ -23801,7 +23801,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="45.6">
+    <row r="16" spans="1:20" ht="36">
       <c r="A16">
         <v>55020013</v>
       </c>
@@ -23847,7 +23847,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="45.6">
+    <row r="17" spans="1:20" ht="36">
       <c r="A17">
         <v>55020014</v>
       </c>
@@ -23893,7 +23893,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="45.6">
+    <row r="18" spans="1:20" ht="36">
       <c r="A18">
         <v>55020015</v>
       </c>
@@ -23939,7 +23939,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="45.6">
+    <row r="19" spans="1:20" ht="36">
       <c r="A19">
         <v>55020016</v>
       </c>
@@ -24004,9 +24004,9 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -24596,7 +24596,7 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
skill mark max 10000 -> 100
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3108" uniqueCount="1495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3107" uniqueCount="1495">
   <si>
     <t>夜色</t>
   </si>
@@ -9368,10 +9368,10 @@
   <dimension ref="A1:X303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="K189" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="P186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V190" sqref="V190"/>
+      <selection pane="bottomRight" activeCell="X191" sqref="X191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9657,7 +9657,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -9705,7 +9705,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>5</v>
@@ -9753,7 +9753,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>8</v>
@@ -9803,7 +9803,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>11</v>
@@ -9853,7 +9853,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>13</v>
@@ -9903,7 +9903,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>15</v>
@@ -9953,7 +9953,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>17</v>
@@ -10003,7 +10003,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>19</v>
@@ -10053,7 +10053,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W12" s="1" t="s">
         <v>21</v>
@@ -10103,7 +10103,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>23</v>
@@ -10153,7 +10153,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>25</v>
@@ -10203,7 +10203,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W15" s="1" t="s">
         <v>27</v>
@@ -10253,7 +10253,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W16" s="1" t="s">
         <v>29</v>
@@ -10303,7 +10303,7 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>31</v>
@@ -10353,7 +10353,7 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>33</v>
@@ -10403,7 +10403,7 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W19" s="1" t="s">
         <v>35</v>
@@ -10453,7 +10453,7 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>37</v>
@@ -10503,7 +10503,7 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>39</v>
@@ -10553,7 +10553,7 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W22" s="1" t="s">
         <v>41</v>
@@ -10603,7 +10603,7 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1">
-        <v>160</v>
+        <v>1</v>
       </c>
       <c r="W23" s="1" t="s">
         <v>43</v>
@@ -10697,7 +10697,7 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>62</v>
@@ -10747,7 +10747,7 @@
         <v>1019</v>
       </c>
       <c r="V26" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W26" s="1" t="s">
         <v>65</v>
@@ -10797,7 +10797,7 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W27" s="1" t="s">
         <v>67</v>
@@ -10847,7 +10847,7 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W28" s="1" t="s">
         <v>69</v>
@@ -10895,7 +10895,7 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W29" s="1" t="s">
         <v>671</v>
@@ -10943,7 +10943,7 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W30" s="1" t="s">
         <v>71</v>
@@ -10991,7 +10991,7 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1">
-        <v>800</v>
+        <v>8</v>
       </c>
       <c r="W31" s="1" t="s">
         <v>74</v>
@@ -11041,7 +11041,7 @@
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W32" s="1" t="s">
         <v>77</v>
@@ -11089,7 +11089,7 @@
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>79</v>
@@ -11137,7 +11137,7 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>81</v>
@@ -11185,7 +11185,7 @@
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1">
-        <v>2000</v>
+        <v>20</v>
       </c>
       <c r="W35" s="1" t="s">
         <v>83</v>
@@ -11233,7 +11233,7 @@
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1">
-        <v>4000</v>
+        <v>40</v>
       </c>
       <c r="W36" s="1" t="s">
         <v>85</v>
@@ -11285,7 +11285,7 @@
         <v>1019</v>
       </c>
       <c r="V37" s="1">
-        <v>2000</v>
+        <v>20</v>
       </c>
       <c r="W37" s="1" t="s">
         <v>89</v>
@@ -11335,7 +11335,7 @@
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>91</v>
@@ -11383,7 +11383,7 @@
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>93</v>
@@ -11431,7 +11431,7 @@
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1">
-        <v>2500</v>
+        <v>25</v>
       </c>
       <c r="W40" s="1" t="s">
         <v>95</v>
@@ -11479,7 +11479,7 @@
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>97</v>
@@ -11527,7 +11527,7 @@
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>99</v>
@@ -11577,7 +11577,7 @@
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>102</v>
@@ -11627,7 +11627,7 @@
         <v>1021</v>
       </c>
       <c r="V44" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W44" s="1" t="s">
         <v>105</v>
@@ -11675,7 +11675,7 @@
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W45" s="1" t="s">
         <v>107</v>
@@ -11725,7 +11725,7 @@
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1">
-        <v>160</v>
+        <v>1</v>
       </c>
       <c r="W46" s="1" t="s">
         <v>109</v>
@@ -11773,7 +11773,7 @@
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
       <c r="V47" s="25">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>112</v>
@@ -11823,7 +11823,7 @@
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1">
-        <v>175</v>
+        <v>1</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>132</v>
@@ -11871,7 +11871,7 @@
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
       <c r="V49" s="1">
-        <v>450</v>
+        <v>4</v>
       </c>
       <c r="W49" s="1" t="s">
         <v>134</v>
@@ -11921,7 +11921,7 @@
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
       <c r="V50" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W50" s="1" t="s">
         <v>137</v>
@@ -11973,7 +11973,7 @@
         <v>1021</v>
       </c>
       <c r="V51" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W51" s="1" t="s">
         <v>139</v>
@@ -12023,7 +12023,7 @@
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W52" s="1" t="s">
         <v>141</v>
@@ -12073,7 +12073,7 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
       <c r="V53" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W53" s="1" t="s">
         <v>143</v>
@@ -12123,7 +12123,7 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>145</v>
@@ -12173,7 +12173,7 @@
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
       <c r="V55" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W55" s="1" t="s">
         <v>147</v>
@@ -12223,7 +12223,7 @@
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W56" s="1" t="s">
         <v>149</v>
@@ -12273,7 +12273,7 @@
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
       <c r="V57" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>151</v>
@@ -12323,7 +12323,7 @@
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
       <c r="V58" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W58" s="1" t="s">
         <v>153</v>
@@ -12373,7 +12373,7 @@
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
       <c r="V59" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W59" s="1" t="s">
         <v>155</v>
@@ -12423,7 +12423,7 @@
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
       <c r="V60" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W60" s="1" t="s">
         <v>157</v>
@@ -12471,7 +12471,7 @@
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>159</v>
@@ -12523,7 +12523,7 @@
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
       <c r="V62" s="1">
-        <v>1250</v>
+        <v>12</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>164</v>
@@ -12571,7 +12571,7 @@
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
       <c r="V63" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W63" s="1" t="s">
         <v>167</v>
@@ -12621,7 +12621,7 @@
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
       <c r="V64" s="1">
-        <v>2600</v>
+        <v>26</v>
       </c>
       <c r="W64" s="1" t="s">
         <v>169</v>
@@ -12669,7 +12669,7 @@
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
       <c r="V65" s="1">
-        <v>-400</v>
+        <v>-4</v>
       </c>
       <c r="W65" s="1" t="s">
         <v>171</v>
@@ -12719,7 +12719,7 @@
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
       <c r="V66" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W66" s="1" t="s">
         <v>174</v>
@@ -12769,7 +12769,7 @@
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
       <c r="V67" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W67" s="1" t="s">
         <v>177</v>
@@ -12817,7 +12817,7 @@
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
       <c r="V68" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W68" s="1" t="s">
         <v>180</v>
@@ -12867,7 +12867,7 @@
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
       <c r="V69" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>182</v>
@@ -12919,7 +12919,7 @@
         <v>1023</v>
       </c>
       <c r="V70" s="1">
-        <v>1500</v>
+        <v>15</v>
       </c>
       <c r="W70" s="1" t="s">
         <v>186</v>
@@ -12979,7 +12979,7 @@
         <v>1022</v>
       </c>
       <c r="V71" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W71" s="1" t="s">
         <v>188</v>
@@ -13029,7 +13029,7 @@
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
       <c r="V72" s="1">
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="W72" s="1" t="s">
         <v>190</v>
@@ -13079,7 +13079,7 @@
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
       <c r="V73" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W73" s="1" t="s">
         <v>192</v>
@@ -13127,7 +13127,7 @@
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
       <c r="V74" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W74" s="1" t="s">
         <v>194</v>
@@ -13175,7 +13175,7 @@
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
       <c r="V75" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W75" s="1" t="s">
         <v>196</v>
@@ -13223,7 +13223,7 @@
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
       <c r="V76" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W76" s="1" t="s">
         <v>198</v>
@@ -13271,7 +13271,7 @@
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
       <c r="V77" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W77" s="1" t="s">
         <v>201</v>
@@ -13319,7 +13319,7 @@
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
       <c r="V78" s="1">
-        <v>-1425</v>
+        <v>-15</v>
       </c>
       <c r="W78" s="1" t="s">
         <v>203</v>
@@ -13371,7 +13371,7 @@
         <v>1022</v>
       </c>
       <c r="V79" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W79" s="1" t="s">
         <v>204</v>
@@ -13419,7 +13419,7 @@
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
       <c r="V80" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W80" s="1" t="s">
         <v>206</v>
@@ -13467,7 +13467,7 @@
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
       <c r="V81" s="1">
-        <v>3000</v>
+        <v>30</v>
       </c>
       <c r="W81" s="1" t="s">
         <v>208</v>
@@ -13515,7 +13515,7 @@
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
       <c r="V82" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W82" s="1" t="s">
         <v>210</v>
@@ -13563,7 +13563,7 @@
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
       <c r="V83" s="1">
-        <v>280</v>
+        <v>2</v>
       </c>
       <c r="W83" s="1" t="s">
         <v>212</v>
@@ -13613,7 +13613,7 @@
         <v>1021</v>
       </c>
       <c r="V84" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="W84" s="1" t="s">
         <v>214</v>
@@ -13675,8 +13675,7 @@
         <v>1026</v>
       </c>
       <c r="V85" s="1">
-        <f>800*3*2/12</f>
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W85" s="1" t="s">
         <v>217</v>
@@ -13724,7 +13723,7 @@
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
       <c r="V86" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="W86" s="1" t="s">
         <v>220</v>
@@ -13776,7 +13775,7 @@
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
       <c r="V87" s="1">
-        <v>555</v>
+        <v>5</v>
       </c>
       <c r="W87" s="1" t="s">
         <v>223</v>
@@ -13824,7 +13823,7 @@
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
       <c r="V88" s="1">
-        <v>180</v>
+        <v>1</v>
       </c>
       <c r="W88" s="1" t="s">
         <v>225</v>
@@ -13872,7 +13871,7 @@
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
       <c r="V89" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>227</v>
@@ -13918,7 +13917,7 @@
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
       <c r="V90" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W90" s="1" t="s">
         <v>229</v>
@@ -13968,7 +13967,7 @@
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
       <c r="V91" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W91" s="1" t="s">
         <v>231</v>
@@ -14030,8 +14029,7 @@
         <v>1026</v>
       </c>
       <c r="V92" s="1">
-        <f>1000*1.5*2/12</f>
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="W92" s="1" t="s">
         <v>233</v>
@@ -14081,7 +14079,7 @@
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
       <c r="V93" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W93" s="1" t="s">
         <v>235</v>
@@ -14131,7 +14129,7 @@
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
       <c r="V94" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W94" s="1" t="s">
         <v>237</v>
@@ -14181,7 +14179,7 @@
         <v>1021</v>
       </c>
       <c r="V95" s="1">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="W95" s="1" t="s">
         <v>239</v>
@@ -14229,7 +14227,7 @@
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
       <c r="V96" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="W96" s="1" t="s">
         <v>242</v>
@@ -14277,7 +14275,7 @@
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
       <c r="V97" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W97" s="1" t="s">
         <v>245</v>
@@ -14329,7 +14327,7 @@
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
       <c r="V98" s="1">
-        <v>555</v>
+        <v>5</v>
       </c>
       <c r="W98" s="1" t="s">
         <v>248</v>
@@ -14379,7 +14377,7 @@
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
       <c r="V99" s="1">
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="W99" s="1" t="s">
         <v>250</v>
@@ -14429,7 +14427,7 @@
         <v>1021</v>
       </c>
       <c r="V100" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W100" s="1" t="s">
         <v>252</v>
@@ -14477,7 +14475,7 @@
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
       <c r="V101" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W101" s="1" t="s">
         <v>254</v>
@@ -14529,7 +14527,7 @@
         <v>1019</v>
       </c>
       <c r="V102" s="1">
-        <v>2000</v>
+        <v>20</v>
       </c>
       <c r="W102" s="1" t="s">
         <v>256</v>
@@ -14577,7 +14575,7 @@
       <c r="T103" s="1"/>
       <c r="U103" s="1"/>
       <c r="V103" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W103" s="1" t="s">
         <v>258</v>
@@ -14627,7 +14625,7 @@
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
       <c r="V104" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W104" s="1" t="s">
         <v>260</v>
@@ -14677,7 +14675,7 @@
         <v>1021</v>
       </c>
       <c r="V105" s="1">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="W105" s="1" t="s">
         <v>262</v>
@@ -14727,7 +14725,7 @@
         <v>1019</v>
       </c>
       <c r="V106" s="1">
-        <v>700</v>
+        <v>7</v>
       </c>
       <c r="W106" s="1" t="s">
         <v>264</v>
@@ -14775,7 +14773,7 @@
       <c r="T107" s="1"/>
       <c r="U107" s="1"/>
       <c r="V107" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W107" s="1" t="s">
         <v>266</v>
@@ -14827,7 +14825,7 @@
       <c r="T108" s="1"/>
       <c r="U108" s="1"/>
       <c r="V108" s="1">
-        <v>333</v>
+        <v>3</v>
       </c>
       <c r="W108" s="1" t="s">
         <v>269</v>
@@ -14877,7 +14875,7 @@
       <c r="T109" s="1"/>
       <c r="U109" s="1"/>
       <c r="V109" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W109" s="1" t="s">
         <v>271</v>
@@ -14927,7 +14925,7 @@
       <c r="T110" s="1"/>
       <c r="U110" s="1"/>
       <c r="V110" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W110" s="1" t="s">
         <v>273</v>
@@ -14977,7 +14975,7 @@
         <v>1021</v>
       </c>
       <c r="V111" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W111" s="1" t="s">
         <v>275</v>
@@ -15025,7 +15023,7 @@
       <c r="T112" s="1"/>
       <c r="U112" s="1"/>
       <c r="V112" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="W112" s="1" t="s">
         <v>278</v>
@@ -15073,7 +15071,7 @@
       <c r="T113" s="1"/>
       <c r="U113" s="1"/>
       <c r="V113" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W113" s="1" t="s">
         <v>280</v>
@@ -15119,7 +15117,7 @@
       <c r="T114" s="1"/>
       <c r="U114" s="1"/>
       <c r="V114" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W114" s="1" t="s">
         <v>282</v>
@@ -15165,7 +15163,7 @@
       <c r="T115" s="1"/>
       <c r="U115" s="1"/>
       <c r="V115" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W115" s="1" t="s">
         <v>284</v>
@@ -15213,7 +15211,7 @@
       <c r="T116" s="1"/>
       <c r="U116" s="1"/>
       <c r="V116" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W116" s="1" t="s">
         <v>286</v>
@@ -15261,7 +15259,7 @@
       <c r="T117" s="1"/>
       <c r="U117" s="1"/>
       <c r="V117" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W117" s="1" t="s">
         <v>288</v>
@@ -15309,7 +15307,7 @@
       <c r="T118" s="1"/>
       <c r="U118" s="1"/>
       <c r="V118" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W118" s="1" t="s">
         <v>290</v>
@@ -15357,7 +15355,7 @@
       <c r="T119" s="1"/>
       <c r="U119" s="1"/>
       <c r="V119" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W119" s="1" t="s">
         <v>292</v>
@@ -15413,7 +15411,7 @@
       </c>
       <c r="U120" s="1"/>
       <c r="V120" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W120" s="1" t="s">
         <v>294</v>
@@ -15463,7 +15461,7 @@
       <c r="T121" s="1"/>
       <c r="U121" s="1"/>
       <c r="V121" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W121" s="1" t="s">
         <v>296</v>
@@ -15511,7 +15509,7 @@
       <c r="T122" s="1"/>
       <c r="U122" s="1"/>
       <c r="V122" s="1">
-        <v>-500</v>
+        <v>-5</v>
       </c>
       <c r="W122" s="1" t="s">
         <v>298</v>
@@ -15559,7 +15557,7 @@
       <c r="T123" s="1"/>
       <c r="U123" s="1"/>
       <c r="V123" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W123" s="1" t="s">
         <v>300</v>
@@ -15609,7 +15607,7 @@
         <v>1021</v>
       </c>
       <c r="V124" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W124" s="1" t="s">
         <v>302</v>
@@ -15657,7 +15655,7 @@
       <c r="T125" s="1"/>
       <c r="U125" s="1"/>
       <c r="V125" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="W125" s="1" t="s">
         <v>305</v>
@@ -15707,7 +15705,7 @@
         <v>1021</v>
       </c>
       <c r="V126" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W126" s="1" t="s">
         <v>307</v>
@@ -15757,7 +15755,7 @@
         <v>1021</v>
       </c>
       <c r="V127" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W127" s="1" t="s">
         <v>309</v>
@@ -15807,7 +15805,7 @@
         <v>1021</v>
       </c>
       <c r="V128" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W128" s="1" t="s">
         <v>311</v>
@@ -15855,7 +15853,7 @@
       <c r="T129" s="1"/>
       <c r="U129" s="1"/>
       <c r="V129" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="W129" s="1" t="s">
         <v>314</v>
@@ -15907,8 +15905,7 @@
       <c r="T130" s="1"/>
       <c r="U130" s="1"/>
       <c r="V130" s="1">
-        <f>600-200</f>
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W130" s="1" t="s">
         <v>317</v>
@@ -15958,7 +15955,7 @@
         <v>1021</v>
       </c>
       <c r="V131" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W131" s="1" t="s">
         <v>319</v>
@@ -16006,7 +16003,7 @@
       <c r="T132" s="1"/>
       <c r="U132" s="1"/>
       <c r="V132" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="W132" s="1" t="s">
         <v>322</v>
@@ -16056,7 +16053,7 @@
         <v>1021</v>
       </c>
       <c r="V133" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W133" s="1" t="s">
         <v>324</v>
@@ -16104,7 +16101,7 @@
       <c r="T134" s="1"/>
       <c r="U134" s="1"/>
       <c r="V134" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="W134" s="1" t="s">
         <v>327</v>
@@ -16154,7 +16151,7 @@
         <v>1021</v>
       </c>
       <c r="V135" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W135" s="1" t="s">
         <v>329</v>
@@ -16202,7 +16199,7 @@
       <c r="T136" s="1"/>
       <c r="U136" s="1"/>
       <c r="V136" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="W136" s="1" t="s">
         <v>332</v>
@@ -16250,7 +16247,7 @@
       <c r="T137" s="1"/>
       <c r="U137" s="1"/>
       <c r="V137" s="1">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="W137" s="1" t="s">
         <v>334</v>
@@ -16300,7 +16297,7 @@
         <v>1021</v>
       </c>
       <c r="V138" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W138" s="1" t="s">
         <v>336</v>
@@ -16352,7 +16349,7 @@
         <v>1022</v>
       </c>
       <c r="V139" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W139" s="1" t="s">
         <v>338</v>
@@ -16402,7 +16399,7 @@
         <v>1021</v>
       </c>
       <c r="V140" s="1">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="W140" s="1" t="s">
         <v>340</v>
@@ -16450,7 +16447,7 @@
       <c r="T141" s="1"/>
       <c r="U141" s="1"/>
       <c r="V141" s="31">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W141" s="1" t="s">
         <v>343</v>
@@ -16498,7 +16495,7 @@
       <c r="T142" s="1"/>
       <c r="U142" s="1"/>
       <c r="V142" s="1">
-        <v>-120</v>
+        <v>-2</v>
       </c>
       <c r="W142" s="1" t="s">
         <v>346</v>
@@ -16546,7 +16543,7 @@
       <c r="T143" s="1"/>
       <c r="U143" s="1"/>
       <c r="V143" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="W143" s="1" t="s">
         <v>348</v>
@@ -16594,7 +16591,7 @@
       <c r="T144" s="1"/>
       <c r="U144" s="1"/>
       <c r="V144" s="1">
-        <v>3000</v>
+        <v>30</v>
       </c>
       <c r="W144" s="1" t="s">
         <v>350</v>
@@ -16644,7 +16641,7 @@
       <c r="T145" s="1"/>
       <c r="U145" s="1"/>
       <c r="V145" s="1">
-        <v>700</v>
+        <v>7</v>
       </c>
       <c r="W145" s="1" t="s">
         <v>353</v>
@@ -16694,7 +16691,7 @@
       <c r="T146" s="1"/>
       <c r="U146" s="1"/>
       <c r="V146" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W146" s="1" t="s">
         <v>355</v>
@@ -16742,7 +16739,7 @@
       <c r="T147" s="1"/>
       <c r="U147" s="1"/>
       <c r="V147" s="1">
-        <v>950</v>
+        <v>9</v>
       </c>
       <c r="W147" s="1" t="s">
         <v>357</v>
@@ -16792,7 +16789,7 @@
         <v>1021</v>
       </c>
       <c r="V148" s="1">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="W148" s="1" t="s">
         <v>359</v>
@@ -16842,7 +16839,7 @@
         <v>1021</v>
       </c>
       <c r="V149" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W149" s="1" t="s">
         <v>361</v>
@@ -16896,7 +16893,7 @@
         <v>1019</v>
       </c>
       <c r="V150" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W150" s="1" t="s">
         <v>364</v>
@@ -16944,7 +16941,7 @@
       <c r="T151" s="1"/>
       <c r="U151" s="1"/>
       <c r="V151" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W151" s="1" t="s">
         <v>366</v>
@@ -16994,7 +16991,7 @@
       <c r="T152" s="1"/>
       <c r="U152" s="1"/>
       <c r="V152" s="1">
-        <v>266</v>
+        <v>2</v>
       </c>
       <c r="W152" s="1" t="s">
         <v>368</v>
@@ -17042,7 +17039,7 @@
       <c r="T153" s="1"/>
       <c r="U153" s="1"/>
       <c r="V153" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W153" s="1" t="s">
         <v>370</v>
@@ -17092,7 +17089,7 @@
       <c r="T154" s="1"/>
       <c r="U154" s="1"/>
       <c r="V154" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W154" s="1" t="s">
         <v>372</v>
@@ -17142,8 +17139,7 @@
       <c r="T155" s="1"/>
       <c r="U155" s="1"/>
       <c r="V155" s="1">
-        <f>600/3</f>
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W155" s="1" t="s">
         <v>374</v>
@@ -17195,7 +17191,7 @@
       <c r="T156" s="1"/>
       <c r="U156" s="1"/>
       <c r="V156" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W156" s="1" t="s">
         <v>377</v>
@@ -17245,7 +17241,7 @@
         <v>1021</v>
       </c>
       <c r="V157" s="1">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="W157" s="1" t="s">
         <v>379</v>
@@ -17291,7 +17287,7 @@
       <c r="T158" s="1"/>
       <c r="U158" s="1"/>
       <c r="V158" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W158" s="1" t="s">
         <v>381</v>
@@ -17341,7 +17337,7 @@
       <c r="T159" s="1"/>
       <c r="U159" s="1"/>
       <c r="V159" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W159" s="1" t="s">
         <v>383</v>
@@ -17391,7 +17387,7 @@
       <c r="T160" s="1"/>
       <c r="U160" s="1"/>
       <c r="V160" s="1">
-        <v>160</v>
+        <v>1</v>
       </c>
       <c r="W160" s="1" t="s">
         <v>385</v>
@@ -17443,7 +17439,7 @@
       <c r="T161" s="1"/>
       <c r="U161" s="1"/>
       <c r="V161" s="1">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="W161" s="1" t="s">
         <v>387</v>
@@ -17493,7 +17489,7 @@
       <c r="T162" s="1"/>
       <c r="U162" s="1"/>
       <c r="V162" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W162" s="1" t="s">
         <v>389</v>
@@ -17545,7 +17541,7 @@
       <c r="T163" s="1"/>
       <c r="U163" s="1"/>
       <c r="V163" s="1">
-        <v>555</v>
+        <v>5</v>
       </c>
       <c r="W163" s="1" t="s">
         <v>392</v>
@@ -17595,7 +17591,7 @@
       <c r="T164" s="1"/>
       <c r="U164" s="1"/>
       <c r="V164" s="1">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="W164" s="1" t="s">
         <v>394</v>
@@ -17645,7 +17641,7 @@
       <c r="T165" s="1"/>
       <c r="U165" s="1"/>
       <c r="V165" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W165" s="1" t="s">
         <v>396</v>
@@ -17695,7 +17691,7 @@
       <c r="T166" s="1"/>
       <c r="U166" s="1"/>
       <c r="V166" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W166" s="1" t="s">
         <v>398</v>
@@ -17747,7 +17743,7 @@
       <c r="T167" s="1"/>
       <c r="U167" s="1"/>
       <c r="V167" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W167" s="1" t="s">
         <v>400</v>
@@ -17795,7 +17791,7 @@
       <c r="T168" s="1"/>
       <c r="U168" s="1"/>
       <c r="V168" s="1">
-        <v>4000</v>
+        <v>40</v>
       </c>
       <c r="W168" s="1" t="s">
         <v>402</v>
@@ -17847,7 +17843,7 @@
       <c r="T169" s="1"/>
       <c r="U169" s="1"/>
       <c r="V169" s="1">
-        <v>333</v>
+        <v>3</v>
       </c>
       <c r="W169" s="1" t="s">
         <v>405</v>
@@ -17903,7 +17899,7 @@
       </c>
       <c r="U170" s="10"/>
       <c r="V170" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W170" s="1" t="s">
         <v>407</v>
@@ -17951,7 +17947,7 @@
       <c r="T171" s="1"/>
       <c r="U171" s="1"/>
       <c r="V171" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W171" s="1" t="s">
         <v>409</v>
@@ -17999,7 +17995,7 @@
       <c r="T172" s="1"/>
       <c r="U172" s="1"/>
       <c r="V172" s="1">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="W172" s="1" t="s">
         <v>411</v>
@@ -18049,7 +18045,7 @@
       <c r="T173" s="1"/>
       <c r="U173" s="1"/>
       <c r="V173" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W173" s="1" t="s">
         <v>413</v>
@@ -18097,7 +18093,7 @@
       <c r="T174" s="1"/>
       <c r="U174" s="1"/>
       <c r="V174" s="1">
-        <v>-1200</v>
+        <v>-12</v>
       </c>
       <c r="W174" s="1" t="s">
         <v>1218</v>
@@ -18145,7 +18141,7 @@
       <c r="T175" s="1"/>
       <c r="U175" s="1"/>
       <c r="V175" s="1">
-        <v>-36</v>
+        <v>-1</v>
       </c>
       <c r="W175" s="1" t="s">
         <v>415</v>
@@ -18197,7 +18193,7 @@
       <c r="T176" s="1"/>
       <c r="U176" s="1"/>
       <c r="V176" s="1">
-        <v>2000</v>
+        <v>20</v>
       </c>
       <c r="W176" s="1" t="s">
         <v>417</v>
@@ -18247,7 +18243,7 @@
       <c r="T177" s="1"/>
       <c r="U177" s="1"/>
       <c r="V177" s="1">
-        <v>175</v>
+        <v>1</v>
       </c>
       <c r="W177" s="1" t="s">
         <v>419</v>
@@ -18299,7 +18295,7 @@
       <c r="T178" s="1"/>
       <c r="U178" s="1"/>
       <c r="V178" s="1">
-        <v>2222</v>
+        <v>22</v>
       </c>
       <c r="W178" s="1" t="s">
         <v>422</v>
@@ -18349,7 +18345,7 @@
       <c r="T179" s="1"/>
       <c r="U179" s="1"/>
       <c r="V179" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W179" s="1" t="s">
         <v>424</v>
@@ -18399,7 +18395,7 @@
       <c r="T180" s="1"/>
       <c r="U180" s="1"/>
       <c r="V180" s="1">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="W180" s="1" t="s">
         <v>426</v>
@@ -18449,7 +18445,7 @@
         <v>1021</v>
       </c>
       <c r="V181" s="1">
-        <v>166</v>
+        <v>1</v>
       </c>
       <c r="W181" s="1" t="s">
         <v>428</v>
@@ -18497,7 +18493,7 @@
       <c r="T182" s="1"/>
       <c r="U182" s="1"/>
       <c r="V182" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W182" s="1" t="s">
         <v>430</v>
@@ -18545,7 +18541,7 @@
       <c r="T183" s="1"/>
       <c r="U183" s="1"/>
       <c r="V183" s="1">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="W183" s="1" t="s">
         <v>432</v>
@@ -18593,7 +18589,7 @@
       <c r="T184" s="1"/>
       <c r="U184" s="1"/>
       <c r="V184" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W184" s="1" t="s">
         <v>434</v>
@@ -18643,7 +18639,7 @@
         <v>1021</v>
       </c>
       <c r="V185" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W185" s="1" t="s">
         <v>436</v>
@@ -18689,7 +18685,7 @@
       <c r="T186" s="1"/>
       <c r="U186" s="1"/>
       <c r="V186" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W186" s="1" t="s">
         <v>438</v>
@@ -18737,7 +18733,7 @@
       <c r="T187" s="1"/>
       <c r="U187" s="1"/>
       <c r="V187" s="1">
-        <v>1400</v>
+        <v>14</v>
       </c>
       <c r="W187" s="1" t="s">
         <v>440</v>
@@ -18787,7 +18783,7 @@
         <v>1021</v>
       </c>
       <c r="V188" s="1">
-        <v>225</v>
+        <v>2</v>
       </c>
       <c r="W188" s="1" t="s">
         <v>442</v>
@@ -18837,7 +18833,7 @@
         <v>1021</v>
       </c>
       <c r="V189" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W189" s="1" t="s">
         <v>444</v>
@@ -18887,14 +18883,12 @@
       <c r="T190" s="1"/>
       <c r="U190" s="1"/>
       <c r="V190" s="1">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="W190" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="X190" s="53" t="s">
-        <v>1406</v>
-      </c>
+      <c r="X190" s="53"/>
     </row>
     <row r="191" spans="1:24" ht="48">
       <c r="A191">
@@ -18937,7 +18931,7 @@
       <c r="T191" s="1"/>
       <c r="U191" s="1"/>
       <c r="V191" s="1">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="W191" s="1" t="s">
         <v>448</v>
@@ -18985,7 +18979,7 @@
       <c r="T192" s="1"/>
       <c r="U192" s="1"/>
       <c r="V192" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W192" s="1" t="s">
         <v>450</v>
@@ -19035,7 +19029,7 @@
       <c r="T193" s="1"/>
       <c r="U193" s="1"/>
       <c r="V193" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W193" s="1" t="s">
         <v>452</v>
@@ -19085,7 +19079,7 @@
       <c r="T194" s="1"/>
       <c r="U194" s="1"/>
       <c r="V194" s="1">
-        <v>2500</v>
+        <v>25</v>
       </c>
       <c r="W194" s="1" t="s">
         <v>951</v>
@@ -19131,7 +19125,7 @@
       <c r="T195" s="1"/>
       <c r="U195" s="1"/>
       <c r="V195" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="W195" s="1" t="s">
         <v>454</v>
@@ -19181,7 +19175,7 @@
       <c r="T196" s="1"/>
       <c r="U196" s="1"/>
       <c r="V196" s="1">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="W196" s="1" t="s">
         <v>456</v>
@@ -19233,7 +19227,7 @@
       <c r="T197" s="1"/>
       <c r="U197" s="1"/>
       <c r="V197" s="1">
-        <v>666</v>
+        <v>6</v>
       </c>
       <c r="W197" s="1" t="s">
         <v>459</v>
@@ -19283,7 +19277,7 @@
         <v>1021</v>
       </c>
       <c r="V198" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="W198" s="1" t="s">
         <v>461</v>
@@ -19333,7 +19327,7 @@
       <c r="T199" s="1"/>
       <c r="U199" s="1"/>
       <c r="V199" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W199" s="1" t="s">
         <v>464</v>
@@ -19383,7 +19377,7 @@
         <v>1021</v>
       </c>
       <c r="V200" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="W200" s="1" t="s">
         <v>466</v>
@@ -19431,7 +19425,7 @@
       <c r="T201" s="1"/>
       <c r="U201" s="1"/>
       <c r="V201" s="1">
-        <v>1500</v>
+        <v>15</v>
       </c>
       <c r="W201" s="1" t="s">
         <v>468</v>
@@ -19493,8 +19487,7 @@
         <v>1026</v>
       </c>
       <c r="V202" s="1">
-        <f>200*2</f>
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W202" s="1" t="s">
         <v>471</v>
@@ -19544,7 +19537,7 @@
       <c r="T203" s="1"/>
       <c r="U203" s="1"/>
       <c r="V203" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W203" s="1" t="s">
         <v>473</v>
@@ -19594,7 +19587,7 @@
       <c r="T204" s="1"/>
       <c r="U204" s="1"/>
       <c r="V204" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W204" s="1" t="s">
         <v>476</v>
@@ -19642,7 +19635,7 @@
       <c r="T205" s="1"/>
       <c r="U205" s="1"/>
       <c r="V205" s="1">
-        <v>800</v>
+        <v>8</v>
       </c>
       <c r="W205" s="1" t="s">
         <v>479</v>
@@ -19690,7 +19683,7 @@
       <c r="T206" s="1"/>
       <c r="U206" s="1"/>
       <c r="V206" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W206" s="1" t="s">
         <v>482</v>
@@ -19740,7 +19733,7 @@
       <c r="T207" s="1"/>
       <c r="U207" s="1"/>
       <c r="V207" s="1">
-        <v>120</v>
+        <v>1</v>
       </c>
       <c r="W207" s="1" t="s">
         <v>484</v>
@@ -19788,7 +19781,7 @@
       <c r="T208" s="1"/>
       <c r="U208" s="1"/>
       <c r="V208" s="1">
-        <v>1200</v>
+        <v>12</v>
       </c>
       <c r="W208" s="1" t="s">
         <v>950</v>
@@ -19838,7 +19831,7 @@
       <c r="T209" s="1"/>
       <c r="U209" s="1"/>
       <c r="V209" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W209" s="1" t="s">
         <v>486</v>
@@ -19888,7 +19881,7 @@
       <c r="T210" s="1"/>
       <c r="U210" s="1"/>
       <c r="V210" s="1">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="W210" s="1" t="s">
         <v>488</v>
@@ -19938,7 +19931,7 @@
       <c r="T211" s="1"/>
       <c r="U211" s="1"/>
       <c r="V211" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W211" s="1" t="s">
         <v>490</v>
@@ -19988,7 +19981,7 @@
       <c r="T212" s="1"/>
       <c r="U212" s="1"/>
       <c r="V212" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W212" s="1" t="s">
         <v>492</v>
@@ -20038,7 +20031,7 @@
       <c r="T213" s="1"/>
       <c r="U213" s="1"/>
       <c r="V213" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W213" s="1" t="s">
         <v>494</v>
@@ -20088,7 +20081,7 @@
       <c r="T214" s="1"/>
       <c r="U214" s="1"/>
       <c r="V214" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W214" s="1" t="s">
         <v>673</v>
@@ -20136,7 +20129,7 @@
       <c r="T215" s="1"/>
       <c r="U215" s="1"/>
       <c r="V215" s="1">
-        <v>180</v>
+        <v>1</v>
       </c>
       <c r="W215" s="1" t="s">
         <v>496</v>
@@ -20186,7 +20179,7 @@
       <c r="T216" s="1"/>
       <c r="U216" s="1"/>
       <c r="V216" s="1">
-        <v>3000</v>
+        <v>30</v>
       </c>
       <c r="W216" s="1" t="s">
         <v>498</v>
@@ -20234,7 +20227,7 @@
       <c r="T217" s="1"/>
       <c r="U217" s="1"/>
       <c r="V217" s="1">
-        <v>-1800</v>
+        <v>-18</v>
       </c>
       <c r="W217" s="1" t="s">
         <v>500</v>
@@ -20282,7 +20275,7 @@
       <c r="T218" s="1"/>
       <c r="U218" s="1"/>
       <c r="V218" s="1">
-        <v>1500</v>
+        <v>15</v>
       </c>
       <c r="W218" s="1" t="s">
         <v>502</v>
@@ -20330,7 +20323,7 @@
       <c r="T219" s="1"/>
       <c r="U219" s="1"/>
       <c r="V219" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W219" s="1" t="s">
         <v>504</v>
@@ -20378,7 +20371,7 @@
       <c r="T220" s="1"/>
       <c r="U220" s="1"/>
       <c r="V220" s="1">
-        <v>-200</v>
+        <v>-2</v>
       </c>
       <c r="W220" s="1" t="s">
         <v>506</v>
@@ -20428,7 +20421,7 @@
       <c r="T221" s="1"/>
       <c r="U221" s="1"/>
       <c r="V221" s="1">
-        <v>333</v>
+        <v>3</v>
       </c>
       <c r="W221" s="1" t="s">
         <v>508</v>
@@ -20476,7 +20469,7 @@
       <c r="T222" s="1"/>
       <c r="U222" s="1"/>
       <c r="V222" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W222" s="1" t="s">
         <v>510</v>
@@ -20524,7 +20517,7 @@
       <c r="T223" s="1"/>
       <c r="U223" s="1"/>
       <c r="V223" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W223" s="1" t="s">
         <v>512</v>
@@ -20618,7 +20611,7 @@
       <c r="T225" s="1"/>
       <c r="U225" s="1"/>
       <c r="V225" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W225" s="1" t="s">
         <v>517</v>
@@ -20666,7 +20659,7 @@
       <c r="T226" s="1"/>
       <c r="U226" s="1"/>
       <c r="V226" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W226" s="1" t="s">
         <v>519</v>
@@ -20728,8 +20721,7 @@
         <v>1026</v>
       </c>
       <c r="V227" s="1">
-        <f>2000*1.5*2/12</f>
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W227" s="1" t="s">
         <v>521</v>
@@ -20779,8 +20771,7 @@
       <c r="T228" s="1"/>
       <c r="U228" s="1"/>
       <c r="V228" s="1">
-        <f>100*0.3</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W228" s="1" t="s">
         <v>523</v>
@@ -20830,7 +20821,7 @@
       <c r="T229" s="1"/>
       <c r="U229" s="1"/>
       <c r="V229" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W229" s="1" t="s">
         <v>525</v>
@@ -20878,7 +20869,7 @@
       <c r="T230" s="1"/>
       <c r="U230" s="1"/>
       <c r="V230" s="1">
-        <v>222</v>
+        <v>2</v>
       </c>
       <c r="W230" s="1" t="s">
         <v>527</v>
@@ -20940,7 +20931,7 @@
         <v>1026</v>
       </c>
       <c r="V231" s="1">
-        <v>280</v>
+        <v>2</v>
       </c>
       <c r="W231" s="1" t="s">
         <v>529</v>
@@ -20988,7 +20979,7 @@
       <c r="T232" s="1"/>
       <c r="U232" s="1"/>
       <c r="V232" s="1">
-        <v>450</v>
+        <v>4</v>
       </c>
       <c r="W232" s="1" t="s">
         <v>531</v>
@@ -21038,7 +21029,7 @@
       <c r="T233" s="1"/>
       <c r="U233" s="1"/>
       <c r="V233" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W233" s="1" t="s">
         <v>533</v>
@@ -21088,7 +21079,7 @@
       <c r="T234" s="1"/>
       <c r="U234" s="1"/>
       <c r="V234" s="1">
-        <v>132</v>
+        <v>1</v>
       </c>
       <c r="W234" s="1" t="s">
         <v>535</v>
@@ -21140,7 +21131,7 @@
       <c r="T235" s="1"/>
       <c r="U235" s="1"/>
       <c r="V235" s="1">
-        <v>800</v>
+        <v>8</v>
       </c>
       <c r="W235" s="1" t="s">
         <v>537</v>
@@ -21190,7 +21181,7 @@
       <c r="T236" s="1"/>
       <c r="U236" s="1"/>
       <c r="V236" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W236" s="1" t="s">
         <v>539</v>
@@ -21238,7 +21229,7 @@
       <c r="T237" s="1"/>
       <c r="U237" s="1"/>
       <c r="V237" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W237" s="1" t="s">
         <v>541</v>
@@ -21286,7 +21277,7 @@
       <c r="T238" s="1"/>
       <c r="U238" s="1"/>
       <c r="V238" s="31">
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="W238" s="1" t="s">
         <v>543</v>
@@ -21336,7 +21327,7 @@
       <c r="T239" s="1"/>
       <c r="U239" s="1"/>
       <c r="V239" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W239" s="1" t="s">
         <v>545</v>
@@ -21386,7 +21377,7 @@
       <c r="T240" s="1"/>
       <c r="U240" s="1"/>
       <c r="V240" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W240" s="1" t="s">
         <v>547</v>
@@ -21434,7 +21425,7 @@
       <c r="T241" s="1"/>
       <c r="U241" s="1"/>
       <c r="V241" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W241" s="1" t="s">
         <v>549</v>
@@ -21482,7 +21473,7 @@
       <c r="T242" s="1"/>
       <c r="U242" s="1"/>
       <c r="V242" s="31">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W242" s="1" t="s">
         <v>551</v>
@@ -21528,7 +21519,7 @@
       <c r="T243" s="1"/>
       <c r="U243" s="1"/>
       <c r="V243" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W243" s="1" t="s">
         <v>553</v>
@@ -21580,7 +21571,7 @@
       <c r="T244" s="1"/>
       <c r="U244" s="1"/>
       <c r="V244" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W244" s="1" t="s">
         <v>555</v>
@@ -21628,7 +21619,7 @@
       <c r="T245" s="1"/>
       <c r="U245" s="1"/>
       <c r="V245" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W245" s="1" t="s">
         <v>557</v>
@@ -21680,7 +21671,7 @@
       <c r="T246" s="1"/>
       <c r="U246" s="1"/>
       <c r="V246" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W246" s="1" t="s">
         <v>559</v>
@@ -21738,7 +21729,7 @@
       </c>
       <c r="U247" s="10"/>
       <c r="V247" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W247" s="1" t="s">
         <v>561</v>
@@ -21786,7 +21777,7 @@
       <c r="T248" s="1"/>
       <c r="U248" s="1"/>
       <c r="V248" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W248" s="1" t="s">
         <v>563</v>
@@ -21834,7 +21825,7 @@
       <c r="T249" s="1"/>
       <c r="U249" s="1"/>
       <c r="V249" s="1">
-        <v>2200</v>
+        <v>22</v>
       </c>
       <c r="W249" s="1" t="s">
         <v>565</v>
@@ -21886,7 +21877,7 @@
       <c r="T250" s="1"/>
       <c r="U250" s="1"/>
       <c r="V250" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W250" s="1" t="s">
         <v>569</v>
@@ -21936,7 +21927,7 @@
       <c r="T251" s="1"/>
       <c r="U251" s="1"/>
       <c r="V251" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W251" s="1" t="s">
         <v>571</v>
@@ -21984,7 +21975,7 @@
       <c r="T252" s="1"/>
       <c r="U252" s="1"/>
       <c r="V252" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W252" s="1" t="s">
         <v>574</v>
@@ -22032,7 +22023,7 @@
       <c r="T253" s="1"/>
       <c r="U253" s="1"/>
       <c r="V253" s="1">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="W253" s="1" t="s">
         <v>576</v>
@@ -22082,7 +22073,7 @@
       <c r="T254" s="1"/>
       <c r="U254" s="1"/>
       <c r="V254" s="1">
-        <v>2500</v>
+        <v>25</v>
       </c>
       <c r="W254" s="1" t="s">
         <v>579</v>
@@ -22130,7 +22121,7 @@
       <c r="T255" s="1"/>
       <c r="U255" s="1"/>
       <c r="V255" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W255" s="1" t="s">
         <v>582</v>
@@ -22178,7 +22169,7 @@
       <c r="T256" s="1"/>
       <c r="U256" s="1"/>
       <c r="V256" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W256" s="1" t="s">
         <v>585</v>
@@ -22228,7 +22219,7 @@
         <v>1021</v>
       </c>
       <c r="V257" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="W257" s="1" t="s">
         <v>587</v>
@@ -22278,7 +22269,7 @@
       <c r="T258" s="1"/>
       <c r="U258" s="1"/>
       <c r="V258" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W258" s="1" t="s">
         <v>589</v>
@@ -22326,7 +22317,7 @@
       <c r="T259" s="1"/>
       <c r="U259" s="1"/>
       <c r="V259" s="1">
-        <v>2500</v>
+        <v>25</v>
       </c>
       <c r="W259" s="1" t="s">
         <v>591</v>
@@ -22374,7 +22365,7 @@
       <c r="T260" s="1"/>
       <c r="U260" s="1"/>
       <c r="V260" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W260" s="1" t="s">
         <v>593</v>
@@ -22422,7 +22413,7 @@
       <c r="T261" s="1"/>
       <c r="U261" s="1"/>
       <c r="V261" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W261" s="1" t="s">
         <v>595</v>
@@ -22472,7 +22463,7 @@
       <c r="T262" s="1"/>
       <c r="U262" s="1"/>
       <c r="V262" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W262" s="1" t="s">
         <v>597</v>
@@ -22522,7 +22513,7 @@
       <c r="T263" s="1"/>
       <c r="U263" s="1"/>
       <c r="V263" s="1">
-        <v>3000</v>
+        <v>30</v>
       </c>
       <c r="W263" s="1" t="s">
         <v>599</v>
@@ -22570,7 +22561,7 @@
       <c r="T264" s="1"/>
       <c r="U264" s="1"/>
       <c r="V264" s="1">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="W264" s="1" t="s">
         <v>601</v>
@@ -22618,7 +22609,7 @@
       <c r="T265" s="1"/>
       <c r="U265" s="1"/>
       <c r="V265" s="1">
-        <v>900</v>
+        <v>9</v>
       </c>
       <c r="W265" s="1" t="s">
         <v>603</v>
@@ -22666,7 +22657,7 @@
       <c r="T266" s="1"/>
       <c r="U266" s="1"/>
       <c r="V266" s="1">
-        <v>800</v>
+        <v>8</v>
       </c>
       <c r="W266" s="1" t="s">
         <v>605</v>
@@ -22714,7 +22705,7 @@
       <c r="T267" s="1"/>
       <c r="U267" s="1"/>
       <c r="V267" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W267" s="1" t="s">
         <v>607</v>
@@ -22762,7 +22753,7 @@
       <c r="T268" s="1"/>
       <c r="U268" s="1"/>
       <c r="V268" s="1">
-        <v>1500</v>
+        <v>15</v>
       </c>
       <c r="W268" s="1" t="s">
         <v>609</v>
@@ -22820,7 +22811,7 @@
       </c>
       <c r="U269" s="1"/>
       <c r="V269" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W269" s="1" t="s">
         <v>611</v>
@@ -22872,7 +22863,7 @@
       <c r="T270" s="1"/>
       <c r="U270" s="1"/>
       <c r="V270" s="1">
-        <v>666</v>
+        <v>6</v>
       </c>
       <c r="W270" s="1" t="s">
         <v>613</v>
@@ -22922,7 +22913,7 @@
         <v>1021</v>
       </c>
       <c r="V271" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W271" s="1" t="s">
         <v>615</v>
@@ -22968,7 +22959,7 @@
       <c r="T272" s="1"/>
       <c r="U272" s="1"/>
       <c r="V272" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W272" s="1" t="s">
         <v>617</v>
@@ -23018,7 +23009,7 @@
         <v>1021</v>
       </c>
       <c r="V273" s="1">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="W273" s="1" t="s">
         <v>619</v>
@@ -23068,7 +23059,7 @@
       <c r="T274" s="1"/>
       <c r="U274" s="1"/>
       <c r="V274" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W274" s="1" t="s">
         <v>622</v>
@@ -23124,7 +23115,7 @@
       </c>
       <c r="U275" s="1"/>
       <c r="V275" s="1">
-        <v>800</v>
+        <v>8</v>
       </c>
       <c r="W275" s="1" t="s">
         <v>623</v>
@@ -23172,7 +23163,7 @@
       <c r="T276" s="1"/>
       <c r="U276" s="1"/>
       <c r="V276" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W276" s="1" t="s">
         <v>625</v>
@@ -23220,7 +23211,7 @@
       <c r="T277" s="1"/>
       <c r="U277" s="1"/>
       <c r="V277" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W277" s="1" t="s">
         <v>627</v>
@@ -23272,7 +23263,7 @@
       <c r="T278" s="1"/>
       <c r="U278" s="1"/>
       <c r="V278" s="1">
-        <v>900</v>
+        <v>9</v>
       </c>
       <c r="W278" s="1" t="s">
         <v>629</v>
@@ -23320,7 +23311,7 @@
       <c r="T279" s="1"/>
       <c r="U279" s="1"/>
       <c r="V279" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W279" s="1" t="s">
         <v>631</v>
@@ -23382,8 +23373,7 @@
         <v>1026</v>
       </c>
       <c r="V280" s="1">
-        <f>600*3*2/12</f>
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W280" s="1" t="s">
         <v>633</v>
@@ -23429,7 +23419,7 @@
       <c r="T281" s="1"/>
       <c r="U281" s="1"/>
       <c r="V281" s="1">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W281" s="1" t="s">
         <v>635</v>
@@ -23477,7 +23467,7 @@
       <c r="T282" s="1"/>
       <c r="U282" s="1"/>
       <c r="V282" s="1">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="W282" s="1" t="s">
         <v>637</v>
@@ -23527,7 +23517,7 @@
       <c r="T283" s="1"/>
       <c r="U283" s="1"/>
       <c r="V283" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W283" s="1" t="s">
         <v>639</v>
@@ -23577,7 +23567,7 @@
       <c r="T284" s="1"/>
       <c r="U284" s="1"/>
       <c r="V284" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W284" s="1" t="s">
         <v>641</v>
@@ -23629,7 +23619,7 @@
       <c r="T285" s="1"/>
       <c r="U285" s="1"/>
       <c r="V285" s="1">
-        <v>333</v>
+        <v>3</v>
       </c>
       <c r="W285" s="1" t="s">
         <v>644</v>
@@ -23681,7 +23671,7 @@
       <c r="T286" s="1"/>
       <c r="U286" s="1"/>
       <c r="V286" s="1">
-        <v>6000</v>
+        <v>60</v>
       </c>
       <c r="W286" s="31" t="s">
         <v>1424</v>
@@ -23743,8 +23733,7 @@
         <v>1026</v>
       </c>
       <c r="V287" s="1">
-        <f>1000*3*2/12</f>
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W287" s="1" t="s">
         <v>646</v>
@@ -23806,7 +23795,7 @@
         <v>1026</v>
       </c>
       <c r="V288" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
       <c r="W288" s="1" t="s">
         <v>648</v>
@@ -23868,7 +23857,7 @@
         <v>1026</v>
       </c>
       <c r="V289" s="1">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="W289" s="1" t="s">
         <v>650</v>
@@ -23928,7 +23917,7 @@
         <v>1026</v>
       </c>
       <c r="V290" s="1">
-        <v>833</v>
+        <v>8</v>
       </c>
       <c r="W290" s="1" t="s">
         <v>652</v>
@@ -23990,8 +23979,7 @@
         <v>1026</v>
       </c>
       <c r="V291" s="1">
-        <f>1400*3*2/12</f>
-        <v>700</v>
+        <v>7</v>
       </c>
       <c r="W291" s="1" t="s">
         <v>654</v>
@@ -24053,8 +24041,7 @@
         <v>1026</v>
       </c>
       <c r="V292" s="1">
-        <f>1200*3*2/12</f>
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W292" s="1" t="s">
         <v>656</v>
@@ -24116,8 +24103,7 @@
         <v>1026</v>
       </c>
       <c r="V293" s="1">
-        <f>240*2</f>
-        <v>480</v>
+        <v>4</v>
       </c>
       <c r="W293" s="1" t="s">
         <v>658</v>
@@ -24179,8 +24165,7 @@
         <v>1026</v>
       </c>
       <c r="V294" s="1">
-        <f>300*2</f>
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W294" s="1" t="s">
         <v>660</v>
@@ -24228,7 +24213,7 @@
       <c r="T295" s="1"/>
       <c r="U295" s="1"/>
       <c r="V295" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="W295" s="1" t="s">
         <v>662</v>
@@ -24276,7 +24261,7 @@
       <c r="T296" s="1"/>
       <c r="U296" s="1"/>
       <c r="V296" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="W296" s="1" t="s">
         <v>664</v>
@@ -24338,8 +24323,7 @@
         <v>1026</v>
       </c>
       <c r="V297" s="1">
-        <f>300*5*2/12</f>
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="W297" s="1" t="s">
         <v>666</v>
@@ -24395,7 +24379,7 @@
       </c>
       <c r="U298" s="10"/>
       <c r="V298" s="1">
-        <v>1500</v>
+        <v>15</v>
       </c>
       <c r="W298" s="1" t="s">
         <v>668</v>
@@ -24447,7 +24431,7 @@
         <v>1020</v>
       </c>
       <c r="V299" s="1">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="W299" s="1" t="s">
         <v>1004</v>
@@ -24497,7 +24481,7 @@
       <c r="T300" s="1"/>
       <c r="U300" s="1"/>
       <c r="V300" s="1">
-        <v>800</v>
+        <v>8</v>
       </c>
       <c r="W300" s="1" t="s">
         <v>1174</v>
@@ -24553,7 +24537,7 @@
       </c>
       <c r="U301" s="36"/>
       <c r="V301" s="36">
-        <v>400</v>
+        <v>4</v>
       </c>
       <c r="W301" s="1" t="s">
         <v>1229</v>
@@ -24609,7 +24593,7 @@
       </c>
       <c r="U302" s="36"/>
       <c r="V302" s="36">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="W302" s="1" t="s">
         <v>1231</v>
@@ -24657,7 +24641,7 @@
       <c r="T303" s="1"/>
       <c r="U303" s="1"/>
       <c r="V303" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="W303" s="1" t="s">
         <v>130</v>
@@ -24682,10 +24666,10 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1:F3"/>
+      <selection pane="bottomRight" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -24965,7 +24949,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1">
-        <v>-44</v>
+        <v>0</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>675</v>
@@ -25013,7 +24997,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>675</v>
@@ -25038,10 +25022,10 @@
   <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="K4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1:F3"/>
+      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -25323,7 +25307,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>45</v>
@@ -25373,7 +25357,7 @@
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>47</v>
@@ -25423,7 +25407,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>49</v>
@@ -25473,7 +25457,7 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>51</v>
@@ -25523,7 +25507,7 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>53</v>
@@ -25573,7 +25557,7 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>55</v>
@@ -25623,7 +25607,7 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>57</v>
@@ -25673,7 +25657,7 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>59</v>
@@ -25723,7 +25707,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W12" s="1" t="s">
         <v>114</v>
@@ -25773,7 +25757,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>116</v>
@@ -25823,7 +25807,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>118</v>
@@ -25873,7 +25857,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W15" s="1" t="s">
         <v>120</v>
@@ -25923,7 +25907,7 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W16" s="1" t="s">
         <v>122</v>
@@ -25973,7 +25957,7 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>124</v>
@@ -26023,7 +26007,7 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>126</v>
@@ -26073,7 +26057,7 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="W19" s="1" t="s">
         <v>128</v>
@@ -26097,8 +26081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
close #25 now there is no ice and thunder
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5448,10 +5448,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>击中目标后对1.5卡片距离敌人造成30%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>s.Summon(5,51013000);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -5581,6 +5577,10 @@
   </si>
   <si>
     <t>对方下一张怪物卡消耗+5（一回合有效）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合对1.5卡片距离敌人造成30%伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9435,10 +9435,10 @@
   <dimension ref="A1:X304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="P68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="E303" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W41" sqref="W41"/>
+      <selection pane="bottomRight" activeCell="Q304" sqref="Q304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -11854,7 +11854,7 @@
         <v>55000052</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>1</v>
@@ -11863,7 +11863,7 @@
       <c r="E48" s="1"/>
       <c r="F48" s="67"/>
       <c r="G48" s="33" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="H48" s="33"/>
       <c r="I48" s="32"/>
@@ -11879,7 +11879,7 @@
         <v>684</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="R48" s="1">
         <v>0</v>
@@ -11891,7 +11891,7 @@
         <v>25</v>
       </c>
       <c r="W48" s="1" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="X48" s="53"/>
     </row>
@@ -14658,16 +14658,16 @@
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="E104" s="1">
         <v>20</v>
       </c>
       <c r="F104" s="67" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="G104" s="33" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="H104" s="33"/>
       <c r="I104" s="32"/>
@@ -14683,7 +14683,7 @@
         <v>684</v>
       </c>
       <c r="Q104" s="10" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="R104" s="10">
         <v>0</v>
@@ -14698,7 +14698,7 @@
         <v>258</v>
       </c>
       <c r="X104" s="53" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="105" spans="1:24" ht="60">
@@ -15202,7 +15202,7 @@
         <v>55000127</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>1</v>
@@ -15211,7 +15211,7 @@
       <c r="E115" s="1"/>
       <c r="F115" s="67"/>
       <c r="G115" s="33" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="H115" s="33"/>
       <c r="I115" s="32"/>
@@ -15227,7 +15227,7 @@
         <v>684</v>
       </c>
       <c r="Q115" s="10" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="R115" s="10">
         <v>0</v>
@@ -15239,7 +15239,7 @@
         <v>80</v>
       </c>
       <c r="W115" s="1" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="X115" s="53"/>
     </row>
@@ -15455,7 +15455,7 @@
         <v>1457</v>
       </c>
       <c r="G120" s="33" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="H120" s="33"/>
       <c r="I120" s="29"/>
@@ -15496,7 +15496,7 @@
         <v>55000134</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>104</v>
@@ -15505,10 +15505,10 @@
       <c r="E121" s="1"/>
       <c r="F121" s="67"/>
       <c r="G121" s="33" t="s">
+        <v>1501</v>
+      </c>
+      <c r="H121" s="33" t="s">
         <v>1502</v>
-      </c>
-      <c r="H121" s="33" t="s">
-        <v>1503</v>
       </c>
       <c r="I121" s="32"/>
       <c r="J121" s="18"/>
@@ -17676,7 +17676,7 @@
         <v>55000178</v>
       </c>
       <c r="B165" s="11" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>104</v>
@@ -17685,10 +17685,10 @@
       <c r="E165" s="1"/>
       <c r="F165" s="67"/>
       <c r="G165" s="33" t="s">
+        <v>1489</v>
+      </c>
+      <c r="H165" s="33" t="s">
         <v>1490</v>
-      </c>
-      <c r="H165" s="33" t="s">
-        <v>1491</v>
       </c>
       <c r="I165" s="32"/>
       <c r="J165" s="18"/>
@@ -17726,7 +17726,7 @@
         <v>55000179</v>
       </c>
       <c r="B166" s="11" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>104</v>
@@ -17735,10 +17735,10 @@
       <c r="E166" s="1"/>
       <c r="F166" s="67"/>
       <c r="G166" s="33" t="s">
+        <v>1492</v>
+      </c>
+      <c r="H166" s="33" t="s">
         <v>1493</v>
-      </c>
-      <c r="H166" s="33" t="s">
-        <v>1494</v>
       </c>
       <c r="I166" s="32"/>
       <c r="J166" s="18"/>
@@ -19824,16 +19824,16 @@
         <v>1</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="E208" s="1">
         <v>10</v>
       </c>
       <c r="F208" s="67" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="G208" s="33" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="H208" s="33"/>
       <c r="I208" s="32"/>
@@ -19849,7 +19849,7 @@
         <v>684</v>
       </c>
       <c r="Q208" s="10" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="R208" s="10">
         <v>0</v>
@@ -20020,7 +20020,7 @@
         <v>55000225</v>
       </c>
       <c r="B212" s="11" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>104</v>
@@ -20029,10 +20029,10 @@
       <c r="E212" s="1"/>
       <c r="F212" s="67"/>
       <c r="G212" s="33" t="s">
+        <v>1495</v>
+      </c>
+      <c r="H212" s="33" t="s">
         <v>1496</v>
-      </c>
-      <c r="H212" s="33" t="s">
-        <v>1497</v>
       </c>
       <c r="I212" s="32"/>
       <c r="J212" s="18"/>
@@ -20070,7 +20070,7 @@
         <v>55000226</v>
       </c>
       <c r="B213" s="11" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>104</v>
@@ -20079,10 +20079,10 @@
       <c r="E213" s="1"/>
       <c r="F213" s="67"/>
       <c r="G213" s="33" t="s">
+        <v>1498</v>
+      </c>
+      <c r="H213" s="33" t="s">
         <v>1499</v>
-      </c>
-      <c r="H213" s="33" t="s">
-        <v>1500</v>
       </c>
       <c r="I213" s="32"/>
       <c r="J213" s="18"/>
@@ -24759,7 +24759,7 @@
         <v>684</v>
       </c>
       <c r="Q304" s="16" t="s">
-        <v>1474</v>
+        <v>1507</v>
       </c>
       <c r="R304" s="28">
         <v>0</v>

</xml_diff>

<commit_message>
finish new card magic misiile
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5466,140 +5466,140 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>刚印</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对野兽造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对恶魔造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对龙族造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对机械造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对爬行造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>净化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>驱逐</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsRace("Devil")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsRace("Machine")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsRace("Bird")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对鸟类造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>惊弓</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinggong</t>
+  </si>
+  <si>
+    <t>d.IsRace("Goblin")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsRace("Totem")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对地精造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对图腾造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yanwu</t>
+  </si>
+  <si>
+    <t>烟雾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhendang</t>
+  </si>
+  <si>
+    <t>震荡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkinvasion</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>水球</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>waterball2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NER</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>部署时对最近的3个敌人造成伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuiqiu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) s.Transform(mon.CardId);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>刚印</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对野兽造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对恶魔造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对龙族造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对机械造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对爬行造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>净化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>驱逐</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsRace("Devil")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsRace("Machine")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsRace("Bird")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对鸟类造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>惊弓</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>jinggong</t>
-  </si>
-  <si>
-    <t>d.IsRace("Goblin")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsRace("Totem")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对地精造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对图腾造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yanwu</t>
-  </si>
-  <si>
-    <t>烟雾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhendang</t>
-  </si>
-  <si>
-    <t>震荡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkinvasion</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>水球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>waterball2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NER</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>部署时对最近的3个敌人造成伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortRandom().Top(3)) s.AddMissile(mon, "waterball");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuiqiu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -10311,10 +10311,10 @@
   <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -10668,13 +10668,13 @@
         <v>55200002</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>197</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="E6" s="27">
         <v>30</v>
@@ -10683,7 +10683,7 @@
         <v>1396</v>
       </c>
       <c r="G6" s="69" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="H6" s="69"/>
       <c r="I6" s="28"/>
@@ -10699,13 +10699,13 @@
         <v>657</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="R6" s="27">
         <v>0</v>
       </c>
       <c r="S6" s="27" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="T6" s="27"/>
       <c r="U6" s="27"/>
@@ -10713,7 +10713,7 @@
         <v>15</v>
       </c>
       <c r="W6" s="27" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="X6" s="70"/>
     </row>
@@ -10995,7 +10995,7 @@
         <v>0</v>
       </c>
       <c r="S12" s="27" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
@@ -11012,7 +11012,7 @@
         <v>55300007</v>
       </c>
       <c r="B13" s="75" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>85</v>
@@ -11221,11 +11221,11 @@
       <c r="G17" s="69"/>
       <c r="H17" s="69"/>
       <c r="I17" s="28" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="J17" s="29"/>
       <c r="K17" s="34" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="21"/>
@@ -11237,7 +11237,7 @@
         <v>657</v>
       </c>
       <c r="Q17" s="16" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="R17" s="27">
         <v>0</v>
@@ -11269,11 +11269,11 @@
       <c r="G18" s="69"/>
       <c r="H18" s="69"/>
       <c r="I18" s="28" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="J18" s="29"/>
       <c r="K18" s="34" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="L18" s="17"/>
       <c r="M18" s="21"/>
@@ -11285,7 +11285,7 @@
         <v>657</v>
       </c>
       <c r="Q18" s="16" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="R18" s="27">
         <v>0</v>
@@ -11306,7 +11306,7 @@
         <v>55500003</v>
       </c>
       <c r="B19" s="78" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>6</v>
@@ -11417,7 +11417,7 @@
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="34" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="L21" s="17"/>
       <c r="M21" s="21"/>
@@ -11429,7 +11429,7 @@
         <v>657</v>
       </c>
       <c r="Q21" s="16" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="R21" s="52">
         <v>0</v>
@@ -11450,7 +11450,7 @@
         <v>55500006</v>
       </c>
       <c r="B22" s="78" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>6</v>
@@ -11461,11 +11461,11 @@
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
       <c r="I22" s="28" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="J22" s="29"/>
       <c r="K22" s="34" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="L22" s="17"/>
       <c r="M22" s="21"/>
@@ -11477,7 +11477,7 @@
         <v>657</v>
       </c>
       <c r="Q22" s="16" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="R22" s="52">
         <v>0</v>
@@ -11489,7 +11489,7 @@
         <v>5</v>
       </c>
       <c r="W22" s="27" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="X22" s="54"/>
     </row>
@@ -11513,7 +11513,7 @@
       </c>
       <c r="J23" s="29"/>
       <c r="K23" s="34" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="L23" s="17"/>
       <c r="M23" s="21"/>
@@ -11525,7 +11525,7 @@
         <v>657</v>
       </c>
       <c r="Q23" s="16" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="R23" s="52">
         <v>0</v>
@@ -11642,7 +11642,7 @@
         <v>55500010</v>
       </c>
       <c r="B26" s="78" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>6</v>
@@ -11705,7 +11705,7 @@
       </c>
       <c r="J27" s="29"/>
       <c r="K27" s="34" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="L27" s="17"/>
       <c r="M27" s="21"/>
@@ -11717,7 +11717,7 @@
         <v>657</v>
       </c>
       <c r="Q27" s="16" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="R27" s="52">
         <v>0</v>
@@ -11882,7 +11882,7 @@
         <v>55500015</v>
       </c>
       <c r="B31" s="78" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>6</v>
@@ -11893,7 +11893,7 @@
       <c r="G31" s="69"/>
       <c r="H31" s="69"/>
       <c r="I31" s="28" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="J31" s="29"/>
       <c r="K31" s="34" t="s">
@@ -11909,7 +11909,7 @@
         <v>657</v>
       </c>
       <c r="Q31" s="16" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="R31" s="27">
         <v>0</v>
@@ -11921,7 +11921,7 @@
         <v>5</v>
       </c>
       <c r="W31" s="27" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="X31" s="70"/>
     </row>
@@ -11930,7 +11930,7 @@
         <v>55500016</v>
       </c>
       <c r="B32" s="78" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>6</v>
@@ -11941,7 +11941,7 @@
       <c r="G32" s="69"/>
       <c r="H32" s="69"/>
       <c r="I32" s="28" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="J32" s="29"/>
       <c r="K32" s="34" t="s">
@@ -11957,7 +11957,7 @@
         <v>657</v>
       </c>
       <c r="Q32" s="16" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="R32" s="27">
         <v>0</v>
@@ -11969,7 +11969,7 @@
         <v>5</v>
       </c>
       <c r="W32" s="27" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="X32" s="70"/>
     </row>
@@ -11993,7 +11993,7 @@
         <v>1396</v>
       </c>
       <c r="G33" s="69" t="s">
-        <v>1446</v>
+        <v>1479</v>
       </c>
       <c r="H33" s="69"/>
       <c r="I33" s="28"/>

</xml_diff>

<commit_message>
#8 a new summon card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -438,7 +438,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3089" uniqueCount="1474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3097" uniqueCount="1478">
   <si>
     <t>特殊</t>
   </si>
@@ -4993,10 +4993,6 @@
     <t>s.Atk.Source*=1.15;</t>
   </si>
   <si>
-    <t>s.Summon(3,51000019);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>gebulin</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -5575,6 +5571,25 @@
   </si>
   <si>
     <t>猛砍</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在自己周围随机位置召唤一个光精灵射手</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>guangdian</t>
+  </si>
+  <si>
+    <t>光点</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(4,51000019);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(4,51000008);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9853,8 +9868,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:X38" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
-  <autoFilter ref="A3:X38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:X39" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
+  <autoFilter ref="A3:X39"/>
   <sortState ref="A4:X31">
     <sortCondition ref="A3:A31"/>
   </sortState>
@@ -10283,13 +10298,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10322,13 +10337,13 @@
         <v>651</v>
       </c>
       <c r="D1" s="67" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E1" s="67" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="F1" s="67" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>667</v>
@@ -10370,7 +10385,7 @@
         <v>930</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>949</v>
@@ -10396,13 +10411,13 @@
         <v>643</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>960</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>936</v>
@@ -10470,13 +10485,13 @@
         <v>646</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1107</v>
@@ -10518,7 +10533,7 @@
         <v>879</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>947</v>
@@ -10553,7 +10568,7 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="21" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="N4" s="59">
         <v>1</v>
@@ -10565,7 +10580,7 @@
         <v>656</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="R4" s="1">
         <v>0</v>
@@ -10601,7 +10616,7 @@
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="17" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="21"/>
@@ -10613,7 +10628,7 @@
         <v>656</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="R5" s="51">
         <v>0</v>
@@ -10649,7 +10664,7 @@
       </c>
       <c r="J6" s="18"/>
       <c r="K6" s="17" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="21"/>
@@ -10661,7 +10676,7 @@
         <v>656</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="R6" s="10">
         <v>0</v>
@@ -10682,7 +10697,7 @@
         <v>55100004</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>931</v>
@@ -10696,7 +10711,7 @@
       <c r="J7" s="18"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="M7" s="21"/>
       <c r="N7" s="59"/>
@@ -10707,7 +10722,7 @@
         <v>656</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="R7" s="10">
         <v>0</v>
@@ -10728,13 +10743,13 @@
         <v>55200001</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>197</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="E8" s="27">
         <v>15</v>
@@ -10747,7 +10762,7 @@
       <c r="K8" s="34"/>
       <c r="L8" s="17"/>
       <c r="M8" s="21" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="N8" s="59">
         <v>1</v>
@@ -10759,7 +10774,7 @@
         <v>656</v>
       </c>
       <c r="Q8" s="16" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="R8" s="27">
         <v>0</v>
@@ -10768,7 +10783,7 @@
         <v>856</v>
       </c>
       <c r="T8" s="27" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="U8" s="27" t="s">
         <v>957</v>
@@ -10777,7 +10792,7 @@
         <v>40</v>
       </c>
       <c r="W8" s="27" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="X8" s="70"/>
     </row>
@@ -10786,22 +10801,22 @@
         <v>55200002</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>197</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="E9" s="27">
         <v>30</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="G9" s="69" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="H9" s="69"/>
       <c r="I9" s="28"/>
@@ -10817,13 +10832,13 @@
         <v>656</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="R9" s="27">
         <v>0</v>
       </c>
       <c r="S9" s="27" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="T9" s="27"/>
       <c r="U9" s="27"/>
@@ -10831,7 +10846,7 @@
         <v>15</v>
       </c>
       <c r="W9" s="27" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="X9" s="70"/>
     </row>
@@ -10890,7 +10905,7 @@
         <v>55300002</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>85</v>
@@ -10899,10 +10914,10 @@
       <c r="E11" s="27"/>
       <c r="F11" s="66"/>
       <c r="G11" s="69" t="s">
+        <v>1407</v>
+      </c>
+      <c r="H11" s="69" t="s">
         <v>1408</v>
-      </c>
-      <c r="H11" s="69" t="s">
-        <v>1409</v>
       </c>
       <c r="I11" s="28"/>
       <c r="J11" s="29"/>
@@ -10917,7 +10932,7 @@
         <v>656</v>
       </c>
       <c r="Q11" s="16" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="R11" s="27">
         <v>0</v>
@@ -10938,7 +10953,7 @@
         <v>55300003</v>
       </c>
       <c r="B12" s="75" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>85</v>
@@ -10947,10 +10962,10 @@
       <c r="E12" s="27"/>
       <c r="F12" s="66"/>
       <c r="G12" s="32" t="s">
+        <v>1410</v>
+      </c>
+      <c r="H12" s="32" t="s">
         <v>1411</v>
-      </c>
-      <c r="H12" s="32" t="s">
-        <v>1412</v>
       </c>
       <c r="I12" s="28"/>
       <c r="J12" s="29"/>
@@ -10965,7 +10980,7 @@
         <v>656</v>
       </c>
       <c r="Q12" s="16" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="R12" s="27">
         <v>0</v>
@@ -10986,7 +11001,7 @@
         <v>55300004</v>
       </c>
       <c r="B13" s="75" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>85</v>
@@ -10995,10 +11010,10 @@
       <c r="E13" s="27"/>
       <c r="F13" s="66"/>
       <c r="G13" s="69" t="s">
+        <v>1413</v>
+      </c>
+      <c r="H13" s="69" t="s">
         <v>1414</v>
-      </c>
-      <c r="H13" s="69" t="s">
-        <v>1415</v>
       </c>
       <c r="I13" s="28"/>
       <c r="J13" s="29"/>
@@ -11034,7 +11049,7 @@
         <v>55300005</v>
       </c>
       <c r="B14" s="75" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>85</v>
@@ -11043,10 +11058,10 @@
       <c r="E14" s="27"/>
       <c r="F14" s="66"/>
       <c r="G14" s="69" t="s">
+        <v>1416</v>
+      </c>
+      <c r="H14" s="69" t="s">
         <v>1417</v>
-      </c>
-      <c r="H14" s="69" t="s">
-        <v>1418</v>
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="29"/>
@@ -11082,7 +11097,7 @@
         <v>55300006</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>0</v>
@@ -11091,7 +11106,7 @@
       <c r="E15" s="27"/>
       <c r="F15" s="66"/>
       <c r="G15" s="69" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="H15" s="69"/>
       <c r="I15" s="28"/>
@@ -11107,13 +11122,13 @@
         <v>656</v>
       </c>
       <c r="Q15" s="71" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="R15" s="27">
         <v>0</v>
       </c>
       <c r="S15" s="27" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="T15" s="27"/>
       <c r="U15" s="27"/>
@@ -11121,7 +11136,7 @@
         <v>25</v>
       </c>
       <c r="W15" s="27" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="X15" s="70"/>
     </row>
@@ -11130,7 +11145,7 @@
         <v>55300007</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>85</v>
@@ -11139,10 +11154,10 @@
       <c r="E16" s="27"/>
       <c r="F16" s="66"/>
       <c r="G16" s="69" t="s">
+        <v>1418</v>
+      </c>
+      <c r="H16" s="69" t="s">
         <v>1419</v>
-      </c>
-      <c r="H16" s="69" t="s">
-        <v>1420</v>
       </c>
       <c r="I16" s="28"/>
       <c r="J16" s="29"/>
@@ -11157,7 +11172,7 @@
         <v>656</v>
       </c>
       <c r="Q16" s="16" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="R16" s="27">
         <v>0</v>
@@ -11193,7 +11208,7 @@
       <c r="K17" s="34"/>
       <c r="L17" s="17"/>
       <c r="M17" s="21" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="N17" s="59">
         <v>1</v>
@@ -11205,7 +11220,7 @@
         <v>656</v>
       </c>
       <c r="Q17" s="16" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="R17" s="27">
         <v>0</v>
@@ -11221,7 +11236,7 @@
       </c>
       <c r="X17" s="70"/>
     </row>
-    <row r="18" spans="1:24" ht="36">
+    <row r="18" spans="1:24" ht="28.8">
       <c r="A18" s="76">
         <v>55400001</v>
       </c>
@@ -11241,7 +11256,7 @@
       <c r="K18" s="34"/>
       <c r="L18" s="17"/>
       <c r="M18" s="21" t="s">
-        <v>1324</v>
+        <v>1476</v>
       </c>
       <c r="N18" s="59">
         <v>2</v>
@@ -11267,7 +11282,7 @@
         <v>80</v>
       </c>
       <c r="W18" s="72" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="X18" s="70"/>
     </row>
@@ -11282,16 +11297,16 @@
         <v>0</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="E19" s="27">
         <v>10</v>
       </c>
       <c r="F19" s="66" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="G19" s="69" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="H19" s="69"/>
       <c r="I19" s="28"/>
@@ -11307,7 +11322,7 @@
         <v>656</v>
       </c>
       <c r="Q19" s="16" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="R19" s="27">
         <v>0</v>
@@ -11323,31 +11338,31 @@
       </c>
       <c r="X19" s="70"/>
     </row>
-    <row r="20" spans="1:24" ht="48">
-      <c r="A20" s="78">
-        <v>55500001</v>
-      </c>
-      <c r="B20" s="78" t="s">
-        <v>17</v>
+    <row r="20" spans="1:24" ht="28.8">
+      <c r="A20" s="76">
+        <v>55400003</v>
+      </c>
+      <c r="B20" s="76" t="s">
+        <v>1475</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>6</v>
+        <v>931</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
       <c r="F20" s="66"/>
       <c r="G20" s="69"/>
       <c r="H20" s="69"/>
-      <c r="I20" s="28" t="s">
-        <v>1444</v>
-      </c>
+      <c r="I20" s="28"/>
       <c r="J20" s="29"/>
-      <c r="K20" s="34" t="s">
-        <v>1434</v>
-      </c>
+      <c r="K20" s="34"/>
       <c r="L20" s="17"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="59"/>
+      <c r="M20" s="21" t="s">
+        <v>1477</v>
+      </c>
+      <c r="N20" s="59">
+        <v>2</v>
+      </c>
       <c r="O20" s="68" t="s">
         <v>661</v>
       </c>
@@ -11355,28 +11370,30 @@
         <v>656</v>
       </c>
       <c r="Q20" s="16" t="s">
-        <v>1435</v>
+        <v>1473</v>
       </c>
       <c r="R20" s="27">
         <v>0</v>
       </c>
-      <c r="S20" s="27"/>
+      <c r="S20" s="27" t="s">
+        <v>889</v>
+      </c>
       <c r="T20" s="27"/>
       <c r="U20" s="27"/>
       <c r="V20" s="27">
-        <v>5</v>
-      </c>
-      <c r="W20" s="27" t="s">
-        <v>18</v>
+        <v>80</v>
+      </c>
+      <c r="W20" s="72" t="s">
+        <v>1474</v>
       </c>
       <c r="X20" s="70"/>
     </row>
     <row r="21" spans="1:24" ht="48">
       <c r="A21" s="78">
-        <v>55500002</v>
+        <v>55500001</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>6</v>
@@ -11387,11 +11404,11 @@
       <c r="G21" s="69"/>
       <c r="H21" s="69"/>
       <c r="I21" s="28" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="34" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="L21" s="17"/>
       <c r="M21" s="21"/>
@@ -11403,7 +11420,7 @@
         <v>656</v>
       </c>
       <c r="Q21" s="16" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
       <c r="R21" s="27">
         <v>0</v>
@@ -11415,16 +11432,16 @@
         <v>5</v>
       </c>
       <c r="W21" s="27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="X21" s="70"/>
     </row>
     <row r="22" spans="1:24" ht="48">
       <c r="A22" s="78">
-        <v>55500003</v>
+        <v>55500002</v>
       </c>
       <c r="B22" s="78" t="s">
-        <v>1443</v>
+        <v>21</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>6</v>
@@ -11435,11 +11452,11 @@
       <c r="G22" s="69"/>
       <c r="H22" s="69"/>
       <c r="I22" s="28" t="s">
-        <v>685</v>
+        <v>1444</v>
       </c>
       <c r="J22" s="29"/>
       <c r="K22" s="34" t="s">
-        <v>703</v>
+        <v>1437</v>
       </c>
       <c r="L22" s="17"/>
       <c r="M22" s="21"/>
@@ -11451,7 +11468,7 @@
         <v>656</v>
       </c>
       <c r="Q22" s="16" t="s">
-        <v>672</v>
+        <v>1438</v>
       </c>
       <c r="R22" s="27">
         <v>0</v>
@@ -11463,16 +11480,16 @@
         <v>5</v>
       </c>
       <c r="W22" s="27" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="X22" s="70"/>
     </row>
     <row r="23" spans="1:24" ht="48">
       <c r="A23" s="78">
-        <v>55500004</v>
+        <v>55500003</v>
       </c>
       <c r="B23" s="78" t="s">
-        <v>362</v>
+        <v>1442</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>6</v>
@@ -11480,10 +11497,10 @@
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="66"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="28" t="s">
-        <v>700</v>
+        <v>685</v>
       </c>
       <c r="J23" s="29"/>
       <c r="K23" s="34" t="s">
@@ -11499,7 +11516,7 @@
         <v>656</v>
       </c>
       <c r="Q23" s="16" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="R23" s="27">
         <v>0</v>
@@ -11511,16 +11528,16 @@
         <v>5</v>
       </c>
       <c r="W23" s="27" t="s">
-        <v>363</v>
+        <v>13</v>
       </c>
       <c r="X23" s="70"/>
     </row>
     <row r="24" spans="1:24" ht="48">
       <c r="A24" s="78">
-        <v>55500005</v>
+        <v>55500004</v>
       </c>
       <c r="B24" s="78" t="s">
-        <v>19</v>
+        <v>362</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>6</v>
@@ -11531,11 +11548,11 @@
       <c r="G24" s="32"/>
       <c r="H24" s="32"/>
       <c r="I24" s="28" t="s">
-        <v>688</v>
+        <v>700</v>
       </c>
       <c r="J24" s="29"/>
       <c r="K24" s="34" t="s">
-        <v>1437</v>
+        <v>703</v>
       </c>
       <c r="L24" s="17"/>
       <c r="M24" s="21"/>
@@ -11547,9 +11564,9 @@
         <v>656</v>
       </c>
       <c r="Q24" s="16" t="s">
-        <v>1436</v>
-      </c>
-      <c r="R24" s="52">
+        <v>680</v>
+      </c>
+      <c r="R24" s="27">
         <v>0</v>
       </c>
       <c r="S24" s="27"/>
@@ -11559,16 +11576,16 @@
         <v>5</v>
       </c>
       <c r="W24" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="X24" s="54"/>
+        <v>363</v>
+      </c>
+      <c r="X24" s="70"/>
     </row>
     <row r="25" spans="1:24" ht="48">
       <c r="A25" s="78">
-        <v>55500006</v>
+        <v>55500005</v>
       </c>
       <c r="B25" s="78" t="s">
-        <v>1448</v>
+        <v>19</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>6</v>
@@ -11579,11 +11596,11 @@
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
       <c r="I25" s="28" t="s">
-        <v>1446</v>
+        <v>688</v>
       </c>
       <c r="J25" s="29"/>
       <c r="K25" s="34" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="L25" s="17"/>
       <c r="M25" s="21"/>
@@ -11595,7 +11612,7 @@
         <v>656</v>
       </c>
       <c r="Q25" s="16" t="s">
-        <v>1447</v>
+        <v>1435</v>
       </c>
       <c r="R25" s="52">
         <v>0</v>
@@ -11607,16 +11624,16 @@
         <v>5</v>
       </c>
       <c r="W25" s="27" t="s">
-        <v>1449</v>
+        <v>20</v>
       </c>
       <c r="X25" s="54"/>
     </row>
     <row r="26" spans="1:24" ht="48">
       <c r="A26" s="78">
-        <v>55500007</v>
+        <v>55500006</v>
       </c>
       <c r="B26" s="78" t="s">
-        <v>459</v>
+        <v>1447</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>6</v>
@@ -11627,11 +11644,11 @@
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
       <c r="I26" s="28" t="s">
-        <v>707</v>
+        <v>1445</v>
       </c>
       <c r="J26" s="29"/>
       <c r="K26" s="34" t="s">
-        <v>1440</v>
+        <v>1436</v>
       </c>
       <c r="L26" s="17"/>
       <c r="M26" s="21"/>
@@ -11643,7 +11660,7 @@
         <v>656</v>
       </c>
       <c r="Q26" s="16" t="s">
-        <v>1441</v>
+        <v>1446</v>
       </c>
       <c r="R26" s="52">
         <v>0</v>
@@ -11655,16 +11672,16 @@
         <v>5</v>
       </c>
       <c r="W26" s="27" t="s">
-        <v>460</v>
+        <v>1448</v>
       </c>
       <c r="X26" s="54"/>
     </row>
     <row r="27" spans="1:24" ht="48">
       <c r="A27" s="78">
-        <v>55500008</v>
+        <v>55500007</v>
       </c>
       <c r="B27" s="78" t="s">
-        <v>7</v>
+        <v>459</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>6</v>
@@ -11675,11 +11692,11 @@
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
       <c r="I27" s="28" t="s">
-        <v>683</v>
+        <v>707</v>
       </c>
       <c r="J27" s="29"/>
       <c r="K27" s="34" t="s">
-        <v>703</v>
+        <v>1439</v>
       </c>
       <c r="L27" s="17"/>
       <c r="M27" s="21"/>
@@ -11691,7 +11708,7 @@
         <v>656</v>
       </c>
       <c r="Q27" s="16" t="s">
-        <v>670</v>
+        <v>1440</v>
       </c>
       <c r="R27" s="52">
         <v>0</v>
@@ -11703,16 +11720,16 @@
         <v>5</v>
       </c>
       <c r="W27" s="27" t="s">
-        <v>8</v>
+        <v>460</v>
       </c>
       <c r="X27" s="54"/>
     </row>
     <row r="28" spans="1:24" ht="48">
       <c r="A28" s="78">
-        <v>55500009</v>
+        <v>55500008</v>
       </c>
       <c r="B28" s="78" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>6</v>
@@ -11723,7 +11740,7 @@
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
       <c r="I28" s="28" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J28" s="29"/>
       <c r="K28" s="34" t="s">
@@ -11739,7 +11756,7 @@
         <v>656</v>
       </c>
       <c r="Q28" s="16" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="R28" s="52">
         <v>0</v>
@@ -11751,16 +11768,16 @@
         <v>5</v>
       </c>
       <c r="W28" s="27" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="X28" s="54"/>
     </row>
     <row r="29" spans="1:24" ht="48">
       <c r="A29" s="78">
-        <v>55500010</v>
+        <v>55500009</v>
       </c>
       <c r="B29" s="78" t="s">
-        <v>1442</v>
+        <v>11</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>6</v>
@@ -11771,7 +11788,7 @@
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
       <c r="I29" s="28" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="J29" s="29"/>
       <c r="K29" s="34" t="s">
@@ -11787,7 +11804,7 @@
         <v>656</v>
       </c>
       <c r="Q29" s="16" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="R29" s="52">
         <v>0</v>
@@ -11799,16 +11816,16 @@
         <v>5</v>
       </c>
       <c r="W29" s="27" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="X29" s="54"/>
     </row>
     <row r="30" spans="1:24" ht="48">
       <c r="A30" s="78">
-        <v>55500011</v>
+        <v>55500010</v>
       </c>
       <c r="B30" s="78" t="s">
-        <v>9</v>
+        <v>1441</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>6</v>
@@ -11819,11 +11836,11 @@
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
       <c r="I30" s="28" t="s">
-        <v>682</v>
+        <v>687</v>
       </c>
       <c r="J30" s="29"/>
       <c r="K30" s="34" t="s">
-        <v>1432</v>
+        <v>703</v>
       </c>
       <c r="L30" s="17"/>
       <c r="M30" s="21"/>
@@ -11835,7 +11852,7 @@
         <v>656</v>
       </c>
       <c r="Q30" s="16" t="s">
-        <v>1433</v>
+        <v>674</v>
       </c>
       <c r="R30" s="52">
         <v>0</v>
@@ -11847,16 +11864,16 @@
         <v>5</v>
       </c>
       <c r="W30" s="27" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="X30" s="54"/>
     </row>
     <row r="31" spans="1:24" ht="48">
       <c r="A31" s="78">
-        <v>55500012</v>
+        <v>55500011</v>
       </c>
       <c r="B31" s="78" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>6</v>
@@ -11867,11 +11884,11 @@
       <c r="G31" s="32"/>
       <c r="H31" s="32"/>
       <c r="I31" s="28" t="s">
-        <v>698</v>
+        <v>682</v>
       </c>
       <c r="J31" s="29"/>
       <c r="K31" s="34" t="s">
-        <v>703</v>
+        <v>1431</v>
       </c>
       <c r="L31" s="17"/>
       <c r="M31" s="21"/>
@@ -11883,7 +11900,7 @@
         <v>656</v>
       </c>
       <c r="Q31" s="16" t="s">
-        <v>676</v>
+        <v>1432</v>
       </c>
       <c r="R31" s="52">
         <v>0</v>
@@ -11895,16 +11912,16 @@
         <v>5</v>
       </c>
       <c r="W31" s="27" t="s">
-        <v>210</v>
+        <v>10</v>
       </c>
       <c r="X31" s="54"/>
     </row>
     <row r="32" spans="1:24" ht="48">
       <c r="A32" s="78">
-        <v>55500013</v>
+        <v>55500012</v>
       </c>
       <c r="B32" s="78" t="s">
-        <v>14</v>
+        <v>209</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>6</v>
@@ -11912,10 +11929,10 @@
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
       <c r="F32" s="66"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
       <c r="I32" s="28" t="s">
-        <v>686</v>
+        <v>698</v>
       </c>
       <c r="J32" s="29"/>
       <c r="K32" s="34" t="s">
@@ -11931,7 +11948,7 @@
         <v>656</v>
       </c>
       <c r="Q32" s="16" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="R32" s="52">
         <v>0</v>
@@ -11943,16 +11960,16 @@
         <v>5</v>
       </c>
       <c r="W32" s="27" t="s">
-        <v>15</v>
+        <v>210</v>
       </c>
       <c r="X32" s="54"/>
     </row>
     <row r="33" spans="1:24" ht="48">
       <c r="A33" s="78">
-        <v>55500014</v>
+        <v>55500013</v>
       </c>
       <c r="B33" s="78" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>6</v>
@@ -11963,7 +11980,7 @@
       <c r="G33" s="69"/>
       <c r="H33" s="69"/>
       <c r="I33" s="28" t="s">
-        <v>697</v>
+        <v>686</v>
       </c>
       <c r="J33" s="29"/>
       <c r="K33" s="34" t="s">
@@ -11979,9 +11996,9 @@
         <v>656</v>
       </c>
       <c r="Q33" s="16" t="s">
-        <v>675</v>
-      </c>
-      <c r="R33" s="27">
+        <v>673</v>
+      </c>
+      <c r="R33" s="52">
         <v>0</v>
       </c>
       <c r="S33" s="27"/>
@@ -11991,16 +12008,16 @@
         <v>5</v>
       </c>
       <c r="W33" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="X33" s="70"/>
+        <v>15</v>
+      </c>
+      <c r="X33" s="54"/>
     </row>
     <row r="34" spans="1:24" ht="48">
       <c r="A34" s="78">
-        <v>55500015</v>
+        <v>55500014</v>
       </c>
       <c r="B34" s="78" t="s">
-        <v>1455</v>
+        <v>172</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>6</v>
@@ -12011,7 +12028,7 @@
       <c r="G34" s="69"/>
       <c r="H34" s="69"/>
       <c r="I34" s="28" t="s">
-        <v>1450</v>
+        <v>697</v>
       </c>
       <c r="J34" s="29"/>
       <c r="K34" s="34" t="s">
@@ -12027,7 +12044,7 @@
         <v>656</v>
       </c>
       <c r="Q34" s="16" t="s">
-        <v>1452</v>
+        <v>675</v>
       </c>
       <c r="R34" s="27">
         <v>0</v>
@@ -12039,16 +12056,16 @@
         <v>5</v>
       </c>
       <c r="W34" s="27" t="s">
-        <v>1454</v>
+        <v>173</v>
       </c>
       <c r="X34" s="70"/>
     </row>
     <row r="35" spans="1:24" ht="48">
       <c r="A35" s="78">
-        <v>55500016</v>
+        <v>55500015</v>
       </c>
       <c r="B35" s="78" t="s">
-        <v>1457</v>
+        <v>1454</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>6</v>
@@ -12059,7 +12076,7 @@
       <c r="G35" s="69"/>
       <c r="H35" s="69"/>
       <c r="I35" s="28" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="J35" s="29"/>
       <c r="K35" s="34" t="s">
@@ -12075,7 +12092,7 @@
         <v>656</v>
       </c>
       <c r="Q35" s="16" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="R35" s="27">
         <v>0</v>
@@ -12087,36 +12104,32 @@
         <v>5</v>
       </c>
       <c r="W35" s="27" t="s">
+        <v>1453</v>
+      </c>
+      <c r="X35" s="70"/>
+    </row>
+    <row r="36" spans="1:24" ht="48">
+      <c r="A36" s="78">
+        <v>55500016</v>
+      </c>
+      <c r="B36" s="78" t="s">
         <v>1456</v>
       </c>
-      <c r="X35" s="70"/>
-    </row>
-    <row r="36" spans="1:24" ht="168">
-      <c r="A36" s="77">
-        <v>55900001</v>
-      </c>
-      <c r="B36" s="77" t="s">
-        <v>168</v>
-      </c>
       <c r="C36" s="27" t="s">
-        <v>955</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>1340</v>
-      </c>
-      <c r="E36" s="27">
-        <v>40</v>
-      </c>
-      <c r="F36" s="66" t="s">
-        <v>1382</v>
-      </c>
-      <c r="G36" s="69" t="s">
-        <v>1464</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="69"/>
       <c r="H36" s="69"/>
-      <c r="I36" s="28"/>
+      <c r="I36" s="28" t="s">
+        <v>1450</v>
+      </c>
       <c r="J36" s="29"/>
-      <c r="K36" s="34"/>
+      <c r="K36" s="34" t="s">
+        <v>703</v>
+      </c>
       <c r="L36" s="17"/>
       <c r="M36" s="21"/>
       <c r="N36" s="59"/>
@@ -12127,49 +12140,43 @@
         <v>656</v>
       </c>
       <c r="Q36" s="16" t="s">
-        <v>1326</v>
+        <v>1452</v>
       </c>
       <c r="R36" s="27">
         <v>0</v>
       </c>
-      <c r="S36" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="T36" s="27" t="s">
-        <v>450</v>
-      </c>
-      <c r="U36" s="27" t="s">
-        <v>953</v>
-      </c>
+      <c r="S36" s="27"/>
+      <c r="T36" s="27"/>
+      <c r="U36" s="27"/>
       <c r="V36" s="27">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="W36" s="27" t="s">
-        <v>169</v>
+        <v>1455</v>
       </c>
       <c r="X36" s="70"/>
     </row>
-    <row r="37" spans="1:24" ht="144">
+    <row r="37" spans="1:24" ht="168">
       <c r="A37" s="77">
-        <v>55900002</v>
+        <v>55900001</v>
       </c>
       <c r="B37" s="77" t="s">
-        <v>236</v>
+        <v>168</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>0</v>
+        <v>955</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="E37" s="27">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F37" s="66" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="G37" s="69" t="s">
-        <v>1404</v>
+        <v>1463</v>
       </c>
       <c r="H37" s="69"/>
       <c r="I37" s="28"/>
@@ -12185,39 +12192,49 @@
         <v>656</v>
       </c>
       <c r="Q37" s="16" t="s">
-        <v>1405</v>
+        <v>1325</v>
       </c>
       <c r="R37" s="27">
         <v>0</v>
       </c>
-      <c r="S37" s="27"/>
-      <c r="T37" s="27"/>
-      <c r="U37" s="27"/>
+      <c r="S37" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="T37" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="U37" s="27" t="s">
+        <v>953</v>
+      </c>
       <c r="V37" s="27">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W37" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="X37" s="70" t="s">
-        <v>1406</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" ht="36">
+        <v>169</v>
+      </c>
+      <c r="X37" s="70"/>
+    </row>
+    <row r="38" spans="1:24" ht="144">
       <c r="A38" s="77">
-        <v>55900003</v>
+        <v>55900002</v>
       </c>
       <c r="B38" s="77" t="s">
-        <v>1399</v>
+        <v>236</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="66"/>
+      <c r="D38" s="27" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E38" s="27">
+        <v>20</v>
+      </c>
+      <c r="F38" s="66" t="s">
+        <v>1381</v>
+      </c>
       <c r="G38" s="69" t="s">
-        <v>1401</v>
+        <v>1403</v>
       </c>
       <c r="H38" s="69"/>
       <c r="I38" s="28"/>
@@ -12233,7 +12250,7 @@
         <v>656</v>
       </c>
       <c r="Q38" s="16" t="s">
-        <v>1402</v>
+        <v>1404</v>
       </c>
       <c r="R38" s="27">
         <v>0</v>
@@ -12242,12 +12259,60 @@
       <c r="T38" s="27"/>
       <c r="U38" s="27"/>
       <c r="V38" s="27">
+        <v>30</v>
+      </c>
+      <c r="W38" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="X38" s="70" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" ht="36">
+      <c r="A39" s="77">
+        <v>55900003</v>
+      </c>
+      <c r="B39" s="77" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="69" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H39" s="69"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="59"/>
+      <c r="O39" s="68" t="s">
+        <v>661</v>
+      </c>
+      <c r="P39" s="66" t="s">
+        <v>656</v>
+      </c>
+      <c r="Q39" s="16" t="s">
+        <v>1401</v>
+      </c>
+      <c r="R39" s="27">
+        <v>0</v>
+      </c>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="27">
         <v>80</v>
       </c>
-      <c r="W38" s="27" t="s">
-        <v>1400</v>
-      </c>
-      <c r="X38" s="70"/>
+      <c r="W39" s="27" t="s">
+        <v>1399</v>
+      </c>
+      <c r="X39" s="70"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -12302,13 +12367,13 @@
         <v>651</v>
       </c>
       <c r="D1" s="67" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E1" s="67" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="F1" s="67" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>667</v>
@@ -12350,7 +12415,7 @@
         <v>930</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>949</v>
@@ -12376,13 +12441,13 @@
         <v>643</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>960</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>1213</v>
@@ -12450,13 +12515,13 @@
         <v>646</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1212</v>
@@ -12498,7 +12563,7 @@
         <v>1242</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>947</v>
@@ -15370,13 +15435,13 @@
         <v>197</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="E62" s="1">
         <v>20</v>
       </c>
       <c r="F62" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G62" s="32"/>
       <c r="H62" s="32"/>
@@ -15386,7 +15451,7 @@
       <c r="J62" s="18"/>
       <c r="K62" s="17"/>
       <c r="L62" s="17" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="M62" s="21"/>
       <c r="N62" s="59"/>
@@ -15406,7 +15471,7 @@
         <v>848</v>
       </c>
       <c r="T62" s="10" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="U62" s="10" t="s">
         <v>957</v>
@@ -15626,13 +15691,13 @@
         <v>197</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="E67" s="1">
         <v>10</v>
       </c>
       <c r="F67" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G67" s="32"/>
       <c r="H67" s="32"/>
@@ -15642,7 +15707,7 @@
       <c r="J67" s="18"/>
       <c r="K67" s="17"/>
       <c r="L67" s="17" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="M67" s="21"/>
       <c r="N67" s="59"/>
@@ -15662,7 +15727,7 @@
         <v>850</v>
       </c>
       <c r="T67" s="10" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="U67" s="10" t="s">
         <v>957</v>
@@ -16868,16 +16933,16 @@
         <v>85</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="E92" s="1">
         <v>20</v>
       </c>
       <c r="F92" s="65" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="G92" s="32" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="H92" s="32"/>
       <c r="I92" s="28"/>
@@ -19156,13 +19221,13 @@
         <v>931</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="E138" s="1">
         <v>15</v>
       </c>
       <c r="F138" s="65" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G138" s="32"/>
       <c r="H138" s="32"/>
@@ -19171,7 +19236,7 @@
       <c r="K138" s="17"/>
       <c r="L138" s="22"/>
       <c r="M138" s="21" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="N138" s="59"/>
       <c r="O138" s="1" t="s">
@@ -20690,13 +20755,13 @@
         <v>197</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="E169" s="1">
         <v>0</v>
       </c>
       <c r="F169" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G169" s="32"/>
       <c r="H169" s="32"/>
@@ -20706,7 +20771,7 @@
       <c r="J169" s="18"/>
       <c r="K169" s="17"/>
       <c r="L169" s="17" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="M169" s="21"/>
       <c r="N169" s="59"/>
@@ -21674,13 +21739,13 @@
         <v>197</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="E189" s="1">
         <v>10</v>
       </c>
       <c r="F189" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G189" s="32"/>
       <c r="H189" s="32"/>
@@ -21690,7 +21755,7 @@
       <c r="J189" s="18"/>
       <c r="K189" s="17"/>
       <c r="L189" s="17" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="M189" s="21"/>
       <c r="N189" s="59"/>
@@ -21884,13 +21949,13 @@
         <v>197</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="E193" s="1">
         <v>10</v>
       </c>
       <c r="F193" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G193" s="32"/>
       <c r="H193" s="32"/>
@@ -21900,7 +21965,7 @@
       <c r="J193" s="18"/>
       <c r="K193" s="17"/>
       <c r="L193" s="17" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="M193" s="21"/>
       <c r="N193" s="59"/>
@@ -22686,13 +22751,13 @@
         <v>931</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="E209" s="1">
         <v>0</v>
       </c>
       <c r="F209" s="65" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="G209" s="32"/>
       <c r="H209" s="32"/>
@@ -22701,7 +22766,7 @@
       <c r="K209" s="17"/>
       <c r="L209" s="17"/>
       <c r="M209" s="21" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="N209" s="59"/>
       <c r="O209" s="1" t="s">
@@ -22720,7 +22785,7 @@
         <v>884</v>
       </c>
       <c r="T209" s="10" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="U209" s="10"/>
       <c r="V209" s="1">
@@ -23716,16 +23781,16 @@
         <v>931</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="E230" s="1">
         <v>10</v>
       </c>
       <c r="F230" s="65" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="G230" s="32" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="H230" s="32"/>
       <c r="I230" s="31"/>
@@ -24022,16 +24087,16 @@
         <v>931</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="E236" s="1">
         <v>100</v>
       </c>
       <c r="F236" s="65" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="G236" s="32" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="H236" s="32"/>
       <c r="I236" s="31"/>
@@ -24274,13 +24339,13 @@
         <v>197</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="E241" s="1">
         <v>10</v>
       </c>
       <c r="F241" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G241" s="32"/>
       <c r="H241" s="32"/>
@@ -24290,7 +24355,7 @@
       <c r="J241" s="18"/>
       <c r="K241" s="17"/>
       <c r="L241" s="17" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="M241" s="21"/>
       <c r="N241" s="59"/>
@@ -24310,7 +24375,7 @@
         <v>1080</v>
       </c>
       <c r="T241" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="U241" s="10" t="s">
         <v>957</v>
@@ -24480,13 +24545,13 @@
         <v>197</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="E245" s="1">
         <v>10</v>
       </c>
       <c r="F245" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G245" s="32"/>
       <c r="H245" s="32"/>
@@ -24496,7 +24561,7 @@
       <c r="J245" s="18"/>
       <c r="K245" s="17"/>
       <c r="L245" s="17" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="M245" s="21"/>
       <c r="N245" s="59"/>
@@ -24516,7 +24581,7 @@
         <v>854</v>
       </c>
       <c r="T245" s="10" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="U245" s="10" t="s">
         <v>957</v>
@@ -24542,13 +24607,13 @@
         <v>197</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E246" s="1">
         <v>10</v>
       </c>
       <c r="F246" s="65" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="G246" s="32"/>
       <c r="H246" s="32"/>
@@ -24558,7 +24623,7 @@
       <c r="J246" s="18"/>
       <c r="K246" s="17"/>
       <c r="L246" s="17" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="M246" s="21"/>
       <c r="N246" s="59"/>
@@ -24578,7 +24643,7 @@
         <v>855</v>
       </c>
       <c r="T246" s="10" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="U246" s="10" t="s">
         <v>957</v>
@@ -24604,13 +24669,13 @@
         <v>197</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="E247" s="1">
         <v>10</v>
       </c>
       <c r="F247" s="65" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="G247" s="32"/>
       <c r="H247" s="32"/>
@@ -24620,7 +24685,7 @@
       <c r="J247" s="18"/>
       <c r="K247" s="17"/>
       <c r="L247" s="17" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="M247" s="21"/>
       <c r="N247" s="59"/>
@@ -24640,7 +24705,7 @@
         <v>856</v>
       </c>
       <c r="T247" s="10" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="U247" s="10" t="s">
         <v>957</v>
@@ -24666,7 +24731,7 @@
         <v>197</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="E248" s="1">
         <v>15</v>
@@ -24680,7 +24745,7 @@
       <c r="J248" s="18"/>
       <c r="K248" s="17"/>
       <c r="L248" s="17" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="M248" s="21"/>
       <c r="N248" s="59"/>
@@ -24700,7 +24765,7 @@
         <v>857</v>
       </c>
       <c r="T248" s="10" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="U248" s="10" t="s">
         <v>957</v>
@@ -24726,13 +24791,13 @@
         <v>197</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="E249" s="1">
         <v>30</v>
       </c>
       <c r="F249" s="65" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="G249" s="32"/>
       <c r="H249" s="32"/>
@@ -24742,7 +24807,7 @@
       <c r="J249" s="18"/>
       <c r="K249" s="17"/>
       <c r="L249" s="17" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="M249" s="21"/>
       <c r="N249" s="59"/>
@@ -24762,7 +24827,7 @@
         <v>858</v>
       </c>
       <c r="T249" s="10" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="U249" s="10" t="s">
         <v>957</v>
@@ -24788,13 +24853,13 @@
         <v>197</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="E250" s="1">
         <v>15</v>
       </c>
       <c r="F250" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G250" s="32"/>
       <c r="H250" s="32"/>
@@ -24804,7 +24869,7 @@
       <c r="J250" s="18"/>
       <c r="K250" s="17"/>
       <c r="L250" s="17" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="M250" s="21"/>
       <c r="N250" s="59"/>
@@ -24850,13 +24915,13 @@
         <v>197</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="E251" s="1">
         <v>0</v>
       </c>
       <c r="F251" s="65" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="G251" s="32"/>
       <c r="H251" s="32"/>
@@ -24866,7 +24931,7 @@
       <c r="J251" s="18"/>
       <c r="K251" s="17"/>
       <c r="L251" s="17" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="M251" s="21"/>
       <c r="N251" s="59"/>
@@ -24912,13 +24977,13 @@
         <v>197</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="E252" s="1">
         <v>0</v>
       </c>
       <c r="F252" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G252" s="32"/>
       <c r="H252" s="32"/>
@@ -24928,7 +24993,7 @@
       <c r="J252" s="18"/>
       <c r="K252" s="17"/>
       <c r="L252" s="17" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="M252" s="21"/>
       <c r="N252" s="59"/>
@@ -25070,13 +25135,13 @@
         <v>197</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="E255" s="1">
         <v>15</v>
       </c>
       <c r="F255" s="65" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G255" s="32"/>
       <c r="H255" s="32"/>
@@ -25086,7 +25151,7 @@
       <c r="J255" s="18"/>
       <c r="K255" s="17"/>
       <c r="L255" s="17" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="M255" s="21"/>
       <c r="N255" s="59"/>
@@ -25106,7 +25171,7 @@
         <v>865</v>
       </c>
       <c r="T255" s="10" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="U255" s="10" t="s">
         <v>957</v>
@@ -25132,13 +25197,13 @@
         <v>931</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="E256" s="1">
         <v>10</v>
       </c>
       <c r="F256" s="65" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="G256" s="32"/>
       <c r="H256" s="32"/>
@@ -25147,7 +25212,7 @@
       <c r="K256" s="17"/>
       <c r="L256" s="17"/>
       <c r="M256" s="21" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="N256" s="59"/>
       <c r="O256" s="1" t="s">
@@ -25164,7 +25229,7 @@
       </c>
       <c r="S256" s="10"/>
       <c r="T256" s="10" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="U256" s="10"/>
       <c r="V256" s="1">
@@ -25290,16 +25355,16 @@
         <v>1146</v>
       </c>
       <c r="D259" s="27" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="E259" s="35">
         <v>10</v>
       </c>
       <c r="F259" s="66" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="G259" s="32" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="H259" s="36"/>
       <c r="I259" s="49"/>
@@ -25346,16 +25411,16 @@
         <v>1146</v>
       </c>
       <c r="D260" s="27" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="E260" s="35">
         <v>10</v>
       </c>
       <c r="F260" s="66" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="G260" s="32" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="H260" s="36"/>
       <c r="I260" s="37"/>
@@ -25393,7 +25458,7 @@
     </row>
     <row r="261" spans="1:24" ht="36">
       <c r="A261" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="B261" s="11" t="s">
         <v>110</v>
@@ -25488,13 +25553,13 @@
         <v>651</v>
       </c>
       <c r="D1" s="67" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E1" s="67" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="F1" s="67" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>667</v>
@@ -25536,7 +25601,7 @@
         <v>930</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>949</v>
@@ -25562,13 +25627,13 @@
         <v>643</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>960</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>958</v>
@@ -25636,13 +25701,13 @@
         <v>646</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1107</v>
@@ -25684,7 +25749,7 @@
         <v>879</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>947</v>
@@ -25844,13 +25909,13 @@
         <v>651</v>
       </c>
       <c r="D1" s="67" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="E1" s="67" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="F1" s="67" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>667</v>
@@ -25892,7 +25957,7 @@
         <v>930</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>949</v>
@@ -25918,13 +25983,13 @@
         <v>643</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>960</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>936</v>
@@ -25992,13 +26057,13 @@
         <v>646</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1107</v>
@@ -26040,7 +26105,7 @@
         <v>879</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>947</v>

</xml_diff>

<commit_message>
close #32 refine card Chiwen
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -438,7 +438,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3095" uniqueCount="1477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3103" uniqueCount="1481">
   <si>
     <t>特殊</t>
   </si>
@@ -5592,6 +5592,22 @@
   </si>
   <si>
     <t>每2.5回合在周围随机位置召唤一个跳跳菇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鱼群</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yuqun</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(2,51000018);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每2回合在周围随机位置召唤一个鱼人</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9882,8 +9898,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:X42" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
-  <autoFilter ref="A3:X42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:X43" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
+  <autoFilter ref="A3:X43"/>
   <sortState ref="A4:X31">
     <sortCondition ref="A3:A31"/>
   </sortState>
@@ -10312,13 +10328,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X42"/>
+  <dimension ref="A1:X43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11506,31 +11522,31 @@
       </c>
       <c r="X22" s="70"/>
     </row>
-    <row r="23" spans="1:24" ht="48">
-      <c r="A23" s="78">
-        <v>55500001</v>
-      </c>
-      <c r="B23" s="78" t="s">
-        <v>17</v>
+    <row r="23" spans="1:24" ht="28.8">
+      <c r="A23" s="76">
+        <v>55400006</v>
+      </c>
+      <c r="B23" s="76" t="s">
+        <v>1477</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>6</v>
+        <v>1475</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="66"/>
       <c r="G23" s="69"/>
       <c r="H23" s="69"/>
-      <c r="I23" s="28" t="s">
-        <v>1425</v>
-      </c>
+      <c r="I23" s="28"/>
       <c r="J23" s="29"/>
-      <c r="K23" s="34" t="s">
-        <v>1415</v>
-      </c>
+      <c r="K23" s="34"/>
       <c r="L23" s="17"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="59"/>
+      <c r="M23" s="21" t="s">
+        <v>1479</v>
+      </c>
+      <c r="N23" s="59">
+        <v>2</v>
+      </c>
       <c r="O23" s="68" t="s">
         <v>661</v>
       </c>
@@ -11538,28 +11554,30 @@
         <v>656</v>
       </c>
       <c r="Q23" s="16" t="s">
-        <v>1416</v>
+        <v>1480</v>
       </c>
       <c r="R23" s="27">
         <v>0</v>
       </c>
-      <c r="S23" s="27"/>
+      <c r="S23" s="27" t="s">
+        <v>883</v>
+      </c>
       <c r="T23" s="27"/>
       <c r="U23" s="27"/>
       <c r="V23" s="27">
-        <v>5</v>
-      </c>
-      <c r="W23" s="27" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="W23" s="72" t="s">
+        <v>1478</v>
       </c>
       <c r="X23" s="70"/>
     </row>
     <row r="24" spans="1:24" ht="48">
       <c r="A24" s="78">
-        <v>55500002</v>
+        <v>55500001</v>
       </c>
       <c r="B24" s="78" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>6</v>
@@ -11570,11 +11588,11 @@
       <c r="G24" s="69"/>
       <c r="H24" s="69"/>
       <c r="I24" s="28" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="J24" s="29"/>
       <c r="K24" s="34" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="L24" s="17"/>
       <c r="M24" s="21"/>
@@ -11586,7 +11604,7 @@
         <v>656</v>
       </c>
       <c r="Q24" s="16" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
       <c r="R24" s="27">
         <v>0</v>
@@ -11598,16 +11616,16 @@
         <v>5</v>
       </c>
       <c r="W24" s="27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="X24" s="70"/>
     </row>
     <row r="25" spans="1:24" ht="48">
       <c r="A25" s="78">
-        <v>55500003</v>
+        <v>55500002</v>
       </c>
       <c r="B25" s="78" t="s">
-        <v>1424</v>
+        <v>21</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>6</v>
@@ -11618,11 +11636,11 @@
       <c r="G25" s="69"/>
       <c r="H25" s="69"/>
       <c r="I25" s="28" t="s">
-        <v>685</v>
+        <v>1426</v>
       </c>
       <c r="J25" s="29"/>
       <c r="K25" s="34" t="s">
-        <v>701</v>
+        <v>1419</v>
       </c>
       <c r="L25" s="17"/>
       <c r="M25" s="21"/>
@@ -11634,7 +11652,7 @@
         <v>656</v>
       </c>
       <c r="Q25" s="16" t="s">
-        <v>672</v>
+        <v>1420</v>
       </c>
       <c r="R25" s="27">
         <v>0</v>
@@ -11646,16 +11664,16 @@
         <v>5</v>
       </c>
       <c r="W25" s="27" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:24" ht="48">
       <c r="A26" s="78">
-        <v>55500004</v>
+        <v>55500003</v>
       </c>
       <c r="B26" s="78" t="s">
-        <v>362</v>
+        <v>1424</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>6</v>
@@ -11663,10 +11681,10 @@
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="66"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
       <c r="I26" s="28" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
       <c r="J26" s="29"/>
       <c r="K26" s="34" t="s">
@@ -11682,7 +11700,7 @@
         <v>656</v>
       </c>
       <c r="Q26" s="16" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="R26" s="27">
         <v>0</v>
@@ -11694,16 +11712,16 @@
         <v>5</v>
       </c>
       <c r="W26" s="27" t="s">
-        <v>363</v>
+        <v>13</v>
       </c>
       <c r="X26" s="70"/>
     </row>
     <row r="27" spans="1:24" ht="48">
       <c r="A27" s="78">
-        <v>55500005</v>
+        <v>55500004</v>
       </c>
       <c r="B27" s="78" t="s">
-        <v>19</v>
+        <v>362</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>6</v>
@@ -11714,11 +11732,11 @@
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
       <c r="I27" s="28" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="J27" s="29"/>
       <c r="K27" s="34" t="s">
-        <v>1418</v>
+        <v>701</v>
       </c>
       <c r="L27" s="17"/>
       <c r="M27" s="21"/>
@@ -11730,9 +11748,9 @@
         <v>656</v>
       </c>
       <c r="Q27" s="16" t="s">
-        <v>1417</v>
-      </c>
-      <c r="R27" s="52">
+        <v>680</v>
+      </c>
+      <c r="R27" s="27">
         <v>0</v>
       </c>
       <c r="S27" s="27"/>
@@ -11742,16 +11760,16 @@
         <v>5</v>
       </c>
       <c r="W27" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="X27" s="54"/>
+        <v>363</v>
+      </c>
+      <c r="X27" s="70"/>
     </row>
     <row r="28" spans="1:24" ht="48">
       <c r="A28" s="78">
-        <v>55500006</v>
+        <v>55500005</v>
       </c>
       <c r="B28" s="78" t="s">
-        <v>1429</v>
+        <v>19</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>6</v>
@@ -11762,7 +11780,7 @@
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
       <c r="I28" s="28" t="s">
-        <v>1427</v>
+        <v>688</v>
       </c>
       <c r="J28" s="29"/>
       <c r="K28" s="34" t="s">
@@ -11778,7 +11796,7 @@
         <v>656</v>
       </c>
       <c r="Q28" s="16" t="s">
-        <v>1428</v>
+        <v>1417</v>
       </c>
       <c r="R28" s="52">
         <v>0</v>
@@ -11790,16 +11808,16 @@
         <v>5</v>
       </c>
       <c r="W28" s="27" t="s">
-        <v>1430</v>
+        <v>20</v>
       </c>
       <c r="X28" s="54"/>
     </row>
     <row r="29" spans="1:24" ht="48">
       <c r="A29" s="78">
-        <v>55500007</v>
+        <v>55500006</v>
       </c>
       <c r="B29" s="78" t="s">
-        <v>459</v>
+        <v>1429</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>6</v>
@@ -11810,11 +11828,11 @@
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
       <c r="I29" s="28" t="s">
-        <v>705</v>
+        <v>1427</v>
       </c>
       <c r="J29" s="29"/>
       <c r="K29" s="34" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="L29" s="17"/>
       <c r="M29" s="21"/>
@@ -11826,7 +11844,7 @@
         <v>656</v>
       </c>
       <c r="Q29" s="16" t="s">
-        <v>1422</v>
+        <v>1428</v>
       </c>
       <c r="R29" s="52">
         <v>0</v>
@@ -11838,16 +11856,16 @@
         <v>5</v>
       </c>
       <c r="W29" s="27" t="s">
-        <v>460</v>
+        <v>1430</v>
       </c>
       <c r="X29" s="54"/>
     </row>
     <row r="30" spans="1:24" ht="48">
       <c r="A30" s="78">
-        <v>55500008</v>
+        <v>55500007</v>
       </c>
       <c r="B30" s="78" t="s">
-        <v>7</v>
+        <v>459</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>6</v>
@@ -11858,11 +11876,11 @@
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
       <c r="I30" s="28" t="s">
-        <v>683</v>
+        <v>705</v>
       </c>
       <c r="J30" s="29"/>
       <c r="K30" s="34" t="s">
-        <v>701</v>
+        <v>1421</v>
       </c>
       <c r="L30" s="17"/>
       <c r="M30" s="21"/>
@@ -11874,7 +11892,7 @@
         <v>656</v>
       </c>
       <c r="Q30" s="16" t="s">
-        <v>670</v>
+        <v>1422</v>
       </c>
       <c r="R30" s="52">
         <v>0</v>
@@ -11886,16 +11904,16 @@
         <v>5</v>
       </c>
       <c r="W30" s="27" t="s">
-        <v>8</v>
+        <v>460</v>
       </c>
       <c r="X30" s="54"/>
     </row>
     <row r="31" spans="1:24" ht="48">
       <c r="A31" s="78">
-        <v>55500009</v>
+        <v>55500008</v>
       </c>
       <c r="B31" s="78" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>6</v>
@@ -11906,7 +11924,7 @@
       <c r="G31" s="32"/>
       <c r="H31" s="32"/>
       <c r="I31" s="28" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J31" s="29"/>
       <c r="K31" s="34" t="s">
@@ -11922,7 +11940,7 @@
         <v>656</v>
       </c>
       <c r="Q31" s="16" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="R31" s="52">
         <v>0</v>
@@ -11934,16 +11952,16 @@
         <v>5</v>
       </c>
       <c r="W31" s="27" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="X31" s="54"/>
     </row>
     <row r="32" spans="1:24" ht="48">
       <c r="A32" s="78">
-        <v>55500010</v>
+        <v>55500009</v>
       </c>
       <c r="B32" s="78" t="s">
-        <v>1423</v>
+        <v>11</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>6</v>
@@ -11954,7 +11972,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="28" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="J32" s="29"/>
       <c r="K32" s="34" t="s">
@@ -11970,7 +11988,7 @@
         <v>656</v>
       </c>
       <c r="Q32" s="16" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="R32" s="52">
         <v>0</v>
@@ -11982,16 +12000,16 @@
         <v>5</v>
       </c>
       <c r="W32" s="27" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="X32" s="54"/>
     </row>
     <row r="33" spans="1:24" ht="48">
       <c r="A33" s="78">
-        <v>55500011</v>
+        <v>55500010</v>
       </c>
       <c r="B33" s="78" t="s">
-        <v>9</v>
+        <v>1423</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>6</v>
@@ -12002,11 +12020,11 @@
       <c r="G33" s="32"/>
       <c r="H33" s="32"/>
       <c r="I33" s="28" t="s">
-        <v>682</v>
+        <v>687</v>
       </c>
       <c r="J33" s="29"/>
       <c r="K33" s="34" t="s">
-        <v>1413</v>
+        <v>701</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="21"/>
@@ -12018,7 +12036,7 @@
         <v>656</v>
       </c>
       <c r="Q33" s="16" t="s">
-        <v>1414</v>
+        <v>674</v>
       </c>
       <c r="R33" s="52">
         <v>0</v>
@@ -12030,16 +12048,16 @@
         <v>5</v>
       </c>
       <c r="W33" s="27" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="X33" s="54"/>
     </row>
     <row r="34" spans="1:24" ht="48">
       <c r="A34" s="78">
-        <v>55500012</v>
+        <v>55500011</v>
       </c>
       <c r="B34" s="78" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>6</v>
@@ -12050,11 +12068,11 @@
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
       <c r="I34" s="28" t="s">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="J34" s="29"/>
       <c r="K34" s="34" t="s">
-        <v>701</v>
+        <v>1413</v>
       </c>
       <c r="L34" s="17"/>
       <c r="M34" s="21"/>
@@ -12066,7 +12084,7 @@
         <v>656</v>
       </c>
       <c r="Q34" s="16" t="s">
-        <v>676</v>
+        <v>1414</v>
       </c>
       <c r="R34" s="52">
         <v>0</v>
@@ -12078,16 +12096,16 @@
         <v>5</v>
       </c>
       <c r="W34" s="27" t="s">
-        <v>210</v>
+        <v>10</v>
       </c>
       <c r="X34" s="54"/>
     </row>
     <row r="35" spans="1:24" ht="48">
       <c r="A35" s="78">
-        <v>55500013</v>
+        <v>55500012</v>
       </c>
       <c r="B35" s="78" t="s">
-        <v>14</v>
+        <v>209</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>6</v>
@@ -12095,10 +12113,10 @@
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="66"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
       <c r="I35" s="28" t="s">
-        <v>686</v>
+        <v>696</v>
       </c>
       <c r="J35" s="29"/>
       <c r="K35" s="34" t="s">
@@ -12114,7 +12132,7 @@
         <v>656</v>
       </c>
       <c r="Q35" s="16" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="R35" s="52">
         <v>0</v>
@@ -12126,16 +12144,16 @@
         <v>5</v>
       </c>
       <c r="W35" s="27" t="s">
-        <v>15</v>
+        <v>210</v>
       </c>
       <c r="X35" s="54"/>
     </row>
     <row r="36" spans="1:24" ht="48">
       <c r="A36" s="78">
-        <v>55500014</v>
+        <v>55500013</v>
       </c>
       <c r="B36" s="78" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>6</v>
@@ -12146,7 +12164,7 @@
       <c r="G36" s="69"/>
       <c r="H36" s="69"/>
       <c r="I36" s="28" t="s">
-        <v>695</v>
+        <v>686</v>
       </c>
       <c r="J36" s="29"/>
       <c r="K36" s="34" t="s">
@@ -12162,9 +12180,9 @@
         <v>656</v>
       </c>
       <c r="Q36" s="16" t="s">
-        <v>675</v>
-      </c>
-      <c r="R36" s="27">
+        <v>673</v>
+      </c>
+      <c r="R36" s="52">
         <v>0</v>
       </c>
       <c r="S36" s="27"/>
@@ -12174,16 +12192,16 @@
         <v>5</v>
       </c>
       <c r="W36" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="X36" s="70"/>
+        <v>15</v>
+      </c>
+      <c r="X36" s="54"/>
     </row>
     <row r="37" spans="1:24" ht="48">
       <c r="A37" s="78">
-        <v>55500015</v>
+        <v>55500014</v>
       </c>
       <c r="B37" s="78" t="s">
-        <v>1436</v>
+        <v>172</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>6</v>
@@ -12194,7 +12212,7 @@
       <c r="G37" s="69"/>
       <c r="H37" s="69"/>
       <c r="I37" s="28" t="s">
-        <v>1431</v>
+        <v>695</v>
       </c>
       <c r="J37" s="29"/>
       <c r="K37" s="34" t="s">
@@ -12210,7 +12228,7 @@
         <v>656</v>
       </c>
       <c r="Q37" s="16" t="s">
-        <v>1433</v>
+        <v>675</v>
       </c>
       <c r="R37" s="27">
         <v>0</v>
@@ -12222,16 +12240,16 @@
         <v>5</v>
       </c>
       <c r="W37" s="27" t="s">
-        <v>1435</v>
+        <v>173</v>
       </c>
       <c r="X37" s="70"/>
     </row>
     <row r="38" spans="1:24" ht="48">
       <c r="A38" s="78">
-        <v>55500016</v>
+        <v>55500015</v>
       </c>
       <c r="B38" s="78" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>6</v>
@@ -12242,7 +12260,7 @@
       <c r="G38" s="69"/>
       <c r="H38" s="69"/>
       <c r="I38" s="28" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="J38" s="29"/>
       <c r="K38" s="34" t="s">
@@ -12258,7 +12276,7 @@
         <v>656</v>
       </c>
       <c r="Q38" s="16" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="R38" s="27">
         <v>0</v>
@@ -12270,137 +12288,127 @@
         <v>5</v>
       </c>
       <c r="W38" s="27" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="X38" s="70"/>
     </row>
     <row r="39" spans="1:24" ht="48">
-      <c r="A39" s="79">
-        <v>55600016</v>
-      </c>
-      <c r="B39" s="80" t="s">
-        <v>217</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="32" t="s">
-        <v>1461</v>
-      </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="17"/>
+      <c r="A39" s="78">
+        <v>55500016</v>
+      </c>
+      <c r="B39" s="78" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="28" t="s">
+        <v>1432</v>
+      </c>
+      <c r="J39" s="29"/>
+      <c r="K39" s="34" t="s">
+        <v>701</v>
+      </c>
       <c r="L39" s="17"/>
       <c r="M39" s="21"/>
       <c r="N39" s="59"/>
-      <c r="O39" s="1" t="s">
+      <c r="O39" s="68" t="s">
         <v>661</v>
       </c>
-      <c r="P39" s="9" t="s">
-        <v>656</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>1181</v>
-      </c>
-      <c r="R39" s="10">
-        <v>56000101</v>
-      </c>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1" t="s">
-        <v>946</v>
-      </c>
-      <c r="V39" s="1">
-        <v>10</v>
-      </c>
-      <c r="W39" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="X39" s="52"/>
-    </row>
-    <row r="40" spans="1:24" ht="168">
-      <c r="A40" s="77">
-        <v>55900001</v>
-      </c>
-      <c r="B40" s="77" t="s">
-        <v>168</v>
-      </c>
-      <c r="C40" s="27" t="s">
-        <v>949</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>1322</v>
-      </c>
-      <c r="E40" s="27">
-        <v>40</v>
-      </c>
-      <c r="F40" s="66" t="s">
-        <v>1364</v>
-      </c>
-      <c r="G40" s="69" t="s">
-        <v>1445</v>
-      </c>
-      <c r="H40" s="69"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="34"/>
+      <c r="P39" s="66" t="s">
+        <v>656</v>
+      </c>
+      <c r="Q39" s="16" t="s">
+        <v>1434</v>
+      </c>
+      <c r="R39" s="27">
+        <v>0</v>
+      </c>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="27">
+        <v>5</v>
+      </c>
+      <c r="W39" s="27" t="s">
+        <v>1437</v>
+      </c>
+      <c r="X39" s="70"/>
+    </row>
+    <row r="40" spans="1:24" ht="48">
+      <c r="A40" s="79">
+        <v>55600016</v>
+      </c>
+      <c r="B40" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="32" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H40" s="32"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="17"/>
       <c r="L40" s="17"/>
       <c r="M40" s="21"/>
       <c r="N40" s="59"/>
-      <c r="O40" s="68" t="s">
+      <c r="O40" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="P40" s="66" t="s">
-        <v>656</v>
-      </c>
-      <c r="Q40" s="16" t="s">
-        <v>1308</v>
-      </c>
-      <c r="R40" s="27">
-        <v>0</v>
-      </c>
-      <c r="S40" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="T40" s="27" t="s">
-        <v>450</v>
-      </c>
-      <c r="U40" s="27" t="s">
-        <v>947</v>
-      </c>
-      <c r="V40" s="27">
-        <v>35</v>
-      </c>
-      <c r="W40" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="X40" s="70"/>
-    </row>
-    <row r="41" spans="1:24" ht="144">
+      <c r="P40" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="R40" s="10">
+        <v>56000101</v>
+      </c>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="V40" s="1">
+        <v>10</v>
+      </c>
+      <c r="W40" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="X40" s="52"/>
+    </row>
+    <row r="41" spans="1:24" ht="168">
       <c r="A41" s="77">
-        <v>55900002</v>
+        <v>55900001</v>
       </c>
       <c r="B41" s="77" t="s">
-        <v>236</v>
+        <v>168</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>0</v>
+        <v>949</v>
       </c>
       <c r="D41" s="27" t="s">
         <v>1322</v>
       </c>
       <c r="E41" s="27">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F41" s="66" t="s">
         <v>1364</v>
       </c>
       <c r="G41" s="69" t="s">
-        <v>1385</v>
+        <v>1445</v>
       </c>
       <c r="H41" s="69"/>
       <c r="I41" s="28"/>
@@ -12416,39 +12424,49 @@
         <v>656</v>
       </c>
       <c r="Q41" s="16" t="s">
-        <v>1386</v>
+        <v>1308</v>
       </c>
       <c r="R41" s="27">
         <v>0</v>
       </c>
-      <c r="S41" s="27"/>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
+      <c r="S41" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="T41" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="U41" s="27" t="s">
+        <v>947</v>
+      </c>
       <c r="V41" s="27">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W41" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="X41" s="70" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" ht="36">
+        <v>169</v>
+      </c>
+      <c r="X41" s="70"/>
+    </row>
+    <row r="42" spans="1:24" ht="144">
       <c r="A42" s="77">
-        <v>55900003</v>
+        <v>55900002</v>
       </c>
       <c r="B42" s="77" t="s">
-        <v>1380</v>
+        <v>236</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="66"/>
+      <c r="D42" s="27" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E42" s="27">
+        <v>20</v>
+      </c>
+      <c r="F42" s="66" t="s">
+        <v>1364</v>
+      </c>
       <c r="G42" s="69" t="s">
-        <v>1382</v>
+        <v>1385</v>
       </c>
       <c r="H42" s="69"/>
       <c r="I42" s="28"/>
@@ -12464,7 +12482,7 @@
         <v>656</v>
       </c>
       <c r="Q42" s="16" t="s">
-        <v>1383</v>
+        <v>1386</v>
       </c>
       <c r="R42" s="27">
         <v>0</v>
@@ -12473,12 +12491,60 @@
       <c r="T42" s="27"/>
       <c r="U42" s="27"/>
       <c r="V42" s="27">
+        <v>30</v>
+      </c>
+      <c r="W42" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="X42" s="70" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="36">
+      <c r="A43" s="77">
+        <v>55900003</v>
+      </c>
+      <c r="B43" s="77" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="69" t="s">
+        <v>1382</v>
+      </c>
+      <c r="H43" s="69"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="59"/>
+      <c r="O43" s="68" t="s">
+        <v>661</v>
+      </c>
+      <c r="P43" s="66" t="s">
+        <v>656</v>
+      </c>
+      <c r="Q43" s="16" t="s">
+        <v>1383</v>
+      </c>
+      <c r="R43" s="27">
+        <v>0</v>
+      </c>
+      <c r="S43" s="27"/>
+      <c r="T43" s="27"/>
+      <c r="U43" s="27"/>
+      <c r="V43" s="27">
         <v>80</v>
       </c>
-      <c r="W42" s="27" t="s">
+      <c r="W43" s="27" t="s">
         <v>1381</v>
       </c>
-      <c r="X42" s="70"/>
+      <c r="X43" s="70"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -12496,10 +12562,10 @@
   <dimension ref="A1:X259"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C158" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A159" sqref="A159"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
def weapon test fin
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="7" r:id="rId1"/>
@@ -10604,33 +10604,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.21875" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
-    <col min="10" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="22.21875" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" customWidth="1"/>
-    <col min="15" max="15" width="8.44140625" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" customWidth="1"/>
-    <col min="18" max="18" width="23.44140625" customWidth="1"/>
-    <col min="19" max="19" width="8.77734375" customWidth="1"/>
-    <col min="20" max="22" width="7.6640625" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" customWidth="1"/>
+    <col min="3" max="7" width="7.25" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="9" max="9" width="12.875" customWidth="1"/>
+    <col min="10" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="22.25" customWidth="1"/>
+    <col min="14" max="14" width="14.875" customWidth="1"/>
+    <col min="15" max="15" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="7.375" customWidth="1"/>
+    <col min="17" max="17" width="6.375" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="19" width="8.75" customWidth="1"/>
+    <col min="20" max="22" width="7.625" customWidth="1"/>
+    <col min="23" max="23" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="58.8">
+    <row r="1" spans="1:25" ht="55.5">
       <c r="A1" s="6" t="s">
         <v>647</v>
       </c>
@@ -10910,7 +10910,7 @@
       </c>
       <c r="Y4" s="54"/>
     </row>
-    <row r="5" spans="1:25" ht="48">
+    <row r="5" spans="1:25" ht="36">
       <c r="A5" s="73">
         <v>55100002</v>
       </c>
@@ -10961,7 +10961,7 @@
       </c>
       <c r="Y5" s="52"/>
     </row>
-    <row r="6" spans="1:25" ht="48">
+    <row r="6" spans="1:25" ht="36">
       <c r="A6" s="73">
         <v>55100003</v>
       </c>
@@ -11012,7 +11012,7 @@
       </c>
       <c r="Y6" s="52"/>
     </row>
-    <row r="7" spans="1:25" ht="36">
+    <row r="7" spans="1:25" ht="24">
       <c r="A7" s="73">
         <v>55100004</v>
       </c>
@@ -11153,7 +11153,7 @@
       </c>
       <c r="Y9" s="92"/>
     </row>
-    <row r="10" spans="1:25" ht="72">
+    <row r="10" spans="1:25" ht="60">
       <c r="A10" s="73">
         <v>55100007</v>
       </c>
@@ -11349,7 +11349,7 @@
       </c>
       <c r="Y13" s="52"/>
     </row>
-    <row r="14" spans="1:25" ht="132">
+    <row r="14" spans="1:25" ht="120">
       <c r="A14" s="12">
         <v>55200001</v>
       </c>
@@ -11408,7 +11408,7 @@
       </c>
       <c r="Y14" s="70"/>
     </row>
-    <row r="15" spans="1:25" ht="168">
+    <row r="15" spans="1:25" ht="144">
       <c r="A15" s="12">
         <v>55200002</v>
       </c>
@@ -11463,7 +11463,7 @@
       </c>
       <c r="Y15" s="70"/>
     </row>
-    <row r="16" spans="1:25" ht="60">
+    <row r="16" spans="1:25" ht="48">
       <c r="A16" s="75">
         <v>55300001</v>
       </c>
@@ -11857,7 +11857,7 @@
       </c>
       <c r="Y23" s="70"/>
     </row>
-    <row r="24" spans="1:25" ht="28.8">
+    <row r="24" spans="1:25" ht="27">
       <c r="A24" s="76">
         <v>55400001</v>
       </c>
@@ -11908,7 +11908,7 @@
       </c>
       <c r="Y24" s="70"/>
     </row>
-    <row r="25" spans="1:25" ht="28.8">
+    <row r="25" spans="1:25" ht="24">
       <c r="A25" s="76">
         <v>55400002</v>
       </c>
@@ -11961,7 +11961,7 @@
       </c>
       <c r="Y25" s="70"/>
     </row>
-    <row r="26" spans="1:25" ht="28.8">
+    <row r="26" spans="1:25" ht="27">
       <c r="A26" s="76">
         <v>55400003</v>
       </c>
@@ -12012,7 +12012,7 @@
       </c>
       <c r="Y26" s="70"/>
     </row>
-    <row r="27" spans="1:25" ht="28.8">
+    <row r="27" spans="1:25" ht="27">
       <c r="A27" s="76">
         <v>55400004</v>
       </c>
@@ -12063,7 +12063,7 @@
       </c>
       <c r="Y27" s="70"/>
     </row>
-    <row r="28" spans="1:25" ht="28.8">
+    <row r="28" spans="1:25" ht="27">
       <c r="A28" s="76">
         <v>55400005</v>
       </c>
@@ -12114,7 +12114,7 @@
       </c>
       <c r="Y28" s="70"/>
     </row>
-    <row r="29" spans="1:25" ht="28.8">
+    <row r="29" spans="1:25" ht="27">
       <c r="A29" s="76">
         <v>55400006</v>
       </c>
@@ -12165,7 +12165,7 @@
       </c>
       <c r="Y29" s="70"/>
     </row>
-    <row r="30" spans="1:25" ht="48">
+    <row r="30" spans="1:25" ht="36">
       <c r="A30" s="78">
         <v>55500001</v>
       </c>
@@ -12214,7 +12214,7 @@
       </c>
       <c r="Y30" s="70"/>
     </row>
-    <row r="31" spans="1:25" ht="48">
+    <row r="31" spans="1:25" ht="36">
       <c r="A31" s="78">
         <v>55500002</v>
       </c>
@@ -12263,7 +12263,7 @@
       </c>
       <c r="Y31" s="70"/>
     </row>
-    <row r="32" spans="1:25" ht="48">
+    <row r="32" spans="1:25" ht="36">
       <c r="A32" s="78">
         <v>55500003</v>
       </c>
@@ -12312,7 +12312,7 @@
       </c>
       <c r="Y32" s="70"/>
     </row>
-    <row r="33" spans="1:25" ht="48">
+    <row r="33" spans="1:25" ht="36">
       <c r="A33" s="78">
         <v>55500004</v>
       </c>
@@ -12361,7 +12361,7 @@
       </c>
       <c r="Y33" s="70"/>
     </row>
-    <row r="34" spans="1:25" ht="48">
+    <row r="34" spans="1:25" ht="36">
       <c r="A34" s="78">
         <v>55500005</v>
       </c>
@@ -12410,7 +12410,7 @@
       </c>
       <c r="Y34" s="54"/>
     </row>
-    <row r="35" spans="1:25" ht="48">
+    <row r="35" spans="1:25" ht="36">
       <c r="A35" s="78">
         <v>55500006</v>
       </c>
@@ -12459,7 +12459,7 @@
       </c>
       <c r="Y35" s="54"/>
     </row>
-    <row r="36" spans="1:25" ht="48">
+    <row r="36" spans="1:25" ht="36">
       <c r="A36" s="78">
         <v>55500007</v>
       </c>
@@ -12508,7 +12508,7 @@
       </c>
       <c r="Y36" s="54"/>
     </row>
-    <row r="37" spans="1:25" ht="48">
+    <row r="37" spans="1:25" ht="36">
       <c r="A37" s="78">
         <v>55500008</v>
       </c>
@@ -12557,7 +12557,7 @@
       </c>
       <c r="Y37" s="54"/>
     </row>
-    <row r="38" spans="1:25" ht="48">
+    <row r="38" spans="1:25" ht="36">
       <c r="A38" s="78">
         <v>55500009</v>
       </c>
@@ -12606,7 +12606,7 @@
       </c>
       <c r="Y38" s="54"/>
     </row>
-    <row r="39" spans="1:25" ht="48">
+    <row r="39" spans="1:25" ht="36">
       <c r="A39" s="78">
         <v>55500010</v>
       </c>
@@ -12655,7 +12655,7 @@
       </c>
       <c r="Y39" s="54"/>
     </row>
-    <row r="40" spans="1:25" ht="48">
+    <row r="40" spans="1:25" ht="36">
       <c r="A40" s="78">
         <v>55500011</v>
       </c>
@@ -12704,7 +12704,7 @@
       </c>
       <c r="Y40" s="54"/>
     </row>
-    <row r="41" spans="1:25" ht="48">
+    <row r="41" spans="1:25" ht="36">
       <c r="A41" s="78">
         <v>55500012</v>
       </c>
@@ -12753,7 +12753,7 @@
       </c>
       <c r="Y41" s="54"/>
     </row>
-    <row r="42" spans="1:25" ht="48">
+    <row r="42" spans="1:25" ht="36">
       <c r="A42" s="78">
         <v>55500013</v>
       </c>
@@ -12802,7 +12802,7 @@
       </c>
       <c r="Y42" s="54"/>
     </row>
-    <row r="43" spans="1:25" ht="48">
+    <row r="43" spans="1:25" ht="36">
       <c r="A43" s="78">
         <v>55500014</v>
       </c>
@@ -12851,7 +12851,7 @@
       </c>
       <c r="Y43" s="70"/>
     </row>
-    <row r="44" spans="1:25" ht="48">
+    <row r="44" spans="1:25" ht="36">
       <c r="A44" s="78">
         <v>55500015</v>
       </c>
@@ -12900,7 +12900,7 @@
       </c>
       <c r="Y44" s="70"/>
     </row>
-    <row r="45" spans="1:25" ht="48">
+    <row r="45" spans="1:25" ht="36">
       <c r="A45" s="78">
         <v>55500016</v>
       </c>
@@ -12998,7 +12998,7 @@
       </c>
       <c r="Y46" s="52"/>
     </row>
-    <row r="47" spans="1:25" ht="168">
+    <row r="47" spans="1:25" ht="156">
       <c r="A47" s="77">
         <v>55900001</v>
       </c>
@@ -13057,7 +13057,7 @@
       </c>
       <c r="Y47" s="70"/>
     </row>
-    <row r="48" spans="1:25" ht="144">
+    <row r="48" spans="1:25" ht="132">
       <c r="A48" s="77">
         <v>55900002</v>
       </c>
@@ -13174,34 +13174,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y258"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C242" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R243" sqref="R243"/>
+      <selection pane="bottomRight" activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.21875" customWidth="1"/>
+    <col min="3" max="7" width="7.25" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
-    <col min="10" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="17.375" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="15" max="15" width="8.109375" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" customWidth="1"/>
-    <col min="18" max="18" width="23.44140625" customWidth="1"/>
+    <col min="15" max="15" width="8.125" customWidth="1"/>
+    <col min="16" max="16" width="7.375" customWidth="1"/>
+    <col min="17" max="17" width="6.375" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
     <col min="19" max="19" width="9" customWidth="1"/>
-    <col min="20" max="22" width="7.6640625" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" customWidth="1"/>
-    <col min="26" max="26" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="7.625" customWidth="1"/>
+    <col min="23" max="23" width="7.125" customWidth="1"/>
+    <col min="26" max="26" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="58.8">
+    <row r="1" spans="1:25" ht="55.5">
       <c r="A1" s="6" t="s">
         <v>647</v>
       </c>
@@ -13432,7 +13432,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="60">
+    <row r="4" spans="1:25" ht="48">
       <c r="A4">
         <v>55000002</v>
       </c>
@@ -13481,7 +13481,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="28.8">
+    <row r="5" spans="1:25" ht="27">
       <c r="A5">
         <v>55000021</v>
       </c>
@@ -13528,7 +13528,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="36">
+    <row r="6" spans="1:25" ht="24">
       <c r="A6">
         <v>55000029</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="48">
+    <row r="7" spans="1:25" ht="36">
       <c r="A7">
         <v>55000030</v>
       </c>
@@ -13628,7 +13628,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="36">
+    <row r="8" spans="1:25" ht="24">
       <c r="A8">
         <v>55000031</v>
       </c>
@@ -13679,7 +13679,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="36">
+    <row r="9" spans="1:25" ht="24">
       <c r="A9">
         <v>55000032</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="60">
+    <row r="11" spans="1:25" ht="48">
       <c r="A11">
         <v>55000034</v>
       </c>
@@ -13828,7 +13828,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="36">
+    <row r="12" spans="1:25" ht="24">
       <c r="A12">
         <v>55000035</v>
       </c>
@@ -13877,7 +13877,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="48">
+    <row r="13" spans="1:25" ht="36">
       <c r="A13">
         <v>55000036</v>
       </c>
@@ -13977,7 +13977,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="48">
+    <row r="15" spans="1:25" ht="36">
       <c r="A15">
         <v>55000038</v>
       </c>
@@ -14026,7 +14026,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="48">
+    <row r="16" spans="1:25" ht="36">
       <c r="A16">
         <v>55000039</v>
       </c>
@@ -14075,7 +14075,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="48">
+    <row r="17" spans="1:25" ht="36">
       <c r="A17">
         <v>55000040</v>
       </c>
@@ -14124,7 +14124,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="48">
+    <row r="18" spans="1:25" ht="36">
       <c r="A18">
         <v>55000041</v>
       </c>
@@ -14277,7 +14277,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="36">
+    <row r="21" spans="1:25" ht="24">
       <c r="A21">
         <v>55000044</v>
       </c>
@@ -14424,7 +14424,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="48">
+    <row r="24" spans="1:25" ht="36">
       <c r="A24">
         <v>55000047</v>
       </c>
@@ -14624,7 +14624,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="48">
+    <row r="28" spans="1:25" ht="36">
       <c r="A28">
         <v>55000061</v>
       </c>
@@ -14675,7 +14675,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="36">
+    <row r="29" spans="1:25" ht="24">
       <c r="A29">
         <v>55000062</v>
       </c>
@@ -14724,7 +14724,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="48">
+    <row r="30" spans="1:25" ht="36">
       <c r="A30">
         <v>55000063</v>
       </c>
@@ -15183,7 +15183,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="48">
+    <row r="39" spans="1:25" ht="36">
       <c r="A39">
         <v>55000073</v>
       </c>
@@ -15283,7 +15283,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="144">
+    <row r="41" spans="1:25" ht="120">
       <c r="A41">
         <v>55000075</v>
       </c>
@@ -15336,7 +15336,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="36">
+    <row r="42" spans="1:25" ht="24">
       <c r="A42">
         <v>55000076</v>
       </c>
@@ -15385,7 +15385,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="48">
+    <row r="43" spans="1:25" ht="36">
       <c r="A43">
         <v>55000077</v>
       </c>
@@ -15636,7 +15636,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="36">
+    <row r="48" spans="1:25" ht="24">
       <c r="A48">
         <v>55000082</v>
       </c>
@@ -15687,7 +15687,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="60">
+    <row r="49" spans="1:25" ht="48">
       <c r="A49">
         <v>55000083</v>
       </c>
@@ -15740,7 +15740,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="48">
+    <row r="50" spans="1:25" ht="36">
       <c r="A50">
         <v>55000085</v>
       </c>
@@ -15791,7 +15791,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="36">
+    <row r="51" spans="1:25" ht="24">
       <c r="A51">
         <v>55000087</v>
       </c>
@@ -15840,7 +15840,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="36">
+    <row r="52" spans="1:25" ht="24">
       <c r="A52">
         <v>55000088</v>
       </c>
@@ -16036,7 +16036,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="48">
+    <row r="56" spans="1:25" ht="36">
       <c r="A56">
         <v>55000092</v>
       </c>
@@ -16089,7 +16089,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="36">
+    <row r="57" spans="1:25" ht="24">
       <c r="A57">
         <v>55000093</v>
       </c>
@@ -16138,7 +16138,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="36">
+    <row r="58" spans="1:25" ht="24">
       <c r="A58">
         <v>55000094</v>
       </c>
@@ -16187,7 +16187,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="36">
+    <row r="59" spans="1:25" ht="24">
       <c r="A59">
         <v>55000095</v>
       </c>
@@ -16236,7 +16236,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="108">
+    <row r="60" spans="1:25" ht="84">
       <c r="A60">
         <v>55000096</v>
       </c>
@@ -16285,7 +16285,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="60">
+    <row r="61" spans="1:25" ht="48">
       <c r="A61">
         <v>55000097</v>
       </c>
@@ -16336,7 +16336,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="120">
+    <row r="62" spans="1:25" ht="96">
       <c r="A62">
         <v>55000098</v>
       </c>
@@ -16499,7 +16499,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="24">
+    <row r="65" spans="1:25">
       <c r="A65">
         <v>55000102</v>
       </c>
@@ -16595,7 +16595,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="120">
+    <row r="67" spans="1:25" ht="96">
       <c r="A67">
         <v>55000105</v>
       </c>
@@ -16658,7 +16658,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="72">
+    <row r="68" spans="1:25" ht="48">
       <c r="A68">
         <v>55000106</v>
       </c>
@@ -16709,7 +16709,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="48">
+    <row r="69" spans="1:25" ht="36">
       <c r="A69">
         <v>55000107</v>
       </c>
@@ -16809,7 +16809,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="36">
+    <row r="71" spans="1:25" ht="24">
       <c r="A71">
         <v>55000110</v>
       </c>
@@ -17011,7 +17011,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="36">
+    <row r="75" spans="1:25" ht="24">
       <c r="A75">
         <v>55000114</v>
       </c>
@@ -17060,7 +17060,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="48">
+    <row r="76" spans="1:25" ht="36">
       <c r="A76">
         <v>55000115</v>
       </c>
@@ -17113,7 +17113,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="72">
+    <row r="77" spans="1:25" ht="60">
       <c r="A77">
         <v>55000117</v>
       </c>
@@ -17266,7 +17266,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="36">
+    <row r="80" spans="1:25" ht="24">
       <c r="A80">
         <v>55000120</v>
       </c>
@@ -17315,7 +17315,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="36">
+    <row r="81" spans="1:25" ht="24">
       <c r="A81">
         <v>55000121</v>
       </c>
@@ -17368,7 +17368,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="48">
+    <row r="82" spans="1:25" ht="36">
       <c r="A82">
         <v>55000122</v>
       </c>
@@ -17419,7 +17419,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="83" spans="1:25" ht="48">
+    <row r="83" spans="1:25" ht="36">
       <c r="A83">
         <v>55000123</v>
       </c>
@@ -17570,7 +17570,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="60">
+    <row r="86" spans="1:25" ht="48">
       <c r="A86">
         <v>55000126</v>
       </c>
@@ -17713,7 +17713,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="89" spans="1:25" ht="36">
+    <row r="89" spans="1:25" ht="24">
       <c r="A89">
         <v>55000131</v>
       </c>
@@ -17809,7 +17809,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="91" spans="1:25" ht="144">
+    <row r="91" spans="1:25" ht="120">
       <c r="A91">
         <v>55000133</v>
       </c>
@@ -17866,7 +17866,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="92" spans="1:25" ht="48">
+    <row r="92" spans="1:25" ht="36">
       <c r="A92">
         <v>55000135</v>
       </c>
@@ -17915,7 +17915,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="93" spans="1:25" ht="36">
+    <row r="93" spans="1:25" ht="24">
       <c r="A93">
         <v>55000136</v>
       </c>
@@ -18613,7 +18613,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="36">
+    <row r="107" spans="1:25" ht="24">
       <c r="A107">
         <v>55000150</v>
       </c>
@@ -19064,7 +19064,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="116" spans="1:25" ht="48">
+    <row r="116" spans="1:25" ht="36">
       <c r="A116">
         <v>55000159</v>
       </c>
@@ -19115,7 +19115,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="117" spans="1:25" ht="36">
+    <row r="117" spans="1:25" ht="24">
       <c r="A117">
         <v>55000160</v>
       </c>
@@ -19164,7 +19164,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="60">
+    <row r="118" spans="1:25" ht="48">
       <c r="A118">
         <v>55000161</v>
       </c>
@@ -19266,7 +19266,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="120" spans="1:25" ht="48">
+    <row r="120" spans="1:25" ht="36">
       <c r="A120">
         <v>55000163</v>
       </c>
@@ -19321,7 +19321,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="121" spans="1:25" ht="48">
+    <row r="121" spans="1:25" ht="36">
       <c r="A121">
         <v>55000164</v>
       </c>
@@ -19370,7 +19370,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="122" spans="1:25" ht="36">
+    <row r="122" spans="1:25" ht="24">
       <c r="A122">
         <v>55000165</v>
       </c>
@@ -19470,7 +19470,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="124" spans="1:25" ht="36">
+    <row r="124" spans="1:25" ht="24">
       <c r="A124">
         <v>55000167</v>
       </c>
@@ -19521,7 +19521,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="125" spans="1:25" ht="84">
+    <row r="125" spans="1:25" ht="72">
       <c r="A125">
         <v>55000168</v>
       </c>
@@ -19572,7 +19572,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="126" spans="1:25" ht="72">
+    <row r="126" spans="1:25" ht="60">
       <c r="A126">
         <v>55000169</v>
       </c>
@@ -19723,7 +19723,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="129" spans="1:25" ht="48">
+    <row r="129" spans="1:25" ht="36">
       <c r="A129">
         <v>55000172</v>
       </c>
@@ -19774,7 +19774,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="130" spans="1:25" ht="48">
+    <row r="130" spans="1:25" ht="36">
       <c r="A130">
         <v>55000173</v>
       </c>
@@ -19825,7 +19825,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="131" spans="1:25" ht="48">
+    <row r="131" spans="1:25" ht="36">
       <c r="A131">
         <v>55000174</v>
       </c>
@@ -19982,7 +19982,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="134" spans="1:25" ht="48">
+    <row r="134" spans="1:25" ht="36">
       <c r="A134">
         <v>55000180</v>
       </c>
@@ -20035,7 +20035,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="135" spans="1:25" ht="36">
+    <row r="135" spans="1:25" ht="24">
       <c r="A135">
         <v>55000181</v>
       </c>
@@ -20084,7 +20084,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="136" spans="1:25" ht="36">
+    <row r="136" spans="1:25" ht="24">
       <c r="A136">
         <v>55000182</v>
       </c>
@@ -20137,7 +20137,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="137" spans="1:25" ht="96">
+    <row r="137" spans="1:25" ht="84">
       <c r="A137">
         <v>55000183</v>
       </c>
@@ -20292,7 +20292,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="140" spans="1:25" ht="48">
+    <row r="140" spans="1:25" ht="36">
       <c r="A140">
         <v>55000186</v>
       </c>
@@ -20343,7 +20343,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="141" spans="1:25" ht="60">
+    <row r="141" spans="1:25" ht="48">
       <c r="A141">
         <v>55000187</v>
       </c>
@@ -20441,7 +20441,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="143" spans="1:25" ht="48">
+    <row r="143" spans="1:25" ht="36">
       <c r="A143">
         <v>55000189</v>
       </c>
@@ -20494,7 +20494,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="144" spans="1:25" ht="48">
+    <row r="144" spans="1:25" ht="36">
       <c r="A144">
         <v>55000190</v>
       </c>
@@ -20545,7 +20545,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="145" spans="1:25" ht="60">
+    <row r="145" spans="1:25" ht="48">
       <c r="A145">
         <v>55000191</v>
       </c>
@@ -20598,7 +20598,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="146" spans="1:25" ht="72">
+    <row r="146" spans="1:25" ht="60">
       <c r="A146">
         <v>55000192</v>
       </c>
@@ -20649,7 +20649,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="147" spans="1:25" ht="36">
+    <row r="147" spans="1:25" ht="24">
       <c r="A147">
         <v>55000193</v>
       </c>
@@ -20751,7 +20751,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="149" spans="1:25" ht="72">
+    <row r="149" spans="1:25" ht="60">
       <c r="A149">
         <v>55000195</v>
       </c>
@@ -20800,7 +20800,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="150" spans="1:25" ht="72">
+    <row r="150" spans="1:25" ht="60">
       <c r="A150">
         <v>55000196</v>
       </c>
@@ -20849,7 +20849,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="151" spans="1:25" ht="36">
+    <row r="151" spans="1:25" ht="24">
       <c r="A151">
         <v>55000197</v>
       </c>
@@ -21247,7 +21247,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="159" spans="1:25" ht="132">
+    <row r="159" spans="1:25" ht="96">
       <c r="A159">
         <v>55000206</v>
       </c>
@@ -21349,7 +21349,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="161" spans="1:25" ht="60">
+    <row r="161" spans="1:25" ht="48">
       <c r="A161">
         <v>55000210</v>
       </c>
@@ -21555,7 +21555,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="165" spans="1:25" ht="36">
+    <row r="165" spans="1:25" ht="24">
       <c r="A165">
         <v>55000214</v>
       </c>
@@ -21604,7 +21604,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="166" spans="1:25" ht="120">
+    <row r="166" spans="1:25" ht="96">
       <c r="A166">
         <v>55000215</v>
       </c>
@@ -21667,7 +21667,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="167" spans="1:25" ht="48">
+    <row r="167" spans="1:25" ht="36">
       <c r="A167">
         <v>55000216</v>
       </c>
@@ -21867,7 +21867,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="171" spans="1:25" ht="48">
+    <row r="171" spans="1:25" ht="36">
       <c r="A171">
         <v>55000220</v>
       </c>
@@ -21918,7 +21918,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="172" spans="1:25" ht="48">
+    <row r="172" spans="1:25" ht="36">
       <c r="A172">
         <v>55000222</v>
       </c>
@@ -21969,7 +21969,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="173" spans="1:25" ht="36">
+    <row r="173" spans="1:25" ht="24">
       <c r="A173">
         <v>55000227</v>
       </c>
@@ -22069,7 +22069,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="175" spans="1:25" ht="36">
+    <row r="175" spans="1:25" ht="24">
       <c r="A175">
         <v>55000229</v>
       </c>
@@ -22120,7 +22120,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="176" spans="1:25" ht="36">
+    <row r="176" spans="1:25" ht="24">
       <c r="A176">
         <v>55000230</v>
       </c>
@@ -22218,7 +22218,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="178" spans="1:25" ht="60">
+    <row r="178" spans="1:25" ht="48">
       <c r="A178">
         <v>55000232</v>
       </c>
@@ -22267,7 +22267,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="179" spans="1:25" ht="48">
+    <row r="179" spans="1:25" ht="36">
       <c r="A179">
         <v>55000233</v>
       </c>
@@ -22316,7 +22316,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="180" spans="1:25" ht="48">
+    <row r="180" spans="1:25" ht="36">
       <c r="A180">
         <v>55000234</v>
       </c>
@@ -22367,7 +22367,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="181" spans="1:25" ht="84">
+    <row r="181" spans="1:25" ht="72">
       <c r="A181">
         <v>55000235</v>
       </c>
@@ -22416,7 +22416,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="182" spans="1:25" ht="36">
+    <row r="182" spans="1:25" ht="24">
       <c r="A182">
         <v>55000236</v>
       </c>
@@ -22608,7 +22608,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="186" spans="1:25" ht="108">
+    <row r="186" spans="1:25" ht="96">
       <c r="A186">
         <v>55000240</v>
       </c>
@@ -22722,7 +22722,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="188" spans="1:25" ht="36">
+    <row r="188" spans="1:25" ht="24">
       <c r="A188">
         <v>55000242</v>
       </c>
@@ -22822,7 +22822,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="190" spans="1:25" ht="120">
+    <row r="190" spans="1:25" ht="96">
       <c r="A190">
         <v>55000244</v>
       </c>
@@ -22885,7 +22885,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="191" spans="1:25" ht="36">
+    <row r="191" spans="1:25" ht="24">
       <c r="A191">
         <v>55000245</v>
       </c>
@@ -22985,7 +22985,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="193" spans="1:25" ht="72">
+    <row r="193" spans="1:25" ht="48">
       <c r="A193">
         <v>55000247</v>
       </c>
@@ -23036,7 +23036,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="194" spans="1:25" ht="48">
+    <row r="194" spans="1:25" ht="36">
       <c r="A194">
         <v>55000248</v>
       </c>
@@ -23089,7 +23089,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="195" spans="1:25" ht="36">
+    <row r="195" spans="1:25" ht="24">
       <c r="A195">
         <v>55000249</v>
       </c>
@@ -23140,7 +23140,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="196" spans="1:25" ht="48">
+    <row r="196" spans="1:25" ht="36">
       <c r="A196">
         <v>55000250</v>
       </c>
@@ -23189,7 +23189,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="197" spans="1:25" ht="28.8">
+    <row r="197" spans="1:25" ht="27">
       <c r="A197">
         <v>55000251</v>
       </c>
@@ -23485,7 +23485,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="203" spans="1:25" ht="48">
+    <row r="203" spans="1:25" ht="36">
       <c r="A203">
         <v>55000257</v>
       </c>
@@ -23538,7 +23538,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="204" spans="1:25" ht="36">
+    <row r="204" spans="1:25" ht="24">
       <c r="A204">
         <v>55000258</v>
       </c>
@@ -23587,7 +23587,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="205" spans="1:25" ht="48">
+    <row r="205" spans="1:25" ht="36">
       <c r="A205">
         <v>55000259</v>
       </c>
@@ -23640,7 +23640,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="206" spans="1:25" ht="108">
+    <row r="206" spans="1:25" ht="84">
       <c r="A206">
         <v>55000260</v>
       </c>
@@ -23699,7 +23699,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="207" spans="1:25" ht="96">
+    <row r="207" spans="1:25" ht="84">
       <c r="A207">
         <v>55000261</v>
       </c>
@@ -23748,7 +23748,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="208" spans="1:25" ht="36">
+    <row r="208" spans="1:25" ht="24">
       <c r="A208">
         <v>55000262</v>
       </c>
@@ -23850,7 +23850,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="210" spans="1:25" ht="48">
+    <row r="210" spans="1:25" ht="36">
       <c r="A210">
         <v>55000264</v>
       </c>
@@ -23901,7 +23901,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="211" spans="1:25" ht="48">
+    <row r="211" spans="1:25" ht="36">
       <c r="A211">
         <v>55000265</v>
       </c>
@@ -24246,7 +24246,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="218" spans="1:25" ht="36">
+    <row r="218" spans="1:25" ht="24">
       <c r="A218">
         <v>55000272</v>
       </c>
@@ -24295,7 +24295,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="219" spans="1:25" ht="48">
+    <row r="219" spans="1:25" ht="36">
       <c r="A219">
         <v>55000273</v>
       </c>
@@ -24344,7 +24344,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="220" spans="1:25" ht="96">
+    <row r="220" spans="1:25" ht="84">
       <c r="A220">
         <v>55000274</v>
       </c>
@@ -24393,7 +24393,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="221" spans="1:25" ht="48">
+    <row r="221" spans="1:25" ht="36">
       <c r="A221">
         <v>55000275</v>
       </c>
@@ -24444,7 +24444,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="222" spans="1:25" ht="48">
+    <row r="222" spans="1:25" ht="36">
       <c r="A222">
         <v>55000276</v>
       </c>
@@ -24495,7 +24495,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="223" spans="1:25" ht="24">
+    <row r="223" spans="1:25">
       <c r="A223">
         <v>55000277</v>
       </c>
@@ -24593,7 +24593,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="225" spans="1:25" ht="48">
+    <row r="225" spans="1:25" ht="36">
       <c r="A225">
         <v>55000280</v>
       </c>
@@ -24691,7 +24691,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="227" spans="1:25" ht="180">
+    <row r="227" spans="1:25" ht="144">
       <c r="A227">
         <v>55000282</v>
       </c>
@@ -24750,7 +24750,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="228" spans="1:25" ht="48">
+    <row r="228" spans="1:25" ht="36">
       <c r="A228">
         <v>55000284</v>
       </c>
@@ -25003,7 +25003,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="233" spans="1:25" ht="144">
+    <row r="233" spans="1:25" ht="120">
       <c r="A233">
         <v>55000289</v>
       </c>
@@ -25060,7 +25060,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="234" spans="1:25" ht="96">
+    <row r="234" spans="1:25" ht="84">
       <c r="A234">
         <v>55000290</v>
       </c>
@@ -25109,7 +25109,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="235" spans="1:25" ht="84">
+    <row r="235" spans="1:25" ht="60">
       <c r="A235">
         <v>55000291</v>
       </c>
@@ -25158,7 +25158,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="236" spans="1:25" ht="48">
+    <row r="236" spans="1:25" ht="36">
       <c r="A236">
         <v>55000292</v>
       </c>
@@ -25211,7 +25211,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="237" spans="1:25" ht="60">
+    <row r="237" spans="1:25" ht="48">
       <c r="A237">
         <v>55000293</v>
       </c>
@@ -25260,7 +25260,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="238" spans="1:25" ht="120">
+    <row r="238" spans="1:25" ht="96">
       <c r="A238">
         <v>55000294</v>
       </c>
@@ -25417,7 +25417,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="241" spans="1:25" ht="36">
+    <row r="241" spans="1:25" ht="24">
       <c r="A241">
         <v>55000299</v>
       </c>
@@ -25470,7 +25470,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="242" spans="1:25" ht="120">
+    <row r="242" spans="1:25" ht="96">
       <c r="A242">
         <v>55000324</v>
       </c>
@@ -25533,7 +25533,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="243" spans="1:25" ht="120">
+    <row r="243" spans="1:25" ht="96">
       <c r="A243">
         <v>55000325</v>
       </c>
@@ -25596,7 +25596,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="244" spans="1:25" ht="108">
+    <row r="244" spans="1:25" ht="96">
       <c r="A244">
         <v>55000326</v>
       </c>
@@ -25659,7 +25659,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="245" spans="1:25" ht="120">
+    <row r="245" spans="1:25" ht="96">
       <c r="A245">
         <v>55000327</v>
       </c>
@@ -25720,7 +25720,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="246" spans="1:25" ht="120">
+    <row r="246" spans="1:25" ht="96">
       <c r="A246">
         <v>55000328</v>
       </c>
@@ -25783,7 +25783,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="247" spans="1:25" ht="120">
+    <row r="247" spans="1:25" ht="96">
       <c r="A247">
         <v>55000329</v>
       </c>
@@ -25846,7 +25846,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="248" spans="1:25" ht="108">
+    <row r="248" spans="1:25" ht="96">
       <c r="A248">
         <v>55000330</v>
       </c>
@@ -25909,7 +25909,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="249" spans="1:25" ht="120">
+    <row r="249" spans="1:25" ht="96">
       <c r="A249">
         <v>55000331</v>
       </c>
@@ -25972,7 +25972,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="250" spans="1:25" ht="96">
+    <row r="250" spans="1:25" ht="72">
       <c r="A250">
         <v>55000332</v>
       </c>
@@ -26021,7 +26021,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="251" spans="1:25" ht="228">
+    <row r="251" spans="1:25" ht="180">
       <c r="A251">
         <v>55000333</v>
       </c>
@@ -26070,7 +26070,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="252" spans="1:25" ht="108">
+    <row r="252" spans="1:25" ht="96">
       <c r="A252">
         <v>55000334</v>
       </c>
@@ -26133,7 +26133,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="253" spans="1:25" ht="96">
+    <row r="253" spans="1:25" ht="84">
       <c r="A253">
         <v>55000335</v>
       </c>
@@ -26190,7 +26190,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="254" spans="1:25" ht="48">
+    <row r="254" spans="1:25" ht="36">
       <c r="A254">
         <v>55000340</v>
       </c>
@@ -26243,7 +26243,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="255" spans="1:25" ht="36">
+    <row r="255" spans="1:25" ht="24">
       <c r="A255">
         <v>55000341</v>
       </c>
@@ -26294,7 +26294,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="256" spans="1:25" ht="180">
+    <row r="256" spans="1:25" ht="144">
       <c r="A256">
         <v>55000342</v>
       </c>
@@ -26351,7 +26351,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="257" spans="1:25" ht="180">
+    <row r="257" spans="1:25" ht="144">
       <c r="A257">
         <v>55000343</v>
       </c>
@@ -26479,23 +26479,23 @@
       <selection pane="bottomRight" activeCell="G1" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.21875" customWidth="1"/>
-    <col min="8" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="22.21875" customWidth="1"/>
-    <col min="14" max="15" width="8.44140625" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" customWidth="1"/>
-    <col min="18" max="18" width="23.44140625" customWidth="1"/>
-    <col min="19" max="19" width="6.6640625" customWidth="1"/>
-    <col min="20" max="22" width="7.6640625" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" customWidth="1"/>
+    <col min="3" max="7" width="7.25" customWidth="1"/>
+    <col min="8" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="22.25" customWidth="1"/>
+    <col min="14" max="15" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="7.375" customWidth="1"/>
+    <col min="17" max="17" width="6.375" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="19" width="6.625" customWidth="1"/>
+    <col min="20" max="22" width="7.625" customWidth="1"/>
+    <col min="23" max="23" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="58.8">
+    <row r="1" spans="1:25" ht="55.5">
       <c r="A1" s="6" t="s">
         <v>647</v>
       </c>
@@ -26773,7 +26773,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="96">
+    <row r="5" spans="1:25" ht="84">
       <c r="A5">
         <v>55010004</v>
       </c>
@@ -26844,23 +26844,23 @@
       <selection pane="bottomRight" activeCell="G1" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.75" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.21875" customWidth="1"/>
-    <col min="8" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="22.21875" customWidth="1"/>
-    <col min="14" max="15" width="8.44140625" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" customWidth="1"/>
-    <col min="18" max="18" width="23.44140625" customWidth="1"/>
-    <col min="19" max="19" width="6.6640625" customWidth="1"/>
-    <col min="20" max="22" width="7.6640625" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" customWidth="1"/>
+    <col min="3" max="7" width="7.25" customWidth="1"/>
+    <col min="8" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="22.25" customWidth="1"/>
+    <col min="14" max="15" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="7.375" customWidth="1"/>
+    <col min="17" max="17" width="6.375" customWidth="1"/>
+    <col min="18" max="18" width="23.5" customWidth="1"/>
+    <col min="19" max="19" width="6.625" customWidth="1"/>
+    <col min="20" max="22" width="7.625" customWidth="1"/>
+    <col min="23" max="23" width="7.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="58.8">
+    <row r="1" spans="1:25" ht="55.5">
       <c r="A1" s="6" t="s">
         <v>647</v>
       </c>
@@ -27091,7 +27091,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="48">
+    <row r="4" spans="1:25" ht="36">
       <c r="A4">
         <v>55020001</v>
       </c>
@@ -27142,7 +27142,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="48">
+    <row r="5" spans="1:25" ht="36">
       <c r="A5">
         <v>55020002</v>
       </c>
@@ -27193,7 +27193,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="48">
+    <row r="6" spans="1:25" ht="36">
       <c r="A6">
         <v>55020003</v>
       </c>
@@ -27244,7 +27244,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="48">
+    <row r="7" spans="1:25" ht="36">
       <c r="A7">
         <v>55020004</v>
       </c>
@@ -27295,7 +27295,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="48">
+    <row r="8" spans="1:25" ht="36">
       <c r="A8">
         <v>55020005</v>
       </c>
@@ -27344,7 +27344,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="48">
+    <row r="9" spans="1:25" ht="36">
       <c r="A9">
         <v>55020006</v>
       </c>
@@ -27393,7 +27393,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="48">
+    <row r="10" spans="1:25" ht="36">
       <c r="A10">
         <v>55020007</v>
       </c>
@@ -27444,7 +27444,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="48">
+    <row r="11" spans="1:25" ht="36">
       <c r="A11">
         <v>55020008</v>
       </c>
@@ -27495,7 +27495,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="48">
+    <row r="12" spans="1:25" ht="36">
       <c r="A12">
         <v>55020009</v>
       </c>
@@ -27546,7 +27546,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="48">
+    <row r="13" spans="1:25" ht="36">
       <c r="A13">
         <v>55020010</v>
       </c>
@@ -27597,7 +27597,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="48">
+    <row r="14" spans="1:25" ht="36">
       <c r="A14">
         <v>55020011</v>
       </c>
@@ -27648,7 +27648,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="48">
+    <row r="15" spans="1:25" ht="36">
       <c r="A15">
         <v>55020012</v>
       </c>
@@ -27699,7 +27699,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="48">
+    <row r="16" spans="1:25" ht="36">
       <c r="A16">
         <v>55020013</v>
       </c>
@@ -27748,7 +27748,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="48">
+    <row r="17" spans="1:25" ht="36">
       <c r="A17">
         <v>55020014</v>
       </c>
@@ -27797,7 +27797,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="48">
+    <row r="18" spans="1:25" ht="36">
       <c r="A18">
         <v>55020015</v>
       </c>
@@ -27848,7 +27848,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="48">
+    <row r="19" spans="1:25" ht="36">
       <c r="A19">
         <v>55020016</v>
       </c>
@@ -27918,9 +27918,9 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -28510,7 +28510,7 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
#10 update the monster attr
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="7" r:id="rId1"/>
@@ -2914,11 +2914,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>对野兽造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>damage.SetPDamageRate(2);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>对野兽造成200%伤害</t>
+    <t>对恶魔造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对龙族造成200%伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -2926,1064 +2934,1056 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>对恶魔造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对龙族造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>damage.SetPDamageRate(2);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>对机械造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>damage.SetPDamageRate(2);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>对机械造成200%伤害</t>
+    <t>对爬行造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>净化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>驱逐</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsRace("Devil")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsRace("Machine")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsRace("Bird")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对鸟类造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>惊弓</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinggong</t>
+  </si>
+  <si>
+    <t>d.IsRace("Goblin")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsRace("Totem")</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对地精造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对图腾造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yanwu</t>
+  </si>
+  <si>
+    <t>烟雾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhendang</t>
+  </si>
+  <si>
+    <t>震荡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkinvasion</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>水球</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>waterball2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NER</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuiqiu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortRandom().Top(3)) s.AddMissile(mon, "waterball");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命低于30%时降低50%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.AddHp(-s.Atk*0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk.Source*=1.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次命中目标永久提高10%攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>猛砍</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>guangdian</t>
+  </si>
+  <si>
+    <t>光点</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(4,51000019);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(4,51000008);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(1,51000141);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每2回合在前方召唤一个哥布林</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每2回合在前方召唤一个光精灵射手</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每3回合在上下各召唤一个骷髅守卫</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000101,lv,"A").AddRace("Undead");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>墓地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mudi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkinvasion</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(1.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.AddBuff(56000201,lv,1.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddBuff(56000201,lv,1.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.HpRate&lt;=30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.HpRate&lt;=35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命低于35%时提高50%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>孢子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在自身四周各召唤一个粉球</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(2,51000205);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每2.5回合在周围随机位置召唤一个跳跳菇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鱼群</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yuqun</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(2,51000018);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每2回合在周围随机位置召唤一个鱼人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特殊标记</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲锋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rush</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以布置到整张地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>chongfeng</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣盾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shengdun</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddBuff(56000202,lv,99);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时给自己添加圣盾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>双子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>溅射</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘲讽</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐藏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yincang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>chaofeng</t>
+  </si>
+  <si>
+    <t>jianshe</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuangzi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>taunt</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hide</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>更不容易成为敌方目标</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>更容易成为敌方目标</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(5,51013000);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时会复制一个自身</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后对1卡片距离敌人造成50%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后对1卡片距离敌人造成同等伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,d.Position)) o.AddHp(-damage.Value);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon(2,s.CardId);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000007,lv,"A");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔免</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAntiMagic("All",100);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>coverstar</t>
+  </si>
+  <si>
+    <t>coverstar</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后使其石化99回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后使其睡眠1回合(不造成伤害)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后使其诅咒1回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后使其恐惧1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其混乱1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其中毒1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其致盲1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其晕眩1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其静止1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其麻痹1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其削弱1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其冰冻1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其灼伤1回合</t>
+  </si>
+  <si>
+    <t>击中目标后使其流血1回合</t>
+  </si>
+  <si>
+    <t>buff添加的技能=buff*0.5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckDamage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>nodef=true;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>无视目标防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成长</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标时自身混乱1回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddBuff(56000006,lv,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>受到攻击时使攻击者晕眩1回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后使其恐惧、削弱1回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死敌人后回复30%生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>射术</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次击中目标永久提升1点命中</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Hit.Source+=1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>凶恶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死敌人后吸收其30%攻击和生命上限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怨铃</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死敌人提高10%攻击和生命上限</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成长</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>掩体</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yanti</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圈套</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>quantao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>地主</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在支援地形提高30%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在支援地形降低30%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在支援地形降低60%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0.4);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dizhu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>尸毒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>venom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死一个单位后自杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillAfterHitEffectDelegate</t>
+  </si>
+  <si>
+    <t>SkillAfterHitEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死后判定</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeathHit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddHpRate(0.3);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000001,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000002,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000003,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000004,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000006,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000007,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000009,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000010,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000011,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000012,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000013,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000014,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000018,lv,99);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000019,lv,1);</t>
+  </si>
+  <si>
+    <t>s.AddBuff(56000012,lv,1);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000003,lv,1);d.AddBuff(56000004,lv,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk.Source+=d.Atk.Source*0.3;s.AddMaxHp(d.MaxHp.Source*0.3);</t>
+  </si>
+  <si>
+    <t>s.Atk.Source*=1.1;s.AddMaxHp(s.MaxHp.Source*0.1);</t>
+  </si>
+  <si>
+    <t>s.AddHp(-s.Hp);</t>
+  </si>
+  <si>
+    <t>毁灭</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) s.Transform(mon.CardId);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时对凶手造成自身最大生命30%的伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddHp(-d.MaxHp*0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魂守</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时永久增加0-50%攻击和防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk.Source*=MathTool.GetRandom(1f,1.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.StealWeapon(d);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>盗取</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>破甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>破坏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>25分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>20分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>灵性</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用本系卷轴造成额外30%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetMDamageRate(1.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AttackType==s.Attr&amp;&amp;s.HasScroll</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通魔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AttackType==0</t>
+  </si>
+  <si>
+    <t>攻击默认为自身属性魔法攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yuanbao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>元爆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mattack</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖刺</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反弹20%所受伤害(自己仍受到100%伤害)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>欺压</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>猎杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(1.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Star&gt;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对星级低于3的敌人造成150%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对星级高于5的敌人造成150%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>武装</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wuzhuang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sidekicker</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以为其他单位提供支援</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>援护</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sidekickee</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以令其他单位提供支援</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>空灵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.AddMaxHp(o.MaxHp.Source*0.15);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时提高所有无属性单位15%最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillInitialEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectArea</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂液体</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>venom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时使周围单位基础攻击力变为基础生命的1/5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>扭曲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>亡眼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击追加10%最大生命伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.AddPDamage(d.MaxHp.Source*0.10);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>威严</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.WeaponId&gt;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打造</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡后装备武器返回召唤师手牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.WeaponReturn();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>幻化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEF</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时对选定目标造成魔法伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时对最近的3个敌人造成伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortDistance(true).Top(1)) mon.OnMagicDamage(s.Atk.Source*1.5,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillDamageEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillBurstCheckDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>气化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>躲闪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit-=20;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>!isMelee</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>受到远程单位攻击提高20%回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>重生</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>chongsheng</t>
+  </si>
+  <si>
+    <t>生命值低于30%时直接回复所有生命值（cd5回合）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变形</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckSpecial</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Transform(MathTool.GetRandom(51000001,51000300));</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Transform((MathTool.GetRandom(2) == 0) ? 51000001 : 51000047);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddActionRate(0.3);d.AddActionRate(-0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>乱刃</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奏乐</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000002,lv,"E");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔王</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id)) o.MadDrug();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(s.Attr)){o.AddMaxHp(o.MaxHp.Source*0.2);o.Atk*=0.2;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时永久提高同属性单位20%最大生命值和攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mowang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.AddPDamage(s.GetMonsterCountByType(2)*10-10);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反弹所有物理攻击(自己不承受伤害)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反弹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddHp(-damage.NoDefenceValue);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Owner.AddMana(s,1,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣光</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>闪击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Spd&gt;d.Spd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对速度低于自身的单位造成130%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>虚无</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit-=40;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命满时拥有40%额外回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>招架</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>抵挡50%伤害，但会永久降低5%攻击力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0.5);d.Atk.Source*=0.95;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>立场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时减少对方召唤师1点LP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时回复召唤师1点MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Transform(51000114);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对爬行造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>净化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>驱逐</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsRace("Devil")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsRace("Machine")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsRace("Bird")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对鸟类造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>惊弓</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>jinggong</t>
-  </si>
-  <si>
-    <t>d.IsRace("Goblin")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsRace("Totem")</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对地精造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对图腾造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yanwu</t>
-  </si>
-  <si>
-    <t>烟雾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhendang</t>
-  </si>
-  <si>
-    <t>震荡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkinvasion</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>水球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>waterball2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NER</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuiqiu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortRandom().Top(3)) s.AddMissile(mon, "waterball");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命低于30%时降低50%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.AddHp(-s.Atk*0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk.Source*=1.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次命中目标永久提高10%攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>猛砍</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>guangdian</t>
-  </si>
-  <si>
-    <t>光点</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon(4,51000019);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon(4,51000008);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon(1,51000141);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每2回合在前方召唤一个哥布林</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每2回合在前方召唤一个光精灵射手</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每3回合在上下各召唤一个骷髅守卫</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000101,lv,"A").AddRace("Undead");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>墓地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mudi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkinvasion</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(1.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.AddBuff(56000201,lv,1.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddBuff(56000201,lv,1.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.HpRate&lt;=30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.HpRate&lt;=35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命低于35%时提高50%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>孢子</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在自身四周各召唤一个粉球</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon(2,51000205);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每2.5回合在周围随机位置召唤一个跳跳菇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>鱼群</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yuqun</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon(2,51000018);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每2回合在周围随机位置召唤一个鱼人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>特殊标记</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tag</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冲锋</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>rush</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以布置到整张地图</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>chongfeng</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣盾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shengdun</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddBuff(56000202,lv,99);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时给自己添加圣盾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>双子</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>溅射</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>嘲讽</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>隐藏</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yincang</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>chaofeng</t>
-  </si>
-  <si>
-    <t>jianshe</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuangzi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>taunt</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hide</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>更不容易成为敌方目标</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>更容易成为敌方目标</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon(5,51013000);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时会复制一个自身</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后对1卡片距离敌人造成50%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后对1卡片距离敌人造成同等伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,d.Position)) o.AddHp(-damage.Value);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon(2,s.CardId);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000007,lv,"A");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔免</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAntiMagic("All",100);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>coverstar</t>
-  </si>
-  <si>
-    <t>coverstar</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后使其石化99回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后使其睡眠1回合(不造成伤害)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后使其诅咒1回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后使其恐惧1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其混乱1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其中毒1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其致盲1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其晕眩1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其静止1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其麻痹1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其削弱1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其冰冻1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其灼伤1回合</t>
-  </si>
-  <si>
-    <t>击中目标后使其流血1回合</t>
-  </si>
-  <si>
-    <t>buff添加的技能=buff*0.5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CheckDamage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>nodef=true;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>无视目标防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>成长</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标时自身混乱1回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddBuff(56000006,lv,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>受到攻击时使攻击者晕眩1回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后使其恐惧、削弱1回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>杀死敌人后回复30%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>射术</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次击中目标永久提升1点命中</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Hit.Source+=1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>凶恶</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>杀死敌人后吸收其30%攻击和生命上限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>怨铃</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>杀死敌人提高10%攻击和生命上限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>成长</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>掩体</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yanti</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圈套</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>quantao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>地主</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在支援地形提高30%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在支援地形降低30%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在支援地形降低60%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0.4);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dizhu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>尸毒</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>venom</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>杀死一个单位后自杀</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillAfterHitEffectDelegate</t>
-  </si>
-  <si>
-    <t>SkillAfterHitEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>杀死后判定</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeathHit</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddHpRate(0.3);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000001,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000002,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000003,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000004,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000006,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000007,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000009,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000010,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000011,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000012,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000013,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000014,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000018,lv,99);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000019,lv,1);</t>
-  </si>
-  <si>
-    <t>s.AddBuff(56000012,lv,1);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000003,lv,1);d.AddBuff(56000004,lv,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk.Source+=d.Atk.Source*0.3;s.AddMaxHp(d.MaxHp.Source*0.3);</t>
-  </si>
-  <si>
-    <t>s.Atk.Source*=1.1;s.AddMaxHp(s.MaxHp.Source*0.1);</t>
-  </si>
-  <si>
-    <t>s.AddHp(-s.Hp);</t>
-  </si>
-  <si>
-    <t>毁灭</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) s.Transform(mon.CardId);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时对凶手造成自身最大生命30%的伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddHp(-d.MaxHp*0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魂守</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时永久增加0-50%攻击和防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk.Source*=MathTool.GetRandom(1f,1.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.StealWeapon(d);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>盗取</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>破甲</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>破坏</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>25分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>20分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>灵性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用本系卷轴造成额外30%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetMDamageRate(1.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AttackType==s.Attr&amp;&amp;s.HasScroll</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>通魔</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AttackType==0</t>
-  </si>
-  <si>
-    <t>攻击默认为自身属性魔法攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yuanbao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>元爆</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mattack</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>尖刺</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反弹20%所受伤害(自己仍受到100%伤害)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>欺压</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>猎杀</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(1.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Star&gt;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对星级低于3的敌人造成150%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对星级高于5的敌人造成150%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>探索</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>武装</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wuzhuang</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sidekicker</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以为其他单位提供支援</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>援护</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sidekickee</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以令其他单位提供支援</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>空灵</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.AddMaxHp(o.MaxHp.Source*0.15);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时提高所有无属性单位15%最大生命值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillInitialEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EffectArea</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>狂液体</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>venom</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时使周围单位基础攻击力变为基础生命的1/5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>扭曲</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>亡眼</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击追加10%最大生命伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.AddPDamage(d.MaxHp.Source*0.10);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>威严</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.WeaponId&gt;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打造</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡后装备武器返回召唤师手牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.WeaponReturn();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>幻化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时对选定目标造成魔法伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时对最近的3个敌人造成伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortDistance(true).Top(1)) mon.OnMagicDamage(s.Atk.Source*1.5,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillDamageEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillBurstCheckDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>气化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>躲闪</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit-=20;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>!isMelee</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>受到远程单位攻击提高20%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>重生</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>chongsheng</t>
-  </si>
-  <si>
-    <t>生命值低于30%时直接回复所有生命值（cd5回合）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>变形</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>进化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CheckSpecial</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Transform(MathTool.GetRandom(51000001,51000300));</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Transform(51000097);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Transform((MathTool.GetRandom(2) == 0) ? 51000001 : 51000047);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddActionRate(0.3);d.AddActionRate(-0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>乱刃</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奏乐</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000002,lv,"E");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔王</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id)) o.MadDrug();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NFR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(s.Attr)){o.AddMaxHp(o.MaxHp.Source*0.2);o.Atk*=0.2;}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时永久提高同属性单位20%最大生命值和攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mowang</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.AddPDamage(s.GetMonsterCountByType(2)*10-10);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反弹所有物理攻击(自己不承受伤害)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反弹</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddHp(-damage.NoDefenceValue);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Owner.AddMana(s,1,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣光</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>闪击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Spd&gt;d.Spd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对速度低于自身的单位造成130%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>虚无</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit-=40;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命满时拥有40%额外回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>招架</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>抵挡50%伤害，但会永久降低5%攻击力</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0.5);d.Atk.Source*=0.95;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>立场</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时减少对方召唤师1点LP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时回复召唤师1点MP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9081,12 +9081,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C70" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9096,7 +9096,8 @@
     <col min="3" max="7" width="7.21875" customWidth="1"/>
     <col min="8" max="8" width="21.21875" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" customWidth="1"/>
-    <col min="10" max="12" width="8.44140625" customWidth="1"/>
+    <col min="10" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
     <col min="13" max="14" width="22.21875" customWidth="1"/>
     <col min="15" max="15" width="14.88671875" customWidth="1"/>
     <col min="16" max="16" width="8.44140625" customWidth="1"/>
@@ -9128,7 +9129,7 @@
         <v>668</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>324</v>
@@ -9149,7 +9150,7 @@
         <v>392</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>422</v>
@@ -9208,10 +9209,10 @@
         <v>667</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>452</v>
@@ -9226,10 +9227,10 @@
         <v>444</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>399</v>
@@ -9288,7 +9289,7 @@
         <v>666</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>532</v>
@@ -9309,10 +9310,10 @@
         <v>391</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>615</v>
@@ -9333,7 +9334,7 @@
         <v>426</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>458</v>
@@ -9415,13 +9416,13 @@
       <c r="H5" s="32"/>
       <c r="I5" s="32"/>
       <c r="J5" s="31" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
@@ -9434,7 +9435,7 @@
         <v>313</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="T5" s="40">
         <v>0</v>
@@ -9467,13 +9468,13 @@
       <c r="H6" s="32"/>
       <c r="I6" s="32"/>
       <c r="J6" s="31" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
@@ -9486,7 +9487,7 @@
         <v>313</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="T6" s="10">
         <v>0</v>
@@ -9507,7 +9508,7 @@
         <v>55100004</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
@@ -9517,7 +9518,7 @@
       <c r="F7" s="47"/>
       <c r="G7" s="63"/>
       <c r="H7" s="32" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="I7" s="32"/>
       <c r="J7" s="31"/>
@@ -9534,7 +9535,7 @@
         <v>313</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="T7" s="10">
         <v>56000202</v>
@@ -9546,7 +9547,7 @@
         <v>15</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="Z7" s="41"/>
     </row>
@@ -9555,7 +9556,7 @@
         <v>55100005</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>449</v>
@@ -9564,7 +9565,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="47"/>
       <c r="G8" s="63" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="32"/>
@@ -9582,7 +9583,7 @@
         <v>313</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="T8" s="10">
         <v>0</v>
@@ -9594,7 +9595,7 @@
         <v>35</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="Z8" s="41"/>
     </row>
@@ -9603,17 +9604,17 @@
         <v>55100006</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="65"/>
       <c r="F9" s="66"/>
       <c r="G9" s="63"/>
       <c r="H9" s="32" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I9" s="67"/>
       <c r="J9" s="68"/>
@@ -9630,7 +9631,7 @@
         <v>313</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="T9" s="10">
         <v>0</v>
@@ -9642,7 +9643,7 @@
         <v>45</v>
       </c>
       <c r="Y9" s="27" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="Z9" s="74"/>
     </row>
@@ -9651,7 +9652,7 @@
         <v>55100007</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>108</v>
@@ -9669,12 +9670,12 @@
       <c r="H10" s="32"/>
       <c r="I10" s="32"/>
       <c r="J10" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="17"/>
       <c r="M10" s="17" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="21"/>
@@ -9686,7 +9687,7 @@
         <v>313</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="T10" s="10">
         <v>0</v>
@@ -9698,7 +9699,7 @@
         <v>35</v>
       </c>
       <c r="Y10" s="27" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="Z10" s="52"/>
     </row>
@@ -9707,7 +9708,7 @@
         <v>55100008</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>449</v>
@@ -9716,7 +9717,7 @@
       <c r="E11" s="27"/>
       <c r="F11" s="48"/>
       <c r="G11" s="63" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
@@ -9734,7 +9735,7 @@
         <v>313</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="T11" s="10">
         <v>0</v>
@@ -9746,7 +9747,7 @@
         <v>15</v>
       </c>
       <c r="Y11" s="27" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="Z11" s="52"/>
     </row>
@@ -9755,7 +9756,7 @@
         <v>55100009</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>449</v>
@@ -9764,7 +9765,7 @@
       <c r="E12" s="27"/>
       <c r="F12" s="48"/>
       <c r="G12" s="63" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
@@ -9782,7 +9783,7 @@
         <v>313</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="T12" s="10">
         <v>0</v>
@@ -9794,7 +9795,7 @@
         <v>15</v>
       </c>
       <c r="Y12" s="27" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="Z12" s="52"/>
     </row>
@@ -9803,7 +9804,7 @@
         <v>55100010</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>44</v>
@@ -9813,7 +9814,7 @@
       <c r="F13" s="47"/>
       <c r="G13" s="63"/>
       <c r="H13" s="32" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="31"/>
@@ -9838,7 +9839,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="X13" s="1">
         <v>5</v>
@@ -9853,7 +9854,7 @@
         <v>55100011</v>
       </c>
       <c r="B14" s="55" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>44</v>
@@ -9865,11 +9866,11 @@
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="31" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="17" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -9882,7 +9883,7 @@
         <v>313</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="T14" s="10">
         <v>0</v>
@@ -9903,7 +9904,7 @@
         <v>55100012</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>450</v>
@@ -9940,7 +9941,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="X15" s="1">
         <v>15</v>
@@ -9955,7 +9956,7 @@
         <v>55100013</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>44</v>
@@ -9964,7 +9965,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="47"/>
       <c r="G16" s="63" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
@@ -9982,7 +9983,7 @@
         <v>313</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="T16" s="1">
         <v>0</v>
@@ -9994,7 +9995,7 @@
         <v>10</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="Z16" s="41"/>
     </row>
@@ -10003,7 +10004,7 @@
         <v>55100014</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>464</v>
@@ -10067,7 +10068,7 @@
       <c r="J18" s="31"/>
       <c r="K18" s="18"/>
       <c r="L18" s="17" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
@@ -10080,7 +10081,7 @@
         <v>313</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="T18" s="10">
         <v>0</v>
@@ -10117,7 +10118,7 @@
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="O19" s="21"/>
       <c r="P19" s="45"/>
@@ -10128,7 +10129,7 @@
         <v>313</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="T19" s="10">
         <v>0</v>
@@ -10197,7 +10198,7 @@
         <v>55110004</v>
       </c>
       <c r="B21" s="79" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
@@ -10207,7 +10208,7 @@
       <c r="F21" s="47"/>
       <c r="G21" s="63"/>
       <c r="H21" s="32" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="31"/>
@@ -10224,7 +10225,7 @@
         <v>313</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="T21" s="10">
         <v>0</v>
@@ -10245,7 +10246,7 @@
         <v>55110005</v>
       </c>
       <c r="B22" s="79" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>40</v>
@@ -10257,7 +10258,7 @@
       <c r="H22" s="32"/>
       <c r="I22" s="32"/>
       <c r="J22" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K22" s="18"/>
       <c r="L22" s="17"/>
@@ -10274,7 +10275,7 @@
         <v>313</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="T22" s="14">
         <v>0</v>
@@ -10295,7 +10296,7 @@
         <v>55110006</v>
       </c>
       <c r="B23" s="79" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>1</v>
@@ -10311,7 +10312,7 @@
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="17" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -10324,7 +10325,7 @@
         <v>313</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T23" s="10">
         <v>0</v>
@@ -10345,7 +10346,7 @@
         <v>55110007</v>
       </c>
       <c r="B24" s="79" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
@@ -10357,11 +10358,11 @@
       <c r="H24" s="32"/>
       <c r="I24" s="32"/>
       <c r="J24" s="31" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="K24" s="18"/>
       <c r="L24" s="17" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -10374,7 +10375,7 @@
         <v>313</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="T24" s="10">
         <v>0</v>
@@ -10395,7 +10396,7 @@
         <v>55110008</v>
       </c>
       <c r="B25" s="79" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -10443,7 +10444,7 @@
         <v>55110009</v>
       </c>
       <c r="B26" s="79" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -10457,7 +10458,7 @@
       <c r="J26" s="31"/>
       <c r="K26" s="18"/>
       <c r="L26" s="17" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
@@ -10470,7 +10471,7 @@
         <v>313</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="T26" s="10">
         <v>0</v>
@@ -10491,7 +10492,7 @@
         <v>55110010</v>
       </c>
       <c r="B27" s="79" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>40</v>
@@ -10503,7 +10504,7 @@
       <c r="H27" s="32"/>
       <c r="I27" s="32"/>
       <c r="J27" s="31" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="K27" s="18"/>
       <c r="L27" s="17" t="s">
@@ -10541,7 +10542,7 @@
         <v>55110011</v>
       </c>
       <c r="B28" s="79" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>40</v>
@@ -10553,10 +10554,10 @@
       <c r="H28" s="32"/>
       <c r="I28" s="32"/>
       <c r="J28" s="31" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
@@ -10570,7 +10571,7 @@
         <v>313</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="T28" s="10">
         <v>0</v>
@@ -10591,7 +10592,7 @@
         <v>55110012</v>
       </c>
       <c r="B29" s="79" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>1</v>
@@ -10606,7 +10607,7 @@
       <c r="K29" s="18"/>
       <c r="L29" s="17"/>
       <c r="M29" s="17" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="N29" s="17"/>
       <c r="O29" s="21"/>
@@ -10639,7 +10640,7 @@
         <v>55110013</v>
       </c>
       <c r="B30" s="79" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>40</v>
@@ -10651,14 +10652,14 @@
       <c r="H30" s="32"/>
       <c r="I30" s="32"/>
       <c r="J30" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K30" s="18"/>
       <c r="L30" s="17" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="N30" s="17"/>
       <c r="O30" s="21"/>
@@ -10670,7 +10671,7 @@
         <v>313</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="T30" s="10">
         <v>0</v>
@@ -10691,7 +10692,7 @@
         <v>55110014</v>
       </c>
       <c r="B31" s="79" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>40</v>
@@ -10739,7 +10740,7 @@
         <v>55110015</v>
       </c>
       <c r="B32" s="79" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>1</v>
@@ -10751,7 +10752,7 @@
       <c r="H32" s="32"/>
       <c r="I32" s="32"/>
       <c r="J32" s="31" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="K32" s="18"/>
       <c r="L32" s="17" t="s">
@@ -10768,7 +10769,7 @@
         <v>313</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="T32" s="10">
         <v>0</v>
@@ -10789,7 +10790,7 @@
         <v>55110016</v>
       </c>
       <c r="B33" s="79" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>40</v>
@@ -10804,7 +10805,7 @@
         <v>389</v>
       </c>
       <c r="K33" s="18" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="17"/>
@@ -10818,7 +10819,7 @@
         <v>313</v>
       </c>
       <c r="S33" s="10" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="T33" s="10">
         <v>0</v>
@@ -10839,7 +10840,7 @@
         <v>55110017</v>
       </c>
       <c r="B34" s="79" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>40</v>
@@ -10853,7 +10854,7 @@
       <c r="J34" s="31"/>
       <c r="K34" s="18"/>
       <c r="L34" s="17" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
@@ -10866,7 +10867,7 @@
         <v>313</v>
       </c>
       <c r="S34" s="10" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="T34" s="10">
         <v>0</v>
@@ -10887,7 +10888,7 @@
         <v>55110018</v>
       </c>
       <c r="B35" s="79" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>40</v>
@@ -10960,7 +10961,7 @@
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
       <c r="O36" s="21" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="P36" s="45">
         <v>1</v>
@@ -10999,13 +11000,13 @@
         <v>55200002</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>108</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E37" s="27">
         <v>30</v>
@@ -11015,7 +11016,7 @@
       </c>
       <c r="G37" s="64"/>
       <c r="H37" s="32" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="31"/>
@@ -11032,13 +11033,13 @@
         <v>313</v>
       </c>
       <c r="S37" s="16" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="T37" s="27">
         <v>0</v>
       </c>
       <c r="U37" s="27" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="V37" s="27"/>
       <c r="W37" s="27"/>
@@ -11046,7 +11047,7 @@
         <v>15</v>
       </c>
       <c r="Y37" s="27" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Z37" s="43"/>
     </row>
@@ -11061,7 +11062,7 @@
         <v>544</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E38" s="34">
         <v>30</v>
@@ -11071,7 +11072,7 @@
       </c>
       <c r="G38" s="64"/>
       <c r="H38" s="51" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I38" s="93"/>
       <c r="J38" s="95"/>
@@ -11088,7 +11089,7 @@
         <v>545</v>
       </c>
       <c r="S38" s="16" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="T38" s="34">
         <v>0</v>
@@ -11396,7 +11397,7 @@
         <v>0</v>
       </c>
       <c r="U44" s="27" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="V44" s="27"/>
       <c r="W44" s="27"/>
@@ -11529,7 +11530,7 @@
       <c r="L47" s="17"/>
       <c r="M47" s="17"/>
       <c r="N47" s="17" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="O47" s="21"/>
       <c r="P47" s="45"/>
@@ -11540,7 +11541,7 @@
         <v>313</v>
       </c>
       <c r="S47" s="10" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="T47" s="10">
         <v>0</v>
@@ -11588,7 +11589,7 @@
         <v>313</v>
       </c>
       <c r="S48" s="10" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="T48" s="10">
         <v>0</v>
@@ -11612,7 +11613,7 @@
         <v>611</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
@@ -11626,7 +11627,7 @@
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
       <c r="O49" s="21" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="P49" s="45">
         <v>2</v>
@@ -11638,7 +11639,7 @@
         <v>313</v>
       </c>
       <c r="S49" s="16" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="T49" s="27">
         <v>0</v>
@@ -11664,7 +11665,7 @@
         <v>434</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D50" s="27" t="s">
         <v>650</v>
@@ -11677,7 +11678,7 @@
       </c>
       <c r="G50" s="64"/>
       <c r="H50" s="51" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="I50" s="51"/>
       <c r="J50" s="28"/>
@@ -11694,7 +11695,7 @@
         <v>313</v>
       </c>
       <c r="S50" s="16" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="T50" s="27">
         <v>0</v>
@@ -11715,10 +11716,10 @@
         <v>55400003</v>
       </c>
       <c r="B51" s="58" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
@@ -11732,7 +11733,7 @@
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
       <c r="O51" s="21" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="P51" s="45">
         <v>2</v>
@@ -11744,7 +11745,7 @@
         <v>313</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="T51" s="27">
         <v>0</v>
@@ -11758,7 +11759,7 @@
         <v>80</v>
       </c>
       <c r="Y51" s="54" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="Z51" s="52"/>
     </row>
@@ -11767,10 +11768,10 @@
         <v>55400004</v>
       </c>
       <c r="B52" s="58" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D52" s="27"/>
       <c r="E52" s="27"/>
@@ -11784,7 +11785,7 @@
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
       <c r="O52" s="21" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="P52" s="45">
         <v>3</v>
@@ -11796,13 +11797,13 @@
         <v>313</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="T52" s="27">
         <v>0</v>
       </c>
       <c r="U52" s="27" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="V52" s="27"/>
       <c r="W52" s="27"/>
@@ -11810,7 +11811,7 @@
         <v>80</v>
       </c>
       <c r="Y52" s="54" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="Z52" s="52"/>
     </row>
@@ -11819,10 +11820,10 @@
         <v>55400005</v>
       </c>
       <c r="B53" s="58" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
@@ -11836,7 +11837,7 @@
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
       <c r="O53" s="21" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="P53" s="45">
         <v>2.5</v>
@@ -11848,7 +11849,7 @@
         <v>313</v>
       </c>
       <c r="S53" s="16" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="T53" s="27">
         <v>0</v>
@@ -11871,10 +11872,10 @@
         <v>55400006</v>
       </c>
       <c r="B54" s="58" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="27"/>
@@ -11888,7 +11889,7 @@
       <c r="M54" s="17"/>
       <c r="N54" s="17"/>
       <c r="O54" s="21" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="P54" s="45">
         <v>2</v>
@@ -11900,7 +11901,7 @@
         <v>313</v>
       </c>
       <c r="S54" s="16" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="T54" s="27">
         <v>0</v>
@@ -11914,7 +11915,7 @@
         <v>30</v>
       </c>
       <c r="Y54" s="54" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="Z54" s="52"/>
     </row>
@@ -11935,11 +11936,11 @@
       <c r="H55" s="51"/>
       <c r="I55" s="51"/>
       <c r="J55" s="28" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="K55" s="29"/>
       <c r="L55" s="33" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
@@ -11952,7 +11953,7 @@
         <v>313</v>
       </c>
       <c r="S55" s="16" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="T55" s="27">
         <v>0</v>
@@ -11985,11 +11986,11 @@
       <c r="H56" s="51"/>
       <c r="I56" s="51"/>
       <c r="J56" s="28" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="K56" s="29"/>
       <c r="L56" s="33" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="M56" s="17"/>
       <c r="N56" s="17"/>
@@ -12002,7 +12003,7 @@
         <v>313</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="T56" s="27">
         <v>0</v>
@@ -12023,7 +12024,7 @@
         <v>55500003</v>
       </c>
       <c r="B57" s="60" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C57" s="27" t="s">
         <v>4</v>
@@ -12139,7 +12140,7 @@
       </c>
       <c r="K59" s="29"/>
       <c r="L59" s="33" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
@@ -12152,7 +12153,7 @@
         <v>313</v>
       </c>
       <c r="S59" s="16" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T59" s="41">
         <v>0</v>
@@ -12173,7 +12174,7 @@
         <v>55500006</v>
       </c>
       <c r="B60" s="60" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C60" s="27" t="s">
         <v>4</v>
@@ -12185,11 +12186,11 @@
       <c r="H60" s="32"/>
       <c r="I60" s="32"/>
       <c r="J60" s="28" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="K60" s="29"/>
       <c r="L60" s="33" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="M60" s="17"/>
       <c r="N60" s="17"/>
@@ -12202,7 +12203,7 @@
         <v>313</v>
       </c>
       <c r="S60" s="16" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="T60" s="41">
         <v>0</v>
@@ -12214,7 +12215,7 @@
         <v>5</v>
       </c>
       <c r="Y60" s="27" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="Z60" s="43"/>
     </row>
@@ -12239,7 +12240,7 @@
       </c>
       <c r="K61" s="29"/>
       <c r="L61" s="33" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
@@ -12252,7 +12253,7 @@
         <v>313</v>
       </c>
       <c r="S61" s="16" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T61" s="41">
         <v>0</v>
@@ -12373,7 +12374,7 @@
         <v>55500010</v>
       </c>
       <c r="B64" s="60" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C64" s="27" t="s">
         <v>4</v>
@@ -12418,7 +12419,7 @@
       </c>
       <c r="Z64" s="43"/>
     </row>
-    <row r="65" spans="1:26" ht="48">
+    <row r="65" spans="1:26" ht="36">
       <c r="A65" s="60">
         <v>55500011</v>
       </c>
@@ -12439,7 +12440,7 @@
       </c>
       <c r="K65" s="29"/>
       <c r="L65" s="33" t="s">
-        <v>713</v>
+        <v>990</v>
       </c>
       <c r="M65" s="17"/>
       <c r="N65" s="17"/>
@@ -12452,7 +12453,7 @@
         <v>313</v>
       </c>
       <c r="S65" s="16" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="T65" s="41">
         <v>0</v>
@@ -12623,7 +12624,7 @@
         <v>55500015</v>
       </c>
       <c r="B69" s="60" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C69" s="27" t="s">
         <v>4</v>
@@ -12635,7 +12636,7 @@
       <c r="H69" s="51"/>
       <c r="I69" s="51"/>
       <c r="J69" s="28" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="K69" s="29"/>
       <c r="L69" s="33" t="s">
@@ -12652,7 +12653,7 @@
         <v>313</v>
       </c>
       <c r="S69" s="16" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="T69" s="27">
         <v>0</v>
@@ -12664,7 +12665,7 @@
         <v>5</v>
       </c>
       <c r="Y69" s="27" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="Z69" s="52"/>
     </row>
@@ -12673,7 +12674,7 @@
         <v>55500016</v>
       </c>
       <c r="B70" s="60" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C70" s="27" t="s">
         <v>4</v>
@@ -12685,7 +12686,7 @@
       <c r="H70" s="51"/>
       <c r="I70" s="51"/>
       <c r="J70" s="28" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="K70" s="29"/>
       <c r="L70" s="33" t="s">
@@ -12702,7 +12703,7 @@
         <v>313</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="T70" s="27">
         <v>0</v>
@@ -12714,7 +12715,7 @@
         <v>5</v>
       </c>
       <c r="Y70" s="27" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="Z70" s="52"/>
     </row>
@@ -12738,7 +12739,7 @@
       <c r="K71" s="18"/>
       <c r="L71" s="17"/>
       <c r="M71" s="17" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="N71" s="17"/>
       <c r="O71" s="21"/>
@@ -12750,7 +12751,7 @@
         <v>313</v>
       </c>
       <c r="S71" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="T71" s="1">
         <v>0</v>
@@ -12786,7 +12787,7 @@
       <c r="K72" s="18"/>
       <c r="L72" s="17"/>
       <c r="M72" s="17" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="N72" s="17"/>
       <c r="O72" s="21"/>
@@ -12798,7 +12799,7 @@
         <v>313</v>
       </c>
       <c r="S72" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="T72" s="1">
         <v>0</v>
@@ -12834,7 +12835,7 @@
       <c r="K73" s="18"/>
       <c r="L73" s="17"/>
       <c r="M73" s="17" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="N73" s="17"/>
       <c r="O73" s="21"/>
@@ -12846,7 +12847,7 @@
         <v>313</v>
       </c>
       <c r="S73" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="T73" s="1">
         <v>0</v>
@@ -12882,7 +12883,7 @@
       <c r="K74" s="18"/>
       <c r="L74" s="17"/>
       <c r="M74" s="17" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="N74" s="17"/>
       <c r="O74" s="21"/>
@@ -12894,7 +12895,7 @@
         <v>313</v>
       </c>
       <c r="S74" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="T74" s="1">
         <v>0</v>
@@ -12930,7 +12931,7 @@
       <c r="K75" s="18"/>
       <c r="L75" s="17"/>
       <c r="M75" s="17" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="N75" s="17"/>
       <c r="O75" s="21"/>
@@ -12939,10 +12940,10 @@
         <v>318</v>
       </c>
       <c r="R75" s="47" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="S75" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="T75" s="1">
         <v>0</v>
@@ -12978,7 +12979,7 @@
       <c r="K76" s="18"/>
       <c r="L76" s="17"/>
       <c r="M76" s="17" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="N76" s="17"/>
       <c r="O76" s="21"/>
@@ -12990,7 +12991,7 @@
         <v>313</v>
       </c>
       <c r="S76" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="T76" s="1">
         <v>0</v>
@@ -13026,7 +13027,7 @@
       <c r="K77" s="18"/>
       <c r="L77" s="17"/>
       <c r="M77" s="17" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="N77" s="17"/>
       <c r="O77" s="21"/>
@@ -13038,7 +13039,7 @@
         <v>313</v>
       </c>
       <c r="S77" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="T77" s="1">
         <v>0</v>
@@ -13074,7 +13075,7 @@
       <c r="K78" s="18"/>
       <c r="L78" s="17"/>
       <c r="M78" s="17" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="N78" s="17"/>
       <c r="O78" s="21"/>
@@ -13086,7 +13087,7 @@
         <v>313</v>
       </c>
       <c r="S78" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="T78" s="1">
         <v>0</v>
@@ -13122,7 +13123,7 @@
       <c r="K79" s="18"/>
       <c r="L79" s="17"/>
       <c r="M79" s="17" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="N79" s="17"/>
       <c r="O79" s="21"/>
@@ -13131,10 +13132,10 @@
         <v>318</v>
       </c>
       <c r="R79" s="47" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="S79" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="T79" s="1">
         <v>0</v>
@@ -13170,7 +13171,7 @@
       <c r="K80" s="18"/>
       <c r="L80" s="17"/>
       <c r="M80" s="17" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="N80" s="17"/>
       <c r="O80" s="21"/>
@@ -13179,10 +13180,10 @@
         <v>318</v>
       </c>
       <c r="R80" s="47" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="T80" s="1">
         <v>0</v>
@@ -13218,7 +13219,7 @@
       <c r="K81" s="18"/>
       <c r="L81" s="17"/>
       <c r="M81" s="17" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="N81" s="17"/>
       <c r="O81" s="21"/>
@@ -13230,7 +13231,7 @@
         <v>313</v>
       </c>
       <c r="S81" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="T81" s="1">
         <v>0</v>
@@ -13266,7 +13267,7 @@
       <c r="K82" s="18"/>
       <c r="L82" s="17"/>
       <c r="M82" s="17" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="N82" s="17"/>
       <c r="O82" s="21"/>
@@ -13278,7 +13279,7 @@
         <v>313</v>
       </c>
       <c r="S82" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="T82" s="1">
         <v>0</v>
@@ -13314,7 +13315,7 @@
       <c r="K83" s="18"/>
       <c r="L83" s="17"/>
       <c r="M83" s="17" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="N83" s="17"/>
       <c r="O83" s="21"/>
@@ -13326,7 +13327,7 @@
         <v>313</v>
       </c>
       <c r="S83" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="T83" s="1">
         <v>0</v>
@@ -13362,7 +13363,7 @@
       <c r="K84" s="18"/>
       <c r="L84" s="17"/>
       <c r="M84" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="N84" s="17"/>
       <c r="O84" s="21"/>
@@ -13374,7 +13375,7 @@
         <v>313</v>
       </c>
       <c r="S84" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="T84" s="1">
         <v>0</v>
@@ -13410,7 +13411,7 @@
       <c r="K85" s="18"/>
       <c r="L85" s="17"/>
       <c r="M85" s="17" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="N85" s="17"/>
       <c r="O85" s="21"/>
@@ -13422,7 +13423,7 @@
         <v>313</v>
       </c>
       <c r="S85" s="10" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="T85" s="10">
         <v>0</v>
@@ -13458,7 +13459,7 @@
       <c r="K86" s="18"/>
       <c r="L86" s="17"/>
       <c r="M86" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="N86" s="17"/>
       <c r="O86" s="21"/>
@@ -13470,7 +13471,7 @@
         <v>313</v>
       </c>
       <c r="S86" s="10" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="T86" s="10">
         <v>0</v>
@@ -13506,7 +13507,7 @@
       <c r="K87" s="18"/>
       <c r="L87" s="17"/>
       <c r="M87" s="17" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="N87" s="17"/>
       <c r="O87" s="21"/>
@@ -13518,7 +13519,7 @@
         <v>313</v>
       </c>
       <c r="S87" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="T87" s="10">
         <v>0</v>
@@ -13549,7 +13550,7 @@
       <c r="F88" s="47"/>
       <c r="G88" s="64"/>
       <c r="H88" s="32" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I88" s="32"/>
       <c r="J88" s="31"/>
@@ -13839,7 +13840,7 @@
         <v>55600007</v>
       </c>
       <c r="B94" s="62" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>54</v>
@@ -13999,7 +14000,7 @@
       <c r="F97" s="47"/>
       <c r="G97" s="64"/>
       <c r="H97" s="32" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="I97" s="32"/>
       <c r="J97" s="31"/>
@@ -14085,7 +14086,7 @@
         <v>55610002</v>
       </c>
       <c r="B99" s="80" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>52</v>
@@ -14114,7 +14115,7 @@
         <v>313</v>
       </c>
       <c r="S99" s="10" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="T99" s="10">
         <v>0</v>
@@ -14126,7 +14127,7 @@
         <v>5</v>
       </c>
       <c r="Y99" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="Z99" s="41"/>
     </row>
@@ -14135,7 +14136,7 @@
         <v>55610003</v>
       </c>
       <c r="B100" s="80" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>52</v>
@@ -14164,7 +14165,7 @@
         <v>313</v>
       </c>
       <c r="S100" s="10" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="T100" s="10">
         <v>0</v>
@@ -14176,7 +14177,7 @@
         <v>5</v>
       </c>
       <c r="Y100" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="Z100" s="41"/>
     </row>
@@ -14185,7 +14186,7 @@
         <v>55610004</v>
       </c>
       <c r="B101" s="80" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>52</v>
@@ -14201,7 +14202,7 @@
       </c>
       <c r="K101" s="18"/>
       <c r="L101" s="17" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="M101" s="17"/>
       <c r="N101" s="17"/>
@@ -14214,7 +14215,7 @@
         <v>313</v>
       </c>
       <c r="S101" s="10" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="T101" s="10">
         <v>0</v>
@@ -14226,7 +14227,7 @@
         <v>10</v>
       </c>
       <c r="Y101" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Z101" s="41"/>
     </row>
@@ -14235,10 +14236,10 @@
         <v>55700001</v>
       </c>
       <c r="B102" s="56" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -14250,7 +14251,7 @@
       <c r="K102" s="18"/>
       <c r="L102" s="17"/>
       <c r="M102" s="17" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="N102" s="17"/>
       <c r="O102" s="21"/>
@@ -14262,7 +14263,7 @@
         <v>313</v>
       </c>
       <c r="S102" s="10" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="T102" s="10">
         <v>0</v>
@@ -14277,7 +14278,7 @@
         <v>255</v>
       </c>
       <c r="Z102" s="41" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="103" spans="1:26">
@@ -14285,7 +14286,7 @@
         <v>55700002</v>
       </c>
       <c r="B103" s="56" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>151</v>
@@ -14300,7 +14301,7 @@
       <c r="K103" s="18"/>
       <c r="L103" s="17"/>
       <c r="M103" s="17" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="N103" s="17"/>
       <c r="O103" s="21"/>
@@ -14312,7 +14313,7 @@
         <v>313</v>
       </c>
       <c r="S103" s="10" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="T103" s="10">
         <v>0</v>
@@ -14327,7 +14328,7 @@
         <v>234</v>
       </c>
       <c r="Z103" s="41" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="104" spans="1:26" ht="36">
@@ -14335,7 +14336,7 @@
         <v>55700003</v>
       </c>
       <c r="B104" s="56" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>151</v>
@@ -14351,7 +14352,7 @@
       <c r="L104" s="17"/>
       <c r="M104" s="17"/>
       <c r="N104" s="17" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="O104" s="21"/>
       <c r="P104" s="45"/>
@@ -14362,7 +14363,7 @@
         <v>313</v>
       </c>
       <c r="S104" s="10" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="T104" s="10">
         <v>0</v>
@@ -14377,7 +14378,7 @@
         <v>174</v>
       </c>
       <c r="Z104" s="41" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="105" spans="1:26" ht="36">
@@ -14385,7 +14386,7 @@
         <v>55700004</v>
       </c>
       <c r="B105" s="56" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>151</v>
@@ -14401,7 +14402,7 @@
       <c r="L105" s="33"/>
       <c r="M105" s="17"/>
       <c r="N105" s="17" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="O105" s="21"/>
       <c r="P105" s="45"/>
@@ -14412,7 +14413,7 @@
         <v>313</v>
       </c>
       <c r="S105" s="10" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="T105" s="10">
         <v>0</v>
@@ -14427,7 +14428,7 @@
         <v>173</v>
       </c>
       <c r="Z105" s="27" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="106" spans="1:26" ht="120">
@@ -14451,7 +14452,7 @@
       </c>
       <c r="G106" s="64"/>
       <c r="H106" s="51" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I106" s="51"/>
       <c r="J106" s="28"/>
@@ -14511,7 +14512,7 @@
       </c>
       <c r="G107" s="64"/>
       <c r="H107" s="51" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I107" s="51"/>
       <c r="J107" s="28"/>
@@ -14599,7 +14600,7 @@
         <v>55900004</v>
       </c>
       <c r="B109" s="59" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C109" s="27" t="s">
         <v>0</v>
@@ -14615,7 +14616,7 @@
       <c r="L109" s="33"/>
       <c r="M109" s="17"/>
       <c r="N109" s="17" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="O109" s="21"/>
       <c r="P109" s="45"/>
@@ -14626,13 +14627,13 @@
         <v>313</v>
       </c>
       <c r="S109" s="16" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="T109" s="27">
         <v>0</v>
       </c>
       <c r="U109" s="27" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="V109" s="27"/>
       <c r="W109" s="27"/>
@@ -14649,7 +14650,7 @@
         <v>55900005</v>
       </c>
       <c r="B110" s="59" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C110" s="27" t="s">
         <v>0</v>
@@ -14665,7 +14666,7 @@
       <c r="L110" s="17"/>
       <c r="M110" s="17"/>
       <c r="N110" s="17" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="O110" s="21"/>
       <c r="P110" s="45"/>
@@ -14676,7 +14677,7 @@
         <v>313</v>
       </c>
       <c r="S110" s="53" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="T110" s="27">
         <v>0</v>
@@ -14697,7 +14698,7 @@
         <v>55900006</v>
       </c>
       <c r="B111" s="59" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>0</v>
@@ -14714,7 +14715,7 @@
       <c r="K111" s="18"/>
       <c r="L111" s="17"/>
       <c r="M111" s="17" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="N111" s="17"/>
       <c r="O111" s="21"/>
@@ -14747,7 +14748,7 @@
         <v>55900007</v>
       </c>
       <c r="B112" s="59" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>0</v>
@@ -14795,7 +14796,7 @@
         <v>55900008</v>
       </c>
       <c r="B113" s="59" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>0</v>
@@ -14843,7 +14844,7 @@
         <v>55900009</v>
       </c>
       <c r="B114" s="59" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>0</v>
@@ -14852,7 +14853,7 @@
       <c r="E114" s="1"/>
       <c r="F114" s="47"/>
       <c r="G114" s="64" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="H114" s="32"/>
       <c r="I114" s="32"/>
@@ -14870,7 +14871,7 @@
         <v>313</v>
       </c>
       <c r="S114" s="10" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="T114" s="10">
         <v>0</v>
@@ -14882,7 +14883,7 @@
         <v>30</v>
       </c>
       <c r="Y114" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="Z114" s="41"/>
     </row>
@@ -14891,7 +14892,7 @@
         <v>55900010</v>
       </c>
       <c r="B115" s="59" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>0</v>
@@ -14900,7 +14901,7 @@
       <c r="E115" s="1"/>
       <c r="F115" s="47"/>
       <c r="G115" s="64" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="H115" s="32"/>
       <c r="I115" s="32"/>
@@ -14918,7 +14919,7 @@
         <v>313</v>
       </c>
       <c r="S115" s="10" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="T115" s="1">
         <v>0</v>
@@ -14939,7 +14940,7 @@
         <v>55900011</v>
       </c>
       <c r="B116" s="59" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>0</v>
@@ -14949,7 +14950,7 @@
       <c r="F116" s="47"/>
       <c r="G116" s="64"/>
       <c r="H116" s="51" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="I116" s="51"/>
       <c r="J116" s="28"/>
@@ -14966,7 +14967,7 @@
         <v>313</v>
       </c>
       <c r="S116" s="10" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="T116" s="10">
         <v>0</v>
@@ -14987,7 +14988,7 @@
         <v>55900012</v>
       </c>
       <c r="B117" s="59" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C117" s="27" t="s">
         <v>449</v>
@@ -15003,7 +15004,7 @@
       </c>
       <c r="G117" s="64"/>
       <c r="H117" s="32" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="I117" s="32"/>
       <c r="J117" s="31"/>
@@ -15020,14 +15021,14 @@
         <v>313</v>
       </c>
       <c r="S117" s="16" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="T117" s="27">
         <v>0</v>
       </c>
       <c r="U117" s="27"/>
       <c r="V117" s="27" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="W117" s="27"/>
       <c r="X117" s="27">
@@ -15043,7 +15044,7 @@
         <v>55900013</v>
       </c>
       <c r="B118" s="59" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>0</v>
@@ -15055,7 +15056,7 @@
       <c r="H118" s="32"/>
       <c r="I118" s="32"/>
       <c r="J118" s="31" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="K118" s="18"/>
       <c r="L118" s="17" t="s">
@@ -15093,7 +15094,7 @@
         <v>55900014</v>
       </c>
       <c r="B119" s="59" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>0</v>
@@ -15111,7 +15112,7 @@
       <c r="L119" s="17"/>
       <c r="M119" s="17"/>
       <c r="N119" s="17" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="O119" s="21"/>
       <c r="P119" s="45"/>
@@ -15122,7 +15123,7 @@
         <v>313</v>
       </c>
       <c r="S119" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="T119" s="1">
         <v>0</v>
@@ -15143,7 +15144,7 @@
         <v>55900015</v>
       </c>
       <c r="B120" s="59" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>0</v>
@@ -15191,7 +15192,7 @@
         <v>55900016</v>
       </c>
       <c r="B121" s="59" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>449</v>
@@ -15222,7 +15223,7 @@
         <v>313</v>
       </c>
       <c r="S121" s="10" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="T121" s="10">
         <v>0</v>
@@ -15236,7 +15237,7 @@
         <v>45</v>
       </c>
       <c r="Y121" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Z121" s="52"/>
     </row>
@@ -15245,7 +15246,7 @@
         <v>55900017</v>
       </c>
       <c r="B122" s="59" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>449</v>
@@ -15262,7 +15263,7 @@
       <c r="M122" s="22"/>
       <c r="N122" s="22"/>
       <c r="O122" s="21" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="P122" s="45">
         <v>1</v>
@@ -15299,7 +15300,7 @@
         <v>55900018</v>
       </c>
       <c r="B123" s="59" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>449</v>
@@ -15316,7 +15317,7 @@
       <c r="M123" s="22"/>
       <c r="N123" s="22"/>
       <c r="O123" s="19" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="P123" s="45">
         <v>1</v>
@@ -15353,7 +15354,7 @@
         <v>55900019</v>
       </c>
       <c r="B124" s="59" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>449</v>
@@ -15370,7 +15371,7 @@
       <c r="M124" s="22"/>
       <c r="N124" s="22"/>
       <c r="O124" s="21" t="s">
-        <v>959</v>
+        <v>989</v>
       </c>
       <c r="P124" s="45">
         <v>1</v>
@@ -15407,13 +15408,13 @@
         <v>55900020</v>
       </c>
       <c r="B125" s="59" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C125" s="82" t="s">
         <v>449</v>
       </c>
       <c r="D125" s="27" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="E125" s="27">
         <v>30</v>
@@ -15423,7 +15424,7 @@
       </c>
       <c r="G125" s="83"/>
       <c r="H125" s="32" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="I125" s="92"/>
       <c r="J125" s="94"/>
@@ -15440,7 +15441,7 @@
         <v>313</v>
       </c>
       <c r="S125" s="10" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="T125" s="82">
         <v>0</v>
@@ -15452,7 +15453,7 @@
         <v>20</v>
       </c>
       <c r="Y125" s="27" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="Z125" s="87"/>
     </row>
@@ -15461,7 +15462,7 @@
         <v>55900021</v>
       </c>
       <c r="B126" s="59" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C126" s="27" t="s">
         <v>0</v>
@@ -15521,7 +15522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
@@ -15569,7 +15570,7 @@
         <v>668</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>324</v>
@@ -15590,7 +15591,7 @@
         <v>392</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>422</v>
@@ -15649,7 +15650,7 @@
         <v>667</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>581</v>
@@ -15658,19 +15659,19 @@
         <v>452</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>440</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>585</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>616</v>
@@ -15729,7 +15730,7 @@
         <v>666</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>580</v>
@@ -15744,13 +15745,13 @@
         <v>441</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>391</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>612</v>
@@ -15812,7 +15813,7 @@
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
       <c r="J4" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K4" s="18"/>
       <c r="L4" s="17"/>
@@ -15876,7 +15877,7 @@
       <c r="H5" s="32"/>
       <c r="I5" s="32"/>
       <c r="J5" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K5" s="18"/>
       <c r="L5" s="17"/>
@@ -16230,7 +16231,7 @@
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
       <c r="H12" s="32" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="31"/>
@@ -16658,7 +16659,7 @@
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
       <c r="J20" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K20" s="18"/>
       <c r="L20" s="17"/>
@@ -16918,7 +16919,7 @@
       <c r="H25" s="32"/>
       <c r="I25" s="32"/>
       <c r="J25" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K25" s="18"/>
       <c r="L25" s="17"/>
@@ -16982,7 +16983,7 @@
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
       <c r="J26" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K26" s="18"/>
       <c r="L26" s="17"/>
@@ -17256,7 +17257,7 @@
       <c r="H31" s="32"/>
       <c r="I31" s="32"/>
       <c r="J31" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K31" s="18"/>
       <c r="L31" s="17" t="s">
@@ -17694,7 +17695,7 @@
       <c r="H39" s="32"/>
       <c r="I39" s="32"/>
       <c r="J39" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K39" s="18"/>
       <c r="L39" s="17"/>
@@ -17806,7 +17807,7 @@
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
       <c r="J41" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K41" s="18"/>
       <c r="L41" s="17"/>
@@ -17870,7 +17871,7 @@
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
       <c r="J42" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K42" s="18"/>
       <c r="L42" s="17"/>
@@ -17887,7 +17888,7 @@
         <v>313</v>
       </c>
       <c r="S42" s="10" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="T42" s="10">
         <v>0</v>
@@ -17934,7 +17935,7 @@
       <c r="H43" s="32"/>
       <c r="I43" s="32"/>
       <c r="J43" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K43" s="18"/>
       <c r="L43" s="17"/>
@@ -17996,7 +17997,7 @@
       <c r="H44" s="32"/>
       <c r="I44" s="32"/>
       <c r="J44" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="17"/>
@@ -18060,7 +18061,7 @@
       <c r="H45" s="32"/>
       <c r="I45" s="32"/>
       <c r="J45" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K45" s="18"/>
       <c r="L45" s="17"/>
@@ -18124,7 +18125,7 @@
       <c r="H46" s="32"/>
       <c r="I46" s="32"/>
       <c r="J46" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K46" s="18"/>
       <c r="L46" s="17"/>
@@ -18184,7 +18185,7 @@
       <c r="J47" s="31"/>
       <c r="K47" s="18"/>
       <c r="L47" s="17" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -18286,7 +18287,7 @@
       <c r="H49" s="32"/>
       <c r="I49" s="32"/>
       <c r="J49" s="31" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K49" s="18"/>
       <c r="L49" s="17"/>
@@ -18443,7 +18444,7 @@
         <v>668</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>324</v>
@@ -18464,7 +18465,7 @@
         <v>392</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>422</v>
@@ -18523,7 +18524,7 @@
         <v>667</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>467</v>
@@ -18544,7 +18545,7 @@
         <v>542</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>399</v>
@@ -18603,7 +18604,7 @@
         <v>666</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>532</v>
@@ -18624,7 +18625,7 @@
         <v>391</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>423</v>
@@ -18771,7 +18772,7 @@
         <v>668</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>324</v>
@@ -18792,7 +18793,7 @@
         <v>392</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>422</v>
@@ -18851,7 +18852,7 @@
         <v>667</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>452</v>
@@ -18872,7 +18873,7 @@
         <v>542</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>399</v>
@@ -18931,7 +18932,7 @@
         <v>666</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>532</v>
@@ -18952,7 +18953,7 @@
         <v>391</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>423</v>
@@ -20397,7 +20398,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -20405,7 +20406,7 @@
         <v>493</v>
       </c>
       <c r="B32" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -20413,7 +20414,7 @@
         <v>513</v>
       </c>
       <c r="B33" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove some out monster
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="7" r:id="rId1"/>
@@ -437,7 +437,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="975">
   <si>
     <t>特殊</t>
   </si>
@@ -3898,10 +3898,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr("Water")){o.AddMaxHp(o.MaxHp.Source*0.2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>神射</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3918,6 +3914,26 @@
   </si>
   <si>
     <t>延长范围内敌方怪物负面状态2回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillAfterHitEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.AddCard(d.CardId, d.Level);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死目标后获得该卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>过牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(1)){o.AddMaxHp(o.MaxHp.Source*0.2);}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4259,6 +4275,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -8600,8 +8617,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z134" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114" tableBorderDxfId="113">
-  <autoFilter ref="A3:Z134"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z135" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114" tableBorderDxfId="113">
+  <autoFilter ref="A3:Z135"/>
   <sortState ref="A4:Z118">
     <sortCondition ref="A3:A118"/>
   </sortState>
@@ -9038,37 +9055,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z134"/>
+  <dimension ref="A1:Z135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C130" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="A134" sqref="A134"/>
+      <selection pane="bottomRight" activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.25" customWidth="1"/>
-    <col min="8" max="8" width="21.25" customWidth="1"/>
-    <col min="9" max="9" width="12.875" customWidth="1"/>
-    <col min="10" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="14" width="22.25" customWidth="1"/>
-    <col min="15" max="15" width="14.875" customWidth="1"/>
-    <col min="16" max="16" width="8.5" customWidth="1"/>
-    <col min="17" max="17" width="7.375" customWidth="1"/>
-    <col min="18" max="18" width="6.375" customWidth="1"/>
-    <col min="19" max="19" width="23.5" customWidth="1"/>
-    <col min="20" max="20" width="8.75" customWidth="1"/>
-    <col min="21" max="23" width="7.625" customWidth="1"/>
-    <col min="24" max="24" width="7.125" customWidth="1"/>
+    <col min="3" max="7" width="7.21875" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="14" width="22.21875" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" customWidth="1"/>
+    <col min="16" max="16" width="8.44140625" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" customWidth="1"/>
+    <col min="19" max="19" width="23.44140625" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" customWidth="1"/>
+    <col min="21" max="23" width="7.6640625" customWidth="1"/>
+    <col min="24" max="24" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="55.5">
+    <row r="1" spans="1:26" ht="58.8">
       <c r="A1" s="6" t="s">
         <v>295</v>
       </c>
@@ -9189,7 +9206,7 @@
         <v>814</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>813</v>
+        <v>970</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>386</v>
@@ -9358,7 +9375,7 @@
       </c>
       <c r="Z4" s="43"/>
     </row>
-    <row r="5" spans="1:26" ht="36">
+    <row r="5" spans="1:26" ht="48">
       <c r="A5" s="55">
         <v>55100002</v>
       </c>
@@ -9410,7 +9427,7 @@
       </c>
       <c r="Z5" s="41"/>
     </row>
-    <row r="6" spans="1:26" ht="36">
+    <row r="6" spans="1:26" ht="48">
       <c r="A6" s="55">
         <v>55100003</v>
       </c>
@@ -9558,7 +9575,7 @@
       </c>
       <c r="Z8" s="41"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="24">
       <c r="A9" s="55">
         <v>55100006</v>
       </c>
@@ -9606,7 +9623,7 @@
       </c>
       <c r="Z9" s="74"/>
     </row>
-    <row r="10" spans="1:26" ht="60">
+    <row r="10" spans="1:26" ht="72">
       <c r="A10" s="55">
         <v>55100007</v>
       </c>
@@ -9808,7 +9825,7 @@
       </c>
       <c r="Z13" s="41"/>
     </row>
-    <row r="14" spans="1:26" ht="48">
+    <row r="14" spans="1:26" ht="60">
       <c r="A14" s="55">
         <v>55100011</v>
       </c>
@@ -10152,7 +10169,7 @@
       </c>
       <c r="Z20" s="41"/>
     </row>
-    <row r="21" spans="1:26" ht="24">
+    <row r="21" spans="1:26" ht="36">
       <c r="A21" s="79">
         <v>55110004</v>
       </c>
@@ -10200,7 +10217,7 @@
       </c>
       <c r="Z21" s="41"/>
     </row>
-    <row r="22" spans="1:26" ht="24">
+    <row r="22" spans="1:26" ht="36">
       <c r="A22" s="79">
         <v>55110005</v>
       </c>
@@ -10250,7 +10267,7 @@
       </c>
       <c r="Z22" s="41"/>
     </row>
-    <row r="23" spans="1:26" ht="24">
+    <row r="23" spans="1:26" ht="36">
       <c r="A23" s="79">
         <v>55110006</v>
       </c>
@@ -10300,7 +10317,7 @@
       </c>
       <c r="Z23" s="52"/>
     </row>
-    <row r="24" spans="1:26" ht="24">
+    <row r="24" spans="1:26" ht="36">
       <c r="A24" s="79">
         <v>55110007</v>
       </c>
@@ -10446,7 +10463,7 @@
       </c>
       <c r="Z26" s="41"/>
     </row>
-    <row r="27" spans="1:26" ht="24">
+    <row r="27" spans="1:26" ht="36">
       <c r="A27" s="79">
         <v>55110010</v>
       </c>
@@ -10496,7 +10513,7 @@
       </c>
       <c r="Z27" s="41"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" ht="24">
       <c r="A28" s="79">
         <v>55110011</v>
       </c>
@@ -10546,7 +10563,7 @@
       </c>
       <c r="Z28" s="41"/>
     </row>
-    <row r="29" spans="1:26" ht="24">
+    <row r="29" spans="1:26" ht="36">
       <c r="A29" s="79">
         <v>55110012</v>
       </c>
@@ -10594,7 +10611,7 @@
       </c>
       <c r="Z29" s="41"/>
     </row>
-    <row r="30" spans="1:26" ht="24">
+    <row r="30" spans="1:26" ht="36">
       <c r="A30" s="79">
         <v>55110013</v>
       </c>
@@ -10646,7 +10663,7 @@
       </c>
       <c r="Z30" s="43"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" ht="24">
       <c r="A31" s="79">
         <v>55110014</v>
       </c>
@@ -10694,7 +10711,7 @@
       </c>
       <c r="Z31" s="41"/>
     </row>
-    <row r="32" spans="1:26" ht="24">
+    <row r="32" spans="1:26" ht="36">
       <c r="A32" s="79">
         <v>55110015</v>
       </c>
@@ -10794,7 +10811,7 @@
       </c>
       <c r="Z33" s="52"/>
     </row>
-    <row r="34" spans="1:26" ht="36">
+    <row r="34" spans="1:26" ht="48">
       <c r="A34" s="79">
         <v>55110017</v>
       </c>
@@ -10842,7 +10859,7 @@
       </c>
       <c r="Z34" s="52"/>
     </row>
-    <row r="35" spans="1:26" ht="24">
+    <row r="35" spans="1:26" ht="36">
       <c r="A35" s="79">
         <v>55110018</v>
       </c>
@@ -10894,7 +10911,7 @@
       </c>
       <c r="Z35" s="41"/>
     </row>
-    <row r="36" spans="1:26" ht="120">
+    <row r="36" spans="1:26" ht="132">
       <c r="A36" s="12">
         <v>55200001</v>
       </c>
@@ -10954,7 +10971,7 @@
       </c>
       <c r="Z36" s="52"/>
     </row>
-    <row r="37" spans="1:26" ht="84">
+    <row r="37" spans="1:26" ht="108">
       <c r="A37" s="77">
         <v>55200002</v>
       </c>
@@ -11010,7 +11027,7 @@
       </c>
       <c r="Z37" s="43"/>
     </row>
-    <row r="38" spans="1:26" ht="96">
+    <row r="38" spans="1:26" ht="108">
       <c r="A38" s="12">
         <v>55200003</v>
       </c>
@@ -11066,7 +11083,7 @@
       </c>
       <c r="Z38" s="27"/>
     </row>
-    <row r="39" spans="1:26" ht="120">
+    <row r="39" spans="1:26" ht="132">
       <c r="A39" s="77">
         <v>55200004</v>
       </c>
@@ -11124,7 +11141,7 @@
       </c>
       <c r="Z39" s="100"/>
     </row>
-    <row r="40" spans="1:26" ht="108">
+    <row r="40" spans="1:26" ht="132">
       <c r="A40" s="12">
         <v>55200005</v>
       </c>
@@ -11184,7 +11201,7 @@
       </c>
       <c r="Z40" s="52"/>
     </row>
-    <row r="41" spans="1:26" ht="48">
+    <row r="41" spans="1:26" ht="60">
       <c r="A41" s="57">
         <v>55300001</v>
       </c>
@@ -11436,7 +11453,7 @@
       </c>
       <c r="Z45" s="52"/>
     </row>
-    <row r="46" spans="1:26" ht="27">
+    <row r="46" spans="1:26" ht="28.8">
       <c r="A46" s="57">
         <v>55300006</v>
       </c>
@@ -11586,7 +11603,7 @@
       </c>
       <c r="Z48" s="52"/>
     </row>
-    <row r="49" spans="1:26">
+    <row r="49" spans="1:26" ht="24">
       <c r="A49" s="57">
         <v>55310002</v>
       </c>
@@ -11634,7 +11651,7 @@
       </c>
       <c r="Z49" s="41"/>
     </row>
-    <row r="50" spans="1:26">
+    <row r="50" spans="1:26" ht="24">
       <c r="A50" s="57">
         <v>55310003</v>
       </c>
@@ -11682,7 +11699,7 @@
       </c>
       <c r="Z50" s="41"/>
     </row>
-    <row r="51" spans="1:26" ht="27">
+    <row r="51" spans="1:26" ht="28.8">
       <c r="A51" s="58">
         <v>55400001</v>
       </c>
@@ -11734,7 +11751,7 @@
       </c>
       <c r="Z51" s="52"/>
     </row>
-    <row r="52" spans="1:26">
+    <row r="52" spans="1:26" ht="28.8">
       <c r="A52" s="58">
         <v>55400002</v>
       </c>
@@ -11788,7 +11805,7 @@
       </c>
       <c r="Z52" s="52"/>
     </row>
-    <row r="53" spans="1:26" ht="27">
+    <row r="53" spans="1:26" ht="28.8">
       <c r="A53" s="58">
         <v>55400003</v>
       </c>
@@ -11840,7 +11857,7 @@
       </c>
       <c r="Z53" s="52"/>
     </row>
-    <row r="54" spans="1:26" ht="27">
+    <row r="54" spans="1:26" ht="28.8">
       <c r="A54" s="58">
         <v>55400004</v>
       </c>
@@ -11892,7 +11909,7 @@
       </c>
       <c r="Z54" s="52"/>
     </row>
-    <row r="55" spans="1:26" ht="27">
+    <row r="55" spans="1:26" ht="28.8">
       <c r="A55" s="58">
         <v>55400005</v>
       </c>
@@ -11944,7 +11961,7 @@
       </c>
       <c r="Z55" s="52"/>
     </row>
-    <row r="56" spans="1:26" ht="27">
+    <row r="56" spans="1:26" ht="28.8">
       <c r="A56" s="58">
         <v>55400006</v>
       </c>
@@ -11996,7 +12013,7 @@
       </c>
       <c r="Z56" s="52"/>
     </row>
-    <row r="57" spans="1:26" ht="24">
+    <row r="57" spans="1:26" ht="36">
       <c r="A57" s="60">
         <v>55500001</v>
       </c>
@@ -12096,7 +12113,7 @@
       </c>
       <c r="Z58" s="52"/>
     </row>
-    <row r="59" spans="1:26" ht="24">
+    <row r="59" spans="1:26" ht="36">
       <c r="A59" s="60">
         <v>55500003</v>
       </c>
@@ -12146,7 +12163,7 @@
       </c>
       <c r="Z59" s="52"/>
     </row>
-    <row r="60" spans="1:26" ht="24">
+    <row r="60" spans="1:26" ht="36">
       <c r="A60" s="60">
         <v>55500004</v>
       </c>
@@ -12196,7 +12213,7 @@
       </c>
       <c r="Z60" s="52"/>
     </row>
-    <row r="61" spans="1:26" ht="24">
+    <row r="61" spans="1:26" ht="36">
       <c r="A61" s="60">
         <v>55500005</v>
       </c>
@@ -12246,7 +12263,7 @@
       </c>
       <c r="Z61" s="43"/>
     </row>
-    <row r="62" spans="1:26" ht="24">
+    <row r="62" spans="1:26" ht="36">
       <c r="A62" s="60">
         <v>55500006</v>
       </c>
@@ -12346,7 +12363,7 @@
       </c>
       <c r="Z63" s="43"/>
     </row>
-    <row r="64" spans="1:26" ht="24">
+    <row r="64" spans="1:26" ht="36">
       <c r="A64" s="60">
         <v>55500008</v>
       </c>
@@ -12396,7 +12413,7 @@
       </c>
       <c r="Z64" s="43"/>
     </row>
-    <row r="65" spans="1:26" ht="24">
+    <row r="65" spans="1:26" ht="36">
       <c r="A65" s="60">
         <v>55500009</v>
       </c>
@@ -12446,7 +12463,7 @@
       </c>
       <c r="Z65" s="43"/>
     </row>
-    <row r="66" spans="1:26" ht="24">
+    <row r="66" spans="1:26" ht="36">
       <c r="A66" s="60">
         <v>55500010</v>
       </c>
@@ -12496,7 +12513,7 @@
       </c>
       <c r="Z66" s="43"/>
     </row>
-    <row r="67" spans="1:26" ht="24">
+    <row r="67" spans="1:26" ht="36">
       <c r="A67" s="60">
         <v>55500011</v>
       </c>
@@ -12546,7 +12563,7 @@
       </c>
       <c r="Z67" s="43"/>
     </row>
-    <row r="68" spans="1:26" ht="24">
+    <row r="68" spans="1:26" ht="36">
       <c r="A68" s="60">
         <v>55500012</v>
       </c>
@@ -12646,7 +12663,7 @@
       </c>
       <c r="Z69" s="43"/>
     </row>
-    <row r="70" spans="1:26" ht="24">
+    <row r="70" spans="1:26" ht="36">
       <c r="A70" s="60">
         <v>55500014</v>
       </c>
@@ -12696,7 +12713,7 @@
       </c>
       <c r="Z70" s="52"/>
     </row>
-    <row r="71" spans="1:26" ht="24">
+    <row r="71" spans="1:26" ht="36">
       <c r="A71" s="60">
         <v>55500015</v>
       </c>
@@ -12746,7 +12763,7 @@
       </c>
       <c r="Z71" s="52"/>
     </row>
-    <row r="72" spans="1:26" ht="24">
+    <row r="72" spans="1:26" ht="36">
       <c r="A72" s="60">
         <v>55500016</v>
       </c>
@@ -13612,7 +13629,7 @@
       </c>
       <c r="Z89" s="27"/>
     </row>
-    <row r="90" spans="1:26" ht="24">
+    <row r="90" spans="1:26" ht="36">
       <c r="A90" s="61">
         <v>55600001</v>
       </c>
@@ -13662,7 +13679,7 @@
       </c>
       <c r="Z90" s="41"/>
     </row>
-    <row r="91" spans="1:26" ht="24">
+    <row r="91" spans="1:26" ht="36">
       <c r="A91" s="61">
         <v>55600002</v>
       </c>
@@ -13712,7 +13729,7 @@
       </c>
       <c r="Z91" s="41"/>
     </row>
-    <row r="92" spans="1:26" ht="24">
+    <row r="92" spans="1:26" ht="36">
       <c r="A92" s="61">
         <v>55600003</v>
       </c>
@@ -13762,7 +13779,7 @@
       </c>
       <c r="Z92" s="41"/>
     </row>
-    <row r="93" spans="1:26" ht="24">
+    <row r="93" spans="1:26" ht="36">
       <c r="A93" s="61">
         <v>55600004</v>
       </c>
@@ -13812,7 +13829,7 @@
       </c>
       <c r="Z93" s="41"/>
     </row>
-    <row r="94" spans="1:26" ht="24">
+    <row r="94" spans="1:26" ht="36">
       <c r="A94" s="61">
         <v>55600005</v>
       </c>
@@ -13862,7 +13879,7 @@
       </c>
       <c r="Z94" s="41"/>
     </row>
-    <row r="95" spans="1:26" ht="24">
+    <row r="95" spans="1:26" ht="36">
       <c r="A95" s="61">
         <v>55600006</v>
       </c>
@@ -14012,7 +14029,7 @@
       </c>
       <c r="Z97" s="41"/>
     </row>
-    <row r="98" spans="1:26" ht="24">
+    <row r="98" spans="1:26" ht="36">
       <c r="A98" s="61">
         <v>55600009</v>
       </c>
@@ -14112,7 +14129,7 @@
       </c>
       <c r="Z99" s="41"/>
     </row>
-    <row r="100" spans="1:26" ht="24">
+    <row r="100" spans="1:26" ht="36">
       <c r="A100" s="61">
         <v>55600011</v>
       </c>
@@ -14208,7 +14225,7 @@
       </c>
       <c r="Z101" s="41"/>
     </row>
-    <row r="102" spans="1:26" ht="24">
+    <row r="102" spans="1:26" ht="36">
       <c r="A102" s="81">
         <v>55610002</v>
       </c>
@@ -14258,7 +14275,7 @@
       </c>
       <c r="Z102" s="41"/>
     </row>
-    <row r="103" spans="1:26" ht="24">
+    <row r="103" spans="1:26" ht="36">
       <c r="A103" s="81">
         <v>55610003</v>
       </c>
@@ -14308,7 +14325,7 @@
       </c>
       <c r="Z103" s="41"/>
     </row>
-    <row r="104" spans="1:26" ht="24">
+    <row r="104" spans="1:26" ht="36">
       <c r="A104" s="90">
         <v>55610004</v>
       </c>
@@ -14563,7 +14580,7 @@
         <v>55700005</v>
       </c>
       <c r="B109" s="56" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C109" s="27" t="s">
         <v>523</v>
@@ -14580,7 +14597,7 @@
       <c r="M109" s="17"/>
       <c r="N109" s="17"/>
       <c r="O109" s="21" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="P109" s="45">
         <v>1</v>
@@ -14592,7 +14609,7 @@
         <v>524</v>
       </c>
       <c r="S109" s="16" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="T109" s="27">
         <v>0</v>
@@ -14610,7 +14627,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="110" spans="1:26" ht="96">
+    <row r="110" spans="1:26" ht="120">
       <c r="A110" s="59">
         <v>55900001</v>
       </c>
@@ -14670,7 +14687,7 @@
       </c>
       <c r="Z110" s="52"/>
     </row>
-    <row r="111" spans="1:26" ht="84">
+    <row r="111" spans="1:26" ht="96">
       <c r="A111" s="59">
         <v>55900002</v>
       </c>
@@ -14726,7 +14743,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="112" spans="1:26" ht="24">
+    <row r="112" spans="1:26" ht="28.8">
       <c r="A112" s="59">
         <v>55900003</v>
       </c>
@@ -14824,7 +14841,7 @@
       </c>
       <c r="Z113" s="52"/>
     </row>
-    <row r="114" spans="1:26" ht="27">
+    <row r="114" spans="1:26" ht="28.8">
       <c r="A114" s="59">
         <v>55900005</v>
       </c>
@@ -15114,7 +15131,7 @@
       </c>
       <c r="Z119" s="41"/>
     </row>
-    <row r="120" spans="1:26" ht="60">
+    <row r="120" spans="1:26" ht="84">
       <c r="A120" s="59">
         <v>55900011</v>
       </c>
@@ -15162,7 +15179,7 @@
       </c>
       <c r="Z120" s="27"/>
     </row>
-    <row r="121" spans="1:26" ht="72">
+    <row r="121" spans="1:26" ht="84">
       <c r="A121" s="59">
         <v>55900012</v>
       </c>
@@ -15218,7 +15235,7 @@
       </c>
       <c r="Z121" s="43"/>
     </row>
-    <row r="122" spans="1:26" ht="24">
+    <row r="122" spans="1:26" ht="36">
       <c r="A122" s="59">
         <v>55900013</v>
       </c>
@@ -15582,7 +15599,7 @@
       </c>
       <c r="Z128" s="52"/>
     </row>
-    <row r="129" spans="1:26" ht="84">
+    <row r="129" spans="1:26" ht="108">
       <c r="A129" s="89">
         <v>55900020</v>
       </c>
@@ -15636,7 +15653,7 @@
       </c>
       <c r="Z129" s="87"/>
     </row>
-    <row r="130" spans="1:26">
+    <row r="130" spans="1:26" ht="24">
       <c r="A130" s="59">
         <v>55900021</v>
       </c>
@@ -15686,7 +15703,7 @@
       </c>
       <c r="Z130" s="52"/>
     </row>
-    <row r="131" spans="1:26" ht="84">
+    <row r="131" spans="1:26" ht="108">
       <c r="A131" s="89">
         <v>55900022</v>
       </c>
@@ -15742,7 +15759,7 @@
       </c>
       <c r="Z131" s="52"/>
     </row>
-    <row r="132" spans="1:26" ht="27">
+    <row r="132" spans="1:26" ht="28.8">
       <c r="A132" s="59">
         <v>55900023</v>
       </c>
@@ -15790,7 +15807,7 @@
       </c>
       <c r="Z132" s="52"/>
     </row>
-    <row r="133" spans="1:26" ht="84">
+    <row r="133" spans="1:26" ht="96">
       <c r="A133" s="89">
         <v>55900024</v>
       </c>
@@ -15811,7 +15828,7 @@
       </c>
       <c r="G133" s="64"/>
       <c r="H133" s="32" t="s">
-        <v>965</v>
+        <v>974</v>
       </c>
       <c r="I133" s="32"/>
       <c r="J133" s="28"/>
@@ -15844,7 +15861,7 @@
       </c>
       <c r="Z133" s="52"/>
     </row>
-    <row r="134" spans="1:26" ht="108">
+    <row r="134" spans="1:26" ht="120">
       <c r="A134" s="59">
         <v>55900025</v>
       </c>
@@ -15872,7 +15889,7 @@
       <c r="M134" s="17"/>
       <c r="N134" s="17"/>
       <c r="O134" s="21" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="P134" s="45">
         <v>2</v>
@@ -15884,7 +15901,7 @@
         <v>524</v>
       </c>
       <c r="S134" s="16" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="T134" s="27">
         <v>0</v>
@@ -15903,6 +15920,56 @@
         <v>232</v>
       </c>
       <c r="Z134" s="52"/>
+    </row>
+    <row r="135" spans="1:26" ht="24">
+      <c r="A135" s="59">
+        <v>55900026</v>
+      </c>
+      <c r="B135" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="C135" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D135" s="27"/>
+      <c r="E135" s="27"/>
+      <c r="F135" s="48"/>
+      <c r="G135" s="64"/>
+      <c r="H135" s="88"/>
+      <c r="I135" s="51"/>
+      <c r="J135" s="28"/>
+      <c r="K135" s="29"/>
+      <c r="L135" s="33"/>
+      <c r="M135" s="17"/>
+      <c r="N135" s="17" t="s">
+        <v>971</v>
+      </c>
+      <c r="O135" s="21"/>
+      <c r="P135" s="45"/>
+      <c r="Q135" s="50" t="s">
+        <v>307</v>
+      </c>
+      <c r="R135" s="48" t="s">
+        <v>524</v>
+      </c>
+      <c r="S135" s="16" t="s">
+        <v>972</v>
+      </c>
+      <c r="T135" s="27">
+        <v>0</v>
+      </c>
+      <c r="U135" s="27"/>
+      <c r="V135" s="27"/>
+      <c r="W135" s="27"/>
+      <c r="X135" s="27">
+        <v>20</v>
+      </c>
+      <c r="Y135" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="Z135" s="52" t="s">
+        <v>973</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -15919,35 +15986,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N19" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="I22" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="P20" sqref="P20"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.25" customWidth="1"/>
+    <col min="3" max="7" width="7.21875" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="12" width="8.5" customWidth="1"/>
-    <col min="13" max="14" width="17.375" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="10" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="14" width="17.33203125" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="8.125" customWidth="1"/>
-    <col min="17" max="17" width="7.375" customWidth="1"/>
-    <col min="18" max="18" width="6.375" customWidth="1"/>
-    <col min="19" max="19" width="23.5" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" customWidth="1"/>
+    <col min="19" max="19" width="23.44140625" customWidth="1"/>
     <col min="20" max="20" width="9" customWidth="1"/>
-    <col min="21" max="23" width="7.625" customWidth="1"/>
-    <col min="24" max="24" width="7.125" customWidth="1"/>
-    <col min="27" max="27" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="7.6640625" customWidth="1"/>
+    <col min="24" max="24" width="7.109375" customWidth="1"/>
+    <col min="27" max="27" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="55.5">
+    <row r="1" spans="1:26" ht="58.8">
       <c r="A1" s="6" t="s">
         <v>295</v>
       </c>
@@ -16187,7 +16254,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="96">
+    <row r="4" spans="1:26" ht="120">
       <c r="A4">
         <v>55000098</v>
       </c>
@@ -16251,7 +16318,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="96">
+    <row r="5" spans="1:26" ht="120">
       <c r="A5">
         <v>55000105</v>
       </c>
@@ -16367,7 +16434,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="60">
+    <row r="7" spans="1:26" ht="72">
       <c r="A7">
         <v>55000117</v>
       </c>
@@ -16665,7 +16732,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="36">
+    <row r="13" spans="1:26" ht="48">
       <c r="A13">
         <v>55000180</v>
       </c>
@@ -16769,7 +16836,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="96">
+    <row r="15" spans="1:26" ht="120">
       <c r="A15">
         <v>55000215</v>
       </c>
@@ -16833,7 +16900,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="24">
+    <row r="16" spans="1:26" ht="36">
       <c r="A16">
         <v>55000230</v>
       </c>
@@ -16979,7 +17046,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="96">
+    <row r="19" spans="1:26" ht="108">
       <c r="A19">
         <v>55000240</v>
       </c>
@@ -17043,7 +17110,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="96">
+    <row r="20" spans="1:26" ht="120">
       <c r="A20">
         <v>55000244</v>
       </c>
@@ -17161,7 +17228,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="84">
+    <row r="22" spans="1:26" ht="96">
       <c r="A22">
         <v>55000274</v>
       </c>
@@ -17211,7 +17278,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="36">
+    <row r="23" spans="1:26" ht="48">
       <c r="A23">
         <v>55000284</v>
       </c>
@@ -17369,7 +17436,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="120">
+    <row r="26" spans="1:26" ht="144">
       <c r="A26">
         <v>55000289</v>
       </c>
@@ -17427,7 +17494,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="36">
+    <row r="27" spans="1:26" ht="48">
       <c r="A27">
         <v>55000292</v>
       </c>
@@ -17481,7 +17548,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="96">
+    <row r="28" spans="1:26" ht="120">
       <c r="A28">
         <v>55000294</v>
       </c>
@@ -17593,7 +17660,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="96">
+    <row r="30" spans="1:26" ht="120">
       <c r="A30">
         <v>55000324</v>
       </c>
@@ -17657,7 +17724,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="96">
+    <row r="31" spans="1:26" ht="120">
       <c r="A31">
         <v>55000325</v>
       </c>
@@ -17721,7 +17788,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="96">
+    <row r="32" spans="1:26" ht="108">
       <c r="A32">
         <v>55000326</v>
       </c>
@@ -17785,7 +17852,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="96">
+    <row r="33" spans="1:26" ht="120">
       <c r="A33">
         <v>55000327</v>
       </c>
@@ -17847,7 +17914,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="96">
+    <row r="34" spans="1:26" ht="108">
       <c r="A34">
         <v>55000330</v>
       </c>
@@ -17911,7 +17978,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="96">
+    <row r="35" spans="1:26" ht="120">
       <c r="A35">
         <v>55000331</v>
       </c>
@@ -17975,7 +18042,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="72">
+    <row r="36" spans="1:26" ht="96">
       <c r="A36">
         <v>55000332</v>
       </c>
@@ -18073,7 +18140,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="96">
+    <row r="38" spans="1:26" ht="108">
       <c r="A38">
         <v>55000334</v>
       </c>
@@ -18159,23 +18226,23 @@
       <selection pane="bottomRight" activeCell="N1" sqref="N1:N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.25" customWidth="1"/>
-    <col min="8" max="12" width="8.5" customWidth="1"/>
-    <col min="13" max="14" width="22.25" customWidth="1"/>
-    <col min="15" max="16" width="8.5" customWidth="1"/>
-    <col min="17" max="17" width="7.375" customWidth="1"/>
-    <col min="18" max="18" width="6.375" customWidth="1"/>
-    <col min="19" max="19" width="23.5" customWidth="1"/>
-    <col min="20" max="20" width="6.625" customWidth="1"/>
-    <col min="21" max="23" width="7.625" customWidth="1"/>
-    <col min="24" max="24" width="7.125" customWidth="1"/>
+    <col min="3" max="7" width="7.21875" customWidth="1"/>
+    <col min="8" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="14" width="22.21875" customWidth="1"/>
+    <col min="15" max="16" width="8.44140625" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" customWidth="1"/>
+    <col min="19" max="19" width="23.44140625" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" customWidth="1"/>
+    <col min="21" max="23" width="7.6640625" customWidth="1"/>
+    <col min="24" max="24" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="55.5">
+    <row r="1" spans="1:26" ht="58.8">
       <c r="A1" s="6" t="s">
         <v>295</v>
       </c>
@@ -18415,7 +18482,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="84">
+    <row r="4" spans="1:26" ht="96">
       <c r="A4">
         <v>55010004</v>
       </c>
@@ -18487,23 +18554,23 @@
       <selection pane="bottomRight" activeCell="N1" sqref="N1:N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.75" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.25" customWidth="1"/>
-    <col min="8" max="12" width="8.5" customWidth="1"/>
-    <col min="13" max="14" width="22.25" customWidth="1"/>
-    <col min="15" max="16" width="8.5" customWidth="1"/>
-    <col min="17" max="17" width="7.375" customWidth="1"/>
-    <col min="18" max="18" width="6.375" customWidth="1"/>
-    <col min="19" max="19" width="23.5" customWidth="1"/>
-    <col min="20" max="20" width="6.625" customWidth="1"/>
-    <col min="21" max="23" width="7.625" customWidth="1"/>
-    <col min="24" max="24" width="7.125" customWidth="1"/>
+    <col min="3" max="7" width="7.21875" customWidth="1"/>
+    <col min="8" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="14" width="22.21875" customWidth="1"/>
+    <col min="15" max="16" width="8.44140625" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" customWidth="1"/>
+    <col min="19" max="19" width="23.44140625" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" customWidth="1"/>
+    <col min="21" max="23" width="7.6640625" customWidth="1"/>
+    <col min="24" max="24" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="55.5">
+    <row r="1" spans="1:26" ht="58.8">
       <c r="A1" s="6" t="s">
         <v>295</v>
       </c>
@@ -18743,7 +18810,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="36">
+    <row r="4" spans="1:26" ht="48">
       <c r="A4">
         <v>55020001</v>
       </c>
@@ -18795,7 +18862,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="36">
+    <row r="5" spans="1:26" ht="48">
       <c r="A5">
         <v>55020002</v>
       </c>
@@ -18847,7 +18914,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="36">
+    <row r="6" spans="1:26" ht="48">
       <c r="A6">
         <v>55020003</v>
       </c>
@@ -18899,7 +18966,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="36">
+    <row r="7" spans="1:26" ht="48">
       <c r="A7">
         <v>55020004</v>
       </c>
@@ -18951,7 +19018,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="36">
+    <row r="8" spans="1:26" ht="48">
       <c r="A8">
         <v>55020005</v>
       </c>
@@ -19001,7 +19068,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="36">
+    <row r="9" spans="1:26" ht="48">
       <c r="A9">
         <v>55020006</v>
       </c>
@@ -19051,7 +19118,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="36">
+    <row r="10" spans="1:26" ht="48">
       <c r="A10">
         <v>55020007</v>
       </c>
@@ -19103,7 +19170,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="36">
+    <row r="11" spans="1:26" ht="48">
       <c r="A11">
         <v>55020008</v>
       </c>
@@ -19155,7 +19222,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="36">
+    <row r="12" spans="1:26" ht="48">
       <c r="A12">
         <v>55020009</v>
       </c>
@@ -19207,7 +19274,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="36">
+    <row r="13" spans="1:26" ht="48">
       <c r="A13">
         <v>55020010</v>
       </c>
@@ -19259,7 +19326,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="36">
+    <row r="14" spans="1:26" ht="48">
       <c r="A14">
         <v>55020011</v>
       </c>
@@ -19311,7 +19378,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="36">
+    <row r="15" spans="1:26" ht="48">
       <c r="A15">
         <v>55020012</v>
       </c>
@@ -19363,7 +19430,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="36">
+    <row r="16" spans="1:26" ht="48">
       <c r="A16">
         <v>55020013</v>
       </c>
@@ -19413,7 +19480,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="36">
+    <row r="17" spans="1:26" ht="48">
       <c r="A17">
         <v>55020014</v>
       </c>
@@ -19463,7 +19530,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="36">
+    <row r="18" spans="1:26" ht="48">
       <c r="A18">
         <v>55020015</v>
       </c>
@@ -19515,7 +19582,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="36">
+    <row r="19" spans="1:26" ht="48">
       <c r="A19">
         <v>55020016</v>
       </c>
@@ -19586,9 +19653,9 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">

</xml_diff>

<commit_message>
fix some attr related spell card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5761,11 +5761,11 @@
   <dimension ref="A1:Z164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="S56" sqref="S56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
close #12 finish spell data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -2785,488 +2785,488 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>s.Transform((MathTool.GetRandom(2) == 0) ? 51000001 : 51000047);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddActionRate(0.3);d.AddActionRate(-0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>乱刃</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奏乐</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000002,lv,"E");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔王</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id)) o.MadDrug();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(s.Attr)){o.AddMaxHp(o.MaxHp.Source*0.2);o.Atk*=0.2;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时永久提高同属性单位20%最大生命值和攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mowang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反弹所有物理攻击(自己不承受伤害)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反弹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddHp(-damage.NoDefenceValue);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Owner.AddMana(s,1,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣光</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>闪击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Spd&gt;d.Spd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对速度低于自身的单位造成130%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>虚无</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit-=40;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命满时拥有40%额外回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>招架</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>抵挡50%伤害，但会永久降低5%攻击力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0.5);d.Atk.Source*=0.95;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>立场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时减少对方召唤师1点LP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时回复召唤师1点MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Transform(51000114);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变向</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时将范围内的所有目标传到临近行</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.SetToPosition("side");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAW</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时，如果自身手牌数&gt;6，提高50%攻击力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.AddHpRate(0.2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合对1.5卡片距离友方恢复20%生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhiliao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckSpecial</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.ClearDebuff();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每2回合清除2.5卡片范围内友军负面状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000023,lv,"F").AddAttr("Water");</t>
+  </si>
+  <si>
+    <t>我方水系单位</t>
+  </si>
+  <si>
+    <t>coverauro</t>
+  </si>
+  <si>
+    <t>召唤时永久提高水属性单位20%最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>神射</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk.Source*=1.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合提高10%攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) o.ExtendDebuff(2);</t>
+  </si>
+  <si>
+    <t>延长范围内敌方怪物负面状态2回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillAfterHitEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.AddCard(d.CardId, d.Level);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死目标后获得该卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>过牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(1)){o.AddMaxHp(o.MaxHp.Source*0.2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.SetToPosition("back");</t>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(1.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(1.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高30%伤害，击中目标后使其后退1卡片距离</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>停留</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌我等级&gt;5单位</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000001,lv,"A").SetStar(6,10);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>震退</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk*=(s.GetMonsterCountByRace(4)*0.2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时场上每有一只昆虫，提高20%攻击力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Star&lt;3</t>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0);</t>
+  </si>
+  <si>
+    <t>抵挡一次星级低于3敌人的物理攻击</t>
+  </si>
+  <si>
+    <t>小盾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEC</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,d.Position)) o.AddHp(-damage.Value*0.4);</t>
+  </si>
+  <si>
+    <t>击中目标后造成目标同一列敌人40%伤害</t>
+  </si>
+  <si>
+    <t>coveraoe</t>
+  </si>
+  <si>
+    <t>guimian</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时，如果对方手牌数&gt;5，提高30%攻击和防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillInitialEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Owner.CardNumber&gt;=6) s.Atk*=0.5;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk*=s.Owner.CardNumber;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Rival.CardNumber&gt;5) {s.Atk*=0.3;s.Def*=0.3;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Star&lt;5</t>
+  </si>
+  <si>
+    <t>d.Transform(51010002);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000001,lv,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000101,lv,"F").AddRace("Plant");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时对10格内敌方恐惧3回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) s.AddBuff(55510003,lv,3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>xieqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAntiMagic("All",100);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔抗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAntiMagic("All",50);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有魔法伤害下降50%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsDefence</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>破坏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对防御型单位造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>silie</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>撕裂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pohuai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷途</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魅惑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Rebel();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后使目标反叛</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>meihuo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆破</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baopo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后对1卡片距离敌人造成100%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baopo2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后对2卡片距离敌人造成100%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AttackType==0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆破改</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectArea</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>curseoff</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rocket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>s.Transform(MathTool.GetRandom(51000001,51000300));</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Transform((MathTool.GetRandom(2) == 0) ? 51000001 : 51000047);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddActionRate(0.3);d.AddActionRate(-0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>乱刃</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奏乐</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000002,lv,"E");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔王</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id)) o.MadDrug();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NFR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(s.Attr)){o.AddMaxHp(o.MaxHp.Source*0.2);o.Atk*=0.2;}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时永久提高同属性单位20%最大生命值和攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mowang</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反弹所有物理攻击(自己不承受伤害)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反弹</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddHp(-damage.NoDefenceValue);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Owner.AddMana(s,1,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣光</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>闪击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Spd&gt;d.Spd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对速度低于自身的单位造成130%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>虚无</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit-=40;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命满时拥有40%额外回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>招架</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>抵挡50%伤害，但会永久降低5%攻击力</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0.5);d.Atk.Source*=0.95;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>立场</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时减少对方召唤师1点LP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时回复召唤师1点MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Transform(51000114);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>变向</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时将范围内的所有目标传到临近行</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.SetToPosition("side");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NAW</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时，如果自身手牌数&gt;6，提高50%攻击力</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NFR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.AddHpRate(0.2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合对1.5卡片距离友方恢复20%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhiliao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CheckSpecial</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.ClearDebuff();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每2回合清除2.5卡片范围内友军负面状态</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000023,lv,"F").AddAttr("Water");</t>
-  </si>
-  <si>
-    <t>我方水系单位</t>
-  </si>
-  <si>
-    <t>coverauro</t>
-  </si>
-  <si>
-    <t>召唤时永久提高水属性单位20%最大生命值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>神射</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk.Source*=1.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合提高10%攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) o.ExtendDebuff(2);</t>
-  </si>
-  <si>
-    <t>延长范围内敌方怪物负面状态2回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillAfterHitEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Owner.AddCard(d.CardId, d.Level);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>杀死目标后获得该卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>过牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(1)){o.AddMaxHp(o.MaxHp.Source*0.2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.SetToPosition("back");</t>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(1.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(1.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高30%伤害，击中目标后使其后退1卡片距离</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>停留</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>敌我等级&gt;5单位</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000001,lv,"A").SetStar(6,10);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>震退</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk*=(s.GetMonsterCountByRace(4)*0.2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时场上每有一只昆虫，提高20%攻击力</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Star&lt;3</t>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0);</t>
-  </si>
-  <si>
-    <t>抵挡一次星级低于3敌人的物理攻击</t>
-  </si>
-  <si>
-    <t>小盾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEC</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,d.Position)) o.AddHp(-damage.Value*0.4);</t>
-  </si>
-  <si>
-    <t>击中目标后造成目标同一列敌人40%伤害</t>
-  </si>
-  <si>
-    <t>coveraoe</t>
-  </si>
-  <si>
-    <t>guimian</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时，如果对方手牌数&gt;5，提高30%攻击和防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillInitialEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Owner.CardNumber&gt;=6) s.Atk*=0.5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk*=s.Owner.CardNumber;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Rival.CardNumber&gt;5) {s.Atk*=0.3;s.Def*=0.3;}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Star&lt;5</t>
-  </si>
-  <si>
-    <t>d.Transform(51010002);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000001,lv,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000101,lv,"F").AddRace("Plant");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时对10格内敌方恐惧3回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) s.AddBuff(55510003,lv,3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>xieqi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkball</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAntiMagic("All",100);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔抗</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAntiMagic("All",50);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有魔法伤害下降50%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsDefence</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>破坏</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对防御型单位造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>silie</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>撕裂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>pohuai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷途</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魅惑</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Rebel();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后使目标反叛</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>meihuo</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>爆破</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>baopo</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后对1卡片距离敌人造成100%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>baopo2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后对2卡片距离敌人造成100%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AttackType==0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>爆破改</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EffectArea</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>curseoff</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>rocket</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5761,11 +5761,11 @@
   <dimension ref="A1:Z164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C127" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="S56" sqref="S56"/>
+      <selection pane="bottomRight" activeCell="F136" sqref="F136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5891,7 +5891,7 @@
         <v>574</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>341</v>
@@ -5909,7 +5909,7 @@
         <v>650</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>309</v>
@@ -5992,7 +5992,7 @@
         <v>652</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>445</v>
@@ -6013,7 +6013,7 @@
         <v>320</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>347</v>
@@ -6360,10 +6360,10 @@
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="25" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="61">
@@ -6481,7 +6481,7 @@
       <c r="F13" s="43"/>
       <c r="G13" s="59"/>
       <c r="H13" s="29" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="I13" s="29"/>
       <c r="J13" s="28"/>
@@ -6959,7 +6959,7 @@
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="17" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -7227,7 +7227,7 @@
         <v>55110012</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>1</v>
@@ -7242,7 +7242,7 @@
       <c r="K29" s="18"/>
       <c r="L29" s="17"/>
       <c r="M29" s="17" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="N29" s="17"/>
       <c r="O29" s="20"/>
@@ -7273,7 +7273,7 @@
         <v>55110013</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>36</v>
@@ -7289,10 +7289,10 @@
       </c>
       <c r="K30" s="18"/>
       <c r="L30" s="17" t="s">
+        <v>754</v>
+      </c>
+      <c r="M30" s="17" t="s">
         <v>755</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>756</v>
       </c>
       <c r="N30" s="17"/>
       <c r="O30" s="20"/>
@@ -7304,7 +7304,7 @@
         <v>239</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="T30" s="10"/>
       <c r="U30" s="1"/>
@@ -7323,7 +7323,7 @@
         <v>55110014</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>36</v>
@@ -7369,7 +7369,7 @@
         <v>55110015</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>1</v>
@@ -7381,7 +7381,7 @@
       <c r="H32" s="29"/>
       <c r="I32" s="29"/>
       <c r="J32" s="28" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K32" s="18"/>
       <c r="L32" s="17" t="s">
@@ -7398,7 +7398,7 @@
         <v>239</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="T32" s="10"/>
       <c r="U32" s="1"/>
@@ -7417,7 +7417,7 @@
         <v>55110016</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>36</v>
@@ -7432,7 +7432,7 @@
         <v>303</v>
       </c>
       <c r="K33" s="18" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="17"/>
@@ -7446,7 +7446,7 @@
         <v>239</v>
       </c>
       <c r="S33" s="10" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="T33" s="10"/>
       <c r="U33" s="1"/>
@@ -7465,7 +7465,7 @@
         <v>55110017</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>36</v>
@@ -7479,7 +7479,7 @@
       <c r="J34" s="28"/>
       <c r="K34" s="18"/>
       <c r="L34" s="17" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
@@ -7492,7 +7492,7 @@
         <v>239</v>
       </c>
       <c r="S34" s="10" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="T34" s="10"/>
       <c r="U34" s="1"/>
@@ -7511,7 +7511,7 @@
         <v>55110018</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>36</v>
@@ -7561,7 +7561,7 @@
         <v>55110019</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C36" s="25" t="s">
         <v>36</v>
@@ -7573,11 +7573,11 @@
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
       <c r="J36" s="26" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="30" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
@@ -7590,7 +7590,7 @@
         <v>407</v>
       </c>
       <c r="S36" s="16" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="T36" s="25"/>
       <c r="U36" s="25" t="s">
@@ -7783,7 +7783,7 @@
         <v>99</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E40" s="25">
         <v>15</v>
@@ -7798,7 +7798,7 @@
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
       <c r="O40" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="P40" s="41">
         <v>1</v>
@@ -7810,7 +7810,7 @@
         <v>239</v>
       </c>
       <c r="S40" s="16" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="T40" s="25"/>
       <c r="U40" s="10" t="s">
@@ -7824,7 +7824,7 @@
         <v>40</v>
       </c>
       <c r="Y40" s="25" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="Z40" s="96"/>
     </row>
@@ -7839,13 +7839,13 @@
         <v>99</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E41" s="25">
         <v>25</v>
       </c>
       <c r="F41" s="44" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="G41" s="59"/>
       <c r="H41" s="47"/>
@@ -7856,7 +7856,7 @@
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="O41" s="20" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="P41" s="41">
         <v>2</v>
@@ -7868,7 +7868,7 @@
         <v>239</v>
       </c>
       <c r="S41" s="16" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="T41" s="25"/>
       <c r="U41" s="10" t="s">
@@ -8017,13 +8017,13 @@
         <v>99</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E44" s="25">
         <v>20</v>
       </c>
       <c r="F44" s="44" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G44" s="60"/>
       <c r="H44" s="29"/>
@@ -8034,7 +8034,7 @@
       <c r="K44" s="27"/>
       <c r="L44" s="30"/>
       <c r="M44" s="17" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="N44" s="17"/>
       <c r="O44" s="20"/>
@@ -8046,7 +8046,7 @@
         <v>407</v>
       </c>
       <c r="S44" s="16" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="T44" s="25"/>
       <c r="U44" s="25" t="s">
@@ -8056,7 +8056,7 @@
         <v>450</v>
       </c>
       <c r="W44" s="25" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="X44" s="25">
         <v>25</v>
@@ -8145,7 +8145,7 @@
       </c>
       <c r="G46" s="60"/>
       <c r="H46" s="29" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="I46" s="29"/>
       <c r="J46" s="28"/>
@@ -8162,11 +8162,11 @@
         <v>239</v>
       </c>
       <c r="S46" s="16" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="T46" s="25"/>
       <c r="U46" s="25" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="V46" s="25"/>
       <c r="W46" s="25"/>
@@ -8174,7 +8174,7 @@
         <v>25</v>
       </c>
       <c r="Y46" s="25" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="Z46" s="39"/>
     </row>
@@ -8585,7 +8585,7 @@
       <c r="L55" s="17"/>
       <c r="M55" s="17"/>
       <c r="N55" s="17" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="O55" s="20"/>
       <c r="P55" s="41"/>
@@ -8596,7 +8596,7 @@
         <v>239</v>
       </c>
       <c r="S55" s="10" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="T55" s="10"/>
       <c r="U55" s="1"/>
@@ -8642,7 +8642,7 @@
         <v>239</v>
       </c>
       <c r="S56" s="10" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="T56" s="10"/>
       <c r="U56" s="1"/>
@@ -9459,7 +9459,7 @@
       </c>
       <c r="K73" s="27"/>
       <c r="L73" s="30" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="M73" s="17"/>
       <c r="N73" s="17"/>
@@ -9746,7 +9746,7 @@
       <c r="K79" s="18"/>
       <c r="L79" s="17"/>
       <c r="M79" s="17" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="N79" s="17"/>
       <c r="O79" s="20"/>
@@ -10421,7 +10421,7 @@
         <v>55520002</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>35</v>
@@ -10513,7 +10513,7 @@
         <v>55520004</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>35</v>
@@ -10528,7 +10528,7 @@
       <c r="K96" s="18"/>
       <c r="L96" s="17"/>
       <c r="M96" s="17" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="N96" s="17"/>
       <c r="O96" s="20"/>
@@ -10540,7 +10540,7 @@
         <v>239</v>
       </c>
       <c r="S96" s="10" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="T96" s="10"/>
       <c r="U96" s="1"/>
@@ -10550,7 +10550,7 @@
         <v>150</v>
       </c>
       <c r="Y96" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Z96" s="25"/>
     </row>
@@ -10619,7 +10619,7 @@
       <c r="F98" s="43"/>
       <c r="G98" s="60"/>
       <c r="H98" s="29" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="I98" s="29"/>
       <c r="J98" s="28"/>
@@ -10859,7 +10859,7 @@
         <v>55600007</v>
       </c>
       <c r="B103" s="58" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>49</v>
@@ -11019,7 +11019,7 @@
       <c r="F106" s="43"/>
       <c r="G106" s="60"/>
       <c r="H106" s="29" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="I106" s="29"/>
       <c r="J106" s="28"/>
@@ -11069,7 +11069,7 @@
       <c r="F107" s="43"/>
       <c r="G107" s="60"/>
       <c r="H107" s="29" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="I107" s="29"/>
       <c r="J107" s="28"/>
@@ -11086,7 +11086,7 @@
         <v>407</v>
       </c>
       <c r="S107" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="T107" s="10">
         <v>56000023</v>
@@ -11094,7 +11094,7 @@
       <c r="U107" s="1"/>
       <c r="V107" s="1"/>
       <c r="W107" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="X107" s="1">
         <v>20</v>
@@ -11159,7 +11159,7 @@
         <v>55600013</v>
       </c>
       <c r="B109" s="58" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>49</v>
@@ -11169,7 +11169,7 @@
       <c r="F109" s="43"/>
       <c r="G109" s="60"/>
       <c r="H109" s="29" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I109" s="29"/>
       <c r="J109" s="28"/>
@@ -11186,7 +11186,7 @@
         <v>239</v>
       </c>
       <c r="S109" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="T109" s="10">
         <v>56000001</v>
@@ -11589,7 +11589,7 @@
         <v>55700005</v>
       </c>
       <c r="B118" s="52" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C118" s="25" t="s">
         <v>406</v>
@@ -11606,7 +11606,7 @@
       <c r="M118" s="17"/>
       <c r="N118" s="17"/>
       <c r="O118" s="20" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="P118" s="41">
         <v>1</v>
@@ -11618,7 +11618,7 @@
         <v>407</v>
       </c>
       <c r="S118" s="16" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="T118" s="25"/>
       <c r="U118" s="25"/>
@@ -11713,7 +11713,7 @@
       </c>
       <c r="G120" s="60"/>
       <c r="H120" s="47" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I120" s="47"/>
       <c r="J120" s="26"/>
@@ -11761,7 +11761,7 @@
       <c r="F121" s="44"/>
       <c r="G121" s="60"/>
       <c r="H121" s="47" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="I121" s="47"/>
       <c r="J121" s="26"/>
@@ -11985,7 +11985,7 @@
         <v>55900008</v>
       </c>
       <c r="B126" s="55" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>0</v>
@@ -12022,7 +12022,7 @@
         <v>40</v>
       </c>
       <c r="Y126" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="Z126" s="39"/>
     </row>
@@ -12185,7 +12185,7 @@
       </c>
       <c r="G130" s="60"/>
       <c r="H130" s="29" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="I130" s="29"/>
       <c r="J130" s="28"/>
@@ -12434,7 +12434,7 @@
       <c r="M135" s="21"/>
       <c r="N135" s="21"/>
       <c r="O135" s="20" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="P135" s="41">
         <v>1</v>
@@ -12486,7 +12486,7 @@
       <c r="M136" s="21"/>
       <c r="N136" s="21"/>
       <c r="O136" s="19" t="s">
-        <v>741</v>
+        <v>865</v>
       </c>
       <c r="P136" s="41">
         <v>1</v>
@@ -12538,7 +12538,7 @@
       <c r="M137" s="21"/>
       <c r="N137" s="21"/>
       <c r="O137" s="20" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="P137" s="41">
         <v>1</v>
@@ -12573,13 +12573,13 @@
         <v>55900020</v>
       </c>
       <c r="B138" s="55" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C138" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D138" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E138" s="25">
         <v>30</v>
@@ -12589,7 +12589,7 @@
       </c>
       <c r="G138" s="79"/>
       <c r="H138" s="29" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="I138" s="88"/>
       <c r="J138" s="90"/>
@@ -12606,7 +12606,7 @@
         <v>239</v>
       </c>
       <c r="S138" s="10" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="T138" s="78"/>
       <c r="U138" s="78"/>
@@ -12616,7 +12616,7 @@
         <v>20</v>
       </c>
       <c r="Y138" s="25" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="Z138" s="83"/>
     </row>
@@ -12625,7 +12625,7 @@
         <v>55900021</v>
       </c>
       <c r="B139" s="55" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C139" s="25" t="s">
         <v>0</v>
@@ -12673,13 +12673,13 @@
         <v>55900022</v>
       </c>
       <c r="B140" s="55" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C140" s="25" t="s">
         <v>406</v>
       </c>
       <c r="D140" s="25" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E140" s="25">
         <v>200</v>
@@ -12687,7 +12687,7 @@
       <c r="F140" s="25"/>
       <c r="G140" s="60"/>
       <c r="H140" s="84" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I140" s="47"/>
       <c r="J140" s="26"/>
@@ -12704,7 +12704,7 @@
         <v>407</v>
       </c>
       <c r="S140" s="16" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="T140" s="25"/>
       <c r="U140" s="25" t="s">
@@ -12730,14 +12730,14 @@
         <v>149</v>
       </c>
       <c r="C141" s="25" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D141" s="25"/>
       <c r="E141" s="25"/>
       <c r="F141" s="25"/>
       <c r="G141" s="60"/>
       <c r="H141" s="84" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="I141" s="47"/>
       <c r="J141" s="26"/>
@@ -12754,7 +12754,7 @@
         <v>407</v>
       </c>
       <c r="S141" s="16" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="T141" s="25"/>
       <c r="U141" s="25"/>
@@ -12789,7 +12789,7 @@
       </c>
       <c r="G142" s="60"/>
       <c r="H142" s="29" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="I142" s="29"/>
       <c r="J142" s="26"/>
@@ -12806,7 +12806,7 @@
         <v>407</v>
       </c>
       <c r="S142" s="10" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="T142" s="25"/>
       <c r="U142" s="25"/>
@@ -12848,7 +12848,7 @@
       <c r="M143" s="17"/>
       <c r="N143" s="17"/>
       <c r="O143" s="20" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="P143" s="41">
         <v>2</v>
@@ -12860,7 +12860,7 @@
         <v>407</v>
       </c>
       <c r="S143" s="16" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="T143" s="25"/>
       <c r="U143" s="25" t="s">
@@ -12899,7 +12899,7 @@
       <c r="L144" s="30"/>
       <c r="M144" s="17"/>
       <c r="N144" s="17" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="O144" s="20"/>
       <c r="P144" s="41"/>
@@ -12910,7 +12910,7 @@
         <v>407</v>
       </c>
       <c r="S144" s="16" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="T144" s="25"/>
       <c r="U144" s="25"/>
@@ -12923,7 +12923,7 @@
         <v>191</v>
       </c>
       <c r="Z144" s="48" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="145" spans="1:26" ht="27">
@@ -12931,7 +12931,7 @@
         <v>55900027</v>
       </c>
       <c r="B145" s="55" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C145" s="25" t="s">
         <v>0</v>
@@ -12945,10 +12945,10 @@
       <c r="J145" s="26"/>
       <c r="K145" s="27"/>
       <c r="L145" s="30" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="M145" s="17" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="N145" s="17"/>
       <c r="O145" s="20"/>
@@ -12960,7 +12960,7 @@
         <v>407</v>
       </c>
       <c r="S145" s="16" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="T145" s="25"/>
       <c r="U145" s="25"/>
@@ -12989,7 +12989,7 @@
       <c r="F146" s="44"/>
       <c r="G146" s="60"/>
       <c r="H146" s="84" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I146" s="47"/>
       <c r="J146" s="26"/>
@@ -13006,7 +13006,7 @@
         <v>407</v>
       </c>
       <c r="S146" s="16" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="T146" s="25"/>
       <c r="U146" s="25"/>
@@ -13033,7 +13033,7 @@
       <c r="F147" s="25"/>
       <c r="G147" s="60"/>
       <c r="H147" s="84" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="I147" s="47"/>
       <c r="J147" s="26"/>
@@ -13050,7 +13050,7 @@
         <v>407</v>
       </c>
       <c r="S147" s="16" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="T147" s="25"/>
       <c r="U147" s="25"/>
@@ -13060,7 +13060,7 @@
         <v>15</v>
       </c>
       <c r="Y147" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="Z147" s="48"/>
     </row>
@@ -13081,12 +13081,12 @@
       <c r="H148" s="84"/>
       <c r="I148" s="47"/>
       <c r="J148" s="26" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="K148" s="27"/>
       <c r="L148" s="30"/>
       <c r="M148" s="17" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="N148" s="17"/>
       <c r="O148" s="20"/>
@@ -13122,7 +13122,7 @@
         <v>23</v>
       </c>
       <c r="C149" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25"/>
@@ -13161,7 +13161,7 @@
         <v>24</v>
       </c>
       <c r="Z149" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="150" spans="1:26" ht="36">
@@ -13172,7 +13172,7 @@
         <v>25</v>
       </c>
       <c r="C150" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="25"/>
@@ -13211,7 +13211,7 @@
         <v>26</v>
       </c>
       <c r="Z150" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="151" spans="1:26" ht="36">
@@ -13222,7 +13222,7 @@
         <v>27</v>
       </c>
       <c r="C151" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D151" s="25"/>
       <c r="E151" s="25"/>
@@ -13261,7 +13261,7 @@
         <v>28</v>
       </c>
       <c r="Z151" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="152" spans="1:26" ht="36">
@@ -13272,7 +13272,7 @@
         <v>29</v>
       </c>
       <c r="C152" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="25"/>
@@ -13311,7 +13311,7 @@
         <v>30</v>
       </c>
       <c r="Z152" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="153" spans="1:26" ht="36">
@@ -13322,7 +13322,7 @@
         <v>31</v>
       </c>
       <c r="C153" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="25"/>
@@ -13361,7 +13361,7 @@
         <v>32</v>
       </c>
       <c r="Z153" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="154" spans="1:26" ht="36">
@@ -13372,7 +13372,7 @@
         <v>33</v>
       </c>
       <c r="C154" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25"/>
@@ -13411,7 +13411,7 @@
         <v>34</v>
       </c>
       <c r="Z154" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="155" spans="1:26" ht="36">
@@ -13422,7 +13422,7 @@
         <v>55</v>
       </c>
       <c r="C155" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25"/>
@@ -13461,7 +13461,7 @@
         <v>56</v>
       </c>
       <c r="Z155" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="156" spans="1:26" ht="36">
@@ -13472,7 +13472,7 @@
         <v>57</v>
       </c>
       <c r="C156" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D156" s="25"/>
       <c r="E156" s="25"/>
@@ -13511,7 +13511,7 @@
         <v>58</v>
       </c>
       <c r="Z156" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="157" spans="1:26" ht="36">
@@ -13522,7 +13522,7 @@
         <v>59</v>
       </c>
       <c r="C157" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D157" s="25"/>
       <c r="E157" s="25"/>
@@ -13561,7 +13561,7 @@
         <v>60</v>
       </c>
       <c r="Z157" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="158" spans="1:26" ht="36">
@@ -13572,7 +13572,7 @@
         <v>61</v>
       </c>
       <c r="C158" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D158" s="25"/>
       <c r="E158" s="25"/>
@@ -13611,7 +13611,7 @@
         <v>62</v>
       </c>
       <c r="Z158" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="159" spans="1:26" ht="36">
@@ -13622,7 +13622,7 @@
         <v>63</v>
       </c>
       <c r="C159" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25"/>
@@ -13661,7 +13661,7 @@
         <v>64</v>
       </c>
       <c r="Z159" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="160" spans="1:26" ht="36">
@@ -13672,7 +13672,7 @@
         <v>65</v>
       </c>
       <c r="C160" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25"/>
@@ -13711,7 +13711,7 @@
         <v>66</v>
       </c>
       <c r="Z160" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="161" spans="1:26" ht="24">
@@ -13719,17 +13719,17 @@
         <v>55990101</v>
       </c>
       <c r="B161" s="98" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C161" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D161" s="25"/>
       <c r="E161" s="25"/>
       <c r="F161" s="44"/>
       <c r="G161" s="60"/>
       <c r="H161" s="84" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="I161" s="47"/>
       <c r="J161" s="26"/>
@@ -13746,7 +13746,7 @@
         <v>239</v>
       </c>
       <c r="S161" s="49" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="T161" s="25"/>
       <c r="U161" s="25"/>
@@ -13759,7 +13759,7 @@
         <v>109</v>
       </c>
       <c r="Z161" s="48" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="162" spans="1:26" ht="24">
@@ -13767,10 +13767,10 @@
         <v>55990102</v>
       </c>
       <c r="B162" s="98" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C162" s="25" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25"/>
@@ -13779,11 +13779,11 @@
       <c r="H162" s="84"/>
       <c r="I162" s="47"/>
       <c r="J162" s="26" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="K162" s="27"/>
       <c r="L162" s="30" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="M162" s="17"/>
       <c r="N162" s="17"/>
@@ -13796,7 +13796,7 @@
         <v>239</v>
       </c>
       <c r="S162" s="16" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="T162" s="25"/>
       <c r="U162" s="25"/>
@@ -13806,10 +13806,10 @@
         <v>25</v>
       </c>
       <c r="Y162" s="25" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="Z162" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="163" spans="1:26" ht="60">
@@ -13817,7 +13817,7 @@
         <v>55990103</v>
       </c>
       <c r="B163" s="98" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C163" s="25" t="s">
         <v>99</v>
@@ -13852,24 +13852,24 @@
         <v>239</v>
       </c>
       <c r="S163" s="16" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="T163" s="25"/>
       <c r="U163" s="25" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="V163" s="25" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="W163" s="25"/>
       <c r="X163" s="25">
         <v>35</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="Z163" s="48" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="164" spans="1:26" ht="60">
@@ -13877,7 +13877,7 @@
         <v>55990104</v>
       </c>
       <c r="B164" s="98" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C164" s="25" t="s">
         <v>99</v>
@@ -13895,7 +13895,7 @@
       <c r="H164" s="84"/>
       <c r="I164" s="47"/>
       <c r="J164" s="26" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="K164" s="27"/>
       <c r="L164" s="30"/>
@@ -13912,24 +13912,24 @@
         <v>239</v>
       </c>
       <c r="S164" s="16" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="V164" s="25" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="W164" s="25"/>
       <c r="X164" s="25">
         <v>50</v>
       </c>
       <c r="Y164" s="25" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="Z164" s="48" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #38 finish the crt dam skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="7" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="870">
   <si>
     <t>特殊</t>
   </si>
@@ -3267,6 +3267,22 @@
   </si>
   <si>
     <t>s.Transform(MathTool.GetRandom(51000001,51000300));</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.CrtDamAddRate+=0.5;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴击伤害提升50%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baoji</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5434,8 +5450,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z164" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:Z164"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z165" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:Z165"/>
   <sortState ref="A4:Z118">
     <sortCondition ref="A3:A118"/>
   </sortState>
@@ -5758,14 +5774,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z164"/>
+  <dimension ref="A1:Z165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C127" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C142" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="F136" sqref="F136"/>
+      <selection pane="bottomRight" activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -13114,29 +13130,27 @@
       </c>
       <c r="Z148" s="48"/>
     </row>
-    <row r="149" spans="1:26" ht="36">
-      <c r="A149" s="98">
-        <v>55990001</v>
-      </c>
-      <c r="B149" s="98" t="s">
-        <v>23</v>
+    <row r="149" spans="1:26">
+      <c r="A149" s="55">
+        <v>55900031</v>
+      </c>
+      <c r="B149" s="55" t="s">
+        <v>867</v>
       </c>
       <c r="C149" s="25" t="s">
-        <v>837</v>
+        <v>0</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25"/>
       <c r="F149" s="25"/>
       <c r="G149" s="60"/>
-      <c r="H149" s="97"/>
-      <c r="I149" s="29"/>
-      <c r="J149" s="26" t="s">
-        <v>411</v>
-      </c>
+      <c r="H149" s="84" t="s">
+        <v>866</v>
+      </c>
+      <c r="I149" s="47"/>
+      <c r="J149" s="26"/>
       <c r="K149" s="27"/>
-      <c r="L149" s="30" t="s">
-        <v>282</v>
-      </c>
+      <c r="L149" s="30"/>
       <c r="M149" s="17"/>
       <c r="N149" s="17"/>
       <c r="O149" s="20"/>
@@ -13145,31 +13159,29 @@
         <v>244</v>
       </c>
       <c r="R149" s="44" t="s">
-        <v>239</v>
+        <v>407</v>
       </c>
       <c r="S149" s="16" t="s">
-        <v>400</v>
+        <v>868</v>
       </c>
       <c r="T149" s="25"/>
       <c r="U149" s="25"/>
       <c r="V149" s="25"/>
       <c r="W149" s="25"/>
       <c r="X149" s="25">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="Y149" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z149" s="48" t="s">
-        <v>835</v>
-      </c>
+        <v>869</v>
+      </c>
+      <c r="Z149" s="48"/>
     </row>
     <row r="150" spans="1:26" ht="36">
       <c r="A150" s="98">
-        <v>55990002</v>
+        <v>55990001</v>
       </c>
       <c r="B150" s="98" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C150" s="25" t="s">
         <v>837</v>
@@ -13181,7 +13193,7 @@
       <c r="H150" s="97"/>
       <c r="I150" s="29"/>
       <c r="J150" s="26" t="s">
-        <v>270</v>
+        <v>411</v>
       </c>
       <c r="K150" s="27"/>
       <c r="L150" s="30" t="s">
@@ -13197,8 +13209,8 @@
       <c r="R150" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="S150" s="49" t="s">
-        <v>401</v>
+      <c r="S150" s="16" t="s">
+        <v>400</v>
       </c>
       <c r="T150" s="25"/>
       <c r="U150" s="25"/>
@@ -13208,7 +13220,7 @@
         <v>15</v>
       </c>
       <c r="Y150" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Z150" s="48" t="s">
         <v>835</v>
@@ -13216,10 +13228,10 @@
     </row>
     <row r="151" spans="1:26" ht="36">
       <c r="A151" s="98">
-        <v>55990003</v>
+        <v>55990002</v>
       </c>
       <c r="B151" s="98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C151" s="25" t="s">
         <v>837</v>
@@ -13231,7 +13243,7 @@
       <c r="H151" s="97"/>
       <c r="I151" s="29"/>
       <c r="J151" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K151" s="27"/>
       <c r="L151" s="30" t="s">
@@ -13248,7 +13260,7 @@
         <v>239</v>
       </c>
       <c r="S151" s="49" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="T151" s="25"/>
       <c r="U151" s="25"/>
@@ -13258,7 +13270,7 @@
         <v>15</v>
       </c>
       <c r="Y151" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Z151" s="48" t="s">
         <v>835</v>
@@ -13266,10 +13278,10 @@
     </row>
     <row r="152" spans="1:26" ht="36">
       <c r="A152" s="98">
-        <v>55990004</v>
+        <v>55990003</v>
       </c>
       <c r="B152" s="98" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C152" s="25" t="s">
         <v>837</v>
@@ -13281,7 +13293,7 @@
       <c r="H152" s="97"/>
       <c r="I152" s="29"/>
       <c r="J152" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K152" s="27"/>
       <c r="L152" s="30" t="s">
@@ -13298,7 +13310,7 @@
         <v>239</v>
       </c>
       <c r="S152" s="49" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="T152" s="25"/>
       <c r="U152" s="25"/>
@@ -13308,7 +13320,7 @@
         <v>15</v>
       </c>
       <c r="Y152" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z152" s="48" t="s">
         <v>835</v>
@@ -13316,10 +13328,10 @@
     </row>
     <row r="153" spans="1:26" ht="36">
       <c r="A153" s="98">
-        <v>55990005</v>
+        <v>55990004</v>
       </c>
       <c r="B153" s="98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C153" s="25" t="s">
         <v>837</v>
@@ -13331,7 +13343,7 @@
       <c r="H153" s="97"/>
       <c r="I153" s="29"/>
       <c r="J153" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K153" s="27"/>
       <c r="L153" s="30" t="s">
@@ -13348,7 +13360,7 @@
         <v>239</v>
       </c>
       <c r="S153" s="49" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="T153" s="25"/>
       <c r="U153" s="25"/>
@@ -13358,7 +13370,7 @@
         <v>15</v>
       </c>
       <c r="Y153" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Z153" s="48" t="s">
         <v>835</v>
@@ -13366,10 +13378,10 @@
     </row>
     <row r="154" spans="1:26" ht="36">
       <c r="A154" s="98">
-        <v>55990006</v>
+        <v>55990005</v>
       </c>
       <c r="B154" s="98" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C154" s="25" t="s">
         <v>837</v>
@@ -13381,7 +13393,7 @@
       <c r="H154" s="97"/>
       <c r="I154" s="29"/>
       <c r="J154" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K154" s="27"/>
       <c r="L154" s="30" t="s">
@@ -13398,7 +13410,7 @@
         <v>239</v>
       </c>
       <c r="S154" s="49" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="T154" s="25"/>
       <c r="U154" s="25"/>
@@ -13408,7 +13420,7 @@
         <v>15</v>
       </c>
       <c r="Y154" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Z154" s="48" t="s">
         <v>835</v>
@@ -13416,10 +13428,10 @@
     </row>
     <row r="155" spans="1:26" ht="36">
       <c r="A155" s="98">
-        <v>55990011</v>
+        <v>55990006</v>
       </c>
       <c r="B155" s="98" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C155" s="25" t="s">
         <v>837</v>
@@ -13431,24 +13443,24 @@
       <c r="H155" s="97"/>
       <c r="I155" s="29"/>
       <c r="J155" s="26" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="K155" s="27"/>
       <c r="L155" s="30" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="M155" s="17"/>
       <c r="N155" s="17"/>
       <c r="O155" s="20"/>
       <c r="P155" s="41"/>
       <c r="Q155" s="46" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="R155" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="S155" s="16" t="s">
-        <v>286</v>
+      <c r="S155" s="49" t="s">
+        <v>415</v>
       </c>
       <c r="T155" s="25"/>
       <c r="U155" s="25"/>
@@ -13458,7 +13470,7 @@
         <v>15</v>
       </c>
       <c r="Y155" s="25" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="Z155" s="48" t="s">
         <v>835</v>
@@ -13466,10 +13478,10 @@
     </row>
     <row r="156" spans="1:26" ht="36">
       <c r="A156" s="98">
-        <v>55990012</v>
+        <v>55990011</v>
       </c>
       <c r="B156" s="98" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C156" s="25" t="s">
         <v>837</v>
@@ -13481,7 +13493,7 @@
       <c r="H156" s="97"/>
       <c r="I156" s="29"/>
       <c r="J156" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K156" s="27"/>
       <c r="L156" s="30" t="s">
@@ -13498,7 +13510,7 @@
         <v>239</v>
       </c>
       <c r="S156" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T156" s="25"/>
       <c r="U156" s="25"/>
@@ -13508,7 +13520,7 @@
         <v>15</v>
       </c>
       <c r="Y156" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Z156" s="48" t="s">
         <v>835</v>
@@ -13516,10 +13528,10 @@
     </row>
     <row r="157" spans="1:26" ht="36">
       <c r="A157" s="98">
-        <v>55990013</v>
+        <v>55990012</v>
       </c>
       <c r="B157" s="98" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C157" s="25" t="s">
         <v>837</v>
@@ -13531,7 +13543,7 @@
       <c r="H157" s="97"/>
       <c r="I157" s="29"/>
       <c r="J157" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K157" s="27"/>
       <c r="L157" s="30" t="s">
@@ -13548,7 +13560,7 @@
         <v>239</v>
       </c>
       <c r="S157" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T157" s="25"/>
       <c r="U157" s="25"/>
@@ -13558,7 +13570,7 @@
         <v>15</v>
       </c>
       <c r="Y157" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Z157" s="48" t="s">
         <v>835</v>
@@ -13566,10 +13578,10 @@
     </row>
     <row r="158" spans="1:26" ht="36">
       <c r="A158" s="98">
-        <v>55990014</v>
+        <v>55990013</v>
       </c>
       <c r="B158" s="98" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C158" s="25" t="s">
         <v>837</v>
@@ -13581,7 +13593,7 @@
       <c r="H158" s="97"/>
       <c r="I158" s="29"/>
       <c r="J158" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K158" s="27"/>
       <c r="L158" s="30" t="s">
@@ -13598,7 +13610,7 @@
         <v>239</v>
       </c>
       <c r="S158" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T158" s="25"/>
       <c r="U158" s="25"/>
@@ -13608,7 +13620,7 @@
         <v>15</v>
       </c>
       <c r="Y158" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Z158" s="48" t="s">
         <v>835</v>
@@ -13616,10 +13628,10 @@
     </row>
     <row r="159" spans="1:26" ht="36">
       <c r="A159" s="98">
-        <v>55990015</v>
+        <v>55990014</v>
       </c>
       <c r="B159" s="98" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C159" s="25" t="s">
         <v>837</v>
@@ -13631,7 +13643,7 @@
       <c r="H159" s="97"/>
       <c r="I159" s="29"/>
       <c r="J159" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K159" s="27"/>
       <c r="L159" s="30" t="s">
@@ -13648,7 +13660,7 @@
         <v>239</v>
       </c>
       <c r="S159" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T159" s="25"/>
       <c r="U159" s="25"/>
@@ -13658,7 +13670,7 @@
         <v>15</v>
       </c>
       <c r="Y159" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Z159" s="48" t="s">
         <v>835</v>
@@ -13666,10 +13678,10 @@
     </row>
     <row r="160" spans="1:26" ht="36">
       <c r="A160" s="98">
-        <v>55990016</v>
+        <v>55990015</v>
       </c>
       <c r="B160" s="98" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C160" s="25" t="s">
         <v>837</v>
@@ -13678,10 +13690,10 @@
       <c r="E160" s="25"/>
       <c r="F160" s="25"/>
       <c r="G160" s="60"/>
-      <c r="H160" s="84"/>
-      <c r="I160" s="47"/>
+      <c r="H160" s="97"/>
+      <c r="I160" s="29"/>
       <c r="J160" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K160" s="27"/>
       <c r="L160" s="30" t="s">
@@ -13698,7 +13710,7 @@
         <v>239</v>
       </c>
       <c r="S160" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T160" s="25"/>
       <c r="U160" s="25"/>
@@ -13708,33 +13720,35 @@
         <v>15</v>
       </c>
       <c r="Y160" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z160" s="48" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="161" spans="1:26" ht="24">
+    <row r="161" spans="1:26" ht="36">
       <c r="A161" s="98">
-        <v>55990101</v>
+        <v>55990016</v>
       </c>
       <c r="B161" s="98" t="s">
-        <v>838</v>
+        <v>65</v>
       </c>
       <c r="C161" s="25" t="s">
         <v>837</v>
       </c>
       <c r="D161" s="25"/>
       <c r="E161" s="25"/>
-      <c r="F161" s="44"/>
+      <c r="F161" s="25"/>
       <c r="G161" s="60"/>
-      <c r="H161" s="84" t="s">
-        <v>839</v>
-      </c>
+      <c r="H161" s="84"/>
       <c r="I161" s="47"/>
-      <c r="J161" s="26"/>
+      <c r="J161" s="26" t="s">
+        <v>297</v>
+      </c>
       <c r="K161" s="27"/>
-      <c r="L161" s="30"/>
+      <c r="L161" s="30" t="s">
+        <v>285</v>
+      </c>
       <c r="M161" s="17"/>
       <c r="N161" s="17"/>
       <c r="O161" s="20"/>
@@ -13745,103 +13759,95 @@
       <c r="R161" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="S161" s="49" t="s">
-        <v>840</v>
+      <c r="S161" s="16" t="s">
+        <v>291</v>
       </c>
       <c r="T161" s="25"/>
       <c r="U161" s="25"/>
       <c r="V161" s="25"/>
       <c r="W161" s="25"/>
       <c r="X161" s="25">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Y161" s="25" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="Z161" s="48" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="162" spans="1:26" ht="24">
       <c r="A162" s="98">
-        <v>55990102</v>
+        <v>55990101</v>
       </c>
       <c r="B162" s="98" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="C162" s="25" t="s">
         <v>837</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25"/>
-      <c r="F162" s="25"/>
+      <c r="F162" s="44"/>
       <c r="G162" s="60"/>
-      <c r="H162" s="84"/>
+      <c r="H162" s="84" t="s">
+        <v>839</v>
+      </c>
       <c r="I162" s="47"/>
-      <c r="J162" s="26" t="s">
-        <v>842</v>
-      </c>
+      <c r="J162" s="26"/>
       <c r="K162" s="27"/>
-      <c r="L162" s="30" t="s">
-        <v>845</v>
-      </c>
+      <c r="L162" s="30"/>
       <c r="M162" s="17"/>
       <c r="N162" s="17"/>
       <c r="O162" s="20"/>
       <c r="P162" s="41"/>
       <c r="Q162" s="46" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="R162" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="S162" s="16" t="s">
-        <v>844</v>
+      <c r="S162" s="49" t="s">
+        <v>840</v>
       </c>
       <c r="T162" s="25"/>
       <c r="U162" s="25"/>
       <c r="V162" s="25"/>
       <c r="W162" s="25"/>
       <c r="X162" s="25">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Y162" s="25" t="s">
-        <v>848</v>
+        <v>109</v>
       </c>
       <c r="Z162" s="48" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="163" spans="1:26" ht="60">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="163" spans="1:26" ht="24">
       <c r="A163" s="98">
-        <v>55990103</v>
+        <v>55990102</v>
       </c>
       <c r="B163" s="98" t="s">
-        <v>854</v>
+        <v>843</v>
       </c>
       <c r="C163" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D163" s="25" t="s">
-        <v>464</v>
-      </c>
-      <c r="E163" s="25">
-        <v>10</v>
-      </c>
-      <c r="F163" s="44" t="s">
-        <v>474</v>
-      </c>
+        <v>837</v>
+      </c>
+      <c r="D163" s="25"/>
+      <c r="E163" s="25"/>
+      <c r="F163" s="25"/>
       <c r="G163" s="60"/>
       <c r="H163" s="84"/>
       <c r="I163" s="47"/>
       <c r="J163" s="26" t="s">
-        <v>689</v>
+        <v>842</v>
       </c>
       <c r="K163" s="27"/>
-      <c r="L163" s="30"/>
-      <c r="M163" s="17" t="s">
-        <v>599</v>
-      </c>
+      <c r="L163" s="30" t="s">
+        <v>845</v>
+      </c>
+      <c r="M163" s="17"/>
       <c r="N163" s="17"/>
       <c r="O163" s="20"/>
       <c r="P163" s="41"/>
@@ -13852,32 +13858,28 @@
         <v>239</v>
       </c>
       <c r="S163" s="16" t="s">
-        <v>857</v>
+        <v>844</v>
       </c>
       <c r="T163" s="25"/>
-      <c r="U163" s="25" t="s">
-        <v>864</v>
-      </c>
-      <c r="V163" s="25" t="s">
-        <v>864</v>
-      </c>
+      <c r="U163" s="25"/>
+      <c r="V163" s="25"/>
       <c r="W163" s="25"/>
       <c r="X163" s="25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
       <c r="Z163" s="48" t="s">
-        <v>855</v>
+        <v>835</v>
       </c>
     </row>
     <row r="164" spans="1:26" ht="60">
       <c r="A164" s="98">
-        <v>55990104</v>
+        <v>55990103</v>
       </c>
       <c r="B164" s="98" t="s">
-        <v>861</v>
+        <v>854</v>
       </c>
       <c r="C164" s="25" t="s">
         <v>99</v>
@@ -13886,7 +13888,7 @@
         <v>464</v>
       </c>
       <c r="E164" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F164" s="44" t="s">
         <v>474</v>
@@ -13895,7 +13897,7 @@
       <c r="H164" s="84"/>
       <c r="I164" s="47"/>
       <c r="J164" s="26" t="s">
-        <v>860</v>
+        <v>689</v>
       </c>
       <c r="K164" s="27"/>
       <c r="L164" s="30"/>
@@ -13912,7 +13914,7 @@
         <v>239</v>
       </c>
       <c r="S164" s="16" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25" t="s">
@@ -13923,12 +13925,72 @@
       </c>
       <c r="W164" s="25"/>
       <c r="X164" s="25">
+        <v>35</v>
+      </c>
+      <c r="Y164" s="25" t="s">
+        <v>856</v>
+      </c>
+      <c r="Z164" s="48" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="165" spans="1:26" ht="60">
+      <c r="A165" s="98">
+        <v>55990104</v>
+      </c>
+      <c r="B165" s="98" t="s">
+        <v>861</v>
+      </c>
+      <c r="C165" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D165" s="25" t="s">
+        <v>464</v>
+      </c>
+      <c r="E165" s="25">
+        <v>20</v>
+      </c>
+      <c r="F165" s="44" t="s">
+        <v>474</v>
+      </c>
+      <c r="G165" s="60"/>
+      <c r="H165" s="84"/>
+      <c r="I165" s="47"/>
+      <c r="J165" s="26" t="s">
+        <v>860</v>
+      </c>
+      <c r="K165" s="27"/>
+      <c r="L165" s="30"/>
+      <c r="M165" s="17" t="s">
+        <v>599</v>
+      </c>
+      <c r="N165" s="17"/>
+      <c r="O165" s="20"/>
+      <c r="P165" s="41"/>
+      <c r="Q165" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="R165" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="S165" s="16" t="s">
+        <v>859</v>
+      </c>
+      <c r="T165" s="25"/>
+      <c r="U165" s="25" t="s">
+        <v>864</v>
+      </c>
+      <c r="V165" s="25" t="s">
+        <v>864</v>
+      </c>
+      <c r="W165" s="25"/>
+      <c r="X165" s="25">
         <v>50</v>
       </c>
-      <c r="Y164" s="25" t="s">
+      <c r="Y165" s="25" t="s">
         <v>858</v>
       </c>
-      <c r="Z164" s="48" t="s">
+      <c r="Z165" s="48" t="s">
         <v>855</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new panda card monster
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="892">
   <si>
     <t>特殊</t>
   </si>
@@ -2487,301 +2487,874 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>死亡时对凶手造成自身最大生命30%的伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddHp(-d.MaxHp*0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魂守</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时永久增加0-50%攻击和防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk.Source*=MathTool.GetRandom(1f,1.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.StealWeapon(d);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>盗取</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>破甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>25分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>20分</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>灵性</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用本系卷轴造成额外30%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetMDamageRate(1.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AttackType==s.Attr&amp;&amp;s.HasScroll</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通魔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AttackType==0</t>
+  </si>
+  <si>
+    <t>攻击默认为自身属性魔法攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yuanbao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>元爆</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mattack</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖刺</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反弹20%所受伤害(自己仍受到100%伤害)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>欺压</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>猎杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(1.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Star&gt;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对星级低于3的敌人造成150%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对星级高于5的敌人造成150%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>武装</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wuzhuang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sidekicker</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以为其他单位提供支援</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>援护</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sidekickee</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以令其他单位提供支援</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>空灵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.AddMaxHp(o.MaxHp.Source*0.15);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时提高所有无属性单位15%最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂液体</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>venom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时使周围单位基础攻击力变为基础生命的1/5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>扭曲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>亡眼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击追加10%最大生命伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.AddPDamage(d.MaxHp.Source*0.10);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>威严</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.WeaponId&gt;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>打造</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡后装备武器返回召唤师手牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.WeaponReturn();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>幻化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEF</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时对选定目标造成魔法伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时对最近的3个敌人造成伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortDistance(true).Top(1)) mon.OnMagicDamage(s.Atk.Source*1.5,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>气化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>躲闪</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit-=20;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>!isMelee</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>受到远程单位攻击提高20%回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>重生</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>chongsheng</t>
+  </si>
+  <si>
+    <t>生命值低于30%时直接回复所有生命值（cd5回合）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变形</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Transform((MathTool.GetRandom(2) == 0) ? 51000001 : 51000047);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddActionRate(0.3);d.AddActionRate(-0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>乱刃</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奏乐</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000002,lv,"E");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔王</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id)) o.MadDrug();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(s.Attr)){o.AddMaxHp(o.MaxHp.Source*0.2);o.Atk*=0.2;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时永久提高同属性单位20%最大生命值和攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mowang</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反弹所有物理攻击(自己不承受伤害)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反弹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddHp(-damage.NoDefenceValue);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>反击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Owner.AddMana(s,1,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣光</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>闪击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Spd&gt;d.Spd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对速度低于自身的单位造成130%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>虚无</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit-=40;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命满时拥有40%额外回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>招架</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>抵挡50%伤害，但会永久降低5%攻击力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0.5);d.Atk.Source*=0.95;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>立场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时减少对方召唤师1点LP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时回复召唤师1点MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Transform(51000114);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变向</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时将范围内的所有目标传到临近行</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.SetToPosition("side");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAW</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时，如果自身手牌数&gt;6，提高50%攻击力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.AddHpRate(0.2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合对1.5卡片距离友方恢复20%生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhiliao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckSpecial</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.ClearDebuff();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每2回合清除2.5卡片范围内友军负面状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000023,lv,"F").AddAttr("Water");</t>
+  </si>
+  <si>
+    <t>我方水系单位</t>
+  </si>
+  <si>
+    <t>coverauro</t>
+  </si>
+  <si>
+    <t>召唤时永久提高水属性单位20%最大生命值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>神射</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk.Source*=1.1;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合提高10%攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) o.ExtendDebuff(2);</t>
+  </si>
+  <si>
+    <t>延长范围内敌方怪物负面状态2回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillAfterHitEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.AddCard(d.CardId, d.Level);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死目标后获得该卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>过牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(1)){o.AddMaxHp(o.MaxHp.Source*0.2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.SetToPosition("back");</t>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(1.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(1.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>提高30%伤害，击中目标后使其后退1卡片距离</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>停留</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌我等级&gt;5单位</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000001,lv,"A").SetStar(6,10);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>震退</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk*=(s.GetMonsterCountByRace(4)*0.2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时场上每有一只昆虫，提高20%攻击力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Star&lt;3</t>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0);</t>
+  </si>
+  <si>
+    <t>抵挡一次星级低于3敌人的物理攻击</t>
+  </si>
+  <si>
+    <t>小盾</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEC</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,d.Position)) o.AddHp(-damage.Value*0.4);</t>
+  </si>
+  <si>
+    <t>击中目标后造成目标同一列敌人40%伤害</t>
+  </si>
+  <si>
+    <t>coveraoe</t>
+  </si>
+  <si>
+    <t>guimian</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时，如果对方手牌数&gt;5，提高30%攻击和防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillInitialEffectDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Owner.CardNumber&gt;=6) s.Atk*=0.5;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk*=s.Owner.CardNumber;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Rival.CardNumber&gt;5) {s.Atk*=0.3;s.Def*=0.3;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Star&lt;5</t>
+  </si>
+  <si>
+    <t>d.Transform(51010002);</t>
+  </si>
+  <si>
+    <t>d.AddBuff(56000001,lv,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000101,lv,"F").AddRace("Plant");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时对10格内敌方恐惧3回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) s.AddBuff(55510003,lv,3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>xieqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkball</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAntiMagic("All",100);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔抗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAntiMagic("All",50);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有魔法伤害下降50%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.IsDefence</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>破坏</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对防御型单位造成200%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>silie</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>撕裂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pohuai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷途</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魅惑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Rebel();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后使目标反叛</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>meihuo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆破</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baopo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后对1卡片距离敌人造成100%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baopo2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>击中目标后对2卡片距离敌人造成100%伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AttackType==0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆破改</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EffectArea</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>curseoff</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rocket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Transform(MathTool.GetRandom(51000001,51000300));</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.CrtDamAddRate+=0.5;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴击伤害提升50%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baoji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddAuro(56000131,lv,"E");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>噩梦</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>emeng</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.AddSpike(57000008);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.RemoveSpike(57000008);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>学徒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有玩家每回合多抽一张牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有玩家使用魔法卡消耗+3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有玩家使用魔法卡消耗-3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有玩家使用怪物卡消耗-3</t>
+  </si>
+  <si>
+    <t>所有玩家使用卡片消耗+1</t>
+  </si>
+  <si>
+    <t>所有玩家使用武器卡消耗-2</t>
+  </si>
+  <si>
+    <t>使用魔法卡消耗-1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.AddHpRate(0.2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bluebubble</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>气泡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qipao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时恢复1.2卡片距离友方20%生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tanqiu</t>
+  </si>
+  <si>
+    <t>探求</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时抽一张牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeathHit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Owner.GetNextNCard(1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) s.Transform(mon.CardId);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>死亡时对凶手造成自身最大生命30%的伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddHp(-d.MaxHp*0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魂守</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时永久增加0-50%攻击和防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk.Source*=MathTool.GetRandom(1f,1.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.StealWeapon(d);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>盗取</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>破甲</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>25分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>20分</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>灵性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用本系卷轴造成额外30%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetMDamageRate(1.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AttackType==s.Attr&amp;&amp;s.HasScroll</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>通魔</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AttackType==0</t>
-  </si>
-  <si>
-    <t>攻击默认为自身属性魔法攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yuanbao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>元爆</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mattack</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>尖刺</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反弹20%所受伤害(自己仍受到100%伤害)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>欺压</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>猎杀</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(1.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Star&gt;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对星级低于3的敌人造成150%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对星级高于5的敌人造成150%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>探索</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>武装</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wuzhuang</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sidekicker</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以为其他单位提供支援</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>援护</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sidekickee</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以令其他单位提供支援</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>空灵</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.AddMaxHp(o.MaxHp.Source*0.15);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时提高所有无属性单位15%最大生命值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>狂液体</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>venom</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时使周围单位基础攻击力变为基础生命的1/5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>扭曲</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>亡眼</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击追加10%最大生命伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.AddPDamage(d.MaxHp.Source*0.10);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>威严</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.WeaponId&gt;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>打造</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡后装备武器返回召唤师手牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.WeaponReturn();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>幻化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEF</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时对选定目标造成魔法伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时对最近的3个敌人造成伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortDistance(true).Top(1)) mon.OnMagicDamage(s.Atk.Source*1.5,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>气化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>躲闪</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit-=20;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>!isMelee</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>受到远程单位攻击提高20%回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>重生</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>chongsheng</t>
-  </si>
-  <si>
-    <t>生命值低于30%时直接回复所有生命值（cd5回合）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>变形</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>进化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Transform((MathTool.GetRandom(2) == 0) ? 51000001 : 51000047);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddActionRate(0.3);d.AddActionRate(-0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>乱刃</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奏乐</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000002,lv,"E");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔王</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id)) o.MadDrug();</t>
+    <t>酒桶</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>jiutong</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>transmitred</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -2789,560 +3362,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(s.Attr)){o.AddMaxHp(o.MaxHp.Source*0.2);o.Atk*=0.2;}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时永久提高同属性单位20%最大生命值和攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mowang</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反弹所有物理攻击(自己不承受伤害)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反弹</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddHp(-damage.NoDefenceValue);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>反击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Owner.AddMana(s,1,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣光</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>闪击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Spd&gt;d.Spd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对速度低于自身的单位造成130%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>虚无</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit-=40;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命满时拥有40%额外回避</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>招架</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>抵挡50%伤害，但会永久降低5%攻击力</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0.5);d.Atk.Source*=0.95;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>立场</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时减少对方召唤师1点LP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时回复召唤师1点MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Transform(51000114);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>变向</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时将范围内的所有目标传到临近行</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.SetToPosition("side");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NAW</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时，如果自身手牌数&gt;6，提高50%攻击力</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NFR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.AddHpRate(0.2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合对1.5卡片距离友方恢复20%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhiliao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CheckSpecial</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.ClearDebuff();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每2回合清除2.5卡片范围内友军负面状态</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000023,lv,"F").AddAttr("Water");</t>
-  </si>
-  <si>
-    <t>我方水系单位</t>
-  </si>
-  <si>
-    <t>coverauro</t>
-  </si>
-  <si>
-    <t>召唤时永久提高水属性单位20%最大生命值</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>神射</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk.Source*=1.1;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合提高10%攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) o.ExtendDebuff(2);</t>
-  </si>
-  <si>
-    <t>延长范围内敌方怪物负面状态2回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillAfterHitEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Owner.AddCard(d.CardId, d.Level);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>杀死目标后获得该卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>过牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterAttr(1)){o.AddMaxHp(o.MaxHp.Source*0.2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.SetToPosition("back");</t>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(1.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(1.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>提高30%伤害，击中目标后使其后退1卡片距离</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>停留</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>敌我等级&gt;5单位</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000001,lv,"A").SetStar(6,10);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>震退</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk*=(s.GetMonsterCountByRace(4)*0.2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时场上每有一只昆虫，提高20%攻击力</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Star&lt;3</t>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0);</t>
-  </si>
-  <si>
-    <t>抵挡一次星级低于3敌人的物理攻击</t>
-  </si>
-  <si>
-    <t>小盾</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEC</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,d.Position)) o.AddHp(-damage.Value*0.4);</t>
-  </si>
-  <si>
-    <t>击中目标后造成目标同一列敌人40%伤害</t>
-  </si>
-  <si>
-    <t>coveraoe</t>
-  </si>
-  <si>
-    <t>guimian</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时，如果对方手牌数&gt;5，提高30%攻击和防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SkillInitialEffectDelegate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Owner.CardNumber&gt;=6) s.Atk*=0.5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk*=s.Owner.CardNumber;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Rival.CardNumber&gt;5) {s.Atk*=0.3;s.Def*=0.3;}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Star&lt;5</t>
-  </si>
-  <si>
-    <t>d.Transform(51010002);</t>
-  </si>
-  <si>
-    <t>d.AddBuff(56000001,lv,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000101,lv,"F").AddRace("Plant");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时对10格内敌方恐惧3回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) s.AddBuff(55510003,lv,3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>xieqi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkball</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAntiMagic("All",100);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔抗</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAntiMagic("All",50);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有魔法伤害下降50%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.IsDefence</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>破坏</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对防御型单位造成200%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>silie</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>撕裂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>pohuai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷途</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>魅惑</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Rebel();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后使目标反叛</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>meihuo</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>爆破</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>baopo</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后对1卡片距离敌人造成100%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>baopo2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>击中目标后对2卡片距离敌人造成100%伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AttackType==0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>爆破改</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EffectArea</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>curseoff</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>rocket</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Transform(MathTool.GetRandom(51000001,51000300));</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.CrtDamAddRate+=0.5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>暴击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>暴击伤害提升50%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>baoji</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddAuro(56000131,lv,"E");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>噩梦</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>emeng</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Owner.AddSpike(57000008);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Owner.RemoveSpike(57000008);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>学徒</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有玩家每回合多抽一张牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有玩家使用魔法卡消耗+3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有玩家使用魔法卡消耗-3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有玩家使用怪物卡消耗-3</t>
-  </si>
-  <si>
-    <t>所有玩家使用卡片消耗+1</t>
-  </si>
-  <si>
-    <t>所有玩家使用武器卡消耗-2</t>
-  </si>
-  <si>
-    <t>使用魔法卡消耗-1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.AddHpRate(0.2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bluebubble</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>气泡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qipao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时恢复1.2卡片距离友方20%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tanqiu</t>
-  </si>
-  <si>
-    <t>探求</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时抽一张牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DeathHit</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Owner.GetNextNCard(1);</t>
+    <t>使最近的友方单位返回手牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Return();</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5510,8 +5534,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z169" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:Z169"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z170" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:Z170"/>
   <sortState ref="A4:Z118">
     <sortCondition ref="A3:A118"/>
   </sortState>
@@ -5834,14 +5858,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z169"/>
+  <dimension ref="A1:Z170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C146" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomRight" activeCell="H154" sqref="H154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5967,7 +5991,7 @@
         <v>568</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>341</v>
@@ -5985,7 +6009,7 @@
         <v>644</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>309</v>
@@ -6065,10 +6089,10 @@
         <v>304</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>442</v>
@@ -6089,7 +6113,7 @@
         <v>320</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>347</v>
@@ -6415,7 +6439,7 @@
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="17"/>
@@ -6436,10 +6460,10 @@
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="25" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="61">
@@ -6557,7 +6581,7 @@
       <c r="F13" s="43"/>
       <c r="G13" s="59"/>
       <c r="H13" s="29" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="I13" s="29"/>
       <c r="J13" s="28"/>
@@ -6595,7 +6619,7 @@
         <v>55100011</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
@@ -6607,11 +6631,11 @@
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
       <c r="J14" s="28" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="17" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -6624,7 +6648,7 @@
         <v>239</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="T14" s="10"/>
       <c r="U14" s="1"/>
@@ -6643,7 +6667,7 @@
         <v>55100012</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>339</v>
@@ -6693,7 +6717,7 @@
         <v>55100013</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>
@@ -6702,7 +6726,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="43"/>
       <c r="G16" s="59" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
@@ -6720,7 +6744,7 @@
         <v>239</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -6730,7 +6754,7 @@
         <v>10</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="Z16" s="37"/>
     </row>
@@ -6739,7 +6763,7 @@
         <v>55100014</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>352</v>
@@ -6787,7 +6811,7 @@
         <v>55100015</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>352</v>
@@ -6803,7 +6827,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="O18" s="20"/>
       <c r="P18" s="41"/>
@@ -6814,7 +6838,7 @@
         <v>239</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="1" t="s">
@@ -6826,7 +6850,7 @@
         <v>16</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Z18" s="37"/>
     </row>
@@ -6973,7 +6997,7 @@
         <v>55110004</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>0</v>
@@ -6983,7 +7007,7 @@
       <c r="F22" s="43"/>
       <c r="G22" s="59"/>
       <c r="H22" s="29" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I22" s="29"/>
       <c r="J22" s="28"/>
@@ -7000,7 +7024,7 @@
         <v>239</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="T22" s="10"/>
       <c r="U22" s="1"/>
@@ -7019,7 +7043,7 @@
         <v>55110005</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>36</v>
@@ -7031,7 +7055,7 @@
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
       <c r="J23" s="28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="17"/>
@@ -7048,7 +7072,7 @@
         <v>239</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="T23" s="14"/>
       <c r="U23" s="1"/>
@@ -7067,7 +7091,7 @@
         <v>55110006</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
@@ -7083,7 +7107,7 @@
       </c>
       <c r="K24" s="18"/>
       <c r="L24" s="17" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -7096,7 +7120,7 @@
         <v>239</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="T24" s="10"/>
       <c r="U24" s="1"/>
@@ -7115,7 +7139,7 @@
         <v>55110007</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>1</v>
@@ -7127,11 +7151,11 @@
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
       <c r="J25" s="28" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="K25" s="18"/>
       <c r="L25" s="17" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
@@ -7144,7 +7168,7 @@
         <v>239</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="T25" s="10"/>
       <c r="U25" s="1"/>
@@ -7163,7 +7187,7 @@
         <v>55110008</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -7209,7 +7233,7 @@
         <v>55110009</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -7223,7 +7247,7 @@
       <c r="J27" s="28"/>
       <c r="K27" s="18"/>
       <c r="L27" s="17" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
@@ -7236,7 +7260,7 @@
         <v>239</v>
       </c>
       <c r="S27" s="10" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="T27" s="10"/>
       <c r="U27" s="1"/>
@@ -7255,7 +7279,7 @@
         <v>55110010</v>
       </c>
       <c r="B28" s="75" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>36</v>
@@ -7267,7 +7291,7 @@
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
       <c r="J28" s="28" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="K28" s="18"/>
       <c r="L28" s="17" t="s">
@@ -7303,7 +7327,7 @@
         <v>55110011</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>36</v>
@@ -7315,10 +7339,10 @@
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
       <c r="J29" s="28" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
@@ -7332,7 +7356,7 @@
         <v>239</v>
       </c>
       <c r="S29" s="10" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="T29" s="10"/>
       <c r="U29" s="1"/>
@@ -7351,7 +7375,7 @@
         <v>55110012</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>1</v>
@@ -7366,7 +7390,7 @@
       <c r="K30" s="18"/>
       <c r="L30" s="17"/>
       <c r="M30" s="17" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="N30" s="17"/>
       <c r="O30" s="20"/>
@@ -7397,7 +7421,7 @@
         <v>55110013</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>36</v>
@@ -7409,14 +7433,14 @@
       <c r="H31" s="29"/>
       <c r="I31" s="29"/>
       <c r="J31" s="28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K31" s="18"/>
       <c r="L31" s="17" t="s">
+        <v>746</v>
+      </c>
+      <c r="M31" s="17" t="s">
         <v>747</v>
-      </c>
-      <c r="M31" s="17" t="s">
-        <v>748</v>
       </c>
       <c r="N31" s="17"/>
       <c r="O31" s="20"/>
@@ -7428,7 +7452,7 @@
         <v>239</v>
       </c>
       <c r="S31" s="10" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="T31" s="10"/>
       <c r="U31" s="1"/>
@@ -7447,7 +7471,7 @@
         <v>55110014</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>36</v>
@@ -7493,7 +7517,7 @@
         <v>55110015</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>1</v>
@@ -7505,7 +7529,7 @@
       <c r="H33" s="29"/>
       <c r="I33" s="29"/>
       <c r="J33" s="28" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="K33" s="18"/>
       <c r="L33" s="17" t="s">
@@ -7522,7 +7546,7 @@
         <v>239</v>
       </c>
       <c r="S33" s="10" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="T33" s="10"/>
       <c r="U33" s="1"/>
@@ -7541,7 +7565,7 @@
         <v>55110016</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>36</v>
@@ -7556,7 +7580,7 @@
         <v>303</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="L34" s="17"/>
       <c r="M34" s="17"/>
@@ -7570,7 +7594,7 @@
         <v>239</v>
       </c>
       <c r="S34" s="10" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="T34" s="10"/>
       <c r="U34" s="1"/>
@@ -7589,7 +7613,7 @@
         <v>55110017</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>36</v>
@@ -7603,7 +7627,7 @@
       <c r="J35" s="28"/>
       <c r="K35" s="18"/>
       <c r="L35" s="17" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -7616,7 +7640,7 @@
         <v>239</v>
       </c>
       <c r="S35" s="10" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="T35" s="10"/>
       <c r="U35" s="1"/>
@@ -7635,7 +7659,7 @@
         <v>55110018</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>36</v>
@@ -7685,7 +7709,7 @@
         <v>55110019</v>
       </c>
       <c r="B37" s="75" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>36</v>
@@ -7697,11 +7721,11 @@
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
       <c r="J37" s="26" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K37" s="27"/>
       <c r="L37" s="30" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
@@ -7714,7 +7738,7 @@
         <v>407</v>
       </c>
       <c r="S37" s="16" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="T37" s="25"/>
       <c r="U37" s="25" t="s">
@@ -7826,7 +7850,7 @@
         <v>239</v>
       </c>
       <c r="S39" s="16" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="T39" s="25"/>
       <c r="U39" s="25" t="s">
@@ -7853,7 +7877,7 @@
         <v>99</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E40" s="31">
         <v>30</v>
@@ -7863,7 +7887,7 @@
       </c>
       <c r="G40" s="60"/>
       <c r="H40" s="47" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I40" s="89"/>
       <c r="J40" s="91"/>
@@ -7880,7 +7904,7 @@
         <v>407</v>
       </c>
       <c r="S40" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="T40" s="31"/>
       <c r="U40" s="31"/>
@@ -7907,7 +7931,7 @@
         <v>99</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E41" s="25">
         <v>15</v>
@@ -7922,7 +7946,7 @@
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="O41" s="20" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="P41" s="41">
         <v>1</v>
@@ -7934,7 +7958,7 @@
         <v>239</v>
       </c>
       <c r="S41" s="16" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="T41" s="25"/>
       <c r="U41" s="10" t="s">
@@ -7948,7 +7972,7 @@
         <v>40</v>
       </c>
       <c r="Y41" s="25" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="Z41" s="96"/>
     </row>
@@ -7963,13 +7987,13 @@
         <v>99</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E42" s="25">
         <v>25</v>
       </c>
       <c r="F42" s="44" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="G42" s="59"/>
       <c r="H42" s="47"/>
@@ -7980,7 +8004,7 @@
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
       <c r="O42" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="P42" s="41">
         <v>2</v>
@@ -7992,7 +8016,7 @@
         <v>239</v>
       </c>
       <c r="S42" s="16" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="T42" s="25"/>
       <c r="U42" s="10" t="s">
@@ -8033,7 +8057,7 @@
       <c r="H43" s="29"/>
       <c r="I43" s="29"/>
       <c r="J43" s="28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K43" s="18"/>
       <c r="L43" s="17"/>
@@ -8093,7 +8117,7 @@
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
       <c r="J44" s="28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="17"/>
@@ -8141,24 +8165,24 @@
         <v>99</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E45" s="25">
         <v>20</v>
       </c>
       <c r="F45" s="44" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G45" s="60"/>
       <c r="H45" s="29"/>
       <c r="I45" s="29"/>
       <c r="J45" s="26" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K45" s="27"/>
       <c r="L45" s="30"/>
       <c r="M45" s="17" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="N45" s="17"/>
       <c r="O45" s="20"/>
@@ -8170,7 +8194,7 @@
         <v>407</v>
       </c>
       <c r="S45" s="16" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="T45" s="25"/>
       <c r="U45" s="25" t="s">
@@ -8180,7 +8204,7 @@
         <v>447</v>
       </c>
       <c r="W45" s="25" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="X45" s="25">
         <v>25</v>
@@ -8211,7 +8235,7 @@
       <c r="H46" s="29"/>
       <c r="I46" s="29"/>
       <c r="J46" s="28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K46" s="18"/>
       <c r="L46" s="17"/>
@@ -8269,7 +8293,7 @@
       </c>
       <c r="G47" s="60"/>
       <c r="H47" s="29" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="I47" s="29"/>
       <c r="J47" s="28"/>
@@ -8286,11 +8310,11 @@
         <v>239</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="T47" s="25"/>
       <c r="U47" s="25" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="V47" s="25"/>
       <c r="W47" s="25"/>
@@ -8298,7 +8322,7 @@
         <v>25</v>
       </c>
       <c r="Y47" s="25" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="Z47" s="39"/>
     </row>
@@ -8307,13 +8331,13 @@
         <v>55200011</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C48" s="25" t="s">
         <v>99</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E48" s="25">
         <v>12</v>
@@ -8321,7 +8345,7 @@
       <c r="F48" s="44"/>
       <c r="G48" s="59"/>
       <c r="H48" s="47" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="I48" s="47"/>
       <c r="J48" s="26"/>
@@ -8338,21 +8362,21 @@
         <v>239</v>
       </c>
       <c r="S48" s="16" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="T48" s="25"/>
       <c r="U48" s="10" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="V48" s="10" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="W48" s="10"/>
       <c r="X48" s="25">
         <v>20</v>
       </c>
       <c r="Y48" s="25" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Z48" s="96"/>
     </row>
@@ -8390,7 +8414,7 @@
         <v>239</v>
       </c>
       <c r="S49" s="16" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="T49" s="25"/>
       <c r="U49" s="25"/>
@@ -8440,7 +8464,7 @@
         <v>239</v>
       </c>
       <c r="S50" s="16" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="T50" s="25"/>
       <c r="U50" s="25"/>
@@ -8488,7 +8512,7 @@
         <v>239</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="T51" s="25"/>
       <c r="U51" s="25"/>
@@ -8536,7 +8560,7 @@
         <v>239</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="T52" s="25"/>
       <c r="U52" s="25"/>
@@ -8584,7 +8608,7 @@
         <v>239</v>
       </c>
       <c r="S53" s="16" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="T53" s="25"/>
       <c r="U53" s="25"/>
@@ -8680,7 +8704,7 @@
         <v>239</v>
       </c>
       <c r="S55" s="16" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="T55" s="25"/>
       <c r="U55" s="25"/>
@@ -8699,7 +8723,7 @@
         <v>55300008</v>
       </c>
       <c r="B56" s="53" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>49</v>
@@ -8709,10 +8733,10 @@
       <c r="F56" s="44"/>
       <c r="G56" s="60"/>
       <c r="H56" s="47" t="s">
+        <v>865</v>
+      </c>
+      <c r="I56" s="47" t="s">
         <v>866</v>
-      </c>
-      <c r="I56" s="47" t="s">
-        <v>867</v>
       </c>
       <c r="J56" s="26"/>
       <c r="K56" s="27"/>
@@ -8728,7 +8752,7 @@
         <v>239</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="T56" s="25"/>
       <c r="U56" s="25"/>
@@ -8811,7 +8835,7 @@
       <c r="L58" s="17"/>
       <c r="M58" s="17"/>
       <c r="N58" s="17" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="O58" s="20"/>
       <c r="P58" s="41"/>
@@ -8822,7 +8846,7 @@
         <v>239</v>
       </c>
       <c r="S58" s="10" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="T58" s="10"/>
       <c r="U58" s="1"/>
@@ -8868,7 +8892,7 @@
         <v>239</v>
       </c>
       <c r="S59" s="10" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="T59" s="10"/>
       <c r="U59" s="1"/>
@@ -9685,7 +9709,7 @@
       </c>
       <c r="K76" s="27"/>
       <c r="L76" s="30" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="M76" s="17"/>
       <c r="N76" s="17"/>
@@ -9972,7 +9996,7 @@
       <c r="K82" s="18"/>
       <c r="L82" s="17"/>
       <c r="M82" s="17" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="N82" s="17"/>
       <c r="O82" s="20"/>
@@ -10647,7 +10671,7 @@
         <v>55520002</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>35</v>
@@ -10739,7 +10763,7 @@
         <v>55520004</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>35</v>
@@ -10754,7 +10778,7 @@
       <c r="K99" s="18"/>
       <c r="L99" s="17"/>
       <c r="M99" s="17" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="N99" s="17"/>
       <c r="O99" s="20"/>
@@ -10766,7 +10790,7 @@
         <v>239</v>
       </c>
       <c r="S99" s="10" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="T99" s="10"/>
       <c r="U99" s="1"/>
@@ -10776,7 +10800,7 @@
         <v>150</v>
       </c>
       <c r="Y99" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="Z99" s="25"/>
     </row>
@@ -10845,7 +10869,7 @@
       <c r="F101" s="43"/>
       <c r="G101" s="60"/>
       <c r="H101" s="29" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="I101" s="29"/>
       <c r="J101" s="28"/>
@@ -11085,7 +11109,7 @@
         <v>55600007</v>
       </c>
       <c r="B106" s="58" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>49</v>
@@ -11245,7 +11269,7 @@
       <c r="F109" s="43"/>
       <c r="G109" s="60"/>
       <c r="H109" s="29" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="I109" s="29"/>
       <c r="J109" s="28"/>
@@ -11295,7 +11319,7 @@
       <c r="F110" s="43"/>
       <c r="G110" s="60"/>
       <c r="H110" s="29" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I110" s="29"/>
       <c r="J110" s="28"/>
@@ -11312,7 +11336,7 @@
         <v>407</v>
       </c>
       <c r="S110" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="T110" s="10">
         <v>56000023</v>
@@ -11320,7 +11344,7 @@
       <c r="U110" s="1"/>
       <c r="V110" s="1"/>
       <c r="W110" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="X110" s="1">
         <v>20</v>
@@ -11385,7 +11409,7 @@
         <v>55600013</v>
       </c>
       <c r="B112" s="58" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>49</v>
@@ -11395,7 +11419,7 @@
       <c r="F112" s="43"/>
       <c r="G112" s="60"/>
       <c r="H112" s="29" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="I112" s="29"/>
       <c r="J112" s="28"/>
@@ -11412,7 +11436,7 @@
         <v>239</v>
       </c>
       <c r="S112" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="T112" s="10">
         <v>56000001</v>
@@ -11435,7 +11459,7 @@
         <v>55600014</v>
       </c>
       <c r="B113" s="58" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>49</v>
@@ -11445,7 +11469,7 @@
       <c r="F113" s="43"/>
       <c r="G113" s="60"/>
       <c r="H113" s="29" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="I113" s="29"/>
       <c r="J113" s="28"/>
@@ -11476,7 +11500,7 @@
         <v>30</v>
       </c>
       <c r="Y113" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="Z113" s="37"/>
     </row>
@@ -11865,7 +11889,7 @@
         <v>55700005</v>
       </c>
       <c r="B122" s="52" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C122" s="25" t="s">
         <v>406</v>
@@ -11882,7 +11906,7 @@
       <c r="M122" s="17"/>
       <c r="N122" s="17"/>
       <c r="O122" s="20" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="P122" s="41">
         <v>1</v>
@@ -11894,7 +11918,7 @@
         <v>407</v>
       </c>
       <c r="S122" s="16" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="T122" s="25"/>
       <c r="U122" s="25"/>
@@ -11931,7 +11955,7 @@
       </c>
       <c r="G123" s="60"/>
       <c r="H123" s="47" t="s">
-        <v>666</v>
+        <v>885</v>
       </c>
       <c r="I123" s="47"/>
       <c r="J123" s="26"/>
@@ -11989,7 +12013,7 @@
       </c>
       <c r="G124" s="60"/>
       <c r="H124" s="47" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I124" s="47"/>
       <c r="J124" s="26"/>
@@ -12037,7 +12061,7 @@
       <c r="F125" s="44"/>
       <c r="G125" s="60"/>
       <c r="H125" s="47" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="I125" s="47"/>
       <c r="J125" s="26"/>
@@ -12137,7 +12161,7 @@
       <c r="L127" s="17"/>
       <c r="M127" s="17"/>
       <c r="N127" s="17" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="O127" s="20"/>
       <c r="P127" s="41"/>
@@ -12148,7 +12172,7 @@
         <v>239</v>
       </c>
       <c r="S127" s="49" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="T127" s="25"/>
       <c r="U127" s="25"/>
@@ -12167,7 +12191,7 @@
         <v>55900006</v>
       </c>
       <c r="B128" s="55" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>0</v>
@@ -12184,7 +12208,7 @@
       <c r="K128" s="18"/>
       <c r="L128" s="17"/>
       <c r="M128" s="17" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="N128" s="17"/>
       <c r="O128" s="20"/>
@@ -12215,7 +12239,7 @@
         <v>55900007</v>
       </c>
       <c r="B129" s="55" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>0</v>
@@ -12261,7 +12285,7 @@
         <v>55900008</v>
       </c>
       <c r="B130" s="55" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>0</v>
@@ -12298,7 +12322,7 @@
         <v>40</v>
       </c>
       <c r="Y130" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="Z130" s="39"/>
     </row>
@@ -12307,7 +12331,7 @@
         <v>55900009</v>
       </c>
       <c r="B131" s="55" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>0</v>
@@ -12316,7 +12340,7 @@
       <c r="E131" s="1"/>
       <c r="F131" s="43"/>
       <c r="G131" s="60" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H131" s="29"/>
       <c r="I131" s="29"/>
@@ -12334,7 +12358,7 @@
         <v>239</v>
       </c>
       <c r="S131" s="10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="T131" s="10"/>
       <c r="U131" s="1"/>
@@ -12344,7 +12368,7 @@
         <v>30</v>
       </c>
       <c r="Y131" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Z131" s="37"/>
     </row>
@@ -12353,7 +12377,7 @@
         <v>55900010</v>
       </c>
       <c r="B132" s="55" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>0</v>
@@ -12362,7 +12386,7 @@
       <c r="E132" s="1"/>
       <c r="F132" s="43"/>
       <c r="G132" s="60" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H132" s="29"/>
       <c r="I132" s="29"/>
@@ -12380,7 +12404,7 @@
         <v>239</v>
       </c>
       <c r="S132" s="10" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="T132" s="1"/>
       <c r="U132" s="1"/>
@@ -12399,7 +12423,7 @@
         <v>55900011</v>
       </c>
       <c r="B133" s="55" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>0</v>
@@ -12409,7 +12433,7 @@
       <c r="F133" s="43"/>
       <c r="G133" s="60"/>
       <c r="H133" s="47" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I133" s="47"/>
       <c r="J133" s="26"/>
@@ -12426,7 +12450,7 @@
         <v>239</v>
       </c>
       <c r="S133" s="10" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="T133" s="10"/>
       <c r="U133" s="1"/>
@@ -12445,7 +12469,7 @@
         <v>55900012</v>
       </c>
       <c r="B134" s="55" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C134" s="25" t="s">
         <v>338</v>
@@ -12461,7 +12485,7 @@
       </c>
       <c r="G134" s="60"/>
       <c r="H134" s="29" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I134" s="29"/>
       <c r="J134" s="28"/>
@@ -12478,12 +12502,12 @@
         <v>239</v>
       </c>
       <c r="S134" s="16" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="T134" s="25"/>
       <c r="U134" s="25"/>
       <c r="V134" s="25" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="W134" s="25"/>
       <c r="X134" s="25">
@@ -12499,7 +12523,7 @@
         <v>55900013</v>
       </c>
       <c r="B135" s="55" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>0</v>
@@ -12511,7 +12535,7 @@
       <c r="H135" s="29"/>
       <c r="I135" s="29"/>
       <c r="J135" s="28" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="K135" s="18"/>
       <c r="L135" s="17" t="s">
@@ -12547,7 +12571,7 @@
         <v>55900014</v>
       </c>
       <c r="B136" s="55" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>0</v>
@@ -12565,7 +12589,7 @@
       <c r="L136" s="17"/>
       <c r="M136" s="17"/>
       <c r="N136" s="17" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="O136" s="20"/>
       <c r="P136" s="41"/>
@@ -12576,7 +12600,7 @@
         <v>239</v>
       </c>
       <c r="S136" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="T136" s="1"/>
       <c r="U136" s="1"/>
@@ -12595,7 +12619,7 @@
         <v>55900015</v>
       </c>
       <c r="B137" s="55" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>0</v>
@@ -12641,7 +12665,7 @@
         <v>55900016</v>
       </c>
       <c r="B138" s="55" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>338</v>
@@ -12672,7 +12696,7 @@
         <v>239</v>
       </c>
       <c r="S138" s="10" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="T138" s="10"/>
       <c r="U138" s="1" t="s">
@@ -12684,7 +12708,7 @@
         <v>45</v>
       </c>
       <c r="Y138" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="Z138" s="48"/>
     </row>
@@ -12693,7 +12717,7 @@
         <v>55900017</v>
       </c>
       <c r="B139" s="55" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>338</v>
@@ -12710,7 +12734,7 @@
       <c r="M139" s="21"/>
       <c r="N139" s="21"/>
       <c r="O139" s="20" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="P139" s="41">
         <v>1</v>
@@ -12745,7 +12769,7 @@
         <v>55900018</v>
       </c>
       <c r="B140" s="55" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>338</v>
@@ -12762,7 +12786,7 @@
       <c r="M140" s="21"/>
       <c r="N140" s="21"/>
       <c r="O140" s="19" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="P140" s="41">
         <v>1</v>
@@ -12797,7 +12821,7 @@
         <v>55900019</v>
       </c>
       <c r="B141" s="55" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>338</v>
@@ -12814,7 +12838,7 @@
       <c r="M141" s="21"/>
       <c r="N141" s="21"/>
       <c r="O141" s="20" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="P141" s="41">
         <v>1</v>
@@ -12849,13 +12873,13 @@
         <v>55900020</v>
       </c>
       <c r="B142" s="55" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C142" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D142" s="25" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E142" s="25">
         <v>30</v>
@@ -12865,7 +12889,7 @@
       </c>
       <c r="G142" s="79"/>
       <c r="H142" s="29" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="I142" s="88"/>
       <c r="J142" s="90"/>
@@ -12882,7 +12906,7 @@
         <v>239</v>
       </c>
       <c r="S142" s="10" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="T142" s="78"/>
       <c r="U142" s="78"/>
@@ -12892,7 +12916,7 @@
         <v>20</v>
       </c>
       <c r="Y142" s="25" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Z142" s="83"/>
     </row>
@@ -12901,7 +12925,7 @@
         <v>55900021</v>
       </c>
       <c r="B143" s="55" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C143" s="25" t="s">
         <v>0</v>
@@ -12949,13 +12973,13 @@
         <v>55900022</v>
       </c>
       <c r="B144" s="55" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C144" s="25" t="s">
         <v>406</v>
       </c>
       <c r="D144" s="25" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E144" s="25">
         <v>200</v>
@@ -12963,7 +12987,7 @@
       <c r="F144" s="25"/>
       <c r="G144" s="60"/>
       <c r="H144" s="84" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I144" s="47"/>
       <c r="J144" s="26"/>
@@ -12980,7 +13004,7 @@
         <v>407</v>
       </c>
       <c r="S144" s="16" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="T144" s="25"/>
       <c r="U144" s="25" t="s">
@@ -13006,14 +13030,14 @@
         <v>149</v>
       </c>
       <c r="C145" s="25" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="25"/>
       <c r="F145" s="25"/>
       <c r="G145" s="60"/>
       <c r="H145" s="84" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I145" s="47"/>
       <c r="J145" s="26"/>
@@ -13030,7 +13054,7 @@
         <v>407</v>
       </c>
       <c r="S145" s="16" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="T145" s="25"/>
       <c r="U145" s="25"/>
@@ -13065,7 +13089,7 @@
       </c>
       <c r="G146" s="60"/>
       <c r="H146" s="29" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="I146" s="29"/>
       <c r="J146" s="26"/>
@@ -13082,7 +13106,7 @@
         <v>407</v>
       </c>
       <c r="S146" s="10" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="T146" s="25"/>
       <c r="U146" s="25"/>
@@ -13124,7 +13148,7 @@
       <c r="M147" s="17"/>
       <c r="N147" s="17"/>
       <c r="O147" s="20" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="P147" s="41">
         <v>2</v>
@@ -13136,7 +13160,7 @@
         <v>407</v>
       </c>
       <c r="S147" s="16" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="T147" s="25"/>
       <c r="U147" s="25" t="s">
@@ -13175,7 +13199,7 @@
       <c r="L148" s="30"/>
       <c r="M148" s="17"/>
       <c r="N148" s="17" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="O148" s="20"/>
       <c r="P148" s="41"/>
@@ -13186,7 +13210,7 @@
         <v>407</v>
       </c>
       <c r="S148" s="16" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="T148" s="25"/>
       <c r="U148" s="25"/>
@@ -13199,7 +13223,7 @@
         <v>191</v>
       </c>
       <c r="Z148" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="149" spans="1:26" ht="27">
@@ -13207,7 +13231,7 @@
         <v>55900027</v>
       </c>
       <c r="B149" s="55" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C149" s="25" t="s">
         <v>0</v>
@@ -13221,10 +13245,10 @@
       <c r="J149" s="26"/>
       <c r="K149" s="27"/>
       <c r="L149" s="30" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="M149" s="17" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="N149" s="17"/>
       <c r="O149" s="20"/>
@@ -13236,7 +13260,7 @@
         <v>407</v>
       </c>
       <c r="S149" s="16" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="T149" s="25"/>
       <c r="U149" s="25"/>
@@ -13265,7 +13289,7 @@
       <c r="F150" s="44"/>
       <c r="G150" s="60"/>
       <c r="H150" s="84" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I150" s="47"/>
       <c r="J150" s="26"/>
@@ -13282,7 +13306,7 @@
         <v>407</v>
       </c>
       <c r="S150" s="16" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="T150" s="25"/>
       <c r="U150" s="25"/>
@@ -13309,7 +13333,7 @@
       <c r="F151" s="25"/>
       <c r="G151" s="60"/>
       <c r="H151" s="84" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="I151" s="47"/>
       <c r="J151" s="26"/>
@@ -13326,7 +13350,7 @@
         <v>407</v>
       </c>
       <c r="S151" s="16" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="T151" s="25"/>
       <c r="U151" s="25"/>
@@ -13336,7 +13360,7 @@
         <v>15</v>
       </c>
       <c r="Y151" s="25" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="Z151" s="48"/>
     </row>
@@ -13357,12 +13381,12 @@
       <c r="H152" s="84"/>
       <c r="I152" s="47"/>
       <c r="J152" s="26" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K152" s="27"/>
       <c r="L152" s="30"/>
       <c r="M152" s="17" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="N152" s="17"/>
       <c r="O152" s="20"/>
@@ -13395,7 +13419,7 @@
         <v>55900031</v>
       </c>
       <c r="B153" s="55" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C153" s="25" t="s">
         <v>0</v>
@@ -13405,7 +13429,7 @@
       <c r="F153" s="25"/>
       <c r="G153" s="60"/>
       <c r="H153" s="84" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I153" s="47"/>
       <c r="J153" s="26"/>
@@ -13422,7 +13446,7 @@
         <v>407</v>
       </c>
       <c r="S153" s="16" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="T153" s="25"/>
       <c r="U153" s="25"/>
@@ -13432,33 +13456,37 @@
         <v>5</v>
       </c>
       <c r="Y153" s="25" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="Z153" s="48"/>
     </row>
-    <row r="154" spans="1:26" ht="36">
-      <c r="A154" s="98">
-        <v>55990001</v>
-      </c>
-      <c r="B154" s="98" t="s">
-        <v>23</v>
+    <row r="154" spans="1:26" ht="84">
+      <c r="A154" s="55">
+        <v>55900032</v>
+      </c>
+      <c r="B154" s="55" t="s">
+        <v>886</v>
       </c>
       <c r="C154" s="25" t="s">
-        <v>830</v>
-      </c>
-      <c r="D154" s="25"/>
-      <c r="E154" s="25"/>
-      <c r="F154" s="25"/>
+        <v>0</v>
+      </c>
+      <c r="D154" s="25" t="s">
+        <v>889</v>
+      </c>
+      <c r="E154" s="25">
+        <v>12</v>
+      </c>
+      <c r="F154" s="44" t="s">
+        <v>470</v>
+      </c>
       <c r="G154" s="60"/>
-      <c r="H154" s="97"/>
+      <c r="H154" s="97" t="s">
+        <v>891</v>
+      </c>
       <c r="I154" s="29"/>
-      <c r="J154" s="26" t="s">
-        <v>411</v>
-      </c>
+      <c r="J154" s="26"/>
       <c r="K154" s="27"/>
-      <c r="L154" s="30" t="s">
-        <v>282</v>
-      </c>
+      <c r="L154" s="30"/>
       <c r="M154" s="17"/>
       <c r="N154" s="17"/>
       <c r="O154" s="20"/>
@@ -13467,34 +13495,34 @@
         <v>244</v>
       </c>
       <c r="R154" s="44" t="s">
-        <v>239</v>
+        <v>407</v>
       </c>
       <c r="S154" s="16" t="s">
-        <v>400</v>
+        <v>890</v>
       </c>
       <c r="T154" s="25"/>
-      <c r="U154" s="25"/>
+      <c r="U154" s="25" t="s">
+        <v>888</v>
+      </c>
       <c r="V154" s="25"/>
       <c r="W154" s="25"/>
       <c r="X154" s="25">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Y154" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z154" s="48" t="s">
-        <v>828</v>
-      </c>
+        <v>887</v>
+      </c>
+      <c r="Z154" s="48"/>
     </row>
     <row r="155" spans="1:26" ht="36">
       <c r="A155" s="98">
-        <v>55990002</v>
+        <v>55990001</v>
       </c>
       <c r="B155" s="98" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C155" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25"/>
@@ -13503,7 +13531,7 @@
       <c r="H155" s="97"/>
       <c r="I155" s="29"/>
       <c r="J155" s="26" t="s">
-        <v>270</v>
+        <v>411</v>
       </c>
       <c r="K155" s="27"/>
       <c r="L155" s="30" t="s">
@@ -13519,8 +13547,8 @@
       <c r="R155" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="S155" s="49" t="s">
-        <v>401</v>
+      <c r="S155" s="16" t="s">
+        <v>400</v>
       </c>
       <c r="T155" s="25"/>
       <c r="U155" s="25"/>
@@ -13530,21 +13558,21 @@
         <v>15</v>
       </c>
       <c r="Y155" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Z155" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="156" spans="1:26" ht="36">
       <c r="A156" s="98">
-        <v>55990003</v>
+        <v>55990002</v>
       </c>
       <c r="B156" s="98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C156" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D156" s="25"/>
       <c r="E156" s="25"/>
@@ -13553,7 +13581,7 @@
       <c r="H156" s="97"/>
       <c r="I156" s="29"/>
       <c r="J156" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K156" s="27"/>
       <c r="L156" s="30" t="s">
@@ -13570,7 +13598,7 @@
         <v>239</v>
       </c>
       <c r="S156" s="49" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="T156" s="25"/>
       <c r="U156" s="25"/>
@@ -13580,21 +13608,21 @@
         <v>15</v>
       </c>
       <c r="Y156" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Z156" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="157" spans="1:26" ht="36">
       <c r="A157" s="98">
-        <v>55990004</v>
+        <v>55990003</v>
       </c>
       <c r="B157" s="98" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C157" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D157" s="25"/>
       <c r="E157" s="25"/>
@@ -13603,7 +13631,7 @@
       <c r="H157" s="97"/>
       <c r="I157" s="29"/>
       <c r="J157" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K157" s="27"/>
       <c r="L157" s="30" t="s">
@@ -13620,7 +13648,7 @@
         <v>239</v>
       </c>
       <c r="S157" s="49" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="T157" s="25"/>
       <c r="U157" s="25"/>
@@ -13630,21 +13658,21 @@
         <v>15</v>
       </c>
       <c r="Y157" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z157" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="158" spans="1:26" ht="36">
       <c r="A158" s="98">
-        <v>55990005</v>
+        <v>55990004</v>
       </c>
       <c r="B158" s="98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C158" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D158" s="25"/>
       <c r="E158" s="25"/>
@@ -13653,7 +13681,7 @@
       <c r="H158" s="97"/>
       <c r="I158" s="29"/>
       <c r="J158" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K158" s="27"/>
       <c r="L158" s="30" t="s">
@@ -13670,7 +13698,7 @@
         <v>239</v>
       </c>
       <c r="S158" s="49" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="T158" s="25"/>
       <c r="U158" s="25"/>
@@ -13680,21 +13708,21 @@
         <v>15</v>
       </c>
       <c r="Y158" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Z158" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="159" spans="1:26" ht="36">
       <c r="A159" s="98">
-        <v>55990006</v>
+        <v>55990005</v>
       </c>
       <c r="B159" s="98" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C159" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25"/>
@@ -13703,7 +13731,7 @@
       <c r="H159" s="97"/>
       <c r="I159" s="29"/>
       <c r="J159" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K159" s="27"/>
       <c r="L159" s="30" t="s">
@@ -13720,7 +13748,7 @@
         <v>239</v>
       </c>
       <c r="S159" s="49" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="T159" s="25"/>
       <c r="U159" s="25"/>
@@ -13730,21 +13758,21 @@
         <v>15</v>
       </c>
       <c r="Y159" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Z159" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="160" spans="1:26" ht="36">
       <c r="A160" s="98">
-        <v>55990011</v>
+        <v>55990006</v>
       </c>
       <c r="B160" s="98" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C160" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25"/>
@@ -13753,24 +13781,24 @@
       <c r="H160" s="97"/>
       <c r="I160" s="29"/>
       <c r="J160" s="26" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="K160" s="27"/>
       <c r="L160" s="30" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="M160" s="17"/>
       <c r="N160" s="17"/>
       <c r="O160" s="20"/>
       <c r="P160" s="41"/>
       <c r="Q160" s="46" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="R160" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="S160" s="16" t="s">
-        <v>286</v>
+      <c r="S160" s="49" t="s">
+        <v>415</v>
       </c>
       <c r="T160" s="25"/>
       <c r="U160" s="25"/>
@@ -13780,21 +13808,21 @@
         <v>15</v>
       </c>
       <c r="Y160" s="25" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="Z160" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="161" spans="1:26" ht="36">
       <c r="A161" s="98">
-        <v>55990012</v>
+        <v>55990011</v>
       </c>
       <c r="B161" s="98" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C161" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D161" s="25"/>
       <c r="E161" s="25"/>
@@ -13803,7 +13831,7 @@
       <c r="H161" s="97"/>
       <c r="I161" s="29"/>
       <c r="J161" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K161" s="27"/>
       <c r="L161" s="30" t="s">
@@ -13820,7 +13848,7 @@
         <v>239</v>
       </c>
       <c r="S161" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T161" s="25"/>
       <c r="U161" s="25"/>
@@ -13830,21 +13858,21 @@
         <v>15</v>
       </c>
       <c r="Y161" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Z161" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="162" spans="1:26" ht="36">
       <c r="A162" s="98">
-        <v>55990013</v>
+        <v>55990012</v>
       </c>
       <c r="B162" s="98" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C162" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25"/>
@@ -13853,7 +13881,7 @@
       <c r="H162" s="97"/>
       <c r="I162" s="29"/>
       <c r="J162" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K162" s="27"/>
       <c r="L162" s="30" t="s">
@@ -13870,7 +13898,7 @@
         <v>239</v>
       </c>
       <c r="S162" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T162" s="25"/>
       <c r="U162" s="25"/>
@@ -13880,21 +13908,21 @@
         <v>15</v>
       </c>
       <c r="Y162" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Z162" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="163" spans="1:26" ht="36">
       <c r="A163" s="98">
-        <v>55990014</v>
+        <v>55990013</v>
       </c>
       <c r="B163" s="98" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C163" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D163" s="25"/>
       <c r="E163" s="25"/>
@@ -13903,7 +13931,7 @@
       <c r="H163" s="97"/>
       <c r="I163" s="29"/>
       <c r="J163" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K163" s="27"/>
       <c r="L163" s="30" t="s">
@@ -13920,7 +13948,7 @@
         <v>239</v>
       </c>
       <c r="S163" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T163" s="25"/>
       <c r="U163" s="25"/>
@@ -13930,21 +13958,21 @@
         <v>15</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Z163" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="164" spans="1:26" ht="36">
       <c r="A164" s="98">
-        <v>55990015</v>
+        <v>55990014</v>
       </c>
       <c r="B164" s="98" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C164" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D164" s="25"/>
       <c r="E164" s="25"/>
@@ -13953,7 +13981,7 @@
       <c r="H164" s="97"/>
       <c r="I164" s="29"/>
       <c r="J164" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K164" s="27"/>
       <c r="L164" s="30" t="s">
@@ -13970,7 +13998,7 @@
         <v>239</v>
       </c>
       <c r="S164" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25"/>
@@ -13980,30 +14008,30 @@
         <v>15</v>
       </c>
       <c r="Y164" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Z164" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="165" spans="1:26" ht="36">
       <c r="A165" s="98">
-        <v>55990016</v>
+        <v>55990015</v>
       </c>
       <c r="B165" s="98" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C165" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D165" s="25"/>
       <c r="E165" s="25"/>
       <c r="F165" s="25"/>
       <c r="G165" s="60"/>
-      <c r="H165" s="84"/>
-      <c r="I165" s="47"/>
+      <c r="H165" s="97"/>
+      <c r="I165" s="29"/>
       <c r="J165" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K165" s="27"/>
       <c r="L165" s="30" t="s">
@@ -14020,7 +14048,7 @@
         <v>239</v>
       </c>
       <c r="S165" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T165" s="25"/>
       <c r="U165" s="25"/>
@@ -14030,33 +14058,35 @@
         <v>15</v>
       </c>
       <c r="Y165" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z165" s="48" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="166" spans="1:26" ht="24">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="166" spans="1:26" ht="36">
       <c r="A166" s="98">
-        <v>55990101</v>
+        <v>55990016</v>
       </c>
       <c r="B166" s="98" t="s">
-        <v>831</v>
+        <v>65</v>
       </c>
       <c r="C166" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D166" s="25"/>
       <c r="E166" s="25"/>
-      <c r="F166" s="44"/>
+      <c r="F166" s="25"/>
       <c r="G166" s="60"/>
-      <c r="H166" s="84" t="s">
-        <v>832</v>
-      </c>
+      <c r="H166" s="84"/>
       <c r="I166" s="47"/>
-      <c r="J166" s="26"/>
+      <c r="J166" s="26" t="s">
+        <v>297</v>
+      </c>
       <c r="K166" s="27"/>
-      <c r="L166" s="30"/>
+      <c r="L166" s="30" t="s">
+        <v>285</v>
+      </c>
       <c r="M166" s="17"/>
       <c r="N166" s="17"/>
       <c r="O166" s="20"/>
@@ -14067,103 +14097,95 @@
       <c r="R166" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="S166" s="49" t="s">
-        <v>833</v>
+      <c r="S166" s="16" t="s">
+        <v>291</v>
       </c>
       <c r="T166" s="25"/>
       <c r="U166" s="25"/>
       <c r="V166" s="25"/>
       <c r="W166" s="25"/>
       <c r="X166" s="25">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Y166" s="25" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="Z166" s="48" t="s">
-        <v>834</v>
+        <v>827</v>
       </c>
     </row>
     <row r="167" spans="1:26" ht="24">
       <c r="A167" s="98">
-        <v>55990102</v>
+        <v>55990101</v>
       </c>
       <c r="B167" s="98" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="C167" s="25" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D167" s="25"/>
       <c r="E167" s="25"/>
-      <c r="F167" s="25"/>
+      <c r="F167" s="44"/>
       <c r="G167" s="60"/>
-      <c r="H167" s="84"/>
+      <c r="H167" s="84" t="s">
+        <v>831</v>
+      </c>
       <c r="I167" s="47"/>
-      <c r="J167" s="26" t="s">
-        <v>835</v>
-      </c>
+      <c r="J167" s="26"/>
       <c r="K167" s="27"/>
-      <c r="L167" s="30" t="s">
-        <v>838</v>
-      </c>
+      <c r="L167" s="30"/>
       <c r="M167" s="17"/>
       <c r="N167" s="17"/>
       <c r="O167" s="20"/>
       <c r="P167" s="41"/>
       <c r="Q167" s="46" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="R167" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="S167" s="16" t="s">
-        <v>837</v>
+      <c r="S167" s="49" t="s">
+        <v>832</v>
       </c>
       <c r="T167" s="25"/>
       <c r="U167" s="25"/>
       <c r="V167" s="25"/>
       <c r="W167" s="25"/>
       <c r="X167" s="25">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Y167" s="25" t="s">
-        <v>841</v>
+        <v>109</v>
       </c>
       <c r="Z167" s="48" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="168" spans="1:26" ht="60">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="168" spans="1:26" ht="24">
       <c r="A168" s="98">
-        <v>55990103</v>
+        <v>55990102</v>
       </c>
       <c r="B168" s="98" t="s">
-        <v>847</v>
+        <v>835</v>
       </c>
       <c r="C168" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D168" s="25" t="s">
-        <v>461</v>
-      </c>
-      <c r="E168" s="25">
-        <v>10</v>
-      </c>
-      <c r="F168" s="44" t="s">
-        <v>471</v>
-      </c>
+        <v>829</v>
+      </c>
+      <c r="D168" s="25"/>
+      <c r="E168" s="25"/>
+      <c r="F168" s="25"/>
       <c r="G168" s="60"/>
       <c r="H168" s="84"/>
       <c r="I168" s="47"/>
       <c r="J168" s="26" t="s">
-        <v>682</v>
+        <v>834</v>
       </c>
       <c r="K168" s="27"/>
-      <c r="L168" s="30"/>
-      <c r="M168" s="17" t="s">
-        <v>593</v>
-      </c>
+      <c r="L168" s="30" t="s">
+        <v>837</v>
+      </c>
+      <c r="M168" s="17"/>
       <c r="N168" s="17"/>
       <c r="O168" s="20"/>
       <c r="P168" s="41"/>
@@ -14174,32 +14196,28 @@
         <v>239</v>
       </c>
       <c r="S168" s="16" t="s">
-        <v>850</v>
+        <v>836</v>
       </c>
       <c r="T168" s="25"/>
-      <c r="U168" s="25" t="s">
-        <v>857</v>
-      </c>
-      <c r="V168" s="25" t="s">
-        <v>857</v>
-      </c>
+      <c r="U168" s="25"/>
+      <c r="V168" s="25"/>
       <c r="W168" s="25"/>
       <c r="X168" s="25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Y168" s="25" t="s">
-        <v>849</v>
+        <v>840</v>
       </c>
       <c r="Z168" s="48" t="s">
-        <v>848</v>
+        <v>827</v>
       </c>
     </row>
     <row r="169" spans="1:26" ht="60">
       <c r="A169" s="98">
-        <v>55990104</v>
+        <v>55990103</v>
       </c>
       <c r="B169" s="98" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="C169" s="25" t="s">
         <v>99</v>
@@ -14208,7 +14226,7 @@
         <v>461</v>
       </c>
       <c r="E169" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F169" s="44" t="s">
         <v>471</v>
@@ -14217,7 +14235,7 @@
       <c r="H169" s="84"/>
       <c r="I169" s="47"/>
       <c r="J169" s="26" t="s">
-        <v>853</v>
+        <v>681</v>
       </c>
       <c r="K169" s="27"/>
       <c r="L169" s="30"/>
@@ -14234,24 +14252,84 @@
         <v>239</v>
       </c>
       <c r="S169" s="16" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="T169" s="25"/>
       <c r="U169" s="25" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="V169" s="25" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="W169" s="25"/>
       <c r="X169" s="25">
+        <v>35</v>
+      </c>
+      <c r="Y169" s="25" t="s">
+        <v>848</v>
+      </c>
+      <c r="Z169" s="48" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="170" spans="1:26" ht="60">
+      <c r="A170" s="98">
+        <v>55990104</v>
+      </c>
+      <c r="B170" s="98" t="s">
+        <v>853</v>
+      </c>
+      <c r="C170" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D170" s="25" t="s">
+        <v>461</v>
+      </c>
+      <c r="E170" s="25">
+        <v>20</v>
+      </c>
+      <c r="F170" s="44" t="s">
+        <v>471</v>
+      </c>
+      <c r="G170" s="60"/>
+      <c r="H170" s="84"/>
+      <c r="I170" s="47"/>
+      <c r="J170" s="26" t="s">
+        <v>852</v>
+      </c>
+      <c r="K170" s="27"/>
+      <c r="L170" s="30"/>
+      <c r="M170" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="N170" s="17"/>
+      <c r="O170" s="20"/>
+      <c r="P170" s="41"/>
+      <c r="Q170" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="R170" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="S170" s="16" t="s">
+        <v>851</v>
+      </c>
+      <c r="T170" s="25"/>
+      <c r="U170" s="25" t="s">
+        <v>856</v>
+      </c>
+      <c r="V170" s="25" t="s">
+        <v>856</v>
+      </c>
+      <c r="W170" s="25"/>
+      <c r="X170" s="25">
         <v>50</v>
       </c>
-      <c r="Y169" s="25" t="s">
-        <v>851</v>
-      </c>
-      <c r="Z169" s="48" t="s">
-        <v>848</v>
+      <c r="Y170" s="25" t="s">
+        <v>850</v>
+      </c>
+      <c r="Z170" s="48" t="s">
+        <v>847</v>
       </c>
     </row>
   </sheetData>
@@ -14844,7 +14922,7 @@
         <v>376</v>
       </c>
       <c r="B32" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -14852,7 +14930,7 @@
         <v>393</v>
       </c>
       <c r="B33" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finsh a card cathith
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="912">
   <si>
     <t>特殊</t>
   </si>
@@ -3432,6 +3432,22 @@
   </si>
   <si>
     <t>d.Summon(2,51000010);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>包裹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>baoguo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时获得一张随机武器卡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Owner.AddRandomCard(2,d.Level);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5599,8 +5615,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z174" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:Z174"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z175" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:Z175"/>
   <sortState ref="A4:Z118">
     <sortCondition ref="A3:A118"/>
   </sortState>
@@ -5923,14 +5939,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z174"/>
+  <dimension ref="A1:Z175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C156" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="N66" sqref="N66"/>
+      <selection pane="bottomRight" activeCell="H158" sqref="H158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13775,62 +13791,58 @@
       </c>
       <c r="Z158" s="48"/>
     </row>
-    <row r="159" spans="1:26" ht="36">
-      <c r="A159" s="98">
-        <v>55990001</v>
-      </c>
-      <c r="B159" s="98" t="s">
-        <v>23</v>
+    <row r="159" spans="1:26" ht="28.8">
+      <c r="A159" s="55">
+        <v>55900034</v>
+      </c>
+      <c r="B159" s="55" t="s">
+        <v>908</v>
       </c>
       <c r="C159" s="25" t="s">
-        <v>823</v>
+        <v>0</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25"/>
       <c r="F159" s="25"/>
       <c r="G159" s="60"/>
-      <c r="H159" s="97"/>
-      <c r="I159" s="29"/>
-      <c r="J159" s="26" t="s">
-        <v>409</v>
-      </c>
+      <c r="H159" s="84"/>
+      <c r="I159" s="47"/>
+      <c r="J159" s="26"/>
       <c r="K159" s="27"/>
-      <c r="L159" s="30" t="s">
-        <v>281</v>
-      </c>
+      <c r="L159" s="30"/>
       <c r="M159" s="17"/>
-      <c r="N159" s="17"/>
+      <c r="N159" s="17" t="s">
+        <v>911</v>
+      </c>
       <c r="O159" s="20"/>
       <c r="P159" s="41"/>
-      <c r="Q159" s="46" t="s">
-        <v>243</v>
+      <c r="Q159" s="10" t="s">
+        <v>317</v>
       </c>
       <c r="R159" s="44" t="s">
-        <v>238</v>
+        <v>405</v>
       </c>
       <c r="S159" s="16" t="s">
-        <v>398</v>
+        <v>910</v>
       </c>
       <c r="T159" s="25"/>
       <c r="U159" s="25"/>
       <c r="V159" s="25"/>
       <c r="W159" s="25"/>
       <c r="X159" s="25">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y159" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z159" s="48" t="s">
-        <v>821</v>
-      </c>
+        <v>909</v>
+      </c>
+      <c r="Z159" s="48"/>
     </row>
     <row r="160" spans="1:26" ht="36">
       <c r="A160" s="98">
-        <v>55990002</v>
+        <v>55990001</v>
       </c>
       <c r="B160" s="98" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C160" s="25" t="s">
         <v>823</v>
@@ -13842,7 +13854,7 @@
       <c r="H160" s="97"/>
       <c r="I160" s="29"/>
       <c r="J160" s="26" t="s">
-        <v>269</v>
+        <v>409</v>
       </c>
       <c r="K160" s="27"/>
       <c r="L160" s="30" t="s">
@@ -13858,8 +13870,8 @@
       <c r="R160" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="S160" s="49" t="s">
-        <v>399</v>
+      <c r="S160" s="16" t="s">
+        <v>398</v>
       </c>
       <c r="T160" s="25"/>
       <c r="U160" s="25"/>
@@ -13869,7 +13881,7 @@
         <v>15</v>
       </c>
       <c r="Y160" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Z160" s="48" t="s">
         <v>821</v>
@@ -13877,10 +13889,10 @@
     </row>
     <row r="161" spans="1:26" ht="36">
       <c r="A161" s="98">
-        <v>55990003</v>
+        <v>55990002</v>
       </c>
       <c r="B161" s="98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C161" s="25" t="s">
         <v>823</v>
@@ -13892,7 +13904,7 @@
       <c r="H161" s="97"/>
       <c r="I161" s="29"/>
       <c r="J161" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K161" s="27"/>
       <c r="L161" s="30" t="s">
@@ -13909,7 +13921,7 @@
         <v>238</v>
       </c>
       <c r="S161" s="49" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="T161" s="25"/>
       <c r="U161" s="25"/>
@@ -13919,7 +13931,7 @@
         <v>15</v>
       </c>
       <c r="Y161" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Z161" s="48" t="s">
         <v>821</v>
@@ -13927,10 +13939,10 @@
     </row>
     <row r="162" spans="1:26" ht="36">
       <c r="A162" s="98">
-        <v>55990004</v>
+        <v>55990003</v>
       </c>
       <c r="B162" s="98" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C162" s="25" t="s">
         <v>823</v>
@@ -13942,7 +13954,7 @@
       <c r="H162" s="97"/>
       <c r="I162" s="29"/>
       <c r="J162" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K162" s="27"/>
       <c r="L162" s="30" t="s">
@@ -13959,7 +13971,7 @@
         <v>238</v>
       </c>
       <c r="S162" s="49" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T162" s="25"/>
       <c r="U162" s="25"/>
@@ -13969,7 +13981,7 @@
         <v>15</v>
       </c>
       <c r="Y162" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z162" s="48" t="s">
         <v>821</v>
@@ -13977,10 +13989,10 @@
     </row>
     <row r="163" spans="1:26" ht="36">
       <c r="A163" s="98">
-        <v>55990005</v>
+        <v>55990004</v>
       </c>
       <c r="B163" s="98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C163" s="25" t="s">
         <v>823</v>
@@ -13992,7 +14004,7 @@
       <c r="H163" s="97"/>
       <c r="I163" s="29"/>
       <c r="J163" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K163" s="27"/>
       <c r="L163" s="30" t="s">
@@ -14009,7 +14021,7 @@
         <v>238</v>
       </c>
       <c r="S163" s="49" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="T163" s="25"/>
       <c r="U163" s="25"/>
@@ -14019,7 +14031,7 @@
         <v>15</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Z163" s="48" t="s">
         <v>821</v>
@@ -14027,10 +14039,10 @@
     </row>
     <row r="164" spans="1:26" ht="36">
       <c r="A164" s="98">
-        <v>55990006</v>
+        <v>55990005</v>
       </c>
       <c r="B164" s="98" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C164" s="25" t="s">
         <v>823</v>
@@ -14042,7 +14054,7 @@
       <c r="H164" s="97"/>
       <c r="I164" s="29"/>
       <c r="J164" s="26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K164" s="27"/>
       <c r="L164" s="30" t="s">
@@ -14059,7 +14071,7 @@
         <v>238</v>
       </c>
       <c r="S164" s="49" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25"/>
@@ -14069,7 +14081,7 @@
         <v>15</v>
       </c>
       <c r="Y164" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Z164" s="48" t="s">
         <v>821</v>
@@ -14077,10 +14089,10 @@
     </row>
     <row r="165" spans="1:26" ht="36">
       <c r="A165" s="98">
-        <v>55990011</v>
+        <v>55990006</v>
       </c>
       <c r="B165" s="98" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C165" s="25" t="s">
         <v>823</v>
@@ -14092,24 +14104,24 @@
       <c r="H165" s="97"/>
       <c r="I165" s="29"/>
       <c r="J165" s="26" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="K165" s="27"/>
       <c r="L165" s="30" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="M165" s="17"/>
       <c r="N165" s="17"/>
       <c r="O165" s="20"/>
       <c r="P165" s="41"/>
       <c r="Q165" s="46" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="R165" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="S165" s="16" t="s">
-        <v>285</v>
+      <c r="S165" s="49" t="s">
+        <v>413</v>
       </c>
       <c r="T165" s="25"/>
       <c r="U165" s="25"/>
@@ -14119,7 +14131,7 @@
         <v>15</v>
       </c>
       <c r="Y165" s="25" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="Z165" s="48" t="s">
         <v>821</v>
@@ -14127,10 +14139,10 @@
     </row>
     <row r="166" spans="1:26" ht="36">
       <c r="A166" s="98">
-        <v>55990012</v>
+        <v>55990011</v>
       </c>
       <c r="B166" s="98" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C166" s="25" t="s">
         <v>823</v>
@@ -14142,7 +14154,7 @@
       <c r="H166" s="97"/>
       <c r="I166" s="29"/>
       <c r="J166" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K166" s="27"/>
       <c r="L166" s="30" t="s">
@@ -14159,7 +14171,7 @@
         <v>238</v>
       </c>
       <c r="S166" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T166" s="25"/>
       <c r="U166" s="25"/>
@@ -14169,7 +14181,7 @@
         <v>15</v>
       </c>
       <c r="Y166" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Z166" s="48" t="s">
         <v>821</v>
@@ -14177,10 +14189,10 @@
     </row>
     <row r="167" spans="1:26" ht="36">
       <c r="A167" s="98">
-        <v>55990013</v>
+        <v>55990012</v>
       </c>
       <c r="B167" s="98" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>823</v>
@@ -14192,7 +14204,7 @@
       <c r="H167" s="97"/>
       <c r="I167" s="29"/>
       <c r="J167" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K167" s="27"/>
       <c r="L167" s="30" t="s">
@@ -14209,7 +14221,7 @@
         <v>238</v>
       </c>
       <c r="S167" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T167" s="25"/>
       <c r="U167" s="25"/>
@@ -14219,7 +14231,7 @@
         <v>15</v>
       </c>
       <c r="Y167" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z167" s="48" t="s">
         <v>821</v>
@@ -14227,10 +14239,10 @@
     </row>
     <row r="168" spans="1:26" ht="36">
       <c r="A168" s="98">
-        <v>55990014</v>
+        <v>55990013</v>
       </c>
       <c r="B168" s="98" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C168" s="25" t="s">
         <v>823</v>
@@ -14242,7 +14254,7 @@
       <c r="H168" s="97"/>
       <c r="I168" s="29"/>
       <c r="J168" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K168" s="27"/>
       <c r="L168" s="30" t="s">
@@ -14259,7 +14271,7 @@
         <v>238</v>
       </c>
       <c r="S168" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T168" s="25"/>
       <c r="U168" s="25"/>
@@ -14269,7 +14281,7 @@
         <v>15</v>
       </c>
       <c r="Y168" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z168" s="48" t="s">
         <v>821</v>
@@ -14277,10 +14289,10 @@
     </row>
     <row r="169" spans="1:26" ht="36">
       <c r="A169" s="98">
-        <v>55990015</v>
+        <v>55990014</v>
       </c>
       <c r="B169" s="98" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C169" s="25" t="s">
         <v>823</v>
@@ -14292,7 +14304,7 @@
       <c r="H169" s="97"/>
       <c r="I169" s="29"/>
       <c r="J169" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K169" s="27"/>
       <c r="L169" s="30" t="s">
@@ -14309,7 +14321,7 @@
         <v>238</v>
       </c>
       <c r="S169" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T169" s="25"/>
       <c r="U169" s="25"/>
@@ -14319,7 +14331,7 @@
         <v>15</v>
       </c>
       <c r="Y169" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Z169" s="48" t="s">
         <v>821</v>
@@ -14327,10 +14339,10 @@
     </row>
     <row r="170" spans="1:26" ht="36">
       <c r="A170" s="98">
-        <v>55990016</v>
+        <v>55990015</v>
       </c>
       <c r="B170" s="98" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C170" s="25" t="s">
         <v>823</v>
@@ -14339,10 +14351,10 @@
       <c r="E170" s="25"/>
       <c r="F170" s="25"/>
       <c r="G170" s="60"/>
-      <c r="H170" s="84"/>
-      <c r="I170" s="47"/>
+      <c r="H170" s="97"/>
+      <c r="I170" s="29"/>
       <c r="J170" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K170" s="27"/>
       <c r="L170" s="30" t="s">
@@ -14359,7 +14371,7 @@
         <v>238</v>
       </c>
       <c r="S170" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T170" s="25"/>
       <c r="U170" s="25"/>
@@ -14369,33 +14381,35 @@
         <v>15</v>
       </c>
       <c r="Y170" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Z170" s="48" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="171" spans="1:26" ht="24">
+    <row r="171" spans="1:26" ht="36">
       <c r="A171" s="98">
-        <v>55990101</v>
+        <v>55990016</v>
       </c>
       <c r="B171" s="98" t="s">
-        <v>824</v>
+        <v>64</v>
       </c>
       <c r="C171" s="25" t="s">
         <v>823</v>
       </c>
       <c r="D171" s="25"/>
       <c r="E171" s="25"/>
-      <c r="F171" s="44"/>
+      <c r="F171" s="25"/>
       <c r="G171" s="60"/>
-      <c r="H171" s="84" t="s">
-        <v>825</v>
-      </c>
+      <c r="H171" s="84"/>
       <c r="I171" s="47"/>
-      <c r="J171" s="26"/>
+      <c r="J171" s="26" t="s">
+        <v>296</v>
+      </c>
       <c r="K171" s="27"/>
-      <c r="L171" s="30"/>
+      <c r="L171" s="30" t="s">
+        <v>284</v>
+      </c>
       <c r="M171" s="17"/>
       <c r="N171" s="17"/>
       <c r="O171" s="20"/>
@@ -14406,103 +14420,95 @@
       <c r="R171" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="S171" s="49" t="s">
-        <v>826</v>
+      <c r="S171" s="16" t="s">
+        <v>290</v>
       </c>
       <c r="T171" s="25"/>
       <c r="U171" s="25"/>
       <c r="V171" s="25"/>
       <c r="W171" s="25"/>
       <c r="X171" s="25">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Y171" s="25" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="Z171" s="48" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="172" spans="1:26" ht="28.8">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="172" spans="1:26" ht="24">
       <c r="A172" s="98">
-        <v>55990102</v>
+        <v>55990101</v>
       </c>
       <c r="B172" s="98" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="C172" s="25" t="s">
         <v>823</v>
       </c>
       <c r="D172" s="25"/>
       <c r="E172" s="25"/>
-      <c r="F172" s="25"/>
+      <c r="F172" s="44"/>
       <c r="G172" s="60"/>
-      <c r="H172" s="84"/>
+      <c r="H172" s="84" t="s">
+        <v>825</v>
+      </c>
       <c r="I172" s="47"/>
-      <c r="J172" s="26" t="s">
-        <v>828</v>
-      </c>
+      <c r="J172" s="26"/>
       <c r="K172" s="27"/>
-      <c r="L172" s="30" t="s">
-        <v>831</v>
-      </c>
+      <c r="L172" s="30"/>
       <c r="M172" s="17"/>
       <c r="N172" s="17"/>
       <c r="O172" s="20"/>
       <c r="P172" s="41"/>
       <c r="Q172" s="46" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="R172" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="S172" s="16" t="s">
-        <v>830</v>
+      <c r="S172" s="49" t="s">
+        <v>826</v>
       </c>
       <c r="T172" s="25"/>
       <c r="U172" s="25"/>
       <c r="V172" s="25"/>
       <c r="W172" s="25"/>
       <c r="X172" s="25">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Y172" s="25" t="s">
-        <v>834</v>
+        <v>108</v>
       </c>
       <c r="Z172" s="48" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="173" spans="1:26" ht="72">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="173" spans="1:26" ht="28.8">
       <c r="A173" s="98">
-        <v>55990103</v>
+        <v>55990102</v>
       </c>
       <c r="B173" s="98" t="s">
-        <v>840</v>
+        <v>829</v>
       </c>
       <c r="C173" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="D173" s="25" t="s">
-        <v>459</v>
-      </c>
-      <c r="E173" s="25">
-        <v>10</v>
-      </c>
-      <c r="F173" s="44" t="s">
-        <v>469</v>
-      </c>
+        <v>823</v>
+      </c>
+      <c r="D173" s="25"/>
+      <c r="E173" s="25"/>
+      <c r="F173" s="25"/>
       <c r="G173" s="60"/>
       <c r="H173" s="84"/>
       <c r="I173" s="47"/>
       <c r="J173" s="26" t="s">
-        <v>677</v>
+        <v>828</v>
       </c>
       <c r="K173" s="27"/>
-      <c r="L173" s="30"/>
-      <c r="M173" s="17" t="s">
-        <v>589</v>
-      </c>
+      <c r="L173" s="30" t="s">
+        <v>831</v>
+      </c>
+      <c r="M173" s="17"/>
       <c r="N173" s="17"/>
       <c r="O173" s="20"/>
       <c r="P173" s="41"/>
@@ -14513,32 +14519,28 @@
         <v>238</v>
       </c>
       <c r="S173" s="16" t="s">
-        <v>843</v>
+        <v>830</v>
       </c>
       <c r="T173" s="25"/>
-      <c r="U173" s="25" t="s">
-        <v>850</v>
-      </c>
-      <c r="V173" s="25" t="s">
-        <v>850</v>
-      </c>
+      <c r="U173" s="25"/>
+      <c r="V173" s="25"/>
       <c r="W173" s="25"/>
       <c r="X173" s="25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Y173" s="25" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="Z173" s="48" t="s">
-        <v>841</v>
+        <v>821</v>
       </c>
     </row>
     <row r="174" spans="1:26" ht="72">
       <c r="A174" s="98">
-        <v>55990104</v>
+        <v>55990103</v>
       </c>
       <c r="B174" s="98" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="C174" s="25" t="s">
         <v>98</v>
@@ -14547,7 +14549,7 @@
         <v>459</v>
       </c>
       <c r="E174" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F174" s="44" t="s">
         <v>469</v>
@@ -14556,7 +14558,7 @@
       <c r="H174" s="84"/>
       <c r="I174" s="47"/>
       <c r="J174" s="26" t="s">
-        <v>846</v>
+        <v>677</v>
       </c>
       <c r="K174" s="27"/>
       <c r="L174" s="30"/>
@@ -14573,7 +14575,7 @@
         <v>238</v>
       </c>
       <c r="S174" s="16" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="T174" s="25"/>
       <c r="U174" s="25" t="s">
@@ -14584,12 +14586,72 @@
       </c>
       <c r="W174" s="25"/>
       <c r="X174" s="25">
+        <v>35</v>
+      </c>
+      <c r="Y174" s="25" t="s">
+        <v>842</v>
+      </c>
+      <c r="Z174" s="48" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="175" spans="1:26" ht="72">
+      <c r="A175" s="98">
+        <v>55990104</v>
+      </c>
+      <c r="B175" s="98" t="s">
+        <v>847</v>
+      </c>
+      <c r="C175" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D175" s="25" t="s">
+        <v>459</v>
+      </c>
+      <c r="E175" s="25">
+        <v>20</v>
+      </c>
+      <c r="F175" s="44" t="s">
+        <v>469</v>
+      </c>
+      <c r="G175" s="60"/>
+      <c r="H175" s="84"/>
+      <c r="I175" s="47"/>
+      <c r="J175" s="26" t="s">
+        <v>846</v>
+      </c>
+      <c r="K175" s="27"/>
+      <c r="L175" s="30"/>
+      <c r="M175" s="17" t="s">
+        <v>589</v>
+      </c>
+      <c r="N175" s="17"/>
+      <c r="O175" s="20"/>
+      <c r="P175" s="41"/>
+      <c r="Q175" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="R175" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="S175" s="16" t="s">
+        <v>845</v>
+      </c>
+      <c r="T175" s="25"/>
+      <c r="U175" s="25" t="s">
+        <v>850</v>
+      </c>
+      <c r="V175" s="25" t="s">
+        <v>850</v>
+      </c>
+      <c r="W175" s="25"/>
+      <c r="X175" s="25">
         <v>50</v>
       </c>
-      <c r="Y174" s="25" t="s">
+      <c r="Y175" s="25" t="s">
         <v>844</v>
       </c>
-      <c r="Z174" s="48" t="s">
+      <c r="Z175" s="48" t="s">
         <v>841</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish the card thief
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1553" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="927">
   <si>
     <t>特殊</t>
   </si>
@@ -3493,6 +3493,22 @@
   </si>
   <si>
     <t>jinji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时获得一张随机对方职业卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.AddRandomCardJob(s.Rival.Job,s.Level);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>piaoqie</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>剽窃</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5660,8 +5676,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z177" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:Z177"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z178" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:Z178"/>
   <sortState ref="A4:Z118">
     <sortCondition ref="A3:A118"/>
   </sortState>
@@ -5984,14 +6000,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z177"/>
+  <dimension ref="A1:Z178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C156" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="G57" sqref="G57"/>
+      <selection pane="bottomRight" activeCell="F161" sqref="F161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13987,28 +14003,26 @@
       <c r="Z161" s="48"/>
     </row>
     <row r="162" spans="1:26" ht="36">
-      <c r="A162" s="98">
-        <v>55990001</v>
-      </c>
-      <c r="B162" s="98" t="s">
-        <v>23</v>
+      <c r="A162" s="55">
+        <v>55900035</v>
+      </c>
+      <c r="B162" s="55" t="s">
+        <v>926</v>
       </c>
       <c r="C162" s="25" t="s">
-        <v>819</v>
+        <v>0</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25"/>
       <c r="F162" s="25"/>
       <c r="G162" s="60"/>
-      <c r="H162" s="97"/>
-      <c r="I162" s="29"/>
-      <c r="J162" s="26" t="s">
-        <v>408</v>
-      </c>
+      <c r="H162" s="84" t="s">
+        <v>924</v>
+      </c>
+      <c r="I162" s="47"/>
+      <c r="J162" s="26"/>
       <c r="K162" s="27"/>
-      <c r="L162" s="30" t="s">
-        <v>280</v>
-      </c>
+      <c r="L162" s="30"/>
       <c r="M162" s="17"/>
       <c r="N162" s="17"/>
       <c r="O162" s="20"/>
@@ -14017,31 +14031,29 @@
         <v>242</v>
       </c>
       <c r="R162" s="44" t="s">
-        <v>237</v>
+        <v>404</v>
       </c>
       <c r="S162" s="16" t="s">
-        <v>397</v>
+        <v>923</v>
       </c>
       <c r="T162" s="25"/>
       <c r="U162" s="25"/>
       <c r="V162" s="25"/>
       <c r="W162" s="25"/>
       <c r="X162" s="25">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y162" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z162" s="48" t="s">
-        <v>817</v>
-      </c>
+        <v>925</v>
+      </c>
+      <c r="Z162" s="48"/>
     </row>
     <row r="163" spans="1:26" ht="36">
       <c r="A163" s="98">
-        <v>55990002</v>
+        <v>55990001</v>
       </c>
       <c r="B163" s="98" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C163" s="25" t="s">
         <v>819</v>
@@ -14053,7 +14065,7 @@
       <c r="H163" s="97"/>
       <c r="I163" s="29"/>
       <c r="J163" s="26" t="s">
-        <v>268</v>
+        <v>408</v>
       </c>
       <c r="K163" s="27"/>
       <c r="L163" s="30" t="s">
@@ -14069,8 +14081,8 @@
       <c r="R163" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S163" s="49" t="s">
-        <v>398</v>
+      <c r="S163" s="16" t="s">
+        <v>397</v>
       </c>
       <c r="T163" s="25"/>
       <c r="U163" s="25"/>
@@ -14080,7 +14092,7 @@
         <v>15</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Z163" s="48" t="s">
         <v>817</v>
@@ -14088,10 +14100,10 @@
     </row>
     <row r="164" spans="1:26" ht="36">
       <c r="A164" s="98">
-        <v>55990003</v>
+        <v>55990002</v>
       </c>
       <c r="B164" s="98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C164" s="25" t="s">
         <v>819</v>
@@ -14103,7 +14115,7 @@
       <c r="H164" s="97"/>
       <c r="I164" s="29"/>
       <c r="J164" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K164" s="27"/>
       <c r="L164" s="30" t="s">
@@ -14120,7 +14132,7 @@
         <v>237</v>
       </c>
       <c r="S164" s="49" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25"/>
@@ -14130,7 +14142,7 @@
         <v>15</v>
       </c>
       <c r="Y164" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Z164" s="48" t="s">
         <v>817</v>
@@ -14138,10 +14150,10 @@
     </row>
     <row r="165" spans="1:26" ht="36">
       <c r="A165" s="98">
-        <v>55990004</v>
+        <v>55990003</v>
       </c>
       <c r="B165" s="98" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C165" s="25" t="s">
         <v>819</v>
@@ -14153,7 +14165,7 @@
       <c r="H165" s="97"/>
       <c r="I165" s="29"/>
       <c r="J165" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K165" s="27"/>
       <c r="L165" s="30" t="s">
@@ -14170,7 +14182,7 @@
         <v>237</v>
       </c>
       <c r="S165" s="49" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="T165" s="25"/>
       <c r="U165" s="25"/>
@@ -14180,7 +14192,7 @@
         <v>15</v>
       </c>
       <c r="Y165" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z165" s="48" t="s">
         <v>817</v>
@@ -14188,10 +14200,10 @@
     </row>
     <row r="166" spans="1:26" ht="36">
       <c r="A166" s="98">
-        <v>55990005</v>
+        <v>55990004</v>
       </c>
       <c r="B166" s="98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C166" s="25" t="s">
         <v>819</v>
@@ -14203,7 +14215,7 @@
       <c r="H166" s="97"/>
       <c r="I166" s="29"/>
       <c r="J166" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K166" s="27"/>
       <c r="L166" s="30" t="s">
@@ -14220,7 +14232,7 @@
         <v>237</v>
       </c>
       <c r="S166" s="49" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T166" s="25"/>
       <c r="U166" s="25"/>
@@ -14230,7 +14242,7 @@
         <v>15</v>
       </c>
       <c r="Y166" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Z166" s="48" t="s">
         <v>817</v>
@@ -14238,10 +14250,10 @@
     </row>
     <row r="167" spans="1:26" ht="36">
       <c r="A167" s="98">
-        <v>55990006</v>
+        <v>55990005</v>
       </c>
       <c r="B167" s="98" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>819</v>
@@ -14253,7 +14265,7 @@
       <c r="H167" s="97"/>
       <c r="I167" s="29"/>
       <c r="J167" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K167" s="27"/>
       <c r="L167" s="30" t="s">
@@ -14270,7 +14282,7 @@
         <v>237</v>
       </c>
       <c r="S167" s="49" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="T167" s="25"/>
       <c r="U167" s="25"/>
@@ -14280,7 +14292,7 @@
         <v>15</v>
       </c>
       <c r="Y167" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Z167" s="48" t="s">
         <v>817</v>
@@ -14288,10 +14300,10 @@
     </row>
     <row r="168" spans="1:26" ht="36">
       <c r="A168" s="98">
-        <v>55990011</v>
+        <v>55990006</v>
       </c>
       <c r="B168" s="98" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C168" s="25" t="s">
         <v>819</v>
@@ -14303,24 +14315,24 @@
       <c r="H168" s="97"/>
       <c r="I168" s="29"/>
       <c r="J168" s="26" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="K168" s="27"/>
       <c r="L168" s="30" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="M168" s="17"/>
       <c r="N168" s="17"/>
       <c r="O168" s="20"/>
       <c r="P168" s="41"/>
       <c r="Q168" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="R168" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S168" s="16" t="s">
-        <v>284</v>
+      <c r="S168" s="49" t="s">
+        <v>412</v>
       </c>
       <c r="T168" s="25"/>
       <c r="U168" s="25"/>
@@ -14330,7 +14342,7 @@
         <v>15</v>
       </c>
       <c r="Y168" s="25" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="Z168" s="48" t="s">
         <v>817</v>
@@ -14338,10 +14350,10 @@
     </row>
     <row r="169" spans="1:26" ht="36">
       <c r="A169" s="98">
-        <v>55990012</v>
+        <v>55990011</v>
       </c>
       <c r="B169" s="98" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C169" s="25" t="s">
         <v>819</v>
@@ -14353,7 +14365,7 @@
       <c r="H169" s="97"/>
       <c r="I169" s="29"/>
       <c r="J169" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K169" s="27"/>
       <c r="L169" s="30" t="s">
@@ -14370,7 +14382,7 @@
         <v>237</v>
       </c>
       <c r="S169" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T169" s="25"/>
       <c r="U169" s="25"/>
@@ -14380,7 +14392,7 @@
         <v>15</v>
       </c>
       <c r="Y169" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Z169" s="48" t="s">
         <v>817</v>
@@ -14388,10 +14400,10 @@
     </row>
     <row r="170" spans="1:26" ht="36">
       <c r="A170" s="98">
-        <v>55990013</v>
+        <v>55990012</v>
       </c>
       <c r="B170" s="98" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C170" s="25" t="s">
         <v>819</v>
@@ -14403,7 +14415,7 @@
       <c r="H170" s="97"/>
       <c r="I170" s="29"/>
       <c r="J170" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K170" s="27"/>
       <c r="L170" s="30" t="s">
@@ -14420,7 +14432,7 @@
         <v>237</v>
       </c>
       <c r="S170" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T170" s="25"/>
       <c r="U170" s="25"/>
@@ -14430,7 +14442,7 @@
         <v>15</v>
       </c>
       <c r="Y170" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z170" s="48" t="s">
         <v>817</v>
@@ -14438,10 +14450,10 @@
     </row>
     <row r="171" spans="1:26" ht="36">
       <c r="A171" s="98">
-        <v>55990014</v>
+        <v>55990013</v>
       </c>
       <c r="B171" s="98" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C171" s="25" t="s">
         <v>819</v>
@@ -14453,7 +14465,7 @@
       <c r="H171" s="97"/>
       <c r="I171" s="29"/>
       <c r="J171" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K171" s="27"/>
       <c r="L171" s="30" t="s">
@@ -14470,7 +14482,7 @@
         <v>237</v>
       </c>
       <c r="S171" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T171" s="25"/>
       <c r="U171" s="25"/>
@@ -14480,7 +14492,7 @@
         <v>15</v>
       </c>
       <c r="Y171" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z171" s="48" t="s">
         <v>817</v>
@@ -14488,10 +14500,10 @@
     </row>
     <row r="172" spans="1:26" ht="36">
       <c r="A172" s="98">
-        <v>55990015</v>
+        <v>55990014</v>
       </c>
       <c r="B172" s="98" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C172" s="25" t="s">
         <v>819</v>
@@ -14503,7 +14515,7 @@
       <c r="H172" s="97"/>
       <c r="I172" s="29"/>
       <c r="J172" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K172" s="27"/>
       <c r="L172" s="30" t="s">
@@ -14520,7 +14532,7 @@
         <v>237</v>
       </c>
       <c r="S172" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T172" s="25"/>
       <c r="U172" s="25"/>
@@ -14530,7 +14542,7 @@
         <v>15</v>
       </c>
       <c r="Y172" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Z172" s="48" t="s">
         <v>817</v>
@@ -14538,10 +14550,10 @@
     </row>
     <row r="173" spans="1:26" ht="36">
       <c r="A173" s="98">
-        <v>55990016</v>
+        <v>55990015</v>
       </c>
       <c r="B173" s="98" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C173" s="25" t="s">
         <v>819</v>
@@ -14550,10 +14562,10 @@
       <c r="E173" s="25"/>
       <c r="F173" s="25"/>
       <c r="G173" s="60"/>
-      <c r="H173" s="84"/>
-      <c r="I173" s="47"/>
+      <c r="H173" s="97"/>
+      <c r="I173" s="29"/>
       <c r="J173" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K173" s="27"/>
       <c r="L173" s="30" t="s">
@@ -14570,7 +14582,7 @@
         <v>237</v>
       </c>
       <c r="S173" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T173" s="25"/>
       <c r="U173" s="25"/>
@@ -14580,33 +14592,35 @@
         <v>15</v>
       </c>
       <c r="Y173" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Z173" s="48" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="174" spans="1:26" ht="24">
+    <row r="174" spans="1:26" ht="36">
       <c r="A174" s="98">
-        <v>55990101</v>
+        <v>55990016</v>
       </c>
       <c r="B174" s="98" t="s">
-        <v>820</v>
+        <v>64</v>
       </c>
       <c r="C174" s="25" t="s">
         <v>819</v>
       </c>
       <c r="D174" s="25"/>
       <c r="E174" s="25"/>
-      <c r="F174" s="44"/>
+      <c r="F174" s="25"/>
       <c r="G174" s="60"/>
-      <c r="H174" s="84" t="s">
-        <v>821</v>
-      </c>
+      <c r="H174" s="84"/>
       <c r="I174" s="47"/>
-      <c r="J174" s="26"/>
+      <c r="J174" s="26" t="s">
+        <v>295</v>
+      </c>
       <c r="K174" s="27"/>
-      <c r="L174" s="30"/>
+      <c r="L174" s="30" t="s">
+        <v>283</v>
+      </c>
       <c r="M174" s="17"/>
       <c r="N174" s="17"/>
       <c r="O174" s="20"/>
@@ -14617,103 +14631,95 @@
       <c r="R174" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S174" s="49" t="s">
-        <v>822</v>
+      <c r="S174" s="16" t="s">
+        <v>289</v>
       </c>
       <c r="T174" s="25"/>
       <c r="U174" s="25"/>
       <c r="V174" s="25"/>
       <c r="W174" s="25"/>
       <c r="X174" s="25">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Y174" s="25" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="Z174" s="48" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="175" spans="1:26" ht="28.8">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="175" spans="1:26" ht="24">
       <c r="A175" s="98">
-        <v>55990102</v>
+        <v>55990101</v>
       </c>
       <c r="B175" s="98" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="C175" s="25" t="s">
         <v>819</v>
       </c>
       <c r="D175" s="25"/>
       <c r="E175" s="25"/>
-      <c r="F175" s="25"/>
+      <c r="F175" s="44"/>
       <c r="G175" s="60"/>
-      <c r="H175" s="84"/>
+      <c r="H175" s="84" t="s">
+        <v>821</v>
+      </c>
       <c r="I175" s="47"/>
-      <c r="J175" s="26" t="s">
-        <v>824</v>
-      </c>
+      <c r="J175" s="26"/>
       <c r="K175" s="27"/>
-      <c r="L175" s="30" t="s">
-        <v>827</v>
-      </c>
+      <c r="L175" s="30"/>
       <c r="M175" s="17"/>
       <c r="N175" s="17"/>
       <c r="O175" s="20"/>
       <c r="P175" s="41"/>
       <c r="Q175" s="46" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="R175" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S175" s="16" t="s">
-        <v>826</v>
+      <c r="S175" s="49" t="s">
+        <v>822</v>
       </c>
       <c r="T175" s="25"/>
       <c r="U175" s="25"/>
       <c r="V175" s="25"/>
       <c r="W175" s="25"/>
       <c r="X175" s="25">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Y175" s="25" t="s">
-        <v>830</v>
+        <v>107</v>
       </c>
       <c r="Z175" s="48" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="176" spans="1:26" ht="72">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="176" spans="1:26" ht="28.8">
       <c r="A176" s="98">
-        <v>55990103</v>
+        <v>55990102</v>
       </c>
       <c r="B176" s="98" t="s">
-        <v>836</v>
+        <v>825</v>
       </c>
       <c r="C176" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D176" s="25" t="s">
-        <v>456</v>
-      </c>
-      <c r="E176" s="25">
-        <v>10</v>
-      </c>
-      <c r="F176" s="44" t="s">
-        <v>466</v>
-      </c>
+        <v>819</v>
+      </c>
+      <c r="D176" s="25"/>
+      <c r="E176" s="25"/>
+      <c r="F176" s="25"/>
       <c r="G176" s="60"/>
       <c r="H176" s="84"/>
       <c r="I176" s="47"/>
       <c r="J176" s="26" t="s">
-        <v>674</v>
+        <v>824</v>
       </c>
       <c r="K176" s="27"/>
-      <c r="L176" s="30"/>
-      <c r="M176" s="17" t="s">
-        <v>586</v>
-      </c>
+      <c r="L176" s="30" t="s">
+        <v>827</v>
+      </c>
+      <c r="M176" s="17"/>
       <c r="N176" s="17"/>
       <c r="O176" s="20"/>
       <c r="P176" s="41"/>
@@ -14724,32 +14730,28 @@
         <v>237</v>
       </c>
       <c r="S176" s="16" t="s">
-        <v>839</v>
+        <v>826</v>
       </c>
       <c r="T176" s="25"/>
-      <c r="U176" s="25" t="s">
-        <v>846</v>
-      </c>
-      <c r="V176" s="25" t="s">
-        <v>846</v>
-      </c>
+      <c r="U176" s="25"/>
+      <c r="V176" s="25"/>
       <c r="W176" s="25"/>
       <c r="X176" s="25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Y176" s="25" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="Z176" s="48" t="s">
-        <v>837</v>
+        <v>817</v>
       </c>
     </row>
     <row r="177" spans="1:26" ht="72">
       <c r="A177" s="98">
-        <v>55990104</v>
+        <v>55990103</v>
       </c>
       <c r="B177" s="98" t="s">
-        <v>843</v>
+        <v>836</v>
       </c>
       <c r="C177" s="25" t="s">
         <v>97</v>
@@ -14758,7 +14760,7 @@
         <v>456</v>
       </c>
       <c r="E177" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F177" s="44" t="s">
         <v>466</v>
@@ -14767,7 +14769,7 @@
       <c r="H177" s="84"/>
       <c r="I177" s="47"/>
       <c r="J177" s="26" t="s">
-        <v>842</v>
+        <v>674</v>
       </c>
       <c r="K177" s="27"/>
       <c r="L177" s="30"/>
@@ -14784,7 +14786,7 @@
         <v>237</v>
       </c>
       <c r="S177" s="16" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="T177" s="25"/>
       <c r="U177" s="25" t="s">
@@ -14795,12 +14797,72 @@
       </c>
       <c r="W177" s="25"/>
       <c r="X177" s="25">
+        <v>35</v>
+      </c>
+      <c r="Y177" s="25" t="s">
+        <v>838</v>
+      </c>
+      <c r="Z177" s="48" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="178" spans="1:26" ht="72">
+      <c r="A178" s="98">
+        <v>55990104</v>
+      </c>
+      <c r="B178" s="98" t="s">
+        <v>843</v>
+      </c>
+      <c r="C178" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D178" s="25" t="s">
+        <v>456</v>
+      </c>
+      <c r="E178" s="25">
+        <v>20</v>
+      </c>
+      <c r="F178" s="44" t="s">
+        <v>466</v>
+      </c>
+      <c r="G178" s="60"/>
+      <c r="H178" s="84"/>
+      <c r="I178" s="47"/>
+      <c r="J178" s="26" t="s">
+        <v>842</v>
+      </c>
+      <c r="K178" s="27"/>
+      <c r="L178" s="30"/>
+      <c r="M178" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="N178" s="17"/>
+      <c r="O178" s="20"/>
+      <c r="P178" s="41"/>
+      <c r="Q178" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="R178" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="S178" s="16" t="s">
+        <v>841</v>
+      </c>
+      <c r="T178" s="25"/>
+      <c r="U178" s="25" t="s">
+        <v>846</v>
+      </c>
+      <c r="V178" s="25" t="s">
+        <v>846</v>
+      </c>
+      <c r="W178" s="25"/>
+      <c r="X178" s="25">
         <v>50</v>
       </c>
-      <c r="Y177" s="25" t="s">
+      <c r="Y178" s="25" t="s">
         <v>840</v>
       </c>
-      <c r="Z177" s="48" t="s">
+      <c r="Z178" s="48" t="s">
         <v>837</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix the bug of row/column spell error
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -1673,10 +1673,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>NEO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>NER</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3626,6 +3622,10 @@
   </si>
   <si>
     <t>foreach(IMonster o in s.Map.GetRangeMonsterGhost(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)){s.Map.ReviveUnit(o,(int)(o.MaxHp.Source/2));}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEA</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6120,11 +6120,11 @@
   <dimension ref="A1:Z184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="H168" sqref="H168"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6158,16 +6158,16 @@
         <v>232</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E1" s="45" t="s">
         <v>448</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>247</v>
@@ -6188,7 +6188,7 @@
         <v>303</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>317</v>
@@ -6238,19 +6238,19 @@
         <v>224</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>352</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>338</v>
@@ -6265,10 +6265,10 @@
         <v>331</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>307</v>
@@ -6318,16 +6318,16 @@
         <v>227</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>399</v>
@@ -6348,10 +6348,10 @@
         <v>302</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>437</v>
@@ -6372,7 +6372,7 @@
         <v>318</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>344</v>
@@ -6395,7 +6395,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -6409,7 +6409,7 @@
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="P4" s="41">
         <v>1</v>
@@ -6421,7 +6421,7 @@
         <v>237</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
@@ -6443,7 +6443,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -6452,13 +6452,13 @@
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="28" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
@@ -6471,7 +6471,7 @@
         <v>237</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="T5" s="36"/>
       <c r="U5" s="1"/>
@@ -6493,7 +6493,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -6502,13 +6502,13 @@
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
       <c r="J6" s="28" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K6" s="18" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
@@ -6521,7 +6521,7 @@
         <v>237</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="1"/>
@@ -6540,17 +6540,17 @@
         <v>55100004</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="43"/>
       <c r="G7" s="59"/>
       <c r="H7" s="29" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="28"/>
@@ -6567,7 +6567,7 @@
         <v>237</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="T7" s="10">
         <v>56000202</v>
@@ -6579,7 +6579,7 @@
         <v>15</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="Z7" s="37"/>
     </row>
@@ -6588,16 +6588,16 @@
         <v>55100005</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="43"/>
       <c r="G8" s="59" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
@@ -6615,7 +6615,7 @@
         <v>237</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="T8" s="10"/>
       <c r="U8" s="1"/>
@@ -6625,7 +6625,7 @@
         <v>35</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="Z8" s="37"/>
     </row>
@@ -6634,17 +6634,17 @@
         <v>55100006</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D9" s="61"/>
       <c r="E9" s="61"/>
       <c r="F9" s="62"/>
       <c r="G9" s="59"/>
       <c r="H9" s="29" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I9" s="63"/>
       <c r="J9" s="64"/>
@@ -6661,7 +6661,7 @@
         <v>237</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="T9" s="10"/>
       <c r="U9" s="61"/>
@@ -6671,7 +6671,7 @@
         <v>45</v>
       </c>
       <c r="Y9" s="25" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Z9" s="70"/>
     </row>
@@ -6680,30 +6680,30 @@
         <v>55100007</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G10" s="59"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="28" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="17"/>
       <c r="M10" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="20"/>
@@ -6715,21 +6715,21 @@
         <v>237</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="25" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="61">
         <v>35</v>
       </c>
       <c r="Y10" s="25" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="Z10" s="48"/>
     </row>
@@ -6738,16 +6738,16 @@
         <v>55100008</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="44"/>
       <c r="G11" s="59" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
@@ -6765,7 +6765,7 @@
         <v>237</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="T11" s="10"/>
       <c r="U11" s="25"/>
@@ -6775,7 +6775,7 @@
         <v>15</v>
       </c>
       <c r="Y11" s="25" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="Z11" s="48"/>
     </row>
@@ -6784,16 +6784,16 @@
         <v>55100009</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
       <c r="F12" s="44"/>
       <c r="G12" s="59" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
@@ -6811,7 +6811,7 @@
         <v>237</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="T12" s="10"/>
       <c r="U12" s="25"/>
@@ -6821,7 +6821,7 @@
         <v>15</v>
       </c>
       <c r="Y12" s="25" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="Z12" s="48"/>
     </row>
@@ -6830,17 +6830,17 @@
         <v>55100010</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="43"/>
       <c r="G13" s="59"/>
       <c r="H13" s="29" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I13" s="29"/>
       <c r="J13" s="28"/>
@@ -6863,7 +6863,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="X13" s="1">
         <v>12</v>
@@ -6878,10 +6878,10 @@
         <v>55100011</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -6890,11 +6890,11 @@
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
       <c r="J14" s="28" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="17" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -6907,7 +6907,7 @@
         <v>237</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="T14" s="10"/>
       <c r="U14" s="1"/>
@@ -6926,10 +6926,10 @@
         <v>55100012</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -6961,7 +6961,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="X15" s="1">
         <v>15</v>
@@ -6976,16 +6976,16 @@
         <v>55100013</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="43"/>
       <c r="G16" s="59" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
@@ -7003,7 +7003,7 @@
         <v>237</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -7013,7 +7013,7 @@
         <v>10</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Z16" s="37"/>
     </row>
@@ -7022,10 +7022,10 @@
         <v>55100014</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -7070,10 +7070,10 @@
         <v>55100015</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -7086,7 +7086,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="O18" s="20"/>
       <c r="P18" s="41"/>
@@ -7097,7 +7097,7 @@
         <v>237</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="1" t="s">
@@ -7109,7 +7109,7 @@
         <v>16</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="Z18" s="37"/>
     </row>
@@ -7132,7 +7132,7 @@
       <c r="J19" s="28"/>
       <c r="K19" s="18"/>
       <c r="L19" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
@@ -7145,7 +7145,7 @@
         <v>237</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="T19" s="10"/>
       <c r="U19" s="1"/>
@@ -7180,7 +7180,7 @@
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
       <c r="N20" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="O20" s="20"/>
       <c r="P20" s="41"/>
@@ -7191,7 +7191,7 @@
         <v>237</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="T20" s="10"/>
       <c r="U20" s="1"/>
@@ -7256,7 +7256,7 @@
         <v>55110004</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>0</v>
@@ -7266,7 +7266,7 @@
       <c r="F22" s="43"/>
       <c r="G22" s="59"/>
       <c r="H22" s="29" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I22" s="29"/>
       <c r="J22" s="28"/>
@@ -7283,7 +7283,7 @@
         <v>237</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="T22" s="10"/>
       <c r="U22" s="1"/>
@@ -7302,7 +7302,7 @@
         <v>55110005</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>36</v>
@@ -7314,7 +7314,7 @@
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
       <c r="J23" s="28" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="17"/>
@@ -7331,7 +7331,7 @@
         <v>237</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="T23" s="14"/>
       <c r="U23" s="1"/>
@@ -7350,7 +7350,7 @@
         <v>55110006</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
@@ -7366,7 +7366,7 @@
       </c>
       <c r="K24" s="18"/>
       <c r="L24" s="17" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -7379,7 +7379,7 @@
         <v>237</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="T24" s="10"/>
       <c r="U24" s="1"/>
@@ -7398,7 +7398,7 @@
         <v>55110007</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>1</v>
@@ -7410,11 +7410,11 @@
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
       <c r="J25" s="28" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="K25" s="18"/>
       <c r="L25" s="17" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
@@ -7427,7 +7427,7 @@
         <v>237</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="T25" s="10"/>
       <c r="U25" s="1"/>
@@ -7446,7 +7446,7 @@
         <v>55110008</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -7492,7 +7492,7 @@
         <v>55110009</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
@@ -7506,7 +7506,7 @@
       <c r="J27" s="28"/>
       <c r="K27" s="18"/>
       <c r="L27" s="17" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
@@ -7519,7 +7519,7 @@
         <v>237</v>
       </c>
       <c r="S27" s="10" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="T27" s="10"/>
       <c r="U27" s="1"/>
@@ -7538,7 +7538,7 @@
         <v>55110010</v>
       </c>
       <c r="B28" s="75" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>36</v>
@@ -7550,7 +7550,7 @@
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
       <c r="J28" s="28" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K28" s="18"/>
       <c r="L28" s="17" t="s">
@@ -7586,7 +7586,7 @@
         <v>55110011</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>36</v>
@@ -7598,10 +7598,10 @@
       <c r="H29" s="29"/>
       <c r="I29" s="29"/>
       <c r="J29" s="28" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
@@ -7615,7 +7615,7 @@
         <v>237</v>
       </c>
       <c r="S29" s="10" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T29" s="10"/>
       <c r="U29" s="1"/>
@@ -7634,7 +7634,7 @@
         <v>55110012</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>1</v>
@@ -7649,7 +7649,7 @@
       <c r="K30" s="18"/>
       <c r="L30" s="17"/>
       <c r="M30" s="17" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="N30" s="17"/>
       <c r="O30" s="20"/>
@@ -7680,7 +7680,7 @@
         <v>55110013</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>36</v>
@@ -7692,14 +7692,14 @@
       <c r="H31" s="29"/>
       <c r="I31" s="29"/>
       <c r="J31" s="28" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K31" s="18"/>
       <c r="L31" s="17" t="s">
+        <v>736</v>
+      </c>
+      <c r="M31" s="17" t="s">
         <v>737</v>
-      </c>
-      <c r="M31" s="17" t="s">
-        <v>738</v>
       </c>
       <c r="N31" s="17"/>
       <c r="O31" s="20"/>
@@ -7711,7 +7711,7 @@
         <v>237</v>
       </c>
       <c r="S31" s="10" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="T31" s="10"/>
       <c r="U31" s="1"/>
@@ -7730,7 +7730,7 @@
         <v>55110014</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>36</v>
@@ -7776,7 +7776,7 @@
         <v>55110015</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>1</v>
@@ -7788,7 +7788,7 @@
       <c r="H33" s="29"/>
       <c r="I33" s="29"/>
       <c r="J33" s="28" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="K33" s="18"/>
       <c r="L33" s="17" t="s">
@@ -7805,7 +7805,7 @@
         <v>237</v>
       </c>
       <c r="S33" s="10" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="T33" s="10"/>
       <c r="U33" s="1"/>
@@ -7824,7 +7824,7 @@
         <v>55110016</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>36</v>
@@ -7839,7 +7839,7 @@
         <v>301</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="L34" s="17"/>
       <c r="M34" s="17"/>
@@ -7853,7 +7853,7 @@
         <v>237</v>
       </c>
       <c r="S34" s="10" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="T34" s="10"/>
       <c r="U34" s="1"/>
@@ -7872,7 +7872,7 @@
         <v>55110017</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>36</v>
@@ -7886,7 +7886,7 @@
       <c r="J35" s="28"/>
       <c r="K35" s="18"/>
       <c r="L35" s="17" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -7899,7 +7899,7 @@
         <v>237</v>
       </c>
       <c r="S35" s="10" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="T35" s="10"/>
       <c r="U35" s="1"/>
@@ -7918,7 +7918,7 @@
         <v>55110018</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>36</v>
@@ -7968,7 +7968,7 @@
         <v>55110019</v>
       </c>
       <c r="B37" s="75" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C37" s="25" t="s">
         <v>36</v>
@@ -7980,11 +7980,11 @@
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
       <c r="J37" s="26" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K37" s="27"/>
       <c r="L37" s="30" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
@@ -7997,7 +7997,7 @@
         <v>404</v>
       </c>
       <c r="S37" s="16" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="T37" s="25"/>
       <c r="U37" s="25" t="s">
@@ -8018,7 +8018,7 @@
         <v>55200001</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C38" s="25" t="s">
         <v>97</v>
@@ -8039,7 +8039,7 @@
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
       <c r="O38" s="20" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="P38" s="41">
         <v>1</v>
@@ -8051,7 +8051,7 @@
         <v>237</v>
       </c>
       <c r="S38" s="16" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="T38" s="25"/>
       <c r="U38" s="25" t="s">
@@ -8067,7 +8067,7 @@
         <v>40</v>
       </c>
       <c r="Y38" s="25" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="Z38" s="48"/>
     </row>
@@ -8076,23 +8076,23 @@
         <v>55200002</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C39" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E39" s="25">
         <v>30</v>
       </c>
       <c r="F39" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G39" s="60"/>
       <c r="H39" s="29" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I39" s="29"/>
       <c r="J39" s="28"/>
@@ -8109,11 +8109,11 @@
         <v>237</v>
       </c>
       <c r="S39" s="16" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="T39" s="25"/>
       <c r="U39" s="25" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="V39" s="25"/>
       <c r="W39" s="25"/>
@@ -8121,7 +8121,7 @@
         <v>15</v>
       </c>
       <c r="Y39" s="25" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="Z39" s="39"/>
     </row>
@@ -8136,17 +8136,17 @@
         <v>97</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E40" s="31">
         <v>30</v>
       </c>
       <c r="F40" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G40" s="60"/>
       <c r="H40" s="47" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I40" s="89"/>
       <c r="J40" s="91"/>
@@ -8163,7 +8163,7 @@
         <v>404</v>
       </c>
       <c r="S40" s="16" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="T40" s="31"/>
       <c r="U40" s="31"/>
@@ -8190,7 +8190,7 @@
         <v>97</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E41" s="25">
         <v>15</v>
@@ -8205,7 +8205,7 @@
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="O41" s="20" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="P41" s="41">
         <v>1</v>
@@ -8217,7 +8217,7 @@
         <v>237</v>
       </c>
       <c r="S41" s="16" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="T41" s="25"/>
       <c r="U41" s="10" t="s">
@@ -8231,7 +8231,7 @@
         <v>40</v>
       </c>
       <c r="Y41" s="25" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="Z41" s="96"/>
     </row>
@@ -8246,13 +8246,13 @@
         <v>97</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E42" s="25">
         <v>25</v>
       </c>
       <c r="F42" s="44" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G42" s="59"/>
       <c r="H42" s="47"/>
@@ -8263,7 +8263,7 @@
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
       <c r="O42" s="20" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="P42" s="41">
         <v>2</v>
@@ -8275,7 +8275,7 @@
         <v>237</v>
       </c>
       <c r="S42" s="16" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="T42" s="25"/>
       <c r="U42" s="10" t="s">
@@ -8316,7 +8316,7 @@
       <c r="H43" s="29"/>
       <c r="I43" s="29"/>
       <c r="J43" s="28" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K43" s="18"/>
       <c r="L43" s="17"/>
@@ -8364,7 +8364,7 @@
         <v>97</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E44" s="1">
         <v>15</v>
@@ -8376,12 +8376,12 @@
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
       <c r="J44" s="28" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="17"/>
       <c r="M44" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N44" s="17"/>
       <c r="O44" s="20"/>
@@ -8424,24 +8424,24 @@
         <v>97</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E45" s="25">
         <v>20</v>
       </c>
       <c r="F45" s="44" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G45" s="60"/>
       <c r="H45" s="29"/>
       <c r="I45" s="29"/>
       <c r="J45" s="26" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K45" s="27"/>
       <c r="L45" s="30"/>
       <c r="M45" s="17" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="N45" s="17"/>
       <c r="O45" s="20"/>
@@ -8453,7 +8453,7 @@
         <v>404</v>
       </c>
       <c r="S45" s="16" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="T45" s="25"/>
       <c r="U45" s="25" t="s">
@@ -8463,7 +8463,7 @@
         <v>442</v>
       </c>
       <c r="W45" s="25" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="X45" s="25">
         <v>25</v>
@@ -8484,7 +8484,7 @@
         <v>97</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>453</v>
+        <v>955</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="43" t="s">
@@ -8494,7 +8494,7 @@
       <c r="H46" s="29"/>
       <c r="I46" s="29"/>
       <c r="J46" s="28" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K46" s="18"/>
       <c r="L46" s="17"/>
@@ -8542,17 +8542,17 @@
         <v>97</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E47" s="25">
         <v>100</v>
       </c>
       <c r="F47" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G47" s="60"/>
       <c r="H47" s="29" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="I47" s="29"/>
       <c r="J47" s="28"/>
@@ -8569,11 +8569,11 @@
         <v>237</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="T47" s="25"/>
       <c r="U47" s="25" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="V47" s="25"/>
       <c r="W47" s="25"/>
@@ -8581,7 +8581,7 @@
         <v>25</v>
       </c>
       <c r="Y47" s="25" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="Z47" s="39"/>
     </row>
@@ -8590,13 +8590,13 @@
         <v>55200011</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C48" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E48" s="25">
         <v>12</v>
@@ -8604,7 +8604,7 @@
       <c r="F48" s="44"/>
       <c r="G48" s="59"/>
       <c r="H48" s="47" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="I48" s="47"/>
       <c r="J48" s="26"/>
@@ -8621,21 +8621,21 @@
         <v>237</v>
       </c>
       <c r="S48" s="16" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="T48" s="25"/>
       <c r="U48" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="V48" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="W48" s="10"/>
       <c r="X48" s="25">
         <v>20</v>
       </c>
       <c r="Y48" s="25" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="Z48" s="96"/>
     </row>
@@ -8644,13 +8644,13 @@
         <v>55200012</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C49" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E49" s="31">
         <v>15</v>
@@ -8660,7 +8660,7 @@
       </c>
       <c r="G49" s="60"/>
       <c r="H49" s="47" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="I49" s="89"/>
       <c r="J49" s="91"/>
@@ -8677,21 +8677,21 @@
         <v>404</v>
       </c>
       <c r="S49" s="16" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="T49" s="31"/>
       <c r="U49" s="25" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="V49" s="25" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="W49" s="31"/>
       <c r="X49" s="31">
         <v>30</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="Z49" s="25"/>
     </row>
@@ -8700,13 +8700,13 @@
         <v>55200013</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E50" s="31">
         <v>12</v>
@@ -8716,7 +8716,7 @@
       </c>
       <c r="G50" s="60"/>
       <c r="H50" s="47" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="I50" s="89"/>
       <c r="J50" s="91"/>
@@ -8733,21 +8733,21 @@
         <v>404</v>
       </c>
       <c r="S50" s="16" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="T50" s="31"/>
       <c r="U50" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="V50" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="W50" s="31"/>
       <c r="X50" s="31">
         <v>10</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="Z50" s="25"/>
     </row>
@@ -8756,13 +8756,13 @@
         <v>55200014</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="44" t="s">
@@ -8770,7 +8770,7 @@
       </c>
       <c r="G51" s="60"/>
       <c r="H51" s="97" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="I51" s="29"/>
       <c r="J51" s="26"/>
@@ -8787,21 +8787,21 @@
         <v>237</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="T51" s="25"/>
       <c r="U51" s="25" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="V51" s="25" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="W51" s="25"/>
       <c r="X51" s="25">
         <v>25</v>
       </c>
       <c r="Y51" s="25" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="Z51" s="48"/>
     </row>
@@ -8810,7 +8810,7 @@
         <v>55300001</v>
       </c>
       <c r="B52" s="53" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C52" s="25" t="s">
         <v>48</v>
@@ -8820,10 +8820,10 @@
       <c r="F52" s="44"/>
       <c r="G52" s="60"/>
       <c r="H52" s="47" t="s">
+        <v>911</v>
+      </c>
+      <c r="I52" s="47" t="s">
         <v>912</v>
-      </c>
-      <c r="I52" s="47" t="s">
-        <v>913</v>
       </c>
       <c r="J52" s="26"/>
       <c r="K52" s="27"/>
@@ -8839,7 +8839,7 @@
         <v>237</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="T52" s="25"/>
       <c r="U52" s="25"/>
@@ -8860,7 +8860,7 @@
         <v>55300002</v>
       </c>
       <c r="B53" s="53" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C53" s="25" t="s">
         <v>48</v>
@@ -8870,10 +8870,10 @@
       <c r="F53" s="44"/>
       <c r="G53" s="60"/>
       <c r="H53" s="47" t="s">
+        <v>476</v>
+      </c>
+      <c r="I53" s="47" t="s">
         <v>477</v>
-      </c>
-      <c r="I53" s="47" t="s">
-        <v>478</v>
       </c>
       <c r="J53" s="26"/>
       <c r="K53" s="27"/>
@@ -8889,7 +8889,7 @@
         <v>237</v>
       </c>
       <c r="S53" s="16" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="T53" s="25"/>
       <c r="U53" s="25"/>
@@ -8908,7 +8908,7 @@
         <v>55300003</v>
       </c>
       <c r="B54" s="53" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C54" s="25" t="s">
         <v>48</v>
@@ -8918,10 +8918,10 @@
       <c r="F54" s="44"/>
       <c r="G54" s="60"/>
       <c r="H54" s="29" t="s">
+        <v>479</v>
+      </c>
+      <c r="I54" s="29" t="s">
         <v>480</v>
-      </c>
-      <c r="I54" s="29" t="s">
-        <v>481</v>
       </c>
       <c r="J54" s="26"/>
       <c r="K54" s="27"/>
@@ -8937,7 +8937,7 @@
         <v>237</v>
       </c>
       <c r="S54" s="16" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="T54" s="25"/>
       <c r="U54" s="25"/>
@@ -8956,7 +8956,7 @@
         <v>55300004</v>
       </c>
       <c r="B55" s="53" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>48</v>
@@ -8966,10 +8966,10 @@
       <c r="F55" s="44"/>
       <c r="G55" s="60"/>
       <c r="H55" s="47" t="s">
+        <v>482</v>
+      </c>
+      <c r="I55" s="47" t="s">
         <v>483</v>
-      </c>
-      <c r="I55" s="47" t="s">
-        <v>484</v>
       </c>
       <c r="J55" s="26"/>
       <c r="K55" s="27"/>
@@ -8985,7 +8985,7 @@
         <v>237</v>
       </c>
       <c r="S55" s="16" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="T55" s="25"/>
       <c r="U55" s="25"/>
@@ -9004,7 +9004,7 @@
         <v>55300005</v>
       </c>
       <c r="B56" s="53" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>48</v>
@@ -9014,10 +9014,10 @@
       <c r="F56" s="44"/>
       <c r="G56" s="60"/>
       <c r="H56" s="47" t="s">
+        <v>485</v>
+      </c>
+      <c r="I56" s="47" t="s">
         <v>486</v>
-      </c>
-      <c r="I56" s="47" t="s">
-        <v>487</v>
       </c>
       <c r="J56" s="26"/>
       <c r="K56" s="27"/>
@@ -9033,7 +9033,7 @@
         <v>237</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="T56" s="25"/>
       <c r="U56" s="25"/>
@@ -9052,7 +9052,7 @@
         <v>55300006</v>
       </c>
       <c r="B57" s="53" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C57" s="25" t="s">
         <v>0</v>
@@ -9062,7 +9062,7 @@
       <c r="F57" s="44"/>
       <c r="G57" s="60"/>
       <c r="H57" s="47" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I57" s="47"/>
       <c r="J57" s="26"/>
@@ -9079,11 +9079,11 @@
         <v>237</v>
       </c>
       <c r="S57" s="49" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="T57" s="25"/>
       <c r="U57" s="25" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="V57" s="25"/>
       <c r="W57" s="25"/>
@@ -9091,7 +9091,7 @@
         <v>25</v>
       </c>
       <c r="Y57" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="Z57" s="48"/>
     </row>
@@ -9100,7 +9100,7 @@
         <v>55300007</v>
       </c>
       <c r="B58" s="53" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C58" s="25" t="s">
         <v>48</v>
@@ -9110,10 +9110,10 @@
       <c r="F58" s="44"/>
       <c r="G58" s="60"/>
       <c r="H58" s="47" t="s">
+        <v>487</v>
+      </c>
+      <c r="I58" s="47" t="s">
         <v>488</v>
-      </c>
-      <c r="I58" s="47" t="s">
-        <v>489</v>
       </c>
       <c r="J58" s="26"/>
       <c r="K58" s="27"/>
@@ -9129,7 +9129,7 @@
         <v>237</v>
       </c>
       <c r="S58" s="16" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="T58" s="25"/>
       <c r="U58" s="25"/>
@@ -9148,7 +9148,7 @@
         <v>55300008</v>
       </c>
       <c r="B59" s="53" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>48</v>
@@ -9158,10 +9158,10 @@
       <c r="F59" s="44"/>
       <c r="G59" s="60"/>
       <c r="H59" s="47" t="s">
+        <v>853</v>
+      </c>
+      <c r="I59" s="47" t="s">
         <v>854</v>
-      </c>
-      <c r="I59" s="47" t="s">
-        <v>855</v>
       </c>
       <c r="J59" s="26"/>
       <c r="K59" s="27"/>
@@ -9177,7 +9177,7 @@
         <v>237</v>
       </c>
       <c r="S59" s="16" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="T59" s="25"/>
       <c r="U59" s="25"/>
@@ -9196,7 +9196,7 @@
         <v>55300009</v>
       </c>
       <c r="B60" s="53" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>48</v>
@@ -9206,10 +9206,10 @@
       <c r="F60" s="44"/>
       <c r="G60" s="60"/>
       <c r="H60" s="47" t="s">
+        <v>914</v>
+      </c>
+      <c r="I60" s="47" t="s">
         <v>915</v>
-      </c>
-      <c r="I60" s="47" t="s">
-        <v>916</v>
       </c>
       <c r="J60" s="26"/>
       <c r="K60" s="27"/>
@@ -9225,7 +9225,7 @@
         <v>237</v>
       </c>
       <c r="S60" s="16" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="T60" s="25"/>
       <c r="U60" s="25"/>
@@ -9235,7 +9235,7 @@
         <v>30</v>
       </c>
       <c r="Y60" s="25" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="Z60" s="48"/>
     </row>
@@ -9244,7 +9244,7 @@
         <v>55300010</v>
       </c>
       <c r="B61" s="53" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>48</v>
@@ -9254,10 +9254,10 @@
       <c r="F61" s="44"/>
       <c r="G61" s="60"/>
       <c r="H61" s="47" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="I61" s="47" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="J61" s="26"/>
       <c r="K61" s="27"/>
@@ -9273,7 +9273,7 @@
         <v>237</v>
       </c>
       <c r="S61" s="16" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="T61" s="25"/>
       <c r="U61" s="25"/>
@@ -9283,7 +9283,7 @@
         <v>35</v>
       </c>
       <c r="Y61" s="25" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="Z61" s="48"/>
     </row>
@@ -9309,7 +9309,7 @@
       <c r="M62" s="17"/>
       <c r="N62" s="17"/>
       <c r="O62" s="20" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P62" s="41">
         <v>1</v>
@@ -9321,7 +9321,7 @@
         <v>237</v>
       </c>
       <c r="S62" s="16" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="T62" s="25"/>
       <c r="U62" s="25"/>
@@ -9356,7 +9356,7 @@
       <c r="L63" s="17"/>
       <c r="M63" s="17"/>
       <c r="N63" s="17" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="O63" s="20"/>
       <c r="P63" s="41"/>
@@ -9367,7 +9367,7 @@
         <v>237</v>
       </c>
       <c r="S63" s="10" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="T63" s="10"/>
       <c r="U63" s="1"/>
@@ -9413,7 +9413,7 @@
         <v>237</v>
       </c>
       <c r="S64" s="10" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="T64" s="10"/>
       <c r="U64" s="1"/>
@@ -9435,7 +9435,7 @@
         <v>434</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D65" s="25"/>
       <c r="E65" s="25"/>
@@ -9449,7 +9449,7 @@
       <c r="M65" s="17"/>
       <c r="N65" s="17"/>
       <c r="O65" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="P65" s="41">
         <v>2</v>
@@ -9461,7 +9461,7 @@
         <v>237</v>
       </c>
       <c r="S65" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="T65" s="25"/>
       <c r="U65" s="25" t="s">
@@ -9485,20 +9485,20 @@
         <v>324</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E66" s="25">
         <v>10</v>
       </c>
       <c r="F66" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G66" s="60"/>
       <c r="H66" s="47" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I66" s="47"/>
       <c r="J66" s="26"/>
@@ -9515,7 +9515,7 @@
         <v>237</v>
       </c>
       <c r="S66" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="T66" s="25"/>
       <c r="U66" s="25"/>
@@ -9534,10 +9534,10 @@
         <v>55400003</v>
       </c>
       <c r="B67" s="54" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D67" s="25"/>
       <c r="E67" s="25"/>
@@ -9551,7 +9551,7 @@
       <c r="M67" s="17"/>
       <c r="N67" s="17"/>
       <c r="O67" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P67" s="41">
         <v>2</v>
@@ -9563,7 +9563,7 @@
         <v>237</v>
       </c>
       <c r="S67" s="16" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="T67" s="25"/>
       <c r="U67" s="25" t="s">
@@ -9575,7 +9575,7 @@
         <v>80</v>
       </c>
       <c r="Y67" s="50" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Z67" s="48"/>
     </row>
@@ -9584,10 +9584,10 @@
         <v>55400004</v>
       </c>
       <c r="B68" s="54" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25"/>
@@ -9601,7 +9601,7 @@
       <c r="M68" s="17"/>
       <c r="N68" s="17"/>
       <c r="O68" s="20" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="P68" s="41">
         <v>3</v>
@@ -9613,11 +9613,11 @@
         <v>237</v>
       </c>
       <c r="S68" s="16" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="T68" s="25"/>
       <c r="U68" s="25" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="V68" s="25"/>
       <c r="W68" s="25"/>
@@ -9625,7 +9625,7 @@
         <v>80</v>
       </c>
       <c r="Y68" s="50" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="Z68" s="48"/>
     </row>
@@ -9634,10 +9634,10 @@
         <v>55400005</v>
       </c>
       <c r="B69" s="54" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D69" s="25"/>
       <c r="E69" s="25"/>
@@ -9651,7 +9651,7 @@
       <c r="M69" s="17"/>
       <c r="N69" s="17"/>
       <c r="O69" s="20" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="P69" s="41">
         <v>2.5</v>
@@ -9663,7 +9663,7 @@
         <v>237</v>
       </c>
       <c r="S69" s="16" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="T69" s="25"/>
       <c r="U69" s="25" t="s">
@@ -9684,10 +9684,10 @@
         <v>55400006</v>
       </c>
       <c r="B70" s="54" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
@@ -9701,7 +9701,7 @@
       <c r="M70" s="17"/>
       <c r="N70" s="17"/>
       <c r="O70" s="20" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="P70" s="41">
         <v>2</v>
@@ -9713,7 +9713,7 @@
         <v>237</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="T70" s="25"/>
       <c r="U70" s="25" t="s">
@@ -9725,7 +9725,7 @@
         <v>30</v>
       </c>
       <c r="Y70" s="50" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="Z70" s="48"/>
     </row>
@@ -9734,10 +9734,10 @@
         <v>55410001</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C71" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D71" s="25"/>
       <c r="E71" s="25"/>
@@ -9750,7 +9750,7 @@
       <c r="L71" s="30"/>
       <c r="M71" s="17"/>
       <c r="N71" s="17" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="O71" s="20"/>
       <c r="P71" s="41"/>
@@ -9761,7 +9761,7 @@
         <v>237</v>
       </c>
       <c r="S71" s="16" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="T71" s="25"/>
       <c r="U71" s="25" t="s">
@@ -9773,7 +9773,7 @@
         <v>50</v>
       </c>
       <c r="Y71" s="50" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="Z71" s="48"/>
     </row>
@@ -9794,11 +9794,11 @@
       <c r="H72" s="47"/>
       <c r="I72" s="47"/>
       <c r="J72" s="26" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K72" s="27"/>
       <c r="L72" s="30" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M72" s="17"/>
       <c r="N72" s="17"/>
@@ -9811,7 +9811,7 @@
         <v>237</v>
       </c>
       <c r="S72" s="16" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="T72" s="25"/>
       <c r="U72" s="25"/>
@@ -9842,11 +9842,11 @@
       <c r="H73" s="47"/>
       <c r="I73" s="47"/>
       <c r="J73" s="26" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K73" s="27"/>
       <c r="L73" s="30" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="M73" s="17"/>
       <c r="N73" s="17"/>
@@ -9859,7 +9859,7 @@
         <v>237</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="T73" s="25"/>
       <c r="U73" s="25"/>
@@ -9878,7 +9878,7 @@
         <v>55500003</v>
       </c>
       <c r="B74" s="56" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C74" s="25" t="s">
         <v>4</v>
@@ -9990,7 +9990,7 @@
       </c>
       <c r="K76" s="27"/>
       <c r="L76" s="30" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M76" s="17"/>
       <c r="N76" s="17"/>
@@ -10003,7 +10003,7 @@
         <v>237</v>
       </c>
       <c r="S76" s="16" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T76" s="37"/>
       <c r="U76" s="25"/>
@@ -10022,7 +10022,7 @@
         <v>55500006</v>
       </c>
       <c r="B77" s="56" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C77" s="25" t="s">
         <v>4</v>
@@ -10034,11 +10034,11 @@
       <c r="H77" s="29"/>
       <c r="I77" s="29"/>
       <c r="J77" s="26" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K77" s="27"/>
       <c r="L77" s="30" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M77" s="17"/>
       <c r="N77" s="17"/>
@@ -10051,7 +10051,7 @@
         <v>237</v>
       </c>
       <c r="S77" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="T77" s="37"/>
       <c r="U77" s="25"/>
@@ -10061,7 +10061,7 @@
         <v>5</v>
       </c>
       <c r="Y77" s="25" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="Z77" s="39"/>
     </row>
@@ -10086,7 +10086,7 @@
       </c>
       <c r="K78" s="27"/>
       <c r="L78" s="30" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="M78" s="17"/>
       <c r="N78" s="17"/>
@@ -10099,7 +10099,7 @@
         <v>237</v>
       </c>
       <c r="S78" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="T78" s="37"/>
       <c r="U78" s="25"/>
@@ -10214,7 +10214,7 @@
         <v>55500010</v>
       </c>
       <c r="B81" s="56" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C81" s="25" t="s">
         <v>4</v>
@@ -10278,7 +10278,7 @@
       </c>
       <c r="K82" s="27"/>
       <c r="L82" s="30" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="M82" s="17"/>
       <c r="N82" s="17"/>
@@ -10291,7 +10291,7 @@
         <v>237</v>
       </c>
       <c r="S82" s="16" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T82" s="37"/>
       <c r="U82" s="25"/>
@@ -10454,7 +10454,7 @@
         <v>55500015</v>
       </c>
       <c r="B86" s="56" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C86" s="25" t="s">
         <v>4</v>
@@ -10466,7 +10466,7 @@
       <c r="H86" s="47"/>
       <c r="I86" s="47"/>
       <c r="J86" s="26" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K86" s="27"/>
       <c r="L86" s="30" t="s">
@@ -10483,7 +10483,7 @@
         <v>237</v>
       </c>
       <c r="S86" s="16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="T86" s="25"/>
       <c r="U86" s="25"/>
@@ -10493,7 +10493,7 @@
         <v>5</v>
       </c>
       <c r="Y86" s="25" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="Z86" s="48"/>
     </row>
@@ -10502,7 +10502,7 @@
         <v>55500016</v>
       </c>
       <c r="B87" s="56" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C87" s="25" t="s">
         <v>4</v>
@@ -10514,7 +10514,7 @@
       <c r="H87" s="47"/>
       <c r="I87" s="47"/>
       <c r="J87" s="26" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K87" s="27"/>
       <c r="L87" s="30" t="s">
@@ -10531,7 +10531,7 @@
         <v>237</v>
       </c>
       <c r="S87" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="T87" s="25"/>
       <c r="U87" s="25"/>
@@ -10541,7 +10541,7 @@
         <v>5</v>
       </c>
       <c r="Y87" s="25" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="Z87" s="48"/>
     </row>
@@ -10565,7 +10565,7 @@
       <c r="K88" s="18"/>
       <c r="L88" s="17"/>
       <c r="M88" s="17" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="N88" s="17"/>
       <c r="O88" s="20"/>
@@ -10577,7 +10577,7 @@
         <v>237</v>
       </c>
       <c r="S88" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
@@ -10611,7 +10611,7 @@
       <c r="K89" s="18"/>
       <c r="L89" s="17"/>
       <c r="M89" s="17" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="N89" s="17"/>
       <c r="O89" s="20"/>
@@ -10623,7 +10623,7 @@
         <v>237</v>
       </c>
       <c r="S89" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
@@ -10657,7 +10657,7 @@
       <c r="K90" s="18"/>
       <c r="L90" s="17"/>
       <c r="M90" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="N90" s="17"/>
       <c r="O90" s="20"/>
@@ -10669,7 +10669,7 @@
         <v>237</v>
       </c>
       <c r="S90" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
@@ -10703,7 +10703,7 @@
       <c r="K91" s="18"/>
       <c r="L91" s="17"/>
       <c r="M91" s="17" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="N91" s="17"/>
       <c r="O91" s="20"/>
@@ -10715,7 +10715,7 @@
         <v>237</v>
       </c>
       <c r="S91" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
@@ -10749,7 +10749,7 @@
       <c r="K92" s="18"/>
       <c r="L92" s="17"/>
       <c r="M92" s="17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="N92" s="17"/>
       <c r="O92" s="20"/>
@@ -10758,10 +10758,10 @@
         <v>242</v>
       </c>
       <c r="R92" s="43" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="S92" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
@@ -10795,7 +10795,7 @@
       <c r="K93" s="18"/>
       <c r="L93" s="17"/>
       <c r="M93" s="17" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="N93" s="17"/>
       <c r="O93" s="20"/>
@@ -10807,7 +10807,7 @@
         <v>237</v>
       </c>
       <c r="S93" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
@@ -10841,7 +10841,7 @@
       <c r="K94" s="18"/>
       <c r="L94" s="17"/>
       <c r="M94" s="17" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="N94" s="17"/>
       <c r="O94" s="20"/>
@@ -10853,7 +10853,7 @@
         <v>237</v>
       </c>
       <c r="S94" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
@@ -10887,7 +10887,7 @@
       <c r="K95" s="18"/>
       <c r="L95" s="17"/>
       <c r="M95" s="17" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="N95" s="17"/>
       <c r="O95" s="20"/>
@@ -10899,7 +10899,7 @@
         <v>237</v>
       </c>
       <c r="S95" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
@@ -10933,7 +10933,7 @@
       <c r="K96" s="18"/>
       <c r="L96" s="17"/>
       <c r="M96" s="17" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="N96" s="17"/>
       <c r="O96" s="20"/>
@@ -10942,10 +10942,10 @@
         <v>242</v>
       </c>
       <c r="R96" s="43" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="S96" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
@@ -10979,7 +10979,7 @@
       <c r="K97" s="18"/>
       <c r="L97" s="17"/>
       <c r="M97" s="17" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="N97" s="17"/>
       <c r="O97" s="20"/>
@@ -10988,10 +10988,10 @@
         <v>242</v>
       </c>
       <c r="R97" s="43" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="S97" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
@@ -11025,7 +11025,7 @@
       <c r="K98" s="18"/>
       <c r="L98" s="17"/>
       <c r="M98" s="17" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="N98" s="17"/>
       <c r="O98" s="20"/>
@@ -11037,7 +11037,7 @@
         <v>237</v>
       </c>
       <c r="S98" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
@@ -11071,7 +11071,7 @@
       <c r="K99" s="18"/>
       <c r="L99" s="17"/>
       <c r="M99" s="17" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="N99" s="17"/>
       <c r="O99" s="20"/>
@@ -11083,7 +11083,7 @@
         <v>237</v>
       </c>
       <c r="S99" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
@@ -11117,7 +11117,7 @@
       <c r="K100" s="18"/>
       <c r="L100" s="17"/>
       <c r="M100" s="17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="N100" s="17"/>
       <c r="O100" s="20"/>
@@ -11129,7 +11129,7 @@
         <v>237</v>
       </c>
       <c r="S100" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
@@ -11163,7 +11163,7 @@
       <c r="K101" s="18"/>
       <c r="L101" s="17"/>
       <c r="M101" s="17" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="N101" s="17"/>
       <c r="O101" s="20"/>
@@ -11175,7 +11175,7 @@
         <v>237</v>
       </c>
       <c r="S101" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
@@ -11209,7 +11209,7 @@
       <c r="K102" s="18"/>
       <c r="L102" s="17"/>
       <c r="M102" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="N102" s="17"/>
       <c r="O102" s="20"/>
@@ -11221,7 +11221,7 @@
         <v>237</v>
       </c>
       <c r="S102" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="T102" s="10"/>
       <c r="U102" s="1"/>
@@ -11240,7 +11240,7 @@
         <v>55520002</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>35</v>
@@ -11255,7 +11255,7 @@
       <c r="K103" s="18"/>
       <c r="L103" s="17"/>
       <c r="M103" s="17" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="N103" s="17"/>
       <c r="O103" s="20"/>
@@ -11267,7 +11267,7 @@
         <v>237</v>
       </c>
       <c r="S103" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="T103" s="10"/>
       <c r="U103" s="1"/>
@@ -11301,7 +11301,7 @@
       <c r="K104" s="18"/>
       <c r="L104" s="17"/>
       <c r="M104" s="17" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="N104" s="17"/>
       <c r="O104" s="20"/>
@@ -11313,7 +11313,7 @@
         <v>237</v>
       </c>
       <c r="S104" s="10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T104" s="10"/>
       <c r="U104" s="1"/>
@@ -11332,7 +11332,7 @@
         <v>55520004</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>35</v>
@@ -11347,7 +11347,7 @@
       <c r="K105" s="18"/>
       <c r="L105" s="17"/>
       <c r="M105" s="17" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="N105" s="17"/>
       <c r="O105" s="20"/>
@@ -11359,7 +11359,7 @@
         <v>237</v>
       </c>
       <c r="S105" s="10" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="T105" s="10"/>
       <c r="U105" s="1"/>
@@ -11369,7 +11369,7 @@
         <v>150</v>
       </c>
       <c r="Y105" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="Z105" s="25"/>
     </row>
@@ -11388,7 +11388,7 @@
       <c r="F106" s="43"/>
       <c r="G106" s="60"/>
       <c r="H106" s="29" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I106" s="29"/>
       <c r="J106" s="28"/>
@@ -11438,7 +11438,7 @@
       <c r="F107" s="43"/>
       <c r="G107" s="60"/>
       <c r="H107" s="29" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I107" s="29"/>
       <c r="J107" s="28"/>
@@ -11678,7 +11678,7 @@
         <v>55600007</v>
       </c>
       <c r="B112" s="58" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>48</v>
@@ -11838,7 +11838,7 @@
       <c r="F115" s="43"/>
       <c r="G115" s="60"/>
       <c r="H115" s="29" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I115" s="29"/>
       <c r="J115" s="28"/>
@@ -11888,7 +11888,7 @@
       <c r="F116" s="43"/>
       <c r="G116" s="60"/>
       <c r="H116" s="29" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I116" s="29"/>
       <c r="J116" s="28"/>
@@ -11905,7 +11905,7 @@
         <v>404</v>
       </c>
       <c r="S116" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="T116" s="10">
         <v>56000023</v>
@@ -11913,7 +11913,7 @@
       <c r="U116" s="1"/>
       <c r="V116" s="1"/>
       <c r="W116" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="X116" s="1">
         <v>20</v>
@@ -11938,7 +11938,7 @@
       <c r="F117" s="43"/>
       <c r="G117" s="60"/>
       <c r="H117" s="29" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I117" s="29"/>
       <c r="J117" s="28"/>
@@ -11978,7 +11978,7 @@
         <v>55600013</v>
       </c>
       <c r="B118" s="58" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>48</v>
@@ -11988,7 +11988,7 @@
       <c r="F118" s="43"/>
       <c r="G118" s="60"/>
       <c r="H118" s="29" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="I118" s="29"/>
       <c r="J118" s="28"/>
@@ -12005,7 +12005,7 @@
         <v>237</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="T118" s="10">
         <v>56000001</v>
@@ -12028,7 +12028,7 @@
         <v>55600014</v>
       </c>
       <c r="B119" s="58" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>48</v>
@@ -12038,7 +12038,7 @@
       <c r="F119" s="43"/>
       <c r="G119" s="60"/>
       <c r="H119" s="29" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I119" s="29"/>
       <c r="J119" s="28"/>
@@ -12069,7 +12069,7 @@
         <v>30</v>
       </c>
       <c r="Y119" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Z119" s="37"/>
     </row>
@@ -12078,7 +12078,7 @@
         <v>55600015</v>
       </c>
       <c r="B120" s="58" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>48</v>
@@ -12088,7 +12088,7 @@
       <c r="F120" s="43"/>
       <c r="G120" s="60"/>
       <c r="H120" s="29" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I120" s="29"/>
       <c r="J120" s="28"/>
@@ -12105,7 +12105,7 @@
         <v>237</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="T120" s="10">
         <v>56000101</v>
@@ -12119,7 +12119,7 @@
         <v>10</v>
       </c>
       <c r="Y120" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="Z120" s="37"/>
     </row>
@@ -12128,7 +12128,7 @@
         <v>55600016</v>
       </c>
       <c r="B121" s="58" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>48</v>
@@ -12138,7 +12138,7 @@
       <c r="F121" s="43"/>
       <c r="G121" s="60"/>
       <c r="H121" s="29" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I121" s="29"/>
       <c r="J121" s="28"/>
@@ -12155,7 +12155,7 @@
         <v>237</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="T121" s="10">
         <v>56000101</v>
@@ -12169,7 +12169,7 @@
         <v>15</v>
       </c>
       <c r="Y121" s="1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="Z121" s="37"/>
     </row>
@@ -12222,7 +12222,7 @@
         <v>55610002</v>
       </c>
       <c r="B123" s="76" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>46</v>
@@ -12251,7 +12251,7 @@
         <v>237</v>
       </c>
       <c r="S123" s="10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="T123" s="10"/>
       <c r="U123" s="1"/>
@@ -12261,7 +12261,7 @@
         <v>5</v>
       </c>
       <c r="Y123" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="Z123" s="37"/>
     </row>
@@ -12270,7 +12270,7 @@
         <v>55610003</v>
       </c>
       <c r="B124" s="76" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>46</v>
@@ -12299,7 +12299,7 @@
         <v>237</v>
       </c>
       <c r="S124" s="10" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="T124" s="10"/>
       <c r="U124" s="1"/>
@@ -12309,7 +12309,7 @@
         <v>5</v>
       </c>
       <c r="Y124" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="Z124" s="37"/>
     </row>
@@ -12318,7 +12318,7 @@
         <v>55610004</v>
       </c>
       <c r="B125" s="76" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>46</v>
@@ -12334,7 +12334,7 @@
       </c>
       <c r="K125" s="18"/>
       <c r="L125" s="17" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="M125" s="17"/>
       <c r="N125" s="17"/>
@@ -12347,7 +12347,7 @@
         <v>237</v>
       </c>
       <c r="S125" s="10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="T125" s="10"/>
       <c r="U125" s="1"/>
@@ -12357,7 +12357,7 @@
         <v>10</v>
       </c>
       <c r="Y125" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="Z125" s="37"/>
     </row>
@@ -12366,10 +12366,10 @@
         <v>55700001</v>
       </c>
       <c r="B126" s="52" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
@@ -12381,7 +12381,7 @@
       <c r="K126" s="18"/>
       <c r="L126" s="17"/>
       <c r="M126" s="17" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="N126" s="17"/>
       <c r="O126" s="20"/>
@@ -12393,7 +12393,7 @@
         <v>237</v>
       </c>
       <c r="S126" s="10" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="T126" s="10"/>
       <c r="U126" s="1"/>
@@ -12406,7 +12406,7 @@
         <v>209</v>
       </c>
       <c r="Z126" s="37" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="127" spans="1:26">
@@ -12414,7 +12414,7 @@
         <v>55700002</v>
       </c>
       <c r="B127" s="52" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>126</v>
@@ -12429,7 +12429,7 @@
       <c r="K127" s="18"/>
       <c r="L127" s="17"/>
       <c r="M127" s="17" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="N127" s="17"/>
       <c r="O127" s="20"/>
@@ -12441,7 +12441,7 @@
         <v>237</v>
       </c>
       <c r="S127" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="T127" s="10"/>
       <c r="U127" s="1"/>
@@ -12454,7 +12454,7 @@
         <v>196</v>
       </c>
       <c r="Z127" s="37" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="128" spans="1:26" ht="36">
@@ -12462,7 +12462,7 @@
         <v>55700003</v>
       </c>
       <c r="B128" s="52" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>126</v>
@@ -12478,7 +12478,7 @@
       <c r="L128" s="17"/>
       <c r="M128" s="17"/>
       <c r="N128" s="17" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="O128" s="20"/>
       <c r="P128" s="41"/>
@@ -12489,7 +12489,7 @@
         <v>237</v>
       </c>
       <c r="S128" s="10" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="T128" s="10"/>
       <c r="U128" s="1"/>
@@ -12502,7 +12502,7 @@
         <v>146</v>
       </c>
       <c r="Z128" s="37" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="129" spans="1:26" ht="36">
@@ -12510,7 +12510,7 @@
         <v>55700004</v>
       </c>
       <c r="B129" s="52" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>126</v>
@@ -12526,7 +12526,7 @@
       <c r="L129" s="30"/>
       <c r="M129" s="17"/>
       <c r="N129" s="17" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="O129" s="20"/>
       <c r="P129" s="41"/>
@@ -12537,7 +12537,7 @@
         <v>237</v>
       </c>
       <c r="S129" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="T129" s="10"/>
       <c r="U129" s="1"/>
@@ -12550,7 +12550,7 @@
         <v>145</v>
       </c>
       <c r="Z129" s="25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="130" spans="1:26" ht="24">
@@ -12558,7 +12558,7 @@
         <v>55700005</v>
       </c>
       <c r="B130" s="52" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C130" s="25" t="s">
         <v>403</v>
@@ -12575,7 +12575,7 @@
       <c r="M130" s="17"/>
       <c r="N130" s="17"/>
       <c r="O130" s="20" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="P130" s="41">
         <v>1</v>
@@ -12587,7 +12587,7 @@
         <v>404</v>
       </c>
       <c r="S130" s="16" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="T130" s="25"/>
       <c r="U130" s="25"/>
@@ -12600,7 +12600,7 @@
         <v>208</v>
       </c>
       <c r="Z130" s="25" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="131" spans="1:26" ht="96">
@@ -12620,11 +12620,11 @@
         <v>40</v>
       </c>
       <c r="F131" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G131" s="60"/>
       <c r="H131" s="47" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I131" s="47"/>
       <c r="J131" s="26"/>
@@ -12678,11 +12678,11 @@
         <v>20</v>
       </c>
       <c r="F132" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G132" s="60"/>
       <c r="H132" s="47" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I132" s="47"/>
       <c r="J132" s="26"/>
@@ -12699,7 +12699,7 @@
         <v>237</v>
       </c>
       <c r="S132" s="16" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="T132" s="25"/>
       <c r="U132" s="25"/>
@@ -12712,7 +12712,7 @@
         <v>111</v>
       </c>
       <c r="Z132" s="48" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="133" spans="1:26" ht="24">
@@ -12720,7 +12720,7 @@
         <v>55900003</v>
       </c>
       <c r="B133" s="55" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C133" s="25" t="s">
         <v>0</v>
@@ -12730,7 +12730,7 @@
       <c r="F133" s="44"/>
       <c r="G133" s="60"/>
       <c r="H133" s="47" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I133" s="47"/>
       <c r="J133" s="26"/>
@@ -12747,7 +12747,7 @@
         <v>237</v>
       </c>
       <c r="S133" s="16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="T133" s="25"/>
       <c r="U133" s="25"/>
@@ -12757,7 +12757,7 @@
         <v>80</v>
       </c>
       <c r="Y133" s="25" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Z133" s="48"/>
     </row>
@@ -12766,7 +12766,7 @@
         <v>55900004</v>
       </c>
       <c r="B134" s="55" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C134" s="25" t="s">
         <v>0</v>
@@ -12782,7 +12782,7 @@
       <c r="L134" s="30"/>
       <c r="M134" s="17"/>
       <c r="N134" s="17" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="O134" s="20"/>
       <c r="P134" s="41"/>
@@ -12793,11 +12793,11 @@
         <v>237</v>
       </c>
       <c r="S134" s="16" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="T134" s="25"/>
       <c r="U134" s="25" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="V134" s="25"/>
       <c r="W134" s="25"/>
@@ -12805,7 +12805,7 @@
         <v>-30</v>
       </c>
       <c r="Y134" s="25" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Z134" s="48"/>
     </row>
@@ -12814,7 +12814,7 @@
         <v>55900005</v>
       </c>
       <c r="B135" s="55" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C135" s="25" t="s">
         <v>0</v>
@@ -12830,7 +12830,7 @@
       <c r="L135" s="17"/>
       <c r="M135" s="17"/>
       <c r="N135" s="17" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O135" s="20"/>
       <c r="P135" s="41"/>
@@ -12841,7 +12841,7 @@
         <v>237</v>
       </c>
       <c r="S135" s="49" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="T135" s="25"/>
       <c r="U135" s="25"/>
@@ -12860,7 +12860,7 @@
         <v>55900006</v>
       </c>
       <c r="B136" s="55" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>0</v>
@@ -12877,7 +12877,7 @@
       <c r="K136" s="18"/>
       <c r="L136" s="17"/>
       <c r="M136" s="17" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="N136" s="17"/>
       <c r="O136" s="20"/>
@@ -12908,7 +12908,7 @@
         <v>55900007</v>
       </c>
       <c r="B137" s="55" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>0</v>
@@ -12954,7 +12954,7 @@
         <v>55900008</v>
       </c>
       <c r="B138" s="55" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>0</v>
@@ -12991,7 +12991,7 @@
         <v>40</v>
       </c>
       <c r="Y138" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="Z138" s="39"/>
     </row>
@@ -13000,7 +13000,7 @@
         <v>55900009</v>
       </c>
       <c r="B139" s="55" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>0</v>
@@ -13009,7 +13009,7 @@
       <c r="E139" s="1"/>
       <c r="F139" s="43"/>
       <c r="G139" s="60" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H139" s="29"/>
       <c r="I139" s="29"/>
@@ -13027,7 +13027,7 @@
         <v>237</v>
       </c>
       <c r="S139" s="10" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="T139" s="10"/>
       <c r="U139" s="1"/>
@@ -13037,7 +13037,7 @@
         <v>30</v>
       </c>
       <c r="Y139" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="Z139" s="37"/>
     </row>
@@ -13046,7 +13046,7 @@
         <v>55900010</v>
       </c>
       <c r="B140" s="55" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>0</v>
@@ -13055,7 +13055,7 @@
       <c r="E140" s="1"/>
       <c r="F140" s="43"/>
       <c r="G140" s="60" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="H140" s="29"/>
       <c r="I140" s="29"/>
@@ -13073,7 +13073,7 @@
         <v>237</v>
       </c>
       <c r="S140" s="10" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="T140" s="1"/>
       <c r="U140" s="1"/>
@@ -13092,7 +13092,7 @@
         <v>55900011</v>
       </c>
       <c r="B141" s="55" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>0</v>
@@ -13102,7 +13102,7 @@
       <c r="F141" s="43"/>
       <c r="G141" s="60"/>
       <c r="H141" s="47" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I141" s="47"/>
       <c r="J141" s="26"/>
@@ -13119,7 +13119,7 @@
         <v>237</v>
       </c>
       <c r="S141" s="10" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="T141" s="10"/>
       <c r="U141" s="1"/>
@@ -13138,7 +13138,7 @@
         <v>55900012</v>
       </c>
       <c r="B142" s="55" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C142" s="25" t="s">
         <v>336</v>
@@ -13154,7 +13154,7 @@
       </c>
       <c r="G142" s="60"/>
       <c r="H142" s="29" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I142" s="29"/>
       <c r="J142" s="28"/>
@@ -13171,12 +13171,12 @@
         <v>237</v>
       </c>
       <c r="S142" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="T142" s="25"/>
       <c r="U142" s="25"/>
       <c r="V142" s="25" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="W142" s="25"/>
       <c r="X142" s="25">
@@ -13192,7 +13192,7 @@
         <v>55900013</v>
       </c>
       <c r="B143" s="55" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>0</v>
@@ -13204,7 +13204,7 @@
       <c r="H143" s="29"/>
       <c r="I143" s="29"/>
       <c r="J143" s="28" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K143" s="18"/>
       <c r="L143" s="17" t="s">
@@ -13240,7 +13240,7 @@
         <v>55900014</v>
       </c>
       <c r="B144" s="55" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>0</v>
@@ -13258,7 +13258,7 @@
       <c r="L144" s="17"/>
       <c r="M144" s="17"/>
       <c r="N144" s="17" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="O144" s="20"/>
       <c r="P144" s="41"/>
@@ -13269,7 +13269,7 @@
         <v>237</v>
       </c>
       <c r="S144" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="T144" s="1"/>
       <c r="U144" s="1"/>
@@ -13288,7 +13288,7 @@
         <v>55900015</v>
       </c>
       <c r="B145" s="55" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>0</v>
@@ -13334,7 +13334,7 @@
         <v>55900016</v>
       </c>
       <c r="B146" s="55" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>336</v>
@@ -13365,7 +13365,7 @@
         <v>237</v>
       </c>
       <c r="S146" s="10" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="T146" s="10"/>
       <c r="U146" s="1" t="s">
@@ -13377,7 +13377,7 @@
         <v>45</v>
       </c>
       <c r="Y146" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="Z146" s="48"/>
     </row>
@@ -13386,7 +13386,7 @@
         <v>55900017</v>
       </c>
       <c r="B147" s="55" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>336</v>
@@ -13403,7 +13403,7 @@
       <c r="M147" s="21"/>
       <c r="N147" s="21"/>
       <c r="O147" s="20" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="P147" s="41">
         <v>1</v>
@@ -13438,7 +13438,7 @@
         <v>55900018</v>
       </c>
       <c r="B148" s="55" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>336</v>
@@ -13455,7 +13455,7 @@
       <c r="M148" s="21"/>
       <c r="N148" s="21"/>
       <c r="O148" s="19" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="P148" s="41">
         <v>1</v>
@@ -13490,7 +13490,7 @@
         <v>55900019</v>
       </c>
       <c r="B149" s="55" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>336</v>
@@ -13507,7 +13507,7 @@
       <c r="M149" s="21"/>
       <c r="N149" s="21"/>
       <c r="O149" s="20" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="P149" s="41">
         <v>1</v>
@@ -13542,13 +13542,13 @@
         <v>55900020</v>
       </c>
       <c r="B150" s="55" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C150" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D150" s="25" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E150" s="25">
         <v>30</v>
@@ -13558,7 +13558,7 @@
       </c>
       <c r="G150" s="79"/>
       <c r="H150" s="29" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="I150" s="88"/>
       <c r="J150" s="90"/>
@@ -13575,7 +13575,7 @@
         <v>237</v>
       </c>
       <c r="S150" s="10" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="T150" s="78"/>
       <c r="U150" s="78"/>
@@ -13585,7 +13585,7 @@
         <v>20</v>
       </c>
       <c r="Y150" s="25" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="Z150" s="83"/>
     </row>
@@ -13594,7 +13594,7 @@
         <v>55900021</v>
       </c>
       <c r="B151" s="55" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C151" s="25" t="s">
         <v>0</v>
@@ -13642,13 +13642,13 @@
         <v>55900022</v>
       </c>
       <c r="B152" s="55" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C152" s="25" t="s">
         <v>403</v>
       </c>
       <c r="D152" s="25" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E152" s="25">
         <v>200</v>
@@ -13656,7 +13656,7 @@
       <c r="F152" s="25"/>
       <c r="G152" s="60"/>
       <c r="H152" s="84" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I152" s="47"/>
       <c r="J152" s="26"/>
@@ -13673,7 +13673,7 @@
         <v>404</v>
       </c>
       <c r="S152" s="16" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="T152" s="25"/>
       <c r="U152" s="25" t="s">
@@ -13699,14 +13699,14 @@
         <v>147</v>
       </c>
       <c r="C153" s="25" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="25"/>
       <c r="F153" s="25"/>
       <c r="G153" s="60"/>
       <c r="H153" s="84" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I153" s="47"/>
       <c r="J153" s="26"/>
@@ -13723,7 +13723,7 @@
         <v>404</v>
       </c>
       <c r="S153" s="16" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="T153" s="25"/>
       <c r="U153" s="25"/>
@@ -13748,7 +13748,7 @@
         <v>0</v>
       </c>
       <c r="D154" s="25" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E154" s="25">
         <v>20</v>
@@ -13758,7 +13758,7 @@
       </c>
       <c r="G154" s="60"/>
       <c r="H154" s="29" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I154" s="29"/>
       <c r="J154" s="26"/>
@@ -13775,7 +13775,7 @@
         <v>404</v>
       </c>
       <c r="S154" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="T154" s="25"/>
       <c r="U154" s="25"/>
@@ -13817,7 +13817,7 @@
       <c r="M155" s="17"/>
       <c r="N155" s="17"/>
       <c r="O155" s="20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="P155" s="41">
         <v>2</v>
@@ -13829,7 +13829,7 @@
         <v>404</v>
       </c>
       <c r="S155" s="16" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="T155" s="25"/>
       <c r="U155" s="25" t="s">
@@ -13868,7 +13868,7 @@
       <c r="L156" s="30"/>
       <c r="M156" s="17"/>
       <c r="N156" s="17" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="O156" s="20"/>
       <c r="P156" s="41"/>
@@ -13879,7 +13879,7 @@
         <v>404</v>
       </c>
       <c r="S156" s="16" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="T156" s="25"/>
       <c r="U156" s="25"/>
@@ -13892,7 +13892,7 @@
         <v>189</v>
       </c>
       <c r="Z156" s="48" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="157" spans="1:26" ht="27">
@@ -13900,7 +13900,7 @@
         <v>55900027</v>
       </c>
       <c r="B157" s="55" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C157" s="25" t="s">
         <v>0</v>
@@ -13914,10 +13914,10 @@
       <c r="J157" s="26"/>
       <c r="K157" s="27"/>
       <c r="L157" s="30" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="M157" s="17" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="N157" s="17"/>
       <c r="O157" s="20"/>
@@ -13929,7 +13929,7 @@
         <v>404</v>
       </c>
       <c r="S157" s="16" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="T157" s="25"/>
       <c r="U157" s="25"/>
@@ -13958,7 +13958,7 @@
       <c r="F158" s="44"/>
       <c r="G158" s="60"/>
       <c r="H158" s="84" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="I158" s="47"/>
       <c r="J158" s="26"/>
@@ -13975,7 +13975,7 @@
         <v>404</v>
       </c>
       <c r="S158" s="16" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="T158" s="25"/>
       <c r="U158" s="25"/>
@@ -14002,7 +14002,7 @@
       <c r="F159" s="25"/>
       <c r="G159" s="60"/>
       <c r="H159" s="84" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I159" s="47"/>
       <c r="J159" s="26"/>
@@ -14019,7 +14019,7 @@
         <v>404</v>
       </c>
       <c r="S159" s="16" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="T159" s="25"/>
       <c r="U159" s="25"/>
@@ -14029,7 +14029,7 @@
         <v>15</v>
       </c>
       <c r="Y159" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="Z159" s="48"/>
     </row>
@@ -14050,12 +14050,12 @@
       <c r="H160" s="84"/>
       <c r="I160" s="47"/>
       <c r="J160" s="26" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="K160" s="27"/>
       <c r="L160" s="30"/>
       <c r="M160" s="17" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="N160" s="17"/>
       <c r="O160" s="20"/>
@@ -14088,7 +14088,7 @@
         <v>55900031</v>
       </c>
       <c r="B161" s="55" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C161" s="25" t="s">
         <v>0</v>
@@ -14098,7 +14098,7 @@
       <c r="F161" s="25"/>
       <c r="G161" s="60"/>
       <c r="H161" s="84" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="I161" s="47"/>
       <c r="J161" s="26"/>
@@ -14115,7 +14115,7 @@
         <v>404</v>
       </c>
       <c r="S161" s="16" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="T161" s="25"/>
       <c r="U161" s="25"/>
@@ -14125,7 +14125,7 @@
         <v>5</v>
       </c>
       <c r="Y161" s="25" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="Z161" s="48"/>
     </row>
@@ -14134,23 +14134,23 @@
         <v>55900032</v>
       </c>
       <c r="B162" s="55" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C162" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D162" s="25" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E162" s="25">
         <v>12</v>
       </c>
       <c r="F162" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G162" s="60"/>
       <c r="H162" s="97" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="I162" s="29"/>
       <c r="J162" s="26"/>
@@ -14167,11 +14167,11 @@
         <v>404</v>
       </c>
       <c r="S162" s="16" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="T162" s="25"/>
       <c r="U162" s="25" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="V162" s="25"/>
       <c r="W162" s="25"/>
@@ -14179,7 +14179,7 @@
         <v>20</v>
       </c>
       <c r="Y162" s="25" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="Z162" s="48"/>
     </row>
@@ -14188,7 +14188,7 @@
         <v>55900033</v>
       </c>
       <c r="B163" s="55" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C163" s="25" t="s">
         <v>0</v>
@@ -14200,11 +14200,11 @@
       <c r="H163" s="84"/>
       <c r="I163" s="47"/>
       <c r="J163" s="26" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="K163" s="27"/>
       <c r="L163" s="30" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="M163" s="17"/>
       <c r="N163" s="17"/>
@@ -14217,7 +14217,7 @@
         <v>404</v>
       </c>
       <c r="S163" s="16" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="T163" s="25"/>
       <c r="U163" s="25"/>
@@ -14227,7 +14227,7 @@
         <v>20</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Z163" s="48"/>
     </row>
@@ -14236,7 +14236,7 @@
         <v>55900034</v>
       </c>
       <c r="B164" s="55" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C164" s="25" t="s">
         <v>0</v>
@@ -14252,7 +14252,7 @@
       <c r="L164" s="30"/>
       <c r="M164" s="17"/>
       <c r="N164" s="17" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="O164" s="20"/>
       <c r="P164" s="41"/>
@@ -14263,7 +14263,7 @@
         <v>404</v>
       </c>
       <c r="S164" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25"/>
@@ -14273,7 +14273,7 @@
         <v>14</v>
       </c>
       <c r="Y164" s="25" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="Z164" s="48"/>
     </row>
@@ -14282,7 +14282,7 @@
         <v>55900035</v>
       </c>
       <c r="B165" s="55" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C165" s="25" t="s">
         <v>0</v>
@@ -14292,7 +14292,7 @@
       <c r="F165" s="25"/>
       <c r="G165" s="60"/>
       <c r="H165" s="84" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I165" s="47"/>
       <c r="J165" s="26"/>
@@ -14309,7 +14309,7 @@
         <v>404</v>
       </c>
       <c r="S165" s="16" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="T165" s="25"/>
       <c r="U165" s="25"/>
@@ -14319,7 +14319,7 @@
         <v>14</v>
       </c>
       <c r="Y165" s="25" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="Z165" s="48"/>
     </row>
@@ -14328,13 +14328,13 @@
         <v>55900036</v>
       </c>
       <c r="B166" s="55" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C166" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D166" s="25" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E166" s="25">
         <v>50</v>
@@ -14344,7 +14344,7 @@
       </c>
       <c r="G166" s="60"/>
       <c r="H166" s="97" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I166" s="29"/>
       <c r="J166" s="26"/>
@@ -14361,11 +14361,11 @@
         <v>404</v>
       </c>
       <c r="S166" s="16" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="T166" s="25"/>
       <c r="U166" s="25" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="V166" s="25"/>
       <c r="W166" s="25"/>
@@ -14373,7 +14373,7 @@
         <v>50</v>
       </c>
       <c r="Y166" s="25" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Z166" s="48"/>
     </row>
@@ -14382,13 +14382,13 @@
         <v>55900037</v>
       </c>
       <c r="B167" s="55" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D167" s="25" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E167" s="25">
         <v>15</v>
@@ -14398,7 +14398,7 @@
       </c>
       <c r="G167" s="60"/>
       <c r="H167" s="29" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="I167" s="29"/>
       <c r="J167" s="26"/>
@@ -14415,7 +14415,7 @@
         <v>404</v>
       </c>
       <c r="S167" s="10" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="T167" s="25"/>
       <c r="U167" s="25"/>
@@ -14425,7 +14425,7 @@
         <v>35</v>
       </c>
       <c r="Y167" s="25" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Z167" s="48"/>
     </row>
@@ -14434,13 +14434,13 @@
         <v>55900038</v>
       </c>
       <c r="B168" s="55" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C168" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D168" s="25" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E168" s="25">
         <v>15</v>
@@ -14450,7 +14450,7 @@
       </c>
       <c r="G168" s="60"/>
       <c r="H168" s="29" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I168" s="29"/>
       <c r="J168" s="26"/>
@@ -14467,21 +14467,21 @@
         <v>404</v>
       </c>
       <c r="S168" s="10" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="T168" s="25"/>
       <c r="U168" s="25" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="V168" s="25" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="W168" s="25"/>
       <c r="X168" s="25">
         <v>40</v>
       </c>
       <c r="Y168" s="25" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Z168" s="48"/>
     </row>
@@ -14493,7 +14493,7 @@
         <v>23</v>
       </c>
       <c r="C169" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D169" s="25"/>
       <c r="E169" s="25"/>
@@ -14532,7 +14532,7 @@
         <v>24</v>
       </c>
       <c r="Z169" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="170" spans="1:26" ht="36">
@@ -14543,7 +14543,7 @@
         <v>25</v>
       </c>
       <c r="C170" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D170" s="25"/>
       <c r="E170" s="25"/>
@@ -14582,7 +14582,7 @@
         <v>26</v>
       </c>
       <c r="Z170" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="171" spans="1:26" ht="36">
@@ -14593,7 +14593,7 @@
         <v>27</v>
       </c>
       <c r="C171" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D171" s="25"/>
       <c r="E171" s="25"/>
@@ -14632,7 +14632,7 @@
         <v>28</v>
       </c>
       <c r="Z171" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="172" spans="1:26" ht="36">
@@ -14643,7 +14643,7 @@
         <v>29</v>
       </c>
       <c r="C172" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D172" s="25"/>
       <c r="E172" s="25"/>
@@ -14682,7 +14682,7 @@
         <v>30</v>
       </c>
       <c r="Z172" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="173" spans="1:26" ht="36">
@@ -14693,7 +14693,7 @@
         <v>31</v>
       </c>
       <c r="C173" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D173" s="25"/>
       <c r="E173" s="25"/>
@@ -14732,7 +14732,7 @@
         <v>32</v>
       </c>
       <c r="Z173" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="174" spans="1:26" ht="36">
@@ -14743,7 +14743,7 @@
         <v>33</v>
       </c>
       <c r="C174" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D174" s="25"/>
       <c r="E174" s="25"/>
@@ -14782,7 +14782,7 @@
         <v>34</v>
       </c>
       <c r="Z174" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="175" spans="1:26" ht="36">
@@ -14793,7 +14793,7 @@
         <v>54</v>
       </c>
       <c r="C175" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D175" s="25"/>
       <c r="E175" s="25"/>
@@ -14832,7 +14832,7 @@
         <v>55</v>
       </c>
       <c r="Z175" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="176" spans="1:26" ht="36">
@@ -14843,7 +14843,7 @@
         <v>56</v>
       </c>
       <c r="C176" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D176" s="25"/>
       <c r="E176" s="25"/>
@@ -14882,7 +14882,7 @@
         <v>57</v>
       </c>
       <c r="Z176" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="177" spans="1:26" ht="36">
@@ -14893,7 +14893,7 @@
         <v>58</v>
       </c>
       <c r="C177" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D177" s="25"/>
       <c r="E177" s="25"/>
@@ -14932,7 +14932,7 @@
         <v>59</v>
       </c>
       <c r="Z177" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="178" spans="1:26" ht="36">
@@ -14943,7 +14943,7 @@
         <v>60</v>
       </c>
       <c r="C178" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D178" s="25"/>
       <c r="E178" s="25"/>
@@ -14982,7 +14982,7 @@
         <v>61</v>
       </c>
       <c r="Z178" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="179" spans="1:26" ht="36">
@@ -14993,7 +14993,7 @@
         <v>62</v>
       </c>
       <c r="C179" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D179" s="25"/>
       <c r="E179" s="25"/>
@@ -15032,7 +15032,7 @@
         <v>63</v>
       </c>
       <c r="Z179" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="180" spans="1:26" ht="36">
@@ -15043,7 +15043,7 @@
         <v>64</v>
       </c>
       <c r="C180" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D180" s="25"/>
       <c r="E180" s="25"/>
@@ -15082,7 +15082,7 @@
         <v>65</v>
       </c>
       <c r="Z180" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="181" spans="1:26" ht="24">
@@ -15090,17 +15090,17 @@
         <v>55990101</v>
       </c>
       <c r="B181" s="98" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C181" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D181" s="25"/>
       <c r="E181" s="25"/>
       <c r="F181" s="44"/>
       <c r="G181" s="60"/>
       <c r="H181" s="84" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="I181" s="47"/>
       <c r="J181" s="26"/>
@@ -15117,7 +15117,7 @@
         <v>237</v>
       </c>
       <c r="S181" s="49" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="T181" s="25"/>
       <c r="U181" s="25"/>
@@ -15130,7 +15130,7 @@
         <v>107</v>
       </c>
       <c r="Z181" s="48" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="182" spans="1:26" ht="24">
@@ -15138,10 +15138,10 @@
         <v>55990102</v>
       </c>
       <c r="B182" s="98" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C182" s="25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D182" s="25"/>
       <c r="E182" s="25"/>
@@ -15150,11 +15150,11 @@
       <c r="H182" s="84"/>
       <c r="I182" s="47"/>
       <c r="J182" s="26" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="K182" s="27"/>
       <c r="L182" s="30" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="M182" s="17"/>
       <c r="N182" s="17"/>
@@ -15167,7 +15167,7 @@
         <v>237</v>
       </c>
       <c r="S182" s="16" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="T182" s="25"/>
       <c r="U182" s="25"/>
@@ -15177,10 +15177,10 @@
         <v>25</v>
       </c>
       <c r="Y182" s="25" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="Z182" s="48" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="183" spans="1:26" ht="60">
@@ -15188,30 +15188,30 @@
         <v>55990103</v>
       </c>
       <c r="B183" s="98" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C183" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D183" s="25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E183" s="25">
         <v>10</v>
       </c>
       <c r="F183" s="44" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G183" s="60"/>
       <c r="H183" s="84"/>
       <c r="I183" s="47"/>
       <c r="J183" s="26" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K183" s="27"/>
       <c r="L183" s="30"/>
       <c r="M183" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="N183" s="17"/>
       <c r="O183" s="20"/>
@@ -15223,24 +15223,24 @@
         <v>237</v>
       </c>
       <c r="S183" s="16" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="T183" s="25"/>
       <c r="U183" s="25" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="V183" s="25" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="W183" s="25"/>
       <c r="X183" s="25">
         <v>35</v>
       </c>
       <c r="Y183" s="25" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="Z183" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="184" spans="1:26" ht="60">
@@ -15248,30 +15248,30 @@
         <v>55990104</v>
       </c>
       <c r="B184" s="98" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C184" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D184" s="25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E184" s="25">
         <v>20</v>
       </c>
       <c r="F184" s="44" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G184" s="60"/>
       <c r="H184" s="84"/>
       <c r="I184" s="47"/>
       <c r="J184" s="26" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="K184" s="27"/>
       <c r="L184" s="30"/>
       <c r="M184" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="N184" s="17"/>
       <c r="O184" s="20"/>
@@ -15283,24 +15283,24 @@
         <v>237</v>
       </c>
       <c r="S184" s="16" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="T184" s="25"/>
       <c r="U184" s="25" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="V184" s="25" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="W184" s="25"/>
       <c r="X184" s="25">
         <v>50</v>
       </c>
       <c r="Y184" s="25" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="Z184" s="48" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
   </sheetData>
@@ -15885,7 +15885,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -15893,7 +15893,7 @@
         <v>373</v>
       </c>
       <c r="B32" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -15901,7 +15901,7 @@
         <v>390</v>
       </c>
       <c r="B33" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
close #53 fix 2 monster big boss
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="993">
   <si>
     <t>特殊</t>
   </si>
@@ -3732,31 +3732,47 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>s.CureRandomAlien(0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合回复一个己方生命最低的怪物30%生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lvfeng</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿风</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.SummonRandomAttr(2,2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每2回合在自己周围召唤一个随机风属性怪物</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>灭绝</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>miejue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position))if(s.Id!=o.Id)o.SuddenDeath();s.Owner.DeleteAllCard();</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s.CureRandomAlien(0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合回复一个己方生命最低的怪物30%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lvfeng</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>绿风</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.SummonRandomAttr(2,2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每2回合在自己周围召唤一个随机风属性怪物</t>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.SuddenDeath();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时杀死最近的敌人</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5924,8 +5940,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z191" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:Z191"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z192" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:Z192"/>
   <sortState ref="A4:Z186">
     <sortCondition ref="A3:A186"/>
   </sortState>
@@ -6248,14 +6264,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z191"/>
+  <dimension ref="A1:Z192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J172" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="O174" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="S175" sqref="S175"/>
+      <selection pane="bottomRight" activeCell="R176" sqref="R176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -14789,7 +14805,7 @@
       </c>
       <c r="G172" s="60"/>
       <c r="H172" s="29" t="s">
-        <v>982</v>
+        <v>990</v>
       </c>
       <c r="I172" s="29"/>
       <c r="J172" s="26"/>
@@ -14890,7 +14906,7 @@
       <c r="M174" s="17"/>
       <c r="N174" s="17"/>
       <c r="O174" s="20" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="P174" s="41">
         <v>1</v>
@@ -14902,7 +14918,7 @@
         <v>403</v>
       </c>
       <c r="S174" s="10" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="T174" s="25"/>
       <c r="U174" s="25"/>
@@ -14921,7 +14937,7 @@
         <v>55900044</v>
       </c>
       <c r="B175" s="55" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C175" s="25" t="s">
         <v>0</v>
@@ -14938,7 +14954,7 @@
       <c r="M175" s="17"/>
       <c r="N175" s="17"/>
       <c r="O175" s="20" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="P175" s="41">
         <v>2</v>
@@ -14950,7 +14966,7 @@
         <v>403</v>
       </c>
       <c r="S175" s="10" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="T175" s="25"/>
       <c r="U175" s="25"/>
@@ -14960,33 +14976,37 @@
         <v>40</v>
       </c>
       <c r="Y175" s="25" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="Z175" s="48"/>
     </row>
-    <row r="176" spans="1:26" ht="36">
-      <c r="A176" s="98">
-        <v>55990001</v>
-      </c>
-      <c r="B176" s="98" t="s">
-        <v>23</v>
+    <row r="176" spans="1:26" ht="84">
+      <c r="A176" s="55">
+        <v>55900045</v>
+      </c>
+      <c r="B176" s="55" t="s">
+        <v>988</v>
       </c>
       <c r="C176" s="25" t="s">
-        <v>814</v>
-      </c>
-      <c r="D176" s="25"/>
-      <c r="E176" s="25"/>
-      <c r="F176" s="25"/>
+        <v>0</v>
+      </c>
+      <c r="D176" s="25" t="s">
+        <v>933</v>
+      </c>
+      <c r="E176" s="25">
+        <v>100</v>
+      </c>
+      <c r="F176" s="44" t="s">
+        <v>237</v>
+      </c>
       <c r="G176" s="60"/>
-      <c r="H176" s="97"/>
+      <c r="H176" s="97" t="s">
+        <v>991</v>
+      </c>
       <c r="I176" s="29"/>
-      <c r="J176" s="26" t="s">
-        <v>407</v>
-      </c>
+      <c r="J176" s="26"/>
       <c r="K176" s="27"/>
-      <c r="L176" s="30" t="s">
-        <v>280</v>
-      </c>
+      <c r="L176" s="30"/>
       <c r="M176" s="17"/>
       <c r="N176" s="17"/>
       <c r="O176" s="20"/>
@@ -14995,31 +15015,29 @@
         <v>242</v>
       </c>
       <c r="R176" s="44" t="s">
-        <v>237</v>
-      </c>
-      <c r="S176" s="16" t="s">
-        <v>396</v>
+        <v>403</v>
+      </c>
+      <c r="S176" s="10" t="s">
+        <v>992</v>
       </c>
       <c r="T176" s="25"/>
       <c r="U176" s="25"/>
       <c r="V176" s="25"/>
       <c r="W176" s="25"/>
       <c r="X176" s="25">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="Y176" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z176" s="48" t="s">
-        <v>812</v>
-      </c>
+        <v>989</v>
+      </c>
+      <c r="Z176" s="48"/>
     </row>
     <row r="177" spans="1:26" ht="36">
       <c r="A177" s="98">
-        <v>55990002</v>
+        <v>55990001</v>
       </c>
       <c r="B177" s="98" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C177" s="25" t="s">
         <v>814</v>
@@ -15031,7 +15049,7 @@
       <c r="H177" s="97"/>
       <c r="I177" s="29"/>
       <c r="J177" s="26" t="s">
-        <v>268</v>
+        <v>407</v>
       </c>
       <c r="K177" s="27"/>
       <c r="L177" s="30" t="s">
@@ -15047,8 +15065,8 @@
       <c r="R177" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S177" s="49" t="s">
-        <v>397</v>
+      <c r="S177" s="16" t="s">
+        <v>396</v>
       </c>
       <c r="T177" s="25"/>
       <c r="U177" s="25"/>
@@ -15058,7 +15076,7 @@
         <v>15</v>
       </c>
       <c r="Y177" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Z177" s="48" t="s">
         <v>812</v>
@@ -15066,10 +15084,10 @@
     </row>
     <row r="178" spans="1:26" ht="36">
       <c r="A178" s="98">
-        <v>55990003</v>
+        <v>55990002</v>
       </c>
       <c r="B178" s="98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C178" s="25" t="s">
         <v>814</v>
@@ -15081,7 +15099,7 @@
       <c r="H178" s="97"/>
       <c r="I178" s="29"/>
       <c r="J178" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K178" s="27"/>
       <c r="L178" s="30" t="s">
@@ -15098,7 +15116,7 @@
         <v>237</v>
       </c>
       <c r="S178" s="49" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="T178" s="25"/>
       <c r="U178" s="25"/>
@@ -15108,7 +15126,7 @@
         <v>15</v>
       </c>
       <c r="Y178" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Z178" s="48" t="s">
         <v>812</v>
@@ -15116,10 +15134,10 @@
     </row>
     <row r="179" spans="1:26" ht="36">
       <c r="A179" s="98">
-        <v>55990004</v>
+        <v>55990003</v>
       </c>
       <c r="B179" s="98" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C179" s="25" t="s">
         <v>814</v>
@@ -15131,7 +15149,7 @@
       <c r="H179" s="97"/>
       <c r="I179" s="29"/>
       <c r="J179" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K179" s="27"/>
       <c r="L179" s="30" t="s">
@@ -15148,7 +15166,7 @@
         <v>237</v>
       </c>
       <c r="S179" s="49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="T179" s="25"/>
       <c r="U179" s="25"/>
@@ -15158,7 +15176,7 @@
         <v>15</v>
       </c>
       <c r="Y179" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z179" s="48" t="s">
         <v>812</v>
@@ -15166,10 +15184,10 @@
     </row>
     <row r="180" spans="1:26" ht="36">
       <c r="A180" s="98">
-        <v>55990005</v>
+        <v>55990004</v>
       </c>
       <c r="B180" s="98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C180" s="25" t="s">
         <v>814</v>
@@ -15181,7 +15199,7 @@
       <c r="H180" s="97"/>
       <c r="I180" s="29"/>
       <c r="J180" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K180" s="27"/>
       <c r="L180" s="30" t="s">
@@ -15198,7 +15216,7 @@
         <v>237</v>
       </c>
       <c r="S180" s="49" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="T180" s="25"/>
       <c r="U180" s="25"/>
@@ -15208,7 +15226,7 @@
         <v>15</v>
       </c>
       <c r="Y180" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Z180" s="48" t="s">
         <v>812</v>
@@ -15216,10 +15234,10 @@
     </row>
     <row r="181" spans="1:26" ht="36">
       <c r="A181" s="98">
-        <v>55990006</v>
+        <v>55990005</v>
       </c>
       <c r="B181" s="98" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C181" s="25" t="s">
         <v>814</v>
@@ -15231,7 +15249,7 @@
       <c r="H181" s="97"/>
       <c r="I181" s="29"/>
       <c r="J181" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K181" s="27"/>
       <c r="L181" s="30" t="s">
@@ -15248,7 +15266,7 @@
         <v>237</v>
       </c>
       <c r="S181" s="49" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T181" s="25"/>
       <c r="U181" s="25"/>
@@ -15258,7 +15276,7 @@
         <v>15</v>
       </c>
       <c r="Y181" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Z181" s="48" t="s">
         <v>812</v>
@@ -15266,10 +15284,10 @@
     </row>
     <row r="182" spans="1:26" ht="36">
       <c r="A182" s="98">
-        <v>55990011</v>
+        <v>55990006</v>
       </c>
       <c r="B182" s="98" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C182" s="25" t="s">
         <v>814</v>
@@ -15281,24 +15299,24 @@
       <c r="H182" s="97"/>
       <c r="I182" s="29"/>
       <c r="J182" s="26" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="K182" s="27"/>
       <c r="L182" s="30" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="M182" s="17"/>
       <c r="N182" s="17"/>
       <c r="O182" s="20"/>
       <c r="P182" s="41"/>
       <c r="Q182" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="R182" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S182" s="16" t="s">
-        <v>284</v>
+      <c r="S182" s="49" t="s">
+        <v>411</v>
       </c>
       <c r="T182" s="25"/>
       <c r="U182" s="25"/>
@@ -15308,7 +15326,7 @@
         <v>15</v>
       </c>
       <c r="Y182" s="25" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="Z182" s="48" t="s">
         <v>812</v>
@@ -15316,10 +15334,10 @@
     </row>
     <row r="183" spans="1:26" ht="36">
       <c r="A183" s="98">
-        <v>55990012</v>
+        <v>55990011</v>
       </c>
       <c r="B183" s="98" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C183" s="25" t="s">
         <v>814</v>
@@ -15331,7 +15349,7 @@
       <c r="H183" s="97"/>
       <c r="I183" s="29"/>
       <c r="J183" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K183" s="27"/>
       <c r="L183" s="30" t="s">
@@ -15348,7 +15366,7 @@
         <v>237</v>
       </c>
       <c r="S183" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T183" s="25"/>
       <c r="U183" s="25"/>
@@ -15358,7 +15376,7 @@
         <v>15</v>
       </c>
       <c r="Y183" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Z183" s="48" t="s">
         <v>812</v>
@@ -15366,10 +15384,10 @@
     </row>
     <row r="184" spans="1:26" ht="36">
       <c r="A184" s="98">
-        <v>55990013</v>
+        <v>55990012</v>
       </c>
       <c r="B184" s="98" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C184" s="25" t="s">
         <v>814</v>
@@ -15381,7 +15399,7 @@
       <c r="H184" s="97"/>
       <c r="I184" s="29"/>
       <c r="J184" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K184" s="27"/>
       <c r="L184" s="30" t="s">
@@ -15398,7 +15416,7 @@
         <v>237</v>
       </c>
       <c r="S184" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T184" s="25"/>
       <c r="U184" s="25"/>
@@ -15408,7 +15426,7 @@
         <v>15</v>
       </c>
       <c r="Y184" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z184" s="48" t="s">
         <v>812</v>
@@ -15416,10 +15434,10 @@
     </row>
     <row r="185" spans="1:26" ht="36">
       <c r="A185" s="98">
-        <v>55990014</v>
+        <v>55990013</v>
       </c>
       <c r="B185" s="98" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C185" s="25" t="s">
         <v>814</v>
@@ -15431,7 +15449,7 @@
       <c r="H185" s="97"/>
       <c r="I185" s="29"/>
       <c r="J185" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K185" s="27"/>
       <c r="L185" s="30" t="s">
@@ -15448,7 +15466,7 @@
         <v>237</v>
       </c>
       <c r="S185" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T185" s="25"/>
       <c r="U185" s="25"/>
@@ -15458,7 +15476,7 @@
         <v>15</v>
       </c>
       <c r="Y185" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z185" s="48" t="s">
         <v>812</v>
@@ -15466,10 +15484,10 @@
     </row>
     <row r="186" spans="1:26" ht="36">
       <c r="A186" s="98">
-        <v>55990015</v>
+        <v>55990014</v>
       </c>
       <c r="B186" s="98" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C186" s="25" t="s">
         <v>814</v>
@@ -15481,7 +15499,7 @@
       <c r="H186" s="97"/>
       <c r="I186" s="29"/>
       <c r="J186" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K186" s="27"/>
       <c r="L186" s="30" t="s">
@@ -15498,7 +15516,7 @@
         <v>237</v>
       </c>
       <c r="S186" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T186" s="25"/>
       <c r="U186" s="25"/>
@@ -15508,7 +15526,7 @@
         <v>15</v>
       </c>
       <c r="Y186" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Z186" s="48" t="s">
         <v>812</v>
@@ -15516,10 +15534,10 @@
     </row>
     <row r="187" spans="1:26" ht="36">
       <c r="A187" s="98">
-        <v>55990016</v>
+        <v>55990015</v>
       </c>
       <c r="B187" s="98" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C187" s="25" t="s">
         <v>814</v>
@@ -15528,10 +15546,10 @@
       <c r="E187" s="25"/>
       <c r="F187" s="25"/>
       <c r="G187" s="60"/>
-      <c r="H187" s="84"/>
-      <c r="I187" s="47"/>
+      <c r="H187" s="97"/>
+      <c r="I187" s="29"/>
       <c r="J187" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K187" s="27"/>
       <c r="L187" s="30" t="s">
@@ -15548,7 +15566,7 @@
         <v>237</v>
       </c>
       <c r="S187" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T187" s="25"/>
       <c r="U187" s="25"/>
@@ -15558,33 +15576,35 @@
         <v>15</v>
       </c>
       <c r="Y187" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Z187" s="48" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="188" spans="1:26" ht="24">
+    <row r="188" spans="1:26" ht="36">
       <c r="A188" s="98">
-        <v>55990101</v>
+        <v>55990016</v>
       </c>
       <c r="B188" s="98" t="s">
-        <v>815</v>
+        <v>64</v>
       </c>
       <c r="C188" s="25" t="s">
         <v>814</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25"/>
-      <c r="F188" s="44"/>
+      <c r="F188" s="25"/>
       <c r="G188" s="60"/>
-      <c r="H188" s="84" t="s">
-        <v>816</v>
-      </c>
+      <c r="H188" s="84"/>
       <c r="I188" s="47"/>
-      <c r="J188" s="26"/>
+      <c r="J188" s="26" t="s">
+        <v>295</v>
+      </c>
       <c r="K188" s="27"/>
-      <c r="L188" s="30"/>
+      <c r="L188" s="30" t="s">
+        <v>283</v>
+      </c>
       <c r="M188" s="17"/>
       <c r="N188" s="17"/>
       <c r="O188" s="20"/>
@@ -15595,103 +15615,95 @@
       <c r="R188" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S188" s="49" t="s">
-        <v>817</v>
+      <c r="S188" s="16" t="s">
+        <v>289</v>
       </c>
       <c r="T188" s="25"/>
       <c r="U188" s="25"/>
       <c r="V188" s="25"/>
       <c r="W188" s="25"/>
       <c r="X188" s="25">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Y188" s="25" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="Z188" s="48" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
     </row>
     <row r="189" spans="1:26" ht="24">
       <c r="A189" s="98">
-        <v>55990102</v>
+        <v>55990101</v>
       </c>
       <c r="B189" s="98" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="C189" s="25" t="s">
         <v>814</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25"/>
-      <c r="F189" s="25"/>
+      <c r="F189" s="44"/>
       <c r="G189" s="60"/>
-      <c r="H189" s="84"/>
+      <c r="H189" s="84" t="s">
+        <v>816</v>
+      </c>
       <c r="I189" s="47"/>
-      <c r="J189" s="26" t="s">
-        <v>819</v>
-      </c>
+      <c r="J189" s="26"/>
       <c r="K189" s="27"/>
-      <c r="L189" s="30" t="s">
-        <v>822</v>
-      </c>
+      <c r="L189" s="30"/>
       <c r="M189" s="17"/>
       <c r="N189" s="17"/>
       <c r="O189" s="20"/>
       <c r="P189" s="41"/>
       <c r="Q189" s="46" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="R189" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S189" s="16" t="s">
-        <v>821</v>
+      <c r="S189" s="49" t="s">
+        <v>817</v>
       </c>
       <c r="T189" s="25"/>
       <c r="U189" s="25"/>
       <c r="V189" s="25"/>
       <c r="W189" s="25"/>
       <c r="X189" s="25">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Y189" s="25" t="s">
-        <v>825</v>
+        <v>107</v>
       </c>
       <c r="Z189" s="48" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="190" spans="1:26" ht="60">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="190" spans="1:26" ht="24">
       <c r="A190" s="98">
-        <v>55990103</v>
+        <v>55990102</v>
       </c>
       <c r="B190" s="98" t="s">
-        <v>831</v>
+        <v>820</v>
       </c>
       <c r="C190" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D190" s="25" t="s">
-        <v>454</v>
-      </c>
-      <c r="E190" s="25">
-        <v>10</v>
-      </c>
-      <c r="F190" s="44" t="s">
-        <v>464</v>
-      </c>
+        <v>814</v>
+      </c>
+      <c r="D190" s="25"/>
+      <c r="E190" s="25"/>
+      <c r="F190" s="25"/>
       <c r="G190" s="60"/>
       <c r="H190" s="84"/>
       <c r="I190" s="47"/>
       <c r="J190" s="26" t="s">
-        <v>672</v>
+        <v>819</v>
       </c>
       <c r="K190" s="27"/>
-      <c r="L190" s="30"/>
-      <c r="M190" s="17" t="s">
-        <v>584</v>
-      </c>
+      <c r="L190" s="30" t="s">
+        <v>822</v>
+      </c>
+      <c r="M190" s="17"/>
       <c r="N190" s="17"/>
       <c r="O190" s="20"/>
       <c r="P190" s="41"/>
@@ -15702,32 +15714,28 @@
         <v>237</v>
       </c>
       <c r="S190" s="16" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
       <c r="T190" s="25"/>
-      <c r="U190" s="25" t="s">
-        <v>841</v>
-      </c>
-      <c r="V190" s="25" t="s">
-        <v>841</v>
-      </c>
+      <c r="U190" s="25"/>
+      <c r="V190" s="25"/>
       <c r="W190" s="25"/>
       <c r="X190" s="25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Y190" s="25" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="Z190" s="48" t="s">
-        <v>832</v>
+        <v>812</v>
       </c>
     </row>
     <row r="191" spans="1:26" ht="60">
       <c r="A191" s="98">
-        <v>55990104</v>
+        <v>55990103</v>
       </c>
       <c r="B191" s="98" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="C191" s="25" t="s">
         <v>97</v>
@@ -15736,7 +15744,7 @@
         <v>454</v>
       </c>
       <c r="E191" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F191" s="44" t="s">
         <v>464</v>
@@ -15745,7 +15753,7 @@
       <c r="H191" s="84"/>
       <c r="I191" s="47"/>
       <c r="J191" s="26" t="s">
-        <v>837</v>
+        <v>672</v>
       </c>
       <c r="K191" s="27"/>
       <c r="L191" s="30"/>
@@ -15762,7 +15770,7 @@
         <v>237</v>
       </c>
       <c r="S191" s="16" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="T191" s="25"/>
       <c r="U191" s="25" t="s">
@@ -15773,12 +15781,72 @@
       </c>
       <c r="W191" s="25"/>
       <c r="X191" s="25">
+        <v>35</v>
+      </c>
+      <c r="Y191" s="25" t="s">
+        <v>833</v>
+      </c>
+      <c r="Z191" s="48" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="192" spans="1:26" ht="60">
+      <c r="A192" s="98">
+        <v>55990104</v>
+      </c>
+      <c r="B192" s="98" t="s">
+        <v>838</v>
+      </c>
+      <c r="C192" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D192" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="E192" s="25">
+        <v>20</v>
+      </c>
+      <c r="F192" s="44" t="s">
+        <v>464</v>
+      </c>
+      <c r="G192" s="60"/>
+      <c r="H192" s="84"/>
+      <c r="I192" s="47"/>
+      <c r="J192" s="26" t="s">
+        <v>837</v>
+      </c>
+      <c r="K192" s="27"/>
+      <c r="L192" s="30"/>
+      <c r="M192" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="N192" s="17"/>
+      <c r="O192" s="20"/>
+      <c r="P192" s="41"/>
+      <c r="Q192" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="R192" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="S192" s="16" t="s">
+        <v>836</v>
+      </c>
+      <c r="T192" s="25"/>
+      <c r="U192" s="25" t="s">
+        <v>841</v>
+      </c>
+      <c r="V192" s="25" t="s">
+        <v>841</v>
+      </c>
+      <c r="W192" s="25"/>
+      <c r="X192" s="25">
         <v>50</v>
       </c>
-      <c r="Y191" s="25" t="s">
+      <c r="Y192" s="25" t="s">
         <v>835</v>
       </c>
-      <c r="Z191" s="48" t="s">
+      <c r="Z192" s="48" t="s">
         <v>832</v>
       </c>
     </row>

</xml_diff>

<commit_message>
close #49 revive opponent's monster can rebel it. tomb target spell can distinguish friend and enemy
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="7" r:id="rId1"/>
@@ -3609,10 +3609,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonsterGhost(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)){s.Map.ReviveUnit(o,(int)(o.MaxHp.Source/2));}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>NEA</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3773,6 +3769,10 @@
   </si>
   <si>
     <t>召唤时杀死最近的敌人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonsterGhost(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)){s.Map.ReviveUnit(s.Owner,o,(int)(o.MaxHp.Source/2));}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6267,34 +6267,34 @@
   <dimension ref="A1:Z192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="O174" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="H169" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="R176" sqref="R176"/>
+      <selection pane="bottomRight" activeCell="M169" sqref="M169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="7" width="7.25" customWidth="1"/>
-    <col min="8" max="8" width="21.25" customWidth="1"/>
-    <col min="9" max="9" width="12.875" customWidth="1"/>
-    <col min="10" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="14" width="22.25" customWidth="1"/>
-    <col min="15" max="15" width="14.875" customWidth="1"/>
-    <col min="16" max="16" width="8.5" customWidth="1"/>
-    <col min="17" max="17" width="7.375" customWidth="1"/>
-    <col min="18" max="18" width="6.375" customWidth="1"/>
-    <col min="19" max="19" width="23.5" customWidth="1"/>
-    <col min="20" max="20" width="8.75" customWidth="1"/>
-    <col min="21" max="23" width="7.625" customWidth="1"/>
-    <col min="24" max="24" width="7.125" customWidth="1"/>
+    <col min="3" max="7" width="7.21875" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="14" width="22.21875" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" customWidth="1"/>
+    <col min="16" max="16" width="8.44140625" customWidth="1"/>
+    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" customWidth="1"/>
+    <col min="19" max="19" width="23.44140625" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" customWidth="1"/>
+    <col min="21" max="23" width="7.6640625" customWidth="1"/>
+    <col min="24" max="24" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="55.5">
+    <row r="1" spans="1:26" ht="58.8">
       <c r="A1" s="6" t="s">
         <v>230</v>
       </c>
@@ -6582,7 +6582,7 @@
       </c>
       <c r="Z4" s="39"/>
     </row>
-    <row r="5" spans="1:26" ht="36">
+    <row r="5" spans="1:26" ht="48">
       <c r="A5" s="51">
         <v>55100002</v>
       </c>
@@ -6632,7 +6632,7 @@
       </c>
       <c r="Z5" s="37"/>
     </row>
-    <row r="6" spans="1:26" ht="36">
+    <row r="6" spans="1:26" ht="48">
       <c r="A6" s="51">
         <v>55100003</v>
       </c>
@@ -6776,7 +6776,7 @@
       </c>
       <c r="Z8" s="37"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="24">
       <c r="A9" s="51">
         <v>55100006</v>
       </c>
@@ -6822,7 +6822,7 @@
       </c>
       <c r="Z9" s="70"/>
     </row>
-    <row r="10" spans="1:26" ht="60">
+    <row r="10" spans="1:26" ht="72">
       <c r="A10" s="51">
         <v>55100007</v>
       </c>
@@ -7020,7 +7020,7 @@
       </c>
       <c r="Z13" s="37"/>
     </row>
-    <row r="14" spans="1:26" ht="48">
+    <row r="14" spans="1:26" ht="60">
       <c r="A14" s="51">
         <v>55100011</v>
       </c>
@@ -7083,7 +7083,7 @@
       <c r="F15" s="43"/>
       <c r="G15" s="59"/>
       <c r="H15" s="29" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="I15" s="29" t="s">
         <v>340</v>
@@ -7212,7 +7212,7 @@
       </c>
       <c r="Z17" s="37"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" ht="24">
       <c r="A18" s="51">
         <v>55100015</v>
       </c>
@@ -7398,7 +7398,7 @@
       </c>
       <c r="Z21" s="37"/>
     </row>
-    <row r="22" spans="1:26" ht="24">
+    <row r="22" spans="1:26" ht="36">
       <c r="A22" s="75">
         <v>55110004</v>
       </c>
@@ -7444,7 +7444,7 @@
       </c>
       <c r="Z22" s="37"/>
     </row>
-    <row r="23" spans="1:26" ht="24">
+    <row r="23" spans="1:26" ht="36">
       <c r="A23" s="75">
         <v>55110005</v>
       </c>
@@ -7492,7 +7492,7 @@
       </c>
       <c r="Z23" s="37"/>
     </row>
-    <row r="24" spans="1:26" ht="24">
+    <row r="24" spans="1:26" ht="36">
       <c r="A24" s="75">
         <v>55110006</v>
       </c>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="Z24" s="48"/>
     </row>
-    <row r="25" spans="1:26" ht="24">
+    <row r="25" spans="1:26" ht="36">
       <c r="A25" s="75">
         <v>55110007</v>
       </c>
@@ -7680,7 +7680,7 @@
       </c>
       <c r="Z27" s="37"/>
     </row>
-    <row r="28" spans="1:26" ht="24">
+    <row r="28" spans="1:26" ht="36">
       <c r="A28" s="75">
         <v>55110010</v>
       </c>
@@ -7728,7 +7728,7 @@
       </c>
       <c r="Z28" s="37"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" ht="24">
       <c r="A29" s="75">
         <v>55110011</v>
       </c>
@@ -7776,7 +7776,7 @@
       </c>
       <c r="Z29" s="37"/>
     </row>
-    <row r="30" spans="1:26" ht="24">
+    <row r="30" spans="1:26" ht="36">
       <c r="A30" s="75">
         <v>55110012</v>
       </c>
@@ -7822,7 +7822,7 @@
       </c>
       <c r="Z30" s="37"/>
     </row>
-    <row r="31" spans="1:26" ht="24">
+    <row r="31" spans="1:26" ht="36">
       <c r="A31" s="75">
         <v>55110013</v>
       </c>
@@ -7872,7 +7872,7 @@
       </c>
       <c r="Z31" s="39"/>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" ht="24">
       <c r="A32" s="75">
         <v>55110014</v>
       </c>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="Z32" s="37"/>
     </row>
-    <row r="33" spans="1:26" ht="24">
+    <row r="33" spans="1:26" ht="36">
       <c r="A33" s="75">
         <v>55110015</v>
       </c>
@@ -8014,7 +8014,7 @@
       </c>
       <c r="Z34" s="48"/>
     </row>
-    <row r="35" spans="1:26" ht="36">
+    <row r="35" spans="1:26" ht="48">
       <c r="A35" s="75">
         <v>55110017</v>
       </c>
@@ -8060,7 +8060,7 @@
       </c>
       <c r="Z35" s="48"/>
     </row>
-    <row r="36" spans="1:26" ht="24">
+    <row r="36" spans="1:26" ht="36">
       <c r="A36" s="75">
         <v>55110018</v>
       </c>
@@ -8110,7 +8110,7 @@
       </c>
       <c r="Z36" s="37"/>
     </row>
-    <row r="37" spans="1:26" ht="27">
+    <row r="37" spans="1:26" ht="28.8">
       <c r="A37" s="75">
         <v>55110019</v>
       </c>
@@ -8160,7 +8160,7 @@
       </c>
       <c r="Z37" s="48"/>
     </row>
-    <row r="38" spans="1:26" ht="120">
+    <row r="38" spans="1:26" ht="132">
       <c r="A38" s="12">
         <v>55200001</v>
       </c>
@@ -8218,7 +8218,7 @@
       </c>
       <c r="Z38" s="48"/>
     </row>
-    <row r="39" spans="1:26" ht="84">
+    <row r="39" spans="1:26" ht="108">
       <c r="A39" s="73">
         <v>55200002</v>
       </c>
@@ -8272,7 +8272,7 @@
       </c>
       <c r="Z39" s="39"/>
     </row>
-    <row r="40" spans="1:26" ht="96">
+    <row r="40" spans="1:26" ht="108">
       <c r="A40" s="12">
         <v>55200003</v>
       </c>
@@ -8326,7 +8326,7 @@
       </c>
       <c r="Z40" s="25"/>
     </row>
-    <row r="41" spans="1:26" ht="120">
+    <row r="41" spans="1:26" ht="132">
       <c r="A41" s="73">
         <v>55200004</v>
       </c>
@@ -8382,7 +8382,7 @@
       </c>
       <c r="Z41" s="96"/>
     </row>
-    <row r="42" spans="1:26" ht="108">
+    <row r="42" spans="1:26" ht="132">
       <c r="A42" s="12">
         <v>55200005</v>
       </c>
@@ -8500,7 +8500,7 @@
       </c>
       <c r="Z43" s="37"/>
     </row>
-    <row r="44" spans="1:26" ht="72">
+    <row r="44" spans="1:26" ht="84">
       <c r="A44" s="12">
         <v>55200007</v>
       </c>
@@ -8631,7 +8631,7 @@
         <v>97</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="43" t="s">
@@ -8678,7 +8678,7 @@
       </c>
       <c r="Z46" s="37"/>
     </row>
-    <row r="47" spans="1:26" ht="84">
+    <row r="47" spans="1:26" ht="96">
       <c r="A47" s="12">
         <v>55200010</v>
       </c>
@@ -8732,7 +8732,7 @@
       </c>
       <c r="Z47" s="39"/>
     </row>
-    <row r="48" spans="1:26" ht="72">
+    <row r="48" spans="1:26" ht="96">
       <c r="A48" s="12">
         <v>55200011</v>
       </c>
@@ -8786,7 +8786,7 @@
       </c>
       <c r="Z48" s="96"/>
     </row>
-    <row r="49" spans="1:26" ht="72">
+    <row r="49" spans="1:26" ht="96">
       <c r="A49" s="12">
         <v>55200012</v>
       </c>
@@ -8842,7 +8842,7 @@
       </c>
       <c r="Z49" s="25"/>
     </row>
-    <row r="50" spans="1:26" ht="72">
+    <row r="50" spans="1:26" ht="96">
       <c r="A50" s="12">
         <v>55200013</v>
       </c>
@@ -8898,7 +8898,7 @@
       </c>
       <c r="Z50" s="25"/>
     </row>
-    <row r="51" spans="1:26" ht="72">
+    <row r="51" spans="1:26" ht="96">
       <c r="A51" s="12">
         <v>55200014</v>
       </c>
@@ -9194,7 +9194,7 @@
       </c>
       <c r="Z56" s="48"/>
     </row>
-    <row r="57" spans="1:26" ht="27">
+    <row r="57" spans="1:26" ht="28.8">
       <c r="A57" s="53">
         <v>55300006</v>
       </c>
@@ -9482,7 +9482,7 @@
       </c>
       <c r="Z62" s="48"/>
     </row>
-    <row r="63" spans="1:26">
+    <row r="63" spans="1:26" ht="24">
       <c r="A63" s="53">
         <v>55310002</v>
       </c>
@@ -9528,7 +9528,7 @@
       </c>
       <c r="Z63" s="37"/>
     </row>
-    <row r="64" spans="1:26">
+    <row r="64" spans="1:26" ht="24">
       <c r="A64" s="53">
         <v>55310003</v>
       </c>
@@ -9574,7 +9574,7 @@
       </c>
       <c r="Z64" s="37"/>
     </row>
-    <row r="65" spans="1:26" ht="27">
+    <row r="65" spans="1:26" ht="28.8">
       <c r="A65" s="54">
         <v>55400001</v>
       </c>
@@ -9624,7 +9624,7 @@
       </c>
       <c r="Z65" s="48"/>
     </row>
-    <row r="66" spans="1:26">
+    <row r="66" spans="1:26" ht="28.8">
       <c r="A66" s="54">
         <v>55400002</v>
       </c>
@@ -9676,7 +9676,7 @@
       </c>
       <c r="Z66" s="48"/>
     </row>
-    <row r="67" spans="1:26" ht="27">
+    <row r="67" spans="1:26" ht="28.8">
       <c r="A67" s="54">
         <v>55400003</v>
       </c>
@@ -9726,7 +9726,7 @@
       </c>
       <c r="Z67" s="48"/>
     </row>
-    <row r="68" spans="1:26" ht="27">
+    <row r="68" spans="1:26" ht="28.8">
       <c r="A68" s="54">
         <v>55400004</v>
       </c>
@@ -9776,7 +9776,7 @@
       </c>
       <c r="Z68" s="48"/>
     </row>
-    <row r="69" spans="1:26" ht="27">
+    <row r="69" spans="1:26" ht="28.8">
       <c r="A69" s="54">
         <v>55400005</v>
       </c>
@@ -9826,7 +9826,7 @@
       </c>
       <c r="Z69" s="48"/>
     </row>
-    <row r="70" spans="1:26" ht="27">
+    <row r="70" spans="1:26" ht="28.8">
       <c r="A70" s="54">
         <v>55400006</v>
       </c>
@@ -9876,18 +9876,18 @@
       </c>
       <c r="Z70" s="48"/>
     </row>
-    <row r="71" spans="1:26" ht="27">
+    <row r="71" spans="1:26" ht="28.8">
       <c r="A71" s="54">
         <v>55400007</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C71" s="25" t="s">
         <v>433</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="E71" s="25">
         <v>10</v>
@@ -9897,7 +9897,7 @@
       </c>
       <c r="G71" s="60"/>
       <c r="H71" s="47" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I71" s="47"/>
       <c r="J71" s="26"/>
@@ -9914,7 +9914,7 @@
         <v>237</v>
       </c>
       <c r="S71" s="16" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="T71" s="25"/>
       <c r="U71" s="25"/>
@@ -9924,11 +9924,11 @@
         <v>25</v>
       </c>
       <c r="Y71" s="25" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="Z71" s="48"/>
     </row>
-    <row r="72" spans="1:26" ht="27">
+    <row r="72" spans="1:26" ht="28.8">
       <c r="A72" s="54">
         <v>55410001</v>
       </c>
@@ -9976,7 +9976,7 @@
       </c>
       <c r="Z72" s="48"/>
     </row>
-    <row r="73" spans="1:26" ht="24">
+    <row r="73" spans="1:26" ht="36">
       <c r="A73" s="56">
         <v>55500001</v>
       </c>
@@ -10072,7 +10072,7 @@
       </c>
       <c r="Z74" s="48"/>
     </row>
-    <row r="75" spans="1:26" ht="24">
+    <row r="75" spans="1:26" ht="36">
       <c r="A75" s="56">
         <v>55500003</v>
       </c>
@@ -10120,7 +10120,7 @@
       </c>
       <c r="Z75" s="48"/>
     </row>
-    <row r="76" spans="1:26" ht="24">
+    <row r="76" spans="1:26" ht="36">
       <c r="A76" s="56">
         <v>55500004</v>
       </c>
@@ -10168,7 +10168,7 @@
       </c>
       <c r="Z76" s="48"/>
     </row>
-    <row r="77" spans="1:26" ht="24">
+    <row r="77" spans="1:26" ht="36">
       <c r="A77" s="56">
         <v>55500005</v>
       </c>
@@ -10216,7 +10216,7 @@
       </c>
       <c r="Z77" s="39"/>
     </row>
-    <row r="78" spans="1:26" ht="24">
+    <row r="78" spans="1:26" ht="36">
       <c r="A78" s="56">
         <v>55500006</v>
       </c>
@@ -10312,7 +10312,7 @@
       </c>
       <c r="Z79" s="39"/>
     </row>
-    <row r="80" spans="1:26" ht="24">
+    <row r="80" spans="1:26" ht="36">
       <c r="A80" s="56">
         <v>55500008</v>
       </c>
@@ -10360,7 +10360,7 @@
       </c>
       <c r="Z80" s="39"/>
     </row>
-    <row r="81" spans="1:26" ht="24">
+    <row r="81" spans="1:26" ht="36">
       <c r="A81" s="56">
         <v>55500009</v>
       </c>
@@ -10408,7 +10408,7 @@
       </c>
       <c r="Z81" s="39"/>
     </row>
-    <row r="82" spans="1:26" ht="24">
+    <row r="82" spans="1:26" ht="36">
       <c r="A82" s="56">
         <v>55500010</v>
       </c>
@@ -10456,7 +10456,7 @@
       </c>
       <c r="Z82" s="39"/>
     </row>
-    <row r="83" spans="1:26" ht="24">
+    <row r="83" spans="1:26" ht="36">
       <c r="A83" s="56">
         <v>55500011</v>
       </c>
@@ -10504,7 +10504,7 @@
       </c>
       <c r="Z83" s="39"/>
     </row>
-    <row r="84" spans="1:26" ht="24">
+    <row r="84" spans="1:26" ht="36">
       <c r="A84" s="56">
         <v>55500012</v>
       </c>
@@ -10600,7 +10600,7 @@
       </c>
       <c r="Z85" s="39"/>
     </row>
-    <row r="86" spans="1:26" ht="24">
+    <row r="86" spans="1:26" ht="36">
       <c r="A86" s="56">
         <v>55500014</v>
       </c>
@@ -10648,7 +10648,7 @@
       </c>
       <c r="Z86" s="48"/>
     </row>
-    <row r="87" spans="1:26" ht="24">
+    <row r="87" spans="1:26" ht="36">
       <c r="A87" s="56">
         <v>55500015</v>
       </c>
@@ -10696,7 +10696,7 @@
       </c>
       <c r="Z87" s="48"/>
     </row>
-    <row r="88" spans="1:26" ht="24">
+    <row r="88" spans="1:26" ht="36">
       <c r="A88" s="56">
         <v>55500016</v>
       </c>
@@ -11572,7 +11572,7 @@
       </c>
       <c r="Z106" s="25"/>
     </row>
-    <row r="107" spans="1:26" ht="24">
+    <row r="107" spans="1:26" ht="36">
       <c r="A107" s="57">
         <v>55600001</v>
       </c>
@@ -11622,7 +11622,7 @@
       </c>
       <c r="Z107" s="37"/>
     </row>
-    <row r="108" spans="1:26" ht="24">
+    <row r="108" spans="1:26" ht="36">
       <c r="A108" s="57">
         <v>55600002</v>
       </c>
@@ -11672,7 +11672,7 @@
       </c>
       <c r="Z108" s="37"/>
     </row>
-    <row r="109" spans="1:26" ht="24">
+    <row r="109" spans="1:26" ht="36">
       <c r="A109" s="57">
         <v>55600003</v>
       </c>
@@ -11722,7 +11722,7 @@
       </c>
       <c r="Z109" s="37"/>
     </row>
-    <row r="110" spans="1:26" ht="24">
+    <row r="110" spans="1:26" ht="36">
       <c r="A110" s="57">
         <v>55600004</v>
       </c>
@@ -11772,7 +11772,7 @@
       </c>
       <c r="Z110" s="37"/>
     </row>
-    <row r="111" spans="1:26" ht="24">
+    <row r="111" spans="1:26" ht="36">
       <c r="A111" s="57">
         <v>55600005</v>
       </c>
@@ -11822,7 +11822,7 @@
       </c>
       <c r="Z111" s="37"/>
     </row>
-    <row r="112" spans="1:26" ht="24">
+    <row r="112" spans="1:26" ht="36">
       <c r="A112" s="57">
         <v>55600006</v>
       </c>
@@ -11972,7 +11972,7 @@
       </c>
       <c r="Z114" s="37"/>
     </row>
-    <row r="115" spans="1:26" ht="24">
+    <row r="115" spans="1:26" ht="36">
       <c r="A115" s="57">
         <v>55600009</v>
       </c>
@@ -12072,7 +12072,7 @@
       </c>
       <c r="Z116" s="37"/>
     </row>
-    <row r="117" spans="1:26" ht="24">
+    <row r="117" spans="1:26" ht="36">
       <c r="A117" s="57">
         <v>55600011</v>
       </c>
@@ -12172,7 +12172,7 @@
       </c>
       <c r="Z118" s="37"/>
     </row>
-    <row r="119" spans="1:26" ht="24">
+    <row r="119" spans="1:26" ht="36">
       <c r="A119" s="87">
         <v>55600013</v>
       </c>
@@ -12272,7 +12272,7 @@
       </c>
       <c r="Z120" s="37"/>
     </row>
-    <row r="121" spans="1:26" ht="24">
+    <row r="121" spans="1:26" ht="36">
       <c r="A121" s="87">
         <v>55600015</v>
       </c>
@@ -12322,7 +12322,7 @@
       </c>
       <c r="Z121" s="37"/>
     </row>
-    <row r="122" spans="1:26" ht="24">
+    <row r="122" spans="1:26" ht="36">
       <c r="A122" s="87">
         <v>55600016</v>
       </c>
@@ -12416,7 +12416,7 @@
       </c>
       <c r="Z123" s="37"/>
     </row>
-    <row r="124" spans="1:26" ht="24">
+    <row r="124" spans="1:26" ht="36">
       <c r="A124" s="77">
         <v>55610002</v>
       </c>
@@ -12464,7 +12464,7 @@
       </c>
       <c r="Z124" s="37"/>
     </row>
-    <row r="125" spans="1:26" ht="24">
+    <row r="125" spans="1:26" ht="36">
       <c r="A125" s="77">
         <v>55610003</v>
       </c>
@@ -12512,7 +12512,7 @@
       </c>
       <c r="Z125" s="37"/>
     </row>
-    <row r="126" spans="1:26" ht="24">
+    <row r="126" spans="1:26" ht="36">
       <c r="A126" s="86">
         <v>55610004</v>
       </c>
@@ -12802,7 +12802,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="132" spans="1:26" ht="96">
+    <row r="132" spans="1:26" ht="120">
       <c r="A132" s="55">
         <v>55900001</v>
       </c>
@@ -12860,7 +12860,7 @@
       </c>
       <c r="Z132" s="48"/>
     </row>
-    <row r="133" spans="1:26" ht="84">
+    <row r="133" spans="1:26" ht="96">
       <c r="A133" s="55">
         <v>55900002</v>
       </c>
@@ -12914,7 +12914,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="134" spans="1:26" ht="24">
+    <row r="134" spans="1:26" ht="28.8">
       <c r="A134" s="55">
         <v>55900003</v>
       </c>
@@ -13008,7 +13008,7 @@
       </c>
       <c r="Z135" s="48"/>
     </row>
-    <row r="136" spans="1:26" ht="27">
+    <row r="136" spans="1:26" ht="28.8">
       <c r="A136" s="55">
         <v>55900005</v>
       </c>
@@ -13286,7 +13286,7 @@
       </c>
       <c r="Z141" s="37"/>
     </row>
-    <row r="142" spans="1:26" ht="60">
+    <row r="142" spans="1:26" ht="84">
       <c r="A142" s="55">
         <v>55900011</v>
       </c>
@@ -13332,7 +13332,7 @@
       </c>
       <c r="Z142" s="25"/>
     </row>
-    <row r="143" spans="1:26" ht="72">
+    <row r="143" spans="1:26" ht="84">
       <c r="A143" s="55">
         <v>55900012</v>
       </c>
@@ -13386,7 +13386,7 @@
       </c>
       <c r="Z143" s="39"/>
     </row>
-    <row r="144" spans="1:26" ht="24">
+    <row r="144" spans="1:26" ht="36">
       <c r="A144" s="55">
         <v>55900013</v>
       </c>
@@ -13736,7 +13736,7 @@
       </c>
       <c r="Z150" s="48"/>
     </row>
-    <row r="151" spans="1:26" ht="84">
+    <row r="151" spans="1:26" ht="108">
       <c r="A151" s="85">
         <v>55900020</v>
       </c>
@@ -13751,7 +13751,7 @@
       <c r="F151" s="44"/>
       <c r="G151" s="79"/>
       <c r="H151" s="29" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I151" s="88"/>
       <c r="J151" s="90"/>
@@ -13782,7 +13782,7 @@
       </c>
       <c r="Z151" s="83"/>
     </row>
-    <row r="152" spans="1:26">
+    <row r="152" spans="1:26" ht="24">
       <c r="A152" s="55">
         <v>55900021</v>
       </c>
@@ -13830,7 +13830,7 @@
       </c>
       <c r="Z152" s="48"/>
     </row>
-    <row r="153" spans="1:26" ht="84">
+    <row r="153" spans="1:26" ht="108">
       <c r="A153" s="85">
         <v>55900022</v>
       </c>
@@ -13884,7 +13884,7 @@
       </c>
       <c r="Z153" s="48"/>
     </row>
-    <row r="154" spans="1:26" ht="27">
+    <row r="154" spans="1:26" ht="28.8">
       <c r="A154" s="55">
         <v>55900023</v>
       </c>
@@ -13930,7 +13930,7 @@
       </c>
       <c r="Z154" s="48"/>
     </row>
-    <row r="155" spans="1:26" ht="84">
+    <row r="155" spans="1:26" ht="96">
       <c r="A155" s="85">
         <v>55900024</v>
       </c>
@@ -13982,7 +13982,7 @@
       </c>
       <c r="Z155" s="48"/>
     </row>
-    <row r="156" spans="1:26" ht="108">
+    <row r="156" spans="1:26" ht="120">
       <c r="A156" s="55">
         <v>55900025</v>
       </c>
@@ -14088,7 +14088,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="158" spans="1:26" ht="27">
+    <row r="158" spans="1:26" ht="36">
       <c r="A158" s="55">
         <v>55900027</v>
       </c>
@@ -14136,7 +14136,7 @@
       </c>
       <c r="Z158" s="48"/>
     </row>
-    <row r="159" spans="1:26" ht="27">
+    <row r="159" spans="1:26" ht="28.8">
       <c r="A159" s="55">
         <v>55900028</v>
       </c>
@@ -14226,7 +14226,7 @@
       </c>
       <c r="Z160" s="48"/>
     </row>
-    <row r="161" spans="1:26" ht="27">
+    <row r="161" spans="1:26" ht="28.8">
       <c r="A161" s="55">
         <v>55900030</v>
       </c>
@@ -14276,7 +14276,7 @@
       </c>
       <c r="Z161" s="48"/>
     </row>
-    <row r="162" spans="1:26">
+    <row r="162" spans="1:26" ht="24">
       <c r="A162" s="55">
         <v>55900031</v>
       </c>
@@ -14322,7 +14322,7 @@
       </c>
       <c r="Z162" s="48"/>
     </row>
-    <row r="163" spans="1:26" ht="84">
+    <row r="163" spans="1:26" ht="108">
       <c r="A163" s="55">
         <v>55900032</v>
       </c>
@@ -14376,7 +14376,7 @@
       </c>
       <c r="Z163" s="48"/>
     </row>
-    <row r="164" spans="1:26" ht="27">
+    <row r="164" spans="1:26" ht="28.8">
       <c r="A164" s="55">
         <v>55900033</v>
       </c>
@@ -14424,7 +14424,7 @@
       </c>
       <c r="Z164" s="48"/>
     </row>
-    <row r="165" spans="1:26" ht="24">
+    <row r="165" spans="1:26" ht="28.8">
       <c r="A165" s="55">
         <v>55900034</v>
       </c>
@@ -14470,7 +14470,7 @@
       </c>
       <c r="Z165" s="48"/>
     </row>
-    <row r="166" spans="1:26" ht="27">
+    <row r="166" spans="1:26" ht="36">
       <c r="A166" s="55">
         <v>55900035</v>
       </c>
@@ -14516,7 +14516,7 @@
       </c>
       <c r="Z166" s="48"/>
     </row>
-    <row r="167" spans="1:26" ht="84">
+    <row r="167" spans="1:26" ht="108">
       <c r="A167" s="55">
         <v>55900036</v>
       </c>
@@ -14570,7 +14570,7 @@
       </c>
       <c r="Z167" s="48"/>
     </row>
-    <row r="168" spans="1:26" ht="72">
+    <row r="168" spans="1:26" ht="96">
       <c r="A168" s="55">
         <v>55900037</v>
       </c>
@@ -14622,7 +14622,7 @@
       </c>
       <c r="Z168" s="48"/>
     </row>
-    <row r="169" spans="1:26" ht="84">
+    <row r="169" spans="1:26" ht="108">
       <c r="A169" s="55">
         <v>55900038</v>
       </c>
@@ -14643,7 +14643,7 @@
       </c>
       <c r="G169" s="60"/>
       <c r="H169" s="29" t="s">
-        <v>951</v>
+        <v>992</v>
       </c>
       <c r="I169" s="29"/>
       <c r="J169" s="26"/>
@@ -14683,7 +14683,7 @@
         <v>55900039</v>
       </c>
       <c r="B170" s="55" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C170" s="25" t="s">
         <v>0</v>
@@ -14693,10 +14693,10 @@
       <c r="F170" s="43"/>
       <c r="G170" s="59"/>
       <c r="H170" s="29" t="s">
+        <v>953</v>
+      </c>
+      <c r="I170" s="29" t="s">
         <v>954</v>
-      </c>
-      <c r="I170" s="29" t="s">
-        <v>955</v>
       </c>
       <c r="J170" s="28"/>
       <c r="K170" s="18"/>
@@ -14712,7 +14712,7 @@
         <v>237</v>
       </c>
       <c r="S170" s="10" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="T170" s="10"/>
       <c r="U170" s="1"/>
@@ -14724,22 +14724,22 @@
         <v>40</v>
       </c>
       <c r="Y170" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="Z170" s="37"/>
     </row>
-    <row r="171" spans="1:26" ht="60">
+    <row r="171" spans="1:26" ht="84">
       <c r="A171" s="55">
         <v>55900040</v>
       </c>
       <c r="B171" s="55" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C171" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D171" s="25" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="E171" s="25">
         <v>100</v>
@@ -14749,7 +14749,7 @@
       </c>
       <c r="G171" s="60"/>
       <c r="H171" s="29" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="I171" s="29"/>
       <c r="J171" s="26"/>
@@ -14766,36 +14766,36 @@
         <v>403</v>
       </c>
       <c r="S171" s="10" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="T171" s="25"/>
       <c r="U171" s="25" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="V171" s="25" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="W171" s="25"/>
       <c r="X171" s="25">
         <v>30</v>
       </c>
       <c r="Y171" s="25" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="Z171" s="48"/>
     </row>
-    <row r="172" spans="1:26" ht="60">
+    <row r="172" spans="1:26" ht="84">
       <c r="A172" s="55">
         <v>55900041</v>
       </c>
       <c r="B172" s="55" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C172" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D172" s="25" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E172" s="25">
         <v>100</v>
@@ -14805,7 +14805,7 @@
       </c>
       <c r="G172" s="60"/>
       <c r="H172" s="29" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I172" s="29"/>
       <c r="J172" s="26"/>
@@ -14822,11 +14822,11 @@
         <v>403</v>
       </c>
       <c r="S172" s="10" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="T172" s="25"/>
       <c r="U172" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="V172" s="25"/>
       <c r="W172" s="25"/>
@@ -14834,16 +14834,16 @@
         <v>0</v>
       </c>
       <c r="Y172" s="25" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="Z172" s="48"/>
     </row>
-    <row r="173" spans="1:26" ht="36">
+    <row r="173" spans="1:26" ht="48">
       <c r="A173" s="55">
         <v>55900042</v>
       </c>
       <c r="B173" s="55" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C173" s="25" t="s">
         <v>0</v>
@@ -14859,7 +14859,7 @@
       <c r="L173" s="30"/>
       <c r="M173" s="17"/>
       <c r="N173" s="17" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="O173" s="20"/>
       <c r="P173" s="41"/>
@@ -14870,7 +14870,7 @@
         <v>403</v>
       </c>
       <c r="S173" s="10" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="T173" s="25"/>
       <c r="U173" s="25"/>
@@ -14880,7 +14880,7 @@
         <v>25</v>
       </c>
       <c r="Y173" s="25" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="Z173" s="48"/>
     </row>
@@ -14889,7 +14889,7 @@
         <v>55900043</v>
       </c>
       <c r="B174" s="55" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C174" s="25" t="s">
         <v>0</v>
@@ -14906,7 +14906,7 @@
       <c r="M174" s="17"/>
       <c r="N174" s="17"/>
       <c r="O174" s="20" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="P174" s="41">
         <v>1</v>
@@ -14918,7 +14918,7 @@
         <v>403</v>
       </c>
       <c r="S174" s="10" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="T174" s="25"/>
       <c r="U174" s="25"/>
@@ -14928,7 +14928,7 @@
         <v>30</v>
       </c>
       <c r="Y174" s="25" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="Z174" s="48"/>
     </row>
@@ -14937,7 +14937,7 @@
         <v>55900044</v>
       </c>
       <c r="B175" s="55" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C175" s="25" t="s">
         <v>0</v>
@@ -14954,7 +14954,7 @@
       <c r="M175" s="17"/>
       <c r="N175" s="17"/>
       <c r="O175" s="20" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="P175" s="41">
         <v>2</v>
@@ -14966,7 +14966,7 @@
         <v>403</v>
       </c>
       <c r="S175" s="10" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="T175" s="25"/>
       <c r="U175" s="25"/>
@@ -14976,16 +14976,16 @@
         <v>40</v>
       </c>
       <c r="Y175" s="25" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="Z175" s="48"/>
     </row>
-    <row r="176" spans="1:26" ht="84">
+    <row r="176" spans="1:26" ht="108">
       <c r="A176" s="55">
         <v>55900045</v>
       </c>
       <c r="B176" s="55" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C176" s="25" t="s">
         <v>0</v>
@@ -15001,7 +15001,7 @@
       </c>
       <c r="G176" s="60"/>
       <c r="H176" s="97" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I176" s="29"/>
       <c r="J176" s="26"/>
@@ -15018,7 +15018,7 @@
         <v>403</v>
       </c>
       <c r="S176" s="10" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="T176" s="25"/>
       <c r="U176" s="25"/>
@@ -15028,7 +15028,7 @@
         <v>25</v>
       </c>
       <c r="Y176" s="25" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="Z176" s="48"/>
     </row>
@@ -15680,7 +15680,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="190" spans="1:26" ht="24">
+    <row r="190" spans="1:26" ht="28.8">
       <c r="A190" s="98">
         <v>55990102</v>
       </c>
@@ -15730,7 +15730,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="191" spans="1:26" ht="60">
+    <row r="191" spans="1:26" ht="72">
       <c r="A191" s="98">
         <v>55990103</v>
       </c>
@@ -15790,7 +15790,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="192" spans="1:26" ht="60">
+    <row r="192" spans="1:26" ht="72">
       <c r="A192" s="98">
         <v>55990104</v>
       </c>
@@ -15869,9 +15869,9 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">

</xml_diff>

<commit_message>
#71 two monster now is chenmo monster
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="1003">
   <si>
     <t>特殊</t>
   </si>
@@ -3799,6 +3799,22 @@
   </si>
   <si>
     <t>hundun</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>沉默</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.Silent();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时沉默范围内所有目标</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>chenmo</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5966,8 +5982,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z193" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:Z193"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z194" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:Z194"/>
   <sortState ref="A4:Z186">
     <sortCondition ref="A3:A186"/>
   </sortState>
@@ -6290,14 +6306,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z193"/>
+  <dimension ref="A1:Z194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C176" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="E178" sqref="E178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -15116,29 +15132,31 @@
       </c>
       <c r="Z177" s="48"/>
     </row>
-    <row r="178" spans="1:26" ht="36">
-      <c r="A178" s="98">
-        <v>55990001</v>
-      </c>
-      <c r="B178" s="98" t="s">
-        <v>23</v>
+    <row r="178" spans="1:26" ht="72">
+      <c r="A178" s="55">
+        <v>55900046</v>
+      </c>
+      <c r="B178" s="55" t="s">
+        <v>999</v>
       </c>
       <c r="C178" s="25" t="s">
-        <v>810</v>
-      </c>
-      <c r="D178" s="25"/>
-      <c r="E178" s="25"/>
+        <v>402</v>
+      </c>
+      <c r="D178" s="25" t="s">
+        <v>990</v>
+      </c>
+      <c r="E178" s="25">
+        <v>20</v>
+      </c>
       <c r="F178" s="25"/>
       <c r="G178" s="60"/>
-      <c r="H178" s="97"/>
-      <c r="I178" s="29"/>
-      <c r="J178" s="26" t="s">
-        <v>407</v>
-      </c>
+      <c r="H178" s="84" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I178" s="47"/>
+      <c r="J178" s="26"/>
       <c r="K178" s="27"/>
-      <c r="L178" s="30" t="s">
-        <v>280</v>
-      </c>
+      <c r="L178" s="30"/>
       <c r="M178" s="17"/>
       <c r="N178" s="17"/>
       <c r="O178" s="20"/>
@@ -15147,31 +15165,33 @@
         <v>242</v>
       </c>
       <c r="R178" s="44" t="s">
-        <v>237</v>
+        <v>403</v>
       </c>
       <c r="S178" s="16" t="s">
-        <v>396</v>
+        <v>1001</v>
       </c>
       <c r="T178" s="25"/>
-      <c r="U178" s="25"/>
-      <c r="V178" s="25"/>
+      <c r="U178" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="V178" s="25" t="s">
+        <v>175</v>
+      </c>
       <c r="W178" s="25"/>
       <c r="X178" s="25">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="Y178" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z178" s="48" t="s">
-        <v>808</v>
-      </c>
+        <v>1002</v>
+      </c>
+      <c r="Z178" s="48"/>
     </row>
     <row r="179" spans="1:26" ht="36">
       <c r="A179" s="98">
-        <v>55990002</v>
+        <v>55990001</v>
       </c>
       <c r="B179" s="98" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C179" s="25" t="s">
         <v>810</v>
@@ -15183,7 +15203,7 @@
       <c r="H179" s="97"/>
       <c r="I179" s="29"/>
       <c r="J179" s="26" t="s">
-        <v>268</v>
+        <v>407</v>
       </c>
       <c r="K179" s="27"/>
       <c r="L179" s="30" t="s">
@@ -15199,8 +15219,8 @@
       <c r="R179" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S179" s="49" t="s">
-        <v>397</v>
+      <c r="S179" s="16" t="s">
+        <v>396</v>
       </c>
       <c r="T179" s="25"/>
       <c r="U179" s="25"/>
@@ -15210,7 +15230,7 @@
         <v>15</v>
       </c>
       <c r="Y179" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Z179" s="48" t="s">
         <v>808</v>
@@ -15218,10 +15238,10 @@
     </row>
     <row r="180" spans="1:26" ht="36">
       <c r="A180" s="98">
-        <v>55990003</v>
+        <v>55990002</v>
       </c>
       <c r="B180" s="98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C180" s="25" t="s">
         <v>810</v>
@@ -15233,7 +15253,7 @@
       <c r="H180" s="97"/>
       <c r="I180" s="29"/>
       <c r="J180" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K180" s="27"/>
       <c r="L180" s="30" t="s">
@@ -15250,7 +15270,7 @@
         <v>237</v>
       </c>
       <c r="S180" s="49" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="T180" s="25"/>
       <c r="U180" s="25"/>
@@ -15260,7 +15280,7 @@
         <v>15</v>
       </c>
       <c r="Y180" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Z180" s="48" t="s">
         <v>808</v>
@@ -15268,10 +15288,10 @@
     </row>
     <row r="181" spans="1:26" ht="36">
       <c r="A181" s="98">
-        <v>55990004</v>
+        <v>55990003</v>
       </c>
       <c r="B181" s="98" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C181" s="25" t="s">
         <v>810</v>
@@ -15283,7 +15303,7 @@
       <c r="H181" s="97"/>
       <c r="I181" s="29"/>
       <c r="J181" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K181" s="27"/>
       <c r="L181" s="30" t="s">
@@ -15300,7 +15320,7 @@
         <v>237</v>
       </c>
       <c r="S181" s="49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="T181" s="25"/>
       <c r="U181" s="25"/>
@@ -15310,7 +15330,7 @@
         <v>15</v>
       </c>
       <c r="Y181" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z181" s="48" t="s">
         <v>808</v>
@@ -15318,10 +15338,10 @@
     </row>
     <row r="182" spans="1:26" ht="36">
       <c r="A182" s="98">
-        <v>55990005</v>
+        <v>55990004</v>
       </c>
       <c r="B182" s="98" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C182" s="25" t="s">
         <v>810</v>
@@ -15333,7 +15353,7 @@
       <c r="H182" s="97"/>
       <c r="I182" s="29"/>
       <c r="J182" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K182" s="27"/>
       <c r="L182" s="30" t="s">
@@ -15350,7 +15370,7 @@
         <v>237</v>
       </c>
       <c r="S182" s="49" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="T182" s="25"/>
       <c r="U182" s="25"/>
@@ -15360,7 +15380,7 @@
         <v>15</v>
       </c>
       <c r="Y182" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Z182" s="48" t="s">
         <v>808</v>
@@ -15368,10 +15388,10 @@
     </row>
     <row r="183" spans="1:26" ht="36">
       <c r="A183" s="98">
-        <v>55990006</v>
+        <v>55990005</v>
       </c>
       <c r="B183" s="98" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C183" s="25" t="s">
         <v>810</v>
@@ -15383,7 +15403,7 @@
       <c r="H183" s="97"/>
       <c r="I183" s="29"/>
       <c r="J183" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K183" s="27"/>
       <c r="L183" s="30" t="s">
@@ -15400,7 +15420,7 @@
         <v>237</v>
       </c>
       <c r="S183" s="49" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T183" s="25"/>
       <c r="U183" s="25"/>
@@ -15410,7 +15430,7 @@
         <v>15</v>
       </c>
       <c r="Y183" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Z183" s="48" t="s">
         <v>808</v>
@@ -15418,10 +15438,10 @@
     </row>
     <row r="184" spans="1:26" ht="36">
       <c r="A184" s="98">
-        <v>55990011</v>
+        <v>55990006</v>
       </c>
       <c r="B184" s="98" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C184" s="25" t="s">
         <v>810</v>
@@ -15433,24 +15453,24 @@
       <c r="H184" s="97"/>
       <c r="I184" s="29"/>
       <c r="J184" s="26" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="K184" s="27"/>
       <c r="L184" s="30" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="M184" s="17"/>
       <c r="N184" s="17"/>
       <c r="O184" s="20"/>
       <c r="P184" s="41"/>
       <c r="Q184" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="R184" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S184" s="16" t="s">
-        <v>284</v>
+      <c r="S184" s="49" t="s">
+        <v>411</v>
       </c>
       <c r="T184" s="25"/>
       <c r="U184" s="25"/>
@@ -15460,7 +15480,7 @@
         <v>15</v>
       </c>
       <c r="Y184" s="25" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="Z184" s="48" t="s">
         <v>808</v>
@@ -15468,10 +15488,10 @@
     </row>
     <row r="185" spans="1:26" ht="36">
       <c r="A185" s="98">
-        <v>55990012</v>
+        <v>55990011</v>
       </c>
       <c r="B185" s="98" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C185" s="25" t="s">
         <v>810</v>
@@ -15483,7 +15503,7 @@
       <c r="H185" s="97"/>
       <c r="I185" s="29"/>
       <c r="J185" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K185" s="27"/>
       <c r="L185" s="30" t="s">
@@ -15500,7 +15520,7 @@
         <v>237</v>
       </c>
       <c r="S185" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T185" s="25"/>
       <c r="U185" s="25"/>
@@ -15510,7 +15530,7 @@
         <v>15</v>
       </c>
       <c r="Y185" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Z185" s="48" t="s">
         <v>808</v>
@@ -15518,10 +15538,10 @@
     </row>
     <row r="186" spans="1:26" ht="36">
       <c r="A186" s="98">
-        <v>55990013</v>
+        <v>55990012</v>
       </c>
       <c r="B186" s="98" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C186" s="25" t="s">
         <v>810</v>
@@ -15533,7 +15553,7 @@
       <c r="H186" s="97"/>
       <c r="I186" s="29"/>
       <c r="J186" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K186" s="27"/>
       <c r="L186" s="30" t="s">
@@ -15550,7 +15570,7 @@
         <v>237</v>
       </c>
       <c r="S186" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T186" s="25"/>
       <c r="U186" s="25"/>
@@ -15560,7 +15580,7 @@
         <v>15</v>
       </c>
       <c r="Y186" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z186" s="48" t="s">
         <v>808</v>
@@ -15568,10 +15588,10 @@
     </row>
     <row r="187" spans="1:26" ht="36">
       <c r="A187" s="98">
-        <v>55990014</v>
+        <v>55990013</v>
       </c>
       <c r="B187" s="98" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C187" s="25" t="s">
         <v>810</v>
@@ -15583,7 +15603,7 @@
       <c r="H187" s="97"/>
       <c r="I187" s="29"/>
       <c r="J187" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K187" s="27"/>
       <c r="L187" s="30" t="s">
@@ -15600,7 +15620,7 @@
         <v>237</v>
       </c>
       <c r="S187" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T187" s="25"/>
       <c r="U187" s="25"/>
@@ -15610,7 +15630,7 @@
         <v>15</v>
       </c>
       <c r="Y187" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Z187" s="48" t="s">
         <v>808</v>
@@ -15618,10 +15638,10 @@
     </row>
     <row r="188" spans="1:26" ht="36">
       <c r="A188" s="98">
-        <v>55990015</v>
+        <v>55990014</v>
       </c>
       <c r="B188" s="98" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C188" s="25" t="s">
         <v>810</v>
@@ -15633,7 +15653,7 @@
       <c r="H188" s="97"/>
       <c r="I188" s="29"/>
       <c r="J188" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K188" s="27"/>
       <c r="L188" s="30" t="s">
@@ -15650,7 +15670,7 @@
         <v>237</v>
       </c>
       <c r="S188" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T188" s="25"/>
       <c r="U188" s="25"/>
@@ -15660,7 +15680,7 @@
         <v>15</v>
       </c>
       <c r="Y188" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Z188" s="48" t="s">
         <v>808</v>
@@ -15668,10 +15688,10 @@
     </row>
     <row r="189" spans="1:26" ht="36">
       <c r="A189" s="98">
-        <v>55990016</v>
+        <v>55990015</v>
       </c>
       <c r="B189" s="98" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C189" s="25" t="s">
         <v>810</v>
@@ -15680,10 +15700,10 @@
       <c r="E189" s="25"/>
       <c r="F189" s="25"/>
       <c r="G189" s="60"/>
-      <c r="H189" s="84"/>
-      <c r="I189" s="47"/>
+      <c r="H189" s="97"/>
+      <c r="I189" s="29"/>
       <c r="J189" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K189" s="27"/>
       <c r="L189" s="30" t="s">
@@ -15700,7 +15720,7 @@
         <v>237</v>
       </c>
       <c r="S189" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T189" s="25"/>
       <c r="U189" s="25"/>
@@ -15710,33 +15730,35 @@
         <v>15</v>
       </c>
       <c r="Y189" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Z189" s="48" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="190" spans="1:26" ht="24">
+    <row r="190" spans="1:26" ht="36">
       <c r="A190" s="98">
-        <v>55990101</v>
+        <v>55990016</v>
       </c>
       <c r="B190" s="98" t="s">
-        <v>811</v>
+        <v>64</v>
       </c>
       <c r="C190" s="25" t="s">
         <v>810</v>
       </c>
       <c r="D190" s="25"/>
       <c r="E190" s="25"/>
-      <c r="F190" s="44"/>
+      <c r="F190" s="25"/>
       <c r="G190" s="60"/>
-      <c r="H190" s="84" t="s">
-        <v>812</v>
-      </c>
+      <c r="H190" s="84"/>
       <c r="I190" s="47"/>
-      <c r="J190" s="26"/>
+      <c r="J190" s="26" t="s">
+        <v>295</v>
+      </c>
       <c r="K190" s="27"/>
-      <c r="L190" s="30"/>
+      <c r="L190" s="30" t="s">
+        <v>283</v>
+      </c>
       <c r="M190" s="17"/>
       <c r="N190" s="17"/>
       <c r="O190" s="20"/>
@@ -15747,103 +15769,95 @@
       <c r="R190" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S190" s="49" t="s">
-        <v>813</v>
+      <c r="S190" s="16" t="s">
+        <v>289</v>
       </c>
       <c r="T190" s="25"/>
       <c r="U190" s="25"/>
       <c r="V190" s="25"/>
       <c r="W190" s="25"/>
       <c r="X190" s="25">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Y190" s="25" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="Z190" s="48" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
     </row>
     <row r="191" spans="1:26" ht="24">
       <c r="A191" s="98">
-        <v>55990102</v>
+        <v>55990101</v>
       </c>
       <c r="B191" s="98" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="C191" s="25" t="s">
         <v>810</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25"/>
-      <c r="F191" s="25"/>
+      <c r="F191" s="44"/>
       <c r="G191" s="60"/>
-      <c r="H191" s="84"/>
+      <c r="H191" s="84" t="s">
+        <v>812</v>
+      </c>
       <c r="I191" s="47"/>
-      <c r="J191" s="26" t="s">
-        <v>815</v>
-      </c>
+      <c r="J191" s="26"/>
       <c r="K191" s="27"/>
-      <c r="L191" s="30" t="s">
-        <v>818</v>
-      </c>
+      <c r="L191" s="30"/>
       <c r="M191" s="17"/>
       <c r="N191" s="17"/>
       <c r="O191" s="20"/>
       <c r="P191" s="41"/>
       <c r="Q191" s="46" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="R191" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="S191" s="16" t="s">
-        <v>817</v>
+      <c r="S191" s="49" t="s">
+        <v>813</v>
       </c>
       <c r="T191" s="25"/>
       <c r="U191" s="25"/>
       <c r="V191" s="25"/>
       <c r="W191" s="25"/>
       <c r="X191" s="25">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Y191" s="25" t="s">
-        <v>821</v>
+        <v>107</v>
       </c>
       <c r="Z191" s="48" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="192" spans="1:26" ht="60">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="192" spans="1:26" ht="24">
       <c r="A192" s="98">
-        <v>55990103</v>
+        <v>55990102</v>
       </c>
       <c r="B192" s="98" t="s">
-        <v>827</v>
+        <v>816</v>
       </c>
       <c r="C192" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D192" s="25" t="s">
-        <v>454</v>
-      </c>
-      <c r="E192" s="25">
-        <v>10</v>
-      </c>
-      <c r="F192" s="44" t="s">
-        <v>464</v>
-      </c>
+        <v>810</v>
+      </c>
+      <c r="D192" s="25"/>
+      <c r="E192" s="25"/>
+      <c r="F192" s="25"/>
       <c r="G192" s="60"/>
       <c r="H192" s="84"/>
       <c r="I192" s="47"/>
       <c r="J192" s="26" t="s">
-        <v>668</v>
+        <v>815</v>
       </c>
       <c r="K192" s="27"/>
-      <c r="L192" s="30"/>
-      <c r="M192" s="17" t="s">
-        <v>583</v>
-      </c>
+      <c r="L192" s="30" t="s">
+        <v>818</v>
+      </c>
+      <c r="M192" s="17"/>
       <c r="N192" s="17"/>
       <c r="O192" s="20"/>
       <c r="P192" s="41"/>
@@ -15854,32 +15868,28 @@
         <v>237</v>
       </c>
       <c r="S192" s="16" t="s">
-        <v>830</v>
+        <v>817</v>
       </c>
       <c r="T192" s="25"/>
-      <c r="U192" s="25" t="s">
-        <v>837</v>
-      </c>
-      <c r="V192" s="25" t="s">
-        <v>837</v>
-      </c>
+      <c r="U192" s="25"/>
+      <c r="V192" s="25"/>
       <c r="W192" s="25"/>
       <c r="X192" s="25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="Y192" s="25" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="Z192" s="48" t="s">
-        <v>828</v>
+        <v>808</v>
       </c>
     </row>
     <row r="193" spans="1:26" ht="60">
       <c r="A193" s="98">
-        <v>55990104</v>
+        <v>55990103</v>
       </c>
       <c r="B193" s="98" t="s">
-        <v>834</v>
+        <v>827</v>
       </c>
       <c r="C193" s="25" t="s">
         <v>97</v>
@@ -15888,7 +15898,7 @@
         <v>454</v>
       </c>
       <c r="E193" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F193" s="44" t="s">
         <v>464</v>
@@ -15897,7 +15907,7 @@
       <c r="H193" s="84"/>
       <c r="I193" s="47"/>
       <c r="J193" s="26" t="s">
-        <v>833</v>
+        <v>668</v>
       </c>
       <c r="K193" s="27"/>
       <c r="L193" s="30"/>
@@ -15914,7 +15924,7 @@
         <v>237</v>
       </c>
       <c r="S193" s="16" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="T193" s="25"/>
       <c r="U193" s="25" t="s">
@@ -15925,12 +15935,72 @@
       </c>
       <c r="W193" s="25"/>
       <c r="X193" s="25">
+        <v>35</v>
+      </c>
+      <c r="Y193" s="25" t="s">
+        <v>829</v>
+      </c>
+      <c r="Z193" s="48" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="194" spans="1:26" ht="60">
+      <c r="A194" s="98">
+        <v>55990104</v>
+      </c>
+      <c r="B194" s="98" t="s">
+        <v>834</v>
+      </c>
+      <c r="C194" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D194" s="25" t="s">
+        <v>454</v>
+      </c>
+      <c r="E194" s="25">
+        <v>20</v>
+      </c>
+      <c r="F194" s="44" t="s">
+        <v>464</v>
+      </c>
+      <c r="G194" s="60"/>
+      <c r="H194" s="84"/>
+      <c r="I194" s="47"/>
+      <c r="J194" s="26" t="s">
+        <v>833</v>
+      </c>
+      <c r="K194" s="27"/>
+      <c r="L194" s="30"/>
+      <c r="M194" s="17" t="s">
+        <v>583</v>
+      </c>
+      <c r="N194" s="17"/>
+      <c r="O194" s="20"/>
+      <c r="P194" s="41"/>
+      <c r="Q194" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="R194" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="S194" s="16" t="s">
+        <v>832</v>
+      </c>
+      <c r="T194" s="25"/>
+      <c r="U194" s="25" t="s">
+        <v>837</v>
+      </c>
+      <c r="V194" s="25" t="s">
+        <v>837</v>
+      </c>
+      <c r="W194" s="25"/>
+      <c r="X194" s="25">
         <v>50</v>
       </c>
-      <c r="Y193" s="25" t="s">
+      <c r="Y194" s="25" t="s">
         <v>831</v>
       </c>
-      <c r="Z193" s="48" t="s">
+      <c r="Z194" s="48" t="s">
         <v>828</v>
       </c>
     </row>

</xml_diff>

<commit_message>
close #71 a new effect of silent
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="1003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="1004">
   <si>
     <t>特殊</t>
   </si>
@@ -3815,6 +3815,10 @@
   </si>
   <si>
     <t>chenmo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>silent</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6309,11 +6313,11 @@
   <dimension ref="A1:Z194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C176" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="O176" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="E178" sqref="E178"/>
+      <selection pane="bottomRight" activeCell="V178" sqref="V178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -15172,10 +15176,10 @@
       </c>
       <c r="T178" s="25"/>
       <c r="U178" s="25" t="s">
-        <v>175</v>
+        <v>1003</v>
       </c>
       <c r="V178" s="25" t="s">
-        <v>175</v>
+        <v>1003</v>
       </c>
       <c r="W178" s="25"/>
       <c r="X178" s="25">

</xml_diff>

<commit_message>
fix a bug of skill tranform wolf, adjust the rate of RandomPlayer
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -3015,9 +3015,6 @@
     <t>d.Star&lt;5</t>
   </si>
   <si>
-    <t>d.Transform(51010002);</t>
-  </si>
-  <si>
     <t>d.AddBuff(56000001,lv,1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3842,6 +3839,10 @@
   </si>
   <si>
     <t>xinling</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Transform(51000002);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6342,11 +6343,11 @@
   <dimension ref="A1:Z195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C175" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C157" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="A178" sqref="A178"/>
+      <selection pane="bottomRight" activeCell="N161" sqref="N161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6570,10 +6571,10 @@
         <v>302</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>436</v>
@@ -6594,7 +6595,7 @@
         <v>318</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>343</v>
@@ -6617,7 +6618,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -6665,7 +6666,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -6715,7 +6716,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -6765,7 +6766,7 @@
         <v>564</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -6813,7 +6814,7 @@
         <v>560</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -6859,7 +6860,7 @@
         <v>568</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D9" s="61"/>
       <c r="E9" s="61"/>
@@ -6905,7 +6906,7 @@
         <v>569</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>454</v>
@@ -6941,10 +6942,10 @@
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="25" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="61">
@@ -6963,7 +6964,7 @@
         <v>570</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -7009,7 +7010,7 @@
         <v>571</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -7055,14 +7056,14 @@
         <v>586</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="43"/>
       <c r="G13" s="59"/>
       <c r="H13" s="29" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I13" s="29"/>
       <c r="J13" s="28"/>
@@ -7103,7 +7104,7 @@
         <v>663</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -7151,14 +7152,14 @@
         <v>667</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="43"/>
       <c r="G15" s="59"/>
       <c r="H15" s="29" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="I15" s="29" t="s">
         <v>340</v>
@@ -7201,7 +7202,7 @@
         <v>671</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -7247,7 +7248,7 @@
         <v>681</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -7292,10 +7293,10 @@
         <v>55100015</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -7308,7 +7309,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="O18" s="20"/>
       <c r="P18" s="41"/>
@@ -7319,7 +7320,7 @@
         <v>237</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="1" t="s">
@@ -7331,7 +7332,7 @@
         <v>16</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="Z18" s="37"/>
     </row>
@@ -8240,7 +8241,7 @@
         <v>55110020</v>
       </c>
       <c r="B38" s="75" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>1</v>
@@ -8252,7 +8253,7 @@
       <c r="H38" s="29"/>
       <c r="I38" s="29"/>
       <c r="J38" s="28" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="K38" s="18"/>
       <c r="L38" s="17" t="s">
@@ -8269,7 +8270,7 @@
         <v>237</v>
       </c>
       <c r="S38" s="10" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="T38" s="10"/>
       <c r="U38" s="1"/>
@@ -8279,7 +8280,7 @@
         <v>40</v>
       </c>
       <c r="Y38" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="Z38" s="48"/>
     </row>
@@ -8416,7 +8417,7 @@
       </c>
       <c r="G41" s="60"/>
       <c r="H41" s="47" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I41" s="87"/>
       <c r="J41" s="88"/>
@@ -8754,7 +8755,7 @@
         <v>97</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="43" t="s">
@@ -8822,7 +8823,7 @@
       </c>
       <c r="G48" s="60"/>
       <c r="H48" s="29" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I48" s="29"/>
       <c r="J48" s="28"/>
@@ -8839,11 +8840,11 @@
         <v>237</v>
       </c>
       <c r="S48" s="16" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="T48" s="25"/>
       <c r="U48" s="25" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="V48" s="25"/>
       <c r="W48" s="25"/>
@@ -8851,7 +8852,7 @@
         <v>25</v>
       </c>
       <c r="Y48" s="25" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="Z48" s="39"/>
     </row>
@@ -8860,7 +8861,7 @@
         <v>55200011</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C49" s="25" t="s">
         <v>97</v>
@@ -8874,7 +8875,7 @@
       <c r="F49" s="44"/>
       <c r="G49" s="59"/>
       <c r="H49" s="47" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="I49" s="47"/>
       <c r="J49" s="26"/>
@@ -8891,21 +8892,21 @@
         <v>237</v>
       </c>
       <c r="S49" s="16" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="T49" s="25"/>
       <c r="U49" s="10" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="V49" s="10" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="W49" s="10"/>
       <c r="X49" s="25">
         <v>20</v>
       </c>
       <c r="Y49" s="25" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="Z49" s="92"/>
     </row>
@@ -8914,13 +8915,13 @@
         <v>55200012</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E50" s="31">
         <v>15</v>
@@ -8930,7 +8931,7 @@
       </c>
       <c r="G50" s="60"/>
       <c r="H50" s="47" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="I50" s="87"/>
       <c r="J50" s="88"/>
@@ -8947,21 +8948,21 @@
         <v>403</v>
       </c>
       <c r="S50" s="16" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="T50" s="31"/>
       <c r="U50" s="25" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="V50" s="25" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="W50" s="31"/>
       <c r="X50" s="31">
         <v>30</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="Z50" s="25"/>
     </row>
@@ -8970,13 +8971,13 @@
         <v>55200013</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E51" s="31">
         <v>12</v>
@@ -8986,7 +8987,7 @@
       </c>
       <c r="G51" s="60"/>
       <c r="H51" s="47" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I51" s="87"/>
       <c r="J51" s="88"/>
@@ -9003,21 +9004,21 @@
         <v>403</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="T51" s="31"/>
       <c r="U51" s="10" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="V51" s="10" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="W51" s="31"/>
       <c r="X51" s="31">
         <v>10</v>
       </c>
       <c r="Y51" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="Z51" s="25"/>
     </row>
@@ -9026,13 +9027,13 @@
         <v>55200014</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C52" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="44" t="s">
@@ -9040,7 +9041,7 @@
       </c>
       <c r="G52" s="60"/>
       <c r="H52" s="93" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="I52" s="29"/>
       <c r="J52" s="26"/>
@@ -9057,21 +9058,21 @@
         <v>237</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="T52" s="25"/>
       <c r="U52" s="25" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="V52" s="25" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="W52" s="25"/>
       <c r="X52" s="25">
         <v>25</v>
       </c>
       <c r="Y52" s="25" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="Z52" s="48"/>
     </row>
@@ -9080,7 +9081,7 @@
         <v>55300001</v>
       </c>
       <c r="B53" s="53" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C53" s="25" t="s">
         <v>48</v>
@@ -9090,10 +9091,10 @@
       <c r="F53" s="44"/>
       <c r="G53" s="60"/>
       <c r="H53" s="47" t="s">
+        <v>903</v>
+      </c>
+      <c r="I53" s="47" t="s">
         <v>904</v>
-      </c>
-      <c r="I53" s="47" t="s">
-        <v>905</v>
       </c>
       <c r="J53" s="26"/>
       <c r="K53" s="27"/>
@@ -9109,7 +9110,7 @@
         <v>237</v>
       </c>
       <c r="S53" s="16" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="T53" s="25"/>
       <c r="U53" s="25"/>
@@ -9159,7 +9160,7 @@
         <v>237</v>
       </c>
       <c r="S54" s="16" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="T54" s="25"/>
       <c r="U54" s="25"/>
@@ -9207,7 +9208,7 @@
         <v>237</v>
       </c>
       <c r="S55" s="16" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="T55" s="25"/>
       <c r="U55" s="25"/>
@@ -9255,7 +9256,7 @@
         <v>237</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="T56" s="25"/>
       <c r="U56" s="25"/>
@@ -9303,7 +9304,7 @@
         <v>237</v>
       </c>
       <c r="S57" s="16" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="T57" s="25"/>
       <c r="U57" s="25"/>
@@ -9399,7 +9400,7 @@
         <v>237</v>
       </c>
       <c r="S59" s="16" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="T59" s="25"/>
       <c r="U59" s="25"/>
@@ -9418,7 +9419,7 @@
         <v>55300008</v>
       </c>
       <c r="B60" s="53" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>48</v>
@@ -9428,10 +9429,10 @@
       <c r="F60" s="44"/>
       <c r="G60" s="60"/>
       <c r="H60" s="47" t="s">
+        <v>845</v>
+      </c>
+      <c r="I60" s="47" t="s">
         <v>846</v>
-      </c>
-      <c r="I60" s="47" t="s">
-        <v>847</v>
       </c>
       <c r="J60" s="26"/>
       <c r="K60" s="27"/>
@@ -9447,7 +9448,7 @@
         <v>237</v>
       </c>
       <c r="S60" s="16" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="T60" s="25"/>
       <c r="U60" s="25"/>
@@ -9466,7 +9467,7 @@
         <v>55300009</v>
       </c>
       <c r="B61" s="53" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>48</v>
@@ -9476,10 +9477,10 @@
       <c r="F61" s="44"/>
       <c r="G61" s="60"/>
       <c r="H61" s="47" t="s">
+        <v>906</v>
+      </c>
+      <c r="I61" s="47" t="s">
         <v>907</v>
-      </c>
-      <c r="I61" s="47" t="s">
-        <v>908</v>
       </c>
       <c r="J61" s="26"/>
       <c r="K61" s="27"/>
@@ -9495,7 +9496,7 @@
         <v>237</v>
       </c>
       <c r="S61" s="16" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="T61" s="25"/>
       <c r="U61" s="25"/>
@@ -9505,7 +9506,7 @@
         <v>30</v>
       </c>
       <c r="Y61" s="25" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="Z61" s="48"/>
     </row>
@@ -9514,7 +9515,7 @@
         <v>55300010</v>
       </c>
       <c r="B62" s="53" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>48</v>
@@ -9524,10 +9525,10 @@
       <c r="F62" s="44"/>
       <c r="G62" s="60"/>
       <c r="H62" s="47" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="I62" s="47" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="J62" s="26"/>
       <c r="K62" s="27"/>
@@ -9543,7 +9544,7 @@
         <v>237</v>
       </c>
       <c r="S62" s="16" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="T62" s="25"/>
       <c r="U62" s="25"/>
@@ -9553,7 +9554,7 @@
         <v>35</v>
       </c>
       <c r="Y62" s="25" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="Z62" s="48"/>
     </row>
@@ -9626,7 +9627,7 @@
       <c r="L64" s="17"/>
       <c r="M64" s="17"/>
       <c r="N64" s="17" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="O64" s="20"/>
       <c r="P64" s="41"/>
@@ -9933,7 +9934,7 @@
         <v>237</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="T70" s="25"/>
       <c r="U70" s="25" t="s">
@@ -9971,7 +9972,7 @@
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
       <c r="O71" s="20" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="P71" s="41">
         <v>2</v>
@@ -10004,13 +10005,13 @@
         <v>55400007</v>
       </c>
       <c r="B72" s="54" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C72" s="25" t="s">
         <v>433</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E72" s="25">
         <v>10</v>
@@ -10020,7 +10021,7 @@
       </c>
       <c r="G72" s="60"/>
       <c r="H72" s="47" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I72" s="47"/>
       <c r="J72" s="26"/>
@@ -10037,7 +10038,7 @@
         <v>237</v>
       </c>
       <c r="S72" s="16" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="T72" s="25"/>
       <c r="U72" s="25"/>
@@ -10047,7 +10048,7 @@
         <v>25</v>
       </c>
       <c r="Y72" s="25" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="Z72" s="48"/>
     </row>
@@ -10056,7 +10057,7 @@
         <v>55410001</v>
       </c>
       <c r="B73" s="54" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C73" s="25" t="s">
         <v>553</v>
@@ -10072,7 +10073,7 @@
       <c r="L73" s="30"/>
       <c r="M73" s="17"/>
       <c r="N73" s="17" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="O73" s="20"/>
       <c r="P73" s="41"/>
@@ -10083,7 +10084,7 @@
         <v>237</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="T73" s="25"/>
       <c r="U73" s="25" t="s">
@@ -10095,7 +10096,7 @@
         <v>50</v>
       </c>
       <c r="Y73" s="50" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="Z73" s="48"/>
     </row>
@@ -10887,7 +10888,7 @@
       <c r="K90" s="18"/>
       <c r="L90" s="17"/>
       <c r="M90" s="17" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="N90" s="17"/>
       <c r="O90" s="20"/>
@@ -11562,7 +11563,7 @@
         <v>55520002</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>35</v>
@@ -11649,7 +11650,7 @@
       </c>
       <c r="Z106" s="25"/>
     </row>
-    <row r="107" spans="1:26">
+    <row r="107" spans="1:26" ht="36">
       <c r="A107" s="57">
         <v>55600001</v>
       </c>
@@ -11714,7 +11715,7 @@
       <c r="F108" s="43"/>
       <c r="G108" s="60"/>
       <c r="H108" s="29" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I108" s="29"/>
       <c r="J108" s="28"/>
@@ -11949,7 +11950,7 @@
       </c>
       <c r="Z112" s="37"/>
     </row>
-    <row r="113" spans="1:26" ht="36">
+    <row r="113" spans="1:26" ht="24">
       <c r="A113" s="57">
         <v>55600007</v>
       </c>
@@ -12049,7 +12050,7 @@
       </c>
       <c r="Z114" s="37"/>
     </row>
-    <row r="115" spans="1:26" ht="24">
+    <row r="115" spans="1:26" ht="36">
       <c r="A115" s="57">
         <v>55600009</v>
       </c>
@@ -12099,7 +12100,7 @@
       </c>
       <c r="Z115" s="37"/>
     </row>
-    <row r="116" spans="1:26" ht="36">
+    <row r="116" spans="1:26" ht="24">
       <c r="A116" s="57">
         <v>55600010</v>
       </c>
@@ -12149,7 +12150,7 @@
       </c>
       <c r="Z116" s="37"/>
     </row>
-    <row r="117" spans="1:26" ht="24">
+    <row r="117" spans="1:26" ht="36">
       <c r="A117" s="86">
         <v>55600011</v>
       </c>
@@ -12199,7 +12200,7 @@
       </c>
       <c r="Z117" s="39"/>
     </row>
-    <row r="118" spans="1:26" ht="36">
+    <row r="118" spans="1:26" ht="24">
       <c r="A118" s="57">
         <v>55600012</v>
       </c>
@@ -12249,7 +12250,7 @@
       </c>
       <c r="Z118" s="25"/>
     </row>
-    <row r="119" spans="1:26" ht="24">
+    <row r="119" spans="1:26" ht="36">
       <c r="A119" s="86">
         <v>55600013</v>
       </c>
@@ -12299,12 +12300,12 @@
       </c>
       <c r="Z119" s="37"/>
     </row>
-    <row r="120" spans="1:26" ht="36">
+    <row r="120" spans="1:26" ht="24">
       <c r="A120" s="86">
         <v>55600014</v>
       </c>
       <c r="B120" s="58" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>48</v>
@@ -12314,7 +12315,7 @@
       <c r="F120" s="43"/>
       <c r="G120" s="60"/>
       <c r="H120" s="29" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="I120" s="29"/>
       <c r="J120" s="28"/>
@@ -12345,16 +12346,16 @@
         <v>30</v>
       </c>
       <c r="Y120" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="Z120" s="37"/>
     </row>
-    <row r="121" spans="1:26" ht="24">
+    <row r="121" spans="1:26" ht="36">
       <c r="A121" s="86">
         <v>55600015</v>
       </c>
       <c r="B121" s="58" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>48</v>
@@ -12364,7 +12365,7 @@
       <c r="F121" s="43"/>
       <c r="G121" s="60"/>
       <c r="H121" s="29" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="I121" s="29"/>
       <c r="J121" s="28"/>
@@ -12381,7 +12382,7 @@
         <v>237</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="T121" s="10">
         <v>56000101</v>
@@ -12395,7 +12396,7 @@
         <v>10</v>
       </c>
       <c r="Y121" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="Z121" s="37"/>
     </row>
@@ -12404,7 +12405,7 @@
         <v>55600016</v>
       </c>
       <c r="B122" s="58" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>48</v>
@@ -12414,7 +12415,7 @@
       <c r="F122" s="43"/>
       <c r="G122" s="60"/>
       <c r="H122" s="29" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I122" s="29"/>
       <c r="J122" s="28"/>
@@ -12431,7 +12432,7 @@
         <v>237</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="T122" s="10">
         <v>56000101</v>
@@ -12445,11 +12446,11 @@
         <v>15</v>
       </c>
       <c r="Y122" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Z122" s="37"/>
     </row>
-    <row r="123" spans="1:26" ht="36">
+    <row r="123" spans="1:26">
       <c r="A123" s="77">
         <v>55610001</v>
       </c>
@@ -12493,7 +12494,7 @@
       </c>
       <c r="Z123" s="37"/>
     </row>
-    <row r="124" spans="1:26">
+    <row r="124" spans="1:26" ht="36">
       <c r="A124" s="77">
         <v>55610002</v>
       </c>
@@ -12637,7 +12638,7 @@
       </c>
       <c r="Z126" s="37"/>
     </row>
-    <row r="127" spans="1:26" ht="36">
+    <row r="127" spans="1:26">
       <c r="A127" s="74">
         <v>55700001</v>
       </c>
@@ -12657,7 +12658,7 @@
       <c r="K127" s="18"/>
       <c r="L127" s="17"/>
       <c r="M127" s="17" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="N127" s="17"/>
       <c r="O127" s="20"/>
@@ -12733,7 +12734,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="129" spans="1:26">
+    <row r="129" spans="1:26" ht="36">
       <c r="A129" s="74">
         <v>55700003</v>
       </c>
@@ -12754,7 +12755,7 @@
       <c r="L129" s="17"/>
       <c r="M129" s="17"/>
       <c r="N129" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="O129" s="20"/>
       <c r="P129" s="41"/>
@@ -12781,7 +12782,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="130" spans="1:26" ht="36">
+    <row r="130" spans="1:26" ht="84">
       <c r="A130" s="74">
         <v>55700004</v>
       </c>
@@ -12792,7 +12793,7 @@
         <v>126</v>
       </c>
       <c r="D130" s="25" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E130" s="25">
         <v>12</v>
@@ -12802,7 +12803,7 @@
       </c>
       <c r="G130" s="60"/>
       <c r="H130" s="29" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I130" s="29"/>
       <c r="J130" s="28"/>
@@ -12819,14 +12820,14 @@
         <v>237</v>
       </c>
       <c r="S130" s="10" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="T130" s="10"/>
       <c r="U130" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="W130" s="1"/>
       <c r="X130" s="1">
@@ -12839,7 +12840,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="131" spans="1:26" ht="84">
+    <row r="131" spans="1:26" ht="24">
       <c r="A131" s="74">
         <v>55700005</v>
       </c>
@@ -12889,7 +12890,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="132" spans="1:26" ht="24">
+    <row r="132" spans="1:26" ht="120">
       <c r="A132" s="55">
         <v>55900001</v>
       </c>
@@ -12910,7 +12911,7 @@
       </c>
       <c r="G132" s="60"/>
       <c r="H132" s="93" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="I132" s="29"/>
       <c r="J132" s="26"/>
@@ -12947,7 +12948,7 @@
       </c>
       <c r="Z132" s="48"/>
     </row>
-    <row r="133" spans="1:26" ht="120">
+    <row r="133" spans="1:26" ht="96">
       <c r="A133" s="55">
         <v>55900002</v>
       </c>
@@ -13001,7 +13002,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="134" spans="1:26" ht="96">
+    <row r="134" spans="1:26" ht="28.8">
       <c r="A134" s="55">
         <v>55900003</v>
       </c>
@@ -13047,7 +13048,7 @@
       </c>
       <c r="Z134" s="48"/>
     </row>
-    <row r="135" spans="1:26" ht="28.8">
+    <row r="135" spans="1:26">
       <c r="A135" s="55">
         <v>55900004</v>
       </c>
@@ -13095,7 +13096,7 @@
       </c>
       <c r="Z135" s="48"/>
     </row>
-    <row r="136" spans="1:26">
+    <row r="136" spans="1:26" ht="28.8">
       <c r="A136" s="55">
         <v>55900005</v>
       </c>
@@ -13141,7 +13142,7 @@
       </c>
       <c r="Z136" s="48"/>
     </row>
-    <row r="137" spans="1:26" ht="28.8">
+    <row r="137" spans="1:26" ht="24">
       <c r="A137" s="55">
         <v>55900006</v>
       </c>
@@ -13189,7 +13190,7 @@
       </c>
       <c r="Z137" s="48"/>
     </row>
-    <row r="138" spans="1:26" ht="24">
+    <row r="138" spans="1:26">
       <c r="A138" s="55">
         <v>55900007</v>
       </c>
@@ -13235,12 +13236,12 @@
       </c>
       <c r="Z138" s="37"/>
     </row>
-    <row r="139" spans="1:26">
+    <row r="139" spans="1:26" ht="24">
       <c r="A139" s="55">
         <v>55900008</v>
       </c>
       <c r="B139" s="55" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>0</v>
@@ -13277,11 +13278,11 @@
         <v>40</v>
       </c>
       <c r="Y139" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="Z139" s="48"/>
     </row>
-    <row r="140" spans="1:26" ht="24">
+    <row r="140" spans="1:26">
       <c r="A140" s="55">
         <v>55900009</v>
       </c>
@@ -13373,7 +13374,7 @@
       </c>
       <c r="Z141" s="37"/>
     </row>
-    <row r="142" spans="1:26">
+    <row r="142" spans="1:26" ht="84">
       <c r="A142" s="55">
         <v>55900011</v>
       </c>
@@ -13388,7 +13389,7 @@
       <c r="F142" s="43"/>
       <c r="G142" s="60"/>
       <c r="H142" s="29" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I142" s="29"/>
       <c r="J142" s="28"/>
@@ -13473,7 +13474,7 @@
       </c>
       <c r="Z143" s="48"/>
     </row>
-    <row r="144" spans="1:26" ht="84">
+    <row r="144" spans="1:26" ht="36">
       <c r="A144" s="55">
         <v>55900013</v>
       </c>
@@ -13521,7 +13522,7 @@
       </c>
       <c r="Z144" s="37"/>
     </row>
-    <row r="145" spans="1:26" ht="36">
+    <row r="145" spans="1:26" ht="24">
       <c r="A145" s="55">
         <v>55900014</v>
       </c>
@@ -13667,7 +13668,7 @@
       </c>
       <c r="Z147" s="48"/>
     </row>
-    <row r="148" spans="1:26" ht="24">
+    <row r="148" spans="1:26" ht="60">
       <c r="A148" s="55">
         <v>55900017</v>
       </c>
@@ -13719,7 +13720,7 @@
       </c>
       <c r="Z148" s="48"/>
     </row>
-    <row r="149" spans="1:26" ht="60">
+    <row r="149" spans="1:26" ht="48">
       <c r="A149" s="55">
         <v>55900018</v>
       </c>
@@ -13741,7 +13742,7 @@
       <c r="M149" s="21"/>
       <c r="N149" s="21"/>
       <c r="O149" s="19" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="P149" s="41">
         <v>1</v>
@@ -13771,7 +13772,7 @@
       </c>
       <c r="Z149" s="48"/>
     </row>
-    <row r="150" spans="1:26" ht="48">
+    <row r="150" spans="1:26" ht="24">
       <c r="A150" s="55">
         <v>55900019</v>
       </c>
@@ -13823,7 +13824,7 @@
       </c>
       <c r="Z150" s="48"/>
     </row>
-    <row r="151" spans="1:26" ht="24">
+    <row r="151" spans="1:26" ht="108">
       <c r="A151" s="55">
         <v>55900020</v>
       </c>
@@ -13838,7 +13839,7 @@
       <c r="F151" s="44"/>
       <c r="G151" s="79"/>
       <c r="H151" s="29" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I151" s="95"/>
       <c r="J151" s="96"/>
@@ -13869,7 +13870,7 @@
       </c>
       <c r="Z151" s="83"/>
     </row>
-    <row r="152" spans="1:26" ht="108">
+    <row r="152" spans="1:26" ht="24">
       <c r="A152" s="85">
         <v>55900021</v>
       </c>
@@ -13917,7 +13918,7 @@
       </c>
       <c r="Z152" s="48"/>
     </row>
-    <row r="153" spans="1:26" ht="24">
+    <row r="153" spans="1:26" ht="108">
       <c r="A153" s="55">
         <v>55900022</v>
       </c>
@@ -13971,7 +13972,7 @@
       </c>
       <c r="Z153" s="48"/>
     </row>
-    <row r="154" spans="1:26" ht="108">
+    <row r="154" spans="1:26" ht="28.8">
       <c r="A154" s="85">
         <v>55900023</v>
       </c>
@@ -14017,7 +14018,7 @@
       </c>
       <c r="Z154" s="48"/>
     </row>
-    <row r="155" spans="1:26" ht="28.8">
+    <row r="155" spans="1:26" ht="96">
       <c r="A155" s="55">
         <v>55900024</v>
       </c>
@@ -14069,7 +14070,7 @@
       </c>
       <c r="Z155" s="48"/>
     </row>
-    <row r="156" spans="1:26" ht="96">
+    <row r="156" spans="1:26" ht="120">
       <c r="A156" s="85">
         <v>55900025</v>
       </c>
@@ -14127,7 +14128,7 @@
       </c>
       <c r="Z156" s="48"/>
     </row>
-    <row r="157" spans="1:26" ht="120">
+    <row r="157" spans="1:26" ht="24">
       <c r="A157" s="55">
         <v>55900026</v>
       </c>
@@ -14175,7 +14176,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="158" spans="1:26" ht="24">
+    <row r="158" spans="1:26" ht="36">
       <c r="A158" s="55">
         <v>55900027</v>
       </c>
@@ -14223,7 +14224,7 @@
       </c>
       <c r="Z158" s="48"/>
     </row>
-    <row r="159" spans="1:26" ht="36">
+    <row r="159" spans="1:26" ht="28.8">
       <c r="A159" s="55">
         <v>55900028</v>
       </c>
@@ -14267,7 +14268,7 @@
       </c>
       <c r="Z159" s="48"/>
     </row>
-    <row r="160" spans="1:26" ht="28.8">
+    <row r="160" spans="1:26" ht="48">
       <c r="A160" s="55">
         <v>55900029</v>
       </c>
@@ -14313,7 +14314,7 @@
       </c>
       <c r="Z160" s="48"/>
     </row>
-    <row r="161" spans="1:26" ht="48">
+    <row r="161" spans="1:26" ht="28.8">
       <c r="A161" s="55">
         <v>55900030</v>
       </c>
@@ -14335,7 +14336,7 @@
       <c r="K161" s="27"/>
       <c r="L161" s="30"/>
       <c r="M161" s="17" t="s">
-        <v>801</v>
+        <v>1009</v>
       </c>
       <c r="N161" s="17"/>
       <c r="O161" s="20"/>
@@ -14363,12 +14364,12 @@
       </c>
       <c r="Z161" s="48"/>
     </row>
-    <row r="162" spans="1:26" ht="28.8">
+    <row r="162" spans="1:26" ht="24">
       <c r="A162" s="55">
         <v>55900031</v>
       </c>
       <c r="B162" s="55" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C162" s="25" t="s">
         <v>0</v>
@@ -14378,7 +14379,7 @@
       <c r="F162" s="25"/>
       <c r="G162" s="60"/>
       <c r="H162" s="84" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="I162" s="47"/>
       <c r="J162" s="26"/>
@@ -14395,7 +14396,7 @@
         <v>403</v>
       </c>
       <c r="S162" s="16" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="T162" s="25"/>
       <c r="U162" s="25"/>
@@ -14405,22 +14406,22 @@
         <v>5</v>
       </c>
       <c r="Y162" s="25" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="Z162" s="48"/>
     </row>
-    <row r="163" spans="1:26" ht="24">
+    <row r="163" spans="1:26" ht="108">
       <c r="A163" s="55">
         <v>55900032</v>
       </c>
       <c r="B163" s="55" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C163" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D163" s="25" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E163" s="25">
         <v>12</v>
@@ -14430,7 +14431,7 @@
       </c>
       <c r="G163" s="60"/>
       <c r="H163" s="84" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I163" s="47"/>
       <c r="J163" s="26"/>
@@ -14447,11 +14448,11 @@
         <v>403</v>
       </c>
       <c r="S163" s="16" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="T163" s="25"/>
       <c r="U163" s="25" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="V163" s="25"/>
       <c r="W163" s="25"/>
@@ -14459,16 +14460,16 @@
         <v>20</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="Z163" s="48"/>
     </row>
-    <row r="164" spans="1:26" ht="108">
+    <row r="164" spans="1:26" ht="28.8">
       <c r="A164" s="55">
         <v>55900033</v>
       </c>
       <c r="B164" s="55" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C164" s="25" t="s">
         <v>0</v>
@@ -14480,11 +14481,11 @@
       <c r="H164" s="93"/>
       <c r="I164" s="29"/>
       <c r="J164" s="26" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="K164" s="27"/>
       <c r="L164" s="30" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="M164" s="17"/>
       <c r="N164" s="17"/>
@@ -14497,7 +14498,7 @@
         <v>403</v>
       </c>
       <c r="S164" s="16" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25"/>
@@ -14507,7 +14508,7 @@
         <v>20</v>
       </c>
       <c r="Y164" s="25" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="Z164" s="48"/>
     </row>
@@ -14516,7 +14517,7 @@
         <v>55900034</v>
       </c>
       <c r="B165" s="55" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C165" s="25" t="s">
         <v>0</v>
@@ -14532,7 +14533,7 @@
       <c r="L165" s="30"/>
       <c r="M165" s="17"/>
       <c r="N165" s="17" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="O165" s="20"/>
       <c r="P165" s="41"/>
@@ -14543,7 +14544,7 @@
         <v>403</v>
       </c>
       <c r="S165" s="16" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="T165" s="25"/>
       <c r="U165" s="25"/>
@@ -14553,16 +14554,16 @@
         <v>14</v>
       </c>
       <c r="Y165" s="25" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="Z165" s="48"/>
     </row>
-    <row r="166" spans="1:26" ht="28.8">
+    <row r="166" spans="1:26" ht="36">
       <c r="A166" s="55">
         <v>55900035</v>
       </c>
       <c r="B166" s="55" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C166" s="25" t="s">
         <v>0</v>
@@ -14572,7 +14573,7 @@
       <c r="F166" s="25"/>
       <c r="G166" s="60"/>
       <c r="H166" s="84" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="I166" s="47"/>
       <c r="J166" s="26"/>
@@ -14589,7 +14590,7 @@
         <v>403</v>
       </c>
       <c r="S166" s="16" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="T166" s="25"/>
       <c r="U166" s="25"/>
@@ -14599,16 +14600,16 @@
         <v>14</v>
       </c>
       <c r="Y166" s="25" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Z166" s="48"/>
     </row>
-    <row r="167" spans="1:26" ht="36">
+    <row r="167" spans="1:26" ht="108">
       <c r="A167" s="55">
         <v>55900036</v>
       </c>
       <c r="B167" s="55" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>0</v>
@@ -14624,7 +14625,7 @@
       </c>
       <c r="G167" s="60"/>
       <c r="H167" s="84" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="I167" s="47"/>
       <c r="J167" s="26"/>
@@ -14641,11 +14642,11 @@
         <v>403</v>
       </c>
       <c r="S167" s="16" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="T167" s="25"/>
       <c r="U167" s="25" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="V167" s="25"/>
       <c r="W167" s="25"/>
@@ -14653,16 +14654,16 @@
         <v>50</v>
       </c>
       <c r="Y167" s="25" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="Z167" s="48"/>
     </row>
-    <row r="168" spans="1:26" ht="108">
+    <row r="168" spans="1:26" ht="96">
       <c r="A168" s="55">
         <v>55900037</v>
       </c>
       <c r="B168" s="55" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C168" s="25" t="s">
         <v>0</v>
@@ -14678,7 +14679,7 @@
       </c>
       <c r="G168" s="60"/>
       <c r="H168" s="93" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I168" s="29"/>
       <c r="J168" s="26"/>
@@ -14695,7 +14696,7 @@
         <v>403</v>
       </c>
       <c r="S168" s="10" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="T168" s="25"/>
       <c r="U168" s="25"/>
@@ -14705,16 +14706,16 @@
         <v>35</v>
       </c>
       <c r="Y168" s="25" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="Z168" s="48"/>
     </row>
-    <row r="169" spans="1:26" ht="96">
+    <row r="169" spans="1:26" ht="108">
       <c r="A169" s="55">
         <v>55900038</v>
       </c>
       <c r="B169" s="55" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C169" s="25" t="s">
         <v>0</v>
@@ -14730,7 +14731,7 @@
       </c>
       <c r="G169" s="60"/>
       <c r="H169" s="29" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I169" s="29"/>
       <c r="J169" s="26"/>
@@ -14747,30 +14748,30 @@
         <v>403</v>
       </c>
       <c r="S169" s="10" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="T169" s="25"/>
       <c r="U169" s="25" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="V169" s="25" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="W169" s="25"/>
       <c r="X169" s="25">
         <v>40</v>
       </c>
       <c r="Y169" s="25" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Z169" s="48"/>
     </row>
-    <row r="170" spans="1:26" ht="108">
+    <row r="170" spans="1:26" ht="36">
       <c r="A170" s="55">
         <v>55900039</v>
       </c>
       <c r="B170" s="55" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C170" s="25" t="s">
         <v>0</v>
@@ -14780,10 +14781,10 @@
       <c r="F170" s="43"/>
       <c r="G170" s="59"/>
       <c r="H170" s="29" t="s">
+        <v>948</v>
+      </c>
+      <c r="I170" s="29" t="s">
         <v>949</v>
-      </c>
-      <c r="I170" s="29" t="s">
-        <v>950</v>
       </c>
       <c r="J170" s="26"/>
       <c r="K170" s="27"/>
@@ -14799,7 +14800,7 @@
         <v>237</v>
       </c>
       <c r="S170" s="10" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="T170" s="10"/>
       <c r="U170" s="1"/>
@@ -14811,22 +14812,22 @@
         <v>40</v>
       </c>
       <c r="Y170" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Z170" s="25"/>
     </row>
-    <row r="171" spans="1:26" ht="36">
+    <row r="171" spans="1:26" ht="84">
       <c r="A171" s="55">
         <v>55900040</v>
       </c>
       <c r="B171" s="55" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C171" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D171" s="25" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E171" s="25">
         <v>100</v>
@@ -14836,7 +14837,7 @@
       </c>
       <c r="G171" s="60"/>
       <c r="H171" s="29" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="I171" s="29"/>
       <c r="J171" s="28"/>
@@ -14853,21 +14854,21 @@
         <v>403</v>
       </c>
       <c r="S171" s="10" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="T171" s="25"/>
       <c r="U171" s="25" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="V171" s="25" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="W171" s="25"/>
       <c r="X171" s="25">
         <v>30</v>
       </c>
       <c r="Y171" s="25" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="Z171" s="39"/>
     </row>
@@ -14876,13 +14877,13 @@
         <v>55900041</v>
       </c>
       <c r="B172" s="55" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C172" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D172" s="25" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="E172" s="25">
         <v>100</v>
@@ -14892,7 +14893,7 @@
       </c>
       <c r="G172" s="60"/>
       <c r="H172" s="29" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="I172" s="29"/>
       <c r="J172" s="26"/>
@@ -14909,11 +14910,11 @@
         <v>403</v>
       </c>
       <c r="S172" s="10" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="T172" s="25"/>
       <c r="U172" s="25" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="V172" s="25"/>
       <c r="W172" s="25"/>
@@ -14921,16 +14922,16 @@
         <v>0</v>
       </c>
       <c r="Y172" s="25" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="Z172" s="48"/>
     </row>
-    <row r="173" spans="1:26" ht="84">
+    <row r="173" spans="1:26" ht="48">
       <c r="A173" s="55">
         <v>55900042</v>
       </c>
       <c r="B173" s="55" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C173" s="25" t="s">
         <v>0</v>
@@ -14946,7 +14947,7 @@
       <c r="L173" s="30"/>
       <c r="M173" s="17"/>
       <c r="N173" s="17" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="O173" s="20"/>
       <c r="P173" s="41"/>
@@ -14957,7 +14958,7 @@
         <v>403</v>
       </c>
       <c r="S173" s="10" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="T173" s="25"/>
       <c r="U173" s="25"/>
@@ -14967,16 +14968,16 @@
         <v>25</v>
       </c>
       <c r="Y173" s="25" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="Z173" s="48"/>
     </row>
-    <row r="174" spans="1:26" ht="48">
+    <row r="174" spans="1:26" ht="24">
       <c r="A174" s="55">
         <v>55900043</v>
       </c>
       <c r="B174" s="55" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C174" s="25" t="s">
         <v>0</v>
@@ -14993,7 +14994,7 @@
       <c r="M174" s="17"/>
       <c r="N174" s="17"/>
       <c r="O174" s="20" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="P174" s="41">
         <v>1</v>
@@ -15005,7 +15006,7 @@
         <v>403</v>
       </c>
       <c r="S174" s="10" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="T174" s="25"/>
       <c r="U174" s="25"/>
@@ -15015,7 +15016,7 @@
         <v>30</v>
       </c>
       <c r="Y174" s="25" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="Z174" s="48"/>
     </row>
@@ -15024,7 +15025,7 @@
         <v>55900044</v>
       </c>
       <c r="B175" s="55" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C175" s="25" t="s">
         <v>0</v>
@@ -15041,7 +15042,7 @@
       <c r="M175" s="17"/>
       <c r="N175" s="17"/>
       <c r="O175" s="20" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="P175" s="41">
         <v>2</v>
@@ -15053,7 +15054,7 @@
         <v>403</v>
       </c>
       <c r="S175" s="10" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="T175" s="25"/>
       <c r="U175" s="25"/>
@@ -15063,22 +15064,22 @@
         <v>40</v>
       </c>
       <c r="Y175" s="25" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="Z175" s="48"/>
     </row>
-    <row r="176" spans="1:26" ht="24">
+    <row r="176" spans="1:26" ht="108">
       <c r="A176" s="55">
         <v>55900045</v>
       </c>
       <c r="B176" s="55" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C176" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D176" s="25" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E176" s="25">
         <v>100</v>
@@ -15088,7 +15089,7 @@
       </c>
       <c r="G176" s="60"/>
       <c r="H176" s="93" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I176" s="29"/>
       <c r="J176" s="26"/>
@@ -15105,7 +15106,7 @@
         <v>403</v>
       </c>
       <c r="S176" s="10" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="T176" s="25"/>
       <c r="U176" s="25"/>
@@ -15115,22 +15116,22 @@
         <v>25</v>
       </c>
       <c r="Y176" s="25" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="Z176" s="48"/>
     </row>
-    <row r="177" spans="1:26" ht="108">
+    <row r="177" spans="1:26" ht="96">
       <c r="A177" s="55">
         <v>55900046</v>
       </c>
       <c r="B177" s="55" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C177" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D177" s="25" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E177" s="25">
         <v>20</v>
@@ -15138,7 +15139,7 @@
       <c r="F177" s="25"/>
       <c r="G177" s="60"/>
       <c r="H177" s="93" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I177" s="29"/>
       <c r="J177" s="26"/>
@@ -15155,21 +15156,21 @@
         <v>403</v>
       </c>
       <c r="S177" s="16" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="T177" s="25"/>
       <c r="U177" s="25" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="V177" s="25" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="W177" s="25"/>
       <c r="X177" s="25">
         <v>25</v>
       </c>
       <c r="Y177" s="25" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="Z177" s="48"/>
     </row>
@@ -15178,13 +15179,13 @@
         <v>55900047</v>
       </c>
       <c r="B178" s="55" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C178" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D178" s="25" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="E178" s="25">
         <v>15</v>
@@ -15192,7 +15193,7 @@
       <c r="F178" s="25"/>
       <c r="G178" s="60"/>
       <c r="H178" s="93" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="I178" s="29"/>
       <c r="J178" s="26"/>
@@ -15209,21 +15210,21 @@
         <v>403</v>
       </c>
       <c r="S178" s="16" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="T178" s="25"/>
       <c r="U178" s="25" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="V178" s="25" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="W178" s="25"/>
       <c r="X178" s="25">
         <v>30</v>
       </c>
       <c r="Y178" s="25" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="Z178" s="48"/>
     </row>
@@ -15235,7 +15236,7 @@
         <v>23</v>
       </c>
       <c r="C179" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D179" s="25"/>
       <c r="E179" s="25"/>
@@ -15274,7 +15275,7 @@
         <v>24</v>
       </c>
       <c r="Z179" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="180" spans="1:26" ht="36">
@@ -15285,7 +15286,7 @@
         <v>25</v>
       </c>
       <c r="C180" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D180" s="25"/>
       <c r="E180" s="25"/>
@@ -15324,7 +15325,7 @@
         <v>26</v>
       </c>
       <c r="Z180" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="181" spans="1:26" ht="36">
@@ -15335,7 +15336,7 @@
         <v>27</v>
       </c>
       <c r="C181" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D181" s="25"/>
       <c r="E181" s="25"/>
@@ -15374,7 +15375,7 @@
         <v>28</v>
       </c>
       <c r="Z181" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="182" spans="1:26" ht="36">
@@ -15385,7 +15386,7 @@
         <v>29</v>
       </c>
       <c r="C182" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D182" s="25"/>
       <c r="E182" s="25"/>
@@ -15424,7 +15425,7 @@
         <v>30</v>
       </c>
       <c r="Z182" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="183" spans="1:26" ht="36">
@@ -15435,7 +15436,7 @@
         <v>31</v>
       </c>
       <c r="C183" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D183" s="25"/>
       <c r="E183" s="25"/>
@@ -15474,7 +15475,7 @@
         <v>32</v>
       </c>
       <c r="Z183" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="184" spans="1:26" ht="36">
@@ -15485,7 +15486,7 @@
         <v>33</v>
       </c>
       <c r="C184" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D184" s="25"/>
       <c r="E184" s="25"/>
@@ -15524,7 +15525,7 @@
         <v>34</v>
       </c>
       <c r="Z184" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="185" spans="1:26" ht="36">
@@ -15535,7 +15536,7 @@
         <v>54</v>
       </c>
       <c r="C185" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D185" s="25"/>
       <c r="E185" s="25"/>
@@ -15574,7 +15575,7 @@
         <v>55</v>
       </c>
       <c r="Z185" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="186" spans="1:26" ht="36">
@@ -15585,7 +15586,7 @@
         <v>56</v>
       </c>
       <c r="C186" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25"/>
@@ -15624,7 +15625,7 @@
         <v>57</v>
       </c>
       <c r="Z186" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="187" spans="1:26" ht="36">
@@ -15635,7 +15636,7 @@
         <v>58</v>
       </c>
       <c r="C187" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D187" s="25"/>
       <c r="E187" s="25"/>
@@ -15674,7 +15675,7 @@
         <v>59</v>
       </c>
       <c r="Z187" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="188" spans="1:26" ht="36">
@@ -15685,7 +15686,7 @@
         <v>60</v>
       </c>
       <c r="C188" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25"/>
@@ -15724,7 +15725,7 @@
         <v>61</v>
       </c>
       <c r="Z188" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="189" spans="1:26" ht="36">
@@ -15735,7 +15736,7 @@
         <v>62</v>
       </c>
       <c r="C189" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25"/>
@@ -15774,7 +15775,7 @@
         <v>63</v>
       </c>
       <c r="Z189" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="190" spans="1:26" ht="36">
@@ -15785,7 +15786,7 @@
         <v>64</v>
       </c>
       <c r="C190" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D190" s="25"/>
       <c r="E190" s="25"/>
@@ -15824,7 +15825,7 @@
         <v>65</v>
       </c>
       <c r="Z190" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="191" spans="1:26" ht="24">
@@ -15832,17 +15833,17 @@
         <v>55990101</v>
       </c>
       <c r="B191" s="94" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C191" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25"/>
       <c r="F191" s="44"/>
       <c r="G191" s="60"/>
       <c r="H191" s="84" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I191" s="47"/>
       <c r="J191" s="26"/>
@@ -15859,7 +15860,7 @@
         <v>237</v>
       </c>
       <c r="S191" s="49" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="T191" s="25"/>
       <c r="U191" s="25"/>
@@ -15872,7 +15873,7 @@
         <v>107</v>
       </c>
       <c r="Z191" s="48" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="192" spans="1:26" ht="28.8">
@@ -15880,10 +15881,10 @@
         <v>55990102</v>
       </c>
       <c r="B192" s="94" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C192" s="25" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D192" s="25"/>
       <c r="E192" s="25"/>
@@ -15892,11 +15893,11 @@
       <c r="H192" s="84"/>
       <c r="I192" s="47"/>
       <c r="J192" s="26" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="K192" s="27"/>
       <c r="L192" s="30" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="M192" s="17"/>
       <c r="N192" s="17"/>
@@ -15909,7 +15910,7 @@
         <v>237</v>
       </c>
       <c r="S192" s="16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="T192" s="25"/>
       <c r="U192" s="25"/>
@@ -15919,10 +15920,10 @@
         <v>25</v>
       </c>
       <c r="Y192" s="25" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="Z192" s="48" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="193" spans="1:26" ht="72">
@@ -15930,7 +15931,7 @@
         <v>55990103</v>
       </c>
       <c r="B193" s="94" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C193" s="25" t="s">
         <v>97</v>
@@ -15965,24 +15966,24 @@
         <v>237</v>
       </c>
       <c r="S193" s="16" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="T193" s="25"/>
       <c r="U193" s="25" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="V193" s="25" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="W193" s="25"/>
       <c r="X193" s="25">
         <v>35</v>
       </c>
       <c r="Y193" s="25" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="Z193" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="194" spans="1:26" ht="72">
@@ -15990,7 +15991,7 @@
         <v>55990104</v>
       </c>
       <c r="B194" s="94" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C194" s="25" t="s">
         <v>97</v>
@@ -16008,7 +16009,7 @@
       <c r="H194" s="84"/>
       <c r="I194" s="47"/>
       <c r="J194" s="26" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="K194" s="27"/>
       <c r="L194" s="30"/>
@@ -16025,24 +16026,24 @@
         <v>237</v>
       </c>
       <c r="S194" s="16" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="T194" s="25"/>
       <c r="U194" s="25" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="V194" s="25" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="W194" s="25"/>
       <c r="X194" s="25">
         <v>50</v>
       </c>
       <c r="Y194" s="25" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="Z194" s="48" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="195" spans="1:26">
@@ -16050,10 +16051,10 @@
         <v>55990105</v>
       </c>
       <c r="B195" s="94" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C195" s="25" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -16065,7 +16066,7 @@
       <c r="K195" s="27"/>
       <c r="L195" s="30"/>
       <c r="M195" s="17" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="N195" s="17"/>
       <c r="O195" s="20"/>
@@ -16077,7 +16078,7 @@
         <v>237</v>
       </c>
       <c r="S195" s="10" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="T195" s="10"/>
       <c r="U195" s="1"/>
@@ -16087,7 +16088,7 @@
         <v>150</v>
       </c>
       <c r="Y195" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="Z195" s="25"/>
     </row>

</xml_diff>

<commit_message>
OnMagicDamage now can known who is the maker
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -3349,10 +3349,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortDistance(true).Top(1)) mon.OnMagicDamage(s.Atk.Source*1.5,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>踩踏</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3489,10 +3485,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position)) if(o.IsLeft!=s.IsLeft) o.OnMagicDamage(s.Atk.Source*0.5,5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>tianlei</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3880,6 +3872,14 @@
   </si>
   <si>
     <t>s.Owner.RemoveSpike(57000014);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortDistance(true).Top(1)) mon.OnMagicDamage(s,s.Atk.Source*1.5,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position)) if(o.IsLeft!=s.IsLeft) o.OnMagicDamage(s,s.Atk.Source*0.5,5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6379,11 +6379,11 @@
   <dimension ref="A1:Z197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="A65" sqref="A65"/>
+      <selection pane="bottomRight" activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7195,7 +7195,7 @@
       <c r="F15" s="43"/>
       <c r="G15" s="59"/>
       <c r="H15" s="29" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="I15" s="29" t="s">
         <v>340</v>
@@ -7291,7 +7291,7 @@
       <c r="F17" s="43"/>
       <c r="G17" s="59"/>
       <c r="H17" s="29" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="28"/>
@@ -7345,7 +7345,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="O18" s="20"/>
       <c r="P18" s="41"/>
@@ -8277,7 +8277,7 @@
         <v>55110020</v>
       </c>
       <c r="B38" s="75" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>1</v>
@@ -8289,7 +8289,7 @@
       <c r="H38" s="29"/>
       <c r="I38" s="29"/>
       <c r="J38" s="28" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="K38" s="18"/>
       <c r="L38" s="17" t="s">
@@ -8306,7 +8306,7 @@
         <v>237</v>
       </c>
       <c r="S38" s="10" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="T38" s="10"/>
       <c r="U38" s="1"/>
@@ -8316,7 +8316,7 @@
         <v>40</v>
       </c>
       <c r="Y38" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="Z38" s="48"/>
     </row>
@@ -8453,7 +8453,7 @@
       </c>
       <c r="G41" s="60"/>
       <c r="H41" s="47" t="s">
-        <v>885</v>
+        <v>1018</v>
       </c>
       <c r="I41" s="87"/>
       <c r="J41" s="88"/>
@@ -8791,7 +8791,7 @@
         <v>97</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="43" t="s">
@@ -8911,7 +8911,7 @@
       <c r="F49" s="44"/>
       <c r="G49" s="59"/>
       <c r="H49" s="47" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I49" s="47"/>
       <c r="J49" s="26"/>
@@ -8928,7 +8928,7 @@
         <v>237</v>
       </c>
       <c r="S49" s="16" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="T49" s="25"/>
       <c r="U49" s="10" t="s">
@@ -8951,13 +8951,13 @@
         <v>55200012</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E50" s="31">
         <v>15</v>
@@ -8967,7 +8967,7 @@
       </c>
       <c r="G50" s="60"/>
       <c r="H50" s="47" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I50" s="87"/>
       <c r="J50" s="88"/>
@@ -8984,21 +8984,21 @@
         <v>403</v>
       </c>
       <c r="S50" s="16" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="T50" s="31"/>
       <c r="U50" s="25" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="V50" s="25" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="W50" s="31"/>
       <c r="X50" s="31">
         <v>30</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="Z50" s="25"/>
     </row>
@@ -9007,13 +9007,13 @@
         <v>55200013</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E51" s="31">
         <v>12</v>
@@ -9023,7 +9023,7 @@
       </c>
       <c r="G51" s="60"/>
       <c r="H51" s="47" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="I51" s="87"/>
       <c r="J51" s="88"/>
@@ -9040,7 +9040,7 @@
         <v>403</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="T51" s="31"/>
       <c r="U51" s="10" t="s">
@@ -9054,7 +9054,7 @@
         <v>10</v>
       </c>
       <c r="Y51" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="Z51" s="25"/>
     </row>
@@ -9063,13 +9063,13 @@
         <v>55200014</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C52" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E52" s="31"/>
       <c r="F52" s="44" t="s">
@@ -9077,7 +9077,7 @@
       </c>
       <c r="G52" s="60"/>
       <c r="H52" s="93" t="s">
-        <v>920</v>
+        <v>1019</v>
       </c>
       <c r="I52" s="29"/>
       <c r="J52" s="26"/>
@@ -9094,21 +9094,21 @@
         <v>237</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="T52" s="25"/>
       <c r="U52" s="25" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="V52" s="25" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="W52" s="25"/>
       <c r="X52" s="25">
         <v>25</v>
       </c>
       <c r="Y52" s="25" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="Z52" s="48"/>
     </row>
@@ -9117,7 +9117,7 @@
         <v>55300001</v>
       </c>
       <c r="B53" s="53" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C53" s="25" t="s">
         <v>48</v>
@@ -9127,10 +9127,10 @@
       <c r="F53" s="44"/>
       <c r="G53" s="60"/>
       <c r="H53" s="47" t="s">
+        <v>892</v>
+      </c>
+      <c r="I53" s="47" t="s">
         <v>893</v>
-      </c>
-      <c r="I53" s="47" t="s">
-        <v>894</v>
       </c>
       <c r="J53" s="26"/>
       <c r="K53" s="27"/>
@@ -9161,7 +9161,7 @@
         <v>68</v>
       </c>
       <c r="Z53" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="54" spans="1:26" ht="60">
@@ -9211,7 +9211,7 @@
         <v>140</v>
       </c>
       <c r="Z54" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="55" spans="1:26" ht="60">
@@ -9261,7 +9261,7 @@
         <v>141</v>
       </c>
       <c r="Z55" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="60">
@@ -9311,7 +9311,7 @@
         <v>180</v>
       </c>
       <c r="Z56" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="57" spans="1:26" ht="60">
@@ -9361,7 +9361,7 @@
         <v>181</v>
       </c>
       <c r="Z57" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="58" spans="1:26" ht="28.8">
@@ -9411,7 +9411,7 @@
         <v>486</v>
       </c>
       <c r="Z58" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="59" spans="1:26" ht="60">
@@ -9448,7 +9448,7 @@
         <v>237</v>
       </c>
       <c r="S59" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="T59" s="25"/>
       <c r="U59" s="25"/>
@@ -9461,7 +9461,7 @@
         <v>118</v>
       </c>
       <c r="Z59" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="60" spans="1:26" ht="36">
@@ -9511,7 +9511,7 @@
         <v>181</v>
       </c>
       <c r="Z60" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="61" spans="1:26" ht="60">
@@ -9519,7 +9519,7 @@
         <v>55300009</v>
       </c>
       <c r="B61" s="53" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>48</v>
@@ -9529,10 +9529,10 @@
       <c r="F61" s="44"/>
       <c r="G61" s="60"/>
       <c r="H61" s="47" t="s">
+        <v>895</v>
+      </c>
+      <c r="I61" s="47" t="s">
         <v>896</v>
-      </c>
-      <c r="I61" s="47" t="s">
-        <v>897</v>
       </c>
       <c r="J61" s="26"/>
       <c r="K61" s="27"/>
@@ -9548,7 +9548,7 @@
         <v>237</v>
       </c>
       <c r="S61" s="16" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T61" s="25"/>
       <c r="U61" s="25"/>
@@ -9558,10 +9558,10 @@
         <v>30</v>
       </c>
       <c r="Y61" s="25" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="Z61" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="62" spans="1:26" ht="36">
@@ -9569,7 +9569,7 @@
         <v>55300010</v>
       </c>
       <c r="B62" s="53" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>48</v>
@@ -9579,10 +9579,10 @@
       <c r="F62" s="44"/>
       <c r="G62" s="60"/>
       <c r="H62" s="47" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I62" s="47" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="J62" s="26"/>
       <c r="K62" s="27"/>
@@ -9598,7 +9598,7 @@
         <v>237</v>
       </c>
       <c r="S62" s="16" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="T62" s="25"/>
       <c r="U62" s="25"/>
@@ -9608,10 +9608,10 @@
         <v>35</v>
       </c>
       <c r="Y62" s="25" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Z62" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="63" spans="1:26" ht="36">
@@ -9619,7 +9619,7 @@
         <v>55300011</v>
       </c>
       <c r="B63" s="53" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>48</v>
@@ -9629,10 +9629,10 @@
       <c r="F63" s="44"/>
       <c r="G63" s="60"/>
       <c r="H63" s="47" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="I63" s="47" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="J63" s="26"/>
       <c r="K63" s="27"/>
@@ -9648,7 +9648,7 @@
         <v>237</v>
       </c>
       <c r="S63" s="16" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="T63" s="25"/>
       <c r="U63" s="25"/>
@@ -9658,10 +9658,10 @@
         <v>25</v>
       </c>
       <c r="Y63" s="25" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="Z63" s="48" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="64" spans="1:26" ht="36">
@@ -9669,7 +9669,7 @@
         <v>55300012</v>
       </c>
       <c r="B64" s="53" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>48</v>
@@ -9679,10 +9679,10 @@
       <c r="F64" s="44"/>
       <c r="G64" s="60"/>
       <c r="H64" s="47" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="I64" s="47" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="J64" s="26"/>
       <c r="K64" s="27"/>
@@ -9698,7 +9698,7 @@
         <v>237</v>
       </c>
       <c r="S64" s="16" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="T64" s="25"/>
       <c r="U64" s="25"/>
@@ -9727,10 +9727,10 @@
       <c r="F65" s="43"/>
       <c r="G65" s="60"/>
       <c r="H65" s="47" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="I65" s="47" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="J65" s="28"/>
       <c r="K65" s="18"/>
@@ -9746,7 +9746,7 @@
         <v>237</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="T65" s="10"/>
       <c r="U65" s="1"/>
@@ -9808,7 +9808,7 @@
       </c>
       <c r="Z66" s="39"/>
     </row>
-    <row r="67" spans="1:26" ht="28.8">
+    <row r="67" spans="1:26" ht="24">
       <c r="A67" s="53">
         <v>55310002</v>
       </c>
@@ -9854,7 +9854,7 @@
       </c>
       <c r="Z67" s="25"/>
     </row>
-    <row r="68" spans="1:26" ht="28.8">
+    <row r="68" spans="1:26" ht="24">
       <c r="A68" s="53">
         <v>55310003</v>
       </c>
@@ -10157,13 +10157,13 @@
         <v>55400007</v>
       </c>
       <c r="B74" s="54" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C74" s="25" t="s">
         <v>430</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="E74" s="25">
         <v>10</v>
@@ -10173,7 +10173,7 @@
       </c>
       <c r="G74" s="60"/>
       <c r="H74" s="47" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="I74" s="47"/>
       <c r="J74" s="26"/>
@@ -10190,7 +10190,7 @@
         <v>237</v>
       </c>
       <c r="S74" s="16" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="T74" s="25"/>
       <c r="U74" s="25"/>
@@ -10200,11 +10200,11 @@
         <v>25</v>
       </c>
       <c r="Y74" s="25" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="Z74" s="48"/>
     </row>
-    <row r="75" spans="1:26" ht="36">
+    <row r="75" spans="1:26" ht="28.8">
       <c r="A75" s="54">
         <v>55410001</v>
       </c>
@@ -10972,7 +10972,7 @@
       </c>
       <c r="Z90" s="48"/>
     </row>
-    <row r="91" spans="1:26" ht="24">
+    <row r="91" spans="1:26" ht="36">
       <c r="A91" s="56">
         <v>55500016</v>
       </c>
@@ -11710,7 +11710,7 @@
       </c>
       <c r="Z106" s="37"/>
     </row>
-    <row r="107" spans="1:26" ht="36">
+    <row r="107" spans="1:26" ht="24">
       <c r="A107" s="11">
         <v>55520002</v>
       </c>
@@ -12760,7 +12760,7 @@
       <c r="K128" s="18"/>
       <c r="L128" s="17"/>
       <c r="M128" s="17" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="N128" s="17"/>
       <c r="O128" s="20"/>
@@ -12857,7 +12857,7 @@
       <c r="L130" s="17"/>
       <c r="M130" s="17"/>
       <c r="N130" s="17" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="O130" s="20"/>
       <c r="P130" s="41"/>
@@ -12895,7 +12895,7 @@
         <v>126</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="E131" s="25">
         <v>12</v>
@@ -12905,7 +12905,7 @@
       </c>
       <c r="G131" s="60"/>
       <c r="H131" s="29" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="I131" s="29"/>
       <c r="J131" s="28"/>
@@ -12922,14 +12922,14 @@
         <v>237</v>
       </c>
       <c r="S131" s="10" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="T131" s="10"/>
       <c r="U131" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="W131" s="1"/>
       <c r="X131" s="1">
@@ -13491,7 +13491,7 @@
       <c r="F143" s="43"/>
       <c r="G143" s="60"/>
       <c r="H143" s="29" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="I143" s="29"/>
       <c r="J143" s="28"/>
@@ -13941,7 +13941,7 @@
       <c r="F152" s="44"/>
       <c r="G152" s="79"/>
       <c r="H152" s="29" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="I152" s="95"/>
       <c r="J152" s="96"/>
@@ -14251,7 +14251,7 @@
       <c r="L158" s="30"/>
       <c r="M158" s="17"/>
       <c r="N158" s="17" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="O158" s="20"/>
       <c r="P158" s="41"/>
@@ -14438,7 +14438,7 @@
       <c r="K162" s="27"/>
       <c r="L162" s="30"/>
       <c r="M162" s="17" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="N162" s="17"/>
       <c r="O162" s="20"/>
@@ -14635,7 +14635,7 @@
       <c r="L166" s="30"/>
       <c r="M166" s="17"/>
       <c r="N166" s="17" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="O166" s="20"/>
       <c r="P166" s="41"/>
@@ -14665,7 +14665,7 @@
         <v>55900035</v>
       </c>
       <c r="B167" s="55" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>0</v>
@@ -14675,7 +14675,7 @@
       <c r="F167" s="25"/>
       <c r="G167" s="60"/>
       <c r="H167" s="84" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="I167" s="47"/>
       <c r="J167" s="26"/>
@@ -14692,7 +14692,7 @@
         <v>403</v>
       </c>
       <c r="S167" s="16" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="T167" s="25"/>
       <c r="U167" s="25"/>
@@ -14702,7 +14702,7 @@
         <v>14</v>
       </c>
       <c r="Y167" s="25" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="Z167" s="48"/>
     </row>
@@ -14711,7 +14711,7 @@
         <v>55900036</v>
       </c>
       <c r="B168" s="55" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C168" s="25" t="s">
         <v>0</v>
@@ -14727,7 +14727,7 @@
       </c>
       <c r="G168" s="60"/>
       <c r="H168" s="84" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="I168" s="47"/>
       <c r="J168" s="26"/>
@@ -14744,7 +14744,7 @@
         <v>403</v>
       </c>
       <c r="S168" s="16" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="T168" s="25"/>
       <c r="U168" s="25" t="s">
@@ -14756,7 +14756,7 @@
         <v>50</v>
       </c>
       <c r="Y168" s="25" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="Z168" s="48"/>
     </row>
@@ -14765,7 +14765,7 @@
         <v>55900037</v>
       </c>
       <c r="B169" s="55" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C169" s="25" t="s">
         <v>0</v>
@@ -14781,7 +14781,7 @@
       </c>
       <c r="G169" s="60"/>
       <c r="H169" s="93" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="I169" s="29"/>
       <c r="J169" s="26"/>
@@ -14798,7 +14798,7 @@
         <v>403</v>
       </c>
       <c r="S169" s="10" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="T169" s="25"/>
       <c r="U169" s="25"/>
@@ -14808,7 +14808,7 @@
         <v>35</v>
       </c>
       <c r="Y169" s="25" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="Z169" s="48"/>
     </row>
@@ -14817,7 +14817,7 @@
         <v>55900038</v>
       </c>
       <c r="B170" s="55" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C170" s="25" t="s">
         <v>0</v>
@@ -14833,7 +14833,7 @@
       </c>
       <c r="G170" s="60"/>
       <c r="H170" s="29" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="I170" s="29"/>
       <c r="J170" s="26"/>
@@ -14850,21 +14850,21 @@
         <v>403</v>
       </c>
       <c r="S170" s="10" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="T170" s="25"/>
       <c r="U170" s="25" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="V170" s="25" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="W170" s="25"/>
       <c r="X170" s="25">
         <v>40</v>
       </c>
       <c r="Y170" s="25" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="Z170" s="48"/>
     </row>
@@ -14873,7 +14873,7 @@
         <v>55900039</v>
       </c>
       <c r="B171" s="55" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="C171" s="25" t="s">
         <v>0</v>
@@ -14883,10 +14883,10 @@
       <c r="F171" s="43"/>
       <c r="G171" s="59"/>
       <c r="H171" s="29" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="I171" s="29" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="J171" s="26"/>
       <c r="K171" s="27"/>
@@ -14902,7 +14902,7 @@
         <v>237</v>
       </c>
       <c r="S171" s="10" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="T171" s="10"/>
       <c r="U171" s="1"/>
@@ -14914,7 +14914,7 @@
         <v>40</v>
       </c>
       <c r="Y171" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="Z171" s="25"/>
     </row>
@@ -14923,13 +14923,13 @@
         <v>55900040</v>
       </c>
       <c r="B172" s="55" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C172" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D172" s="25" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E172" s="25">
         <v>100</v>
@@ -14939,7 +14939,7 @@
       </c>
       <c r="G172" s="60"/>
       <c r="H172" s="29" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="I172" s="29"/>
       <c r="J172" s="28"/>
@@ -14956,21 +14956,21 @@
         <v>403</v>
       </c>
       <c r="S172" s="10" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="T172" s="25"/>
       <c r="U172" s="25" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="V172" s="25" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="W172" s="25"/>
       <c r="X172" s="25">
         <v>30</v>
       </c>
       <c r="Y172" s="25" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="Z172" s="39"/>
     </row>
@@ -14979,13 +14979,13 @@
         <v>55900041</v>
       </c>
       <c r="B173" s="55" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C173" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D173" s="25" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="E173" s="25">
         <v>100</v>
@@ -14995,7 +14995,7 @@
       </c>
       <c r="G173" s="60"/>
       <c r="H173" s="29" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="I173" s="29"/>
       <c r="J173" s="26"/>
@@ -15012,11 +15012,11 @@
         <v>403</v>
       </c>
       <c r="S173" s="10" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="T173" s="25"/>
       <c r="U173" s="25" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="V173" s="25"/>
       <c r="W173" s="25"/>
@@ -15024,7 +15024,7 @@
         <v>0</v>
       </c>
       <c r="Y173" s="25" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="Z173" s="48"/>
     </row>
@@ -15033,7 +15033,7 @@
         <v>55900042</v>
       </c>
       <c r="B174" s="55" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C174" s="25" t="s">
         <v>0</v>
@@ -15049,7 +15049,7 @@
       <c r="L174" s="30"/>
       <c r="M174" s="17"/>
       <c r="N174" s="17" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="O174" s="20"/>
       <c r="P174" s="41"/>
@@ -15060,7 +15060,7 @@
         <v>403</v>
       </c>
       <c r="S174" s="10" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="T174" s="25"/>
       <c r="U174" s="25"/>
@@ -15070,7 +15070,7 @@
         <v>25</v>
       </c>
       <c r="Y174" s="25" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="Z174" s="48"/>
     </row>
@@ -15079,7 +15079,7 @@
         <v>55900043</v>
       </c>
       <c r="B175" s="55" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C175" s="25" t="s">
         <v>0</v>
@@ -15096,7 +15096,7 @@
       <c r="M175" s="17"/>
       <c r="N175" s="17"/>
       <c r="O175" s="20" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="P175" s="41">
         <v>1</v>
@@ -15108,7 +15108,7 @@
         <v>403</v>
       </c>
       <c r="S175" s="10" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="T175" s="25"/>
       <c r="U175" s="25"/>
@@ -15118,7 +15118,7 @@
         <v>30</v>
       </c>
       <c r="Y175" s="25" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="Z175" s="48"/>
     </row>
@@ -15127,7 +15127,7 @@
         <v>55900044</v>
       </c>
       <c r="B176" s="55" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="C176" s="25" t="s">
         <v>0</v>
@@ -15144,7 +15144,7 @@
       <c r="M176" s="17"/>
       <c r="N176" s="17"/>
       <c r="O176" s="20" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="P176" s="41">
         <v>2</v>
@@ -15156,7 +15156,7 @@
         <v>403</v>
       </c>
       <c r="S176" s="10" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="T176" s="25"/>
       <c r="U176" s="25"/>
@@ -15166,7 +15166,7 @@
         <v>40</v>
       </c>
       <c r="Y176" s="25" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="Z176" s="48"/>
     </row>
@@ -15175,13 +15175,13 @@
         <v>55900045</v>
       </c>
       <c r="B177" s="55" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C177" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D177" s="25" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E177" s="25">
         <v>100</v>
@@ -15191,7 +15191,7 @@
       </c>
       <c r="G177" s="60"/>
       <c r="H177" s="93" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="I177" s="29"/>
       <c r="J177" s="26"/>
@@ -15208,7 +15208,7 @@
         <v>403</v>
       </c>
       <c r="S177" s="10" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="T177" s="25"/>
       <c r="U177" s="25"/>
@@ -15218,7 +15218,7 @@
         <v>25</v>
       </c>
       <c r="Y177" s="25" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="Z177" s="48"/>
     </row>
@@ -15227,13 +15227,13 @@
         <v>55900046</v>
       </c>
       <c r="B178" s="55" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C178" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D178" s="25" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="E178" s="25">
         <v>20</v>
@@ -15241,7 +15241,7 @@
       <c r="F178" s="25"/>
       <c r="G178" s="60"/>
       <c r="H178" s="93" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="I178" s="29"/>
       <c r="J178" s="26"/>
@@ -15258,21 +15258,21 @@
         <v>403</v>
       </c>
       <c r="S178" s="16" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="T178" s="25"/>
       <c r="U178" s="25" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="V178" s="25" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="W178" s="25"/>
       <c r="X178" s="25">
         <v>25</v>
       </c>
       <c r="Y178" s="25" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="Z178" s="48"/>
     </row>
@@ -15281,13 +15281,13 @@
         <v>55900047</v>
       </c>
       <c r="B179" s="55" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C179" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D179" s="25" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="E179" s="25">
         <v>15</v>
@@ -15295,7 +15295,7 @@
       <c r="F179" s="25"/>
       <c r="G179" s="60"/>
       <c r="H179" s="93" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="I179" s="29"/>
       <c r="J179" s="26"/>
@@ -15312,21 +15312,21 @@
         <v>403</v>
       </c>
       <c r="S179" s="16" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="T179" s="25"/>
       <c r="U179" s="25" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="V179" s="25" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="W179" s="25"/>
       <c r="X179" s="25">
         <v>30</v>
       </c>
       <c r="Y179" s="25" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="Z179" s="48"/>
     </row>
@@ -15335,7 +15335,7 @@
         <v>55900048</v>
       </c>
       <c r="B180" s="55" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="C180" s="25" t="s">
         <v>402</v>
@@ -15350,7 +15350,7 @@
       <c r="K180" s="27"/>
       <c r="L180" s="30"/>
       <c r="M180" s="17" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="N180" s="17"/>
       <c r="O180" s="20"/>
@@ -15362,7 +15362,7 @@
         <v>403</v>
       </c>
       <c r="S180" s="16" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="T180" s="25"/>
       <c r="U180" s="25"/>
@@ -15372,7 +15372,7 @@
         <v>70</v>
       </c>
       <c r="Y180" s="25" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="Z180" s="48"/>
     </row>

</xml_diff>

<commit_message>
recheck the shield crash skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -2440,10 +2440,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s.AttackType==s.Attr&amp;&amp;s.HasScroll</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>通魔</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3891,6 +3887,10 @@
   </si>
   <si>
     <t>false</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AttackType==s.Attr&amp;&amp;s.WeaponType==2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6391,11 +6391,11 @@
   <dimension ref="A1:Z197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6521,7 +6521,7 @@
         <v>550</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>338</v>
@@ -6539,7 +6539,7 @@
         <v>620</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>307</v>
@@ -6595,7 +6595,7 @@
         <v>453</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G3" s="40" t="s">
         <v>551</v>
@@ -6619,10 +6619,10 @@
         <v>302</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>433</v>
@@ -6643,7 +6643,7 @@
         <v>318</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>343</v>
@@ -6666,7 +6666,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -6714,7 +6714,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -6764,7 +6764,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -6814,7 +6814,7 @@
         <v>556</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -6862,7 +6862,7 @@
         <v>552</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -6908,7 +6908,7 @@
         <v>560</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D9" s="61"/>
       <c r="E9" s="61"/>
@@ -6954,7 +6954,7 @@
         <v>561</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>451</v>
@@ -6969,7 +6969,7 @@
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="17"/>
@@ -6990,10 +6990,10 @@
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="25" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="61">
@@ -7012,22 +7012,22 @@
         <v>562</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="E11" s="25">
         <v>30</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="G11" s="60" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="H11" s="93" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I11" s="29"/>
       <c r="J11" s="26"/>
@@ -7066,14 +7066,14 @@
         <v>573</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="43"/>
       <c r="G12" s="59"/>
       <c r="H12" s="29" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="I12" s="29"/>
       <c r="J12" s="28"/>
@@ -7106,7 +7106,7 @@
       </c>
       <c r="Z12" s="37"/>
     </row>
-    <row r="13" spans="1:26" ht="60">
+    <row r="13" spans="1:26" ht="72">
       <c r="A13" s="51">
         <v>55100011</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>650</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -7123,7 +7123,7 @@
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="J13" s="28" t="s">
-        <v>653</v>
+        <v>1022</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="17" t="s">
@@ -7159,17 +7159,17 @@
         <v>55100012</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="43"/>
       <c r="G14" s="59"/>
       <c r="H14" s="29" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I14" s="29" t="s">
         <v>340</v>
@@ -7209,16 +7209,16 @@
         <v>55100013</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="43"/>
       <c r="G15" s="59" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
@@ -7236,7 +7236,7 @@
         <v>237</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
@@ -7246,7 +7246,7 @@
         <v>10</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="Z15" s="37"/>
     </row>
@@ -7255,17 +7255,17 @@
         <v>55100014</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="43"/>
       <c r="G16" s="59"/>
       <c r="H16" s="29" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I16" s="29"/>
       <c r="J16" s="28"/>
@@ -7303,10 +7303,10 @@
         <v>55100015</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -7319,7 +7319,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="O17" s="20"/>
       <c r="P17" s="41"/>
@@ -7330,7 +7330,7 @@
         <v>237</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="T17" s="10"/>
       <c r="U17" s="1" t="s">
@@ -7342,7 +7342,7 @@
         <v>16</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="Z17" s="37"/>
     </row>
@@ -7535,7 +7535,7 @@
         <v>55110005</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>36</v>
@@ -7547,7 +7547,7 @@
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
       <c r="J22" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K22" s="18"/>
       <c r="L22" s="17"/>
@@ -7564,7 +7564,7 @@
         <v>237</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="T22" s="14"/>
       <c r="U22" s="1"/>
@@ -7583,7 +7583,7 @@
         <v>55110006</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>1</v>
@@ -7599,7 +7599,7 @@
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="17" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -7612,7 +7612,7 @@
         <v>237</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="T23" s="10"/>
       <c r="U23" s="1"/>
@@ -7631,7 +7631,7 @@
         <v>55110007</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
@@ -7643,11 +7643,11 @@
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
       <c r="J24" s="28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="K24" s="18"/>
       <c r="L24" s="17" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -7660,7 +7660,7 @@
         <v>237</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="T24" s="10"/>
       <c r="U24" s="1"/>
@@ -7679,7 +7679,7 @@
         <v>55110008</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
@@ -7725,7 +7725,7 @@
         <v>55110009</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -7739,7 +7739,7 @@
       <c r="J26" s="28"/>
       <c r="K26" s="18"/>
       <c r="L26" s="17" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
@@ -7752,7 +7752,7 @@
         <v>237</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="T26" s="10"/>
       <c r="U26" s="1"/>
@@ -7771,7 +7771,7 @@
         <v>55110010</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>36</v>
@@ -7783,7 +7783,7 @@
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
       <c r="J27" s="28" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="K27" s="18"/>
       <c r="L27" s="17" t="s">
@@ -7819,7 +7819,7 @@
         <v>55110011</v>
       </c>
       <c r="B28" s="75" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>36</v>
@@ -7831,10 +7831,10 @@
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
       <c r="J28" s="28" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
@@ -7848,7 +7848,7 @@
         <v>237</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="T28" s="10"/>
       <c r="U28" s="1"/>
@@ -7867,7 +7867,7 @@
         <v>55110012</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>1</v>
@@ -7882,7 +7882,7 @@
       <c r="K29" s="18"/>
       <c r="L29" s="17"/>
       <c r="M29" s="17" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N29" s="17"/>
       <c r="O29" s="20"/>
@@ -7913,7 +7913,7 @@
         <v>55110013</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>36</v>
@@ -7925,14 +7925,14 @@
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
       <c r="J30" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K30" s="18"/>
       <c r="L30" s="17" t="s">
+        <v>715</v>
+      </c>
+      <c r="M30" s="17" t="s">
         <v>716</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>717</v>
       </c>
       <c r="N30" s="17"/>
       <c r="O30" s="20"/>
@@ -7944,7 +7944,7 @@
         <v>237</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="T30" s="10"/>
       <c r="U30" s="1"/>
@@ -7963,7 +7963,7 @@
         <v>55110014</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>36</v>
@@ -8009,7 +8009,7 @@
         <v>55110015</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>1</v>
@@ -8021,7 +8021,7 @@
       <c r="H32" s="29"/>
       <c r="I32" s="29"/>
       <c r="J32" s="28" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K32" s="18"/>
       <c r="L32" s="17" t="s">
@@ -8038,7 +8038,7 @@
         <v>237</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="T32" s="10"/>
       <c r="U32" s="1"/>
@@ -8057,7 +8057,7 @@
         <v>55110016</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>36</v>
@@ -8072,7 +8072,7 @@
         <v>301</v>
       </c>
       <c r="K33" s="18" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="17"/>
@@ -8086,7 +8086,7 @@
         <v>237</v>
       </c>
       <c r="S33" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="T33" s="10"/>
       <c r="U33" s="1"/>
@@ -8105,7 +8105,7 @@
         <v>55110017</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>36</v>
@@ -8119,7 +8119,7 @@
       <c r="J34" s="28"/>
       <c r="K34" s="18"/>
       <c r="L34" s="17" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
@@ -8132,7 +8132,7 @@
         <v>237</v>
       </c>
       <c r="S34" s="10" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="T34" s="10"/>
       <c r="U34" s="1"/>
@@ -8151,7 +8151,7 @@
         <v>55110018</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>36</v>
@@ -8201,7 +8201,7 @@
         <v>55110019</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C36" s="25" t="s">
         <v>36</v>
@@ -8213,11 +8213,11 @@
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
       <c r="J36" s="26" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="30" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
@@ -8230,7 +8230,7 @@
         <v>403</v>
       </c>
       <c r="S36" s="16" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="T36" s="25"/>
       <c r="U36" s="25" t="s">
@@ -8251,7 +8251,7 @@
         <v>55110020</v>
       </c>
       <c r="B37" s="75" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>1</v>
@@ -8263,7 +8263,7 @@
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
       <c r="J37" s="28" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="K37" s="18"/>
       <c r="L37" s="17" t="s">
@@ -8280,7 +8280,7 @@
         <v>237</v>
       </c>
       <c r="S37" s="10" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
@@ -8290,7 +8290,7 @@
         <v>40</v>
       </c>
       <c r="Y37" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="Z37" s="48"/>
     </row>
@@ -8390,7 +8390,7 @@
         <v>237</v>
       </c>
       <c r="S39" s="16" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="T39" s="25"/>
       <c r="U39" s="25" t="s">
@@ -8417,7 +8417,7 @@
         <v>97</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E40" s="31">
         <v>30</v>
@@ -8427,7 +8427,7 @@
       </c>
       <c r="G40" s="60"/>
       <c r="H40" s="47" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I40" s="87"/>
       <c r="J40" s="88"/>
@@ -8444,7 +8444,7 @@
         <v>403</v>
       </c>
       <c r="S40" s="16" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="T40" s="31"/>
       <c r="U40" s="31"/>
@@ -8471,7 +8471,7 @@
         <v>97</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E41" s="25">
         <v>15</v>
@@ -8486,7 +8486,7 @@
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="O41" s="20" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="P41" s="41">
         <v>1</v>
@@ -8498,7 +8498,7 @@
         <v>237</v>
       </c>
       <c r="S41" s="16" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="T41" s="25"/>
       <c r="U41" s="10" t="s">
@@ -8512,7 +8512,7 @@
         <v>40</v>
       </c>
       <c r="Y41" s="25" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Z41" s="92"/>
     </row>
@@ -8527,13 +8527,13 @@
         <v>97</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E42" s="25">
         <v>25</v>
       </c>
       <c r="F42" s="44" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="G42" s="59"/>
       <c r="H42" s="47"/>
@@ -8544,7 +8544,7 @@
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
       <c r="O42" s="20" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="P42" s="41">
         <v>2</v>
@@ -8556,7 +8556,7 @@
         <v>237</v>
       </c>
       <c r="S42" s="16" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="T42" s="25"/>
       <c r="U42" s="10" t="s">
@@ -8597,7 +8597,7 @@
       <c r="H43" s="29"/>
       <c r="I43" s="29"/>
       <c r="J43" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K43" s="18"/>
       <c r="L43" s="17"/>
@@ -8657,7 +8657,7 @@
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
       <c r="J44" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="17"/>
@@ -8705,24 +8705,24 @@
         <v>97</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E45" s="25">
         <v>20</v>
       </c>
       <c r="F45" s="44" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G45" s="60"/>
       <c r="H45" s="29"/>
       <c r="I45" s="29"/>
       <c r="J45" s="26" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K45" s="27"/>
       <c r="L45" s="30"/>
       <c r="M45" s="17" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="N45" s="17"/>
       <c r="O45" s="20"/>
@@ -8734,7 +8734,7 @@
         <v>403</v>
       </c>
       <c r="S45" s="16" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="T45" s="25"/>
       <c r="U45" s="25" t="s">
@@ -8744,7 +8744,7 @@
         <v>438</v>
       </c>
       <c r="W45" s="25" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="X45" s="25">
         <v>25</v>
@@ -8765,7 +8765,7 @@
         <v>97</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="43" t="s">
@@ -8775,7 +8775,7 @@
       <c r="H46" s="29"/>
       <c r="I46" s="29"/>
       <c r="J46" s="28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K46" s="18"/>
       <c r="L46" s="17"/>
@@ -8833,7 +8833,7 @@
       </c>
       <c r="G47" s="60"/>
       <c r="H47" s="29" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="I47" s="29"/>
       <c r="J47" s="28"/>
@@ -8850,11 +8850,11 @@
         <v>237</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="T47" s="25"/>
       <c r="U47" s="25" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="V47" s="25"/>
       <c r="W47" s="25"/>
@@ -8862,7 +8862,7 @@
         <v>25</v>
       </c>
       <c r="Y47" s="25" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="Z47" s="39"/>
     </row>
@@ -8871,13 +8871,13 @@
         <v>55200011</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C48" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E48" s="25">
         <v>12</v>
@@ -8887,7 +8887,7 @@
       </c>
       <c r="G48" s="59"/>
       <c r="H48" s="47" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I48" s="47"/>
       <c r="J48" s="26"/>
@@ -8904,21 +8904,21 @@
         <v>237</v>
       </c>
       <c r="S48" s="16" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="T48" s="25"/>
       <c r="U48" s="10" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="V48" s="10" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="W48" s="10"/>
       <c r="X48" s="25">
         <v>20</v>
       </c>
       <c r="Y48" s="25" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="Z48" s="92"/>
     </row>
@@ -8927,13 +8927,13 @@
         <v>55200012</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C49" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E49" s="31">
         <v>15</v>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="G49" s="60"/>
       <c r="H49" s="47" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I49" s="87"/>
       <c r="J49" s="88"/>
@@ -8960,21 +8960,21 @@
         <v>403</v>
       </c>
       <c r="S49" s="16" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="T49" s="31"/>
       <c r="U49" s="25" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="V49" s="25" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="W49" s="31"/>
       <c r="X49" s="31">
         <v>30</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="Z49" s="25"/>
     </row>
@@ -8983,13 +8983,13 @@
         <v>55200013</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E50" s="31">
         <v>12</v>
@@ -8999,7 +8999,7 @@
       </c>
       <c r="G50" s="60"/>
       <c r="H50" s="47" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I50" s="87"/>
       <c r="J50" s="88"/>
@@ -9016,21 +9016,21 @@
         <v>403</v>
       </c>
       <c r="S50" s="16" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="T50" s="31"/>
       <c r="U50" s="10" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="V50" s="10" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="W50" s="31"/>
       <c r="X50" s="31">
         <v>10</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="Z50" s="25"/>
     </row>
@@ -9039,13 +9039,13 @@
         <v>55200014</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="44" t="s">
@@ -9053,7 +9053,7 @@
       </c>
       <c r="G51" s="60"/>
       <c r="H51" s="93" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I51" s="29"/>
       <c r="J51" s="26"/>
@@ -9070,21 +9070,21 @@
         <v>237</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="T51" s="25"/>
       <c r="U51" s="25" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="V51" s="25" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="W51" s="25"/>
       <c r="X51" s="25">
         <v>25</v>
       </c>
       <c r="Y51" s="25" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="Z51" s="48"/>
     </row>
@@ -9093,7 +9093,7 @@
         <v>55300001</v>
       </c>
       <c r="B52" s="53" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C52" s="25" t="s">
         <v>48</v>
@@ -9103,10 +9103,10 @@
       <c r="F52" s="44"/>
       <c r="G52" s="60"/>
       <c r="H52" s="47" t="s">
+        <v>885</v>
+      </c>
+      <c r="I52" s="47" t="s">
         <v>886</v>
-      </c>
-      <c r="I52" s="47" t="s">
-        <v>887</v>
       </c>
       <c r="J52" s="26"/>
       <c r="K52" s="27"/>
@@ -9122,7 +9122,7 @@
         <v>237</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="T52" s="25"/>
       <c r="U52" s="25"/>
@@ -9137,7 +9137,7 @@
         <v>68</v>
       </c>
       <c r="Z52" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="53" spans="1:26" ht="60">
@@ -9174,7 +9174,7 @@
         <v>237</v>
       </c>
       <c r="S53" s="16" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="T53" s="25"/>
       <c r="U53" s="25"/>
@@ -9187,7 +9187,7 @@
         <v>140</v>
       </c>
       <c r="Z53" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="54" spans="1:26" ht="60">
@@ -9224,7 +9224,7 @@
         <v>237</v>
       </c>
       <c r="S54" s="16" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="T54" s="25"/>
       <c r="U54" s="25"/>
@@ -9237,7 +9237,7 @@
         <v>141</v>
       </c>
       <c r="Z54" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="55" spans="1:26" ht="60">
@@ -9274,7 +9274,7 @@
         <v>237</v>
       </c>
       <c r="S55" s="16" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="T55" s="25"/>
       <c r="U55" s="25"/>
@@ -9287,7 +9287,7 @@
         <v>180</v>
       </c>
       <c r="Z55" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="60">
@@ -9324,7 +9324,7 @@
         <v>237</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="T56" s="25"/>
       <c r="U56" s="25"/>
@@ -9337,7 +9337,7 @@
         <v>181</v>
       </c>
       <c r="Z56" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="57" spans="1:26" ht="28.8">
@@ -9387,7 +9387,7 @@
         <v>485</v>
       </c>
       <c r="Z57" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="58" spans="1:26" ht="60">
@@ -9424,7 +9424,7 @@
         <v>237</v>
       </c>
       <c r="S58" s="16" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="T58" s="25"/>
       <c r="U58" s="25"/>
@@ -9437,7 +9437,7 @@
         <v>118</v>
       </c>
       <c r="Z58" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="59" spans="1:26" ht="36">
@@ -9445,7 +9445,7 @@
         <v>55300008</v>
       </c>
       <c r="B59" s="53" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C59" s="25" t="s">
         <v>48</v>
@@ -9455,10 +9455,10 @@
       <c r="F59" s="44"/>
       <c r="G59" s="60"/>
       <c r="H59" s="47" t="s">
+        <v>830</v>
+      </c>
+      <c r="I59" s="47" t="s">
         <v>831</v>
-      </c>
-      <c r="I59" s="47" t="s">
-        <v>832</v>
       </c>
       <c r="J59" s="26"/>
       <c r="K59" s="27"/>
@@ -9474,7 +9474,7 @@
         <v>237</v>
       </c>
       <c r="S59" s="16" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="T59" s="25"/>
       <c r="U59" s="25"/>
@@ -9487,7 +9487,7 @@
         <v>181</v>
       </c>
       <c r="Z59" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="60" spans="1:26" ht="60">
@@ -9495,7 +9495,7 @@
         <v>55300009</v>
       </c>
       <c r="B60" s="53" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>48</v>
@@ -9505,10 +9505,10 @@
       <c r="F60" s="44"/>
       <c r="G60" s="60"/>
       <c r="H60" s="47" t="s">
+        <v>888</v>
+      </c>
+      <c r="I60" s="47" t="s">
         <v>889</v>
-      </c>
-      <c r="I60" s="47" t="s">
-        <v>890</v>
       </c>
       <c r="J60" s="26"/>
       <c r="K60" s="27"/>
@@ -9524,7 +9524,7 @@
         <v>237</v>
       </c>
       <c r="S60" s="16" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="T60" s="25"/>
       <c r="U60" s="25"/>
@@ -9534,10 +9534,10 @@
         <v>30</v>
       </c>
       <c r="Y60" s="25" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="Z60" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="61" spans="1:26" ht="36">
@@ -9545,7 +9545,7 @@
         <v>55300010</v>
       </c>
       <c r="B61" s="53" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>48</v>
@@ -9555,10 +9555,10 @@
       <c r="F61" s="44"/>
       <c r="G61" s="60"/>
       <c r="H61" s="47" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I61" s="47" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="J61" s="26"/>
       <c r="K61" s="27"/>
@@ -9574,7 +9574,7 @@
         <v>237</v>
       </c>
       <c r="S61" s="16" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="T61" s="25"/>
       <c r="U61" s="25"/>
@@ -9584,10 +9584,10 @@
         <v>35</v>
       </c>
       <c r="Y61" s="25" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="Z61" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="62" spans="1:26" ht="36">
@@ -9595,7 +9595,7 @@
         <v>55300011</v>
       </c>
       <c r="B62" s="53" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>48</v>
@@ -9605,10 +9605,10 @@
       <c r="F62" s="44"/>
       <c r="G62" s="60"/>
       <c r="H62" s="47" t="s">
+        <v>999</v>
+      </c>
+      <c r="I62" s="47" t="s">
         <v>1000</v>
-      </c>
-      <c r="I62" s="47" t="s">
-        <v>1001</v>
       </c>
       <c r="J62" s="26"/>
       <c r="K62" s="27"/>
@@ -9624,7 +9624,7 @@
         <v>237</v>
       </c>
       <c r="S62" s="16" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="T62" s="25"/>
       <c r="U62" s="25"/>
@@ -9634,10 +9634,10 @@
         <v>25</v>
       </c>
       <c r="Y62" s="25" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="Z62" s="48" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="63" spans="1:26" ht="36">
@@ -9645,7 +9645,7 @@
         <v>55300012</v>
       </c>
       <c r="B63" s="53" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>48</v>
@@ -9655,10 +9655,10 @@
       <c r="F63" s="44"/>
       <c r="G63" s="60"/>
       <c r="H63" s="47" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I63" s="47" t="s">
         <v>1007</v>
-      </c>
-      <c r="I63" s="47" t="s">
-        <v>1008</v>
       </c>
       <c r="J63" s="26"/>
       <c r="K63" s="27"/>
@@ -9674,7 +9674,7 @@
         <v>237</v>
       </c>
       <c r="S63" s="16" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="T63" s="25"/>
       <c r="U63" s="25"/>
@@ -9703,10 +9703,10 @@
       <c r="F64" s="43"/>
       <c r="G64" s="60"/>
       <c r="H64" s="47" t="s">
+        <v>1009</v>
+      </c>
+      <c r="I64" s="47" t="s">
         <v>1010</v>
-      </c>
-      <c r="I64" s="47" t="s">
-        <v>1011</v>
       </c>
       <c r="J64" s="28"/>
       <c r="K64" s="18"/>
@@ -9722,7 +9722,7 @@
         <v>237</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="T64" s="10"/>
       <c r="U64" s="1"/>
@@ -9805,7 +9805,7 @@
       <c r="L66" s="30"/>
       <c r="M66" s="17"/>
       <c r="N66" s="17" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="O66" s="20"/>
       <c r="P66" s="41"/>
@@ -9816,7 +9816,7 @@
         <v>237</v>
       </c>
       <c r="S66" s="10" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="T66" s="10"/>
       <c r="U66" s="1"/>
@@ -9862,7 +9862,7 @@
         <v>237</v>
       </c>
       <c r="S67" s="10" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="T67" s="10"/>
       <c r="U67" s="1"/>
@@ -10062,7 +10062,7 @@
         <v>237</v>
       </c>
       <c r="S71" s="16" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="T71" s="25"/>
       <c r="U71" s="25" t="s">
@@ -10100,7 +10100,7 @@
       <c r="M72" s="17"/>
       <c r="N72" s="17"/>
       <c r="O72" s="20" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="P72" s="41">
         <v>2</v>
@@ -10133,13 +10133,13 @@
         <v>55400007</v>
       </c>
       <c r="B73" s="54" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C73" s="25" t="s">
         <v>430</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E73" s="25">
         <v>10</v>
@@ -10149,7 +10149,7 @@
       </c>
       <c r="G73" s="60"/>
       <c r="H73" s="47" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="I73" s="47"/>
       <c r="J73" s="26"/>
@@ -10166,7 +10166,7 @@
         <v>237</v>
       </c>
       <c r="S73" s="16" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="T73" s="25"/>
       <c r="U73" s="25"/>
@@ -10176,7 +10176,7 @@
         <v>25</v>
       </c>
       <c r="Y73" s="25" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="Z73" s="48"/>
     </row>
@@ -10185,7 +10185,7 @@
         <v>55410001</v>
       </c>
       <c r="B74" s="54" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C74" s="25" t="s">
         <v>545</v>
@@ -10201,7 +10201,7 @@
       <c r="L74" s="30"/>
       <c r="M74" s="17"/>
       <c r="N74" s="17" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="O74" s="20"/>
       <c r="P74" s="41"/>
@@ -10212,7 +10212,7 @@
         <v>237</v>
       </c>
       <c r="S74" s="16" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="T74" s="25"/>
       <c r="U74" s="25" t="s">
@@ -10224,7 +10224,7 @@
         <v>50</v>
       </c>
       <c r="Y74" s="50" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="Z74" s="48"/>
     </row>
@@ -10729,7 +10729,7 @@
       </c>
       <c r="K85" s="27"/>
       <c r="L85" s="30" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="M85" s="17"/>
       <c r="N85" s="17"/>
@@ -11016,7 +11016,7 @@
       <c r="K91" s="18"/>
       <c r="L91" s="17"/>
       <c r="M91" s="17" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="N91" s="17"/>
       <c r="O91" s="20"/>
@@ -11691,7 +11691,7 @@
         <v>55520002</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>35</v>
@@ -11843,7 +11843,7 @@
       <c r="F109" s="43"/>
       <c r="G109" s="60"/>
       <c r="H109" s="29" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="I109" s="29"/>
       <c r="J109" s="28"/>
@@ -12033,7 +12033,7 @@
         <v>55600007</v>
       </c>
       <c r="B113" s="58" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>48</v>
@@ -12193,7 +12193,7 @@
       <c r="F116" s="43"/>
       <c r="G116" s="60"/>
       <c r="H116" s="29" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I116" s="29"/>
       <c r="J116" s="28"/>
@@ -12243,7 +12243,7 @@
       <c r="F117" s="43"/>
       <c r="G117" s="60"/>
       <c r="H117" s="29" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="I117" s="29"/>
       <c r="J117" s="28"/>
@@ -12260,7 +12260,7 @@
         <v>403</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="T117" s="10">
         <v>56000023</v>
@@ -12268,7 +12268,7 @@
       <c r="U117" s="1"/>
       <c r="V117" s="1"/>
       <c r="W117" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="X117" s="1">
         <v>20</v>
@@ -12333,7 +12333,7 @@
         <v>55600013</v>
       </c>
       <c r="B119" s="58" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>48</v>
@@ -12343,7 +12343,7 @@
       <c r="F119" s="43"/>
       <c r="G119" s="60"/>
       <c r="H119" s="29" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I119" s="29"/>
       <c r="J119" s="28"/>
@@ -12360,7 +12360,7 @@
         <v>237</v>
       </c>
       <c r="S119" s="1" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="T119" s="10">
         <v>56000001</v>
@@ -12383,7 +12383,7 @@
         <v>55600014</v>
       </c>
       <c r="B120" s="58" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>48</v>
@@ -12393,7 +12393,7 @@
       <c r="F120" s="43"/>
       <c r="G120" s="60"/>
       <c r="H120" s="29" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="I120" s="29"/>
       <c r="J120" s="28"/>
@@ -12424,7 +12424,7 @@
         <v>30</v>
       </c>
       <c r="Y120" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="Z120" s="37"/>
     </row>
@@ -12433,7 +12433,7 @@
         <v>55600015</v>
       </c>
       <c r="B121" s="58" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>48</v>
@@ -12443,7 +12443,7 @@
       <c r="F121" s="43"/>
       <c r="G121" s="60"/>
       <c r="H121" s="29" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I121" s="29"/>
       <c r="J121" s="28"/>
@@ -12460,7 +12460,7 @@
         <v>237</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="T121" s="10">
         <v>56000101</v>
@@ -12474,7 +12474,7 @@
         <v>10</v>
       </c>
       <c r="Y121" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Z121" s="37"/>
     </row>
@@ -12483,7 +12483,7 @@
         <v>55600016</v>
       </c>
       <c r="B122" s="58" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>48</v>
@@ -12493,7 +12493,7 @@
       <c r="F122" s="43"/>
       <c r="G122" s="60"/>
       <c r="H122" s="29" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I122" s="29"/>
       <c r="J122" s="28"/>
@@ -12510,7 +12510,7 @@
         <v>237</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="T122" s="10">
         <v>56000101</v>
@@ -12524,7 +12524,7 @@
         <v>15</v>
       </c>
       <c r="Y122" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="Z122" s="37"/>
     </row>
@@ -12736,7 +12736,7 @@
       <c r="K127" s="18"/>
       <c r="L127" s="17"/>
       <c r="M127" s="17" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="N127" s="17"/>
       <c r="O127" s="20"/>
@@ -12833,7 +12833,7 @@
       <c r="L129" s="17"/>
       <c r="M129" s="17"/>
       <c r="N129" s="17" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="O129" s="20"/>
       <c r="P129" s="41"/>
@@ -12871,7 +12871,7 @@
         <v>126</v>
       </c>
       <c r="D130" s="25" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="E130" s="25">
         <v>12</v>
@@ -12881,7 +12881,7 @@
       </c>
       <c r="G130" s="60"/>
       <c r="H130" s="29" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I130" s="29"/>
       <c r="J130" s="28"/>
@@ -12898,14 +12898,14 @@
         <v>237</v>
       </c>
       <c r="S130" s="10" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="T130" s="10"/>
       <c r="U130" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="W130" s="1"/>
       <c r="X130" s="1">
@@ -12923,7 +12923,7 @@
         <v>55700005</v>
       </c>
       <c r="B131" s="52" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C131" s="25" t="s">
         <v>402</v>
@@ -12940,7 +12940,7 @@
       <c r="M131" s="17"/>
       <c r="N131" s="17"/>
       <c r="O131" s="20" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="P131" s="41">
         <v>1</v>
@@ -12952,7 +12952,7 @@
         <v>403</v>
       </c>
       <c r="S131" s="16" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="T131" s="25"/>
       <c r="U131" s="25"/>
@@ -12989,7 +12989,7 @@
       </c>
       <c r="G132" s="60"/>
       <c r="H132" s="93" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="I132" s="29"/>
       <c r="J132" s="26"/>
@@ -13047,7 +13047,7 @@
       </c>
       <c r="G133" s="60"/>
       <c r="H133" s="47" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I133" s="47"/>
       <c r="J133" s="26"/>
@@ -13095,7 +13095,7 @@
       <c r="F134" s="44"/>
       <c r="G134" s="60"/>
       <c r="H134" s="47" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I134" s="47"/>
       <c r="J134" s="26"/>
@@ -13319,7 +13319,7 @@
         <v>55900008</v>
       </c>
       <c r="B139" s="55" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>0</v>
@@ -13356,7 +13356,7 @@
         <v>40</v>
       </c>
       <c r="Y139" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="Z139" s="48"/>
     </row>
@@ -13365,7 +13365,7 @@
         <v>55900009</v>
       </c>
       <c r="B140" s="55" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>0</v>
@@ -13374,7 +13374,7 @@
       <c r="E140" s="1"/>
       <c r="F140" s="43"/>
       <c r="G140" s="60" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="H140" s="29"/>
       <c r="I140" s="29"/>
@@ -13392,7 +13392,7 @@
         <v>237</v>
       </c>
       <c r="S140" s="10" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="T140" s="10"/>
       <c r="U140" s="1"/>
@@ -13402,7 +13402,7 @@
         <v>30</v>
       </c>
       <c r="Y140" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="Z140" s="37"/>
     </row>
@@ -13411,7 +13411,7 @@
         <v>55900010</v>
       </c>
       <c r="B141" s="55" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>0</v>
@@ -13420,7 +13420,7 @@
       <c r="E141" s="1"/>
       <c r="F141" s="43"/>
       <c r="G141" s="60" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H141" s="29"/>
       <c r="I141" s="29"/>
@@ -13438,7 +13438,7 @@
         <v>237</v>
       </c>
       <c r="S141" s="10" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="T141" s="1"/>
       <c r="U141" s="1"/>
@@ -13457,7 +13457,7 @@
         <v>55900011</v>
       </c>
       <c r="B142" s="55" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>0</v>
@@ -13467,7 +13467,7 @@
       <c r="F142" s="43"/>
       <c r="G142" s="60"/>
       <c r="H142" s="29" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I142" s="29"/>
       <c r="J142" s="28"/>
@@ -13484,7 +13484,7 @@
         <v>237</v>
       </c>
       <c r="S142" s="10" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="T142" s="10"/>
       <c r="U142" s="1"/>
@@ -13503,7 +13503,7 @@
         <v>55900012</v>
       </c>
       <c r="B143" s="55" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C143" s="25" t="s">
         <v>336</v>
@@ -13519,7 +13519,7 @@
       </c>
       <c r="G143" s="60"/>
       <c r="H143" s="47" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I143" s="47"/>
       <c r="J143" s="26"/>
@@ -13536,12 +13536,12 @@
         <v>237</v>
       </c>
       <c r="S143" s="16" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="T143" s="25"/>
       <c r="U143" s="25"/>
       <c r="V143" s="25" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="W143" s="25"/>
       <c r="X143" s="25">
@@ -13557,7 +13557,7 @@
         <v>55900013</v>
       </c>
       <c r="B144" s="55" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>0</v>
@@ -13569,7 +13569,7 @@
       <c r="H144" s="29"/>
       <c r="I144" s="29"/>
       <c r="J144" s="28" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="K144" s="18"/>
       <c r="L144" s="17" t="s">
@@ -13605,7 +13605,7 @@
         <v>55900014</v>
       </c>
       <c r="B145" s="55" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>0</v>
@@ -13623,7 +13623,7 @@
       <c r="L145" s="17"/>
       <c r="M145" s="17"/>
       <c r="N145" s="17" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="O145" s="20"/>
       <c r="P145" s="41"/>
@@ -13634,7 +13634,7 @@
         <v>237</v>
       </c>
       <c r="S145" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="T145" s="1"/>
       <c r="U145" s="1"/>
@@ -13653,7 +13653,7 @@
         <v>55900015</v>
       </c>
       <c r="B146" s="55" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>0</v>
@@ -13699,7 +13699,7 @@
         <v>55900016</v>
       </c>
       <c r="B147" s="55" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>336</v>
@@ -13730,7 +13730,7 @@
         <v>237</v>
       </c>
       <c r="S147" s="10" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="T147" s="10"/>
       <c r="U147" s="1" t="s">
@@ -13742,7 +13742,7 @@
         <v>45</v>
       </c>
       <c r="Y147" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="Z147" s="48"/>
     </row>
@@ -13751,7 +13751,7 @@
         <v>55900017</v>
       </c>
       <c r="B148" s="55" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>336</v>
@@ -13768,7 +13768,7 @@
       <c r="M148" s="21"/>
       <c r="N148" s="21"/>
       <c r="O148" s="20" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="P148" s="41">
         <v>1</v>
@@ -13803,7 +13803,7 @@
         <v>55900018</v>
       </c>
       <c r="B149" s="55" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>336</v>
@@ -13820,7 +13820,7 @@
       <c r="M149" s="21"/>
       <c r="N149" s="21"/>
       <c r="O149" s="19" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="P149" s="41">
         <v>1</v>
@@ -13855,7 +13855,7 @@
         <v>55900019</v>
       </c>
       <c r="B150" s="55" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>336</v>
@@ -13872,7 +13872,7 @@
       <c r="M150" s="21"/>
       <c r="N150" s="21"/>
       <c r="O150" s="20" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="P150" s="41">
         <v>1</v>
@@ -13907,7 +13907,7 @@
         <v>55900020</v>
       </c>
       <c r="B151" s="55" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C151" s="25" t="s">
         <v>0</v>
@@ -13917,7 +13917,7 @@
       <c r="F151" s="44"/>
       <c r="G151" s="79"/>
       <c r="H151" s="29" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="I151" s="95"/>
       <c r="J151" s="96"/>
@@ -13934,7 +13934,7 @@
         <v>237</v>
       </c>
       <c r="S151" s="10" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="T151" s="78"/>
       <c r="U151" s="78"/>
@@ -13944,7 +13944,7 @@
         <v>20</v>
       </c>
       <c r="Y151" s="25" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="Z151" s="83"/>
     </row>
@@ -13953,7 +13953,7 @@
         <v>55900021</v>
       </c>
       <c r="B152" s="55" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C152" s="25" t="s">
         <v>0</v>
@@ -14001,13 +14001,13 @@
         <v>55900022</v>
       </c>
       <c r="B153" s="55" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C153" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D153" s="25" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E153" s="25">
         <v>200</v>
@@ -14017,7 +14017,7 @@
       </c>
       <c r="G153" s="60"/>
       <c r="H153" s="84" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I153" s="47"/>
       <c r="J153" s="26"/>
@@ -14034,7 +14034,7 @@
         <v>403</v>
       </c>
       <c r="S153" s="16" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="T153" s="25"/>
       <c r="U153" s="25" t="s">
@@ -14060,14 +14060,14 @@
         <v>147</v>
       </c>
       <c r="C154" s="25" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25"/>
       <c r="F154" s="25"/>
       <c r="G154" s="60"/>
       <c r="H154" s="84" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I154" s="47"/>
       <c r="J154" s="26"/>
@@ -14084,7 +14084,7 @@
         <v>403</v>
       </c>
       <c r="S154" s="16" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="T154" s="25"/>
       <c r="U154" s="25"/>
@@ -14119,7 +14119,7 @@
       </c>
       <c r="G155" s="60"/>
       <c r="H155" s="84" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="I155" s="47"/>
       <c r="J155" s="26"/>
@@ -14136,7 +14136,7 @@
         <v>403</v>
       </c>
       <c r="S155" s="10" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="T155" s="25"/>
       <c r="U155" s="25"/>
@@ -14178,7 +14178,7 @@
       <c r="M156" s="17"/>
       <c r="N156" s="17"/>
       <c r="O156" s="20" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="P156" s="41">
         <v>2</v>
@@ -14190,7 +14190,7 @@
         <v>403</v>
       </c>
       <c r="S156" s="16" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="T156" s="25"/>
       <c r="U156" s="25" t="s">
@@ -14229,7 +14229,7 @@
       <c r="L157" s="30"/>
       <c r="M157" s="17"/>
       <c r="N157" s="17" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="O157" s="20"/>
       <c r="P157" s="41"/>
@@ -14240,7 +14240,7 @@
         <v>403</v>
       </c>
       <c r="S157" s="16" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="T157" s="25"/>
       <c r="U157" s="25"/>
@@ -14253,7 +14253,7 @@
         <v>189</v>
       </c>
       <c r="Z157" s="48" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="158" spans="1:26" ht="36">
@@ -14261,7 +14261,7 @@
         <v>55900027</v>
       </c>
       <c r="B158" s="55" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C158" s="25" t="s">
         <v>0</v>
@@ -14275,10 +14275,10 @@
       <c r="J158" s="26"/>
       <c r="K158" s="27"/>
       <c r="L158" s="30" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="M158" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N158" s="17"/>
       <c r="O158" s="20"/>
@@ -14290,7 +14290,7 @@
         <v>403</v>
       </c>
       <c r="S158" s="16" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="T158" s="25"/>
       <c r="U158" s="25"/>
@@ -14319,7 +14319,7 @@
       <c r="F159" s="44"/>
       <c r="G159" s="60"/>
       <c r="H159" s="84" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I159" s="47"/>
       <c r="J159" s="26"/>
@@ -14336,7 +14336,7 @@
         <v>403</v>
       </c>
       <c r="S159" s="16" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="T159" s="25"/>
       <c r="U159" s="25"/>
@@ -14363,7 +14363,7 @@
       <c r="F160" s="25"/>
       <c r="G160" s="60"/>
       <c r="H160" s="84" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="I160" s="47"/>
       <c r="J160" s="26"/>
@@ -14380,7 +14380,7 @@
         <v>403</v>
       </c>
       <c r="S160" s="16" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="T160" s="25"/>
       <c r="U160" s="25"/>
@@ -14390,7 +14390,7 @@
         <v>15</v>
       </c>
       <c r="Y160" s="25" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="Z160" s="48"/>
     </row>
@@ -14411,12 +14411,12 @@
       <c r="H161" s="84"/>
       <c r="I161" s="47"/>
       <c r="J161" s="26" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="K161" s="27"/>
       <c r="L161" s="30"/>
       <c r="M161" s="17" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="N161" s="17"/>
       <c r="O161" s="20"/>
@@ -14449,7 +14449,7 @@
         <v>55900031</v>
       </c>
       <c r="B162" s="55" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C162" s="25" t="s">
         <v>0</v>
@@ -14459,7 +14459,7 @@
       <c r="F162" s="25"/>
       <c r="G162" s="60"/>
       <c r="H162" s="84" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="I162" s="47"/>
       <c r="J162" s="26"/>
@@ -14476,7 +14476,7 @@
         <v>403</v>
       </c>
       <c r="S162" s="16" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="T162" s="25"/>
       <c r="U162" s="25"/>
@@ -14486,7 +14486,7 @@
         <v>5</v>
       </c>
       <c r="Y162" s="25" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="Z162" s="48"/>
     </row>
@@ -14495,13 +14495,13 @@
         <v>55900032</v>
       </c>
       <c r="B163" s="55" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C163" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D163" s="25" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E163" s="25">
         <v>12</v>
@@ -14511,7 +14511,7 @@
       </c>
       <c r="G163" s="60"/>
       <c r="H163" s="84" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="I163" s="47"/>
       <c r="J163" s="26"/>
@@ -14528,11 +14528,11 @@
         <v>403</v>
       </c>
       <c r="S163" s="16" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="T163" s="25"/>
       <c r="U163" s="25" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="V163" s="25"/>
       <c r="W163" s="25"/>
@@ -14540,7 +14540,7 @@
         <v>20</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="Z163" s="48"/>
     </row>
@@ -14549,7 +14549,7 @@
         <v>55900033</v>
       </c>
       <c r="B164" s="55" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C164" s="25" t="s">
         <v>0</v>
@@ -14561,11 +14561,11 @@
       <c r="H164" s="93"/>
       <c r="I164" s="29"/>
       <c r="J164" s="26" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="K164" s="27"/>
       <c r="L164" s="30" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="M164" s="17"/>
       <c r="N164" s="17"/>
@@ -14578,7 +14578,7 @@
         <v>403</v>
       </c>
       <c r="S164" s="16" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25"/>
@@ -14588,7 +14588,7 @@
         <v>20</v>
       </c>
       <c r="Y164" s="25" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="Z164" s="48"/>
     </row>
@@ -14597,7 +14597,7 @@
         <v>55900034</v>
       </c>
       <c r="B165" s="55" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C165" s="25" t="s">
         <v>0</v>
@@ -14613,7 +14613,7 @@
       <c r="L165" s="30"/>
       <c r="M165" s="17"/>
       <c r="N165" s="17" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O165" s="20"/>
       <c r="P165" s="41"/>
@@ -14624,7 +14624,7 @@
         <v>403</v>
       </c>
       <c r="S165" s="16" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="T165" s="25"/>
       <c r="U165" s="25"/>
@@ -14634,7 +14634,7 @@
         <v>14</v>
       </c>
       <c r="Y165" s="25" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Z165" s="48"/>
     </row>
@@ -14643,7 +14643,7 @@
         <v>55900035</v>
       </c>
       <c r="B166" s="55" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C166" s="25" t="s">
         <v>0</v>
@@ -14653,7 +14653,7 @@
       <c r="F166" s="25"/>
       <c r="G166" s="60"/>
       <c r="H166" s="84" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I166" s="47"/>
       <c r="J166" s="26"/>
@@ -14670,7 +14670,7 @@
         <v>403</v>
       </c>
       <c r="S166" s="16" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="T166" s="25"/>
       <c r="U166" s="25"/>
@@ -14680,7 +14680,7 @@
         <v>14</v>
       </c>
       <c r="Y166" s="25" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="Z166" s="48"/>
     </row>
@@ -14689,13 +14689,13 @@
         <v>55900036</v>
       </c>
       <c r="B167" s="55" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D167" s="25" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E167" s="25">
         <v>50</v>
@@ -14705,7 +14705,7 @@
       </c>
       <c r="G167" s="60"/>
       <c r="H167" s="84" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="I167" s="47"/>
       <c r="J167" s="26"/>
@@ -14722,11 +14722,11 @@
         <v>403</v>
       </c>
       <c r="S167" s="16" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="T167" s="25"/>
       <c r="U167" s="25" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="V167" s="25"/>
       <c r="W167" s="25"/>
@@ -14734,7 +14734,7 @@
         <v>50</v>
       </c>
       <c r="Y167" s="25" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="Z167" s="48"/>
     </row>
@@ -14743,7 +14743,7 @@
         <v>55900037</v>
       </c>
       <c r="B168" s="55" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C168" s="25" t="s">
         <v>0</v>
@@ -14759,7 +14759,7 @@
       </c>
       <c r="G168" s="60"/>
       <c r="H168" s="93" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I168" s="29"/>
       <c r="J168" s="26"/>
@@ -14776,7 +14776,7 @@
         <v>403</v>
       </c>
       <c r="S168" s="10" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="T168" s="25"/>
       <c r="U168" s="25"/>
@@ -14786,7 +14786,7 @@
         <v>35</v>
       </c>
       <c r="Y168" s="25" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="Z168" s="48"/>
     </row>
@@ -14795,7 +14795,7 @@
         <v>55900038</v>
       </c>
       <c r="B169" s="55" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C169" s="25" t="s">
         <v>0</v>
@@ -14811,7 +14811,7 @@
       </c>
       <c r="G169" s="60"/>
       <c r="H169" s="29" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I169" s="29"/>
       <c r="J169" s="26"/>
@@ -14828,21 +14828,21 @@
         <v>403</v>
       </c>
       <c r="S169" s="10" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="T169" s="25"/>
       <c r="U169" s="25" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="V169" s="25" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="W169" s="25"/>
       <c r="X169" s="25">
         <v>40</v>
       </c>
       <c r="Y169" s="25" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="Z169" s="48"/>
     </row>
@@ -14851,7 +14851,7 @@
         <v>55900039</v>
       </c>
       <c r="B170" s="55" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C170" s="25" t="s">
         <v>0</v>
@@ -14861,10 +14861,10 @@
       <c r="F170" s="43"/>
       <c r="G170" s="59"/>
       <c r="H170" s="29" t="s">
+        <v>928</v>
+      </c>
+      <c r="I170" s="29" t="s">
         <v>929</v>
-      </c>
-      <c r="I170" s="29" t="s">
-        <v>930</v>
       </c>
       <c r="J170" s="26"/>
       <c r="K170" s="27"/>
@@ -14880,7 +14880,7 @@
         <v>237</v>
       </c>
       <c r="S170" s="10" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="T170" s="10"/>
       <c r="U170" s="1"/>
@@ -14892,7 +14892,7 @@
         <v>40</v>
       </c>
       <c r="Y170" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="Z170" s="25"/>
     </row>
@@ -14901,13 +14901,13 @@
         <v>55900040</v>
       </c>
       <c r="B171" s="55" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C171" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D171" s="25" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E171" s="25">
         <v>100</v>
@@ -14917,7 +14917,7 @@
       </c>
       <c r="G171" s="60"/>
       <c r="H171" s="29" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I171" s="29"/>
       <c r="J171" s="28"/>
@@ -14934,21 +14934,21 @@
         <v>403</v>
       </c>
       <c r="S171" s="10" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="T171" s="25"/>
       <c r="U171" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="V171" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="W171" s="25"/>
       <c r="X171" s="25">
         <v>30</v>
       </c>
       <c r="Y171" s="25" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="Z171" s="39"/>
     </row>
@@ -14957,13 +14957,13 @@
         <v>55900041</v>
       </c>
       <c r="B172" s="55" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C172" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D172" s="25" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E172" s="25">
         <v>100</v>
@@ -14973,7 +14973,7 @@
       </c>
       <c r="G172" s="60"/>
       <c r="H172" s="29" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I172" s="29"/>
       <c r="J172" s="26"/>
@@ -14990,11 +14990,11 @@
         <v>403</v>
       </c>
       <c r="S172" s="10" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="T172" s="25"/>
       <c r="U172" s="25" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="V172" s="25"/>
       <c r="W172" s="25"/>
@@ -15002,7 +15002,7 @@
         <v>0</v>
       </c>
       <c r="Y172" s="25" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Z172" s="48"/>
     </row>
@@ -15011,7 +15011,7 @@
         <v>55900042</v>
       </c>
       <c r="B173" s="55" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C173" s="25" t="s">
         <v>0</v>
@@ -15027,7 +15027,7 @@
       <c r="L173" s="30"/>
       <c r="M173" s="17"/>
       <c r="N173" s="17" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="O173" s="20"/>
       <c r="P173" s="41"/>
@@ -15038,7 +15038,7 @@
         <v>403</v>
       </c>
       <c r="S173" s="10" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="T173" s="25"/>
       <c r="U173" s="25"/>
@@ -15048,7 +15048,7 @@
         <v>25</v>
       </c>
       <c r="Y173" s="25" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Z173" s="48"/>
     </row>
@@ -15057,7 +15057,7 @@
         <v>55900043</v>
       </c>
       <c r="B174" s="55" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C174" s="25" t="s">
         <v>0</v>
@@ -15074,7 +15074,7 @@
       <c r="M174" s="17"/>
       <c r="N174" s="17"/>
       <c r="O174" s="20" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="P174" s="41">
         <v>1</v>
@@ -15086,7 +15086,7 @@
         <v>403</v>
       </c>
       <c r="S174" s="10" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="T174" s="25"/>
       <c r="U174" s="25"/>
@@ -15096,7 +15096,7 @@
         <v>30</v>
       </c>
       <c r="Y174" s="25" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="Z174" s="48"/>
     </row>
@@ -15105,7 +15105,7 @@
         <v>55900044</v>
       </c>
       <c r="B175" s="55" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C175" s="25" t="s">
         <v>0</v>
@@ -15122,7 +15122,7 @@
       <c r="M175" s="17"/>
       <c r="N175" s="17"/>
       <c r="O175" s="20" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="P175" s="41">
         <v>2</v>
@@ -15134,7 +15134,7 @@
         <v>403</v>
       </c>
       <c r="S175" s="10" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="T175" s="25"/>
       <c r="U175" s="25"/>
@@ -15144,7 +15144,7 @@
         <v>40</v>
       </c>
       <c r="Y175" s="25" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="Z175" s="48"/>
     </row>
@@ -15153,13 +15153,13 @@
         <v>55900045</v>
       </c>
       <c r="B176" s="55" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C176" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D176" s="25" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E176" s="25">
         <v>100</v>
@@ -15169,7 +15169,7 @@
       </c>
       <c r="G176" s="60"/>
       <c r="H176" s="93" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I176" s="29"/>
       <c r="J176" s="26"/>
@@ -15186,7 +15186,7 @@
         <v>403</v>
       </c>
       <c r="S176" s="10" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="T176" s="25"/>
       <c r="U176" s="25"/>
@@ -15196,7 +15196,7 @@
         <v>25</v>
       </c>
       <c r="Y176" s="25" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="Z176" s="48"/>
     </row>
@@ -15205,13 +15205,13 @@
         <v>55900046</v>
       </c>
       <c r="B177" s="55" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C177" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D177" s="25" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="E177" s="25">
         <v>20</v>
@@ -15221,7 +15221,7 @@
       </c>
       <c r="G177" s="60"/>
       <c r="H177" s="93" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I177" s="29"/>
       <c r="J177" s="26"/>
@@ -15238,21 +15238,21 @@
         <v>403</v>
       </c>
       <c r="S177" s="16" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="T177" s="25"/>
       <c r="U177" s="25" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="V177" s="25" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="W177" s="25"/>
       <c r="X177" s="25">
         <v>25</v>
       </c>
       <c r="Y177" s="25" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="Z177" s="48"/>
     </row>
@@ -15261,13 +15261,13 @@
         <v>55900047</v>
       </c>
       <c r="B178" s="55" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C178" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D178" s="25" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E178" s="25">
         <v>15</v>
@@ -15277,7 +15277,7 @@
       </c>
       <c r="G178" s="60"/>
       <c r="H178" s="93" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="I178" s="29"/>
       <c r="J178" s="26"/>
@@ -15294,21 +15294,21 @@
         <v>403</v>
       </c>
       <c r="S178" s="16" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="T178" s="25"/>
       <c r="U178" s="25" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="V178" s="25" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="W178" s="25"/>
       <c r="X178" s="25">
         <v>30</v>
       </c>
       <c r="Y178" s="25" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="Z178" s="48"/>
     </row>
@@ -15317,7 +15317,7 @@
         <v>55900048</v>
       </c>
       <c r="B179" s="55" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C179" s="25" t="s">
         <v>402</v>
@@ -15332,7 +15332,7 @@
       <c r="K179" s="27"/>
       <c r="L179" s="30"/>
       <c r="M179" s="17" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="N179" s="17"/>
       <c r="O179" s="20"/>
@@ -15344,7 +15344,7 @@
         <v>403</v>
       </c>
       <c r="S179" s="16" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="T179" s="25"/>
       <c r="U179" s="25"/>
@@ -15354,7 +15354,7 @@
         <v>70</v>
       </c>
       <c r="Y179" s="25" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="Z179" s="48"/>
     </row>
@@ -15363,7 +15363,7 @@
         <v>55900049</v>
       </c>
       <c r="B180" s="55" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C180" s="25" t="s">
         <v>402</v>
@@ -15375,13 +15375,13 @@
       <c r="H180" s="29"/>
       <c r="I180" s="29"/>
       <c r="J180" s="28" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="K180" s="18" t="s">
         <v>538</v>
       </c>
       <c r="L180" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="M180" s="17"/>
       <c r="N180" s="17"/>
@@ -15394,7 +15394,7 @@
         <v>237</v>
       </c>
       <c r="S180" s="15" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="T180" s="36"/>
       <c r="U180" s="1"/>
@@ -15416,7 +15416,7 @@
         <v>23</v>
       </c>
       <c r="C181" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D181" s="25"/>
       <c r="E181" s="25"/>
@@ -15455,7 +15455,7 @@
         <v>24</v>
       </c>
       <c r="Z181" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="182" spans="1:26" ht="36">
@@ -15466,7 +15466,7 @@
         <v>25</v>
       </c>
       <c r="C182" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D182" s="25"/>
       <c r="E182" s="25"/>
@@ -15505,7 +15505,7 @@
         <v>26</v>
       </c>
       <c r="Z182" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="183" spans="1:26" ht="36">
@@ -15516,7 +15516,7 @@
         <v>27</v>
       </c>
       <c r="C183" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D183" s="25"/>
       <c r="E183" s="25"/>
@@ -15555,7 +15555,7 @@
         <v>28</v>
       </c>
       <c r="Z183" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="184" spans="1:26" ht="36">
@@ -15566,7 +15566,7 @@
         <v>29</v>
       </c>
       <c r="C184" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D184" s="25"/>
       <c r="E184" s="25"/>
@@ -15605,7 +15605,7 @@
         <v>30</v>
       </c>
       <c r="Z184" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="185" spans="1:26" ht="36">
@@ -15616,7 +15616,7 @@
         <v>31</v>
       </c>
       <c r="C185" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D185" s="25"/>
       <c r="E185" s="25"/>
@@ -15655,7 +15655,7 @@
         <v>32</v>
       </c>
       <c r="Z185" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="186" spans="1:26" ht="36">
@@ -15666,7 +15666,7 @@
         <v>33</v>
       </c>
       <c r="C186" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25"/>
@@ -15705,7 +15705,7 @@
         <v>34</v>
       </c>
       <c r="Z186" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="187" spans="1:26" ht="36">
@@ -15716,7 +15716,7 @@
         <v>54</v>
       </c>
       <c r="C187" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D187" s="25"/>
       <c r="E187" s="25"/>
@@ -15755,7 +15755,7 @@
         <v>55</v>
       </c>
       <c r="Z187" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="188" spans="1:26" ht="36">
@@ -15766,7 +15766,7 @@
         <v>56</v>
       </c>
       <c r="C188" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25"/>
@@ -15805,7 +15805,7 @@
         <v>57</v>
       </c>
       <c r="Z188" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="189" spans="1:26" ht="36">
@@ -15816,7 +15816,7 @@
         <v>58</v>
       </c>
       <c r="C189" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25"/>
@@ -15855,7 +15855,7 @@
         <v>59</v>
       </c>
       <c r="Z189" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="190" spans="1:26" ht="36">
@@ -15866,7 +15866,7 @@
         <v>60</v>
       </c>
       <c r="C190" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D190" s="25"/>
       <c r="E190" s="25"/>
@@ -15905,7 +15905,7 @@
         <v>61</v>
       </c>
       <c r="Z190" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="191" spans="1:26" ht="36">
@@ -15916,7 +15916,7 @@
         <v>62</v>
       </c>
       <c r="C191" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25"/>
@@ -15955,7 +15955,7 @@
         <v>63</v>
       </c>
       <c r="Z191" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="192" spans="1:26" ht="36">
@@ -15966,7 +15966,7 @@
         <v>64</v>
       </c>
       <c r="C192" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D192" s="25"/>
       <c r="E192" s="25"/>
@@ -16005,7 +16005,7 @@
         <v>65</v>
       </c>
       <c r="Z192" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="193" spans="1:26" ht="24">
@@ -16013,17 +16013,17 @@
         <v>55990101</v>
       </c>
       <c r="B193" s="94" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C193" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D193" s="25"/>
       <c r="E193" s="25"/>
       <c r="F193" s="44"/>
       <c r="G193" s="60"/>
       <c r="H193" s="84" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="I193" s="47"/>
       <c r="J193" s="26"/>
@@ -16040,7 +16040,7 @@
         <v>237</v>
       </c>
       <c r="S193" s="49" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="T193" s="25"/>
       <c r="U193" s="25"/>
@@ -16053,7 +16053,7 @@
         <v>107</v>
       </c>
       <c r="Z193" s="48" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="194" spans="1:26" ht="28.8">
@@ -16061,10 +16061,10 @@
         <v>55990102</v>
       </c>
       <c r="B194" s="94" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C194" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25"/>
@@ -16073,11 +16073,11 @@
       <c r="H194" s="84"/>
       <c r="I194" s="47"/>
       <c r="J194" s="26" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="K194" s="27"/>
       <c r="L194" s="30" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="M194" s="17"/>
       <c r="N194" s="17"/>
@@ -16090,7 +16090,7 @@
         <v>237</v>
       </c>
       <c r="S194" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="T194" s="25"/>
       <c r="U194" s="25"/>
@@ -16100,10 +16100,10 @@
         <v>25</v>
       </c>
       <c r="Y194" s="25" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="Z194" s="48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="195" spans="1:26" ht="72">
@@ -16111,7 +16111,7 @@
         <v>55990103</v>
       </c>
       <c r="B195" s="94" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C195" s="25" t="s">
         <v>97</v>
@@ -16129,7 +16129,7 @@
       <c r="H195" s="84"/>
       <c r="I195" s="47"/>
       <c r="J195" s="26" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K195" s="27"/>
       <c r="L195" s="30"/>
@@ -16146,24 +16146,24 @@
         <v>237</v>
       </c>
       <c r="S195" s="16" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="T195" s="25"/>
       <c r="U195" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="V195" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="W195" s="25"/>
       <c r="X195" s="25">
         <v>35</v>
       </c>
       <c r="Y195" s="25" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="Z195" s="48" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="196" spans="1:26" ht="72">
@@ -16171,7 +16171,7 @@
         <v>55990104</v>
       </c>
       <c r="B196" s="94" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C196" s="25" t="s">
         <v>97</v>
@@ -16189,7 +16189,7 @@
       <c r="H196" s="84"/>
       <c r="I196" s="47"/>
       <c r="J196" s="26" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K196" s="27"/>
       <c r="L196" s="30"/>
@@ -16206,24 +16206,24 @@
         <v>237</v>
       </c>
       <c r="S196" s="16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="T196" s="25"/>
       <c r="U196" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="V196" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="W196" s="25"/>
       <c r="X196" s="25">
         <v>50</v>
       </c>
       <c r="Y196" s="25" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="Z196" s="48" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="197" spans="1:26">
@@ -16231,10 +16231,10 @@
         <v>55990105</v>
       </c>
       <c r="B197" s="94" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C197" s="25" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -16246,7 +16246,7 @@
       <c r="K197" s="27"/>
       <c r="L197" s="30"/>
       <c r="M197" s="17" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="N197" s="17"/>
       <c r="O197" s="20"/>
@@ -16258,7 +16258,7 @@
         <v>237</v>
       </c>
       <c r="S197" s="10" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="T197" s="10"/>
       <c r="U197" s="1"/>
@@ -16268,7 +16268,7 @@
         <v>150</v>
       </c>
       <c r="Y197" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="Z197" s="25"/>
     </row>

</xml_diff>

<commit_message>
SetToPosition add a step parameter can dicide the distance of move
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -2714,18 +2714,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>召唤时将范围内的所有目标传到临近行</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.SetToPosition("side");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>NAW</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2814,9 +2806,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>d.SetToPosition("back");</t>
-  </si>
-  <si>
     <t>damage.SetPDamageRate(1.5);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3947,6 +3936,18 @@
   </si>
   <si>
     <t>s.Summon("around",s.CardId,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.SetToPosition("side",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.SetToPosition("back",1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6447,11 +6448,11 @@
   <dimension ref="A1:Z200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C155" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="M159" sqref="M159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6577,7 +6578,7 @@
         <v>541</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>338</v>
@@ -6595,7 +6596,7 @@
         <v>609</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>307</v>
@@ -6651,7 +6652,7 @@
         <v>453</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="G3" s="40" t="s">
         <v>542</v>
@@ -6675,10 +6676,10 @@
         <v>302</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>433</v>
@@ -6699,7 +6700,7 @@
         <v>318</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>343</v>
@@ -6722,7 +6723,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -6770,7 +6771,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -6779,7 +6780,7 @@
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
       <c r="J5" s="28" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="K5" s="18" t="s">
         <v>533</v>
@@ -6798,7 +6799,7 @@
         <v>237</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="T5" s="36"/>
       <c r="U5" s="1"/>
@@ -6820,7 +6821,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -6829,7 +6830,7 @@
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
       <c r="J6" s="28" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="K6" s="18" t="s">
         <v>532</v>
@@ -6848,7 +6849,7 @@
         <v>237</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="1"/>
@@ -6870,7 +6871,7 @@
         <v>547</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -6918,7 +6919,7 @@
         <v>543</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -6964,14 +6965,14 @@
         <v>551</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D9" s="61"/>
       <c r="E9" s="61"/>
       <c r="F9" s="62"/>
       <c r="G9" s="59"/>
       <c r="H9" s="29" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="I9" s="63"/>
       <c r="J9" s="64"/>
@@ -7010,7 +7011,7 @@
         <v>552</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>451</v>
@@ -7046,10 +7047,10 @@
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="25" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="V10" s="25" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="61">
@@ -7068,22 +7069,22 @@
         <v>553</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="E11" s="25">
         <v>30</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="G11" s="60" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="H11" s="93" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="I11" s="29"/>
       <c r="J11" s="26"/>
@@ -7122,14 +7123,14 @@
         <v>562</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="43"/>
       <c r="G12" s="59"/>
       <c r="H12" s="29" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="I12" s="29"/>
       <c r="J12" s="28"/>
@@ -7170,7 +7171,7 @@
         <v>639</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -7179,7 +7180,7 @@
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="J13" s="28" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="17" t="s">
@@ -7218,14 +7219,14 @@
         <v>642</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="43"/>
       <c r="G14" s="59"/>
       <c r="H14" s="29" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="I14" s="29" t="s">
         <v>340</v>
@@ -7268,7 +7269,7 @@
         <v>646</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -7314,14 +7315,14 @@
         <v>656</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="43"/>
       <c r="G16" s="59"/>
       <c r="H16" s="29" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="I16" s="29"/>
       <c r="J16" s="28"/>
@@ -7359,10 +7360,10 @@
         <v>55100015</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -7375,7 +7376,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="O17" s="20"/>
       <c r="P17" s="41"/>
@@ -7386,7 +7387,7 @@
         <v>237</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="T17" s="10"/>
       <c r="U17" s="1" t="s">
@@ -7398,7 +7399,7 @@
         <v>16</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="Z17" s="37"/>
     </row>
@@ -7655,7 +7656,7 @@
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="17" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -8257,7 +8258,7 @@
         <v>55110019</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="C36" s="25" t="s">
         <v>36</v>
@@ -8269,11 +8270,11 @@
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
       <c r="J36" s="26" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="30" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
@@ -8286,7 +8287,7 @@
         <v>403</v>
       </c>
       <c r="S36" s="16" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="T36" s="25"/>
       <c r="U36" s="25" t="s">
@@ -8307,7 +8308,7 @@
         <v>55110020</v>
       </c>
       <c r="B37" s="75" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>1</v>
@@ -8319,7 +8320,7 @@
       <c r="H37" s="29"/>
       <c r="I37" s="29"/>
       <c r="J37" s="28" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="K37" s="18"/>
       <c r="L37" s="17" t="s">
@@ -8336,7 +8337,7 @@
         <v>237</v>
       </c>
       <c r="S37" s="10" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="T37" s="10"/>
       <c r="U37" s="1"/>
@@ -8346,7 +8347,7 @@
         <v>40</v>
       </c>
       <c r="Y37" s="1" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="Z37" s="48"/>
     </row>
@@ -8376,7 +8377,7 @@
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
       <c r="O38" s="20" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="P38" s="41">
         <v>1</v>
@@ -8388,7 +8389,7 @@
         <v>237</v>
       </c>
       <c r="S38" s="16" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="T38" s="25"/>
       <c r="U38" s="25" t="s">
@@ -8483,7 +8484,7 @@
       </c>
       <c r="G40" s="60"/>
       <c r="H40" s="47" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="I40" s="87"/>
       <c r="J40" s="88"/>
@@ -8500,7 +8501,7 @@
         <v>403</v>
       </c>
       <c r="S40" s="16" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="T40" s="31"/>
       <c r="U40" s="31"/>
@@ -8527,7 +8528,7 @@
         <v>97</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E41" s="25">
         <v>15</v>
@@ -8542,7 +8543,7 @@
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="O41" s="20" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="P41" s="41">
         <v>1</v>
@@ -8554,7 +8555,7 @@
         <v>237</v>
       </c>
       <c r="S41" s="16" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="T41" s="25"/>
       <c r="U41" s="10" t="s">
@@ -8568,7 +8569,7 @@
         <v>40</v>
       </c>
       <c r="Y41" s="25" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="Z41" s="92"/>
     </row>
@@ -8583,13 +8584,13 @@
         <v>97</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E42" s="25">
         <v>25</v>
       </c>
       <c r="F42" s="44" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G42" s="59"/>
       <c r="H42" s="47"/>
@@ -8600,7 +8601,7 @@
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
       <c r="O42" s="20" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="P42" s="41">
         <v>2</v>
@@ -8612,7 +8613,7 @@
         <v>237</v>
       </c>
       <c r="S42" s="16" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="T42" s="25"/>
       <c r="U42" s="10" t="s">
@@ -8761,13 +8762,13 @@
         <v>97</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="E45" s="25">
         <v>20</v>
       </c>
       <c r="F45" s="44" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="G45" s="60"/>
       <c r="H45" s="29"/>
@@ -8778,7 +8779,7 @@
       <c r="K45" s="27"/>
       <c r="L45" s="30"/>
       <c r="M45" s="17" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="N45" s="17"/>
       <c r="O45" s="20"/>
@@ -8790,7 +8791,7 @@
         <v>403</v>
       </c>
       <c r="S45" s="16" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="T45" s="25"/>
       <c r="U45" s="25" t="s">
@@ -8800,7 +8801,7 @@
         <v>438</v>
       </c>
       <c r="W45" s="25" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="X45" s="25">
         <v>25</v>
@@ -8821,7 +8822,7 @@
         <v>97</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="43" t="s">
@@ -8889,7 +8890,7 @@
       </c>
       <c r="G47" s="60"/>
       <c r="H47" s="29" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="I47" s="29"/>
       <c r="J47" s="28"/>
@@ -8906,11 +8907,11 @@
         <v>237</v>
       </c>
       <c r="S47" s="16" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="T47" s="25"/>
       <c r="U47" s="25" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="V47" s="25"/>
       <c r="W47" s="25"/>
@@ -8918,7 +8919,7 @@
         <v>25</v>
       </c>
       <c r="Y47" s="25" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="Z47" s="39"/>
     </row>
@@ -8927,13 +8928,13 @@
         <v>55200011</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="C48" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E48" s="25">
         <v>12</v>
@@ -8943,7 +8944,7 @@
       </c>
       <c r="G48" s="59"/>
       <c r="H48" s="47" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="I48" s="47"/>
       <c r="J48" s="26"/>
@@ -8960,21 +8961,21 @@
         <v>237</v>
       </c>
       <c r="S48" s="16" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="T48" s="25"/>
       <c r="U48" s="10" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="V48" s="10" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="W48" s="10"/>
       <c r="X48" s="25">
         <v>20</v>
       </c>
       <c r="Y48" s="25" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="Z48" s="92"/>
     </row>
@@ -8983,13 +8984,13 @@
         <v>55200012</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="C49" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="E49" s="31">
         <v>15</v>
@@ -8999,7 +9000,7 @@
       </c>
       <c r="G49" s="60"/>
       <c r="H49" s="47" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="I49" s="87"/>
       <c r="J49" s="88"/>
@@ -9016,21 +9017,21 @@
         <v>403</v>
       </c>
       <c r="S49" s="16" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="T49" s="31"/>
       <c r="U49" s="25" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="V49" s="25" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="W49" s="31"/>
       <c r="X49" s="31">
         <v>30</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="Z49" s="25"/>
     </row>
@@ -9039,13 +9040,13 @@
         <v>55200013</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="C50" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="E50" s="31">
         <v>12</v>
@@ -9055,7 +9056,7 @@
       </c>
       <c r="G50" s="60"/>
       <c r="H50" s="47" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="I50" s="87"/>
       <c r="J50" s="88"/>
@@ -9072,21 +9073,21 @@
         <v>403</v>
       </c>
       <c r="S50" s="16" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="T50" s="31"/>
       <c r="U50" s="10" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="V50" s="10" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="W50" s="31"/>
       <c r="X50" s="31">
         <v>10</v>
       </c>
       <c r="Y50" s="1" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="Z50" s="25"/>
     </row>
@@ -9095,13 +9096,13 @@
         <v>55200014</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>97</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="E51" s="31"/>
       <c r="F51" s="44" t="s">
@@ -9109,7 +9110,7 @@
       </c>
       <c r="G51" s="60"/>
       <c r="H51" s="93" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="I51" s="29"/>
       <c r="J51" s="26"/>
@@ -9126,21 +9127,21 @@
         <v>237</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="T51" s="25"/>
       <c r="U51" s="25" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="V51" s="25" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="W51" s="25"/>
       <c r="X51" s="25">
         <v>25</v>
       </c>
       <c r="Y51" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="Z51" s="48"/>
     </row>
@@ -9149,7 +9150,7 @@
         <v>55200015</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="C52" s="25" t="s">
         <v>97</v>
@@ -9165,7 +9166,7 @@
       </c>
       <c r="G52" s="60"/>
       <c r="H52" s="47" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="I52" s="87"/>
       <c r="J52" s="88"/>
@@ -9182,19 +9183,19 @@
         <v>403</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="T52" s="31"/>
       <c r="U52" s="31"/>
       <c r="V52" s="25" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="W52" s="31"/>
       <c r="X52" s="31">
         <v>20</v>
       </c>
       <c r="Y52" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="Z52" s="25"/>
     </row>
@@ -9203,7 +9204,7 @@
         <v>55300001</v>
       </c>
       <c r="B53" s="53" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="C53" s="25" t="s">
         <v>48</v>
@@ -9213,10 +9214,10 @@
       <c r="F53" s="44"/>
       <c r="G53" s="60"/>
       <c r="H53" s="47" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="I53" s="47" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="J53" s="26"/>
       <c r="K53" s="27"/>
@@ -9232,7 +9233,7 @@
         <v>237</v>
       </c>
       <c r="S53" s="16" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="T53" s="25"/>
       <c r="U53" s="25"/>
@@ -9247,7 +9248,7 @@
         <v>68</v>
       </c>
       <c r="Z53" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="54" spans="1:26" ht="60">
@@ -9284,7 +9285,7 @@
         <v>237</v>
       </c>
       <c r="S54" s="16" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="T54" s="25"/>
       <c r="U54" s="25"/>
@@ -9297,7 +9298,7 @@
         <v>140</v>
       </c>
       <c r="Z54" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="55" spans="1:26" ht="60">
@@ -9334,7 +9335,7 @@
         <v>237</v>
       </c>
       <c r="S55" s="16" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="T55" s="25"/>
       <c r="U55" s="25"/>
@@ -9347,7 +9348,7 @@
         <v>141</v>
       </c>
       <c r="Z55" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="60">
@@ -9384,7 +9385,7 @@
         <v>237</v>
       </c>
       <c r="S56" s="16" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="T56" s="25"/>
       <c r="U56" s="25"/>
@@ -9397,7 +9398,7 @@
         <v>180</v>
       </c>
       <c r="Z56" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="57" spans="1:26" ht="60">
@@ -9434,7 +9435,7 @@
         <v>237</v>
       </c>
       <c r="S57" s="16" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="T57" s="25"/>
       <c r="U57" s="25"/>
@@ -9447,7 +9448,7 @@
         <v>181</v>
       </c>
       <c r="Z57" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="58" spans="1:26" ht="28.8">
@@ -9497,7 +9498,7 @@
         <v>485</v>
       </c>
       <c r="Z58" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="59" spans="1:26" ht="60">
@@ -9534,7 +9535,7 @@
         <v>237</v>
       </c>
       <c r="S59" s="16" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="T59" s="25"/>
       <c r="U59" s="25"/>
@@ -9547,7 +9548,7 @@
         <v>118</v>
       </c>
       <c r="Z59" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="60" spans="1:26" ht="36">
@@ -9555,7 +9556,7 @@
         <v>55300008</v>
       </c>
       <c r="B60" s="53" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>48</v>
@@ -9565,10 +9566,10 @@
       <c r="F60" s="44"/>
       <c r="G60" s="60"/>
       <c r="H60" s="47" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="I60" s="47" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="J60" s="26"/>
       <c r="K60" s="27"/>
@@ -9584,7 +9585,7 @@
         <v>237</v>
       </c>
       <c r="S60" s="16" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="T60" s="25"/>
       <c r="U60" s="25"/>
@@ -9597,7 +9598,7 @@
         <v>181</v>
       </c>
       <c r="Z60" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="61" spans="1:26" ht="60">
@@ -9605,7 +9606,7 @@
         <v>55300009</v>
       </c>
       <c r="B61" s="53" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>48</v>
@@ -9615,10 +9616,10 @@
       <c r="F61" s="44"/>
       <c r="G61" s="60"/>
       <c r="H61" s="47" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="I61" s="47" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="J61" s="26"/>
       <c r="K61" s="27"/>
@@ -9634,7 +9635,7 @@
         <v>237</v>
       </c>
       <c r="S61" s="16" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="T61" s="25"/>
       <c r="U61" s="25"/>
@@ -9644,10 +9645,10 @@
         <v>30</v>
       </c>
       <c r="Y61" s="25" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="Z61" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="62" spans="1:26" ht="36">
@@ -9655,7 +9656,7 @@
         <v>55300010</v>
       </c>
       <c r="B62" s="53" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>48</v>
@@ -9665,10 +9666,10 @@
       <c r="F62" s="44"/>
       <c r="G62" s="60"/>
       <c r="H62" s="47" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="I62" s="47" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="J62" s="26"/>
       <c r="K62" s="27"/>
@@ -9684,7 +9685,7 @@
         <v>237</v>
       </c>
       <c r="S62" s="16" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="T62" s="25"/>
       <c r="U62" s="25"/>
@@ -9694,10 +9695,10 @@
         <v>35</v>
       </c>
       <c r="Y62" s="25" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="Z62" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="63" spans="1:26" ht="36">
@@ -9705,7 +9706,7 @@
         <v>55300011</v>
       </c>
       <c r="B63" s="53" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="C63" s="25" t="s">
         <v>48</v>
@@ -9715,10 +9716,10 @@
       <c r="F63" s="44"/>
       <c r="G63" s="60"/>
       <c r="H63" s="47" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="I63" s="47" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="J63" s="26"/>
       <c r="K63" s="27"/>
@@ -9734,7 +9735,7 @@
         <v>237</v>
       </c>
       <c r="S63" s="16" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="T63" s="25"/>
       <c r="U63" s="25"/>
@@ -9744,10 +9745,10 @@
         <v>25</v>
       </c>
       <c r="Y63" s="25" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="Z63" s="48" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="64" spans="1:26" ht="36">
@@ -9755,7 +9756,7 @@
         <v>55300012</v>
       </c>
       <c r="B64" s="53" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C64" s="25" t="s">
         <v>48</v>
@@ -9765,10 +9766,10 @@
       <c r="F64" s="44"/>
       <c r="G64" s="60"/>
       <c r="H64" s="47" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="I64" s="47" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="J64" s="26"/>
       <c r="K64" s="27"/>
@@ -9784,7 +9785,7 @@
         <v>237</v>
       </c>
       <c r="S64" s="16" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="T64" s="25"/>
       <c r="U64" s="25"/>
@@ -9813,10 +9814,10 @@
       <c r="F65" s="43"/>
       <c r="G65" s="60"/>
       <c r="H65" s="47" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="I65" s="47" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="J65" s="28"/>
       <c r="K65" s="18"/>
@@ -9832,7 +9833,7 @@
         <v>237</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="T65" s="10"/>
       <c r="U65" s="1"/>
@@ -9915,7 +9916,7 @@
       <c r="L67" s="30"/>
       <c r="M67" s="17"/>
       <c r="N67" s="17" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="O67" s="20"/>
       <c r="P67" s="41"/>
@@ -10008,7 +10009,7 @@
       <c r="M69" s="17"/>
       <c r="N69" s="17"/>
       <c r="O69" s="20" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="P69" s="41">
         <v>2</v>
@@ -10057,7 +10058,7 @@
       </c>
       <c r="G70" s="60"/>
       <c r="H70" s="47" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="I70" s="47"/>
       <c r="J70" s="26"/>
@@ -10110,7 +10111,7 @@
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
       <c r="O71" s="20" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="P71" s="41">
         <v>2</v>
@@ -10160,7 +10161,7 @@
       <c r="M72" s="17"/>
       <c r="N72" s="17"/>
       <c r="O72" s="20" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="P72" s="41">
         <v>2.5</v>
@@ -10172,7 +10173,7 @@
         <v>237</v>
       </c>
       <c r="S72" s="16" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="T72" s="25"/>
       <c r="U72" s="25" t="s">
@@ -10210,7 +10211,7 @@
       <c r="M73" s="17"/>
       <c r="N73" s="17"/>
       <c r="O73" s="20" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="P73" s="41">
         <v>2</v>
@@ -10243,13 +10244,13 @@
         <v>55400007</v>
       </c>
       <c r="B74" s="54" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="C74" s="25" t="s">
         <v>430</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="E74" s="25">
         <v>10</v>
@@ -10259,7 +10260,7 @@
       </c>
       <c r="G74" s="60"/>
       <c r="H74" s="47" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I74" s="47"/>
       <c r="J74" s="26"/>
@@ -10276,7 +10277,7 @@
         <v>237</v>
       </c>
       <c r="S74" s="16" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="T74" s="25"/>
       <c r="U74" s="25"/>
@@ -10286,7 +10287,7 @@
         <v>25</v>
       </c>
       <c r="Y74" s="25" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="Z74" s="48"/>
     </row>
@@ -10295,7 +10296,7 @@
         <v>55410001</v>
       </c>
       <c r="B75" s="54" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="C75" s="25" t="s">
         <v>536</v>
@@ -10311,7 +10312,7 @@
       <c r="L75" s="30"/>
       <c r="M75" s="17"/>
       <c r="N75" s="17" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="O75" s="20"/>
       <c r="P75" s="41"/>
@@ -10322,7 +10323,7 @@
         <v>237</v>
       </c>
       <c r="S75" s="16" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="T75" s="25"/>
       <c r="U75" s="25" t="s">
@@ -10334,7 +10335,7 @@
         <v>50</v>
       </c>
       <c r="Y75" s="50" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="Z75" s="48"/>
     </row>
@@ -11126,7 +11127,7 @@
       <c r="K92" s="18"/>
       <c r="L92" s="17"/>
       <c r="M92" s="17" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="N92" s="17"/>
       <c r="O92" s="20"/>
@@ -11801,7 +11802,7 @@
         <v>55520002</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>35</v>
@@ -11953,7 +11954,7 @@
       <c r="F110" s="43"/>
       <c r="G110" s="60"/>
       <c r="H110" s="29" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="I110" s="29"/>
       <c r="J110" s="28"/>
@@ -12353,7 +12354,7 @@
       <c r="F118" s="43"/>
       <c r="G118" s="60"/>
       <c r="H118" s="29" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="I118" s="29"/>
       <c r="J118" s="28"/>
@@ -12370,7 +12371,7 @@
         <v>403</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="T118" s="10">
         <v>56000023</v>
@@ -12378,7 +12379,7 @@
       <c r="U118" s="1"/>
       <c r="V118" s="1"/>
       <c r="W118" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="X118" s="1">
         <v>20</v>
@@ -12443,7 +12444,7 @@
         <v>55600013</v>
       </c>
       <c r="B120" s="58" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>48</v>
@@ -12453,7 +12454,7 @@
       <c r="F120" s="43"/>
       <c r="G120" s="60"/>
       <c r="H120" s="29" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="I120" s="29"/>
       <c r="J120" s="28"/>
@@ -12470,7 +12471,7 @@
         <v>237</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="T120" s="10">
         <v>56000001</v>
@@ -12493,7 +12494,7 @@
         <v>55600014</v>
       </c>
       <c r="B121" s="58" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>48</v>
@@ -12503,7 +12504,7 @@
       <c r="F121" s="43"/>
       <c r="G121" s="60"/>
       <c r="H121" s="29" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="I121" s="29"/>
       <c r="J121" s="28"/>
@@ -12534,7 +12535,7 @@
         <v>30</v>
       </c>
       <c r="Y121" s="1" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="Z121" s="37"/>
     </row>
@@ -12543,7 +12544,7 @@
         <v>55600015</v>
       </c>
       <c r="B122" s="58" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>48</v>
@@ -12553,7 +12554,7 @@
       <c r="F122" s="43"/>
       <c r="G122" s="60"/>
       <c r="H122" s="29" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="I122" s="29"/>
       <c r="J122" s="28"/>
@@ -12570,7 +12571,7 @@
         <v>237</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="T122" s="10">
         <v>56000101</v>
@@ -12584,7 +12585,7 @@
         <v>10</v>
       </c>
       <c r="Y122" s="1" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="Z122" s="37"/>
     </row>
@@ -12593,7 +12594,7 @@
         <v>55600016</v>
       </c>
       <c r="B123" s="58" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>48</v>
@@ -12603,7 +12604,7 @@
       <c r="F123" s="43"/>
       <c r="G123" s="60"/>
       <c r="H123" s="29" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="I123" s="29"/>
       <c r="J123" s="28"/>
@@ -12620,7 +12621,7 @@
         <v>237</v>
       </c>
       <c r="S123" s="1" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="T123" s="10">
         <v>56000101</v>
@@ -12634,7 +12635,7 @@
         <v>15</v>
       </c>
       <c r="Y123" s="1" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="Z123" s="37"/>
     </row>
@@ -12846,7 +12847,7 @@
       <c r="K128" s="18"/>
       <c r="L128" s="17"/>
       <c r="M128" s="17" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="N128" s="17"/>
       <c r="O128" s="20"/>
@@ -12943,7 +12944,7 @@
       <c r="L130" s="17"/>
       <c r="M130" s="17"/>
       <c r="N130" s="17" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="O130" s="20"/>
       <c r="P130" s="41"/>
@@ -12981,7 +12982,7 @@
         <v>126</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="E131" s="25">
         <v>12</v>
@@ -12991,7 +12992,7 @@
       </c>
       <c r="G131" s="60"/>
       <c r="H131" s="29" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="I131" s="29"/>
       <c r="J131" s="28"/>
@@ -13008,14 +13009,14 @@
         <v>237</v>
       </c>
       <c r="S131" s="10" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="T131" s="10"/>
       <c r="U131" s="1" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="W131" s="1"/>
       <c r="X131" s="1">
@@ -13033,7 +13034,7 @@
         <v>55700005</v>
       </c>
       <c r="B132" s="52" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C132" s="25" t="s">
         <v>402</v>
@@ -13050,7 +13051,7 @@
       <c r="M132" s="17"/>
       <c r="N132" s="17"/>
       <c r="O132" s="20" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="P132" s="41">
         <v>1</v>
@@ -13062,7 +13063,7 @@
         <v>403</v>
       </c>
       <c r="S132" s="16" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="T132" s="25"/>
       <c r="U132" s="25"/>
@@ -13099,7 +13100,7 @@
       </c>
       <c r="G133" s="60"/>
       <c r="H133" s="93" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="I133" s="29"/>
       <c r="J133" s="26"/>
@@ -13157,7 +13158,7 @@
       </c>
       <c r="G134" s="60"/>
       <c r="H134" s="47" t="s">
-        <v>722</v>
+        <v>1034</v>
       </c>
       <c r="I134" s="47"/>
       <c r="J134" s="26"/>
@@ -13205,7 +13206,7 @@
       <c r="F135" s="44"/>
       <c r="G135" s="60"/>
       <c r="H135" s="47" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="I135" s="47"/>
       <c r="J135" s="26"/>
@@ -13429,7 +13430,7 @@
         <v>55900008</v>
       </c>
       <c r="B140" s="55" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>0</v>
@@ -13466,7 +13467,7 @@
         <v>40</v>
       </c>
       <c r="Y140" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="Z140" s="48"/>
     </row>
@@ -13577,7 +13578,7 @@
       <c r="F143" s="43"/>
       <c r="G143" s="60"/>
       <c r="H143" s="29" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="I143" s="29"/>
       <c r="J143" s="28"/>
@@ -13930,7 +13931,7 @@
       <c r="M150" s="21"/>
       <c r="N150" s="21"/>
       <c r="O150" s="19" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="P150" s="41">
         <v>1</v>
@@ -14027,7 +14028,7 @@
       <c r="F152" s="44"/>
       <c r="G152" s="79"/>
       <c r="H152" s="29" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="I152" s="95"/>
       <c r="J152" s="96"/>
@@ -14117,7 +14118,7 @@
         <v>402</v>
       </c>
       <c r="D154" s="25" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E154" s="25">
         <v>200</v>
@@ -14127,7 +14128,7 @@
       </c>
       <c r="G154" s="60"/>
       <c r="H154" s="84" t="s">
-        <v>724</v>
+        <v>1035</v>
       </c>
       <c r="I154" s="47"/>
       <c r="J154" s="26"/>
@@ -14144,7 +14145,7 @@
         <v>403</v>
       </c>
       <c r="S154" s="16" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="T154" s="25"/>
       <c r="U154" s="25" t="s">
@@ -14170,14 +14171,14 @@
         <v>147</v>
       </c>
       <c r="C155" s="25" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25"/>
       <c r="F155" s="25"/>
       <c r="G155" s="60"/>
       <c r="H155" s="84" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="I155" s="47"/>
       <c r="J155" s="26"/>
@@ -14194,7 +14195,7 @@
         <v>403</v>
       </c>
       <c r="S155" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="T155" s="25"/>
       <c r="U155" s="25"/>
@@ -14229,7 +14230,7 @@
       </c>
       <c r="G156" s="60"/>
       <c r="H156" s="84" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I156" s="47"/>
       <c r="J156" s="26"/>
@@ -14246,7 +14247,7 @@
         <v>403</v>
       </c>
       <c r="S156" s="10" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="T156" s="25"/>
       <c r="U156" s="25"/>
@@ -14288,7 +14289,7 @@
       <c r="M157" s="17"/>
       <c r="N157" s="17"/>
       <c r="O157" s="20" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="P157" s="41">
         <v>2</v>
@@ -14300,7 +14301,7 @@
         <v>403</v>
       </c>
       <c r="S157" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="T157" s="25"/>
       <c r="U157" s="25" t="s">
@@ -14339,7 +14340,7 @@
       <c r="L158" s="30"/>
       <c r="M158" s="17"/>
       <c r="N158" s="17" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="O158" s="20"/>
       <c r="P158" s="41"/>
@@ -14350,7 +14351,7 @@
         <v>403</v>
       </c>
       <c r="S158" s="16" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="T158" s="25"/>
       <c r="U158" s="25"/>
@@ -14363,7 +14364,7 @@
         <v>189</v>
       </c>
       <c r="Z158" s="48" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="159" spans="1:26" ht="36">
@@ -14371,7 +14372,7 @@
         <v>55900027</v>
       </c>
       <c r="B159" s="55" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="C159" s="25" t="s">
         <v>0</v>
@@ -14385,10 +14386,10 @@
       <c r="J159" s="26"/>
       <c r="K159" s="27"/>
       <c r="L159" s="30" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="M159" s="17" t="s">
-        <v>748</v>
+        <v>1036</v>
       </c>
       <c r="N159" s="17"/>
       <c r="O159" s="20"/>
@@ -14400,7 +14401,7 @@
         <v>403</v>
       </c>
       <c r="S159" s="16" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="T159" s="25"/>
       <c r="U159" s="25"/>
@@ -14429,7 +14430,7 @@
       <c r="F160" s="44"/>
       <c r="G160" s="60"/>
       <c r="H160" s="84" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="I160" s="47"/>
       <c r="J160" s="26"/>
@@ -14446,7 +14447,7 @@
         <v>403</v>
       </c>
       <c r="S160" s="16" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="T160" s="25"/>
       <c r="U160" s="25"/>
@@ -14473,7 +14474,7 @@
       <c r="F161" s="25"/>
       <c r="G161" s="60"/>
       <c r="H161" s="84" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="I161" s="47"/>
       <c r="J161" s="26"/>
@@ -14490,7 +14491,7 @@
         <v>403</v>
       </c>
       <c r="S161" s="16" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="T161" s="25"/>
       <c r="U161" s="25"/>
@@ -14500,7 +14501,7 @@
         <v>15</v>
       </c>
       <c r="Y161" s="25" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="Z161" s="48"/>
     </row>
@@ -14521,12 +14522,12 @@
       <c r="H162" s="84"/>
       <c r="I162" s="47"/>
       <c r="J162" s="26" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="K162" s="27"/>
       <c r="L162" s="30"/>
       <c r="M162" s="17" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="N162" s="17"/>
       <c r="O162" s="20"/>
@@ -14559,7 +14560,7 @@
         <v>55900031</v>
       </c>
       <c r="B163" s="55" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="C163" s="25" t="s">
         <v>0</v>
@@ -14569,7 +14570,7 @@
       <c r="F163" s="25"/>
       <c r="G163" s="60"/>
       <c r="H163" s="84" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="I163" s="47"/>
       <c r="J163" s="26"/>
@@ -14586,7 +14587,7 @@
         <v>403</v>
       </c>
       <c r="S163" s="16" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="T163" s="25"/>
       <c r="U163" s="25"/>
@@ -14596,7 +14597,7 @@
         <v>5</v>
       </c>
       <c r="Y163" s="25" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="Z163" s="48"/>
     </row>
@@ -14605,13 +14606,13 @@
         <v>55900032</v>
       </c>
       <c r="B164" s="55" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="C164" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D164" s="25" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="E164" s="25">
         <v>12</v>
@@ -14621,7 +14622,7 @@
       </c>
       <c r="G164" s="60"/>
       <c r="H164" s="84" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="I164" s="47"/>
       <c r="J164" s="26"/>
@@ -14638,11 +14639,11 @@
         <v>403</v>
       </c>
       <c r="S164" s="16" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="T164" s="25"/>
       <c r="U164" s="25" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="V164" s="25"/>
       <c r="W164" s="25"/>
@@ -14650,7 +14651,7 @@
         <v>20</v>
       </c>
       <c r="Y164" s="25" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="Z164" s="48"/>
     </row>
@@ -14659,7 +14660,7 @@
         <v>55900033</v>
       </c>
       <c r="B165" s="55" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="C165" s="25" t="s">
         <v>0</v>
@@ -14671,11 +14672,11 @@
       <c r="H165" s="93"/>
       <c r="I165" s="29"/>
       <c r="J165" s="26" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="K165" s="27"/>
       <c r="L165" s="30" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="M165" s="17"/>
       <c r="N165" s="17"/>
@@ -14688,7 +14689,7 @@
         <v>403</v>
       </c>
       <c r="S165" s="16" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="T165" s="25"/>
       <c r="U165" s="25"/>
@@ -14698,7 +14699,7 @@
         <v>20</v>
       </c>
       <c r="Y165" s="25" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="Z165" s="48"/>
     </row>
@@ -14707,7 +14708,7 @@
         <v>55900034</v>
       </c>
       <c r="B166" s="55" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="C166" s="25" t="s">
         <v>0</v>
@@ -14723,7 +14724,7 @@
       <c r="L166" s="30"/>
       <c r="M166" s="17"/>
       <c r="N166" s="17" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="O166" s="20"/>
       <c r="P166" s="41"/>
@@ -14734,7 +14735,7 @@
         <v>403</v>
       </c>
       <c r="S166" s="16" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="T166" s="25"/>
       <c r="U166" s="25"/>
@@ -14744,7 +14745,7 @@
         <v>14</v>
       </c>
       <c r="Y166" s="25" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="Z166" s="48"/>
     </row>
@@ -14753,7 +14754,7 @@
         <v>55900035</v>
       </c>
       <c r="B167" s="55" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="C167" s="25" t="s">
         <v>0</v>
@@ -14763,7 +14764,7 @@
       <c r="F167" s="25"/>
       <c r="G167" s="60"/>
       <c r="H167" s="84" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="I167" s="47"/>
       <c r="J167" s="26"/>
@@ -14780,7 +14781,7 @@
         <v>403</v>
       </c>
       <c r="S167" s="16" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="T167" s="25"/>
       <c r="U167" s="25"/>
@@ -14790,7 +14791,7 @@
         <v>14</v>
       </c>
       <c r="Y167" s="25" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="Z167" s="48"/>
     </row>
@@ -14799,13 +14800,13 @@
         <v>55900036</v>
       </c>
       <c r="B168" s="55" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="C168" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D168" s="25" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E168" s="25">
         <v>50</v>
@@ -14815,7 +14816,7 @@
       </c>
       <c r="G168" s="60"/>
       <c r="H168" s="84" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="I168" s="47"/>
       <c r="J168" s="26"/>
@@ -14832,11 +14833,11 @@
         <v>403</v>
       </c>
       <c r="S168" s="16" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="T168" s="25"/>
       <c r="U168" s="25" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="V168" s="25"/>
       <c r="W168" s="25"/>
@@ -14844,7 +14845,7 @@
         <v>50</v>
       </c>
       <c r="Y168" s="25" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="Z168" s="48"/>
     </row>
@@ -14853,7 +14854,7 @@
         <v>55900037</v>
       </c>
       <c r="B169" s="55" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="C169" s="25" t="s">
         <v>0</v>
@@ -14869,7 +14870,7 @@
       </c>
       <c r="G169" s="60"/>
       <c r="H169" s="93" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="I169" s="29"/>
       <c r="J169" s="26"/>
@@ -14886,7 +14887,7 @@
         <v>403</v>
       </c>
       <c r="S169" s="10" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="T169" s="25"/>
       <c r="U169" s="25"/>
@@ -14896,7 +14897,7 @@
         <v>35</v>
       </c>
       <c r="Y169" s="25" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="Z169" s="48"/>
     </row>
@@ -14905,7 +14906,7 @@
         <v>55900038</v>
       </c>
       <c r="B170" s="55" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C170" s="25" t="s">
         <v>0</v>
@@ -14921,7 +14922,7 @@
       </c>
       <c r="G170" s="60"/>
       <c r="H170" s="29" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="I170" s="29"/>
       <c r="J170" s="26"/>
@@ -14938,21 +14939,21 @@
         <v>403</v>
       </c>
       <c r="S170" s="10" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="T170" s="25"/>
       <c r="U170" s="25" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="V170" s="25" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="W170" s="25"/>
       <c r="X170" s="25">
         <v>40</v>
       </c>
       <c r="Y170" s="25" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="Z170" s="48"/>
     </row>
@@ -14961,7 +14962,7 @@
         <v>55900039</v>
       </c>
       <c r="B171" s="55" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="C171" s="25" t="s">
         <v>0</v>
@@ -14971,10 +14972,10 @@
       <c r="F171" s="43"/>
       <c r="G171" s="59"/>
       <c r="H171" s="29" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="I171" s="29" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="J171" s="26"/>
       <c r="K171" s="27"/>
@@ -14990,7 +14991,7 @@
         <v>237</v>
       </c>
       <c r="S171" s="10" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="T171" s="10"/>
       <c r="U171" s="1"/>
@@ -15002,7 +15003,7 @@
         <v>40</v>
       </c>
       <c r="Y171" s="1" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="Z171" s="25"/>
     </row>
@@ -15011,13 +15012,13 @@
         <v>55900040</v>
       </c>
       <c r="B172" s="55" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="C172" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D172" s="25" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="E172" s="25">
         <v>100</v>
@@ -15027,7 +15028,7 @@
       </c>
       <c r="G172" s="60"/>
       <c r="H172" s="29" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="I172" s="29"/>
       <c r="J172" s="28"/>
@@ -15044,21 +15045,21 @@
         <v>403</v>
       </c>
       <c r="S172" s="10" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="T172" s="25"/>
       <c r="U172" s="25" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="V172" s="25" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="W172" s="25"/>
       <c r="X172" s="25">
         <v>30</v>
       </c>
       <c r="Y172" s="25" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="Z172" s="39"/>
     </row>
@@ -15067,13 +15068,13 @@
         <v>55900041</v>
       </c>
       <c r="B173" s="55" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="C173" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D173" s="25" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="E173" s="25">
         <v>100</v>
@@ -15083,7 +15084,7 @@
       </c>
       <c r="G173" s="60"/>
       <c r="H173" s="29" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="I173" s="29"/>
       <c r="J173" s="26"/>
@@ -15100,11 +15101,11 @@
         <v>403</v>
       </c>
       <c r="S173" s="10" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="T173" s="25"/>
       <c r="U173" s="25" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="V173" s="25"/>
       <c r="W173" s="25"/>
@@ -15112,7 +15113,7 @@
         <v>0</v>
       </c>
       <c r="Y173" s="25" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="Z173" s="48"/>
     </row>
@@ -15121,7 +15122,7 @@
         <v>55900042</v>
       </c>
       <c r="B174" s="55" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="C174" s="25" t="s">
         <v>0</v>
@@ -15137,7 +15138,7 @@
       <c r="L174" s="30"/>
       <c r="M174" s="17"/>
       <c r="N174" s="17" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="O174" s="20"/>
       <c r="P174" s="41"/>
@@ -15148,7 +15149,7 @@
         <v>403</v>
       </c>
       <c r="S174" s="10" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="T174" s="25"/>
       <c r="U174" s="25"/>
@@ -15158,7 +15159,7 @@
         <v>25</v>
       </c>
       <c r="Y174" s="25" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="Z174" s="48"/>
     </row>
@@ -15167,7 +15168,7 @@
         <v>55900043</v>
       </c>
       <c r="B175" s="55" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="C175" s="25" t="s">
         <v>0</v>
@@ -15184,7 +15185,7 @@
       <c r="M175" s="17"/>
       <c r="N175" s="17"/>
       <c r="O175" s="20" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="P175" s="41">
         <v>1</v>
@@ -15196,7 +15197,7 @@
         <v>403</v>
       </c>
       <c r="S175" s="10" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="T175" s="25"/>
       <c r="U175" s="25"/>
@@ -15206,7 +15207,7 @@
         <v>30</v>
       </c>
       <c r="Y175" s="25" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="Z175" s="48"/>
     </row>
@@ -15215,7 +15216,7 @@
         <v>55900044</v>
       </c>
       <c r="B176" s="55" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="C176" s="25" t="s">
         <v>0</v>
@@ -15232,7 +15233,7 @@
       <c r="M176" s="17"/>
       <c r="N176" s="17"/>
       <c r="O176" s="20" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="P176" s="41">
         <v>2</v>
@@ -15244,7 +15245,7 @@
         <v>403</v>
       </c>
       <c r="S176" s="10" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="T176" s="25"/>
       <c r="U176" s="25"/>
@@ -15254,7 +15255,7 @@
         <v>40</v>
       </c>
       <c r="Y176" s="25" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="Z176" s="48"/>
     </row>
@@ -15263,13 +15264,13 @@
         <v>55900045</v>
       </c>
       <c r="B177" s="55" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="C177" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D177" s="25" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="E177" s="25">
         <v>100</v>
@@ -15279,7 +15280,7 @@
       </c>
       <c r="G177" s="60"/>
       <c r="H177" s="93" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="I177" s="29"/>
       <c r="J177" s="26"/>
@@ -15296,7 +15297,7 @@
         <v>403</v>
       </c>
       <c r="S177" s="10" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="T177" s="25"/>
       <c r="U177" s="25"/>
@@ -15306,7 +15307,7 @@
         <v>25</v>
       </c>
       <c r="Y177" s="25" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="Z177" s="48"/>
     </row>
@@ -15315,13 +15316,13 @@
         <v>55900046</v>
       </c>
       <c r="B178" s="55" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="C178" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D178" s="25" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="E178" s="25">
         <v>20</v>
@@ -15331,7 +15332,7 @@
       </c>
       <c r="G178" s="60"/>
       <c r="H178" s="93" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="I178" s="29"/>
       <c r="J178" s="26"/>
@@ -15348,21 +15349,21 @@
         <v>403</v>
       </c>
       <c r="S178" s="16" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="T178" s="25"/>
       <c r="U178" s="25" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="V178" s="25" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="W178" s="25"/>
       <c r="X178" s="25">
         <v>25</v>
       </c>
       <c r="Y178" s="25" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="Z178" s="48"/>
     </row>
@@ -15371,13 +15372,13 @@
         <v>55900047</v>
       </c>
       <c r="B179" s="55" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="C179" s="25" t="s">
         <v>402</v>
       </c>
       <c r="D179" s="25" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="E179" s="25">
         <v>15</v>
@@ -15387,7 +15388,7 @@
       </c>
       <c r="G179" s="60"/>
       <c r="H179" s="93" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="I179" s="29"/>
       <c r="J179" s="26"/>
@@ -15404,21 +15405,21 @@
         <v>403</v>
       </c>
       <c r="S179" s="16" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="T179" s="25"/>
       <c r="U179" s="25" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="V179" s="25" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="W179" s="25"/>
       <c r="X179" s="25">
         <v>30</v>
       </c>
       <c r="Y179" s="25" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="Z179" s="48"/>
     </row>
@@ -15427,7 +15428,7 @@
         <v>55900048</v>
       </c>
       <c r="B180" s="55" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="C180" s="25" t="s">
         <v>402</v>
@@ -15442,7 +15443,7 @@
       <c r="K180" s="27"/>
       <c r="L180" s="30"/>
       <c r="M180" s="17" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="N180" s="17"/>
       <c r="O180" s="20"/>
@@ -15454,7 +15455,7 @@
         <v>403</v>
       </c>
       <c r="S180" s="16" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="T180" s="25"/>
       <c r="U180" s="25"/>
@@ -15464,7 +15465,7 @@
         <v>70</v>
       </c>
       <c r="Y180" s="25" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="Z180" s="48"/>
     </row>
@@ -15473,7 +15474,7 @@
         <v>55900049</v>
       </c>
       <c r="B181" s="55" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="C181" s="25" t="s">
         <v>402</v>
@@ -15485,13 +15486,13 @@
       <c r="H181" s="29"/>
       <c r="I181" s="29"/>
       <c r="J181" s="28" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="K181" s="18" t="s">
         <v>533</v>
       </c>
       <c r="L181" s="17" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="M181" s="17"/>
       <c r="N181" s="17"/>
@@ -15504,7 +15505,7 @@
         <v>237</v>
       </c>
       <c r="S181" s="15" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="T181" s="36"/>
       <c r="U181" s="1"/>
@@ -15523,7 +15524,7 @@
         <v>55900050</v>
       </c>
       <c r="B182" s="55" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="C182" s="25" t="s">
         <v>0</v>
@@ -15535,12 +15536,12 @@
       <c r="H182" s="84"/>
       <c r="I182" s="47"/>
       <c r="J182" s="26" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="K182" s="27"/>
       <c r="L182" s="30"/>
       <c r="M182" s="17" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="N182" s="17"/>
       <c r="O182" s="20"/>
@@ -15552,7 +15553,7 @@
         <v>403</v>
       </c>
       <c r="S182" s="16" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="T182" s="25"/>
       <c r="U182" s="25"/>
@@ -15562,7 +15563,7 @@
         <v>20</v>
       </c>
       <c r="Y182" s="25" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="Z182" s="48"/>
     </row>
@@ -15571,17 +15572,17 @@
         <v>55900051</v>
       </c>
       <c r="B183" s="55" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="D183" s="61"/>
       <c r="E183" s="61"/>
       <c r="F183" s="62"/>
       <c r="G183" s="59"/>
       <c r="H183" s="29" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="I183" s="63"/>
       <c r="J183" s="64"/>
@@ -15598,7 +15599,7 @@
         <v>237</v>
       </c>
       <c r="S183" s="10" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="T183" s="10"/>
       <c r="U183" s="61"/>
@@ -15608,7 +15609,7 @@
         <v>25</v>
       </c>
       <c r="Y183" s="25" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Z183" s="70"/>
     </row>
@@ -15620,7 +15621,7 @@
         <v>23</v>
       </c>
       <c r="C184" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D184" s="25"/>
       <c r="E184" s="25"/>
@@ -15659,7 +15660,7 @@
         <v>24</v>
       </c>
       <c r="Z184" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="185" spans="1:26" ht="36">
@@ -15670,7 +15671,7 @@
         <v>25</v>
       </c>
       <c r="C185" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D185" s="25"/>
       <c r="E185" s="25"/>
@@ -15709,7 +15710,7 @@
         <v>26</v>
       </c>
       <c r="Z185" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="186" spans="1:26" ht="36">
@@ -15720,7 +15721,7 @@
         <v>27</v>
       </c>
       <c r="C186" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25"/>
@@ -15759,7 +15760,7 @@
         <v>28</v>
       </c>
       <c r="Z186" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="187" spans="1:26" ht="36">
@@ -15770,7 +15771,7 @@
         <v>29</v>
       </c>
       <c r="C187" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D187" s="25"/>
       <c r="E187" s="25"/>
@@ -15809,7 +15810,7 @@
         <v>30</v>
       </c>
       <c r="Z187" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="188" spans="1:26" ht="36">
@@ -15820,7 +15821,7 @@
         <v>31</v>
       </c>
       <c r="C188" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25"/>
@@ -15859,7 +15860,7 @@
         <v>32</v>
       </c>
       <c r="Z188" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="189" spans="1:26" ht="36">
@@ -15870,7 +15871,7 @@
         <v>33</v>
       </c>
       <c r="C189" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25"/>
@@ -15909,7 +15910,7 @@
         <v>34</v>
       </c>
       <c r="Z189" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="190" spans="1:26" ht="36">
@@ -15920,7 +15921,7 @@
         <v>54</v>
       </c>
       <c r="C190" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D190" s="25"/>
       <c r="E190" s="25"/>
@@ -15959,7 +15960,7 @@
         <v>55</v>
       </c>
       <c r="Z190" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="191" spans="1:26" ht="36">
@@ -15970,7 +15971,7 @@
         <v>56</v>
       </c>
       <c r="C191" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25"/>
@@ -16009,7 +16010,7 @@
         <v>57</v>
       </c>
       <c r="Z191" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="192" spans="1:26" ht="36">
@@ -16020,7 +16021,7 @@
         <v>58</v>
       </c>
       <c r="C192" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D192" s="25"/>
       <c r="E192" s="25"/>
@@ -16059,7 +16060,7 @@
         <v>59</v>
       </c>
       <c r="Z192" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="193" spans="1:26" ht="36">
@@ -16070,7 +16071,7 @@
         <v>60</v>
       </c>
       <c r="C193" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D193" s="25"/>
       <c r="E193" s="25"/>
@@ -16109,7 +16110,7 @@
         <v>61</v>
       </c>
       <c r="Z193" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="194" spans="1:26" ht="36">
@@ -16120,7 +16121,7 @@
         <v>62</v>
       </c>
       <c r="C194" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25"/>
@@ -16159,7 +16160,7 @@
         <v>63</v>
       </c>
       <c r="Z194" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="195" spans="1:26" ht="36">
@@ -16170,7 +16171,7 @@
         <v>64</v>
       </c>
       <c r="C195" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D195" s="25"/>
       <c r="E195" s="25"/>
@@ -16209,7 +16210,7 @@
         <v>65</v>
       </c>
       <c r="Z195" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="196" spans="1:26" ht="24">
@@ -16217,17 +16218,17 @@
         <v>55990101</v>
       </c>
       <c r="B196" s="94" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C196" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D196" s="25"/>
       <c r="E196" s="25"/>
       <c r="F196" s="44"/>
       <c r="G196" s="60"/>
       <c r="H196" s="84" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="I196" s="47"/>
       <c r="J196" s="26"/>
@@ -16244,7 +16245,7 @@
         <v>237</v>
       </c>
       <c r="S196" s="49" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="T196" s="25"/>
       <c r="U196" s="25"/>
@@ -16257,7 +16258,7 @@
         <v>107</v>
       </c>
       <c r="Z196" s="48" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
     </row>
     <row r="197" spans="1:26" ht="28.8">
@@ -16265,10 +16266,10 @@
         <v>55990102</v>
       </c>
       <c r="B197" s="94" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="C197" s="25" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D197" s="25"/>
       <c r="E197" s="25"/>
@@ -16277,11 +16278,11 @@
       <c r="H197" s="84"/>
       <c r="I197" s="47"/>
       <c r="J197" s="26" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="K197" s="27"/>
       <c r="L197" s="30" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="M197" s="17"/>
       <c r="N197" s="17"/>
@@ -16294,7 +16295,7 @@
         <v>237</v>
       </c>
       <c r="S197" s="16" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="T197" s="25"/>
       <c r="U197" s="25"/>
@@ -16304,10 +16305,10 @@
         <v>25</v>
       </c>
       <c r="Y197" s="25" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="Z197" s="48" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="198" spans="1:26" ht="72">
@@ -16315,7 +16316,7 @@
         <v>55990103</v>
       </c>
       <c r="B198" s="94" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="C198" s="25" t="s">
         <v>97</v>
@@ -16350,24 +16351,24 @@
         <v>237</v>
       </c>
       <c r="S198" s="16" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="T198" s="25"/>
       <c r="U198" s="25" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="V198" s="25" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="W198" s="25"/>
       <c r="X198" s="25">
         <v>35</v>
       </c>
       <c r="Y198" s="25" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="Z198" s="48" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="199" spans="1:26" ht="72">
@@ -16375,7 +16376,7 @@
         <v>55990104</v>
       </c>
       <c r="B199" s="94" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="C199" s="25" t="s">
         <v>97</v>
@@ -16393,7 +16394,7 @@
       <c r="H199" s="84"/>
       <c r="I199" s="47"/>
       <c r="J199" s="26" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="K199" s="27"/>
       <c r="L199" s="30"/>
@@ -16410,24 +16411,24 @@
         <v>237</v>
       </c>
       <c r="S199" s="16" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="T199" s="25"/>
       <c r="U199" s="25" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="V199" s="25" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="W199" s="25"/>
       <c r="X199" s="25">
         <v>50</v>
       </c>
       <c r="Y199" s="25" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="Z199" s="48" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="200" spans="1:26">
@@ -16435,10 +16436,10 @@
         <v>55990105</v>
       </c>
       <c r="B200" s="94" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C200" s="25" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
@@ -16450,7 +16451,7 @@
       <c r="K200" s="27"/>
       <c r="L200" s="30"/>
       <c r="M200" s="17" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="N200" s="17"/>
       <c r="O200" s="20"/>
@@ -16462,7 +16463,7 @@
         <v>237</v>
       </c>
       <c r="S200" s="10" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="T200" s="10"/>
       <c r="U200" s="1"/>
@@ -16472,7 +16473,7 @@
         <v>150</v>
       </c>
       <c r="Y200" s="1" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="Z200" s="25"/>
     </row>

</xml_diff>

<commit_message>
weapon decrease life by weapon type
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="1063">
   <si>
     <t>特殊</t>
   </si>
@@ -3883,158 +3883,174 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>s.Summon("around",51013000,4);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon("back",51000008,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon("around",51000018,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon("side",51013001,2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.Summon("around",51000010,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Owner.Combo)s.Summon("around",51013005,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Summon("around",s.CardId,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.SetToPosition("side",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>d.SetToPosition("back",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时获得10%生命的物甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.AddPArmor(s.MaxHp.Source*0.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.AddSkill(55100008,100);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>peilian</t>
+  </si>
+  <si>
+    <t>陪练</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>铸甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>给予范围内最近友方单位嘲讽</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合回复一个己方生命最低的怪物30%生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhujia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.AddPArmor(s.Atk.Source*2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合给予2.5卡牌范围内随机友军一些物甲（自身攻击x2）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>兽性</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shouxing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk.Source*=MathTool.GetRandom(1f,1.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(MathTool.GetRandom(0f,1f)&lt;0.5)s.Def.Source+=5;else s.Crt.Source+=5;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始随机提高5点防御或暴击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成长</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>分裂</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fenlie</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合提高40%攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Atk.Source*=1.4;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对方下一张魔法卡消耗+5（一回合有效）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.AddRandomCardRace(s,6,s.Level);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时获得一张随机鸟类手牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>niaoyou</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鹰之友</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>guweishi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>骨卫士</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>s.Summon("back",51000019,1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s.Summon("around",51013000,4);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon("back",51000008,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>s.Summon("around",51000205,1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s.Summon("around",51000018,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon("side",51013001,2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.Summon("around",51000010,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Owner.Combo)s.Summon("around",51013005,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Summon("around",s.CardId,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(o.Id!=s.Id)o.SetToPosition("rand",1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(mon.Id!=s.Id) mon.SetToPosition("side",1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>d.SetToPosition("back",1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时获得10%生命的物甲</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.AddPArmor(s.MaxHp.Source*0.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NFR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.AddSkill(55100008,100);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>peilian</t>
-  </si>
-  <si>
-    <t>陪练</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>铸甲</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>给予范围内最近友方单位嘲讽</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合回复一个己方生命最低的怪物30%生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhujia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.AddPArmor(s.Atk.Source*2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合给予2.5卡牌范围内随机友军一些物甲（自身攻击x2）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>兽性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shouxing</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk.Source*=MathTool.GetRandom(1f,1.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(MathTool.GetRandom(0f,1f)&lt;0.5)s.Def.Source+=5;else s.Crt.Source+=5;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始随机提高5点防御或暴击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>成长</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>分裂</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fenlie</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合提高40%攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Atk.Source*=1.4;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对方下一张魔法卡消耗+5（一回合有效）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Owner.AddRandomCardRace(s,6,s.Level);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时获得一张随机鸟类手牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>niaoyou</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>鹰之友</t>
+    <t>s.Summon("around",51000013,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀死敌人后在附近召唤一个骷髅战士</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6208,8 +6224,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z205" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:Z205"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:Z206" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:Z206"/>
   <sortState ref="A4:Z198">
     <sortCondition ref="A3:A198"/>
   </sortState>
@@ -6566,14 +6582,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z205"/>
+  <dimension ref="A1:Z206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C181" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C194" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="B188" sqref="B188"/>
+      <selection pane="bottomRight" activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6999,7 +7015,7 @@
       <c r="F7" s="43"/>
       <c r="G7" s="59"/>
       <c r="H7" s="29" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="28"/>
@@ -7016,7 +7032,7 @@
         <v>237</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="T7" s="10"/>
       <c r="U7" s="1"/>
@@ -7091,7 +7107,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="59"/>
       <c r="H9" s="29" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I9" s="63"/>
       <c r="J9" s="64"/>
@@ -7675,7 +7691,7 @@
       <c r="F21" s="43"/>
       <c r="G21" s="59"/>
       <c r="H21" s="29" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="28"/>
@@ -9602,7 +9618,7 @@
         <v>237</v>
       </c>
       <c r="S58" s="49" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="T58" s="25"/>
       <c r="U58" s="25" t="s">
@@ -10128,7 +10144,7 @@
       <c r="M69" s="17"/>
       <c r="N69" s="17"/>
       <c r="O69" s="20" t="s">
-        <v>1020</v>
+        <v>1059</v>
       </c>
       <c r="P69" s="41">
         <v>2</v>
@@ -10177,7 +10193,7 @@
       </c>
       <c r="G70" s="60"/>
       <c r="H70" s="47" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I70" s="47"/>
       <c r="J70" s="26"/>
@@ -10230,7 +10246,7 @@
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
       <c r="O71" s="20" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P71" s="41">
         <v>2</v>
@@ -10280,7 +10296,7 @@
       <c r="M72" s="17"/>
       <c r="N72" s="17"/>
       <c r="O72" s="20" t="s">
-        <v>1023</v>
+        <v>1060</v>
       </c>
       <c r="P72" s="41">
         <v>2.5</v>
@@ -10330,7 +10346,7 @@
       <c r="M73" s="17"/>
       <c r="N73" s="17"/>
       <c r="O73" s="20" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="P73" s="41">
         <v>2</v>
@@ -10379,7 +10395,7 @@
       </c>
       <c r="G74" s="60"/>
       <c r="H74" s="47" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="I74" s="47"/>
       <c r="J74" s="26"/>
@@ -10431,7 +10447,7 @@
       <c r="L75" s="30"/>
       <c r="M75" s="17"/>
       <c r="N75" s="17" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="O75" s="20"/>
       <c r="P75" s="41"/>
@@ -13203,10 +13219,10 @@
         <v>55700006</v>
       </c>
       <c r="B133" s="52" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C133" s="25" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D133" s="25"/>
       <c r="E133" s="25"/>
@@ -13220,7 +13236,7 @@
       <c r="M133" s="17"/>
       <c r="N133" s="17"/>
       <c r="O133" s="20" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="P133" s="41">
         <v>1</v>
@@ -13232,7 +13248,7 @@
         <v>403</v>
       </c>
       <c r="S133" s="16" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="T133" s="25"/>
       <c r="U133" s="25"/>
@@ -13242,7 +13258,7 @@
         <v>50</v>
       </c>
       <c r="Y133" s="25" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="Z133" s="25" t="s">
         <v>580</v>
@@ -13327,7 +13343,7 @@
       </c>
       <c r="G135" s="60"/>
       <c r="H135" s="47" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="I135" s="47"/>
       <c r="J135" s="26"/>
@@ -14297,7 +14313,7 @@
       </c>
       <c r="G155" s="60"/>
       <c r="H155" s="84" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="I155" s="47"/>
       <c r="J155" s="26"/>
@@ -14558,7 +14574,7 @@
         <v>743</v>
       </c>
       <c r="M160" s="17" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="N160" s="17"/>
       <c r="O160" s="20"/>
@@ -15366,7 +15382,7 @@
         <v>403</v>
       </c>
       <c r="S176" s="10" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="T176" s="25"/>
       <c r="U176" s="25"/>
@@ -15751,7 +15767,7 @@
       <c r="F184" s="62"/>
       <c r="G184" s="59"/>
       <c r="H184" s="29" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="I184" s="63"/>
       <c r="J184" s="64"/>
@@ -15787,13 +15803,13 @@
         <v>55900052</v>
       </c>
       <c r="B185" s="55" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C185" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D185" s="25" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="E185" s="25">
         <v>15</v>
@@ -15803,7 +15819,7 @@
       </c>
       <c r="G185" s="60"/>
       <c r="H185" s="93" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="I185" s="29"/>
       <c r="J185" s="26"/>
@@ -15820,7 +15836,7 @@
         <v>403</v>
       </c>
       <c r="S185" s="10" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="T185" s="25"/>
       <c r="U185" s="25"/>
@@ -15830,7 +15846,7 @@
         <v>5</v>
       </c>
       <c r="Y185" s="25" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="Z185" s="48"/>
     </row>
@@ -15839,13 +15855,13 @@
         <v>55900053</v>
       </c>
       <c r="B186" s="55" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C186" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D186" s="25" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="E186" s="25">
         <v>25</v>
@@ -15862,7 +15878,7 @@
       <c r="M186" s="17"/>
       <c r="N186" s="17"/>
       <c r="O186" s="20" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="P186" s="41">
         <v>1</v>
@@ -15874,7 +15890,7 @@
         <v>403</v>
       </c>
       <c r="S186" s="10" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="T186" s="25"/>
       <c r="U186" s="25"/>
@@ -15884,7 +15900,7 @@
         <v>30</v>
       </c>
       <c r="Y186" s="25" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="Z186" s="48"/>
     </row>
@@ -15893,7 +15909,7 @@
         <v>55900054</v>
       </c>
       <c r="B187" s="55" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C187" s="25" t="s">
         <v>0</v>
@@ -15903,7 +15919,7 @@
       <c r="F187" s="44"/>
       <c r="G187" s="60"/>
       <c r="H187" s="93" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="I187" s="29"/>
       <c r="J187" s="26"/>
@@ -15920,7 +15936,7 @@
         <v>403</v>
       </c>
       <c r="S187" s="10" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="T187" s="25"/>
       <c r="U187" s="25"/>
@@ -15930,7 +15946,7 @@
         <v>15</v>
       </c>
       <c r="Y187" s="25" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="Z187" s="48"/>
     </row>
@@ -15939,7 +15955,7 @@
         <v>55900055</v>
       </c>
       <c r="B188" s="55" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C188" s="25" t="s">
         <v>0</v>
@@ -15949,7 +15965,7 @@
       <c r="F188" s="44"/>
       <c r="G188" s="60"/>
       <c r="H188" s="93" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="I188" s="29"/>
       <c r="J188" s="26"/>
@@ -15966,7 +15982,7 @@
         <v>403</v>
       </c>
       <c r="S188" s="10" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="T188" s="25"/>
       <c r="U188" s="25"/>
@@ -15976,7 +15992,7 @@
         <v>15</v>
       </c>
       <c r="Y188" s="25" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="Z188" s="48"/>
     </row>
@@ -16842,7 +16858,57 @@
       <c r="Y205" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="Z205" s="25"/>
+      <c r="Z205" s="48" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="206" spans="1:26" ht="24" x14ac:dyDescent="0.15">
+      <c r="A206" s="94">
+        <v>55990106</v>
+      </c>
+      <c r="B206" s="94" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C206" s="25" t="s">
+        <v>773</v>
+      </c>
+      <c r="D206" s="1"/>
+      <c r="E206" s="1"/>
+      <c r="F206" s="43"/>
+      <c r="G206" s="60"/>
+      <c r="H206" s="84"/>
+      <c r="I206" s="47"/>
+      <c r="J206" s="26"/>
+      <c r="K206" s="27"/>
+      <c r="L206" s="30"/>
+      <c r="M206" s="17"/>
+      <c r="N206" s="17" t="s">
+        <v>1061</v>
+      </c>
+      <c r="O206" s="20"/>
+      <c r="P206" s="41"/>
+      <c r="Q206" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="R206" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="S206" s="10" t="s">
+        <v>1062</v>
+      </c>
+      <c r="T206" s="10"/>
+      <c r="U206" s="1"/>
+      <c r="V206" s="1"/>
+      <c r="W206" s="1"/>
+      <c r="X206" s="1">
+        <v>40</v>
+      </c>
+      <c r="Y206" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Z206" s="48" t="s">
+        <v>793</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
fix some bug on skillview
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="1096">
   <si>
     <t>特殊</t>
   </si>
@@ -4075,6 +4075,10 @@
   </si>
   <si>
     <t>工程学</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shidu</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6688,11 +6692,11 @@
   <dimension ref="A1:AB213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="Q189" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="Q137" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="W192" sqref="W192"/>
+      <selection pane="bottomRight" activeCell="AA140" sqref="AA140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -13971,7 +13975,7 @@
         <v>-30</v>
       </c>
       <c r="AA139" s="25" t="s">
-        <v>424</v>
+        <v>1095</v>
       </c>
       <c r="AB139" s="48"/>
     </row>
@@ -16357,8 +16361,8 @@
       <c r="C186" s="55" t="s">
         <v>848</v>
       </c>
-      <c r="D186" s="1" t="s">
-        <v>723</v>
+      <c r="D186" s="25" t="s">
+        <v>0</v>
       </c>
       <c r="E186" s="61"/>
       <c r="F186" s="61"/>
@@ -17438,7 +17442,7 @@
         <v>680</v>
       </c>
       <c r="D207" s="25" t="s">
-        <v>97</v>
+        <v>662</v>
       </c>
       <c r="E207" s="25" t="s">
         <v>410</v>
@@ -17500,7 +17504,7 @@
         <v>687</v>
       </c>
       <c r="D208" s="25" t="s">
-        <v>97</v>
+        <v>662</v>
       </c>
       <c r="E208" s="25" t="s">
         <v>410</v>
@@ -17717,8 +17721,8 @@
       <c r="C212" s="94" t="s">
         <v>892</v>
       </c>
-      <c r="D212" s="1" t="s">
-        <v>723</v>
+      <c r="D212" s="25" t="s">
+        <v>662</v>
       </c>
       <c r="E212" s="1"/>
       <c r="F212" s="1"/>
@@ -17772,7 +17776,7 @@
         <v>894</v>
       </c>
       <c r="D213" s="25" t="s">
-        <v>473</v>
+        <v>662</v>
       </c>
       <c r="E213" s="25"/>
       <c r="F213" s="25"/>

</xml_diff>

<commit_message>
new api for skill missile
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -3653,12 +3653,6 @@
     <t>s.Atk*=(s.Action.GetMonsterCountByRace(4)*0.2);</t>
   </si>
   <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon, "waterball");</t>
-  </si>
-  <si>
-    <t>if(type==3){foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon, "firearrow");eff=true;}</t>
-  </si>
-  <si>
     <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position)) if(s.Id!=o.Id) o.Action.ClearDebuff();</t>
   </si>
   <si>
@@ -4151,6 +4145,14 @@
   </si>
   <si>
     <t>firehit</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon, 1,s.Atk.Source,"waterball");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(type==3){foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,sp.Target,sp.Shape,sp.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon,3,s.Atk.Source, "firearrow");eff=true;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6760,11 +6762,11 @@
   <dimension ref="A1:AB217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="Q55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="N212" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="W56" sqref="W56"/>
+      <selection pane="bottomRight" activeCell="R215" sqref="R215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6794,7 +6796,7 @@
         <v>230</v>
       </c>
       <c r="B1" s="96" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>231</v>
@@ -6880,7 +6882,7 @@
         <v>223</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>224</v>
@@ -6966,7 +6968,7 @@
         <v>225</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>226</v>
@@ -7219,7 +7221,7 @@
       <c r="G7" s="43"/>
       <c r="H7" s="59"/>
       <c r="I7" s="29" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="J7" s="29"/>
       <c r="K7" s="28"/>
@@ -7315,7 +7317,7 @@
       <c r="G9" s="62"/>
       <c r="H9" s="59"/>
       <c r="I9" s="29" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="J9" s="63"/>
       <c r="K9" s="64"/>
@@ -7376,7 +7378,7 @@
       <c r="L10" s="18"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="O10" s="17"/>
       <c r="P10" s="20"/>
@@ -7455,7 +7457,7 @@
       <c r="W11" s="25"/>
       <c r="X11" s="25"/>
       <c r="Y11" s="25" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="Z11" s="61">
         <v>15</v>
@@ -7471,7 +7473,7 @@
       </c>
       <c r="B12" s="51"/>
       <c r="C12" s="51" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>721</v>
@@ -7480,7 +7482,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="44"/>
       <c r="H12" s="60" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="I12" s="93"/>
       <c r="J12" s="29"/>
@@ -7499,19 +7501,19 @@
         <v>237</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="V12" s="25"/>
       <c r="W12" s="25"/>
       <c r="X12" s="25"/>
       <c r="Y12" s="25" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="Z12" s="61">
         <v>15</v>
       </c>
       <c r="AA12" s="25" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="AB12" s="48"/>
     </row>
@@ -7631,10 +7633,10 @@
       <c r="G15" s="43"/>
       <c r="H15" s="59"/>
       <c r="I15" s="29" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="J15" s="29" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="K15" s="28"/>
       <c r="L15" s="18"/>
@@ -7657,7 +7659,7 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="Z15" s="1">
         <v>15</v>
@@ -7731,7 +7733,7 @@
       <c r="G17" s="43"/>
       <c r="H17" s="59"/>
       <c r="I17" s="29" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="J17" s="29"/>
       <c r="K17" s="28"/>
@@ -7787,7 +7789,7 @@
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="17" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="P18" s="20"/>
       <c r="Q18" s="41"/>
@@ -8030,7 +8032,7 @@
       <c r="L23" s="18"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="O23" s="17"/>
       <c r="P23" s="20"/>
@@ -8043,7 +8045,7 @@
         <v>237</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="V23" s="14"/>
       <c r="W23" s="1"/>
@@ -8289,7 +8291,7 @@
         <v>237</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="V28" s="10"/>
       <c r="W28" s="1"/>
@@ -8339,7 +8341,7 @@
         <v>237</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="V29" s="10"/>
       <c r="W29" s="1"/>
@@ -8426,7 +8428,7 @@
         <v>605</v>
       </c>
       <c r="N31" s="17" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="O31" s="17"/>
       <c r="P31" s="20"/>
@@ -8439,7 +8441,7 @@
         <v>237</v>
       </c>
       <c r="U31" s="10" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="V31" s="10"/>
       <c r="W31" s="1"/>
@@ -8861,7 +8863,7 @@
       </c>
       <c r="AB39" s="48"/>
     </row>
-    <row r="40" spans="1:28" ht="84" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:28" ht="108" x14ac:dyDescent="0.15">
       <c r="A40" s="73">
         <v>55200002</v>
       </c>
@@ -8883,7 +8885,7 @@
       </c>
       <c r="H40" s="60"/>
       <c r="I40" s="29" t="s">
-        <v>967</v>
+        <v>1112</v>
       </c>
       <c r="J40" s="29"/>
       <c r="K40" s="28"/>
@@ -9000,7 +9002,7 @@
       <c r="N42" s="17"/>
       <c r="O42" s="17"/>
       <c r="P42" s="20" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="Q42" s="41">
         <v>1</v>
@@ -9013,7 +9015,7 @@
         <v>237</v>
       </c>
       <c r="U42" s="16" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="V42" s="25"/>
       <c r="W42" s="10" t="s">
@@ -9060,7 +9062,7 @@
       <c r="N43" s="17"/>
       <c r="O43" s="17"/>
       <c r="P43" s="20" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="Q43" s="41">
         <v>2</v>
@@ -9120,7 +9122,7 @@
       <c r="L44" s="18"/>
       <c r="M44" s="17"/>
       <c r="N44" s="17" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="O44" s="17"/>
       <c r="P44" s="20"/>
@@ -9240,7 +9242,7 @@
       <c r="L46" s="27"/>
       <c r="M46" s="30"/>
       <c r="N46" s="17" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="O46" s="17"/>
       <c r="P46" s="20"/>
@@ -9298,7 +9300,7 @@
       <c r="L47" s="18"/>
       <c r="M47" s="17"/>
       <c r="N47" s="17" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="O47" s="17"/>
       <c r="P47" s="20"/>
@@ -9407,7 +9409,7 @@
       </c>
       <c r="H49" s="59"/>
       <c r="I49" s="47" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="J49" s="47"/>
       <c r="K49" s="26"/>
@@ -9425,7 +9427,7 @@
         <v>237</v>
       </c>
       <c r="U49" s="16" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="V49" s="25"/>
       <c r="W49" s="10" t="s">
@@ -9465,7 +9467,7 @@
       </c>
       <c r="H50" s="60"/>
       <c r="I50" s="47" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="J50" s="87"/>
       <c r="K50" s="88"/>
@@ -9655,7 +9657,7 @@
         <v>372</v>
       </c>
       <c r="U53" s="16" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="V53" s="31"/>
       <c r="W53" s="31"/>
@@ -9677,7 +9679,7 @@
       </c>
       <c r="B54" s="73"/>
       <c r="C54" s="11" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>97</v>
@@ -9691,7 +9693,7 @@
       <c r="G54" s="44"/>
       <c r="H54" s="59"/>
       <c r="I54" s="47" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="J54" s="47"/>
       <c r="K54" s="26"/>
@@ -9709,21 +9711,21 @@
         <v>237</v>
       </c>
       <c r="U54" s="16" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="V54" s="25"/>
       <c r="W54" s="10" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="X54" s="10" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="Y54" s="10"/>
       <c r="Z54" s="25">
         <v>30</v>
       </c>
       <c r="AA54" s="25" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="AB54" s="92"/>
     </row>
@@ -9733,7 +9735,7 @@
       </c>
       <c r="B55" s="73"/>
       <c r="C55" s="11" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>97</v>
@@ -9755,7 +9757,7 @@
       <c r="M55" s="30"/>
       <c r="N55" s="17"/>
       <c r="O55" s="17" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="P55" s="20"/>
       <c r="Q55" s="41"/>
@@ -9767,7 +9769,7 @@
         <v>372</v>
       </c>
       <c r="U55" s="10" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="V55" s="25"/>
       <c r="W55" s="25" t="s">
@@ -9781,7 +9783,7 @@
         <v>35</v>
       </c>
       <c r="AA55" s="25" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="AB55" s="48"/>
     </row>
@@ -9791,7 +9793,7 @@
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="12" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>97</v>
@@ -9807,7 +9809,7 @@
       </c>
       <c r="H56" s="60"/>
       <c r="I56" s="47" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="J56" s="87"/>
       <c r="K56" s="88"/>
@@ -9825,19 +9827,19 @@
         <v>372</v>
       </c>
       <c r="U56" s="16" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="V56" s="31"/>
       <c r="W56" s="31"/>
       <c r="X56" s="31" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="Y56" s="31"/>
       <c r="Z56" s="31">
         <v>50</v>
       </c>
       <c r="AA56" s="1" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="AB56" s="25"/>
     </row>
@@ -9857,10 +9859,10 @@
       <c r="G57" s="44"/>
       <c r="H57" s="60"/>
       <c r="I57" s="47" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="J57" s="47" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="K57" s="26"/>
       <c r="L57" s="27"/>
@@ -9911,10 +9913,10 @@
       <c r="G58" s="44"/>
       <c r="H58" s="60"/>
       <c r="I58" s="29" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="J58" s="29" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="K58" s="26"/>
       <c r="L58" s="27"/>
@@ -9963,10 +9965,10 @@
       <c r="G59" s="44"/>
       <c r="H59" s="60"/>
       <c r="I59" s="47" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="J59" s="47" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="K59" s="26"/>
       <c r="L59" s="27"/>
@@ -10015,10 +10017,10 @@
       <c r="G60" s="44"/>
       <c r="H60" s="60"/>
       <c r="I60" s="47" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="J60" s="47" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="K60" s="26"/>
       <c r="L60" s="27"/>
@@ -10067,10 +10069,10 @@
       <c r="G61" s="44"/>
       <c r="H61" s="60"/>
       <c r="I61" s="47" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="J61" s="47" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="K61" s="26"/>
       <c r="L61" s="27"/>
@@ -10119,7 +10121,7 @@
       <c r="G62" s="44"/>
       <c r="H62" s="60"/>
       <c r="I62" s="47" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="J62" s="47"/>
       <c r="K62" s="26"/>
@@ -10137,7 +10139,7 @@
         <v>237</v>
       </c>
       <c r="U62" s="49" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="V62" s="25"/>
       <c r="W62" s="25" t="s">
@@ -10171,10 +10173,10 @@
       <c r="G63" s="44"/>
       <c r="H63" s="60"/>
       <c r="I63" s="47" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="J63" s="47" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="K63" s="26"/>
       <c r="L63" s="27"/>
@@ -10223,10 +10225,10 @@
       <c r="G64" s="44"/>
       <c r="H64" s="60"/>
       <c r="I64" s="47" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="J64" s="47" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="K64" s="26"/>
       <c r="L64" s="27"/>
@@ -10275,10 +10277,10 @@
       <c r="G65" s="44"/>
       <c r="H65" s="60"/>
       <c r="I65" s="47" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="J65" s="47" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="K65" s="26"/>
       <c r="L65" s="27"/>
@@ -10327,10 +10329,10 @@
       <c r="G66" s="44"/>
       <c r="H66" s="60"/>
       <c r="I66" s="47" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="J66" s="47" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="K66" s="26"/>
       <c r="L66" s="27"/>
@@ -10379,10 +10381,10 @@
       <c r="G67" s="44"/>
       <c r="H67" s="60"/>
       <c r="I67" s="47" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="J67" s="47" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="K67" s="26"/>
       <c r="L67" s="27"/>
@@ -10431,10 +10433,10 @@
       <c r="G68" s="44"/>
       <c r="H68" s="60"/>
       <c r="I68" s="47" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="J68" s="47" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="K68" s="28"/>
       <c r="L68" s="18"/>
@@ -10481,10 +10483,10 @@
       <c r="G69" s="43"/>
       <c r="H69" s="60"/>
       <c r="I69" s="29" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="J69" s="29" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="K69" s="28"/>
       <c r="L69" s="18"/>
@@ -10684,7 +10686,7 @@
       <c r="N73" s="17"/>
       <c r="O73" s="17"/>
       <c r="P73" s="20" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="Q73" s="41">
         <v>2</v>
@@ -10735,7 +10737,7 @@
       </c>
       <c r="H74" s="60"/>
       <c r="I74" s="47" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="J74" s="47"/>
       <c r="K74" s="26"/>
@@ -10790,7 +10792,7 @@
       <c r="N75" s="17"/>
       <c r="O75" s="17"/>
       <c r="P75" s="20" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="Q75" s="41">
         <v>2</v>
@@ -10842,7 +10844,7 @@
       <c r="N76" s="17"/>
       <c r="O76" s="17"/>
       <c r="P76" s="20" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="Q76" s="41">
         <v>2.5</v>
@@ -10894,7 +10896,7 @@
       <c r="N77" s="17"/>
       <c r="O77" s="17"/>
       <c r="P77" s="20" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="Q77" s="41">
         <v>2</v>
@@ -10945,7 +10947,7 @@
       </c>
       <c r="H78" s="60"/>
       <c r="I78" s="47" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="J78" s="47"/>
       <c r="K78" s="26"/>
@@ -10999,7 +11001,7 @@
       <c r="M79" s="30"/>
       <c r="N79" s="17"/>
       <c r="O79" s="17" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="P79" s="20"/>
       <c r="Q79" s="41"/>
@@ -12485,7 +12487,7 @@
         <v>237</v>
       </c>
       <c r="U109" s="1" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="V109" s="1"/>
       <c r="W109" s="1"/>
@@ -12659,7 +12661,7 @@
       <c r="G113" s="43"/>
       <c r="H113" s="60"/>
       <c r="I113" s="29" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="J113" s="29"/>
       <c r="K113" s="28"/>
@@ -12711,7 +12713,7 @@
       <c r="G114" s="43"/>
       <c r="H114" s="60"/>
       <c r="I114" s="29" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="J114" s="29"/>
       <c r="K114" s="28"/>
@@ -12763,7 +12765,7 @@
       <c r="G115" s="43"/>
       <c r="H115" s="60"/>
       <c r="I115" s="29" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="J115" s="29"/>
       <c r="K115" s="28"/>
@@ -12815,7 +12817,7 @@
       <c r="G116" s="43"/>
       <c r="H116" s="60"/>
       <c r="I116" s="29" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="J116" s="29"/>
       <c r="K116" s="28"/>
@@ -12867,7 +12869,7 @@
       <c r="G117" s="43"/>
       <c r="H117" s="60"/>
       <c r="I117" s="29" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="J117" s="29"/>
       <c r="K117" s="28"/>
@@ -12919,7 +12921,7 @@
       <c r="G118" s="43"/>
       <c r="H118" s="60"/>
       <c r="I118" s="29" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="J118" s="29"/>
       <c r="K118" s="28"/>
@@ -12971,7 +12973,7 @@
       <c r="G119" s="43"/>
       <c r="H119" s="60"/>
       <c r="I119" s="29" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="J119" s="29"/>
       <c r="K119" s="28"/>
@@ -13023,7 +13025,7 @@
       <c r="G120" s="43"/>
       <c r="H120" s="60"/>
       <c r="I120" s="29" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="J120" s="29"/>
       <c r="K120" s="28"/>
@@ -13075,7 +13077,7 @@
       <c r="G121" s="43"/>
       <c r="H121" s="60"/>
       <c r="I121" s="29" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="J121" s="29"/>
       <c r="K121" s="28"/>
@@ -13127,7 +13129,7 @@
       <c r="G122" s="43"/>
       <c r="H122" s="60"/>
       <c r="I122" s="29" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="J122" s="29"/>
       <c r="K122" s="28"/>
@@ -13179,7 +13181,7 @@
       <c r="G123" s="43"/>
       <c r="H123" s="60"/>
       <c r="I123" s="29" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="J123" s="29"/>
       <c r="K123" s="28"/>
@@ -13231,7 +13233,7 @@
       <c r="G124" s="43"/>
       <c r="H124" s="60"/>
       <c r="I124" s="29" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="J124" s="29"/>
       <c r="K124" s="28"/>
@@ -13283,7 +13285,7 @@
       <c r="G125" s="43"/>
       <c r="H125" s="60"/>
       <c r="I125" s="29" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="J125" s="29"/>
       <c r="K125" s="28"/>
@@ -13335,7 +13337,7 @@
       <c r="G126" s="43"/>
       <c r="H126" s="60"/>
       <c r="I126" s="29" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="J126" s="29"/>
       <c r="K126" s="28"/>
@@ -13387,7 +13389,7 @@
       <c r="G127" s="43"/>
       <c r="H127" s="60"/>
       <c r="I127" s="29" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="J127" s="29"/>
       <c r="K127" s="28"/>
@@ -13429,7 +13431,7 @@
       </c>
       <c r="B128" s="86"/>
       <c r="C128" s="58" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>48</v>
@@ -13439,7 +13441,7 @@
       <c r="G128" s="43"/>
       <c r="H128" s="60"/>
       <c r="I128" s="29" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="J128" s="29"/>
       <c r="K128" s="28"/>
@@ -13457,7 +13459,7 @@
         <v>237</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="V128" s="10">
         <v>56000102</v>
@@ -13471,7 +13473,7 @@
         <v>20</v>
       </c>
       <c r="AA128" s="1" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="AB128" s="39"/>
     </row>
@@ -13480,7 +13482,7 @@
         <v>55610001</v>
       </c>
       <c r="B129" s="77" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="C129" s="76" t="s">
         <v>82</v>
@@ -13847,7 +13849,7 @@
       </c>
       <c r="H136" s="60"/>
       <c r="I136" s="47" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="J136" s="47"/>
       <c r="K136" s="26"/>
@@ -14123,7 +14125,7 @@
       </c>
       <c r="H141" s="60"/>
       <c r="I141" s="47" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="J141" s="47"/>
       <c r="K141" s="26"/>
@@ -14227,7 +14229,7 @@
       <c r="M143" s="30"/>
       <c r="N143" s="17"/>
       <c r="O143" s="17" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="P143" s="20"/>
       <c r="Q143" s="41"/>
@@ -14251,7 +14253,7 @@
         <v>-30</v>
       </c>
       <c r="AA143" s="25" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="AB143" s="48"/>
     </row>
@@ -14277,7 +14279,7 @@
       <c r="M144" s="17"/>
       <c r="N144" s="17"/>
       <c r="O144" s="17" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="P144" s="20"/>
       <c r="Q144" s="41"/>
@@ -14422,7 +14424,7 @@
       <c r="L147" s="18"/>
       <c r="M147" s="17"/>
       <c r="N147" s="17" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="O147" s="17"/>
       <c r="P147" s="20"/>
@@ -14615,7 +14617,7 @@
       </c>
       <c r="H151" s="60"/>
       <c r="I151" s="29" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="J151" s="29"/>
       <c r="K151" s="28"/>
@@ -14723,7 +14725,7 @@
       <c r="M153" s="17"/>
       <c r="N153" s="17"/>
       <c r="O153" s="17" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="P153" s="20"/>
       <c r="Q153" s="41"/>
@@ -14835,7 +14837,7 @@
         <v>237</v>
       </c>
       <c r="U155" s="10" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="V155" s="10"/>
       <c r="W155" s="1" t="s">
@@ -15084,7 +15086,7 @@
       <c r="N160" s="17"/>
       <c r="O160" s="17"/>
       <c r="P160" s="20" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="Q160" s="41">
         <v>1</v>
@@ -15133,7 +15135,7 @@
       </c>
       <c r="H161" s="60"/>
       <c r="I161" s="84" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="J161" s="47"/>
       <c r="K161" s="26"/>
@@ -15300,7 +15302,7 @@
       <c r="N164" s="17"/>
       <c r="O164" s="17"/>
       <c r="P164" s="20" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="Q164" s="41">
         <v>2</v>
@@ -15353,7 +15355,7 @@
       <c r="M165" s="30"/>
       <c r="N165" s="17"/>
       <c r="O165" s="17" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="P165" s="20"/>
       <c r="Q165" s="41"/>
@@ -15404,7 +15406,7 @@
         <v>638</v>
       </c>
       <c r="N166" s="17" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="O166" s="17"/>
       <c r="P166" s="20"/>
@@ -15753,7 +15755,7 @@
       <c r="M173" s="30"/>
       <c r="N173" s="17"/>
       <c r="O173" s="17" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="P173" s="20"/>
       <c r="Q173" s="41"/>
@@ -15795,7 +15797,7 @@
       <c r="G174" s="25"/>
       <c r="H174" s="60"/>
       <c r="I174" s="84" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="J174" s="47"/>
       <c r="K174" s="26"/>
@@ -16011,10 +16013,10 @@
       <c r="G178" s="43"/>
       <c r="H178" s="59"/>
       <c r="I178" s="29" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="J178" s="29" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="K178" s="28"/>
       <c r="L178" s="18"/>
@@ -16127,7 +16129,7 @@
       </c>
       <c r="H180" s="60"/>
       <c r="I180" s="29" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="J180" s="29"/>
       <c r="K180" s="26"/>
@@ -16183,7 +16185,7 @@
       <c r="M181" s="30"/>
       <c r="N181" s="17"/>
       <c r="O181" s="17" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="P181" s="20"/>
       <c r="Q181" s="41"/>
@@ -16232,7 +16234,7 @@
       <c r="N182" s="17"/>
       <c r="O182" s="17"/>
       <c r="P182" s="20" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="Q182" s="41">
         <v>1</v>
@@ -16282,7 +16284,7 @@
       <c r="N183" s="17"/>
       <c r="O183" s="17"/>
       <c r="P183" s="20" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="Q183" s="41">
         <v>2</v>
@@ -16331,7 +16333,7 @@
       </c>
       <c r="H184" s="60"/>
       <c r="I184" s="93" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="J184" s="29"/>
       <c r="K184" s="26"/>
@@ -16385,7 +16387,7 @@
       </c>
       <c r="H185" s="60"/>
       <c r="I185" s="93" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="J185" s="29"/>
       <c r="K185" s="26"/>
@@ -16407,10 +16409,10 @@
       </c>
       <c r="V185" s="25"/>
       <c r="W185" s="25" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="X185" s="25" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="Y185" s="25"/>
       <c r="Z185" s="25">
@@ -16443,7 +16445,7 @@
       </c>
       <c r="H186" s="60"/>
       <c r="I186" s="93" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="J186" s="29"/>
       <c r="K186" s="26"/>
@@ -16500,7 +16502,7 @@
       <c r="L187" s="18"/>
       <c r="M187" s="17"/>
       <c r="N187" s="17" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="O187" s="17"/>
       <c r="P187" s="20"/>
@@ -16597,12 +16599,12 @@
       <c r="I189" s="29"/>
       <c r="J189" s="29"/>
       <c r="K189" s="26" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="L189" s="27"/>
       <c r="M189" s="30"/>
       <c r="N189" s="17" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="O189" s="17"/>
       <c r="P189" s="20"/>
@@ -16645,7 +16647,7 @@
       <c r="G190" s="62"/>
       <c r="H190" s="59"/>
       <c r="I190" s="93" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="J190" s="63"/>
       <c r="K190" s="64"/>
@@ -16663,7 +16665,7 @@
         <v>237</v>
       </c>
       <c r="U190" s="10" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="V190" s="10"/>
       <c r="W190" s="61"/>
@@ -16760,7 +16762,7 @@
       <c r="N192" s="17"/>
       <c r="O192" s="17"/>
       <c r="P192" s="20" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="Q192" s="41">
         <v>1</v>
@@ -16773,7 +16775,7 @@
         <v>372</v>
       </c>
       <c r="U192" s="10" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="V192" s="25"/>
       <c r="W192" s="25"/>
@@ -16851,7 +16853,7 @@
       <c r="G194" s="44"/>
       <c r="H194" s="60"/>
       <c r="I194" s="93" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="J194" s="93"/>
       <c r="K194" s="26"/>
@@ -16889,7 +16891,7 @@
       </c>
       <c r="B195" s="55"/>
       <c r="C195" s="55" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="D195" s="25" t="s">
         <v>0</v>
@@ -16899,10 +16901,10 @@
       <c r="G195" s="44"/>
       <c r="H195" s="60"/>
       <c r="I195" s="47" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="J195" s="47" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="K195" s="26"/>
       <c r="L195" s="27"/>
@@ -16919,7 +16921,7 @@
         <v>372</v>
       </c>
       <c r="U195" s="10" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="V195" s="25"/>
       <c r="W195" s="25"/>
@@ -16929,7 +16931,7 @@
         <v>10</v>
       </c>
       <c r="AA195" s="25" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="AB195" s="48"/>
     </row>
@@ -16939,7 +16941,7 @@
       </c>
       <c r="B196" s="55"/>
       <c r="C196" s="55" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="D196" s="25" t="s">
         <v>0</v>
@@ -16949,7 +16951,7 @@
       <c r="G196" s="44"/>
       <c r="H196" s="59"/>
       <c r="I196" s="29" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="J196" s="29"/>
       <c r="K196" s="26"/>
@@ -16967,11 +16969,11 @@
         <v>237</v>
       </c>
       <c r="U196" s="16" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="V196" s="25"/>
       <c r="W196" s="10" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="X196" s="10"/>
       <c r="Y196" s="10"/>
@@ -16979,7 +16981,7 @@
         <v>40</v>
       </c>
       <c r="AA196" s="25" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="AB196" s="48"/>
     </row>
@@ -17738,7 +17740,7 @@
       <c r="L211" s="27"/>
       <c r="M211" s="30"/>
       <c r="N211" s="17" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="O211" s="17"/>
       <c r="P211" s="20"/>
@@ -17800,7 +17802,7 @@
       <c r="L212" s="27"/>
       <c r="M212" s="30"/>
       <c r="N212" s="17" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="O212" s="17"/>
       <c r="P212" s="20"/>
@@ -17854,7 +17856,7 @@
       <c r="L213" s="27"/>
       <c r="M213" s="30"/>
       <c r="N213" s="17" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="O213" s="17"/>
       <c r="P213" s="20"/>
@@ -17904,7 +17906,7 @@
       <c r="L214" s="27"/>
       <c r="M214" s="30"/>
       <c r="N214" s="17" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="O214" s="17"/>
       <c r="P214" s="20"/>
@@ -17933,7 +17935,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="215" spans="1:28" ht="168" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:28" ht="180" x14ac:dyDescent="0.15">
       <c r="A215" s="94">
         <v>55990107</v>
       </c>
@@ -17964,7 +17966,7 @@
       <c r="P215" s="20"/>
       <c r="Q215" s="41"/>
       <c r="R215" s="20" t="s">
-        <v>968</v>
+        <v>1113</v>
       </c>
       <c r="S215" s="35" t="s">
         <v>242</v>
@@ -18066,7 +18068,7 @@
       <c r="N217" s="17"/>
       <c r="O217" s="17"/>
       <c r="P217" s="20" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="Q217" s="41">
         <v>4</v>

</xml_diff>

<commit_message>
simplify the monster attr system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -4021,298 +4021,302 @@
     <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,d.Position)) o.DecHp(damage.Value*0.1);</t>
   </si>
   <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.RepairHp(s.Cure);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) s.Action.Transform(mon.CardId);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(o.Id!=s.Id)o.Action.SetToPosition("rand",1);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id)) o.Action.MadDrug();</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(mon.Id!=s.Id) mon.Action.SetToPosition("side",1);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) o.Action.ExtendDebuff(2);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.Return(0);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.SuddenDeath();</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1))  mon.Action.Silent();</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterStar(1,2).SortRandom().Top(1)) mon.Action.Rebel();</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.AddSkill(55100008,100);</t>
+  </si>
+  <si>
+    <t>s.Action.AddBuff(56000201,skl.Level,1.5);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000201,skl.Level,1.5);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,d.Position)) s.Action.AddBuff(56000001,skl.Level,2);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) s.Action.AddBuff(55510003,skl.Level,3);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000001,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000002,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000003,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000004,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000006,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000007,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000009,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000010,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000011,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000012,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000013,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000014,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000018,skl.Level,99);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000019,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>s.Action.AddBuff(56000006,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>s.Action.AddBuff(56000012,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000003,skl.Level,1);d.Action.AddBuff(56000004,skl.Level,1);</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000101,skl.Level,"A").AddRace("Undead");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000101,skl.Level,"F").AddRace("Plant");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000101,skl.Level,"A").AddRace("Dragon");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000121,skl.Level,"F").AddAttr("Dark");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000121,skl.Level,"F").AddAttr("Light");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000121,skl.Level,"F");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000101,skl.Level,"F");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000101,skl.Level,"A").AddAttr("None");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000002,skl.Level,"E");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000023,skl.Level,"F").AddAttr("Water");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000007,skl.Level,"A");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000001,skl.Level,"A").SetStar(6,10);</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000131,skl.Level,"E");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000101,skl.Level,"F").AddRace("Human");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000101,skl.Level,"F").AddAttr("Fire");</t>
+  </si>
+  <si>
+    <t>s.Action.AddAuro(56000102,skl.Level,"F").AddRace("Bird");</t>
+  </si>
+  <si>
+    <t>s.Action.AddBuff(56000007,skl.Level,3);</t>
+  </si>
+  <si>
+    <t>d.Action.AddBuff(56000203,skl.Level,1.5);</t>
+  </si>
+  <si>
+    <t>skl.Levelfeng</t>
+  </si>
+  <si>
+    <t>s.Action.AddBuff(56000201,skl.Level,1.1);</t>
+  </si>
+  <si>
+    <t>s.Owner.Action.AddSpellVibrate(-0.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.Action.AddSpellVibrate(0.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.ChangeAI("Common");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortDistance(true).Top(1)) s.Action.AddMissile(mon, 1,s.Atk*2,"arrowfast");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon, 1,s.Atk,"waterball");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddPArmor(s.MaxHp*0.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.AddPDamage(d.MaxHp*0.10);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.OnMagicDamage(s,s.Atk,3);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position)) if(o.IsLeft!=s.IsLeft) o.OnMagicDamage(s,s.Atk*1,5);</t>
+  </si>
+  <si>
+    <t>if(s.Owner.Combo)foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortDistance(true).Top(1)) mon.OnMagicDamage(s,s.Atk*3,0);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.OnMagicDamage(s,s.Atk*2,2);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortDistance(true).Top(1)) s.Action.AddMissile(mon, 3,s.Atk*3,"fireball");</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonsterGhost(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){s.Map.ReviveUnit(s.Owner,o,(int)(o.MaxHp/2));}</t>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.AddPArmor(s.Atk*2);</t>
+  </si>
+  <si>
+    <t>if(type==3){foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon,3,s.Atk, "firearrow");eff=true;}</t>
+  </si>
+  <si>
+    <t>召唤时，如果对方手牌数&gt;5，提高30%攻击和2点防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.ChangeAI("Tank");s.Action.AddAttrModify("Skill",skl.Id,"Def",8);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Spd",8);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.15);s.Action.AddAttrModify("Skill",skl.Id,"Def",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*MathTool.GetRandom(0f,0.5));</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0.5);d.Action.AddAttrModify("Skill",skl.Id,"Atk",-d.Atk*0.05);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Rival.CardNumber&gt;5) {s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.3);s.Action.AddAttrModify("Skill",skl.Id,"Def",2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(MathTool.GetRandom(0f,1f)&lt;0.5)s.Action.AddAttrModify("Skill",skl.Id,"Def",5);else s.Action.AddAttrModify("Skill",skl.Id,"Crt",5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*s.Action.GetMonsterCountByRace(4)*0.2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.4);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Hit",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*s.Owner.CardNumber);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Owner.CardNumber&gt;=6) s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.Action.AddAttrModify("Skill",skl.Id,"Def",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterStar(1,3).Top(1)) mon.Action.SuddenDeath();</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.RepairHp(s.Cure);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonsterGhost(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) s.Action.EatTomb(mon);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) s.Action.Transform(mon.CardId);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(o.Id!=s.Id)o.Action.SetToPosition("rand",1);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id)) o.Action.MadDrug();</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(mon.Id!=s.Id) mon.Action.SetToPosition("side",1);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) o.Action.ExtendDebuff(2);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.Return(0);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.SuddenDeath();</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1))  mon.Action.Silent();</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterStar(1,2).SortRandom().Top(1)) mon.Action.Rebel();</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.AddSkill(55100008,100);</t>
-  </si>
-  <si>
-    <t>s.Action.AddBuff(56000201,skl.Level,1.5);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000201,skl.Level,1.5);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,d.Position)) s.Action.AddBuff(56000001,skl.Level,2);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) s.Action.AddBuff(55510003,skl.Level,3);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000001,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000002,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000003,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000004,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000006,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000007,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000009,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000010,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000011,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000012,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000013,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000014,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000018,skl.Level,99);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000019,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>s.Action.AddBuff(56000006,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>s.Action.AddBuff(56000012,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000003,skl.Level,1);d.Action.AddBuff(56000004,skl.Level,1);</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000101,skl.Level,"A").AddRace("Undead");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000101,skl.Level,"F").AddRace("Plant");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000101,skl.Level,"A").AddRace("Dragon");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000121,skl.Level,"F").AddAttr("Dark");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000121,skl.Level,"F").AddAttr("Light");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000121,skl.Level,"F");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000101,skl.Level,"F");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000101,skl.Level,"A").AddAttr("None");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000002,skl.Level,"E");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000023,skl.Level,"F").AddAttr("Water");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000007,skl.Level,"A");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000001,skl.Level,"A").SetStar(6,10);</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000131,skl.Level,"E");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000101,skl.Level,"F").AddRace("Human");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000101,skl.Level,"F").AddAttr("Fire");</t>
-  </si>
-  <si>
-    <t>s.Action.AddAuro(56000102,skl.Level,"F").AddRace("Bird");</t>
-  </si>
-  <si>
-    <t>s.Action.AddBuff(56000007,skl.Level,3);</t>
-  </si>
-  <si>
-    <t>d.Action.AddBuff(56000203,skl.Level,1.5);</t>
-  </si>
-  <si>
-    <t>skl.Levelfeng</t>
-  </si>
-  <si>
-    <t>s.Action.AddBuff(56000201,skl.Level,1.1);</t>
-  </si>
-  <si>
-    <t>s.Owner.Action.AddSpellVibrate(-0.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Owner.Action.AddSpellVibrate(0.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.ChangeAI("Common");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortDistance(true).Top(1)) s.Action.AddMissile(mon, 1,s.Atk*2,"arrowfast");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon, 1,s.Atk,"waterball");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddPArmor(s.MaxHp*0.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.AddPDamage(d.MaxHp*0.10);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.OnMagicDamage(s,s.Atk,3);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position)) if(o.IsLeft!=s.IsLeft) o.OnMagicDamage(s,s.Atk*1,5);</t>
-  </si>
-  <si>
-    <t>if(s.Owner.Combo)foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortDistance(true).Top(1)) mon.OnMagicDamage(s,s.Atk*3,0);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.OnMagicDamage(s,s.Atk*2,2);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortDistance(true).Top(1)) s.Action.AddMissile(mon, 3,s.Atk*3,"fireball");</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.AddMaxHp(o.MaxHp*0.15);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){o.AddMaxHp(o.MaxHp*0.15);}</t>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonsterGhost(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){s.Map.ReviveUnit(s.Owner,o,(int)(o.MaxHp/2));}</t>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.AddPArmor(s.Atk*2);</t>
-  </si>
-  <si>
-    <t>if(type==3){foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon,3,s.Atk, "firearrow");eff=true;}</t>
-  </si>
-  <si>
-    <t>召唤时，如果对方手牌数&gt;5，提高30%攻击和2点防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.ChangeAI("Tank");s.Action.AddAttrModify("Skill",skl.Id,"Def",8);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Spd",8);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.15);s.Action.AddAttrModify("Skill",skl.Id,"Def",1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*MathTool.GetRandom(0f,0.5));</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0.5);d.Action.AddAttrModify("Skill",skl.Id,"Atk",-d.Atk*0.05);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Rival.CardNumber&gt;5) {s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.3);s.Action.AddAttrModify("Skill",skl.Id,"Def",2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterAttr(1)){o.AddMaxHp(o.MaxHp*0.2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(MathTool.GetRandom(0f,1f)&lt;0.5)s.Action.AddAttrModify("Skill",skl.Id,"Def",5);else s.Action.AddAttrModify("Skill",skl.Id,"Crt",5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*s.Action.GetMonsterCountByRace(4)*0.2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(s.Attr))if(s.IsLeft==o.IsLeft&amp;&amp;s.Id!=o.Id){o.AddMaxHp(o.MaxHp*0.2);o.Action.AddAttrModify("Skill",skl.Id,"Atk",o.Atk*0.2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.4);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(p.IsLeft==s.IsLeft){s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);s.AddMaxHp(s.MaxHp*0.1);eff=true;}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Hit",1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",d.Atk*0.3);s.AddMaxHp(d.MaxHp*0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*s.Owner.CardNumber);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Owner.CardNumber&gt;=6) s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.Action.AddAttrModify("Skill",skl.Id,"Def",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",d.Atk*0.3);s.Action.AddMaxHp("Skill",skl.Id,d.MaxHp*0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonsterGhost(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){s.Action.EatTomb(mon);s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);s.Action.AddMaxHp("Skill",skl.Id,s.MaxHp*0.1);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(s.Attr))if(s.IsLeft==o.IsLeft&amp;&amp;s.Id!=o.Id){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.2);o.Action.AddAttrModify("Skill",skl.Id,"Atk",o.Atk*0.2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterAttr(1)){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.15);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(p.IsLeft==s.IsLeft){s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);s.Action.AddMaxHp("Skill",skl.Id, s.MaxHp*0.1);eff=true;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.15);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4640,6 +4644,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4647,6 +4652,7 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Courier New"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -7100,11 +7106,11 @@
   <dimension ref="A1:AD224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="G146" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="I54" sqref="I54"/>
+      <selection pane="bottomRight" activeCell="J155" sqref="J155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7462,7 +7468,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="48" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" ht="60" x14ac:dyDescent="0.15">
       <c r="A5" s="51">
         <v>55100002</v>
       </c>
@@ -7484,7 +7490,7 @@
       <c r="K5" s="29"/>
       <c r="L5" s="82"/>
       <c r="M5" s="18" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="N5" s="17" t="s">
         <v>458</v>
@@ -7518,7 +7524,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="48" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" ht="60" x14ac:dyDescent="0.15">
       <c r="A6" s="51">
         <v>55100003</v>
       </c>
@@ -7540,7 +7546,7 @@
       <c r="K6" s="29"/>
       <c r="L6" s="82"/>
       <c r="M6" s="18" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="N6" s="17" t="s">
         <v>450</v>
@@ -7591,7 +7597,7 @@
       <c r="H7" s="59"/>
       <c r="I7" s="28"/>
       <c r="J7" s="29" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="K7" s="29"/>
       <c r="L7" s="82"/>
@@ -7790,7 +7796,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="60" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:30" ht="72" x14ac:dyDescent="0.15">
       <c r="A11" s="51">
         <v>55100008</v>
       </c>
@@ -8247,11 +8253,11 @@
       <c r="H19" s="59"/>
       <c r="I19" s="28"/>
       <c r="J19" s="29" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="K19" s="29"/>
       <c r="L19" s="82" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="M19" s="18"/>
       <c r="N19" s="17"/>
@@ -8351,7 +8357,7 @@
       <c r="H21" s="59"/>
       <c r="I21" s="26"/>
       <c r="J21" s="29" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
@@ -8405,7 +8411,7 @@
         <v>1054</v>
       </c>
       <c r="J22" s="90" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="K22" s="105"/>
       <c r="L22" s="99"/>
@@ -8611,7 +8617,7 @@
       <c r="H26" s="59"/>
       <c r="I26" s="28"/>
       <c r="J26" s="29" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="K26" s="29"/>
       <c r="L26" s="82"/>
@@ -8871,7 +8877,7 @@
       <c r="L31" s="82"/>
       <c r="M31" s="18"/>
       <c r="N31" s="17" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
@@ -9283,7 +9289,7 @@
       <c r="L39" s="82"/>
       <c r="M39" s="18"/>
       <c r="N39" s="17" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="O39" s="17"/>
       <c r="P39" s="17"/>
@@ -9501,7 +9507,7 @@
       <c r="P43" s="17"/>
       <c r="Q43" s="17"/>
       <c r="R43" s="20" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="S43" s="41">
         <v>1</v>
@@ -9555,7 +9561,7 @@
       <c r="H44" s="60"/>
       <c r="I44" s="28"/>
       <c r="J44" s="29" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="K44" s="29"/>
       <c r="L44" s="82"/>
@@ -9613,7 +9619,7 @@
       <c r="H45" s="60"/>
       <c r="I45" s="86"/>
       <c r="J45" s="47" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="K45" s="85"/>
       <c r="L45" s="100"/>
@@ -9860,7 +9866,7 @@
       <c r="M49" s="18"/>
       <c r="N49" s="17"/>
       <c r="O49" s="17" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="P49" s="17"/>
       <c r="Q49" s="17"/>
@@ -10037,7 +10043,7 @@
       <c r="H52" s="60"/>
       <c r="I52" s="28"/>
       <c r="J52" s="29" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="K52" s="29"/>
       <c r="L52" s="82"/>
@@ -10155,7 +10161,7 @@
       <c r="H54" s="60"/>
       <c r="I54" s="86"/>
       <c r="J54" s="47" t="s">
-        <v>1067</v>
+        <v>1149</v>
       </c>
       <c r="K54" s="85"/>
       <c r="L54" s="100"/>
@@ -10215,7 +10221,7 @@
       <c r="H55" s="60"/>
       <c r="I55" s="86"/>
       <c r="J55" s="47" t="s">
-        <v>1156</v>
+        <v>1148</v>
       </c>
       <c r="K55" s="85"/>
       <c r="L55" s="100"/>
@@ -10273,7 +10279,7 @@
       <c r="H56" s="60"/>
       <c r="I56" s="26"/>
       <c r="J56" s="90" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="K56" s="29"/>
       <c r="L56" s="99"/>
@@ -10333,7 +10339,7 @@
       <c r="H57" s="60"/>
       <c r="I57" s="86"/>
       <c r="J57" s="47" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="K57" s="85"/>
       <c r="L57" s="100"/>
@@ -10391,7 +10397,7 @@
       <c r="H58" s="59"/>
       <c r="I58" s="26"/>
       <c r="J58" s="47" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="K58" s="47"/>
       <c r="L58" s="99"/>
@@ -10458,7 +10464,7 @@
       <c r="O59" s="17"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="17" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="R59" s="20"/>
       <c r="S59" s="41"/>
@@ -10490,7 +10496,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="60" spans="1:30" ht="120" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:30" ht="108" x14ac:dyDescent="0.15">
       <c r="A60" s="72">
         <v>55200018</v>
       </c>
@@ -10513,7 +10519,7 @@
       <c r="H60" s="60"/>
       <c r="I60" s="86"/>
       <c r="J60" s="47" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="K60" s="85"/>
       <c r="L60" s="100"/>
@@ -12698,7 +12704,7 @@
       <c r="M101" s="18"/>
       <c r="N101" s="17"/>
       <c r="O101" s="17" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="P101" s="17"/>
       <c r="Q101" s="17"/>
@@ -12748,7 +12754,7 @@
       <c r="M102" s="18"/>
       <c r="N102" s="17"/>
       <c r="O102" s="17" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="P102" s="17"/>
       <c r="Q102" s="17"/>
@@ -12798,7 +12804,7 @@
       <c r="M103" s="18"/>
       <c r="N103" s="17"/>
       <c r="O103" s="17" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="P103" s="17"/>
       <c r="Q103" s="17"/>
@@ -12848,7 +12854,7 @@
       <c r="M104" s="18"/>
       <c r="N104" s="17"/>
       <c r="O104" s="17" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="P104" s="17"/>
       <c r="Q104" s="17"/>
@@ -12898,7 +12904,7 @@
       <c r="M105" s="18"/>
       <c r="N105" s="17"/>
       <c r="O105" s="17" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="P105" s="17"/>
       <c r="Q105" s="17"/>
@@ -12948,7 +12954,7 @@
       <c r="M106" s="18"/>
       <c r="N106" s="17"/>
       <c r="O106" s="17" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="P106" s="17"/>
       <c r="Q106" s="17"/>
@@ -12998,7 +13004,7 @@
       <c r="M107" s="18"/>
       <c r="N107" s="17"/>
       <c r="O107" s="17" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="P107" s="17"/>
       <c r="Q107" s="17"/>
@@ -13048,7 +13054,7 @@
       <c r="M108" s="18"/>
       <c r="N108" s="17"/>
       <c r="O108" s="17" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="P108" s="17"/>
       <c r="Q108" s="17"/>
@@ -13098,7 +13104,7 @@
       <c r="M109" s="18"/>
       <c r="N109" s="17"/>
       <c r="O109" s="17" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="P109" s="17"/>
       <c r="Q109" s="17"/>
@@ -13148,7 +13154,7 @@
       <c r="M110" s="18"/>
       <c r="N110" s="17"/>
       <c r="O110" s="17" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="P110" s="17"/>
       <c r="Q110" s="17"/>
@@ -13198,7 +13204,7 @@
       <c r="M111" s="18"/>
       <c r="N111" s="17"/>
       <c r="O111" s="17" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="P111" s="17"/>
       <c r="Q111" s="17"/>
@@ -13248,7 +13254,7 @@
       <c r="M112" s="18"/>
       <c r="N112" s="17"/>
       <c r="O112" s="17" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="P112" s="17"/>
       <c r="Q112" s="17"/>
@@ -13298,7 +13304,7 @@
       <c r="M113" s="18"/>
       <c r="N113" s="17"/>
       <c r="O113" s="17" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="P113" s="17"/>
       <c r="Q113" s="17"/>
@@ -13348,7 +13354,7 @@
       <c r="M114" s="18"/>
       <c r="N114" s="17"/>
       <c r="O114" s="17" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="P114" s="17"/>
       <c r="Q114" s="17"/>
@@ -13398,7 +13404,7 @@
       <c r="M115" s="18"/>
       <c r="N115" s="17"/>
       <c r="O115" s="17" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="P115" s="17"/>
       <c r="Q115" s="17"/>
@@ -13448,7 +13454,7 @@
       <c r="M116" s="18"/>
       <c r="N116" s="17"/>
       <c r="O116" s="17" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="P116" s="17"/>
       <c r="Q116" s="17"/>
@@ -13498,7 +13504,7 @@
       <c r="M117" s="18"/>
       <c r="N117" s="17"/>
       <c r="O117" s="17" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="P117" s="17"/>
       <c r="Q117" s="17"/>
@@ -13543,7 +13549,7 @@
       <c r="H118" s="60"/>
       <c r="I118" s="28"/>
       <c r="J118" s="29" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="K118" s="29"/>
       <c r="L118" s="82"/>
@@ -13597,7 +13603,7 @@
       <c r="H119" s="60"/>
       <c r="I119" s="28"/>
       <c r="J119" s="29" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="K119" s="29"/>
       <c r="L119" s="82"/>
@@ -13651,7 +13657,7 @@
       <c r="H120" s="60"/>
       <c r="I120" s="28"/>
       <c r="J120" s="29" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="K120" s="29"/>
       <c r="L120" s="82"/>
@@ -13705,7 +13711,7 @@
       <c r="H121" s="60"/>
       <c r="I121" s="28"/>
       <c r="J121" s="29" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="K121" s="29"/>
       <c r="L121" s="82"/>
@@ -13759,7 +13765,7 @@
       <c r="H122" s="60"/>
       <c r="I122" s="28"/>
       <c r="J122" s="29" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="K122" s="29"/>
       <c r="L122" s="82"/>
@@ -13813,7 +13819,7 @@
       <c r="H123" s="60"/>
       <c r="I123" s="28"/>
       <c r="J123" s="29" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="K123" s="29"/>
       <c r="L123" s="82"/>
@@ -13867,7 +13873,7 @@
       <c r="H124" s="60"/>
       <c r="I124" s="28"/>
       <c r="J124" s="29" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="K124" s="29"/>
       <c r="L124" s="82"/>
@@ -13921,7 +13927,7 @@
       <c r="H125" s="60"/>
       <c r="I125" s="28"/>
       <c r="J125" s="29" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="K125" s="29"/>
       <c r="L125" s="82"/>
@@ -13975,7 +13981,7 @@
       <c r="H126" s="60"/>
       <c r="I126" s="28"/>
       <c r="J126" s="29" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="K126" s="29"/>
       <c r="L126" s="82"/>
@@ -14029,7 +14035,7 @@
       <c r="H127" s="60"/>
       <c r="I127" s="28"/>
       <c r="J127" s="29" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="K127" s="29"/>
       <c r="L127" s="82"/>
@@ -14083,7 +14089,7 @@
       <c r="H128" s="60"/>
       <c r="I128" s="28"/>
       <c r="J128" s="29" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="K128" s="29"/>
       <c r="L128" s="82"/>
@@ -14137,7 +14143,7 @@
       <c r="H129" s="60"/>
       <c r="I129" s="28"/>
       <c r="J129" s="29" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="K129" s="29"/>
       <c r="L129" s="82"/>
@@ -14191,7 +14197,7 @@
       <c r="H130" s="60"/>
       <c r="I130" s="28"/>
       <c r="J130" s="29" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="K130" s="29"/>
       <c r="L130" s="82"/>
@@ -14245,7 +14251,7 @@
       <c r="H131" s="60"/>
       <c r="I131" s="28"/>
       <c r="J131" s="29" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="K131" s="29"/>
       <c r="L131" s="82"/>
@@ -14299,7 +14305,7 @@
       <c r="H132" s="60"/>
       <c r="I132" s="28"/>
       <c r="J132" s="29" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="K132" s="29"/>
       <c r="L132" s="82"/>
@@ -14353,7 +14359,7 @@
       <c r="H133" s="60"/>
       <c r="I133" s="28"/>
       <c r="J133" s="29" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="K133" s="29"/>
       <c r="L133" s="82"/>
@@ -14618,7 +14624,7 @@
       <c r="M138" s="18"/>
       <c r="N138" s="17"/>
       <c r="O138" s="17" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="P138" s="17"/>
       <c r="Q138" s="17"/>
@@ -14668,7 +14674,7 @@
       <c r="M139" s="18"/>
       <c r="N139" s="17"/>
       <c r="O139" s="17" t="s">
-        <v>1152</v>
+        <v>1145</v>
       </c>
       <c r="P139" s="17"/>
       <c r="Q139" s="17"/>
@@ -14696,7 +14702,7 @@
       </c>
       <c r="AD139" s="37"/>
     </row>
-    <row r="140" spans="1:30" ht="48" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:30" ht="60" x14ac:dyDescent="0.15">
       <c r="A140" s="73">
         <v>55700003</v>
       </c>
@@ -14719,7 +14725,7 @@
       <c r="N140" s="17"/>
       <c r="O140" s="17"/>
       <c r="P140" s="17" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="Q140" s="17"/>
       <c r="R140" s="20"/>
@@ -14748,7 +14754,7 @@
       </c>
       <c r="AD140" s="37"/>
     </row>
-    <row r="141" spans="1:30" ht="72" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:30" ht="120" x14ac:dyDescent="0.15">
       <c r="A141" s="73">
         <v>55700004</v>
       </c>
@@ -14771,7 +14777,7 @@
       <c r="H141" s="60"/>
       <c r="I141" s="26"/>
       <c r="J141" s="47" t="s">
-        <v>1069</v>
+        <v>1151</v>
       </c>
       <c r="K141" s="47"/>
       <c r="L141" s="99"/>
@@ -14833,7 +14839,7 @@
       <c r="P142" s="17"/>
       <c r="Q142" s="17"/>
       <c r="R142" s="20" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="S142" s="41">
         <v>1</v>
@@ -14885,7 +14891,7 @@
       <c r="P143" s="17"/>
       <c r="Q143" s="17"/>
       <c r="R143" s="20" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
       <c r="S143" s="41">
         <v>1</v>
@@ -14912,7 +14918,7 @@
       </c>
       <c r="AD143" s="25"/>
     </row>
-    <row r="144" spans="1:30" ht="84" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:30" ht="108" x14ac:dyDescent="0.15">
       <c r="A144" s="73">
         <v>55700007</v>
       </c>
@@ -14939,7 +14945,7 @@
       <c r="R144" s="20"/>
       <c r="S144" s="41"/>
       <c r="T144" s="20" t="s">
-        <v>1151</v>
+        <v>1155</v>
       </c>
       <c r="U144" s="46" t="s">
         <v>235</v>
@@ -14987,7 +14993,7 @@
       <c r="H145" s="60"/>
       <c r="I145" s="26"/>
       <c r="J145" s="47" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="K145" s="47"/>
       <c r="L145" s="99"/>
@@ -15049,7 +15055,7 @@
       <c r="H146" s="60"/>
       <c r="I146" s="26"/>
       <c r="J146" s="47" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="K146" s="47"/>
       <c r="L146" s="99"/>
@@ -15101,7 +15107,7 @@
       <c r="H147" s="60"/>
       <c r="I147" s="26"/>
       <c r="J147" s="47" t="s">
-        <v>1154</v>
+        <v>1146</v>
       </c>
       <c r="K147" s="47"/>
       <c r="L147" s="99"/>
@@ -15157,7 +15163,7 @@
       <c r="N148" s="30"/>
       <c r="O148" s="17"/>
       <c r="P148" s="17" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="Q148" s="17"/>
       <c r="R148" s="20"/>
@@ -15496,7 +15502,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="155" spans="1:30" ht="60" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:30" ht="72" x14ac:dyDescent="0.15">
       <c r="A155" s="55">
         <v>55900011</v>
       </c>
@@ -15513,7 +15519,7 @@
       <c r="H155" s="60"/>
       <c r="I155" s="26"/>
       <c r="J155" s="47" t="s">
-        <v>1133</v>
+        <v>1156</v>
       </c>
       <c r="K155" s="47"/>
       <c r="L155" s="99"/>
@@ -15571,7 +15577,7 @@
       <c r="H156" s="60"/>
       <c r="I156" s="28"/>
       <c r="J156" s="29" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="K156" s="29"/>
       <c r="L156" s="82"/>
@@ -15990,7 +15996,7 @@
       </c>
       <c r="AD163" s="48"/>
     </row>
-    <row r="164" spans="1:30" ht="108" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:30" ht="120" x14ac:dyDescent="0.15">
       <c r="A164" s="83">
         <v>55900020</v>
       </c>
@@ -16007,7 +16013,7 @@
       <c r="H164" s="78"/>
       <c r="I164" s="96"/>
       <c r="J164" s="29" t="s">
-        <v>1148</v>
+        <v>1152</v>
       </c>
       <c r="K164" s="95"/>
       <c r="L164" s="101"/>
@@ -16117,7 +16123,7 @@
       <c r="H166" s="60"/>
       <c r="I166" s="26"/>
       <c r="J166" s="82" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="K166" s="47"/>
       <c r="L166" s="99"/>
@@ -16173,7 +16179,7 @@
       <c r="H167" s="60"/>
       <c r="I167" s="26"/>
       <c r="J167" s="82" t="s">
-        <v>1155</v>
+        <v>1147</v>
       </c>
       <c r="K167" s="47"/>
       <c r="L167" s="99"/>
@@ -16206,7 +16212,7 @@
       </c>
       <c r="AD167" s="48"/>
     </row>
-    <row r="168" spans="1:30" ht="72" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:30" ht="84" x14ac:dyDescent="0.15">
       <c r="A168" s="83">
         <v>55900024</v>
       </c>
@@ -16229,7 +16235,7 @@
       <c r="H168" s="60"/>
       <c r="I168" s="26"/>
       <c r="J168" s="29" t="s">
-        <v>1145</v>
+        <v>1153</v>
       </c>
       <c r="K168" s="29"/>
       <c r="L168" s="99"/>
@@ -16264,7 +16270,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="169" spans="1:30" ht="72" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:30" ht="84" x14ac:dyDescent="0.15">
       <c r="A169" s="55">
         <v>55900025</v>
       </c>
@@ -16295,7 +16301,7 @@
       <c r="P169" s="17"/>
       <c r="Q169" s="17"/>
       <c r="R169" s="20" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="S169" s="41">
         <v>2</v>
@@ -16449,7 +16455,7 @@
       <c r="H172" s="60"/>
       <c r="I172" s="26"/>
       <c r="J172" s="82" t="s">
-        <v>1147</v>
+        <v>1142</v>
       </c>
       <c r="K172" s="47"/>
       <c r="L172" s="99"/>
@@ -16499,7 +16505,7 @@
       <c r="H173" s="60"/>
       <c r="I173" s="26"/>
       <c r="J173" s="82" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="K173" s="47"/>
       <c r="L173" s="99"/>
@@ -16518,7 +16524,7 @@
         <v>362</v>
       </c>
       <c r="W173" s="16" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="X173" s="25"/>
       <c r="Y173" s="25"/>
@@ -16532,7 +16538,7 @@
       </c>
       <c r="AD173" s="48"/>
     </row>
-    <row r="174" spans="1:30" ht="48" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:30" ht="60" x14ac:dyDescent="0.15">
       <c r="A174" s="55">
         <v>55900030</v>
       </c>
@@ -16554,7 +16560,7 @@
       <c r="K174" s="47"/>
       <c r="L174" s="99"/>
       <c r="M174" s="18" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="N174" s="30"/>
       <c r="O174" s="17"/>
@@ -16659,7 +16665,7 @@
       <c r="H176" s="60"/>
       <c r="I176" s="26"/>
       <c r="J176" s="90" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="K176" s="29"/>
       <c r="L176" s="99"/>
@@ -16875,7 +16881,7 @@
       <c r="H180" s="60"/>
       <c r="I180" s="26"/>
       <c r="J180" s="90" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="K180" s="29"/>
       <c r="L180" s="99"/>
@@ -16910,7 +16916,7 @@
       </c>
       <c r="AD180" s="48"/>
     </row>
-    <row r="181" spans="1:30" ht="72" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:30" ht="84" x14ac:dyDescent="0.15">
       <c r="A181" s="55">
         <v>55900037</v>
       </c>
@@ -16933,7 +16939,7 @@
       <c r="H181" s="60"/>
       <c r="I181" s="26"/>
       <c r="J181" s="29" t="s">
-        <v>1134</v>
+        <v>1154</v>
       </c>
       <c r="K181" s="29"/>
       <c r="L181" s="99"/>
@@ -16991,7 +16997,7 @@
       <c r="H182" s="60"/>
       <c r="I182" s="26"/>
       <c r="J182" s="29" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="K182" s="29"/>
       <c r="L182" s="99"/>
@@ -17362,7 +17368,7 @@
         <v>40</v>
       </c>
       <c r="AC188" s="25" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="AD188" s="48" t="s">
         <v>1017</v>
@@ -17391,7 +17397,7 @@
       <c r="H189" s="60"/>
       <c r="I189" s="26"/>
       <c r="J189" s="90" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="K189" s="29"/>
       <c r="L189" s="99"/>
@@ -17447,7 +17453,7 @@
       <c r="H190" s="60"/>
       <c r="I190" s="26"/>
       <c r="J190" s="90" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="K190" s="29"/>
       <c r="L190" s="99"/>
@@ -17507,7 +17513,7 @@
       <c r="H191" s="60"/>
       <c r="I191" s="26"/>
       <c r="J191" s="90" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="K191" s="29"/>
       <c r="L191" s="99"/>
@@ -17594,7 +17600,7 @@
       </c>
       <c r="AD192" s="37"/>
     </row>
-    <row r="193" spans="1:30" ht="48" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:30" ht="60" x14ac:dyDescent="0.15">
       <c r="A193" s="55">
         <v>55900049</v>
       </c>
@@ -17616,7 +17622,7 @@
       <c r="K193" s="29"/>
       <c r="L193" s="82"/>
       <c r="M193" s="18" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="N193" s="17" t="s">
         <v>795</v>
@@ -17775,7 +17781,7 @@
       <c r="H196" s="60"/>
       <c r="I196" s="26"/>
       <c r="J196" s="90" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="K196" s="29"/>
       <c r="L196" s="99"/>
@@ -17841,7 +17847,7 @@
       <c r="P197" s="17"/>
       <c r="Q197" s="17"/>
       <c r="R197" s="20" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="S197" s="41">
         <v>1</v>
@@ -17887,7 +17893,7 @@
       <c r="H198" s="60"/>
       <c r="I198" s="26"/>
       <c r="J198" s="90" t="s">
-        <v>1146</v>
+        <v>1141</v>
       </c>
       <c r="K198" s="29"/>
       <c r="L198" s="99"/>
@@ -17989,13 +17995,13 @@
       <c r="H200" s="60"/>
       <c r="I200" s="26"/>
       <c r="J200" s="90" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="K200" s="90" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="L200" s="90" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="M200" s="27"/>
       <c r="N200" s="30"/>
@@ -19132,7 +19138,7 @@
       </c>
       <c r="AD221" s="48"/>
     </row>
-    <row r="222" spans="1:30" ht="168" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:30" ht="156" x14ac:dyDescent="0.15">
       <c r="A222" s="91">
         <v>55990107</v>
       </c>
@@ -19165,7 +19171,7 @@
       <c r="R222" s="20"/>
       <c r="S222" s="41"/>
       <c r="T222" s="20" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="U222" s="35" t="s">
         <v>235</v>

</xml_diff>

<commit_message>
fix some skill bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="1158">
   <si>
     <t>复原</t>
   </si>
@@ -4317,6 +4317,10 @@
   </si>
   <si>
     <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.15);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.WeaponId&gt;0</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6658,72 +6662,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFFFFF79"/>
       <color rgb="FFAFEAFF"/>
@@ -6790,7 +6728,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -7106,11 +7044,11 @@
   <dimension ref="A1:AD224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="G146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D156" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="J155" sqref="J155"/>
+      <selection pane="bottomRight" activeCell="K156" sqref="K156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -15682,7 +15620,7 @@
       <c r="G158" s="43"/>
       <c r="H158" s="60"/>
       <c r="I158" s="28" t="s">
-        <v>273</v>
+        <v>1157</v>
       </c>
       <c r="J158" s="29"/>
       <c r="K158" s="29"/>

</xml_diff>

<commit_message>
fix a skill icon bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -4157,9 +4157,6 @@
     <t>d.Action.AddBuff(56000203,skl.Level,1.5);</t>
   </si>
   <si>
-    <t>skl.Levelfeng</t>
-  </si>
-  <si>
     <t>s.Action.AddBuff(56000201,skl.Level,1.1);</t>
   </si>
   <si>
@@ -4387,6 +4384,10 @@
   </si>
   <si>
     <t>必杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lvfeng</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7113,11 +7114,11 @@
   <dimension ref="A1:AD227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="R199" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="M5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="W204" sqref="W204"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7604,7 +7605,7 @@
       <c r="H7" s="59"/>
       <c r="I7" s="28"/>
       <c r="J7" s="29" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="K7" s="29"/>
       <c r="L7" s="82"/>
@@ -8260,11 +8261,11 @@
       <c r="H19" s="59"/>
       <c r="I19" s="28"/>
       <c r="J19" s="29" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="K19" s="29"/>
       <c r="L19" s="82" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="M19" s="18"/>
       <c r="N19" s="17"/>
@@ -8364,7 +8365,7 @@
       <c r="H21" s="59"/>
       <c r="I21" s="26"/>
       <c r="J21" s="29" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
@@ -8418,7 +8419,7 @@
         <v>1051</v>
       </c>
       <c r="J22" s="90" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="K22" s="105"/>
       <c r="L22" s="99"/>
@@ -8624,7 +8625,7 @@
       <c r="H26" s="59"/>
       <c r="I26" s="28"/>
       <c r="J26" s="29" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="K26" s="29"/>
       <c r="L26" s="82"/>
@@ -8884,7 +8885,7 @@
       <c r="L31" s="82"/>
       <c r="M31" s="18"/>
       <c r="N31" s="17" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
@@ -9296,7 +9297,7 @@
       <c r="L39" s="82"/>
       <c r="M39" s="18"/>
       <c r="N39" s="17" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="O39" s="17"/>
       <c r="P39" s="17"/>
@@ -9514,7 +9515,7 @@
       <c r="P43" s="17"/>
       <c r="Q43" s="17"/>
       <c r="R43" s="20" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="S43" s="41">
         <v>1</v>
@@ -9575,7 +9576,7 @@
       <c r="O44" s="17"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="17" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="R44" s="20"/>
       <c r="S44" s="41"/>
@@ -9587,7 +9588,7 @@
         <v>230</v>
       </c>
       <c r="W44" s="16" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="X44" s="25"/>
       <c r="Y44" s="25" t="s">
@@ -9602,7 +9603,7 @@
         <v>449</v>
       </c>
       <c r="AD44" s="48" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="45" spans="1:30" ht="108" x14ac:dyDescent="0.15">
@@ -9628,7 +9629,7 @@
       <c r="H45" s="60"/>
       <c r="I45" s="86"/>
       <c r="J45" s="47" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="K45" s="85"/>
       <c r="L45" s="100"/>
@@ -10170,7 +10171,7 @@
       <c r="H54" s="60"/>
       <c r="I54" s="86"/>
       <c r="J54" s="47" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="K54" s="85"/>
       <c r="L54" s="100"/>
@@ -10206,7 +10207,7 @@
         <v>711</v>
       </c>
       <c r="AD54" s="48" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="96" x14ac:dyDescent="0.15">
@@ -10232,7 +10233,7 @@
       <c r="H55" s="60"/>
       <c r="I55" s="86"/>
       <c r="J55" s="47" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="K55" s="85"/>
       <c r="L55" s="100"/>
@@ -10290,7 +10291,7 @@
       <c r="H56" s="60"/>
       <c r="I56" s="26"/>
       <c r="J56" s="90" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="K56" s="29"/>
       <c r="L56" s="99"/>
@@ -10350,7 +10351,7 @@
       <c r="H57" s="60"/>
       <c r="I57" s="86"/>
       <c r="J57" s="47" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="K57" s="85"/>
       <c r="L57" s="100"/>
@@ -10475,7 +10476,7 @@
       <c r="O59" s="17"/>
       <c r="P59" s="17"/>
       <c r="Q59" s="17" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="R59" s="20"/>
       <c r="S59" s="41"/>
@@ -10530,7 +10531,7 @@
       <c r="H60" s="60"/>
       <c r="I60" s="86"/>
       <c r="J60" s="47" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="K60" s="85"/>
       <c r="L60" s="100"/>
@@ -14635,7 +14636,7 @@
       <c r="M138" s="18"/>
       <c r="N138" s="17"/>
       <c r="O138" s="17" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="P138" s="17"/>
       <c r="Q138" s="17"/>
@@ -14685,7 +14686,7 @@
       <c r="M139" s="18"/>
       <c r="N139" s="17"/>
       <c r="O139" s="17" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="P139" s="17"/>
       <c r="Q139" s="17"/>
@@ -14736,7 +14737,7 @@
       <c r="N140" s="17"/>
       <c r="O140" s="17"/>
       <c r="P140" s="17" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="Q140" s="17"/>
       <c r="R140" s="20"/>
@@ -14788,7 +14789,7 @@
       <c r="H141" s="60"/>
       <c r="I141" s="26"/>
       <c r="J141" s="47" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="K141" s="47"/>
       <c r="L141" s="99"/>
@@ -14850,7 +14851,7 @@
       <c r="P142" s="17"/>
       <c r="Q142" s="17"/>
       <c r="R142" s="20" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="S142" s="41">
         <v>1</v>
@@ -14902,7 +14903,7 @@
       <c r="P143" s="17"/>
       <c r="Q143" s="17"/>
       <c r="R143" s="20" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="S143" s="41">
         <v>1</v>
@@ -14956,7 +14957,7 @@
       <c r="R144" s="20"/>
       <c r="S144" s="41"/>
       <c r="T144" s="20" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="U144" s="46" t="s">
         <v>235</v>
@@ -15118,7 +15119,7 @@
       <c r="H147" s="60"/>
       <c r="I147" s="26"/>
       <c r="J147" s="47" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K147" s="47"/>
       <c r="L147" s="99"/>
@@ -15530,7 +15531,7 @@
       <c r="H155" s="60"/>
       <c r="I155" s="26"/>
       <c r="J155" s="47" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="K155" s="47"/>
       <c r="L155" s="99"/>
@@ -15693,7 +15694,7 @@
       <c r="G158" s="43"/>
       <c r="H158" s="60"/>
       <c r="I158" s="28" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J158" s="29"/>
       <c r="K158" s="29"/>
@@ -16024,7 +16025,7 @@
       <c r="H164" s="78"/>
       <c r="I164" s="96"/>
       <c r="J164" s="29" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="K164" s="95"/>
       <c r="L164" s="101"/>
@@ -16190,7 +16191,7 @@
       <c r="H167" s="60"/>
       <c r="I167" s="26"/>
       <c r="J167" s="82" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="K167" s="47"/>
       <c r="L167" s="99"/>
@@ -16246,7 +16247,7 @@
       <c r="H168" s="60"/>
       <c r="I168" s="26"/>
       <c r="J168" s="29" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="K168" s="29"/>
       <c r="L168" s="99"/>
@@ -16466,7 +16467,7 @@
       <c r="H172" s="60"/>
       <c r="I172" s="26"/>
       <c r="J172" s="82" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="K172" s="47"/>
       <c r="L172" s="99"/>
@@ -16516,7 +16517,7 @@
       <c r="H173" s="60"/>
       <c r="I173" s="26"/>
       <c r="J173" s="82" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="K173" s="47"/>
       <c r="L173" s="99"/>
@@ -16535,7 +16536,7 @@
         <v>362</v>
       </c>
       <c r="W173" s="16" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="X173" s="25"/>
       <c r="Y173" s="25"/>
@@ -16950,7 +16951,7 @@
       <c r="H181" s="60"/>
       <c r="I181" s="26"/>
       <c r="J181" s="29" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="K181" s="29"/>
       <c r="L181" s="99"/>
@@ -17008,7 +17009,7 @@
       <c r="H182" s="60"/>
       <c r="I182" s="26"/>
       <c r="J182" s="29" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="K182" s="29"/>
       <c r="L182" s="99"/>
@@ -17224,7 +17225,7 @@
         <v>758</v>
       </c>
       <c r="AD185" s="48" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="186" spans="1:30" ht="48" x14ac:dyDescent="0.15">
@@ -17358,7 +17359,7 @@
       <c r="P188" s="17"/>
       <c r="Q188" s="17"/>
       <c r="R188" s="20" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="S188" s="41">
         <v>2</v>
@@ -17381,7 +17382,7 @@
         <v>40</v>
       </c>
       <c r="AC188" s="25" t="s">
-        <v>1113</v>
+        <v>1173</v>
       </c>
       <c r="AD188" s="48" t="s">
         <v>1014</v>
@@ -17410,7 +17411,7 @@
       <c r="H189" s="60"/>
       <c r="I189" s="26"/>
       <c r="J189" s="90" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="K189" s="29"/>
       <c r="L189" s="99"/>
@@ -17442,7 +17443,7 @@
         <v>768</v>
       </c>
       <c r="AD189" s="48" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="190" spans="1:30" ht="84" x14ac:dyDescent="0.15">
@@ -17637,7 +17638,7 @@
       <c r="K193" s="29"/>
       <c r="L193" s="82"/>
       <c r="M193" s="18" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="N193" s="17" t="s">
         <v>794</v>
@@ -17720,7 +17721,7 @@
         <v>807</v>
       </c>
       <c r="AD194" s="48" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="195" spans="1:30" ht="36" x14ac:dyDescent="0.15">
@@ -17759,7 +17760,7 @@
         <v>230</v>
       </c>
       <c r="W195" s="10" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="X195" s="10"/>
       <c r="Y195" s="61"/>
@@ -17864,7 +17865,7 @@
       <c r="P197" s="17"/>
       <c r="Q197" s="17"/>
       <c r="R197" s="20" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="S197" s="41">
         <v>1</v>
@@ -17910,7 +17911,7 @@
       <c r="H198" s="60"/>
       <c r="I198" s="26"/>
       <c r="J198" s="90" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="K198" s="29"/>
       <c r="L198" s="99"/>
@@ -18012,13 +18013,13 @@
       <c r="H200" s="60"/>
       <c r="I200" s="26"/>
       <c r="J200" s="90" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="K200" s="90" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="L200" s="90" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="M200" s="27"/>
       <c r="N200" s="30"/>
@@ -18211,7 +18212,7 @@
       </c>
       <c r="B204" s="55"/>
       <c r="C204" s="55" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="D204" s="25" t="s">
         <v>309</v>
@@ -18229,7 +18230,7 @@
       <c r="O204" s="17"/>
       <c r="P204" s="17"/>
       <c r="Q204" s="17" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="R204" s="20"/>
       <c r="S204" s="41"/>
@@ -18241,7 +18242,7 @@
         <v>230</v>
       </c>
       <c r="W204" s="16" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="X204" s="25"/>
       <c r="Y204" s="25"/>
@@ -18251,10 +18252,10 @@
         <v>60</v>
       </c>
       <c r="AC204" s="25" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="AD204" s="48" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="205" spans="1:30" ht="24" x14ac:dyDescent="0.15">
@@ -18263,7 +18264,7 @@
       </c>
       <c r="B205" s="55"/>
       <c r="C205" s="55" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="D205" s="25" t="s">
         <v>309</v>
@@ -18280,7 +18281,7 @@
       <c r="N205" s="30"/>
       <c r="O205" s="17"/>
       <c r="P205" s="17" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="Q205" s="17"/>
       <c r="R205" s="20"/>
@@ -18293,7 +18294,7 @@
         <v>230</v>
       </c>
       <c r="W205" s="16" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="X205" s="25"/>
       <c r="Y205" s="25"/>
@@ -18303,10 +18304,10 @@
         <v>20</v>
       </c>
       <c r="AC205" s="25" t="s">
+        <v>1165</v>
+      </c>
+      <c r="AD205" s="48" t="s">
         <v>1166</v>
-      </c>
-      <c r="AD205" s="48" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="206" spans="1:30" ht="84" x14ac:dyDescent="0.15">
@@ -18315,7 +18316,7 @@
       </c>
       <c r="B206" s="83"/>
       <c r="C206" s="55" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="D206" s="25" t="s">
         <v>309</v>
@@ -18326,7 +18327,7 @@
       <c r="H206" s="78"/>
       <c r="I206" s="96"/>
       <c r="J206" s="29" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="K206" s="95"/>
       <c r="L206" s="101"/>
@@ -18345,7 +18346,7 @@
         <v>230</v>
       </c>
       <c r="W206" s="10" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="X206" s="77"/>
       <c r="Y206" s="77"/>
@@ -18355,7 +18356,7 @@
         <v>15</v>
       </c>
       <c r="AC206" s="25" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="AD206" s="48" t="s">
         <v>1019</v>
@@ -19344,7 +19345,7 @@
       <c r="R225" s="20"/>
       <c r="S225" s="41"/>
       <c r="T225" s="20" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="U225" s="35" t="s">
         <v>235</v>

</xml_diff>

<commit_message>
balance the scroll cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{989041ED-5ABB-4C8E-99EF-CF369533F8A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="7" r:id="rId1"/>
@@ -21,13 +20,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Real</author>
     <author>real</author>
   </authors>
   <commentList>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="S1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="AB1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB78" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="AB78" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -144,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="1173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="1176">
   <si>
     <t>复原</t>
   </si>
@@ -4198,200 +4197,213 @@
     <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.AddPArmor(s.Atk*2);</t>
   </si>
   <si>
+    <t>召唤时，如果对方手牌数&gt;5，提高30%攻击和2点防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.ChangeAI("Tank");s.Action.AddAttrModify("Skill",skl.Id,"Def",8);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Spd",8);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.15);s.Action.AddAttrModify("Skill",skl.Id,"Def",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*MathTool.GetRandom(0f,0.5));</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.SetPDamageRate(0.5);d.Action.AddAttrModify("Skill",skl.Id,"Atk",-d.Atk*0.05);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Rival.CardNumber&gt;5) {s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.3);s.Action.AddAttrModify("Skill",skl.Id,"Def",2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(MathTool.GetRandom(0f,1f)&lt;0.5)s.Action.AddAttrModify("Skill",skl.Id,"Def",5);else s.Action.AddAttrModify("Skill",skl.Id,"Crt",5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*s.Action.GetMonsterCountByRace(4)*0.2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.4);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Hit",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*s.Owner.CardNumber);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(s.Owner.CardNumber&gt;=6) s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.5);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.Action.AddAttrModify("Skill",skl.Id,"Def",1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterStar(1,3).Top(1)) mon.Action.SuddenDeath();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",d.Atk*0.3);s.Action.AddMaxHp("Skill",skl.Id,d.MaxHp*0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonsterGhost(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){s.Action.EatTomb(mon);s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);s.Action.AddMaxHp("Skill",skl.Id,s.MaxHp*0.1);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(s.Attr))if(s.IsLeft==o.IsLeft&amp;&amp;s.Id!=o.Id){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.2);o.Action.AddAttrModify("Skill",skl.Id,"Atk",o.Atk*0.2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterAttr(1)){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.15);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(p.IsLeft==s.IsLeft){s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);s.Action.AddMaxHp("Skill",skl.Id, s.MaxHp*0.1);eff=true;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.15);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.WeaponId&gt;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(o, 1,s.Atk,"waterball");</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时对最近的3个敌人造成伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>亡语</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鬼船</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡后召唤2个随机2星亡灵</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤,亡语</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>(连击)召唤时召唤一个怪物</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.SummonRandomAttr("around",2,-1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>guichuan</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.SummonRandomRace("around",10,2);s.Action.SummonRandomRace("around",10,2);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怨念</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Action.AddBuff(56000004,skl.Level,3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时使凶手削弱3回合</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yuannian</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>亡语,状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙暴</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterType(12))if(s.IsLeft==o.IsLeft&amp;&amp;s.Id!=o.Id){o.Action.AddAttrModify("Skill",skl.Id,"Atk",o.Atk*0.2);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>召唤时永久提高场上己方鱼类20%攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shabao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.SuddenDeath();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>必杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lvfeng</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>electhit</t>
+  </si>
+  <si>
+    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.AddHp(s.Cure);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>if(type==3){foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(mon,3,s.Atk, "firearrow");eff=true;}</t>
-  </si>
-  <si>
-    <t>召唤时，如果对方手牌数&gt;5，提高30%攻击和2点防御</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.ChangeAI("Tank");s.Action.AddAttrModify("Skill",skl.Id,"Def",8);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Spd",8);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.15);s.Action.AddAttrModify("Skill",skl.Id,"Def",1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*MathTool.GetRandom(0f,0.5));</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>damage.SetPDamageRate(0.5);d.Action.AddAttrModify("Skill",skl.Id,"Atk",-d.Atk*0.05);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Rival.CardNumber&gt;5) {s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.3);s.Action.AddAttrModify("Skill",skl.Id,"Def",2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(MathTool.GetRandom(0f,1f)&lt;0.5)s.Action.AddAttrModify("Skill",skl.Id,"Def",5);else s.Action.AddAttrModify("Skill",skl.Id,"Crt",5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*s.Action.GetMonsterCountByRace(4)*0.2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.4);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Hit",1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*s.Owner.CardNumber);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(s.Owner.CardNumber&gt;=6) s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.5);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)) if(s.Id!=o.Id) o.Action.AddAttrModify("Skill",skl.Id,"Def",1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterStar(1,3).Top(1)) mon.Action.SuddenDeath();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddAttrModify("Skill",skl.Id,"Atk",d.Atk*0.3);s.Action.AddMaxHp("Skill",skl.Id,d.MaxHp*0.3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonsterGhost(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){s.Action.EatTomb(mon);s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);s.Action.AddMaxHp("Skill",skl.Id,s.MaxHp*0.1);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(s.Attr))if(s.IsLeft==o.IsLeft&amp;&amp;s.Id!=o.Id){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.2);o.Action.AddAttrModify("Skill",skl.Id,"Atk",o.Atk*0.2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterAttr(1)){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position)){o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.15);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(p.IsLeft==s.IsLeft){s.Action.AddAttrModify("Skill",skl.Id,"Atk",s.Atk*0.1);s.Action.AddMaxHp("Skill",skl.Id, s.MaxHp*0.1);eff=true;}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterAttr(0)) o.Action.AddMaxHp("Skill",skl.Id,o.MaxHp*0.15);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.WeaponId&gt;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortRandom().Top(3)) s.Action.AddMissile(o, 1,s.Atk,"waterball");</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时对最近的3个敌人造成伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>亡语</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>鬼船</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡后召唤2个随机2星亡灵</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤,亡语</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>(连击)召唤时召唤一个怪物</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.SummonRandomAttr("around",2,-1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>guichuan</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.SummonRandomRace("around",10,2);s.Action.SummonRandomRace("around",10,2);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>怨念</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>s.Action.AddBuff(56000004,skl.Level,3);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时使凶手削弱3回合</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yuannian</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>亡语,状态</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>沙暴</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster o in s.Map.GetAllMonster(s.Position).FilterType(12))if(s.IsLeft==o.IsLeft&amp;&amp;s.Id!=o.Id){o.Action.AddAttrModify("Skill",skl.Id,"Atk",o.Atk*0.2);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>召唤时永久提高场上己方鱼类20%攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shabao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).FilterId(s.Id).SortDistance(true).Top(1)) mon.Action.SuddenDeath();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>必杀</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lvfeng</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>electhit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次使用法术牌，治疗4格范围内随机友军(200%效果)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(type==3){foreach(IMonster mon in s.Map.GetRangeMonster(s.IsLeft,skl.Target,skl.Shape,skl.Range,s.Position).SortRandom().Top(1)) mon.AddHp(s.Cure*2);eff=true;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6729,6 +6741,72 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFFFFF79"/>
       <color rgb="FFAFEAFF"/>
@@ -6746,42 +6824,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3_25" displayName="表3_25" ref="A3:AD227" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
-  <autoFilter ref="A3:AD227" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:AD228" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
+  <autoFilter ref="A3:AD228"/>
   <sortState ref="A4:AD227">
     <sortCondition ref="A3:A227"/>
   </sortState>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="29"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Alias" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Target" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Range" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="PointSelf" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Tag" dataDxfId="22"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="CanBurst" dataDxfId="21"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="OnAdd" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="OnRemove" dataDxfId="19"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="OnSilent" dataDxfId="18"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="CheckHit" dataDxfId="17"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="CheckDamage" dataDxfId="16"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="AfterHit" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="DeathHit" dataDxfId="14"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="DeathSkill" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CheckSpecial" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="SpecialCd" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="OnUseCard" dataDxfId="10"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Active" dataDxfId="9"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="IsRandom" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="GetDescript" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="DescriptBuffId" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Effect" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="EffectArea" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cover" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Mark" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Icon" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Remark" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="29"/>
+    <tableColumn id="21" name="Alias" dataDxfId="28"/>
+    <tableColumn id="2" name="Name" dataDxfId="27"/>
+    <tableColumn id="3" name="Type" dataDxfId="26"/>
+    <tableColumn id="11" name="Target" dataDxfId="25"/>
+    <tableColumn id="12" name="Range" dataDxfId="24"/>
+    <tableColumn id="13" name="PointSelf" dataDxfId="23"/>
+    <tableColumn id="14" name="Tag" dataDxfId="22"/>
+    <tableColumn id="27" name="CanBurst" dataDxfId="21"/>
+    <tableColumn id="24" name="OnAdd" dataDxfId="20"/>
+    <tableColumn id="4" name="OnRemove" dataDxfId="19"/>
+    <tableColumn id="30" name="OnSilent" dataDxfId="18"/>
+    <tableColumn id="22" name="CheckHit" dataDxfId="17"/>
+    <tableColumn id="26" name="CheckDamage" dataDxfId="16"/>
+    <tableColumn id="29" name="AfterHit" dataDxfId="15"/>
+    <tableColumn id="15" name="DeathHit" dataDxfId="14"/>
+    <tableColumn id="28" name="DeathSkill" dataDxfId="13"/>
+    <tableColumn id="5" name="CheckSpecial" dataDxfId="12"/>
+    <tableColumn id="9" name="SpecialCd" dataDxfId="11"/>
+    <tableColumn id="16" name="OnUseCard" dataDxfId="10"/>
+    <tableColumn id="25" name="Active" dataDxfId="9"/>
+    <tableColumn id="20" name="IsRandom" dataDxfId="8"/>
+    <tableColumn id="23" name="GetDescript" dataDxfId="7"/>
+    <tableColumn id="8" name="DescriptBuffId" dataDxfId="6"/>
+    <tableColumn id="17" name="Effect" dataDxfId="5"/>
+    <tableColumn id="10" name="EffectArea" dataDxfId="4"/>
+    <tableColumn id="6" name="Cover" dataDxfId="3"/>
+    <tableColumn id="18" name="Mark" dataDxfId="2"/>
+    <tableColumn id="19" name="Icon" dataDxfId="1"/>
+    <tableColumn id="7" name="Remark" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6795,7 +6873,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -7107,15 +7185,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD227"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="Q48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="I222" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="T49" sqref="T49"/>
+      <selection pane="bottomRight" activeCell="T227" sqref="T227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7131,9 +7209,9 @@
     <col min="15" max="15" width="18.625" customWidth="1"/>
     <col min="16" max="18" width="22.25" customWidth="1"/>
     <col min="19" max="19" width="7.125" customWidth="1"/>
-    <col min="20" max="20" width="16" customWidth="1"/>
+    <col min="20" max="20" width="17.875" customWidth="1"/>
     <col min="21" max="21" width="8.375" customWidth="1"/>
-    <col min="22" max="22" width="7.375" customWidth="1"/>
+    <col min="22" max="22" width="6.875" customWidth="1"/>
     <col min="23" max="23" width="22.75" customWidth="1"/>
     <col min="24" max="24" width="9.25" customWidth="1"/>
     <col min="25" max="25" width="8.75" customWidth="1"/>
@@ -8258,7 +8336,7 @@
       <c r="H19" s="59"/>
       <c r="I19" s="28"/>
       <c r="J19" s="29" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="K19" s="29"/>
       <c r="L19" s="82" t="s">
@@ -8362,7 +8440,7 @@
       <c r="H21" s="59"/>
       <c r="I21" s="26"/>
       <c r="J21" s="29" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
@@ -8416,7 +8494,7 @@
         <v>1049</v>
       </c>
       <c r="J22" s="90" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="K22" s="105"/>
       <c r="L22" s="99"/>
@@ -8622,7 +8700,7 @@
       <c r="H26" s="59"/>
       <c r="I26" s="28"/>
       <c r="J26" s="29" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="K26" s="29"/>
       <c r="L26" s="82"/>
@@ -9294,7 +9372,7 @@
       <c r="L39" s="82"/>
       <c r="M39" s="18"/>
       <c r="N39" s="17" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="O39" s="17"/>
       <c r="P39" s="17"/>
@@ -9573,7 +9651,7 @@
       <c r="O44" s="17"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="17" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="R44" s="20"/>
       <c r="S44" s="41"/>
@@ -9585,7 +9663,7 @@
         <v>230</v>
       </c>
       <c r="W44" s="16" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="X44" s="25"/>
       <c r="Y44" s="25" t="s">
@@ -9600,7 +9678,7 @@
         <v>448</v>
       </c>
       <c r="AD44" s="48" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="45" spans="1:30" ht="108" x14ac:dyDescent="0.15">
@@ -9688,7 +9766,7 @@
       <c r="P46" s="17"/>
       <c r="Q46" s="17"/>
       <c r="R46" s="20" t="s">
-        <v>1057</v>
+        <v>1172</v>
       </c>
       <c r="S46" s="41">
         <v>1</v>
@@ -9953,10 +10031,10 @@
       </c>
       <c r="X50" s="25"/>
       <c r="Y50" s="25" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="Z50" s="25" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="AA50" s="25"/>
       <c r="AB50" s="25">
@@ -10168,7 +10246,7 @@
       <c r="H54" s="60"/>
       <c r="I54" s="86"/>
       <c r="J54" s="47" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K54" s="85"/>
       <c r="L54" s="100"/>
@@ -10204,7 +10282,7 @@
         <v>710</v>
       </c>
       <c r="AD54" s="48" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="55" spans="1:30" ht="96" x14ac:dyDescent="0.15">
@@ -10230,7 +10308,7 @@
       <c r="H55" s="60"/>
       <c r="I55" s="86"/>
       <c r="J55" s="47" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="K55" s="85"/>
       <c r="L55" s="100"/>
@@ -10311,10 +10389,10 @@
       </c>
       <c r="X56" s="25"/>
       <c r="Y56" s="25" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="Z56" s="25" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="AA56" s="25"/>
       <c r="AB56" s="25">
@@ -14633,7 +14711,7 @@
       <c r="M138" s="18"/>
       <c r="N138" s="17"/>
       <c r="O138" s="17" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="P138" s="17"/>
       <c r="Q138" s="17"/>
@@ -14683,7 +14761,7 @@
       <c r="M139" s="18"/>
       <c r="N139" s="17"/>
       <c r="O139" s="17" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="P139" s="17"/>
       <c r="Q139" s="17"/>
@@ -14734,7 +14812,7 @@
       <c r="N140" s="17"/>
       <c r="O140" s="17"/>
       <c r="P140" s="17" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="Q140" s="17"/>
       <c r="R140" s="20"/>
@@ -14786,7 +14864,7 @@
       <c r="H141" s="60"/>
       <c r="I141" s="26"/>
       <c r="J141" s="47" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="K141" s="47"/>
       <c r="L141" s="99"/>
@@ -14848,7 +14926,7 @@
       <c r="P142" s="17"/>
       <c r="Q142" s="17"/>
       <c r="R142" s="20" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="S142" s="41">
         <v>1</v>
@@ -14900,7 +14978,7 @@
       <c r="P143" s="17"/>
       <c r="Q143" s="17"/>
       <c r="R143" s="20" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="S143" s="41">
         <v>1</v>
@@ -14954,7 +15032,7 @@
       <c r="R144" s="20"/>
       <c r="S144" s="41"/>
       <c r="T144" s="20" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="U144" s="46" t="s">
         <v>235</v>
@@ -15116,7 +15194,7 @@
       <c r="H147" s="60"/>
       <c r="I147" s="26"/>
       <c r="J147" s="47" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="K147" s="47"/>
       <c r="L147" s="99"/>
@@ -15528,7 +15606,7 @@
       <c r="H155" s="60"/>
       <c r="I155" s="26"/>
       <c r="J155" s="47" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="K155" s="47"/>
       <c r="L155" s="99"/>
@@ -15691,7 +15769,7 @@
       <c r="G158" s="43"/>
       <c r="H158" s="60"/>
       <c r="I158" s="28" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="J158" s="29"/>
       <c r="K158" s="29"/>
@@ -16022,7 +16100,7 @@
       <c r="H164" s="78"/>
       <c r="I164" s="96"/>
       <c r="J164" s="29" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="K164" s="95"/>
       <c r="L164" s="101"/>
@@ -16188,7 +16266,7 @@
       <c r="H167" s="60"/>
       <c r="I167" s="26"/>
       <c r="J167" s="82" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="K167" s="47"/>
       <c r="L167" s="99"/>
@@ -16244,7 +16322,7 @@
       <c r="H168" s="60"/>
       <c r="I168" s="26"/>
       <c r="J168" s="29" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="K168" s="29"/>
       <c r="L168" s="99"/>
@@ -16464,7 +16542,7 @@
       <c r="H172" s="60"/>
       <c r="I172" s="26"/>
       <c r="J172" s="82" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="K172" s="47"/>
       <c r="L172" s="99"/>
@@ -16514,7 +16592,7 @@
       <c r="H173" s="60"/>
       <c r="I173" s="26"/>
       <c r="J173" s="82" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="K173" s="47"/>
       <c r="L173" s="99"/>
@@ -16533,7 +16611,7 @@
         <v>362</v>
       </c>
       <c r="W173" s="16" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="X173" s="25"/>
       <c r="Y173" s="25"/>
@@ -16948,7 +17026,7 @@
       <c r="H181" s="60"/>
       <c r="I181" s="26"/>
       <c r="J181" s="29" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="K181" s="29"/>
       <c r="L181" s="99"/>
@@ -17222,7 +17300,7 @@
         <v>756</v>
       </c>
       <c r="AD185" s="48" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="186" spans="1:30" ht="48" x14ac:dyDescent="0.15">
@@ -17356,7 +17434,7 @@
       <c r="P188" s="17"/>
       <c r="Q188" s="17"/>
       <c r="R188" s="20" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="S188" s="41">
         <v>2</v>
@@ -17379,7 +17457,7 @@
         <v>40</v>
       </c>
       <c r="AC188" s="25" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="AD188" s="48" t="s">
         <v>1012</v>
@@ -17408,7 +17486,7 @@
       <c r="H189" s="60"/>
       <c r="I189" s="26"/>
       <c r="J189" s="90" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="K189" s="29"/>
       <c r="L189" s="99"/>
@@ -17440,7 +17518,7 @@
         <v>766</v>
       </c>
       <c r="AD189" s="48" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="190" spans="1:30" ht="84" x14ac:dyDescent="0.15">
@@ -17718,7 +17796,7 @@
         <v>805</v>
       </c>
       <c r="AD194" s="48" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="195" spans="1:30" ht="36" x14ac:dyDescent="0.15">
@@ -17757,7 +17835,7 @@
         <v>230</v>
       </c>
       <c r="W195" s="10" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="X195" s="10"/>
       <c r="Y195" s="61"/>
@@ -17908,7 +17986,7 @@
       <c r="H198" s="60"/>
       <c r="I198" s="26"/>
       <c r="J198" s="90" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="K198" s="29"/>
       <c r="L198" s="99"/>
@@ -18209,7 +18287,7 @@
       </c>
       <c r="B204" s="55"/>
       <c r="C204" s="55" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="D204" s="25" t="s">
         <v>309</v>
@@ -18227,7 +18305,7 @@
       <c r="O204" s="17"/>
       <c r="P204" s="17"/>
       <c r="Q204" s="17" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="R204" s="20"/>
       <c r="S204" s="41"/>
@@ -18239,7 +18317,7 @@
         <v>230</v>
       </c>
       <c r="W204" s="16" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="X204" s="25"/>
       <c r="Y204" s="25"/>
@@ -18249,10 +18327,10 @@
         <v>60</v>
       </c>
       <c r="AC204" s="25" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="AD204" s="48" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="205" spans="1:30" ht="24" x14ac:dyDescent="0.15">
@@ -18261,7 +18339,7 @@
       </c>
       <c r="B205" s="55"/>
       <c r="C205" s="55" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D205" s="25" t="s">
         <v>309</v>
@@ -18278,7 +18356,7 @@
       <c r="N205" s="30"/>
       <c r="O205" s="17"/>
       <c r="P205" s="17" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="Q205" s="17"/>
       <c r="R205" s="20"/>
@@ -18291,7 +18369,7 @@
         <v>230</v>
       </c>
       <c r="W205" s="16" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="X205" s="25"/>
       <c r="Y205" s="25"/>
@@ -18301,10 +18379,10 @@
         <v>20</v>
       </c>
       <c r="AC205" s="25" t="s">
+        <v>1162</v>
+      </c>
+      <c r="AD205" s="48" t="s">
         <v>1163</v>
-      </c>
-      <c r="AD205" s="48" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="206" spans="1:30" ht="84" x14ac:dyDescent="0.15">
@@ -18313,7 +18391,7 @@
       </c>
       <c r="B206" s="83"/>
       <c r="C206" s="55" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="D206" s="25" t="s">
         <v>309</v>
@@ -18324,7 +18402,7 @@
       <c r="H206" s="78"/>
       <c r="I206" s="96"/>
       <c r="J206" s="29" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="K206" s="95"/>
       <c r="L206" s="101"/>
@@ -18343,7 +18421,7 @@
         <v>230</v>
       </c>
       <c r="W206" s="10" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="X206" s="77"/>
       <c r="Y206" s="77"/>
@@ -18353,7 +18431,7 @@
         <v>15</v>
       </c>
       <c r="AC206" s="25" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="AD206" s="48" t="s">
         <v>1017</v>
@@ -19309,7 +19387,7 @@
       </c>
       <c r="AD224" s="48"/>
     </row>
-    <row r="225" spans="1:30" ht="156" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:30" ht="132" x14ac:dyDescent="0.15">
       <c r="A225" s="91">
         <v>55990107</v>
       </c>
@@ -19342,7 +19420,7 @@
       <c r="R225" s="20"/>
       <c r="S225" s="41"/>
       <c r="T225" s="20" t="s">
-        <v>1125</v>
+        <v>1173</v>
       </c>
       <c r="U225" s="35" t="s">
         <v>235</v>
@@ -19354,7 +19432,9 @@
         <v>846</v>
       </c>
       <c r="X225" s="10"/>
-      <c r="Y225" s="1"/>
+      <c r="Y225" s="25" t="s">
+        <v>523</v>
+      </c>
       <c r="Z225" s="1"/>
       <c r="AA225" s="1"/>
       <c r="AB225" s="1">
@@ -19399,8 +19479,8 @@
       <c r="U226" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="V226" s="9" t="s">
-        <v>230</v>
+      <c r="V226" s="44" t="s">
+        <v>232</v>
       </c>
       <c r="W226" s="10" t="s">
         <v>847</v>
@@ -19454,7 +19534,7 @@
         <v>235</v>
       </c>
       <c r="V227" s="44" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="W227" s="16" t="s">
         <v>850</v>
@@ -19472,6 +19552,64 @@
         <v>215</v>
       </c>
       <c r="AD227" s="48"/>
+    </row>
+    <row r="228" spans="1:30" ht="108" x14ac:dyDescent="0.15">
+      <c r="A228" s="91">
+        <v>55990110</v>
+      </c>
+      <c r="B228" s="91"/>
+      <c r="C228" s="91" t="s">
+        <v>591</v>
+      </c>
+      <c r="D228" s="25" t="s">
+        <v>637</v>
+      </c>
+      <c r="E228" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="F228" s="25">
+        <v>40</v>
+      </c>
+      <c r="G228" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="H228" s="60"/>
+      <c r="I228" s="112"/>
+      <c r="J228" s="82"/>
+      <c r="K228" s="47"/>
+      <c r="L228" s="99"/>
+      <c r="M228" s="27"/>
+      <c r="N228" s="30"/>
+      <c r="O228" s="17"/>
+      <c r="P228" s="17"/>
+      <c r="Q228" s="17"/>
+      <c r="R228" s="20"/>
+      <c r="S228" s="41"/>
+      <c r="T228" s="20" t="s">
+        <v>1175</v>
+      </c>
+      <c r="U228" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="V228" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="W228" s="16" t="s">
+        <v>1174</v>
+      </c>
+      <c r="X228" s="25"/>
+      <c r="Y228" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="Z228" s="25"/>
+      <c r="AA228" s="25"/>
+      <c r="AB228" s="25">
+        <v>25</v>
+      </c>
+      <c r="AC228" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD228" s="48"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -19485,7 +19623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
fix a anti magic passive skill bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{59EA7E45-AF3D-4386-BBFC-5FD97747623E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C8A46FD1-5427-460A-B88A-A9E990D0A9B4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="1194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="1195">
   <si>
     <t>复原</t>
   </si>
@@ -4469,6 +4469,10 @@
   </si>
   <si>
     <t>if(type==3){s.Action.SetToPosition("rand",1);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7195,11 +7199,11 @@
   <dimension ref="A1:AD233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D203" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="D210" sqref="D210"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8029,7 +8033,7 @@
       <c r="S13" s="41"/>
       <c r="T13" s="20"/>
       <c r="U13" s="1" t="s">
-        <v>237</v>
+        <v>1194</v>
       </c>
       <c r="V13" s="9" t="s">
         <v>230</v>
@@ -8141,7 +8145,7 @@
       <c r="S15" s="41"/>
       <c r="T15" s="20"/>
       <c r="U15" s="1" t="s">
-        <v>237</v>
+        <v>1194</v>
       </c>
       <c r="V15" s="9" t="s">
         <v>230</v>
@@ -8247,7 +8251,7 @@
       <c r="S17" s="41"/>
       <c r="T17" s="20"/>
       <c r="U17" s="1" t="s">
-        <v>237</v>
+        <v>1194</v>
       </c>
       <c r="V17" s="9" t="s">
         <v>230</v>
@@ -17319,7 +17323,7 @@
       <c r="S186" s="41"/>
       <c r="T186" s="20"/>
       <c r="U186" s="1" t="s">
-        <v>237</v>
+        <v>1194</v>
       </c>
       <c r="V186" s="9" t="s">
         <v>230</v>
@@ -19301,7 +19305,7 @@
       <c r="S223" s="41"/>
       <c r="T223" s="20"/>
       <c r="U223" s="46" t="s">
-        <v>237</v>
+        <v>1194</v>
       </c>
       <c r="V223" s="44" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
add the dream cardset
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="1198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="1201">
   <si>
     <t>复原</t>
   </si>
@@ -4472,10 +4472,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>部件</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>s.Owner.Action.AddCard(s,d.CardId, d.Level);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4484,7 +4480,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>每回合获得一张随机部件卡</t>
+    <t>每回合获得一张随机【圣言】卡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣言</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>入梦</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合获得一张随机【梦境】卡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.Owner.Action.AddGroupCard(s,59000002,s.Level);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -6915,10 +6927,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:AD234" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
-  <autoFilter ref="A3:AD234"/>
-  <sortState ref="A4:AD232">
-    <sortCondition ref="A3:A232"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表3_25" displayName="表3_25" ref="A3:AD235" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
+  <autoFilter ref="A3:AD235"/>
+  <sortState ref="A4:AD233">
+    <sortCondition ref="A3:A233"/>
   </sortState>
   <tableColumns count="30">
     <tableColumn id="1" name="Id" dataDxfId="29"/>
@@ -7277,14 +7289,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD234"/>
+  <dimension ref="A1:AD235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="O203" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="O205" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="D211" sqref="D211"/>
+      <selection pane="bottomRight" activeCell="AB211" sqref="AB211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -16689,7 +16701,7 @@
       <c r="N173" s="30"/>
       <c r="O173" s="17"/>
       <c r="P173" s="17" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="Q173" s="17"/>
       <c r="R173" s="20"/>
@@ -18740,7 +18752,7 @@
       </c>
       <c r="B211" s="83"/>
       <c r="C211" s="55" t="s">
-        <v>1194</v>
+        <v>1197</v>
       </c>
       <c r="D211" s="25" t="s">
         <v>309</v>
@@ -18759,7 +18771,7 @@
       <c r="P211" s="79"/>
       <c r="Q211" s="79"/>
       <c r="R211" s="20" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="S211" s="81">
         <v>1</v>
@@ -18772,79 +18784,79 @@
         <v>230</v>
       </c>
       <c r="W211" s="10" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="X211" s="77"/>
       <c r="Y211" s="77"/>
       <c r="Z211" s="77"/>
       <c r="AA211" s="77"/>
       <c r="AB211" s="77">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AC211" s="113" t="s">
         <v>1189</v>
       </c>
       <c r="AD211" s="48"/>
     </row>
-    <row r="212" spans="1:30" ht="36" x14ac:dyDescent="0.15">
-      <c r="A212" s="91">
-        <v>55990001</v>
-      </c>
-      <c r="B212" s="91"/>
-      <c r="C212" s="91" t="s">
-        <v>20</v>
+    <row r="212" spans="1:30" ht="24" x14ac:dyDescent="0.15">
+      <c r="A212" s="55">
+        <v>55900065</v>
+      </c>
+      <c r="B212" s="83"/>
+      <c r="C212" s="55" t="s">
+        <v>1198</v>
       </c>
       <c r="D212" s="25" t="s">
-        <v>639</v>
+        <v>309</v>
       </c>
       <c r="E212" s="25"/>
       <c r="F212" s="25"/>
-      <c r="G212" s="25"/>
-      <c r="H212" s="60"/>
-      <c r="I212" s="26" t="s">
-        <v>855</v>
-      </c>
-      <c r="J212" s="82"/>
-      <c r="K212" s="47"/>
-      <c r="L212" s="99"/>
-      <c r="M212" s="27"/>
-      <c r="N212" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="O212" s="17"/>
-      <c r="P212" s="17"/>
-      <c r="Q212" s="17"/>
-      <c r="R212" s="20"/>
-      <c r="S212" s="41"/>
+      <c r="G212" s="44"/>
+      <c r="H212" s="78"/>
+      <c r="I212" s="96"/>
+      <c r="J212" s="29"/>
+      <c r="K212" s="95"/>
+      <c r="L212" s="101"/>
+      <c r="M212" s="97"/>
+      <c r="N212" s="79"/>
+      <c r="O212" s="79"/>
+      <c r="P212" s="79"/>
+      <c r="Q212" s="79"/>
+      <c r="R212" s="20" t="s">
+        <v>1200</v>
+      </c>
+      <c r="S212" s="81">
+        <v>1</v>
+      </c>
       <c r="T212" s="20"/>
-      <c r="U212" s="46" t="s">
+      <c r="U212" s="77" t="s">
         <v>235</v>
       </c>
-      <c r="V212" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="W212" s="16" t="s">
-        <v>356</v>
-      </c>
-      <c r="X212" s="25"/>
-      <c r="Y212" s="25"/>
-      <c r="Z212" s="25"/>
-      <c r="AA212" s="25"/>
-      <c r="AB212" s="25">
-        <v>10</v>
-      </c>
-      <c r="AC212" s="25" t="s">
-        <v>21</v>
+      <c r="V212" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="W212" s="10" t="s">
+        <v>1199</v>
+      </c>
+      <c r="X212" s="77"/>
+      <c r="Y212" s="77"/>
+      <c r="Z212" s="77"/>
+      <c r="AA212" s="77"/>
+      <c r="AB212" s="77">
+        <v>20</v>
+      </c>
+      <c r="AC212" s="113" t="s">
+        <v>1189</v>
       </c>
       <c r="AD212" s="48"/>
     </row>
     <row r="213" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A213" s="91">
-        <v>55990002</v>
+        <v>55990001</v>
       </c>
       <c r="B213" s="91"/>
       <c r="C213" s="91" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D213" s="25" t="s">
         <v>639</v>
@@ -18854,10 +18866,10 @@
       <c r="G213" s="25"/>
       <c r="H213" s="60"/>
       <c r="I213" s="26" t="s">
-        <v>856</v>
-      </c>
-      <c r="J213" s="90"/>
-      <c r="K213" s="29"/>
+        <v>855</v>
+      </c>
+      <c r="J213" s="82"/>
+      <c r="K213" s="47"/>
       <c r="L213" s="99"/>
       <c r="M213" s="27"/>
       <c r="N213" s="30" t="s">
@@ -18875,8 +18887,8 @@
       <c r="V213" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="W213" s="49" t="s">
-        <v>357</v>
+      <c r="W213" s="16" t="s">
+        <v>356</v>
       </c>
       <c r="X213" s="25"/>
       <c r="Y213" s="25"/>
@@ -18886,17 +18898,17 @@
         <v>10</v>
       </c>
       <c r="AC213" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AD213" s="48"/>
     </row>
     <row r="214" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A214" s="91">
-        <v>55990003</v>
+        <v>55990002</v>
       </c>
       <c r="B214" s="91"/>
       <c r="C214" s="91" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D214" s="25" t="s">
         <v>639</v>
@@ -18906,7 +18918,7 @@
       <c r="G214" s="25"/>
       <c r="H214" s="60"/>
       <c r="I214" s="26" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="J214" s="90"/>
       <c r="K214" s="29"/>
@@ -18928,7 +18940,7 @@
         <v>232</v>
       </c>
       <c r="W214" s="49" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="X214" s="25"/>
       <c r="Y214" s="25"/>
@@ -18938,17 +18950,17 @@
         <v>10</v>
       </c>
       <c r="AC214" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AD214" s="48"/>
     </row>
     <row r="215" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A215" s="91">
-        <v>55990004</v>
+        <v>55990003</v>
       </c>
       <c r="B215" s="91"/>
       <c r="C215" s="91" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D215" s="25" t="s">
         <v>639</v>
@@ -18958,7 +18970,7 @@
       <c r="G215" s="25"/>
       <c r="H215" s="60"/>
       <c r="I215" s="26" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="J215" s="90"/>
       <c r="K215" s="29"/>
@@ -18980,7 +18992,7 @@
         <v>232</v>
       </c>
       <c r="W215" s="49" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="X215" s="25"/>
       <c r="Y215" s="25"/>
@@ -18990,17 +19002,17 @@
         <v>10</v>
       </c>
       <c r="AC215" s="25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AD215" s="48"/>
     </row>
     <row r="216" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A216" s="91">
-        <v>55990005</v>
+        <v>55990004</v>
       </c>
       <c r="B216" s="91"/>
       <c r="C216" s="91" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D216" s="25" t="s">
         <v>639</v>
@@ -19010,7 +19022,7 @@
       <c r="G216" s="25"/>
       <c r="H216" s="60"/>
       <c r="I216" s="26" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="J216" s="90"/>
       <c r="K216" s="29"/>
@@ -19032,7 +19044,7 @@
         <v>232</v>
       </c>
       <c r="W216" s="49" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="X216" s="25"/>
       <c r="Y216" s="25"/>
@@ -19042,17 +19054,17 @@
         <v>10</v>
       </c>
       <c r="AC216" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AD216" s="48"/>
     </row>
     <row r="217" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A217" s="91">
-        <v>55990006</v>
+        <v>55990005</v>
       </c>
       <c r="B217" s="91"/>
       <c r="C217" s="91" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D217" s="25" t="s">
         <v>639</v>
@@ -19062,7 +19074,7 @@
       <c r="G217" s="25"/>
       <c r="H217" s="60"/>
       <c r="I217" s="26" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="J217" s="90"/>
       <c r="K217" s="29"/>
@@ -19084,7 +19096,7 @@
         <v>232</v>
       </c>
       <c r="W217" s="49" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="X217" s="25"/>
       <c r="Y217" s="25"/>
@@ -19094,17 +19106,17 @@
         <v>10</v>
       </c>
       <c r="AC217" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AD217" s="48"/>
     </row>
     <row r="218" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A218" s="91">
-        <v>55990011</v>
+        <v>55990006</v>
       </c>
       <c r="B218" s="91"/>
       <c r="C218" s="91" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D218" s="25" t="s">
         <v>639</v>
@@ -19114,14 +19126,14 @@
       <c r="G218" s="25"/>
       <c r="H218" s="60"/>
       <c r="I218" s="26" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="J218" s="90"/>
       <c r="K218" s="29"/>
       <c r="L218" s="99"/>
       <c r="M218" s="27"/>
       <c r="N218" s="30" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="O218" s="17"/>
       <c r="P218" s="17"/>
@@ -19130,13 +19142,13 @@
       <c r="S218" s="41"/>
       <c r="T218" s="20"/>
       <c r="U218" s="46" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="V218" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="W218" s="16" t="s">
-        <v>260</v>
+      <c r="W218" s="49" t="s">
+        <v>368</v>
       </c>
       <c r="X218" s="25"/>
       <c r="Y218" s="25"/>
@@ -19146,17 +19158,17 @@
         <v>10</v>
       </c>
       <c r="AC218" s="25" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="AD218" s="48"/>
     </row>
     <row r="219" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A219" s="91">
-        <v>55990012</v>
+        <v>55990011</v>
       </c>
       <c r="B219" s="91"/>
       <c r="C219" s="91" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D219" s="25" t="s">
         <v>639</v>
@@ -19166,7 +19178,7 @@
       <c r="G219" s="25"/>
       <c r="H219" s="60"/>
       <c r="I219" s="26" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="J219" s="90"/>
       <c r="K219" s="29"/>
@@ -19188,7 +19200,7 @@
         <v>232</v>
       </c>
       <c r="W219" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="X219" s="25"/>
       <c r="Y219" s="25"/>
@@ -19198,17 +19210,17 @@
         <v>10</v>
       </c>
       <c r="AC219" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AD219" s="48"/>
     </row>
     <row r="220" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A220" s="91">
-        <v>55990013</v>
+        <v>55990012</v>
       </c>
       <c r="B220" s="91"/>
       <c r="C220" s="91" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D220" s="25" t="s">
         <v>639</v>
@@ -19218,7 +19230,7 @@
       <c r="G220" s="25"/>
       <c r="H220" s="60"/>
       <c r="I220" s="26" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="J220" s="90"/>
       <c r="K220" s="29"/>
@@ -19240,7 +19252,7 @@
         <v>232</v>
       </c>
       <c r="W220" s="16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="X220" s="25"/>
       <c r="Y220" s="25"/>
@@ -19250,17 +19262,17 @@
         <v>10</v>
       </c>
       <c r="AC220" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD220" s="48"/>
     </row>
     <row r="221" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A221" s="91">
-        <v>55990014</v>
+        <v>55990013</v>
       </c>
       <c r="B221" s="91"/>
       <c r="C221" s="91" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D221" s="25" t="s">
         <v>639</v>
@@ -19270,7 +19282,7 @@
       <c r="G221" s="25"/>
       <c r="H221" s="60"/>
       <c r="I221" s="26" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="J221" s="90"/>
       <c r="K221" s="29"/>
@@ -19292,7 +19304,7 @@
         <v>232</v>
       </c>
       <c r="W221" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="X221" s="25"/>
       <c r="Y221" s="25"/>
@@ -19302,17 +19314,17 @@
         <v>10</v>
       </c>
       <c r="AC221" s="25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AD221" s="48"/>
     </row>
     <row r="222" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A222" s="91">
-        <v>55990015</v>
+        <v>55990014</v>
       </c>
       <c r="B222" s="91"/>
       <c r="C222" s="91" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D222" s="25" t="s">
         <v>639</v>
@@ -19322,7 +19334,7 @@
       <c r="G222" s="25"/>
       <c r="H222" s="60"/>
       <c r="I222" s="26" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J222" s="90"/>
       <c r="K222" s="29"/>
@@ -19344,7 +19356,7 @@
         <v>232</v>
       </c>
       <c r="W222" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X222" s="25"/>
       <c r="Y222" s="25"/>
@@ -19354,17 +19366,17 @@
         <v>10</v>
       </c>
       <c r="AC222" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AD222" s="48"/>
     </row>
     <row r="223" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A223" s="91">
-        <v>55990016</v>
+        <v>55990015</v>
       </c>
       <c r="B223" s="91"/>
       <c r="C223" s="91" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D223" s="25" t="s">
         <v>639</v>
@@ -19374,7 +19386,7 @@
       <c r="G223" s="25"/>
       <c r="H223" s="60"/>
       <c r="I223" s="26" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="J223" s="90"/>
       <c r="K223" s="29"/>
@@ -19396,7 +19408,7 @@
         <v>232</v>
       </c>
       <c r="W223" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X223" s="25"/>
       <c r="Y223" s="25"/>
@@ -19406,33 +19418,35 @@
         <v>10</v>
       </c>
       <c r="AC223" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AD223" s="48"/>
     </row>
-    <row r="224" spans="1:30" ht="24" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:30" ht="36" x14ac:dyDescent="0.15">
       <c r="A224" s="91">
-        <v>55990101</v>
+        <v>55990016</v>
       </c>
       <c r="B224" s="91"/>
       <c r="C224" s="91" t="s">
-        <v>640</v>
+        <v>60</v>
       </c>
       <c r="D224" s="25" t="s">
         <v>639</v>
       </c>
       <c r="E224" s="25"/>
       <c r="F224" s="25"/>
-      <c r="G224" s="44"/>
+      <c r="G224" s="25"/>
       <c r="H224" s="60"/>
-      <c r="I224" s="26"/>
-      <c r="J224" s="82" t="s">
-        <v>641</v>
-      </c>
-      <c r="K224" s="47"/>
+      <c r="I224" s="26" t="s">
+        <v>866</v>
+      </c>
+      <c r="J224" s="90"/>
+      <c r="K224" s="29"/>
       <c r="L224" s="99"/>
       <c r="M224" s="27"/>
-      <c r="N224" s="30"/>
+      <c r="N224" s="30" t="s">
+        <v>259</v>
+      </c>
       <c r="O224" s="17"/>
       <c r="P224" s="17"/>
       <c r="Q224" s="17"/>
@@ -19440,51 +19454,49 @@
       <c r="S224" s="41"/>
       <c r="T224" s="20"/>
       <c r="U224" s="46" t="s">
-        <v>1193</v>
+        <v>237</v>
       </c>
       <c r="V224" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="W224" s="49" t="s">
-        <v>642</v>
+      <c r="W224" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="X224" s="25"/>
       <c r="Y224" s="25"/>
       <c r="Z224" s="25"/>
       <c r="AA224" s="25"/>
       <c r="AB224" s="25">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AC224" s="25" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="AD224" s="48"/>
     </row>
-    <row r="225" spans="1:30" ht="27" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:30" ht="24" x14ac:dyDescent="0.15">
       <c r="A225" s="91">
-        <v>55990102</v>
+        <v>55990101</v>
       </c>
       <c r="B225" s="91"/>
       <c r="C225" s="91" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D225" s="25" t="s">
         <v>639</v>
       </c>
       <c r="E225" s="25"/>
       <c r="F225" s="25"/>
-      <c r="G225" s="25"/>
+      <c r="G225" s="44"/>
       <c r="H225" s="60"/>
-      <c r="I225" s="26" t="s">
-        <v>643</v>
-      </c>
-      <c r="J225" s="82"/>
+      <c r="I225" s="26"/>
+      <c r="J225" s="82" t="s">
+        <v>641</v>
+      </c>
       <c r="K225" s="47"/>
       <c r="L225" s="99"/>
       <c r="M225" s="27"/>
-      <c r="N225" s="30" t="s">
-        <v>646</v>
-      </c>
+      <c r="N225" s="30"/>
       <c r="O225" s="17"/>
       <c r="P225" s="17"/>
       <c r="Q225" s="17"/>
@@ -19492,58 +19504,52 @@
       <c r="S225" s="41"/>
       <c r="T225" s="20"/>
       <c r="U225" s="46" t="s">
-        <v>235</v>
+        <v>1193</v>
       </c>
       <c r="V225" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="W225" s="16" t="s">
-        <v>645</v>
+      <c r="W225" s="49" t="s">
+        <v>642</v>
       </c>
       <c r="X225" s="25"/>
       <c r="Y225" s="25"/>
       <c r="Z225" s="25"/>
       <c r="AA225" s="25"/>
       <c r="AB225" s="25">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AC225" s="25" t="s">
-        <v>649</v>
+        <v>103</v>
       </c>
       <c r="AD225" s="48"/>
     </row>
-    <row r="226" spans="1:30" ht="96" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:30" ht="27" x14ac:dyDescent="0.15">
       <c r="A226" s="91">
-        <v>55990103</v>
+        <v>55990102</v>
       </c>
       <c r="B226" s="91"/>
       <c r="C226" s="91" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="D226" s="25" t="s">
-        <v>637</v>
-      </c>
-      <c r="E226" s="25" t="s">
-        <v>397</v>
-      </c>
-      <c r="F226" s="25">
-        <v>10</v>
-      </c>
-      <c r="G226" s="44" t="s">
-        <v>405</v>
-      </c>
+        <v>639</v>
+      </c>
+      <c r="E226" s="25"/>
+      <c r="F226" s="25"/>
+      <c r="G226" s="25"/>
       <c r="H226" s="60"/>
       <c r="I226" s="26" t="s">
-        <v>540</v>
+        <v>643</v>
       </c>
       <c r="J226" s="82"/>
       <c r="K226" s="47"/>
       <c r="L226" s="99"/>
       <c r="M226" s="27"/>
-      <c r="N226" s="30"/>
-      <c r="O226" s="17" t="s">
-        <v>1053</v>
-      </c>
+      <c r="N226" s="30" t="s">
+        <v>646</v>
+      </c>
+      <c r="O226" s="17"/>
       <c r="P226" s="17"/>
       <c r="Q226" s="17"/>
       <c r="R226" s="20"/>
@@ -19556,31 +19562,27 @@
         <v>232</v>
       </c>
       <c r="W226" s="16" t="s">
-        <v>656</v>
+        <v>645</v>
       </c>
       <c r="X226" s="25"/>
-      <c r="Y226" s="25" t="s">
-        <v>663</v>
-      </c>
-      <c r="Z226" s="25" t="s">
-        <v>663</v>
-      </c>
+      <c r="Y226" s="25"/>
+      <c r="Z226" s="25"/>
       <c r="AA226" s="25"/>
       <c r="AB226" s="25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AC226" s="25" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="AD226" s="48"/>
     </row>
     <row r="227" spans="1:30" ht="96" x14ac:dyDescent="0.15">
       <c r="A227" s="91">
-        <v>55990104</v>
+        <v>55990103</v>
       </c>
       <c r="B227" s="91"/>
       <c r="C227" s="91" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="D227" s="25" t="s">
         <v>637</v>
@@ -19589,14 +19591,14 @@
         <v>397</v>
       </c>
       <c r="F227" s="25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G227" s="44" t="s">
         <v>405</v>
       </c>
       <c r="H227" s="60"/>
       <c r="I227" s="26" t="s">
-        <v>659</v>
+        <v>540</v>
       </c>
       <c r="J227" s="82"/>
       <c r="K227" s="47"/>
@@ -19618,7 +19620,7 @@
         <v>232</v>
       </c>
       <c r="W227" s="16" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="X227" s="25"/>
       <c r="Y227" s="25" t="s">
@@ -19629,70 +19631,82 @@
       </c>
       <c r="AA227" s="25"/>
       <c r="AB227" s="25">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="AC227" s="25" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AD227" s="48"/>
     </row>
-    <row r="228" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:30" ht="96" x14ac:dyDescent="0.15">
       <c r="A228" s="91">
-        <v>55990105</v>
+        <v>55990104</v>
       </c>
       <c r="B228" s="91"/>
       <c r="C228" s="91" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
       <c r="D228" s="25" t="s">
         <v>637</v>
       </c>
-      <c r="E228" s="1"/>
-      <c r="F228" s="1"/>
-      <c r="G228" s="43"/>
+      <c r="E228" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="F228" s="25">
+        <v>20</v>
+      </c>
+      <c r="G228" s="44" t="s">
+        <v>405</v>
+      </c>
       <c r="H228" s="60"/>
-      <c r="I228" s="26"/>
+      <c r="I228" s="26" t="s">
+        <v>659</v>
+      </c>
       <c r="J228" s="82"/>
       <c r="K228" s="47"/>
       <c r="L228" s="99"/>
       <c r="M228" s="27"/>
       <c r="N228" s="30"/>
       <c r="O228" s="17" t="s">
-        <v>893</v>
+        <v>1053</v>
       </c>
       <c r="P228" s="17"/>
       <c r="Q228" s="17"/>
       <c r="R228" s="20"/>
       <c r="S228" s="41"/>
       <c r="T228" s="20"/>
-      <c r="U228" s="35" t="s">
+      <c r="U228" s="46" t="s">
         <v>235</v>
       </c>
       <c r="V228" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="W228" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="X228" s="10"/>
-      <c r="Y228" s="1"/>
-      <c r="Z228" s="1"/>
-      <c r="AA228" s="1"/>
-      <c r="AB228" s="1">
-        <v>150</v>
-      </c>
-      <c r="AC228" s="1" t="s">
-        <v>653</v>
+      <c r="W228" s="16" t="s">
+        <v>658</v>
+      </c>
+      <c r="X228" s="25"/>
+      <c r="Y228" s="25" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z228" s="25" t="s">
+        <v>663</v>
+      </c>
+      <c r="AA228" s="25"/>
+      <c r="AB228" s="25">
+        <v>50</v>
+      </c>
+      <c r="AC228" s="25" t="s">
+        <v>657</v>
       </c>
       <c r="AD228" s="48"/>
     </row>
-    <row r="229" spans="1:30" ht="24" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A229" s="91">
-        <v>55990106</v>
+        <v>55990105</v>
       </c>
       <c r="B229" s="91"/>
       <c r="C229" s="91" t="s">
-        <v>832</v>
+        <v>651</v>
       </c>
       <c r="D229" s="25" t="s">
         <v>637</v>
@@ -19708,7 +19722,7 @@
       <c r="M229" s="27"/>
       <c r="N229" s="30"/>
       <c r="O229" s="17" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="P229" s="17"/>
       <c r="Q229" s="17"/>
@@ -19722,40 +19736,34 @@
         <v>232</v>
       </c>
       <c r="W229" s="10" t="s">
-        <v>833</v>
+        <v>652</v>
       </c>
       <c r="X229" s="10"/>
       <c r="Y229" s="1"/>
       <c r="Z229" s="1"/>
       <c r="AA229" s="1"/>
       <c r="AB229" s="1">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="AC229" s="1" t="s">
-        <v>831</v>
+        <v>653</v>
       </c>
       <c r="AD229" s="48"/>
     </row>
-    <row r="230" spans="1:30" ht="132" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:30" ht="24" x14ac:dyDescent="0.15">
       <c r="A230" s="91">
-        <v>55990107</v>
+        <v>55990106</v>
       </c>
       <c r="B230" s="91"/>
       <c r="C230" s="91" t="s">
-        <v>845</v>
+        <v>832</v>
       </c>
       <c r="D230" s="25" t="s">
         <v>637</v>
       </c>
-      <c r="E230" s="25" t="s">
-        <v>395</v>
-      </c>
-      <c r="F230" s="25">
-        <v>40</v>
-      </c>
-      <c r="G230" s="44" t="s">
-        <v>404</v>
-      </c>
+      <c r="E230" s="1"/>
+      <c r="F230" s="1"/>
+      <c r="G230" s="43"/>
       <c r="H230" s="60"/>
       <c r="I230" s="26"/>
       <c r="J230" s="82"/>
@@ -19763,14 +19771,14 @@
       <c r="L230" s="99"/>
       <c r="M230" s="27"/>
       <c r="N230" s="30"/>
-      <c r="O230" s="17"/>
+      <c r="O230" s="17" t="s">
+        <v>902</v>
+      </c>
       <c r="P230" s="17"/>
       <c r="Q230" s="17"/>
       <c r="R230" s="20"/>
       <c r="S230" s="41"/>
-      <c r="T230" s="20" t="s">
-        <v>1170</v>
-      </c>
+      <c r="T230" s="20"/>
       <c r="U230" s="35" t="s">
         <v>235</v>
       </c>
@@ -19778,105 +19786,107 @@
         <v>232</v>
       </c>
       <c r="W230" s="10" t="s">
-        <v>846</v>
+        <v>833</v>
       </c>
       <c r="X230" s="10"/>
-      <c r="Y230" s="25" t="s">
-        <v>523</v>
-      </c>
+      <c r="Y230" s="1"/>
       <c r="Z230" s="1"/>
       <c r="AA230" s="1"/>
       <c r="AB230" s="1">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="AC230" s="1" t="s">
         <v>831</v>
       </c>
       <c r="AD230" s="48"/>
     </row>
-    <row r="231" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:30" ht="132" x14ac:dyDescent="0.15">
       <c r="A231" s="91">
-        <v>55990108</v>
+        <v>55990107</v>
       </c>
       <c r="B231" s="91"/>
       <c r="C231" s="91" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="D231" s="25" t="s">
         <v>637</v>
       </c>
-      <c r="E231" s="1"/>
-      <c r="F231" s="1"/>
-      <c r="G231" s="43"/>
-      <c r="H231" s="59"/>
-      <c r="I231" s="28"/>
-      <c r="J231" s="29"/>
-      <c r="K231" s="29"/>
-      <c r="L231" s="82"/>
-      <c r="M231" s="18"/>
-      <c r="N231" s="17"/>
+      <c r="E231" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="F231" s="25">
+        <v>40</v>
+      </c>
+      <c r="G231" s="44" t="s">
+        <v>404</v>
+      </c>
+      <c r="H231" s="60"/>
+      <c r="I231" s="26"/>
+      <c r="J231" s="82"/>
+      <c r="K231" s="47"/>
+      <c r="L231" s="99"/>
+      <c r="M231" s="27"/>
+      <c r="N231" s="30"/>
       <c r="O231" s="17"/>
       <c r="P231" s="17"/>
       <c r="Q231" s="17"/>
-      <c r="R231" s="20" t="s">
-        <v>848</v>
-      </c>
-      <c r="S231" s="41">
-        <v>1</v>
-      </c>
-      <c r="T231" s="20"/>
-      <c r="U231" s="46" t="s">
+      <c r="R231" s="20"/>
+      <c r="S231" s="41"/>
+      <c r="T231" s="20" t="s">
+        <v>1170</v>
+      </c>
+      <c r="U231" s="35" t="s">
         <v>235</v>
       </c>
       <c r="V231" s="44" t="s">
         <v>232</v>
       </c>
       <c r="W231" s="10" t="s">
-        <v>847</v>
-      </c>
-      <c r="X231" s="1"/>
-      <c r="Y231" s="1" t="s">
-        <v>843</v>
+        <v>846</v>
+      </c>
+      <c r="X231" s="10"/>
+      <c r="Y231" s="25" t="s">
+        <v>523</v>
       </c>
       <c r="Z231" s="1"/>
       <c r="AA231" s="1"/>
       <c r="AB231" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="AC231" s="1" t="s">
-        <v>215</v>
+        <v>831</v>
       </c>
       <c r="AD231" s="48"/>
     </row>
-    <row r="232" spans="1:30" ht="27" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A232" s="91">
-        <v>55990109</v>
+        <v>55990108</v>
       </c>
       <c r="B232" s="91"/>
       <c r="C232" s="91" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D232" s="25" t="s">
         <v>637</v>
       </c>
-      <c r="E232" s="25"/>
-      <c r="F232" s="25"/>
-      <c r="G232" s="44"/>
-      <c r="H232" s="60"/>
-      <c r="I232" s="26"/>
-      <c r="J232" s="82"/>
-      <c r="K232" s="47"/>
-      <c r="L232" s="99"/>
-      <c r="M232" s="27"/>
-      <c r="N232" s="30"/>
+      <c r="E232" s="1"/>
+      <c r="F232" s="1"/>
+      <c r="G232" s="43"/>
+      <c r="H232" s="59"/>
+      <c r="I232" s="28"/>
+      <c r="J232" s="29"/>
+      <c r="K232" s="29"/>
+      <c r="L232" s="82"/>
+      <c r="M232" s="18"/>
+      <c r="N232" s="17"/>
       <c r="O232" s="17"/>
       <c r="P232" s="17"/>
       <c r="Q232" s="17"/>
       <c r="R232" s="20" t="s">
-        <v>903</v>
+        <v>848</v>
       </c>
       <c r="S232" s="41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T232" s="20"/>
       <c r="U232" s="46" t="s">
@@ -19885,45 +19895,39 @@
       <c r="V232" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="W232" s="16" t="s">
-        <v>850</v>
-      </c>
-      <c r="X232" s="25"/>
-      <c r="Y232" s="25" t="s">
-        <v>290</v>
-      </c>
-      <c r="Z232" s="25"/>
-      <c r="AA232" s="25"/>
-      <c r="AB232" s="25">
-        <v>15</v>
+      <c r="W232" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="X232" s="1"/>
+      <c r="Y232" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="Z232" s="1"/>
+      <c r="AA232" s="1"/>
+      <c r="AB232" s="1">
+        <v>4</v>
       </c>
       <c r="AC232" s="1" t="s">
         <v>215</v>
       </c>
       <c r="AD232" s="48"/>
     </row>
-    <row r="233" spans="1:30" ht="108" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:30" ht="27" x14ac:dyDescent="0.15">
       <c r="A233" s="91">
-        <v>55990110</v>
+        <v>55990109</v>
       </c>
       <c r="B233" s="91"/>
       <c r="C233" s="91" t="s">
-        <v>591</v>
+        <v>851</v>
       </c>
       <c r="D233" s="25" t="s">
         <v>637</v>
       </c>
-      <c r="E233" s="25" t="s">
-        <v>396</v>
-      </c>
-      <c r="F233" s="25">
-        <v>40</v>
-      </c>
-      <c r="G233" s="44" t="s">
-        <v>230</v>
-      </c>
+      <c r="E233" s="25"/>
+      <c r="F233" s="25"/>
+      <c r="G233" s="44"/>
       <c r="H233" s="60"/>
-      <c r="I233" s="112"/>
+      <c r="I233" s="26"/>
       <c r="J233" s="82"/>
       <c r="K233" s="47"/>
       <c r="L233" s="99"/>
@@ -19932,11 +19936,13 @@
       <c r="O233" s="17"/>
       <c r="P233" s="17"/>
       <c r="Q233" s="17"/>
-      <c r="R233" s="20"/>
-      <c r="S233" s="41"/>
-      <c r="T233" s="20" t="s">
-        <v>1172</v>
-      </c>
+      <c r="R233" s="20" t="s">
+        <v>903</v>
+      </c>
+      <c r="S233" s="41">
+        <v>4</v>
+      </c>
+      <c r="T233" s="20"/>
       <c r="U233" s="46" t="s">
         <v>235</v>
       </c>
@@ -19944,36 +19950,42 @@
         <v>232</v>
       </c>
       <c r="W233" s="16" t="s">
-        <v>1171</v>
+        <v>850</v>
       </c>
       <c r="X233" s="25"/>
-      <c r="Y233" s="1" t="s">
-        <v>843</v>
+      <c r="Y233" s="25" t="s">
+        <v>290</v>
       </c>
       <c r="Z233" s="25"/>
       <c r="AA233" s="25"/>
       <c r="AB233" s="25">
-        <v>25</v>
-      </c>
-      <c r="AC233" s="25" t="s">
-        <v>214</v>
+        <v>15</v>
+      </c>
+      <c r="AC233" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="AD233" s="48"/>
     </row>
-    <row r="234" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:30" ht="108" x14ac:dyDescent="0.15">
       <c r="A234" s="91">
-        <v>55990111</v>
+        <v>55990110</v>
       </c>
       <c r="B234" s="91"/>
       <c r="C234" s="91" t="s">
-        <v>1173</v>
+        <v>591</v>
       </c>
       <c r="D234" s="25" t="s">
         <v>637</v>
       </c>
-      <c r="E234" s="25"/>
-      <c r="F234" s="25"/>
-      <c r="G234" s="44"/>
+      <c r="E234" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="F234" s="25">
+        <v>40</v>
+      </c>
+      <c r="G234" s="44" t="s">
+        <v>230</v>
+      </c>
       <c r="H234" s="60"/>
       <c r="I234" s="112"/>
       <c r="J234" s="82"/>
@@ -19984,33 +19996,85 @@
       <c r="O234" s="17"/>
       <c r="P234" s="17"/>
       <c r="Q234" s="17"/>
-      <c r="R234" s="20" t="s">
-        <v>406</v>
-      </c>
-      <c r="S234" s="41">
-        <v>1</v>
-      </c>
-      <c r="T234" s="20"/>
+      <c r="R234" s="20"/>
+      <c r="S234" s="41"/>
+      <c r="T234" s="20" t="s">
+        <v>1172</v>
+      </c>
       <c r="U234" s="46" t="s">
         <v>235</v>
       </c>
       <c r="V234" s="44" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="W234" s="16" t="s">
-        <v>407</v>
+        <v>1171</v>
       </c>
       <c r="X234" s="25"/>
-      <c r="Y234" s="25"/>
+      <c r="Y234" s="1" t="s">
+        <v>843</v>
+      </c>
       <c r="Z234" s="25"/>
       <c r="AA234" s="25"/>
       <c r="AB234" s="25">
+        <v>25</v>
+      </c>
+      <c r="AC234" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD234" s="48"/>
+    </row>
+    <row r="235" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A235" s="91">
+        <v>55990111</v>
+      </c>
+      <c r="B235" s="91"/>
+      <c r="C235" s="91" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D235" s="25" t="s">
+        <v>637</v>
+      </c>
+      <c r="E235" s="25"/>
+      <c r="F235" s="25"/>
+      <c r="G235" s="44"/>
+      <c r="H235" s="60"/>
+      <c r="I235" s="112"/>
+      <c r="J235" s="82"/>
+      <c r="K235" s="47"/>
+      <c r="L235" s="99"/>
+      <c r="M235" s="27"/>
+      <c r="N235" s="30"/>
+      <c r="O235" s="17"/>
+      <c r="P235" s="17"/>
+      <c r="Q235" s="17"/>
+      <c r="R235" s="20" t="s">
+        <v>406</v>
+      </c>
+      <c r="S235" s="41">
+        <v>1</v>
+      </c>
+      <c r="T235" s="20"/>
+      <c r="U235" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="V235" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="W235" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="X235" s="25"/>
+      <c r="Y235" s="25"/>
+      <c r="Z235" s="25"/>
+      <c r="AA235" s="25"/>
+      <c r="AB235" s="25">
         <v>50</v>
       </c>
-      <c r="AC234" s="25" t="s">
+      <c r="AC235" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="AD234" s="48"/>
+      <c r="AD235" s="48"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
support hit change skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Skill.xlsx
+++ b/ConfigData/Xlsx/Skill.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2114" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="1207">
   <si>
     <t>复原</t>
   </si>
@@ -3506,10 +3506,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>s.DecHp(damage.NoDefenceValue);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>修理</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4375,10 +4371,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>damage.IsNoDef=true;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>事件类型</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4502,6 +4494,26 @@
   </si>
   <si>
     <t>if(d.IsAlive){result=false;return;}s.Action.AddBuff(56000004,skl.Level,3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillEventDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>s.DecHp(damage.SourceValue);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.UseSource=true;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.AddPDamage(-20);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage.AddPDamage(-40);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5475,7 +5487,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5806,9 +5818,6 @@
     <xf numFmtId="0" fontId="22" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5869,7 +5878,6 @@
         <sz val="9"/>
         <color theme="1"/>
         <name val="Courier New"/>
-        <family val="3"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -5880,8 +5888,12 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
         <top style="thin">
           <color theme="4"/>
         </top>
@@ -6197,6 +6209,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <name val="Courier New"/>
+        <family val="3"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -6867,8 +6880,8 @@
     <tableColumn id="26" name="CheckDamage" dataDxfId="15"/>
     <tableColumn id="29" name="AfterHit" dataDxfId="14"/>
     <tableColumn id="5" name="CheckSpecial" dataDxfId="13"/>
-    <tableColumn id="9" name="SpecialCd" dataDxfId="12"/>
-    <tableColumn id="30" name="EventType" dataDxfId="0"/>
+    <tableColumn id="9" name="SpecialCd" dataDxfId="0"/>
+    <tableColumn id="30" name="EventType" dataDxfId="12"/>
     <tableColumn id="16" name="EventChecker" dataDxfId="11"/>
     <tableColumn id="25" name="Active" dataDxfId="10"/>
     <tableColumn id="20" name="IsRandom" dataDxfId="9"/>
@@ -7209,11 +7222,11 @@
   <dimension ref="A1:AB235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D17" sqref="D17"/>
       <selection pane="topRight" activeCell="D17" sqref="D17"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
-      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7289,10 +7302,10 @@
         <v>377</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>234</v>
@@ -7354,31 +7367,31 @@
         <v>250</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>1165</v>
+        <v>1202</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>378</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>233</v>
@@ -7461,10 +7474,10 @@
         <v>379</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>236</v>
@@ -7521,7 +7534,7 @@
       <c r="O4" s="20" t="s">
         <v>419</v>
       </c>
-      <c r="P4" s="41">
+      <c r="P4" s="20">
         <v>1</v>
       </c>
       <c r="Q4" s="41"/>
@@ -7548,7 +7561,7 @@
         <v>215</v>
       </c>
       <c r="AB4" s="39" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -7572,14 +7585,14 @@
       <c r="J5" s="29"/>
       <c r="K5" s="29"/>
       <c r="L5" s="18" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="M5" s="17" t="s">
         <v>454</v>
       </c>
       <c r="N5" s="17"/>
       <c r="O5" s="20"/>
-      <c r="P5" s="41"/>
+      <c r="P5" s="20"/>
       <c r="Q5" s="41"/>
       <c r="R5" s="20"/>
       <c r="S5" s="46" t="s">
@@ -7602,7 +7615,7 @@
         <v>19</v>
       </c>
       <c r="AB5" s="37" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -7626,14 +7639,14 @@
       <c r="J6" s="29"/>
       <c r="K6" s="29"/>
       <c r="L6" s="18" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="M6" s="17" t="s">
         <v>446</v>
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="20"/>
-      <c r="P6" s="41"/>
+      <c r="P6" s="20"/>
       <c r="Q6" s="41"/>
       <c r="R6" s="20"/>
       <c r="S6" s="46" t="s">
@@ -7656,7 +7669,7 @@
         <v>47</v>
       </c>
       <c r="AB6" s="37" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -7676,14 +7689,14 @@
       <c r="H7" s="59"/>
       <c r="I7" s="28"/>
       <c r="J7" s="29" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="K7" s="29"/>
       <c r="L7" s="18"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="41"/>
+      <c r="P7" s="20"/>
       <c r="Q7" s="41"/>
       <c r="R7" s="20"/>
       <c r="S7" s="46" t="s">
@@ -7724,14 +7737,14 @@
       <c r="H8" s="59"/>
       <c r="I8" s="28"/>
       <c r="J8" s="29" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="K8" s="29"/>
       <c r="L8" s="18"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="20"/>
-      <c r="P8" s="41"/>
+      <c r="P8" s="20"/>
       <c r="Q8" s="41"/>
       <c r="R8" s="20"/>
       <c r="S8" s="46" t="s">
@@ -7741,7 +7754,7 @@
         <v>230</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="1"/>
@@ -7779,7 +7792,7 @@
       <c r="M9" s="66"/>
       <c r="N9" s="67"/>
       <c r="O9" s="68"/>
-      <c r="P9" s="69"/>
+      <c r="P9" s="68"/>
       <c r="Q9" s="69"/>
       <c r="R9" s="20"/>
       <c r="S9" s="46" t="s">
@@ -7802,7 +7815,7 @@
         <v>475</v>
       </c>
       <c r="AB9" s="48" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="96" x14ac:dyDescent="0.15">
@@ -7834,10 +7847,10 @@
       <c r="L10" s="18"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="O10" s="20"/>
-      <c r="P10" s="41"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="41"/>
       <c r="R10" s="20"/>
       <c r="S10" s="46" t="s">
@@ -7864,7 +7877,7 @@
         <v>474</v>
       </c>
       <c r="AB10" s="48" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="72" x14ac:dyDescent="0.15">
@@ -7892,14 +7905,14 @@
       </c>
       <c r="I11" s="26"/>
       <c r="J11" s="90" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="K11" s="29"/>
       <c r="L11" s="27"/>
       <c r="M11" s="30"/>
       <c r="N11" s="17"/>
       <c r="O11" s="20"/>
-      <c r="P11" s="41"/>
+      <c r="P11" s="20"/>
       <c r="Q11" s="41"/>
       <c r="R11" s="20"/>
       <c r="S11" s="46" t="s">
@@ -7915,7 +7928,7 @@
       <c r="W11" s="25"/>
       <c r="X11" s="25"/>
       <c r="Y11" s="25" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="Z11" s="61">
         <v>15</v>
@@ -7931,7 +7944,7 @@
       </c>
       <c r="B12" s="51"/>
       <c r="C12" s="51" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>686</v>
@@ -7940,7 +7953,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="44"/>
       <c r="H12" s="60" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I12" s="26"/>
       <c r="J12" s="90"/>
@@ -7949,7 +7962,7 @@
       <c r="M12" s="30"/>
       <c r="N12" s="17"/>
       <c r="O12" s="20"/>
-      <c r="P12" s="41"/>
+      <c r="P12" s="20"/>
       <c r="Q12" s="41"/>
       <c r="R12" s="20"/>
       <c r="S12" s="46" t="s">
@@ -7959,19 +7972,19 @@
         <v>230</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="V12" s="25"/>
       <c r="W12" s="25"/>
       <c r="X12" s="25"/>
       <c r="Y12" s="25" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="Z12" s="61">
         <v>15</v>
       </c>
       <c r="AA12" s="25" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="AB12" s="48"/>
     </row>
@@ -7995,17 +8008,17 @@
         <v>628</v>
       </c>
       <c r="K13" s="82" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="L13" s="18"/>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="20"/>
-      <c r="P13" s="41"/>
+      <c r="P13" s="20"/>
       <c r="Q13" s="41"/>
       <c r="R13" s="20"/>
       <c r="S13" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="T13" s="9" t="s">
         <v>230</v>
@@ -8026,7 +8039,7 @@
         <v>103</v>
       </c>
       <c r="AB13" s="37" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="48" x14ac:dyDescent="0.15">
@@ -8055,7 +8068,7 @@
       </c>
       <c r="N14" s="17"/>
       <c r="O14" s="20"/>
-      <c r="P14" s="41"/>
+      <c r="P14" s="20"/>
       <c r="Q14" s="41"/>
       <c r="R14" s="20"/>
       <c r="S14" s="1" t="s">
@@ -8078,7 +8091,7 @@
         <v>35</v>
       </c>
       <c r="AB14" s="37" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -8101,17 +8114,17 @@
         <v>922</v>
       </c>
       <c r="K15" s="29" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="L15" s="18"/>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="20"/>
-      <c r="P15" s="41"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="41"/>
       <c r="R15" s="20"/>
       <c r="S15" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="T15" s="9" t="s">
         <v>230</v>
@@ -8123,7 +8136,7 @@
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="Z15" s="1">
         <v>15</v>
@@ -8132,7 +8145,7 @@
         <v>297</v>
       </c>
       <c r="AB15" s="37" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.15">
@@ -8159,7 +8172,7 @@
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="20"/>
-      <c r="P16" s="41"/>
+      <c r="P16" s="20"/>
       <c r="Q16" s="41"/>
       <c r="R16" s="20"/>
       <c r="S16" s="1" t="s">
@@ -8182,7 +8195,7 @@
         <v>535</v>
       </c>
       <c r="AB16" s="37" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -8209,11 +8222,11 @@
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="20"/>
-      <c r="P17" s="41"/>
+      <c r="P17" s="20"/>
       <c r="Q17" s="41"/>
       <c r="R17" s="20"/>
       <c r="S17" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="T17" s="9" t="s">
         <v>230</v>
@@ -8234,7 +8247,7 @@
         <v>352</v>
       </c>
       <c r="AB17" s="37" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="48" x14ac:dyDescent="0.15">
@@ -8259,12 +8272,12 @@
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="20"/>
-      <c r="P18" s="41"/>
+      <c r="P18" s="20"/>
       <c r="Q18" s="41" t="s">
+        <v>1174</v>
+      </c>
+      <c r="R18" s="20" t="s">
         <v>1176</v>
-      </c>
-      <c r="R18" s="20" t="s">
-        <v>1178</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>235</v>
@@ -8288,7 +8301,7 @@
         <v>670</v>
       </c>
       <c r="AB18" s="37" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="48" x14ac:dyDescent="0.15">
@@ -8297,7 +8310,7 @@
       </c>
       <c r="B19" s="51"/>
       <c r="C19" s="51" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>686</v>
@@ -8308,16 +8321,16 @@
       <c r="H19" s="59"/>
       <c r="I19" s="28"/>
       <c r="J19" s="29" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="K19" s="82" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="20"/>
-      <c r="P19" s="41"/>
+      <c r="P19" s="20"/>
       <c r="Q19" s="41"/>
       <c r="R19" s="20"/>
       <c r="S19" s="1" t="s">
@@ -8327,7 +8340,7 @@
         <v>230</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="V19" s="10"/>
       <c r="W19" s="1"/>
@@ -8337,10 +8350,10 @@
         <v>0</v>
       </c>
       <c r="AA19" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="AB19" s="37" t="s">
         <v>994</v>
-      </c>
-      <c r="AB19" s="37" t="s">
-        <v>995</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.15">
@@ -8349,7 +8362,7 @@
       </c>
       <c r="B20" s="51"/>
       <c r="C20" s="52" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>686</v>
@@ -8367,7 +8380,7 @@
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="20"/>
-      <c r="P20" s="41"/>
+      <c r="P20" s="20"/>
       <c r="Q20" s="41"/>
       <c r="R20" s="20"/>
       <c r="S20" s="46" t="s">
@@ -8397,7 +8410,7 @@
       </c>
       <c r="B21" s="51"/>
       <c r="C21" s="52" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>686</v>
@@ -8408,14 +8421,14 @@
       <c r="H21" s="59"/>
       <c r="I21" s="26"/>
       <c r="J21" s="29" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="K21" s="29"/>
       <c r="L21" s="27"/>
       <c r="M21" s="30"/>
       <c r="N21" s="17"/>
       <c r="O21" s="20"/>
-      <c r="P21" s="41"/>
+      <c r="P21" s="20"/>
       <c r="Q21" s="41"/>
       <c r="R21" s="20"/>
       <c r="S21" s="46" t="s">
@@ -8425,7 +8438,7 @@
         <v>230</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="V21" s="25"/>
       <c r="W21" s="25"/>
@@ -8435,10 +8448,10 @@
         <v>40</v>
       </c>
       <c r="AA21" s="25" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="AB21" s="37" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -8457,17 +8470,17 @@
       <c r="G22" s="99"/>
       <c r="H22" s="100"/>
       <c r="I22" s="26" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="J22" s="90" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="K22" s="101"/>
       <c r="L22" s="102"/>
       <c r="M22" s="103"/>
       <c r="N22" s="104"/>
       <c r="O22" s="105"/>
-      <c r="P22" s="106"/>
+      <c r="P22" s="105"/>
       <c r="Q22" s="106"/>
       <c r="R22" s="20"/>
       <c r="S22" s="46" t="s">
@@ -8477,7 +8490,7 @@
         <v>230</v>
       </c>
       <c r="U22" s="16" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="V22" s="98"/>
       <c r="W22" s="98"/>
@@ -8487,10 +8500,10 @@
         <v>10</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="AB22" s="107" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -8499,7 +8512,7 @@
       </c>
       <c r="B23" s="51"/>
       <c r="C23" s="52" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>686</v>
@@ -8509,17 +8522,17 @@
       <c r="G23" s="99"/>
       <c r="H23" s="100"/>
       <c r="I23" s="26" t="s">
+        <v>1145</v>
+      </c>
+      <c r="J23" s="29" t="s">
         <v>1146</v>
-      </c>
-      <c r="J23" s="29" t="s">
-        <v>1147</v>
       </c>
       <c r="K23" s="101"/>
       <c r="L23" s="102"/>
       <c r="M23" s="103"/>
       <c r="N23" s="104"/>
       <c r="O23" s="105"/>
-      <c r="P23" s="106"/>
+      <c r="P23" s="105"/>
       <c r="Q23" s="106"/>
       <c r="R23" s="20"/>
       <c r="S23" s="46" t="s">
@@ -8529,7 +8542,7 @@
         <v>230</v>
       </c>
       <c r="U23" s="16" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="V23" s="98"/>
       <c r="W23" s="98"/>
@@ -8539,7 +8552,7 @@
         <v>0</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="AB23" s="107"/>
     </row>
@@ -8552,7 +8565,7 @@
         <v>149</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -8563,11 +8576,11 @@
       <c r="K24" s="29"/>
       <c r="L24" s="18"/>
       <c r="M24" s="17" t="s">
-        <v>1169</v>
+        <v>1204</v>
       </c>
       <c r="N24" s="17"/>
       <c r="O24" s="20"/>
-      <c r="P24" s="41"/>
+      <c r="P24" s="20"/>
       <c r="Q24" s="41"/>
       <c r="R24" s="20"/>
       <c r="S24" s="35" t="s">
@@ -8600,7 +8613,7 @@
         <v>157</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -8612,10 +8625,10 @@
       <c r="L25" s="18"/>
       <c r="M25" s="17"/>
       <c r="N25" s="17" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="O25" s="20"/>
-      <c r="P25" s="41"/>
+      <c r="P25" s="20"/>
       <c r="Q25" s="41"/>
       <c r="R25" s="20"/>
       <c r="S25" s="1" t="s">
@@ -8638,7 +8651,7 @@
         <v>158</v>
       </c>
       <c r="AB25" s="37" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -8650,7 +8663,7 @@
         <v>76</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -8665,7 +8678,7 @@
         <v>343</v>
       </c>
       <c r="O26" s="20"/>
-      <c r="P26" s="41"/>
+      <c r="P26" s="20"/>
       <c r="Q26" s="41"/>
       <c r="R26" s="20"/>
       <c r="S26" s="1" t="s">
@@ -8688,7 +8701,7 @@
         <v>77</v>
       </c>
       <c r="AB26" s="37" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="27" spans="1:28" ht="48" x14ac:dyDescent="0.15">
@@ -8700,7 +8713,7 @@
         <v>523</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -8708,14 +8721,14 @@
       <c r="H27" s="59"/>
       <c r="I27" s="28"/>
       <c r="J27" s="29" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="K27" s="29"/>
       <c r="L27" s="18"/>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
       <c r="O27" s="20"/>
-      <c r="P27" s="41"/>
+      <c r="P27" s="20"/>
       <c r="Q27" s="41"/>
       <c r="R27" s="20"/>
       <c r="S27" s="1" t="s">
@@ -8748,7 +8761,7 @@
         <v>538</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -8765,7 +8778,7 @@
         <v>932</v>
       </c>
       <c r="O28" s="20"/>
-      <c r="P28" s="41"/>
+      <c r="P28" s="20"/>
       <c r="Q28" s="41"/>
       <c r="R28" s="20"/>
       <c r="S28" s="1" t="s">
@@ -8775,7 +8788,7 @@
         <v>230</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="V28" s="14"/>
       <c r="W28" s="1"/>
@@ -8798,7 +8811,7 @@
         <v>539</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -8815,7 +8828,7 @@
       </c>
       <c r="N29" s="17"/>
       <c r="O29" s="20"/>
-      <c r="P29" s="41"/>
+      <c r="P29" s="20"/>
       <c r="Q29" s="41"/>
       <c r="R29" s="20"/>
       <c r="S29" s="1" t="s">
@@ -8848,7 +8861,7 @@
         <v>540</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -8865,7 +8878,7 @@
       </c>
       <c r="N30" s="17"/>
       <c r="O30" s="20"/>
-      <c r="P30" s="41"/>
+      <c r="P30" s="20"/>
       <c r="Q30" s="41"/>
       <c r="R30" s="20"/>
       <c r="S30" s="1" t="s">
@@ -8898,7 +8911,7 @@
         <v>558</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -8913,7 +8926,7 @@
         <v>272</v>
       </c>
       <c r="O31" s="20"/>
-      <c r="P31" s="41"/>
+      <c r="P31" s="20"/>
       <c r="Q31" s="41"/>
       <c r="R31" s="20"/>
       <c r="S31" s="1" t="s">
@@ -8946,7 +8959,7 @@
         <v>559</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -8957,11 +8970,11 @@
       <c r="K32" s="29"/>
       <c r="L32" s="18"/>
       <c r="M32" s="17" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="N32" s="17"/>
       <c r="O32" s="20"/>
-      <c r="P32" s="41"/>
+      <c r="P32" s="20"/>
       <c r="Q32" s="41"/>
       <c r="R32" s="20"/>
       <c r="S32" s="1" t="s">
@@ -8991,10 +9004,10 @@
       </c>
       <c r="B33" s="74"/>
       <c r="C33" s="74" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -9011,7 +9024,7 @@
       </c>
       <c r="N33" s="17"/>
       <c r="O33" s="20"/>
-      <c r="P33" s="41"/>
+      <c r="P33" s="20"/>
       <c r="Q33" s="41"/>
       <c r="R33" s="20"/>
       <c r="S33" s="1" t="s">
@@ -9021,7 +9034,7 @@
         <v>230</v>
       </c>
       <c r="U33" s="10" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="V33" s="10"/>
       <c r="W33" s="1"/>
@@ -9035,16 +9048,16 @@
       </c>
       <c r="AB33" s="37"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A34" s="74">
         <v>55110011</v>
       </c>
       <c r="B34" s="74"/>
-      <c r="C34" s="110" t="s">
+      <c r="C34" s="74" t="s">
         <v>567</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -9055,11 +9068,13 @@
       </c>
       <c r="J34" s="29"/>
       <c r="K34" s="29"/>
-      <c r="L34" s="18"/>
+      <c r="L34" s="18" t="s">
+        <v>1205</v>
+      </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
       <c r="O34" s="20"/>
-      <c r="P34" s="41"/>
+      <c r="P34" s="20"/>
       <c r="Q34" s="41"/>
       <c r="R34" s="20"/>
       <c r="S34" s="1" t="s">
@@ -9069,7 +9084,7 @@
         <v>230</v>
       </c>
       <c r="U34" s="10" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="V34" s="10"/>
       <c r="W34" s="1"/>
@@ -9092,7 +9107,7 @@
         <v>575</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -9107,7 +9122,7 @@
         <v>574</v>
       </c>
       <c r="O35" s="20"/>
-      <c r="P35" s="41"/>
+      <c r="P35" s="20"/>
       <c r="Q35" s="41"/>
       <c r="R35" s="20"/>
       <c r="S35" s="1" t="s">
@@ -9140,7 +9155,7 @@
         <v>580</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -9156,10 +9171,10 @@
         <v>581</v>
       </c>
       <c r="N36" s="17" t="s">
-        <v>933</v>
+        <v>1203</v>
       </c>
       <c r="O36" s="20"/>
-      <c r="P36" s="41"/>
+      <c r="P36" s="20"/>
       <c r="Q36" s="41"/>
       <c r="R36" s="20"/>
       <c r="S36" s="10" t="s">
@@ -9169,7 +9184,7 @@
         <v>230</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="V36" s="10"/>
       <c r="W36" s="1"/>
@@ -9192,7 +9207,7 @@
         <v>582</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -9207,7 +9222,7 @@
         <v>373</v>
       </c>
       <c r="O37" s="20"/>
-      <c r="P37" s="41"/>
+      <c r="P37" s="20"/>
       <c r="Q37" s="41"/>
       <c r="R37" s="20"/>
       <c r="S37" s="1" t="s">
@@ -9240,7 +9255,7 @@
         <v>584</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -9257,7 +9272,7 @@
       </c>
       <c r="N38" s="17"/>
       <c r="O38" s="20"/>
-      <c r="P38" s="41"/>
+      <c r="P38" s="20"/>
       <c r="Q38" s="41"/>
       <c r="R38" s="20"/>
       <c r="S38" s="1" t="s">
@@ -9281,16 +9296,16 @@
       </c>
       <c r="AB38" s="37"/>
     </row>
-    <row r="39" spans="1:28" ht="24" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A39" s="74">
         <v>55110016</v>
       </c>
       <c r="B39" s="74"/>
-      <c r="C39" s="110" t="s">
+      <c r="C39" s="74" t="s">
         <v>586</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -9301,11 +9316,13 @@
       </c>
       <c r="J39" s="29"/>
       <c r="K39" s="29"/>
-      <c r="L39" s="18"/>
+      <c r="L39" s="18" t="s">
+        <v>1206</v>
+      </c>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
       <c r="O39" s="20"/>
-      <c r="P39" s="41"/>
+      <c r="P39" s="20"/>
       <c r="Q39" s="41"/>
       <c r="R39" s="20"/>
       <c r="S39" s="1" t="s">
@@ -9338,7 +9355,7 @@
         <v>588</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -9349,11 +9366,11 @@
       <c r="K40" s="29"/>
       <c r="L40" s="18"/>
       <c r="M40" s="17" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="N40" s="17"/>
       <c r="O40" s="20"/>
-      <c r="P40" s="41"/>
+      <c r="P40" s="20"/>
       <c r="Q40" s="41"/>
       <c r="R40" s="20"/>
       <c r="S40" s="1" t="s">
@@ -9386,7 +9403,7 @@
         <v>590</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -9403,7 +9420,7 @@
       </c>
       <c r="N41" s="17"/>
       <c r="O41" s="20"/>
-      <c r="P41" s="41"/>
+      <c r="P41" s="20"/>
       <c r="Q41" s="41"/>
       <c r="R41" s="20"/>
       <c r="S41" s="1" t="s">
@@ -9438,7 +9455,7 @@
         <v>619</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E42" s="25"/>
       <c r="F42" s="25"/>
@@ -9455,7 +9472,7 @@
       </c>
       <c r="N42" s="17"/>
       <c r="O42" s="20"/>
-      <c r="P42" s="41"/>
+      <c r="P42" s="20"/>
       <c r="Q42" s="41"/>
       <c r="R42" s="20"/>
       <c r="S42" s="46" t="s">
@@ -9490,7 +9507,7 @@
         <v>761</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -9507,7 +9524,7 @@
       </c>
       <c r="N43" s="17"/>
       <c r="O43" s="20"/>
-      <c r="P43" s="41"/>
+      <c r="P43" s="20"/>
       <c r="Q43" s="41"/>
       <c r="R43" s="20"/>
       <c r="S43" s="1" t="s">
@@ -9537,10 +9554,10 @@
       </c>
       <c r="B44" s="74"/>
       <c r="C44" s="74" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
@@ -9555,7 +9572,7 @@
       </c>
       <c r="N44" s="17"/>
       <c r="O44" s="20"/>
-      <c r="P44" s="41"/>
+      <c r="P44" s="20"/>
       <c r="Q44" s="41"/>
       <c r="R44" s="20"/>
       <c r="S44" s="46" t="s">
@@ -9565,7 +9582,7 @@
         <v>359</v>
       </c>
       <c r="U44" s="16" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="V44" s="25"/>
       <c r="W44" s="25" t="s">
@@ -9577,7 +9594,7 @@
         <v>65</v>
       </c>
       <c r="AA44" s="25" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="AB44" s="48"/>
     </row>
@@ -9607,9 +9624,9 @@
       <c r="M45" s="30"/>
       <c r="N45" s="17"/>
       <c r="O45" s="20" t="s">
-        <v>1086</v>
-      </c>
-      <c r="P45" s="41">
+        <v>1085</v>
+      </c>
+      <c r="P45" s="20">
         <v>1</v>
       </c>
       <c r="Q45" s="41"/>
@@ -9667,12 +9684,12 @@
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="20"/>
-      <c r="P46" s="41"/>
+      <c r="P46" s="20"/>
       <c r="Q46" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R46" s="20" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="S46" s="25" t="s">
         <v>235</v>
@@ -9681,7 +9698,7 @@
         <v>230</v>
       </c>
       <c r="U46" s="16" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="V46" s="25"/>
       <c r="W46" s="25" t="s">
@@ -9696,7 +9713,7 @@
         <v>445</v>
       </c>
       <c r="AB46" s="48" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="47" spans="1:28" ht="108" x14ac:dyDescent="0.15">
@@ -9722,14 +9739,14 @@
       <c r="H47" s="60"/>
       <c r="I47" s="86"/>
       <c r="J47" s="47" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="K47" s="85"/>
       <c r="L47" s="87"/>
       <c r="M47" s="88"/>
       <c r="N47" s="32"/>
       <c r="O47" s="33"/>
-      <c r="P47" s="42"/>
+      <c r="P47" s="33"/>
       <c r="Q47" s="42"/>
       <c r="R47" s="20"/>
       <c r="S47" s="89" t="s">
@@ -9739,7 +9756,7 @@
         <v>359</v>
       </c>
       <c r="U47" s="16" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V47" s="31"/>
       <c r="W47" s="31"/>
@@ -9779,9 +9796,9 @@
       <c r="M48" s="30"/>
       <c r="N48" s="17"/>
       <c r="O48" s="20" t="s">
-        <v>1134</v>
-      </c>
-      <c r="P48" s="41">
+        <v>1133</v>
+      </c>
+      <c r="P48" s="20">
         <v>1</v>
       </c>
       <c r="Q48" s="41"/>
@@ -9793,7 +9810,7 @@
         <v>230</v>
       </c>
       <c r="U48" s="16" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="V48" s="25"/>
       <c r="W48" s="10" t="s">
@@ -9839,9 +9856,9 @@
       <c r="M49" s="30"/>
       <c r="N49" s="17"/>
       <c r="O49" s="20" t="s">
-        <v>1028</v>
-      </c>
-      <c r="P49" s="41">
+        <v>1027</v>
+      </c>
+      <c r="P49" s="20">
         <v>2</v>
       </c>
       <c r="Q49" s="41"/>
@@ -9900,10 +9917,10 @@
       <c r="L50" s="18"/>
       <c r="M50" s="17"/>
       <c r="N50" s="17" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="O50" s="20"/>
-      <c r="P50" s="41"/>
+      <c r="P50" s="20"/>
       <c r="Q50" s="41"/>
       <c r="R50" s="20"/>
       <c r="S50" s="1" t="s">
@@ -9960,10 +9977,10 @@
       <c r="L51" s="18"/>
       <c r="M51" s="17"/>
       <c r="N51" s="17" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="O51" s="20"/>
-      <c r="P51" s="41"/>
+      <c r="P51" s="20"/>
       <c r="Q51" s="41"/>
       <c r="R51" s="20"/>
       <c r="S51" s="1" t="s">
@@ -10020,10 +10037,10 @@
       <c r="L52" s="27"/>
       <c r="M52" s="30"/>
       <c r="N52" s="17" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="O52" s="20"/>
-      <c r="P52" s="41"/>
+      <c r="P52" s="20"/>
       <c r="Q52" s="41"/>
       <c r="R52" s="20"/>
       <c r="S52" s="46" t="s">
@@ -10037,10 +10054,10 @@
       </c>
       <c r="V52" s="25"/>
       <c r="W52" s="25" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="X52" s="25" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="Y52" s="25"/>
       <c r="Z52" s="25">
@@ -10078,10 +10095,10 @@
       <c r="L53" s="18"/>
       <c r="M53" s="17"/>
       <c r="N53" s="17" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="O53" s="20"/>
-      <c r="P53" s="41"/>
+      <c r="P53" s="20"/>
       <c r="Q53" s="41"/>
       <c r="R53" s="20"/>
       <c r="S53" s="1" t="s">
@@ -10132,14 +10149,14 @@
       <c r="H54" s="60"/>
       <c r="I54" s="28"/>
       <c r="J54" s="29" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="K54" s="29"/>
       <c r="L54" s="18"/>
       <c r="M54" s="17"/>
       <c r="N54" s="17"/>
       <c r="O54" s="20"/>
-      <c r="P54" s="41"/>
+      <c r="P54" s="20"/>
       <c r="Q54" s="41"/>
       <c r="R54" s="20"/>
       <c r="S54" s="25" t="s">
@@ -10188,14 +10205,14 @@
       <c r="H55" s="59"/>
       <c r="I55" s="26"/>
       <c r="J55" s="47" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="K55" s="47"/>
       <c r="L55" s="27"/>
       <c r="M55" s="30"/>
       <c r="N55" s="17"/>
       <c r="O55" s="20"/>
-      <c r="P55" s="41"/>
+      <c r="P55" s="20"/>
       <c r="Q55" s="41"/>
       <c r="R55" s="20"/>
       <c r="S55" s="46" t="s">
@@ -10205,7 +10222,7 @@
         <v>230</v>
       </c>
       <c r="U55" s="16" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="V55" s="25"/>
       <c r="W55" s="10" t="s">
@@ -10246,14 +10263,14 @@
       <c r="H56" s="60"/>
       <c r="I56" s="86"/>
       <c r="J56" s="47" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="K56" s="85"/>
       <c r="L56" s="87"/>
       <c r="M56" s="88"/>
       <c r="N56" s="32"/>
       <c r="O56" s="33"/>
-      <c r="P56" s="42"/>
+      <c r="P56" s="33"/>
       <c r="Q56" s="42"/>
       <c r="R56" s="20"/>
       <c r="S56" s="89" t="s">
@@ -10280,7 +10297,7 @@
         <v>700</v>
       </c>
       <c r="AB56" s="48" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="57" spans="1:28" ht="96" x14ac:dyDescent="0.15">
@@ -10306,14 +10323,14 @@
       <c r="H57" s="60"/>
       <c r="I57" s="86"/>
       <c r="J57" s="47" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="K57" s="85"/>
       <c r="L57" s="87"/>
       <c r="M57" s="88"/>
       <c r="N57" s="32"/>
       <c r="O57" s="33"/>
-      <c r="P57" s="42"/>
+      <c r="P57" s="33"/>
       <c r="Q57" s="42"/>
       <c r="R57" s="20"/>
       <c r="S57" s="89" t="s">
@@ -10362,14 +10379,14 @@
       <c r="H58" s="60"/>
       <c r="I58" s="26"/>
       <c r="J58" s="90" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="K58" s="29"/>
       <c r="L58" s="27"/>
       <c r="M58" s="30"/>
       <c r="N58" s="17"/>
       <c r="O58" s="20"/>
-      <c r="P58" s="41"/>
+      <c r="P58" s="20"/>
       <c r="Q58" s="41"/>
       <c r="R58" s="20"/>
       <c r="S58" s="46" t="s">
@@ -10383,10 +10400,10 @@
       </c>
       <c r="V58" s="25"/>
       <c r="W58" s="25" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="X58" s="25" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="Y58" s="25"/>
       <c r="Z58" s="25">
@@ -10420,14 +10437,14 @@
       <c r="H59" s="60"/>
       <c r="I59" s="86"/>
       <c r="J59" s="47" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="K59" s="85"/>
       <c r="L59" s="87"/>
       <c r="M59" s="88"/>
       <c r="N59" s="32"/>
       <c r="O59" s="33"/>
-      <c r="P59" s="42"/>
+      <c r="P59" s="33"/>
       <c r="Q59" s="42"/>
       <c r="R59" s="20"/>
       <c r="S59" s="89" t="s">
@@ -10437,7 +10454,7 @@
         <v>359</v>
       </c>
       <c r="U59" s="16" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="V59" s="31"/>
       <c r="W59" s="31"/>
@@ -10452,7 +10469,7 @@
         <v>790</v>
       </c>
       <c r="AB59" s="48" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="60" spans="1:28" ht="72" x14ac:dyDescent="0.15">
@@ -10461,7 +10478,7 @@
       </c>
       <c r="B60" s="72"/>
       <c r="C60" s="11" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>93</v>
@@ -10476,14 +10493,14 @@
       <c r="H60" s="59"/>
       <c r="I60" s="26"/>
       <c r="J60" s="47" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="K60" s="47"/>
       <c r="L60" s="27"/>
       <c r="M60" s="30"/>
       <c r="N60" s="17"/>
       <c r="O60" s="20"/>
-      <c r="P60" s="41"/>
+      <c r="P60" s="20"/>
       <c r="Q60" s="41"/>
       <c r="R60" s="20"/>
       <c r="S60" s="46" t="s">
@@ -10493,21 +10510,21 @@
         <v>230</v>
       </c>
       <c r="U60" s="16" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="V60" s="25"/>
       <c r="W60" s="10" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="X60" s="10" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="Y60" s="10"/>
       <c r="Z60" s="25">
         <v>30</v>
       </c>
       <c r="AA60" s="25" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AB60" s="48"/>
     </row>
@@ -10517,7 +10534,7 @@
       </c>
       <c r="B61" s="72"/>
       <c r="C61" s="11" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>93</v>
@@ -10539,12 +10556,12 @@
       <c r="M61" s="30"/>
       <c r="N61" s="17"/>
       <c r="O61" s="20"/>
-      <c r="P61" s="41"/>
+      <c r="P61" s="20"/>
       <c r="Q61" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R61" s="20" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="S61" s="1" t="s">
         <v>235</v>
@@ -10553,7 +10570,7 @@
         <v>359</v>
       </c>
       <c r="U61" s="10" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="V61" s="25"/>
       <c r="W61" s="25" t="s">
@@ -10567,10 +10584,10 @@
         <v>35</v>
       </c>
       <c r="AA61" s="25" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="AB61" s="48" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="62" spans="1:28" ht="132" x14ac:dyDescent="0.15">
@@ -10579,7 +10596,7 @@
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="12" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>93</v>
@@ -10596,17 +10613,17 @@
       <c r="H62" s="60"/>
       <c r="I62" s="86"/>
       <c r="J62" s="47" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="K62" s="85"/>
       <c r="L62" s="87"/>
       <c r="M62" s="88"/>
       <c r="N62" s="32"/>
       <c r="O62" s="33"/>
-      <c r="P62" s="42"/>
+      <c r="P62" s="33"/>
       <c r="Q62" s="42"/>
       <c r="R62" s="20" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="S62" s="89" t="s">
         <v>235</v>
@@ -10615,7 +10632,7 @@
         <v>359</v>
       </c>
       <c r="U62" s="16" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="V62" s="31"/>
       <c r="W62" s="31"/>
@@ -10625,7 +10642,7 @@
         <v>50</v>
       </c>
       <c r="AA62" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="AB62" s="48"/>
     </row>
@@ -10638,7 +10655,7 @@
         <v>702</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E63" s="25"/>
       <c r="F63" s="25"/>
@@ -10655,10 +10672,10 @@
       <c r="M63" s="30"/>
       <c r="N63" s="17"/>
       <c r="O63" s="20"/>
-      <c r="P63" s="41"/>
+      <c r="P63" s="20"/>
       <c r="Q63" s="41"/>
       <c r="R63" s="20" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="S63" s="46" t="s">
         <v>235</v>
@@ -10682,7 +10699,7 @@
         <v>64</v>
       </c>
       <c r="AB63" s="48" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="72" x14ac:dyDescent="0.15">
@@ -10694,7 +10711,7 @@
         <v>412</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E64" s="25"/>
       <c r="F64" s="25"/>
@@ -10711,10 +10728,10 @@
       <c r="M64" s="30"/>
       <c r="N64" s="17"/>
       <c r="O64" s="20"/>
-      <c r="P64" s="41"/>
+      <c r="P64" s="20"/>
       <c r="Q64" s="41"/>
       <c r="R64" s="20" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="S64" s="46" t="s">
         <v>235</v>
@@ -10746,7 +10763,7 @@
         <v>413</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E65" s="25"/>
       <c r="F65" s="25"/>
@@ -10763,10 +10780,10 @@
       <c r="M65" s="30"/>
       <c r="N65" s="17"/>
       <c r="O65" s="20"/>
-      <c r="P65" s="41"/>
+      <c r="P65" s="20"/>
       <c r="Q65" s="41"/>
       <c r="R65" s="20" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="S65" s="46" t="s">
         <v>235</v>
@@ -10798,7 +10815,7 @@
         <v>414</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
@@ -10815,10 +10832,10 @@
       <c r="M66" s="30"/>
       <c r="N66" s="17"/>
       <c r="O66" s="20"/>
-      <c r="P66" s="41"/>
+      <c r="P66" s="20"/>
       <c r="Q66" s="41"/>
       <c r="R66" s="20" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="S66" s="46" t="s">
         <v>235</v>
@@ -10850,7 +10867,7 @@
         <v>415</v>
       </c>
       <c r="D67" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E67" s="25"/>
       <c r="F67" s="25"/>
@@ -10867,10 +10884,10 @@
       <c r="M67" s="30"/>
       <c r="N67" s="17"/>
       <c r="O67" s="20"/>
-      <c r="P67" s="41"/>
+      <c r="P67" s="20"/>
       <c r="Q67" s="41"/>
       <c r="R67" s="20" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="S67" s="46" t="s">
         <v>235</v>
@@ -10902,7 +10919,7 @@
         <v>416</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E68" s="25"/>
       <c r="F68" s="25"/>
@@ -10917,10 +10934,10 @@
       <c r="M68" s="30"/>
       <c r="N68" s="17"/>
       <c r="O68" s="20"/>
-      <c r="P68" s="41"/>
+      <c r="P68" s="20"/>
       <c r="Q68" s="41"/>
       <c r="R68" s="20" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="S68" s="46" t="s">
         <v>235</v>
@@ -10929,7 +10946,7 @@
         <v>230</v>
       </c>
       <c r="U68" s="49" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="V68" s="25"/>
       <c r="W68" s="25" t="s">
@@ -10954,7 +10971,7 @@
         <v>420</v>
       </c>
       <c r="D69" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E69" s="25"/>
       <c r="F69" s="25"/>
@@ -10971,10 +10988,10 @@
       <c r="M69" s="30"/>
       <c r="N69" s="17"/>
       <c r="O69" s="20"/>
-      <c r="P69" s="41"/>
+      <c r="P69" s="20"/>
       <c r="Q69" s="41"/>
       <c r="R69" s="20" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="S69" s="46" t="s">
         <v>235</v>
@@ -11006,7 +11023,7 @@
         <v>660</v>
       </c>
       <c r="D70" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E70" s="25"/>
       <c r="F70" s="25"/>
@@ -11023,10 +11040,10 @@
       <c r="M70" s="30"/>
       <c r="N70" s="17"/>
       <c r="O70" s="20"/>
-      <c r="P70" s="41"/>
+      <c r="P70" s="20"/>
       <c r="Q70" s="41"/>
       <c r="R70" s="20" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="S70" s="46" t="s">
         <v>235</v>
@@ -11058,7 +11075,7 @@
         <v>703</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E71" s="25"/>
       <c r="F71" s="25"/>
@@ -11075,7 +11092,7 @@
       <c r="M71" s="30"/>
       <c r="N71" s="17"/>
       <c r="O71" s="20"/>
-      <c r="P71" s="41"/>
+      <c r="P71" s="20"/>
       <c r="Q71" s="41"/>
       <c r="R71" s="20"/>
       <c r="S71" s="46" t="s">
@@ -11108,7 +11125,7 @@
         <v>715</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E72" s="25"/>
       <c r="F72" s="25"/>
@@ -11125,7 +11142,7 @@
       <c r="M72" s="30"/>
       <c r="N72" s="17"/>
       <c r="O72" s="20"/>
-      <c r="P72" s="41"/>
+      <c r="P72" s="20"/>
       <c r="Q72" s="41"/>
       <c r="R72" s="20"/>
       <c r="S72" s="46" t="s">
@@ -11158,7 +11175,7 @@
         <v>775</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E73" s="25"/>
       <c r="F73" s="25"/>
@@ -11175,7 +11192,7 @@
       <c r="M73" s="30"/>
       <c r="N73" s="17"/>
       <c r="O73" s="20"/>
-      <c r="P73" s="41"/>
+      <c r="P73" s="20"/>
       <c r="Q73" s="41"/>
       <c r="R73" s="20"/>
       <c r="S73" s="46" t="s">
@@ -11208,7 +11225,7 @@
         <v>779</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E74" s="25"/>
       <c r="F74" s="25"/>
@@ -11225,7 +11242,7 @@
       <c r="M74" s="17"/>
       <c r="N74" s="17"/>
       <c r="O74" s="20"/>
-      <c r="P74" s="41"/>
+      <c r="P74" s="20"/>
       <c r="Q74" s="41"/>
       <c r="R74" s="20"/>
       <c r="S74" s="25" t="s">
@@ -11258,7 +11275,7 @@
         <v>128</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -11275,7 +11292,7 @@
       <c r="M75" s="17"/>
       <c r="N75" s="17"/>
       <c r="O75" s="20"/>
-      <c r="P75" s="41"/>
+      <c r="P75" s="20"/>
       <c r="Q75" s="41"/>
       <c r="R75" s="20"/>
       <c r="S75" s="1" t="s">
@@ -11308,7 +11325,7 @@
         <v>155</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E76" s="25"/>
       <c r="F76" s="25"/>
@@ -11323,7 +11340,7 @@
       <c r="O76" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="P76" s="41">
+      <c r="P76" s="20">
         <v>1</v>
       </c>
       <c r="Q76" s="41"/>
@@ -11358,7 +11375,7 @@
         <v>178</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -11371,12 +11388,12 @@
       <c r="M77" s="30"/>
       <c r="N77" s="17"/>
       <c r="O77" s="20"/>
-      <c r="P77" s="41"/>
+      <c r="P77" s="20"/>
       <c r="Q77" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R77" s="20" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="S77" s="35" t="s">
         <v>235</v>
@@ -11398,7 +11415,7 @@
         <v>179</v>
       </c>
       <c r="AB77" s="25" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="78" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -11410,7 +11427,7 @@
         <v>203</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -11423,12 +11440,12 @@
       <c r="M78" s="30"/>
       <c r="N78" s="17"/>
       <c r="O78" s="20"/>
-      <c r="P78" s="41"/>
+      <c r="P78" s="20"/>
       <c r="Q78" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R78" s="20" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="S78" s="35" t="s">
         <v>235</v>
@@ -11450,7 +11467,7 @@
         <v>204</v>
       </c>
       <c r="AB78" s="25" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="79" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -11459,10 +11476,10 @@
       </c>
       <c r="B79" s="53"/>
       <c r="C79" s="53" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -11470,14 +11487,14 @@
       <c r="H79" s="60"/>
       <c r="I79" s="26"/>
       <c r="J79" s="47" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="K79" s="47"/>
       <c r="L79" s="27"/>
       <c r="M79" s="30"/>
       <c r="N79" s="17"/>
       <c r="O79" s="20"/>
-      <c r="P79" s="41"/>
+      <c r="P79" s="20"/>
       <c r="Q79" s="41"/>
       <c r="R79" s="20"/>
       <c r="S79" s="35" t="s">
@@ -11487,11 +11504,11 @@
         <v>230</v>
       </c>
       <c r="U79" s="10" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="V79" s="10"/>
       <c r="W79" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="X79" s="1"/>
       <c r="Y79" s="1"/>
@@ -11499,7 +11516,7 @@
         <v>15</v>
       </c>
       <c r="AA79" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="AB79" s="25"/>
     </row>
@@ -11527,7 +11544,7 @@
       <c r="O80" s="20" t="s">
         <v>881</v>
       </c>
-      <c r="P80" s="41">
+      <c r="P80" s="20">
         <v>2</v>
       </c>
       <c r="Q80" s="41"/>
@@ -11585,7 +11602,7 @@
       <c r="M81" s="30"/>
       <c r="N81" s="17"/>
       <c r="O81" s="20"/>
-      <c r="P81" s="41"/>
+      <c r="P81" s="20"/>
       <c r="Q81" s="41"/>
       <c r="R81" s="20"/>
       <c r="S81" s="46" t="s">
@@ -11633,7 +11650,7 @@
       <c r="O82" s="20" t="s">
         <v>883</v>
       </c>
-      <c r="P82" s="41">
+      <c r="P82" s="20">
         <v>2</v>
       </c>
       <c r="Q82" s="41"/>
@@ -11685,7 +11702,7 @@
       <c r="O83" s="20" t="s">
         <v>884</v>
       </c>
-      <c r="P83" s="41">
+      <c r="P83" s="20">
         <v>2.5</v>
       </c>
       <c r="Q83" s="41"/>
@@ -11737,7 +11754,7 @@
       <c r="O84" s="20" t="s">
         <v>885</v>
       </c>
-      <c r="P84" s="41">
+      <c r="P84" s="20">
         <v>2</v>
       </c>
       <c r="Q84" s="41"/>
@@ -11795,7 +11812,7 @@
       <c r="M85" s="30"/>
       <c r="N85" s="17"/>
       <c r="O85" s="20"/>
-      <c r="P85" s="41"/>
+      <c r="P85" s="20"/>
       <c r="Q85" s="41"/>
       <c r="R85" s="20"/>
       <c r="S85" s="46" t="s">
@@ -11825,7 +11842,7 @@
       </c>
       <c r="B86" s="54"/>
       <c r="C86" s="54" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D86" s="25" t="s">
         <v>376</v>
@@ -11842,14 +11859,14 @@
       <c r="H86" s="60"/>
       <c r="I86" s="26"/>
       <c r="J86" s="47" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="K86" s="47"/>
       <c r="L86" s="27"/>
       <c r="M86" s="30"/>
       <c r="N86" s="17"/>
       <c r="O86" s="20"/>
-      <c r="P86" s="41"/>
+      <c r="P86" s="20"/>
       <c r="Q86" s="41"/>
       <c r="R86" s="20"/>
       <c r="S86" s="46" t="s">
@@ -11859,7 +11876,7 @@
         <v>230</v>
       </c>
       <c r="U86" s="16" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="V86" s="25"/>
       <c r="W86" s="25"/>
@@ -11869,7 +11886,7 @@
         <v>35</v>
       </c>
       <c r="AA86" s="25" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="AB86" s="48"/>
     </row>
@@ -11895,12 +11912,12 @@
       <c r="M87" s="30"/>
       <c r="N87" s="17"/>
       <c r="O87" s="20"/>
-      <c r="P87" s="41"/>
+      <c r="P87" s="20"/>
       <c r="Q87" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R87" s="20" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="S87" s="35" t="s">
         <v>235</v>
@@ -11924,7 +11941,7 @@
         <v>693</v>
       </c>
       <c r="AB87" s="25" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="88" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -11953,7 +11970,7 @@
       </c>
       <c r="N88" s="17"/>
       <c r="O88" s="20"/>
-      <c r="P88" s="41"/>
+      <c r="P88" s="20"/>
       <c r="Q88" s="41"/>
       <c r="R88" s="20"/>
       <c r="S88" s="46" t="s">
@@ -12003,7 +12020,7 @@
       </c>
       <c r="N89" s="17"/>
       <c r="O89" s="20"/>
-      <c r="P89" s="41"/>
+      <c r="P89" s="20"/>
       <c r="Q89" s="41"/>
       <c r="R89" s="20"/>
       <c r="S89" s="46" t="s">
@@ -12053,7 +12070,7 @@
       </c>
       <c r="N90" s="17"/>
       <c r="O90" s="20"/>
-      <c r="P90" s="41"/>
+      <c r="P90" s="20"/>
       <c r="Q90" s="41"/>
       <c r="R90" s="20"/>
       <c r="S90" s="46" t="s">
@@ -12103,7 +12120,7 @@
       </c>
       <c r="N91" s="17"/>
       <c r="O91" s="20"/>
-      <c r="P91" s="41"/>
+      <c r="P91" s="20"/>
       <c r="Q91" s="41"/>
       <c r="R91" s="20"/>
       <c r="S91" s="46" t="s">
@@ -12153,7 +12170,7 @@
       </c>
       <c r="N92" s="17"/>
       <c r="O92" s="20"/>
-      <c r="P92" s="41"/>
+      <c r="P92" s="20"/>
       <c r="Q92" s="41"/>
       <c r="R92" s="20"/>
       <c r="S92" s="46" t="s">
@@ -12203,7 +12220,7 @@
       </c>
       <c r="N93" s="17"/>
       <c r="O93" s="20"/>
-      <c r="P93" s="41"/>
+      <c r="P93" s="20"/>
       <c r="Q93" s="41"/>
       <c r="R93" s="20"/>
       <c r="S93" s="46" t="s">
@@ -12253,7 +12270,7 @@
       </c>
       <c r="N94" s="17"/>
       <c r="O94" s="20"/>
-      <c r="P94" s="41"/>
+      <c r="P94" s="20"/>
       <c r="Q94" s="41"/>
       <c r="R94" s="20"/>
       <c r="S94" s="46" t="s">
@@ -12303,7 +12320,7 @@
       </c>
       <c r="N95" s="17"/>
       <c r="O95" s="20"/>
-      <c r="P95" s="41"/>
+      <c r="P95" s="20"/>
       <c r="Q95" s="41"/>
       <c r="R95" s="20"/>
       <c r="S95" s="46" t="s">
@@ -12353,7 +12370,7 @@
       </c>
       <c r="N96" s="17"/>
       <c r="O96" s="20"/>
-      <c r="P96" s="41"/>
+      <c r="P96" s="20"/>
       <c r="Q96" s="41"/>
       <c r="R96" s="20"/>
       <c r="S96" s="46" t="s">
@@ -12403,7 +12420,7 @@
       </c>
       <c r="N97" s="17"/>
       <c r="O97" s="20"/>
-      <c r="P97" s="41"/>
+      <c r="P97" s="20"/>
       <c r="Q97" s="41"/>
       <c r="R97" s="20"/>
       <c r="S97" s="46" t="s">
@@ -12453,7 +12470,7 @@
       </c>
       <c r="N98" s="17"/>
       <c r="O98" s="20"/>
-      <c r="P98" s="41"/>
+      <c r="P98" s="20"/>
       <c r="Q98" s="41"/>
       <c r="R98" s="20"/>
       <c r="S98" s="46" t="s">
@@ -12503,7 +12520,7 @@
       </c>
       <c r="N99" s="17"/>
       <c r="O99" s="20"/>
-      <c r="P99" s="41"/>
+      <c r="P99" s="20"/>
       <c r="Q99" s="41"/>
       <c r="R99" s="20"/>
       <c r="S99" s="46" t="s">
@@ -12553,7 +12570,7 @@
       </c>
       <c r="N100" s="17"/>
       <c r="O100" s="20"/>
-      <c r="P100" s="41"/>
+      <c r="P100" s="20"/>
       <c r="Q100" s="41"/>
       <c r="R100" s="20"/>
       <c r="S100" s="46" t="s">
@@ -12603,7 +12620,7 @@
       </c>
       <c r="N101" s="17"/>
       <c r="O101" s="20"/>
-      <c r="P101" s="41"/>
+      <c r="P101" s="20"/>
       <c r="Q101" s="41"/>
       <c r="R101" s="20"/>
       <c r="S101" s="46" t="s">
@@ -12653,7 +12670,7 @@
       </c>
       <c r="N102" s="17"/>
       <c r="O102" s="20"/>
-      <c r="P102" s="41"/>
+      <c r="P102" s="20"/>
       <c r="Q102" s="41"/>
       <c r="R102" s="20"/>
       <c r="S102" s="25" t="s">
@@ -12703,7 +12720,7 @@
       </c>
       <c r="N103" s="17"/>
       <c r="O103" s="20"/>
-      <c r="P103" s="41"/>
+      <c r="P103" s="20"/>
       <c r="Q103" s="41"/>
       <c r="R103" s="20"/>
       <c r="S103" s="25" t="s">
@@ -12748,10 +12765,10 @@
       <c r="L104" s="18"/>
       <c r="M104" s="17"/>
       <c r="N104" s="17" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="O104" s="20"/>
-      <c r="P104" s="41"/>
+      <c r="P104" s="20"/>
       <c r="Q104" s="41"/>
       <c r="R104" s="20"/>
       <c r="S104" s="1" t="s">
@@ -12796,10 +12813,10 @@
       <c r="L105" s="18"/>
       <c r="M105" s="17"/>
       <c r="N105" s="17" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="O105" s="20"/>
-      <c r="P105" s="41"/>
+      <c r="P105" s="20"/>
       <c r="Q105" s="41"/>
       <c r="R105" s="20"/>
       <c r="S105" s="1" t="s">
@@ -12844,10 +12861,10 @@
       <c r="L106" s="18"/>
       <c r="M106" s="17"/>
       <c r="N106" s="17" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="O106" s="20"/>
-      <c r="P106" s="41"/>
+      <c r="P106" s="20"/>
       <c r="Q106" s="41"/>
       <c r="R106" s="20"/>
       <c r="S106" s="1" t="s">
@@ -12892,10 +12909,10 @@
       <c r="L107" s="18"/>
       <c r="M107" s="17"/>
       <c r="N107" s="17" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="O107" s="20"/>
-      <c r="P107" s="41"/>
+      <c r="P107" s="20"/>
       <c r="Q107" s="41"/>
       <c r="R107" s="20"/>
       <c r="S107" s="1" t="s">
@@ -12940,10 +12957,10 @@
       <c r="L108" s="18"/>
       <c r="M108" s="17"/>
       <c r="N108" s="17" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="O108" s="20"/>
-      <c r="P108" s="41"/>
+      <c r="P108" s="20"/>
       <c r="Q108" s="41"/>
       <c r="R108" s="20"/>
       <c r="S108" s="1" t="s">
@@ -12988,10 +13005,10 @@
       <c r="L109" s="18"/>
       <c r="M109" s="17"/>
       <c r="N109" s="17" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="O109" s="20"/>
-      <c r="P109" s="41"/>
+      <c r="P109" s="20"/>
       <c r="Q109" s="41"/>
       <c r="R109" s="20"/>
       <c r="S109" s="1" t="s">
@@ -13036,10 +13053,10 @@
       <c r="L110" s="18"/>
       <c r="M110" s="17"/>
       <c r="N110" s="17" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="O110" s="20"/>
-      <c r="P110" s="41"/>
+      <c r="P110" s="20"/>
       <c r="Q110" s="41"/>
       <c r="R110" s="20"/>
       <c r="S110" s="1" t="s">
@@ -13084,10 +13101,10 @@
       <c r="L111" s="18"/>
       <c r="M111" s="17"/>
       <c r="N111" s="17" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="O111" s="20"/>
-      <c r="P111" s="41"/>
+      <c r="P111" s="20"/>
       <c r="Q111" s="41"/>
       <c r="R111" s="20"/>
       <c r="S111" s="1" t="s">
@@ -13132,10 +13149,10 @@
       <c r="L112" s="18"/>
       <c r="M112" s="17"/>
       <c r="N112" s="17" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="O112" s="20"/>
-      <c r="P112" s="41"/>
+      <c r="P112" s="20"/>
       <c r="Q112" s="41"/>
       <c r="R112" s="20"/>
       <c r="S112" s="1" t="s">
@@ -13180,10 +13197,10 @@
       <c r="L113" s="18"/>
       <c r="M113" s="17"/>
       <c r="N113" s="17" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="O113" s="20"/>
-      <c r="P113" s="41"/>
+      <c r="P113" s="20"/>
       <c r="Q113" s="41"/>
       <c r="R113" s="20"/>
       <c r="S113" s="1" t="s">
@@ -13228,10 +13245,10 @@
       <c r="L114" s="18"/>
       <c r="M114" s="17"/>
       <c r="N114" s="17" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="O114" s="20"/>
-      <c r="P114" s="41"/>
+      <c r="P114" s="20"/>
       <c r="Q114" s="41"/>
       <c r="R114" s="20"/>
       <c r="S114" s="1" t="s">
@@ -13276,10 +13293,10 @@
       <c r="L115" s="18"/>
       <c r="M115" s="17"/>
       <c r="N115" s="17" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="O115" s="20"/>
-      <c r="P115" s="41"/>
+      <c r="P115" s="20"/>
       <c r="Q115" s="41"/>
       <c r="R115" s="20"/>
       <c r="S115" s="1" t="s">
@@ -13324,10 +13341,10 @@
       <c r="L116" s="18"/>
       <c r="M116" s="17"/>
       <c r="N116" s="17" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="O116" s="20"/>
-      <c r="P116" s="41"/>
+      <c r="P116" s="20"/>
       <c r="Q116" s="41"/>
       <c r="R116" s="20"/>
       <c r="S116" s="1" t="s">
@@ -13372,10 +13389,10 @@
       <c r="L117" s="18"/>
       <c r="M117" s="17"/>
       <c r="N117" s="17" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="O117" s="20"/>
-      <c r="P117" s="41"/>
+      <c r="P117" s="20"/>
       <c r="Q117" s="41"/>
       <c r="R117" s="20"/>
       <c r="S117" s="1" t="s">
@@ -13385,7 +13402,7 @@
         <v>230</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="V117" s="1"/>
       <c r="W117" s="1"/>
@@ -13420,10 +13437,10 @@
       <c r="L118" s="18"/>
       <c r="M118" s="17"/>
       <c r="N118" s="17" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="O118" s="20"/>
-      <c r="P118" s="41"/>
+      <c r="P118" s="20"/>
       <c r="Q118" s="41"/>
       <c r="R118" s="20"/>
       <c r="S118" s="1" t="s">
@@ -13468,10 +13485,10 @@
       <c r="L119" s="18"/>
       <c r="M119" s="17"/>
       <c r="N119" s="17" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="O119" s="20"/>
-      <c r="P119" s="41"/>
+      <c r="P119" s="20"/>
       <c r="Q119" s="41"/>
       <c r="R119" s="20"/>
       <c r="S119" s="1" t="s">
@@ -13516,10 +13533,10 @@
       <c r="L120" s="18"/>
       <c r="M120" s="17"/>
       <c r="N120" s="17" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="O120" s="20"/>
-      <c r="P120" s="41"/>
+      <c r="P120" s="20"/>
       <c r="Q120" s="41"/>
       <c r="R120" s="20"/>
       <c r="S120" s="1" t="s">
@@ -13560,14 +13577,14 @@
       <c r="H121" s="60"/>
       <c r="I121" s="28"/>
       <c r="J121" s="29" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="K121" s="29"/>
       <c r="L121" s="18"/>
       <c r="M121" s="17"/>
       <c r="N121" s="17"/>
       <c r="O121" s="20"/>
-      <c r="P121" s="41"/>
+      <c r="P121" s="20"/>
       <c r="Q121" s="41"/>
       <c r="R121" s="20"/>
       <c r="S121" s="1" t="s">
@@ -13612,14 +13629,14 @@
       <c r="H122" s="60"/>
       <c r="I122" s="28"/>
       <c r="J122" s="29" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="K122" s="29"/>
       <c r="L122" s="18"/>
       <c r="M122" s="17"/>
       <c r="N122" s="17"/>
       <c r="O122" s="20"/>
-      <c r="P122" s="41"/>
+      <c r="P122" s="20"/>
       <c r="Q122" s="41"/>
       <c r="R122" s="20"/>
       <c r="S122" s="1" t="s">
@@ -13664,14 +13681,14 @@
       <c r="H123" s="60"/>
       <c r="I123" s="28"/>
       <c r="J123" s="29" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="K123" s="29"/>
       <c r="L123" s="18"/>
       <c r="M123" s="17"/>
       <c r="N123" s="17"/>
       <c r="O123" s="20"/>
-      <c r="P123" s="41"/>
+      <c r="P123" s="20"/>
       <c r="Q123" s="41"/>
       <c r="R123" s="20"/>
       <c r="S123" s="1" t="s">
@@ -13716,14 +13733,14 @@
       <c r="H124" s="60"/>
       <c r="I124" s="28"/>
       <c r="J124" s="29" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="K124" s="29"/>
       <c r="L124" s="18"/>
       <c r="M124" s="17"/>
       <c r="N124" s="17"/>
       <c r="O124" s="20"/>
-      <c r="P124" s="41"/>
+      <c r="P124" s="20"/>
       <c r="Q124" s="41"/>
       <c r="R124" s="20"/>
       <c r="S124" s="1" t="s">
@@ -13768,14 +13785,14 @@
       <c r="H125" s="60"/>
       <c r="I125" s="28"/>
       <c r="J125" s="29" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="K125" s="29"/>
       <c r="L125" s="18"/>
       <c r="M125" s="17"/>
       <c r="N125" s="17"/>
       <c r="O125" s="20"/>
-      <c r="P125" s="41"/>
+      <c r="P125" s="20"/>
       <c r="Q125" s="41"/>
       <c r="R125" s="20"/>
       <c r="S125" s="1" t="s">
@@ -13820,14 +13837,14 @@
       <c r="H126" s="60"/>
       <c r="I126" s="28"/>
       <c r="J126" s="29" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="K126" s="29"/>
       <c r="L126" s="18"/>
       <c r="M126" s="17"/>
       <c r="N126" s="17"/>
       <c r="O126" s="20"/>
-      <c r="P126" s="41"/>
+      <c r="P126" s="20"/>
       <c r="Q126" s="41"/>
       <c r="R126" s="20"/>
       <c r="S126" s="1" t="s">
@@ -13872,14 +13889,14 @@
       <c r="H127" s="60"/>
       <c r="I127" s="28"/>
       <c r="J127" s="29" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="K127" s="29"/>
       <c r="L127" s="18"/>
       <c r="M127" s="17"/>
       <c r="N127" s="17"/>
       <c r="O127" s="20"/>
-      <c r="P127" s="41"/>
+      <c r="P127" s="20"/>
       <c r="Q127" s="41"/>
       <c r="R127" s="20"/>
       <c r="S127" s="1" t="s">
@@ -13924,14 +13941,14 @@
       <c r="H128" s="60"/>
       <c r="I128" s="28"/>
       <c r="J128" s="29" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="K128" s="29"/>
       <c r="L128" s="18"/>
       <c r="M128" s="17"/>
       <c r="N128" s="17"/>
       <c r="O128" s="20"/>
-      <c r="P128" s="41"/>
+      <c r="P128" s="20"/>
       <c r="Q128" s="41"/>
       <c r="R128" s="20"/>
       <c r="S128" s="1" t="s">
@@ -13976,14 +13993,14 @@
       <c r="H129" s="60"/>
       <c r="I129" s="28"/>
       <c r="J129" s="29" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="K129" s="29"/>
       <c r="L129" s="18"/>
       <c r="M129" s="17"/>
       <c r="N129" s="17"/>
       <c r="O129" s="20"/>
-      <c r="P129" s="41"/>
+      <c r="P129" s="20"/>
       <c r="Q129" s="41"/>
       <c r="R129" s="20"/>
       <c r="S129" s="1" t="s">
@@ -14028,14 +14045,14 @@
       <c r="H130" s="60"/>
       <c r="I130" s="28"/>
       <c r="J130" s="29" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="K130" s="29"/>
       <c r="L130" s="18"/>
       <c r="M130" s="17"/>
       <c r="N130" s="17"/>
       <c r="O130" s="20"/>
-      <c r="P130" s="41"/>
+      <c r="P130" s="20"/>
       <c r="Q130" s="41"/>
       <c r="R130" s="20"/>
       <c r="S130" s="1" t="s">
@@ -14080,14 +14097,14 @@
       <c r="H131" s="60"/>
       <c r="I131" s="28"/>
       <c r="J131" s="29" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="K131" s="29"/>
       <c r="L131" s="18"/>
       <c r="M131" s="17"/>
       <c r="N131" s="17"/>
       <c r="O131" s="20"/>
-      <c r="P131" s="41"/>
+      <c r="P131" s="20"/>
       <c r="Q131" s="41"/>
       <c r="R131" s="20"/>
       <c r="S131" s="1" t="s">
@@ -14132,14 +14149,14 @@
       <c r="H132" s="60"/>
       <c r="I132" s="28"/>
       <c r="J132" s="29" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="K132" s="29"/>
       <c r="L132" s="18"/>
       <c r="M132" s="17"/>
       <c r="N132" s="17"/>
       <c r="O132" s="20"/>
-      <c r="P132" s="41"/>
+      <c r="P132" s="20"/>
       <c r="Q132" s="41"/>
       <c r="R132" s="20"/>
       <c r="S132" s="1" t="s">
@@ -14184,14 +14201,14 @@
       <c r="H133" s="60"/>
       <c r="I133" s="28"/>
       <c r="J133" s="29" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="K133" s="29"/>
       <c r="L133" s="18"/>
       <c r="M133" s="17"/>
       <c r="N133" s="17"/>
       <c r="O133" s="20"/>
-      <c r="P133" s="41"/>
+      <c r="P133" s="20"/>
       <c r="Q133" s="41"/>
       <c r="R133" s="20"/>
       <c r="S133" s="1" t="s">
@@ -14236,14 +14253,14 @@
       <c r="H134" s="60"/>
       <c r="I134" s="28"/>
       <c r="J134" s="29" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="K134" s="29"/>
       <c r="L134" s="18"/>
       <c r="M134" s="17"/>
       <c r="N134" s="17"/>
       <c r="O134" s="20"/>
-      <c r="P134" s="41"/>
+      <c r="P134" s="20"/>
       <c r="Q134" s="41"/>
       <c r="R134" s="20"/>
       <c r="S134" s="1" t="s">
@@ -14288,14 +14305,14 @@
       <c r="H135" s="60"/>
       <c r="I135" s="28"/>
       <c r="J135" s="29" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="K135" s="29"/>
       <c r="L135" s="18"/>
       <c r="M135" s="17"/>
       <c r="N135" s="17"/>
       <c r="O135" s="20"/>
-      <c r="P135" s="41"/>
+      <c r="P135" s="20"/>
       <c r="Q135" s="41"/>
       <c r="R135" s="20"/>
       <c r="S135" s="1" t="s">
@@ -14329,7 +14346,7 @@
       </c>
       <c r="B136" s="84"/>
       <c r="C136" s="58" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>44</v>
@@ -14340,14 +14357,14 @@
       <c r="H136" s="60"/>
       <c r="I136" s="28"/>
       <c r="J136" s="29" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="K136" s="29"/>
       <c r="L136" s="18"/>
       <c r="M136" s="17"/>
       <c r="N136" s="17"/>
       <c r="O136" s="20"/>
-      <c r="P136" s="41"/>
+      <c r="P136" s="20"/>
       <c r="Q136" s="41"/>
       <c r="R136" s="20"/>
       <c r="S136" s="1" t="s">
@@ -14357,7 +14374,7 @@
         <v>230</v>
       </c>
       <c r="U136" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="V136" s="10">
         <v>56000102</v>
@@ -14371,7 +14388,7 @@
         <v>20</v>
       </c>
       <c r="AA136" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="AB136" s="39"/>
     </row>
@@ -14399,7 +14416,7 @@
       <c r="M137" s="17"/>
       <c r="N137" s="17"/>
       <c r="O137" s="20"/>
-      <c r="P137" s="41"/>
+      <c r="P137" s="20"/>
       <c r="Q137" s="41"/>
       <c r="R137" s="20"/>
       <c r="S137" s="1" t="s">
@@ -14449,7 +14466,7 @@
       </c>
       <c r="N138" s="17"/>
       <c r="O138" s="20"/>
-      <c r="P138" s="41"/>
+      <c r="P138" s="20"/>
       <c r="Q138" s="41"/>
       <c r="R138" s="20"/>
       <c r="S138" s="10" t="s">
@@ -14499,7 +14516,7 @@
       </c>
       <c r="N139" s="17"/>
       <c r="O139" s="20"/>
-      <c r="P139" s="41"/>
+      <c r="P139" s="20"/>
       <c r="Q139" s="41"/>
       <c r="R139" s="20"/>
       <c r="S139" s="10" t="s">
@@ -14549,7 +14566,7 @@
       </c>
       <c r="N140" s="17"/>
       <c r="O140" s="20"/>
-      <c r="P140" s="41"/>
+      <c r="P140" s="20"/>
       <c r="Q140" s="41"/>
       <c r="R140" s="20"/>
       <c r="S140" s="10" t="s">
@@ -14594,10 +14611,10 @@
       <c r="L141" s="18"/>
       <c r="M141" s="17"/>
       <c r="N141" s="17" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="O141" s="20"/>
-      <c r="P141" s="41"/>
+      <c r="P141" s="20"/>
       <c r="Q141" s="41"/>
       <c r="R141" s="20"/>
       <c r="S141" s="25" t="s">
@@ -14642,10 +14659,10 @@
       <c r="L142" s="18"/>
       <c r="M142" s="17"/>
       <c r="N142" s="17" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="O142" s="20"/>
-      <c r="P142" s="41"/>
+      <c r="P142" s="20"/>
       <c r="Q142" s="41"/>
       <c r="R142" s="20"/>
       <c r="S142" s="1" t="s">
@@ -14690,10 +14707,10 @@
       <c r="L143" s="18"/>
       <c r="M143" s="17"/>
       <c r="N143" s="17" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="O143" s="20"/>
-      <c r="P143" s="41"/>
+      <c r="P143" s="20"/>
       <c r="Q143" s="41"/>
       <c r="R143" s="20"/>
       <c r="S143" s="1" t="s">
@@ -14742,14 +14759,14 @@
       <c r="H144" s="60"/>
       <c r="I144" s="26"/>
       <c r="J144" s="47" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="K144" s="47"/>
       <c r="L144" s="27"/>
       <c r="M144" s="30"/>
       <c r="N144" s="17"/>
       <c r="O144" s="20"/>
-      <c r="P144" s="41"/>
+      <c r="P144" s="20"/>
       <c r="Q144" s="41"/>
       <c r="R144" s="20"/>
       <c r="S144" s="35" t="s">
@@ -14799,9 +14816,9 @@
       <c r="M145" s="30"/>
       <c r="N145" s="17"/>
       <c r="O145" s="20" t="s">
-        <v>1101</v>
-      </c>
-      <c r="P145" s="41">
+        <v>1100</v>
+      </c>
+      <c r="P145" s="20">
         <v>1</v>
       </c>
       <c r="Q145" s="41"/>
@@ -14849,9 +14866,9 @@
       <c r="M146" s="30"/>
       <c r="N146" s="17"/>
       <c r="O146" s="20" t="s">
-        <v>1102</v>
-      </c>
-      <c r="P146" s="41">
+        <v>1101</v>
+      </c>
+      <c r="P146" s="20">
         <v>1</v>
       </c>
       <c r="Q146" s="41"/>
@@ -14899,12 +14916,12 @@
       <c r="M147" s="30"/>
       <c r="N147" s="17"/>
       <c r="O147" s="20"/>
-      <c r="P147" s="41"/>
+      <c r="P147" s="20"/>
       <c r="Q147" s="41" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="R147" s="20" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="S147" s="46" t="s">
         <v>235</v>
@@ -14952,14 +14969,14 @@
       <c r="H148" s="60"/>
       <c r="I148" s="26"/>
       <c r="J148" s="47" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="K148" s="47"/>
       <c r="L148" s="27"/>
       <c r="M148" s="30"/>
       <c r="N148" s="17"/>
       <c r="O148" s="20"/>
-      <c r="P148" s="41"/>
+      <c r="P148" s="20"/>
       <c r="Q148" s="41"/>
       <c r="R148" s="20"/>
       <c r="S148" s="46" t="s">
@@ -15012,14 +15029,14 @@
       <c r="H149" s="60"/>
       <c r="I149" s="26"/>
       <c r="J149" s="47" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="K149" s="47"/>
       <c r="L149" s="27"/>
       <c r="M149" s="30"/>
       <c r="N149" s="17"/>
       <c r="O149" s="20"/>
-      <c r="P149" s="41"/>
+      <c r="P149" s="20"/>
       <c r="Q149" s="41"/>
       <c r="R149" s="20"/>
       <c r="S149" s="46" t="s">
@@ -15062,14 +15079,14 @@
       <c r="H150" s="60"/>
       <c r="I150" s="26"/>
       <c r="J150" s="47" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="K150" s="47"/>
       <c r="L150" s="27"/>
       <c r="M150" s="30"/>
       <c r="N150" s="17"/>
       <c r="O150" s="20"/>
-      <c r="P150" s="41"/>
+      <c r="P150" s="20"/>
       <c r="Q150" s="41"/>
       <c r="R150" s="20"/>
       <c r="S150" s="46" t="s">
@@ -15114,10 +15131,10 @@
       <c r="L151" s="27"/>
       <c r="M151" s="30"/>
       <c r="N151" s="17" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="O151" s="20"/>
-      <c r="P151" s="41"/>
+      <c r="P151" s="20"/>
       <c r="Q151" s="41"/>
       <c r="R151" s="20"/>
       <c r="S151" s="25" t="s">
@@ -15127,7 +15144,7 @@
         <v>230</v>
       </c>
       <c r="U151" s="16" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="V151" s="25"/>
       <c r="W151" s="25" t="s">
@@ -15139,10 +15156,10 @@
         <v>15</v>
       </c>
       <c r="AA151" s="25" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AB151" s="48" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="152" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -15166,10 +15183,10 @@
       <c r="L152" s="18"/>
       <c r="M152" s="17"/>
       <c r="N152" s="17" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="O152" s="20"/>
-      <c r="P152" s="41"/>
+      <c r="P152" s="20"/>
       <c r="Q152" s="41"/>
       <c r="R152" s="20"/>
       <c r="S152" s="25" t="s">
@@ -15192,7 +15209,7 @@
         <v>162</v>
       </c>
       <c r="AB152" s="48" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="153" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -15221,7 +15238,7 @@
         <v>872</v>
       </c>
       <c r="O153" s="20"/>
-      <c r="P153" s="41"/>
+      <c r="P153" s="20"/>
       <c r="Q153" s="41"/>
       <c r="R153" s="20"/>
       <c r="S153" s="1" t="s">
@@ -15269,7 +15286,7 @@
         <v>873</v>
       </c>
       <c r="O154" s="20"/>
-      <c r="P154" s="41"/>
+      <c r="P154" s="20"/>
       <c r="Q154" s="41"/>
       <c r="R154" s="20"/>
       <c r="S154" s="1" t="s">
@@ -15317,7 +15334,7 @@
         <v>916</v>
       </c>
       <c r="O155" s="20"/>
-      <c r="P155" s="41"/>
+      <c r="P155" s="20"/>
       <c r="Q155" s="41"/>
       <c r="R155" s="20"/>
       <c r="S155" s="1" t="s">
@@ -15365,7 +15382,7 @@
       <c r="M156" s="17"/>
       <c r="N156" s="17"/>
       <c r="O156" s="20"/>
-      <c r="P156" s="41"/>
+      <c r="P156" s="20"/>
       <c r="Q156" s="41"/>
       <c r="R156" s="20"/>
       <c r="S156" s="1" t="s">
@@ -15388,7 +15405,7 @@
         <v>547</v>
       </c>
       <c r="AB156" s="37" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="157" spans="1:28" x14ac:dyDescent="0.15">
@@ -15415,7 +15432,7 @@
       <c r="M157" s="17"/>
       <c r="N157" s="17"/>
       <c r="O157" s="20"/>
-      <c r="P157" s="41"/>
+      <c r="P157" s="20"/>
       <c r="Q157" s="41"/>
       <c r="R157" s="20"/>
       <c r="S157" s="1" t="s">
@@ -15438,7 +15455,7 @@
         <v>199</v>
       </c>
       <c r="AB157" s="37" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="158" spans="1:28" ht="72" x14ac:dyDescent="0.15">
@@ -15458,14 +15475,14 @@
       <c r="H158" s="60"/>
       <c r="I158" s="26"/>
       <c r="J158" s="47" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="K158" s="47"/>
       <c r="L158" s="27"/>
       <c r="M158" s="30"/>
       <c r="N158" s="17"/>
       <c r="O158" s="20"/>
-      <c r="P158" s="41"/>
+      <c r="P158" s="20"/>
       <c r="Q158" s="41"/>
       <c r="R158" s="20"/>
       <c r="S158" s="35" t="s">
@@ -15488,7 +15505,7 @@
         <v>40</v>
       </c>
       <c r="AB158" s="37" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="159" spans="1:28" ht="72" x14ac:dyDescent="0.15">
@@ -15514,14 +15531,14 @@
       <c r="H159" s="60"/>
       <c r="I159" s="28"/>
       <c r="J159" s="29" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="K159" s="29"/>
       <c r="L159" s="18"/>
       <c r="M159" s="17"/>
       <c r="N159" s="17"/>
       <c r="O159" s="20"/>
-      <c r="P159" s="41"/>
+      <c r="P159" s="20"/>
       <c r="Q159" s="41"/>
       <c r="R159" s="20"/>
       <c r="S159" s="25" t="s">
@@ -15546,7 +15563,7 @@
         <v>41</v>
       </c>
       <c r="AB159" s="37" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="160" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -15575,7 +15592,7 @@
       </c>
       <c r="N160" s="17"/>
       <c r="O160" s="20"/>
-      <c r="P160" s="41"/>
+      <c r="P160" s="20"/>
       <c r="Q160" s="41"/>
       <c r="R160" s="20"/>
       <c r="S160" s="1" t="s">
@@ -15615,7 +15632,7 @@
       <c r="G161" s="43"/>
       <c r="H161" s="60"/>
       <c r="I161" s="28" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="J161" s="29"/>
       <c r="K161" s="29"/>
@@ -15623,12 +15640,12 @@
       <c r="M161" s="17"/>
       <c r="N161" s="17"/>
       <c r="O161" s="20"/>
-      <c r="P161" s="41"/>
+      <c r="P161" s="20"/>
       <c r="Q161" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R161" s="20" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="S161" s="46" t="s">
         <v>235</v>
@@ -15650,7 +15667,7 @@
         <v>66</v>
       </c>
       <c r="AB161" s="37" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="162" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -15677,7 +15694,7 @@
       <c r="M162" s="17"/>
       <c r="N162" s="17"/>
       <c r="O162" s="20"/>
-      <c r="P162" s="41"/>
+      <c r="P162" s="20"/>
       <c r="Q162" s="41"/>
       <c r="R162" s="20"/>
       <c r="S162" s="1" t="s">
@@ -15727,7 +15744,7 @@
       <c r="O163" s="20" t="s">
         <v>380</v>
       </c>
-      <c r="P163" s="41">
+      <c r="P163" s="20">
         <v>5</v>
       </c>
       <c r="Q163" s="41"/>
@@ -15739,7 +15756,7 @@
         <v>230</v>
       </c>
       <c r="U163" s="10" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="V163" s="10"/>
       <c r="W163" s="1" t="s">
@@ -15754,7 +15771,7 @@
         <v>570</v>
       </c>
       <c r="AB163" s="48" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="164" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -15781,7 +15798,7 @@
       <c r="O164" s="20" t="s">
         <v>870</v>
       </c>
-      <c r="P164" s="41">
+      <c r="P164" s="20">
         <v>1</v>
       </c>
       <c r="Q164" s="41"/>
@@ -15833,9 +15850,9 @@
       <c r="M165" s="17"/>
       <c r="N165" s="21"/>
       <c r="O165" s="19" t="s">
-        <v>998</v>
-      </c>
-      <c r="P165" s="41">
+        <v>997</v>
+      </c>
+      <c r="P165" s="20">
         <v>1</v>
       </c>
       <c r="Q165" s="41"/>
@@ -15889,7 +15906,7 @@
       <c r="O166" s="20" t="s">
         <v>871</v>
       </c>
-      <c r="P166" s="41">
+      <c r="P166" s="20">
         <v>1</v>
       </c>
       <c r="Q166" s="41"/>
@@ -15936,14 +15953,14 @@
       <c r="H167" s="78"/>
       <c r="I167" s="96"/>
       <c r="J167" s="29" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="K167" s="95"/>
       <c r="L167" s="97"/>
       <c r="M167" s="79"/>
       <c r="N167" s="79"/>
       <c r="O167" s="80"/>
-      <c r="P167" s="81"/>
+      <c r="P167" s="80"/>
       <c r="Q167" s="81"/>
       <c r="R167" s="20"/>
       <c r="S167" s="77" t="s">
@@ -15966,7 +15983,7 @@
         <v>579</v>
       </c>
       <c r="AB167" s="48" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="168" spans="1:28" x14ac:dyDescent="0.15">
@@ -15993,7 +16010,7 @@
       <c r="O168" s="20" t="s">
         <v>875</v>
       </c>
-      <c r="P168" s="41">
+      <c r="P168" s="20">
         <v>1</v>
       </c>
       <c r="Q168" s="41"/>
@@ -16042,14 +16059,14 @@
       <c r="H169" s="60"/>
       <c r="I169" s="26"/>
       <c r="J169" s="82" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="K169" s="47"/>
       <c r="L169" s="27"/>
       <c r="M169" s="30"/>
       <c r="N169" s="17"/>
       <c r="O169" s="20"/>
-      <c r="P169" s="41"/>
+      <c r="P169" s="20"/>
       <c r="Q169" s="41"/>
       <c r="R169" s="20"/>
       <c r="S169" s="46" t="s">
@@ -16076,7 +16093,7 @@
         <v>205</v>
       </c>
       <c r="AB169" s="48" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="170" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -16096,14 +16113,14 @@
       <c r="H170" s="60"/>
       <c r="I170" s="26"/>
       <c r="J170" s="82" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="K170" s="47"/>
       <c r="L170" s="27"/>
       <c r="M170" s="30"/>
       <c r="N170" s="17"/>
       <c r="O170" s="20"/>
-      <c r="P170" s="41"/>
+      <c r="P170" s="20"/>
       <c r="Q170" s="41"/>
       <c r="R170" s="20"/>
       <c r="S170" s="46" t="s">
@@ -16150,14 +16167,14 @@
       <c r="H171" s="60"/>
       <c r="I171" s="26"/>
       <c r="J171" s="29" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="K171" s="29"/>
       <c r="L171" s="27"/>
       <c r="M171" s="30"/>
       <c r="N171" s="17"/>
       <c r="O171" s="20"/>
-      <c r="P171" s="41"/>
+      <c r="P171" s="20"/>
       <c r="Q171" s="41"/>
       <c r="R171" s="20"/>
       <c r="S171" s="46" t="s">
@@ -16180,7 +16197,7 @@
         <v>120</v>
       </c>
       <c r="AB171" s="48" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="172" spans="1:28" ht="84" x14ac:dyDescent="0.15">
@@ -16211,9 +16228,9 @@
       <c r="M172" s="30"/>
       <c r="N172" s="17"/>
       <c r="O172" s="20" t="s">
-        <v>1036</v>
-      </c>
-      <c r="P172" s="41">
+        <v>1035</v>
+      </c>
+      <c r="P172" s="20">
         <v>2</v>
       </c>
       <c r="Q172" s="41"/>
@@ -16264,10 +16281,10 @@
       <c r="L173" s="27"/>
       <c r="M173" s="30"/>
       <c r="N173" s="17" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="O173" s="20"/>
-      <c r="P173" s="41"/>
+      <c r="P173" s="20"/>
       <c r="Q173" s="41"/>
       <c r="R173" s="20"/>
       <c r="S173" s="46" t="s">
@@ -16319,7 +16336,7 @@
         <v>877</v>
       </c>
       <c r="O174" s="20"/>
-      <c r="P174" s="41"/>
+      <c r="P174" s="20"/>
       <c r="Q174" s="41"/>
       <c r="R174" s="20"/>
       <c r="S174" s="46" t="s">
@@ -16342,7 +16359,7 @@
         <v>121</v>
       </c>
       <c r="AB174" s="48" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="175" spans="1:28" ht="48" x14ac:dyDescent="0.15">
@@ -16362,14 +16379,14 @@
       <c r="H175" s="60"/>
       <c r="I175" s="26"/>
       <c r="J175" s="82" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="K175" s="47"/>
       <c r="L175" s="27"/>
       <c r="M175" s="30"/>
       <c r="N175" s="17"/>
       <c r="O175" s="20"/>
-      <c r="P175" s="41"/>
+      <c r="P175" s="20"/>
       <c r="Q175" s="41"/>
       <c r="R175" s="20"/>
       <c r="S175" s="46" t="s">
@@ -16390,7 +16407,7 @@
         <v>210</v>
       </c>
       <c r="AB175" s="48" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="176" spans="1:28" ht="84" x14ac:dyDescent="0.15">
@@ -16410,14 +16427,14 @@
       <c r="H176" s="60"/>
       <c r="I176" s="26"/>
       <c r="J176" s="82" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="K176" s="47"/>
       <c r="L176" s="27"/>
       <c r="M176" s="30"/>
       <c r="N176" s="17"/>
       <c r="O176" s="20"/>
-      <c r="P176" s="41"/>
+      <c r="P176" s="20"/>
       <c r="Q176" s="41"/>
       <c r="R176" s="20"/>
       <c r="S176" s="46" t="s">
@@ -16427,7 +16444,7 @@
         <v>359</v>
       </c>
       <c r="U176" s="16" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="V176" s="25"/>
       <c r="W176" s="25"/>
@@ -16457,17 +16474,17 @@
       <c r="G177" s="25"/>
       <c r="H177" s="60"/>
       <c r="I177" s="26" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="J177" s="82"/>
       <c r="K177" s="47"/>
       <c r="L177" s="18" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="M177" s="30"/>
       <c r="N177" s="17"/>
       <c r="O177" s="20"/>
-      <c r="P177" s="41"/>
+      <c r="P177" s="20"/>
       <c r="Q177" s="41"/>
       <c r="R177" s="20"/>
       <c r="S177" s="46" t="s">
@@ -16477,7 +16494,7 @@
         <v>359</v>
       </c>
       <c r="U177" s="15" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="V177" s="25"/>
       <c r="W177" s="25"/>
@@ -16490,7 +16507,7 @@
         <v>196</v>
       </c>
       <c r="AB177" s="48" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="178" spans="1:28" x14ac:dyDescent="0.15">
@@ -16517,7 +16534,7 @@
       <c r="M178" s="30"/>
       <c r="N178" s="17"/>
       <c r="O178" s="20"/>
-      <c r="P178" s="41"/>
+      <c r="P178" s="20"/>
       <c r="Q178" s="41"/>
       <c r="R178" s="20"/>
       <c r="S178" s="46" t="s">
@@ -16564,14 +16581,14 @@
       <c r="H179" s="60"/>
       <c r="I179" s="26"/>
       <c r="J179" s="90" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="K179" s="29"/>
       <c r="L179" s="27"/>
       <c r="M179" s="30"/>
       <c r="N179" s="17"/>
       <c r="O179" s="20"/>
-      <c r="P179" s="41"/>
+      <c r="P179" s="20"/>
       <c r="Q179" s="41"/>
       <c r="R179" s="20"/>
       <c r="S179" s="46" t="s">
@@ -16596,7 +16613,7 @@
         <v>674</v>
       </c>
       <c r="AB179" s="48" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="180" spans="1:28" ht="27" x14ac:dyDescent="0.15">
@@ -16625,7 +16642,7 @@
       </c>
       <c r="N180" s="17"/>
       <c r="O180" s="20"/>
-      <c r="P180" s="41"/>
+      <c r="P180" s="20"/>
       <c r="Q180" s="41"/>
       <c r="R180" s="20"/>
       <c r="S180" s="46" t="s">
@@ -16671,12 +16688,12 @@
       <c r="M181" s="30"/>
       <c r="N181" s="17"/>
       <c r="O181" s="20"/>
-      <c r="P181" s="41"/>
+      <c r="P181" s="20"/>
       <c r="Q181" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R181" s="20" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="S181" s="46" t="s">
         <v>235</v>
@@ -16698,7 +16715,7 @@
         <v>695</v>
       </c>
       <c r="AB181" s="48" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="182" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -16725,7 +16742,7 @@
       <c r="M182" s="30"/>
       <c r="N182" s="17"/>
       <c r="O182" s="20"/>
-      <c r="P182" s="41"/>
+      <c r="P182" s="20"/>
       <c r="Q182" s="41"/>
       <c r="R182" s="20"/>
       <c r="S182" s="46" t="s">
@@ -16748,7 +16765,7 @@
         <v>706</v>
       </c>
       <c r="AB182" s="48" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="183" spans="1:28" ht="84" x14ac:dyDescent="0.15">
@@ -16774,14 +16791,14 @@
       <c r="H183" s="60"/>
       <c r="I183" s="26"/>
       <c r="J183" s="90" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="K183" s="29"/>
       <c r="L183" s="27"/>
       <c r="M183" s="30"/>
       <c r="N183" s="17"/>
       <c r="O183" s="20"/>
-      <c r="P183" s="41"/>
+      <c r="P183" s="20"/>
       <c r="Q183" s="41"/>
       <c r="R183" s="20"/>
       <c r="S183" s="46" t="s">
@@ -16830,14 +16847,14 @@
       <c r="H184" s="60"/>
       <c r="I184" s="26"/>
       <c r="J184" s="29" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="K184" s="29"/>
       <c r="L184" s="27"/>
       <c r="M184" s="30"/>
       <c r="N184" s="17"/>
       <c r="O184" s="20"/>
-      <c r="P184" s="41"/>
+      <c r="P184" s="20"/>
       <c r="Q184" s="41"/>
       <c r="R184" s="20"/>
       <c r="S184" s="46" t="s">
@@ -16860,7 +16877,7 @@
         <v>724</v>
       </c>
       <c r="AB184" s="48" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="185" spans="1:28" ht="84" x14ac:dyDescent="0.15">
@@ -16886,14 +16903,14 @@
       <c r="H185" s="60"/>
       <c r="I185" s="26"/>
       <c r="J185" s="29" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="K185" s="29"/>
       <c r="L185" s="27"/>
       <c r="M185" s="30"/>
       <c r="N185" s="17"/>
       <c r="O185" s="20"/>
-      <c r="P185" s="41"/>
+      <c r="P185" s="20"/>
       <c r="Q185" s="41"/>
       <c r="R185" s="20"/>
       <c r="S185" s="46" t="s">
@@ -16920,7 +16937,7 @@
         <v>729</v>
       </c>
       <c r="AB185" s="48" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="186" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -16949,11 +16966,11 @@
       <c r="M186" s="17"/>
       <c r="N186" s="17"/>
       <c r="O186" s="20"/>
-      <c r="P186" s="41"/>
+      <c r="P186" s="20"/>
       <c r="Q186" s="41"/>
       <c r="R186" s="20"/>
       <c r="S186" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="T186" s="9" t="s">
         <v>230</v>
@@ -16974,7 +16991,7 @@
         <v>732</v>
       </c>
       <c r="AB186" s="37" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="187" spans="1:28" ht="72" x14ac:dyDescent="0.15">
@@ -17007,7 +17024,7 @@
       <c r="M187" s="30"/>
       <c r="N187" s="17"/>
       <c r="O187" s="20"/>
-      <c r="P187" s="41"/>
+      <c r="P187" s="20"/>
       <c r="Q187" s="41"/>
       <c r="R187" s="20"/>
       <c r="S187" s="46" t="s">
@@ -17034,7 +17051,7 @@
         <v>741</v>
       </c>
       <c r="AB187" s="48" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="188" spans="1:28" ht="72" x14ac:dyDescent="0.15">
@@ -17067,7 +17084,7 @@
       <c r="M188" s="30"/>
       <c r="N188" s="17"/>
       <c r="O188" s="20"/>
-      <c r="P188" s="41"/>
+      <c r="P188" s="20"/>
       <c r="Q188" s="41"/>
       <c r="R188" s="20"/>
       <c r="S188" s="46" t="s">
@@ -17092,7 +17109,7 @@
         <v>746</v>
       </c>
       <c r="AB188" s="48" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="189" spans="1:28" ht="72" x14ac:dyDescent="0.15">
@@ -17117,12 +17134,12 @@
       <c r="M189" s="30"/>
       <c r="N189" s="17"/>
       <c r="O189" s="20"/>
-      <c r="P189" s="41"/>
+      <c r="P189" s="20"/>
       <c r="Q189" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R189" s="20" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="S189" s="46" t="s">
         <v>235</v>
@@ -17144,7 +17161,7 @@
         <v>750</v>
       </c>
       <c r="AB189" s="48" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="190" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -17171,7 +17188,7 @@
       <c r="O190" s="20" t="s">
         <v>890</v>
       </c>
-      <c r="P190" s="41">
+      <c r="P190" s="20">
         <v>1</v>
       </c>
       <c r="Q190" s="41"/>
@@ -17196,7 +17213,7 @@
         <v>752</v>
       </c>
       <c r="AB190" s="48" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="191" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -17221,9 +17238,9 @@
       <c r="M191" s="30"/>
       <c r="N191" s="17"/>
       <c r="O191" s="20" t="s">
-        <v>1120</v>
-      </c>
-      <c r="P191" s="41">
+        <v>1119</v>
+      </c>
+      <c r="P191" s="20">
         <v>2</v>
       </c>
       <c r="Q191" s="41"/>
@@ -17245,10 +17262,10 @@
         <v>40</v>
       </c>
       <c r="AA191" s="25" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="AB191" s="48" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="192" spans="1:28" ht="96" x14ac:dyDescent="0.15">
@@ -17274,14 +17291,14 @@
       <c r="H192" s="60"/>
       <c r="I192" s="26"/>
       <c r="J192" s="90" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="K192" s="29"/>
       <c r="L192" s="27"/>
       <c r="M192" s="30"/>
       <c r="N192" s="17"/>
       <c r="O192" s="20"/>
-      <c r="P192" s="41"/>
+      <c r="P192" s="20"/>
       <c r="Q192" s="41"/>
       <c r="R192" s="20"/>
       <c r="S192" s="46" t="s">
@@ -17304,7 +17321,7 @@
         <v>756</v>
       </c>
       <c r="AB192" s="48" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="193" spans="1:28" ht="84" x14ac:dyDescent="0.15">
@@ -17330,14 +17347,14 @@
       <c r="H193" s="60"/>
       <c r="I193" s="26"/>
       <c r="J193" s="90" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="K193" s="29"/>
       <c r="L193" s="27"/>
       <c r="M193" s="30"/>
       <c r="N193" s="17"/>
       <c r="O193" s="20"/>
-      <c r="P193" s="41"/>
+      <c r="P193" s="20"/>
       <c r="Q193" s="41"/>
       <c r="R193" s="20"/>
       <c r="S193" s="46" t="s">
@@ -17347,14 +17364,14 @@
         <v>359</v>
       </c>
       <c r="U193" s="16" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="V193" s="25"/>
       <c r="W193" s="25" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="X193" s="25" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="Y193" s="25"/>
       <c r="Z193" s="25">
@@ -17388,14 +17405,14 @@
       <c r="H194" s="60"/>
       <c r="I194" s="26"/>
       <c r="J194" s="90" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="K194" s="29"/>
       <c r="L194" s="27"/>
       <c r="M194" s="30"/>
       <c r="N194" s="17"/>
       <c r="O194" s="20"/>
-      <c r="P194" s="41"/>
+      <c r="P194" s="20"/>
       <c r="Q194" s="41"/>
       <c r="R194" s="20"/>
       <c r="S194" s="46" t="s">
@@ -17429,7 +17446,7 @@
       </c>
       <c r="B195" s="55"/>
       <c r="C195" s="55" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D195" s="25" t="s">
         <v>306</v>
@@ -17444,10 +17461,10 @@
       <c r="L195" s="18"/>
       <c r="M195" s="17"/>
       <c r="N195" s="17" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="O195" s="20"/>
-      <c r="P195" s="41"/>
+      <c r="P195" s="20"/>
       <c r="Q195" s="41"/>
       <c r="R195" s="20"/>
       <c r="S195" s="1" t="s">
@@ -17457,7 +17474,7 @@
         <v>230</v>
       </c>
       <c r="U195" s="10" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="V195" s="10"/>
       <c r="W195" s="1"/>
@@ -17492,14 +17509,14 @@
       <c r="J196" s="29"/>
       <c r="K196" s="29"/>
       <c r="L196" s="18" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="M196" s="17" t="s">
         <v>782</v>
       </c>
       <c r="N196" s="17"/>
       <c r="O196" s="20"/>
-      <c r="P196" s="41"/>
+      <c r="P196" s="20"/>
       <c r="Q196" s="41"/>
       <c r="R196" s="20"/>
       <c r="S196" s="46" t="s">
@@ -17549,7 +17566,7 @@
         <v>878</v>
       </c>
       <c r="O197" s="20"/>
-      <c r="P197" s="41"/>
+      <c r="P197" s="20"/>
       <c r="Q197" s="41"/>
       <c r="R197" s="20"/>
       <c r="S197" s="46" t="s">
@@ -17572,7 +17589,7 @@
         <v>795</v>
       </c>
       <c r="AB197" s="48" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="198" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -17599,7 +17616,7 @@
       <c r="M198" s="66"/>
       <c r="N198" s="67"/>
       <c r="O198" s="68"/>
-      <c r="P198" s="69"/>
+      <c r="P198" s="68"/>
       <c r="Q198" s="69"/>
       <c r="R198" s="20"/>
       <c r="S198" s="46" t="s">
@@ -17609,7 +17626,7 @@
         <v>230</v>
       </c>
       <c r="U198" s="10" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="V198" s="10"/>
       <c r="W198" s="61"/>
@@ -17622,7 +17639,7 @@
         <v>797</v>
       </c>
       <c r="AB198" s="48" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="199" spans="1:28" ht="96" x14ac:dyDescent="0.15">
@@ -17648,14 +17665,14 @@
       <c r="H199" s="60"/>
       <c r="I199" s="26"/>
       <c r="J199" s="90" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="K199" s="29"/>
       <c r="L199" s="27"/>
       <c r="M199" s="30"/>
       <c r="N199" s="17"/>
       <c r="O199" s="20"/>
-      <c r="P199" s="41"/>
+      <c r="P199" s="20"/>
       <c r="Q199" s="41"/>
       <c r="R199" s="20"/>
       <c r="S199" s="46" t="s">
@@ -17678,7 +17695,7 @@
         <v>806</v>
       </c>
       <c r="AB199" s="48" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="200" spans="1:28" ht="96" x14ac:dyDescent="0.15">
@@ -17709,9 +17726,9 @@
       <c r="M200" s="30"/>
       <c r="N200" s="17"/>
       <c r="O200" s="20" t="s">
-        <v>1091</v>
-      </c>
-      <c r="P200" s="41">
+        <v>1090</v>
+      </c>
+      <c r="P200" s="20">
         <v>1</v>
       </c>
       <c r="Q200" s="41"/>
@@ -17723,7 +17740,7 @@
         <v>359</v>
       </c>
       <c r="U200" s="10" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="V200" s="25"/>
       <c r="W200" s="25"/>
@@ -17736,7 +17753,7 @@
         <v>811</v>
       </c>
       <c r="AB200" s="48" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="201" spans="1:28" ht="84" x14ac:dyDescent="0.15">
@@ -17756,14 +17773,14 @@
       <c r="H201" s="60"/>
       <c r="I201" s="26"/>
       <c r="J201" s="90" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="K201" s="29"/>
       <c r="L201" s="27"/>
       <c r="M201" s="30"/>
       <c r="N201" s="17"/>
       <c r="O201" s="20"/>
-      <c r="P201" s="41"/>
+      <c r="P201" s="20"/>
       <c r="Q201" s="41"/>
       <c r="R201" s="20"/>
       <c r="S201" s="46" t="s">
@@ -17811,7 +17828,7 @@
       <c r="M202" s="30"/>
       <c r="N202" s="17"/>
       <c r="O202" s="20"/>
-      <c r="P202" s="41"/>
+      <c r="P202" s="20"/>
       <c r="Q202" s="41"/>
       <c r="R202" s="20"/>
       <c r="S202" s="46" t="s">
@@ -17834,7 +17851,7 @@
         <v>819</v>
       </c>
       <c r="AB202" s="48" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="203" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -17854,16 +17871,16 @@
       <c r="H203" s="60"/>
       <c r="I203" s="26"/>
       <c r="J203" s="90" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="K203" s="90" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="L203" s="27"/>
       <c r="M203" s="30"/>
       <c r="N203" s="17"/>
       <c r="O203" s="20"/>
-      <c r="P203" s="41"/>
+      <c r="P203" s="20"/>
       <c r="Q203" s="41"/>
       <c r="R203" s="20"/>
       <c r="S203" s="46" t="s">
@@ -17893,7 +17910,7 @@
       </c>
       <c r="B204" s="55"/>
       <c r="C204" s="55" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D204" s="25" t="s">
         <v>306</v>
@@ -17904,14 +17921,14 @@
       <c r="H204" s="59"/>
       <c r="I204" s="26"/>
       <c r="J204" s="47" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="K204" s="47"/>
       <c r="L204" s="27"/>
       <c r="M204" s="30"/>
       <c r="N204" s="17"/>
       <c r="O204" s="20"/>
-      <c r="P204" s="41"/>
+      <c r="P204" s="20"/>
       <c r="Q204" s="41"/>
       <c r="R204" s="20"/>
       <c r="S204" s="46" t="s">
@@ -17921,11 +17938,11 @@
         <v>230</v>
       </c>
       <c r="U204" s="16" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="V204" s="25"/>
       <c r="W204" s="10" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="X204" s="10"/>
       <c r="Y204" s="10"/>
@@ -17933,7 +17950,7 @@
         <v>40</v>
       </c>
       <c r="AA204" s="25" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="AB204" s="48"/>
     </row>
@@ -17961,7 +17978,7 @@
         <v>918</v>
       </c>
       <c r="O205" s="20"/>
-      <c r="P205" s="41"/>
+      <c r="P205" s="20"/>
       <c r="Q205" s="41"/>
       <c r="R205" s="20"/>
       <c r="S205" s="92" t="s">
@@ -17984,7 +18001,7 @@
         <v>772</v>
       </c>
       <c r="AB205" s="48" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="206" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -17993,7 +18010,7 @@
       </c>
       <c r="B206" s="55"/>
       <c r="C206" s="55" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D206" s="25" t="s">
         <v>306</v>
@@ -18008,10 +18025,10 @@
       <c r="L206" s="27"/>
       <c r="M206" s="30"/>
       <c r="N206" s="17" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="O206" s="20"/>
-      <c r="P206" s="41"/>
+      <c r="P206" s="20"/>
       <c r="Q206" s="41"/>
       <c r="R206" s="20"/>
       <c r="S206" s="46" t="s">
@@ -18033,7 +18050,7 @@
         <v>-30</v>
       </c>
       <c r="AA206" s="25" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="AB206" s="48"/>
     </row>
@@ -18043,7 +18060,7 @@
       </c>
       <c r="B207" s="55"/>
       <c r="C207" s="55" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D207" s="25" t="s">
         <v>306</v>
@@ -18059,12 +18076,12 @@
       <c r="M207" s="30"/>
       <c r="N207" s="17"/>
       <c r="O207" s="20"/>
-      <c r="P207" s="41"/>
+      <c r="P207" s="20"/>
       <c r="Q207" s="41" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="R207" s="20" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="S207" s="46" t="s">
         <v>235</v>
@@ -18073,7 +18090,7 @@
         <v>230</v>
       </c>
       <c r="U207" s="16" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="V207" s="25"/>
       <c r="W207" s="25"/>
@@ -18083,10 +18100,10 @@
         <v>60</v>
       </c>
       <c r="AA207" s="25" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="AB207" s="48" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="208" spans="1:28" ht="48" x14ac:dyDescent="0.15">
@@ -18095,7 +18112,7 @@
       </c>
       <c r="B208" s="55"/>
       <c r="C208" s="55" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D208" s="25" t="s">
         <v>306</v>
@@ -18110,10 +18127,10 @@
       <c r="L208" s="27"/>
       <c r="M208" s="30"/>
       <c r="N208" s="17" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="O208" s="20"/>
-      <c r="P208" s="41"/>
+      <c r="P208" s="20"/>
       <c r="Q208" s="41"/>
       <c r="R208" s="20"/>
       <c r="S208" s="25" t="s">
@@ -18123,7 +18140,7 @@
         <v>230</v>
       </c>
       <c r="U208" s="16" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="V208" s="25"/>
       <c r="W208" s="25"/>
@@ -18133,10 +18150,10 @@
         <v>20</v>
       </c>
       <c r="AA208" s="25" t="s">
+        <v>1123</v>
+      </c>
+      <c r="AB208" s="48" t="s">
         <v>1124</v>
-      </c>
-      <c r="AB208" s="48" t="s">
-        <v>1125</v>
       </c>
     </row>
     <row r="209" spans="1:28" ht="84" x14ac:dyDescent="0.15">
@@ -18145,7 +18162,7 @@
       </c>
       <c r="B209" s="83"/>
       <c r="C209" s="55" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D209" s="25" t="s">
         <v>306</v>
@@ -18156,14 +18173,14 @@
       <c r="H209" s="78"/>
       <c r="I209" s="96"/>
       <c r="J209" s="29" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="K209" s="95"/>
       <c r="L209" s="97"/>
       <c r="M209" s="79"/>
       <c r="N209" s="79"/>
       <c r="O209" s="80"/>
-      <c r="P209" s="81"/>
+      <c r="P209" s="80"/>
       <c r="Q209" s="81"/>
       <c r="R209" s="20"/>
       <c r="S209" s="77" t="s">
@@ -18173,7 +18190,7 @@
         <v>230</v>
       </c>
       <c r="U209" s="10" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="V209" s="77"/>
       <c r="W209" s="77"/>
@@ -18183,10 +18200,10 @@
         <v>15</v>
       </c>
       <c r="AA209" s="25" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="AB209" s="48" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="210" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -18195,7 +18212,7 @@
       </c>
       <c r="B210" s="83"/>
       <c r="C210" s="55" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D210" s="25" t="s">
         <v>306</v>
@@ -18211,12 +18228,12 @@
       <c r="M210" s="79"/>
       <c r="N210" s="79"/>
       <c r="O210" s="80"/>
-      <c r="P210" s="81"/>
+      <c r="P210" s="80"/>
       <c r="Q210" s="81" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="R210" s="20" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="S210" s="77" t="s">
         <v>235</v>
@@ -18225,7 +18242,7 @@
         <v>230</v>
       </c>
       <c r="U210" s="10" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="V210" s="77"/>
       <c r="W210" s="77"/>
@@ -18235,7 +18252,7 @@
         <v>0</v>
       </c>
       <c r="AA210" s="25" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="AB210" s="48"/>
     </row>
@@ -18245,7 +18262,7 @@
       </c>
       <c r="B211" s="83"/>
       <c r="C211" s="55" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="D211" s="25" t="s">
         <v>306</v>
@@ -18261,9 +18278,9 @@
       <c r="M211" s="79"/>
       <c r="N211" s="79"/>
       <c r="O211" s="20" t="s">
-        <v>1157</v>
-      </c>
-      <c r="P211" s="81">
+        <v>1156</v>
+      </c>
+      <c r="P211" s="80">
         <v>2</v>
       </c>
       <c r="Q211" s="81"/>
@@ -18275,11 +18292,11 @@
         <v>230</v>
       </c>
       <c r="U211" s="10" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="V211" s="77"/>
       <c r="W211" s="25" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="X211" s="77"/>
       <c r="Y211" s="77"/>
@@ -18287,7 +18304,7 @@
         <v>40</v>
       </c>
       <c r="AA211" s="109" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="AB211" s="48" t="s">
         <v>609</v>
@@ -18299,7 +18316,7 @@
       </c>
       <c r="B212" s="83"/>
       <c r="C212" s="55" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="D212" s="25" t="s">
         <v>306</v>
@@ -18315,9 +18332,9 @@
       <c r="M212" s="79"/>
       <c r="N212" s="79"/>
       <c r="O212" s="20" t="s">
-        <v>1160</v>
-      </c>
-      <c r="P212" s="81">
+        <v>1159</v>
+      </c>
+      <c r="P212" s="80">
         <v>2</v>
       </c>
       <c r="Q212" s="81"/>
@@ -18329,11 +18346,11 @@
         <v>230</v>
       </c>
       <c r="U212" s="10" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="V212" s="77"/>
       <c r="W212" s="25" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="X212" s="77"/>
       <c r="Y212" s="77"/>
@@ -18341,7 +18358,7 @@
         <v>20</v>
       </c>
       <c r="AA212" s="109" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="AB212" s="48" t="s">
         <v>609</v>
@@ -18373,7 +18390,7 @@
       </c>
       <c r="N213" s="17"/>
       <c r="O213" s="20"/>
-      <c r="P213" s="41"/>
+      <c r="P213" s="20"/>
       <c r="Q213" s="41"/>
       <c r="R213" s="20"/>
       <c r="S213" s="46" t="s">
@@ -18423,7 +18440,7 @@
       </c>
       <c r="N214" s="17"/>
       <c r="O214" s="20"/>
-      <c r="P214" s="41"/>
+      <c r="P214" s="20"/>
       <c r="Q214" s="41"/>
       <c r="R214" s="20"/>
       <c r="S214" s="46" t="s">
@@ -18473,7 +18490,7 @@
       </c>
       <c r="N215" s="17"/>
       <c r="O215" s="20"/>
-      <c r="P215" s="41"/>
+      <c r="P215" s="20"/>
       <c r="Q215" s="41"/>
       <c r="R215" s="20"/>
       <c r="S215" s="46" t="s">
@@ -18523,7 +18540,7 @@
       </c>
       <c r="N216" s="17"/>
       <c r="O216" s="20"/>
-      <c r="P216" s="41"/>
+      <c r="P216" s="20"/>
       <c r="Q216" s="41"/>
       <c r="R216" s="20"/>
       <c r="S216" s="46" t="s">
@@ -18573,7 +18590,7 @@
       </c>
       <c r="N217" s="17"/>
       <c r="O217" s="20"/>
-      <c r="P217" s="41"/>
+      <c r="P217" s="20"/>
       <c r="Q217" s="41"/>
       <c r="R217" s="20"/>
       <c r="S217" s="46" t="s">
@@ -18623,7 +18640,7 @@
       </c>
       <c r="N218" s="17"/>
       <c r="O218" s="20"/>
-      <c r="P218" s="41"/>
+      <c r="P218" s="20"/>
       <c r="Q218" s="41"/>
       <c r="R218" s="20"/>
       <c r="S218" s="46" t="s">
@@ -18673,7 +18690,7 @@
       </c>
       <c r="N219" s="17"/>
       <c r="O219" s="20"/>
-      <c r="P219" s="41"/>
+      <c r="P219" s="20"/>
       <c r="Q219" s="41"/>
       <c r="R219" s="20"/>
       <c r="S219" s="46" t="s">
@@ -18723,7 +18740,7 @@
       </c>
       <c r="N220" s="17"/>
       <c r="O220" s="20"/>
-      <c r="P220" s="41"/>
+      <c r="P220" s="20"/>
       <c r="Q220" s="41"/>
       <c r="R220" s="20"/>
       <c r="S220" s="46" t="s">
@@ -18773,7 +18790,7 @@
       </c>
       <c r="N221" s="17"/>
       <c r="O221" s="20"/>
-      <c r="P221" s="41"/>
+      <c r="P221" s="20"/>
       <c r="Q221" s="41"/>
       <c r="R221" s="20"/>
       <c r="S221" s="46" t="s">
@@ -18823,7 +18840,7 @@
       </c>
       <c r="N222" s="17"/>
       <c r="O222" s="20"/>
-      <c r="P222" s="41"/>
+      <c r="P222" s="20"/>
       <c r="Q222" s="41"/>
       <c r="R222" s="20"/>
       <c r="S222" s="46" t="s">
@@ -18873,7 +18890,7 @@
       </c>
       <c r="N223" s="17"/>
       <c r="O223" s="20"/>
-      <c r="P223" s="41"/>
+      <c r="P223" s="20"/>
       <c r="Q223" s="41"/>
       <c r="R223" s="20"/>
       <c r="S223" s="46" t="s">
@@ -18923,7 +18940,7 @@
       </c>
       <c r="N224" s="17"/>
       <c r="O224" s="20"/>
-      <c r="P224" s="41"/>
+      <c r="P224" s="20"/>
       <c r="Q224" s="41"/>
       <c r="R224" s="20"/>
       <c r="S224" s="46" t="s">
@@ -18971,11 +18988,11 @@
       <c r="M225" s="30"/>
       <c r="N225" s="17"/>
       <c r="O225" s="20"/>
-      <c r="P225" s="41"/>
+      <c r="P225" s="20"/>
       <c r="Q225" s="41"/>
       <c r="R225" s="20"/>
       <c r="S225" s="46" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="T225" s="44" t="s">
         <v>232</v>
@@ -19021,7 +19038,7 @@
       </c>
       <c r="N226" s="17"/>
       <c r="O226" s="20"/>
-      <c r="P226" s="41"/>
+      <c r="P226" s="20"/>
       <c r="Q226" s="41"/>
       <c r="R226" s="20"/>
       <c r="S226" s="46" t="s">
@@ -19074,10 +19091,10 @@
       <c r="L227" s="27"/>
       <c r="M227" s="30"/>
       <c r="N227" s="17" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="O227" s="20"/>
-      <c r="P227" s="41"/>
+      <c r="P227" s="20"/>
       <c r="Q227" s="41"/>
       <c r="R227" s="20"/>
       <c r="S227" s="46" t="s">
@@ -19134,10 +19151,10 @@
       <c r="L228" s="27"/>
       <c r="M228" s="30"/>
       <c r="N228" s="17" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="O228" s="20"/>
-      <c r="P228" s="41"/>
+      <c r="P228" s="20"/>
       <c r="Q228" s="41"/>
       <c r="R228" s="20"/>
       <c r="S228" s="46" t="s">
@@ -19189,7 +19206,7 @@
         <v>879</v>
       </c>
       <c r="O229" s="20"/>
-      <c r="P229" s="41"/>
+      <c r="P229" s="20"/>
       <c r="Q229" s="41"/>
       <c r="R229" s="20"/>
       <c r="S229" s="35" t="s">
@@ -19237,7 +19254,7 @@
         <v>888</v>
       </c>
       <c r="O230" s="20"/>
-      <c r="P230" s="41"/>
+      <c r="P230" s="20"/>
       <c r="Q230" s="41"/>
       <c r="R230" s="20"/>
       <c r="S230" s="35" t="s">
@@ -19289,12 +19306,12 @@
       <c r="M231" s="30"/>
       <c r="N231" s="17"/>
       <c r="O231" s="20"/>
-      <c r="P231" s="41"/>
+      <c r="P231" s="20"/>
       <c r="Q231" s="41" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="R231" s="20" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="S231" s="35" t="s">
         <v>235</v>
@@ -19343,7 +19360,7 @@
       <c r="O232" s="20" t="s">
         <v>834</v>
       </c>
-      <c r="P232" s="41">
+      <c r="P232" s="20">
         <v>1</v>
       </c>
       <c r="Q232" s="41"/>
@@ -19395,7 +19412,7 @@
       <c r="O233" s="20" t="s">
         <v>889</v>
       </c>
-      <c r="P233" s="41">
+      <c r="P233" s="20">
         <v>4</v>
       </c>
       <c r="Q233" s="41"/>
@@ -19451,12 +19468,12 @@
       <c r="M234" s="30"/>
       <c r="N234" s="17"/>
       <c r="O234" s="20"/>
-      <c r="P234" s="41"/>
+      <c r="P234" s="20"/>
       <c r="Q234" s="41" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="R234" s="20" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="S234" s="46" t="s">
         <v>235</v>
@@ -19465,7 +19482,7 @@
         <v>232</v>
       </c>
       <c r="U234" s="16" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="V234" s="25"/>
       <c r="W234" s="1" t="s">
@@ -19487,7 +19504,7 @@
       </c>
       <c r="B235" s="91"/>
       <c r="C235" s="91" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="D235" s="25" t="s">
         <v>627</v>
@@ -19505,7 +19522,7 @@
       <c r="O235" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="P235" s="41">
+      <c r="P235" s="20">
         <v>1</v>
       </c>
       <c r="Q235" s="41"/>

</xml_diff>